<commit_message>
duy lay tien loi ngay 30-31
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -11,13 +11,14 @@
     <sheet name="CHÂU" sheetId="3" r:id="rId2"/>
     <sheet name="HÀ" sheetId="4" r:id="rId3"/>
     <sheet name="GIANG" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="98">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -281,6 +282,36 @@
   </si>
   <si>
     <t>Duy lấy tiền lời 1tr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nguyen tien dinh </t>
+  </si>
+  <si>
+    <t>lam van khoi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tổng = </t>
+  </si>
+  <si>
+    <t>dang minh nhat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hoang thi ngoc linh </t>
+  </si>
+  <si>
+    <t>ha thi dao</t>
+  </si>
+  <si>
+    <t>vo thi dang nga</t>
+  </si>
+  <si>
+    <t>phan chi cuong</t>
+  </si>
+  <si>
+    <t>30/01/2024</t>
+  </si>
+  <si>
+    <t>Duy lấy tiền lời ngày 30-31 - 7tr</t>
   </si>
 </sst>
 </file>
@@ -387,7 +418,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -428,6 +459,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -735,11 +767,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J58"/>
+  <dimension ref="A1:J59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D61" sqref="D61"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,10 +800,10 @@
       <c r="D1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="14"/>
+      <c r="I1" s="15"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -1528,7 +1560,7 @@
         <v>700</v>
       </c>
       <c r="D53" s="6">
-        <f>D52+C53</f>
+        <f t="shared" ref="D53:D58" si="6">D52+C53</f>
         <v>5290</v>
       </c>
     </row>
@@ -1543,7 +1575,7 @@
         <v>700</v>
       </c>
       <c r="D54" s="6">
-        <f>D53+C54</f>
+        <f t="shared" si="6"/>
         <v>5990</v>
       </c>
     </row>
@@ -1558,7 +1590,7 @@
         <v>700</v>
       </c>
       <c r="D55" s="6">
-        <f>D54+C55</f>
+        <f t="shared" si="6"/>
         <v>6690</v>
       </c>
     </row>
@@ -1573,7 +1605,7 @@
         <v>4000</v>
       </c>
       <c r="D56" s="6">
-        <f>D55+C56</f>
+        <f t="shared" si="6"/>
         <v>10690</v>
       </c>
     </row>
@@ -1585,7 +1617,7 @@
         <v>-10000</v>
       </c>
       <c r="D57" s="6">
-        <f>D56+C57</f>
+        <f t="shared" si="6"/>
         <v>690</v>
       </c>
     </row>
@@ -1600,8 +1632,23 @@
         <v>1000</v>
       </c>
       <c r="D58" s="6">
-        <f>D57+C58</f>
+        <f t="shared" si="6"/>
         <v>1690</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C59" s="5">
+        <v>7000</v>
+      </c>
+      <c r="D59" s="6">
+        <f>D58+C59</f>
+        <v>8690</v>
       </c>
     </row>
   </sheetData>
@@ -1652,10 +1699,10 @@
       <c r="E1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="14"/>
+      <c r="I1" s="15"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
@@ -1791,10 +1838,10 @@
       <c r="E1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="14"/>
+      <c r="I1" s="15"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -1927,10 +1974,10 @@
       <c r="E1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="14"/>
+      <c r="I1" s="15"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -1977,4 +2024,87 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1">
+        <v>310</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" s="14">
+        <f>SUM(B:B)</f>
+        <v>5660</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7">
+        <v>500</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
duy chuyen cho co diem 700
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="102">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -321,6 +321,9 @@
   </si>
   <si>
     <t>30/01/2023</t>
+  </si>
+  <si>
+    <t>Duy chuyển cho cô Diễm 700k</t>
   </si>
 </sst>
 </file>
@@ -776,11 +779,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J62"/>
+  <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1690,6 +1693,21 @@
       <c r="D62" s="6">
         <f>D61+C62</f>
         <v>8690</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="9">
+        <v>45293</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C63" s="5">
+        <v>700</v>
+      </c>
+      <c r="D63" s="6">
+        <f>D62+C63</f>
+        <v>9390</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
duy chuyen co co diem 1tr - cho vay 10tr
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="102">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -323,7 +323,7 @@
     <t>30/01/2023</t>
   </si>
   <si>
-    <t>Duy chuyển cho cô Diễm 700k</t>
+    <t>Duy chuyển cho cô Diễm 1.7tr</t>
   </si>
 </sst>
 </file>
@@ -779,11 +779,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J63"/>
+  <dimension ref="A1:J65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D64" sqref="D64"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,8 +854,8 @@
         <v>20</v>
       </c>
       <c r="J3" s="6">
-        <f>SUM(I3:I43)</f>
-        <v>220</v>
+        <f>SUM(I3:I44)</f>
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -884,7 +884,7 @@
         <v>-10000</v>
       </c>
       <c r="D5" s="6">
-        <f t="shared" ref="D5:D19" si="0">D4+C5</f>
+        <f t="shared" ref="D5:D12" si="0">D4+C5</f>
         <v>8490</v>
       </c>
       <c r="H5" s="9" t="s">
@@ -1053,540 +1053,533 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="5">
-        <v>4400</v>
-      </c>
-      <c r="D18" s="6">
-        <f>D16+C18</f>
-        <v>12890</v>
-      </c>
       <c r="H18" s="9">
-        <v>44964</v>
+        <v>45293</v>
       </c>
       <c r="I18" s="5">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="5">
+        <v>4400</v>
+      </c>
+      <c r="D19" s="6">
+        <f>D16+C19</f>
+        <v>12890</v>
+      </c>
+      <c r="H19" s="9">
+        <v>44964</v>
+      </c>
+      <c r="I19" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C20" s="5">
         <v>-10000</v>
       </c>
-      <c r="D19" s="6">
-        <f t="shared" si="0"/>
+      <c r="D20" s="6">
+        <f>D19+C20</f>
         <v>2890</v>
       </c>
-      <c r="H19" s="9">
+      <c r="H20" s="9">
         <v>44966</v>
-      </c>
-      <c r="I19" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="9">
-        <v>44967</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="5">
-        <v>1600</v>
-      </c>
-      <c r="D20" s="6">
-        <f t="shared" ref="D20:D27" si="1">D19+C20</f>
-        <v>4490</v>
-      </c>
-      <c r="H20" s="9">
-        <v>44968</v>
       </c>
       <c r="I20" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="9">
+        <v>44967</v>
+      </c>
       <c r="B21" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="5">
+        <v>1600</v>
+      </c>
+      <c r="D21" s="6">
+        <f t="shared" ref="D21:D28" si="1">D20+C21</f>
+        <v>4490</v>
+      </c>
+      <c r="H21" s="9">
+        <v>44968</v>
+      </c>
+      <c r="I21" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C22" s="5">
         <v>3000</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D22" s="6">
         <f t="shared" si="1"/>
         <v>7490</v>
       </c>
-      <c r="H21" s="9">
+      <c r="H22" s="9">
         <v>44969</v>
       </c>
-      <c r="I21" s="5">
+      <c r="I22" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B23" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C23" s="5">
         <v>2000</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D23" s="6">
         <f t="shared" si="1"/>
         <v>9490</v>
       </c>
-      <c r="H22" s="9">
+      <c r="H23" s="9">
         <v>45334</v>
       </c>
-      <c r="I22" s="5">
+      <c r="I23" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B24" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C24" s="5">
         <v>3000</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D24" s="6">
         <f t="shared" si="1"/>
         <v>12490</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="4" t="s">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C25" s="5">
         <v>-10000</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D25" s="6">
         <f t="shared" si="1"/>
         <v>2490</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B26" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C26" s="5">
         <v>4960</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D26" s="6">
         <f t="shared" si="1"/>
         <v>7450</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B27" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C27" s="5">
         <v>4000</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D27" s="6">
         <f t="shared" si="1"/>
         <v>11450</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="4" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C28" s="5">
         <v>-10000</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D28" s="6">
         <f t="shared" si="1"/>
         <v>1450</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="4" t="s">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C29" s="5">
         <v>7640</v>
       </c>
-      <c r="D28" s="6">
-        <f t="shared" ref="D28:D33" si="2">D27+C28</f>
+      <c r="D29" s="6">
+        <f t="shared" ref="D29:D34" si="2">D28+C29</f>
         <v>9090</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="9">
         <v>44968</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B30" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C30" s="5">
         <v>3000</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D30" s="6">
         <f t="shared" si="2"/>
         <v>12090</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="4" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C31" s="5">
         <v>-10000</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D31" s="6">
         <f t="shared" si="2"/>
         <v>2090</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="9">
         <v>44996</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B32" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C32" s="5">
         <v>800</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D32" s="6">
         <f t="shared" si="2"/>
         <v>2890</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B33" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C33" s="5">
         <v>2000</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D33" s="6">
         <f t="shared" si="2"/>
         <v>4890</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B34" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C34" s="5">
         <v>4000</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D34" s="6">
         <f t="shared" si="2"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B35" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C35" s="5">
         <v>4000</v>
       </c>
-      <c r="D34" s="6">
-        <f t="shared" ref="D34:D39" si="3">D33+C34</f>
+      <c r="D35" s="6">
+        <f t="shared" ref="D35:D40" si="3">D34+C35</f>
         <v>12890</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="4" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C35" s="5">
+      <c r="C36" s="5">
         <v>5000</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D36" s="6">
         <f t="shared" si="3"/>
         <v>17890</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="4" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C36" s="5">
+      <c r="C37" s="5">
         <v>-10000</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D37" s="6">
         <f t="shared" si="3"/>
         <v>7890</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="9">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="9">
         <v>44969</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B38" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C37" s="5">
+      <c r="C38" s="5">
         <v>900</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D38" s="6">
         <f t="shared" si="3"/>
         <v>8790</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B38" s="4" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C38" s="5">
+      <c r="C39" s="5">
         <v>4000</v>
       </c>
-      <c r="D38" s="6">
+      <c r="D39" s="6">
         <f t="shared" si="3"/>
         <v>12790</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B39" s="4" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C39" s="5">
+      <c r="C40" s="5">
         <v>-10000</v>
       </c>
-      <c r="D39" s="6">
+      <c r="D40" s="6">
         <f t="shared" si="3"/>
         <v>2790</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C40" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D40" s="6">
-        <f t="shared" ref="D40:D47" si="4">D39+C40</f>
-        <v>4790</v>
-      </c>
-    </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C41" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D41" s="6">
+        <f t="shared" ref="D41:D48" si="4">D40+C41</f>
+        <v>4790</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B42" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C41" s="5">
+      <c r="C42" s="5">
         <v>700</v>
       </c>
-      <c r="D41" s="6">
+      <c r="D42" s="6">
         <f t="shared" si="4"/>
         <v>5490</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B42" s="4" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C43" s="5">
         <v>4000</v>
       </c>
-      <c r="D42" s="6">
+      <c r="D43" s="6">
         <f t="shared" si="4"/>
         <v>9490</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="9" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B44" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C43" s="5">
+      <c r="C44" s="5">
         <v>600</v>
       </c>
-      <c r="D43" s="6">
+      <c r="D44" s="6">
         <f t="shared" si="4"/>
         <v>10090</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B44" s="4" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C45" s="5">
         <v>-10000</v>
       </c>
-      <c r="D44" s="6">
+      <c r="D45" s="6">
         <f t="shared" si="4"/>
         <v>90</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="9" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B46" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C45" s="5">
+      <c r="C46" s="5">
         <f>700+5000+300+600+400+1000+800</f>
         <v>8800</v>
       </c>
-      <c r="D45" s="6">
+      <c r="D46" s="6">
         <f t="shared" si="4"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B46" s="4" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B47" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C46" s="5">
+      <c r="C47" s="5">
         <v>6000</v>
       </c>
-      <c r="D46" s="6">
+      <c r="D47" s="6">
         <f t="shared" si="4"/>
         <v>14890</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B47" s="4" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B48" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C48" s="5">
         <v>-10000</v>
       </c>
-      <c r="D47" s="6">
+      <c r="D48" s="6">
         <f t="shared" si="4"/>
         <v>4890</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="9" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B49" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C48" s="5">
+      <c r="C49" s="5">
         <v>500</v>
       </c>
-      <c r="D48" s="6">
-        <f t="shared" ref="D48:D53" si="5">D47+C48</f>
+      <c r="D49" s="6">
+        <f t="shared" ref="D49:D54" si="5">D48+C49</f>
         <v>5390</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="9">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="9">
         <v>45323</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B50" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C49" s="5">
+      <c r="C50" s="5">
         <v>700</v>
       </c>
-      <c r="D49" s="6">
+      <c r="D50" s="6">
         <f t="shared" si="5"/>
         <v>6090</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B50" s="4" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B51" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C50" s="5">
+      <c r="C51" s="5">
         <v>1500</v>
       </c>
-      <c r="D50" s="6">
+      <c r="D51" s="6">
         <f t="shared" si="5"/>
         <v>7590</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B51" s="4" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C51" s="5">
+      <c r="C52" s="5">
         <v>5000</v>
       </c>
-      <c r="D51" s="6">
+      <c r="D52" s="6">
         <f t="shared" si="5"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B52" s="4" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B53" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C52" s="5">
+      <c r="C53" s="5">
         <v>-10000</v>
       </c>
-      <c r="D52" s="6">
+      <c r="D53" s="6">
         <f t="shared" si="5"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="9" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B54" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C53" s="5">
+      <c r="C54" s="5">
         <v>2000</v>
       </c>
-      <c r="D53" s="6">
+      <c r="D54" s="6">
         <f t="shared" si="5"/>
         <v>4590</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="9">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="9">
         <v>45474</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C54" s="5">
-        <v>700</v>
-      </c>
-      <c r="D54" s="6">
-        <f t="shared" ref="D54:D59" si="6">D53+C54</f>
-        <v>5290</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="9" t="s">
-        <v>82</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>77</v>
@@ -1595,119 +1588,146 @@
         <v>700</v>
       </c>
       <c r="D55" s="6">
+        <f t="shared" ref="D55:D60" si="6">D54+C55</f>
+        <v>5290</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C56" s="5">
+        <v>700</v>
+      </c>
+      <c r="D56" s="6">
         <f t="shared" si="6"/>
         <v>5990</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="9" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B57" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C56" s="5">
+      <c r="C57" s="5">
         <v>700</v>
       </c>
-      <c r="D56" s="6">
+      <c r="D57" s="6">
         <f t="shared" si="6"/>
         <v>6690</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="9" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B58" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C57" s="5">
+      <c r="C58" s="5">
         <v>4000</v>
       </c>
-      <c r="D57" s="6">
+      <c r="D58" s="6">
         <f t="shared" si="6"/>
         <v>10690</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B58" s="4" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B59" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C58" s="5">
+      <c r="C59" s="5">
         <v>-10000</v>
       </c>
-      <c r="D58" s="6">
+      <c r="D59" s="6">
         <f t="shared" si="6"/>
         <v>690</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="9" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B60" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C59" s="5">
+      <c r="C60" s="5">
         <v>1000</v>
       </c>
-      <c r="D59" s="6">
+      <c r="D60" s="6">
         <f t="shared" si="6"/>
         <v>1690</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="9" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B61" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C60" s="5">
+      <c r="C61" s="5">
         <v>7000</v>
-      </c>
-      <c r="D60" s="6">
-        <f>D59+C60</f>
-        <v>8690</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B61" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C61" s="5">
-        <v>10000</v>
       </c>
       <c r="D61" s="6">
         <f>D60+C61</f>
-        <v>18690</v>
+        <v>8690</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B62" s="4" t="s">
-        <v>20</v>
+        <v>99</v>
       </c>
       <c r="C62" s="5">
-        <v>-10000</v>
+        <v>10000</v>
       </c>
       <c r="D62" s="6">
         <f>D61+C62</f>
-        <v>8690</v>
+        <v>18690</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="9">
-        <v>45293</v>
-      </c>
       <c r="B63" s="4" t="s">
-        <v>101</v>
+        <v>20</v>
       </c>
       <c r="C63" s="5">
-        <v>700</v>
+        <v>-10000</v>
       </c>
       <c r="D63" s="6">
         <f>D62+C63</f>
-        <v>9390</v>
+        <v>8690</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="9">
+        <v>45293</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C64" s="5">
+        <v>1700</v>
+      </c>
+      <c r="D64" s="6">
+        <f>D63+C64</f>
+        <v>10390</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B65" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C65" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D65" s="6">
+        <f>D64+C65</f>
+        <v>390</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Duy lay tien loi ngay 13
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="106">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -330,6 +330,12 @@
   </si>
   <si>
     <t>Duy lấy tiền lời 6tr</t>
+  </si>
+  <si>
+    <t>13/02/2024</t>
+  </si>
+  <si>
+    <t>Duy lấy tiền lời 2tr</t>
   </si>
 </sst>
 </file>
@@ -794,11 +800,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K66"/>
+  <dimension ref="A1:K67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D67" sqref="D67"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1694,7 +1700,7 @@
         <v>7000</v>
       </c>
       <c r="D61" s="6">
-        <f>D60+C61</f>
+        <f t="shared" ref="D61:D66" si="7">D60+C61</f>
         <v>8690</v>
       </c>
     </row>
@@ -1706,7 +1712,7 @@
         <v>10000</v>
       </c>
       <c r="D62" s="6">
-        <f>D61+C62</f>
+        <f t="shared" si="7"/>
         <v>18690</v>
       </c>
     </row>
@@ -1718,7 +1724,7 @@
         <v>-10000</v>
       </c>
       <c r="D63" s="6">
-        <f>D62+C63</f>
+        <f t="shared" si="7"/>
         <v>8690</v>
       </c>
     </row>
@@ -1733,7 +1739,7 @@
         <v>1700</v>
       </c>
       <c r="D64" s="6">
-        <f>D63+C64</f>
+        <f t="shared" si="7"/>
         <v>10390</v>
       </c>
     </row>
@@ -1745,7 +1751,7 @@
         <v>-10000</v>
       </c>
       <c r="D65" s="6">
-        <f>D64+C65</f>
+        <f t="shared" si="7"/>
         <v>390</v>
       </c>
     </row>
@@ -1760,8 +1766,23 @@
         <v>6000</v>
       </c>
       <c r="D66" s="6">
-        <f>D65+C66</f>
+        <f t="shared" si="7"/>
         <v>6390</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C67" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D67" s="6">
+        <f>D66+C67</f>
+        <v>8390</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
duy lay tien lơi ngay 2102 - tong ket 240tr
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="108">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -336,6 +336,12 @@
   </si>
   <si>
     <t>Duy lấy tiền lời 2tr</t>
+  </si>
+  <si>
+    <t>21/02/2024</t>
+  </si>
+  <si>
+    <t>Duy lấy tiền lời 5tr</t>
   </si>
 </sst>
 </file>
@@ -800,11 +806,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K67"/>
+  <dimension ref="A1:K70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D68" sqref="D68"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,7 +827,7 @@
     <col min="12" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -839,7 +845,7 @@
       </c>
       <c r="I1" s="16"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
@@ -859,7 +865,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>13</v>
       </c>
@@ -876,11 +882,11 @@
         <v>20</v>
       </c>
       <c r="J3" s="6">
-        <f>SUM(I3:I44)</f>
-        <v>230</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <f>SUM(I3:I45)</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>16</v>
       </c>
@@ -898,7 +904,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>18</v>
       </c>
@@ -906,7 +912,7 @@
         <v>-10000</v>
       </c>
       <c r="D5" s="6">
-        <f t="shared" ref="D5:D12" si="0">D4+C5</f>
+        <f t="shared" ref="D5:D13" si="0">D4+C5</f>
         <v>8490</v>
       </c>
       <c r="H5" s="9" t="s">
@@ -916,7 +922,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>44966</v>
       </c>
@@ -937,7 +943,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H7" s="9" t="s">
         <v>41</v>
       </c>
@@ -945,7 +951,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H8" s="9" t="s">
         <v>84</v>
       </c>
@@ -953,673 +959,669 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H9" s="9" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
       <c r="I9" s="5">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="5">
-        <v>-10000</v>
-      </c>
-      <c r="D10" s="6">
-        <f>D6+C10</f>
-        <v>490</v>
-      </c>
+      <c r="K9" s="15" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H10" s="9" t="s">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="I10" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D11" s="6">
+        <f>D6+C11</f>
+        <v>490</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C12" s="5">
         <v>2000</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D12" s="6">
         <f t="shared" si="0"/>
         <v>2490</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="H12" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I12" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B13" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C13" s="5">
         <v>3000</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D13" s="6">
         <f t="shared" si="0"/>
         <v>5490</v>
       </c>
-      <c r="H12" s="9" t="s">
+      <c r="H13" s="9" t="s">
         <v>24</v>
-      </c>
-      <c r="I12" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H13" s="9" t="s">
-        <v>59</v>
       </c>
       <c r="I13" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H14" s="9" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="I14" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H15" s="9" t="s">
-        <v>100</v>
+        <v>73</v>
       </c>
       <c r="I15" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="5">
-        <v>3000</v>
-      </c>
-      <c r="D16" s="6">
-        <f>D12+C16</f>
-        <v>8490</v>
-      </c>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H16" s="9" t="s">
-        <v>12</v>
+        <v>100</v>
       </c>
       <c r="I16" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="5">
+        <v>3000</v>
+      </c>
+      <c r="D17" s="6">
+        <f>D13+C17</f>
+        <v>8490</v>
+      </c>
       <c r="H17" s="9" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="I17" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H18" s="9">
-        <v>45293</v>
+      <c r="H18" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="I18" s="5">
         <v>10</v>
       </c>
-      <c r="K18" s="15" t="s">
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H19" s="9">
+        <v>45293</v>
+      </c>
+      <c r="I19" s="5">
+        <v>10</v>
+      </c>
+      <c r="K19" s="15" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="5">
-        <v>4400</v>
-      </c>
-      <c r="D19" s="6">
-        <f>D16+C19</f>
-        <v>12890</v>
-      </c>
-      <c r="H19" s="9">
-        <v>44964</v>
-      </c>
-      <c r="I19" s="5">
-        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="5">
+        <v>4400</v>
+      </c>
+      <c r="D20" s="6">
+        <f>D17+C20</f>
+        <v>12890</v>
+      </c>
+      <c r="H20" s="9">
+        <v>44964</v>
+      </c>
+      <c r="I20" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C21" s="5">
         <v>-10000</v>
       </c>
-      <c r="D20" s="6">
-        <f>D19+C20</f>
+      <c r="D21" s="6">
+        <f>D20+C21</f>
         <v>2890</v>
       </c>
-      <c r="H20" s="9">
+      <c r="H21" s="9">
         <v>44966</v>
-      </c>
-      <c r="I20" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="9">
-        <v>44967</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="5">
-        <v>1600</v>
-      </c>
-      <c r="D21" s="6">
-        <f t="shared" ref="D21:D28" si="1">D20+C21</f>
-        <v>4490</v>
-      </c>
-      <c r="H21" s="9">
-        <v>44968</v>
       </c>
       <c r="I21" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="9">
+        <v>44967</v>
+      </c>
       <c r="B22" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="5">
+        <v>1600</v>
+      </c>
+      <c r="D22" s="6">
+        <f t="shared" ref="D22:D29" si="1">D21+C22</f>
+        <v>4490</v>
+      </c>
+      <c r="H22" s="9">
+        <v>44968</v>
+      </c>
+      <c r="I22" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C23" s="5">
         <v>3000</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D23" s="6">
         <f t="shared" si="1"/>
         <v>7490</v>
       </c>
-      <c r="H22" s="9">
+      <c r="H23" s="9">
         <v>44969</v>
       </c>
-      <c r="I22" s="5">
+      <c r="I23" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B24" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C24" s="5">
         <v>2000</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D24" s="6">
         <f t="shared" si="1"/>
         <v>9490</v>
       </c>
-      <c r="H23" s="9">
+      <c r="H24" s="9">
         <v>45334</v>
       </c>
-      <c r="I23" s="5">
+      <c r="I24" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B25" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C25" s="5">
         <v>3000</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D25" s="6">
         <f t="shared" si="1"/>
         <v>12490</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="4" t="s">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C26" s="5">
         <v>-10000</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D26" s="6">
         <f t="shared" si="1"/>
         <v>2490</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B27" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C27" s="5">
         <v>4960</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D27" s="6">
         <f t="shared" si="1"/>
         <v>7450</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B28" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C28" s="5">
         <v>4000</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D28" s="6">
         <f t="shared" si="1"/>
         <v>11450</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="4" t="s">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C29" s="5">
         <v>-10000</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D29" s="6">
         <f t="shared" si="1"/>
         <v>1450</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="4" t="s">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C30" s="5">
         <v>7640</v>
       </c>
-      <c r="D29" s="6">
-        <f t="shared" ref="D29:D34" si="2">D28+C29</f>
+      <c r="D30" s="6">
+        <f t="shared" ref="D30:D35" si="2">D29+C30</f>
         <v>9090</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="9">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="9">
         <v>44968</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B31" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C31" s="5">
         <v>3000</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D31" s="6">
         <f t="shared" si="2"/>
         <v>12090</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B31" s="4" t="s">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C32" s="5">
         <v>-10000</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D32" s="6">
         <f t="shared" si="2"/>
         <v>2090</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="9">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="9">
         <v>44996</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B33" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C33" s="5">
         <v>800</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D33" s="6">
         <f t="shared" si="2"/>
         <v>2890</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B34" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C34" s="5">
         <v>2000</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D34" s="6">
         <f t="shared" si="2"/>
         <v>4890</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B35" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C35" s="5">
         <v>4000</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D35" s="6">
         <f t="shared" si="2"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B36" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C35" s="5">
+      <c r="C36" s="5">
         <v>4000</v>
       </c>
-      <c r="D35" s="6">
-        <f t="shared" ref="D35:D40" si="3">D34+C35</f>
+      <c r="D36" s="6">
+        <f t="shared" ref="D36:D41" si="3">D35+C36</f>
         <v>12890</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="4" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C36" s="5">
+      <c r="C37" s="5">
         <v>5000</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D37" s="6">
         <f t="shared" si="3"/>
         <v>17890</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="4" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="5">
+      <c r="C38" s="5">
         <v>-10000</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D38" s="6">
         <f t="shared" si="3"/>
         <v>7890</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="9">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="9">
         <v>44969</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B39" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C38" s="5">
+      <c r="C39" s="5">
         <v>900</v>
       </c>
-      <c r="D38" s="6">
+      <c r="D39" s="6">
         <f t="shared" si="3"/>
         <v>8790</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B39" s="4" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C39" s="5">
+      <c r="C40" s="5">
         <v>4000</v>
       </c>
-      <c r="D39" s="6">
+      <c r="D40" s="6">
         <f t="shared" si="3"/>
         <v>12790</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="4" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C40" s="5">
+      <c r="C41" s="5">
         <v>-10000</v>
       </c>
-      <c r="D40" s="6">
+      <c r="D41" s="6">
         <f t="shared" si="3"/>
         <v>2790</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C41" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D41" s="6">
-        <f t="shared" ref="D41:D48" si="4">D40+C41</f>
-        <v>4790</v>
-      </c>
-    </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D42" s="6">
+        <f t="shared" ref="D42:D49" si="4">D41+C42</f>
+        <v>4790</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B43" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C43" s="5">
         <v>700</v>
       </c>
-      <c r="D42" s="6">
+      <c r="D43" s="6">
         <f t="shared" si="4"/>
         <v>5490</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B43" s="4" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C43" s="5">
+      <c r="C44" s="5">
         <v>4000</v>
       </c>
-      <c r="D43" s="6">
+      <c r="D44" s="6">
         <f t="shared" si="4"/>
         <v>9490</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="9" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B45" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C45" s="5">
         <v>600</v>
       </c>
-      <c r="D44" s="6">
+      <c r="D45" s="6">
         <f t="shared" si="4"/>
         <v>10090</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B45" s="4" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C45" s="5">
+      <c r="C46" s="5">
         <v>-10000</v>
       </c>
-      <c r="D45" s="6">
+      <c r="D46" s="6">
         <f t="shared" si="4"/>
         <v>90</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="9" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B47" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C46" s="5">
+      <c r="C47" s="5">
         <f>700+5000+300+600+400+1000+800</f>
         <v>8800</v>
       </c>
-      <c r="D46" s="6">
+      <c r="D47" s="6">
         <f t="shared" si="4"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B47" s="4" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B48" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C48" s="5">
         <v>6000</v>
       </c>
-      <c r="D47" s="6">
+      <c r="D48" s="6">
         <f t="shared" si="4"/>
         <v>14890</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B48" s="4" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C48" s="5">
+      <c r="C49" s="5">
         <v>-10000</v>
       </c>
-      <c r="D48" s="6">
+      <c r="D49" s="6">
         <f t="shared" si="4"/>
         <v>4890</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="9" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B50" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C49" s="5">
+      <c r="C50" s="5">
         <v>500</v>
       </c>
-      <c r="D49" s="6">
-        <f t="shared" ref="D49:D54" si="5">D48+C49</f>
+      <c r="D50" s="6">
+        <f t="shared" ref="D50:D55" si="5">D49+C50</f>
         <v>5390</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="9">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="9">
         <v>45323</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B51" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C50" s="5">
+      <c r="C51" s="5">
         <v>700</v>
       </c>
-      <c r="D50" s="6">
+      <c r="D51" s="6">
         <f t="shared" si="5"/>
         <v>6090</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B51" s="4" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C51" s="5">
+      <c r="C52" s="5">
         <v>1500</v>
       </c>
-      <c r="D51" s="6">
+      <c r="D52" s="6">
         <f t="shared" si="5"/>
         <v>7590</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B52" s="4" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B53" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C52" s="5">
+      <c r="C53" s="5">
         <v>5000</v>
       </c>
-      <c r="D52" s="6">
+      <c r="D53" s="6">
         <f t="shared" si="5"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B53" s="4" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B54" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="5">
+      <c r="C54" s="5">
         <v>-10000</v>
       </c>
-      <c r="D53" s="6">
+      <c r="D54" s="6">
         <f t="shared" si="5"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="9" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B55" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C54" s="5">
+      <c r="C55" s="5">
         <v>2000</v>
       </c>
-      <c r="D54" s="6">
+      <c r="D55" s="6">
         <f t="shared" si="5"/>
         <v>4590</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="9">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="9">
         <v>45474</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C55" s="5">
-        <v>700</v>
-      </c>
-      <c r="D55" s="6">
-        <f t="shared" ref="D55:D60" si="6">D54+C55</f>
-        <v>5290</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="9" t="s">
-        <v>82</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>77</v>
@@ -1628,161 +1630,203 @@
         <v>700</v>
       </c>
       <c r="D56" s="6">
+        <f t="shared" ref="D56:D61" si="6">D55+C56</f>
+        <v>5290</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C57" s="5">
+        <v>700</v>
+      </c>
+      <c r="D57" s="6">
         <f t="shared" si="6"/>
         <v>5990</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="9" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B58" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C57" s="5">
+      <c r="C58" s="5">
         <v>700</v>
       </c>
-      <c r="D57" s="6">
+      <c r="D58" s="6">
         <f t="shared" si="6"/>
         <v>6690</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="9" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B59" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C58" s="5">
+      <c r="C59" s="5">
         <v>4000</v>
       </c>
-      <c r="D58" s="6">
+      <c r="D59" s="6">
         <f t="shared" si="6"/>
         <v>10690</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B59" s="4" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B60" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C59" s="5">
+      <c r="C60" s="5">
         <v>-10000</v>
       </c>
-      <c r="D59" s="6">
+      <c r="D60" s="6">
         <f t="shared" si="6"/>
         <v>690</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="9" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B61" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C60" s="5">
+      <c r="C61" s="5">
         <v>1000</v>
       </c>
-      <c r="D60" s="6">
+      <c r="D61" s="6">
         <f t="shared" si="6"/>
         <v>1690</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="9" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B62" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C61" s="5">
+      <c r="C62" s="5">
         <v>7000</v>
       </c>
-      <c r="D61" s="6">
-        <f t="shared" ref="D61:D66" si="7">D60+C61</f>
+      <c r="D62" s="6">
+        <f t="shared" ref="D62:D67" si="7">D61+C62</f>
         <v>8690</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B62" s="4" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B63" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C62" s="5">
+      <c r="C63" s="5">
         <v>10000</v>
       </c>
-      <c r="D62" s="6">
+      <c r="D63" s="6">
         <f t="shared" si="7"/>
         <v>18690</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B63" s="4" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B64" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C63" s="5">
+      <c r="C64" s="5">
         <v>-10000</v>
       </c>
-      <c r="D63" s="6">
+      <c r="D64" s="6">
         <f t="shared" si="7"/>
         <v>8690</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="9">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="9">
         <v>45293</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B65" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C64" s="5">
+      <c r="C65" s="5">
         <v>1700</v>
       </c>
-      <c r="D64" s="6">
+      <c r="D65" s="6">
         <f t="shared" si="7"/>
         <v>10390</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B65" s="4" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C65" s="5">
+      <c r="C66" s="5">
         <v>-10000</v>
       </c>
-      <c r="D65" s="6">
+      <c r="D66" s="6">
         <f t="shared" si="7"/>
         <v>390</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="9">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="9">
         <v>45324</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B67" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C66" s="5">
+      <c r="C67" s="5">
         <v>6000</v>
       </c>
-      <c r="D66" s="6">
+      <c r="D67" s="6">
         <f t="shared" si="7"/>
         <v>6390</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="9" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B68" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C67" s="5">
+      <c r="C68" s="5">
         <v>2000</v>
       </c>
-      <c r="D67" s="6">
-        <f>D66+C67</f>
+      <c r="D68" s="6">
+        <f>D67+C68</f>
         <v>8390</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C69" s="5">
+        <v>5000</v>
+      </c>
+      <c r="D69" s="6">
+        <f>D68+C69</f>
+        <v>13390</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B70" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C70" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D70" s="6">
+        <f>D69+C70</f>
+        <v>3390</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
duy lay tien loi ngay 23/02/2024
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="110">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -342,6 +342,12 @@
   </si>
   <si>
     <t>Duy lấy tiền lời 5tr</t>
+  </si>
+  <si>
+    <t>23/02/2024</t>
+  </si>
+  <si>
+    <t>Duy lấy tiền lời 1tr</t>
   </si>
 </sst>
 </file>
@@ -806,11 +812,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K70"/>
+  <dimension ref="A1:K71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K27" sqref="K27"/>
+      <selection pane="bottomLeft" activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1827,6 +1833,21 @@
       <c r="D70" s="6">
         <f>D69+C70</f>
         <v>3390</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C71" s="5">
+        <v>1000</v>
+      </c>
+      <c r="D71" s="6">
+        <f>D70+C71</f>
+        <v>4390</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
duy lay tien loi ngay 30,31,01
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -326,9 +326,6 @@
     <t>Duy chuyển cho cô Diễm 1.7tr</t>
   </si>
   <si>
-    <t>chưa làm giấy</t>
-  </si>
-  <si>
     <t>Duy lấy tiền lời 6tr</t>
   </si>
   <si>
@@ -348,6 +345,9 @@
   </si>
   <si>
     <t>Duy lấy tiền lời 1tr</t>
+  </si>
+  <si>
+    <t>Duy lấy tiền lời 9tr</t>
   </si>
 </sst>
 </file>
@@ -374,7 +374,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -390,12 +390,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -460,7 +454,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -502,10 +496,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -812,11 +809,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K71"/>
+  <dimension ref="A1:K74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D72" sqref="D72"/>
+      <selection pane="bottomLeft" activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -828,7 +825,7 @@
     <col min="5" max="7" width="9.140625" style="6"/>
     <col min="8" max="8" width="12.7109375" style="9" customWidth="1"/>
     <col min="9" max="9" width="29.5703125" style="5" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" style="4" customWidth="1"/>
     <col min="11" max="11" width="26" style="6" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="6"/>
   </cols>
@@ -846,10 +843,11 @@
       <c r="D1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="16"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="17"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -867,7 +865,7 @@
       <c r="I2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="12" t="s">
         <v>5</v>
       </c>
     </row>
@@ -887,9 +885,9 @@
       <c r="I3" s="5">
         <v>20</v>
       </c>
-      <c r="J3" s="6">
-        <f>SUM(I3:I45)</f>
-        <v>240</v>
+      <c r="J3" s="4">
+        <f>SUM(I3:I46)</f>
+        <v>250</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -964,17 +962,16 @@
       <c r="I8" s="5">
         <v>10</v>
       </c>
+      <c r="K8" s="16"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H9" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I9" s="5">
         <v>10</v>
       </c>
-      <c r="K9" s="15" t="s">
-        <v>102</v>
-      </c>
+      <c r="K9" s="16"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H10" s="9" t="s">
@@ -983,6 +980,7 @@
       <c r="I10" s="5">
         <v>10</v>
       </c>
+      <c r="K10" s="16"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
@@ -1001,6 +999,7 @@
       <c r="I11" s="5">
         <v>10</v>
       </c>
+      <c r="K11" s="16"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
@@ -1022,6 +1021,7 @@
       <c r="I12" s="5">
         <v>10</v>
       </c>
+      <c r="K12" s="16"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
@@ -1043,6 +1043,7 @@
       <c r="I13" s="5">
         <v>10</v>
       </c>
+      <c r="K13" s="16"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H14" s="9" t="s">
@@ -1051,6 +1052,7 @@
       <c r="I14" s="5">
         <v>10</v>
       </c>
+      <c r="K14" s="16"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H15" s="9" t="s">
@@ -1059,6 +1061,7 @@
       <c r="I15" s="5">
         <v>10</v>
       </c>
+      <c r="K15" s="16"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H16" s="9" t="s">
@@ -1067,6 +1070,7 @@
       <c r="I16" s="5">
         <v>10</v>
       </c>
+      <c r="K16" s="16"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
@@ -1088,6 +1092,7 @@
       <c r="I17" s="5">
         <v>10</v>
       </c>
+      <c r="K17" s="16"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H18" s="9" t="s">
@@ -1096,6 +1101,7 @@
       <c r="I18" s="5">
         <v>10</v>
       </c>
+      <c r="K18" s="16"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H19" s="9">
@@ -1104,545 +1110,540 @@
       <c r="I19" s="5">
         <v>10</v>
       </c>
-      <c r="K19" s="15" t="s">
-        <v>102</v>
-      </c>
+      <c r="K19" s="16"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="5">
-        <v>4400</v>
-      </c>
-      <c r="D20" s="6">
-        <f>D17+C20</f>
-        <v>12890</v>
-      </c>
       <c r="H20" s="9">
-        <v>44964</v>
+        <v>45294</v>
       </c>
       <c r="I20" s="5">
-        <v>20</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="K20" s="16"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="5">
+        <v>4400</v>
+      </c>
+      <c r="D21" s="6">
+        <f>D17+C21</f>
+        <v>12890</v>
+      </c>
+      <c r="H21" s="9">
+        <v>44964</v>
+      </c>
+      <c r="I21" s="5">
+        <v>20</v>
+      </c>
+      <c r="K21" s="16"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C22" s="5">
         <v>-10000</v>
       </c>
-      <c r="D21" s="6">
-        <f>D20+C21</f>
+      <c r="D22" s="6">
+        <f>D21+C22</f>
         <v>2890</v>
       </c>
-      <c r="H21" s="9">
+      <c r="H22" s="9">
         <v>44966</v>
-      </c>
-      <c r="I21" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="9">
-        <v>44967</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="5">
-        <v>1600</v>
-      </c>
-      <c r="D22" s="6">
-        <f t="shared" ref="D22:D29" si="1">D21+C22</f>
-        <v>4490</v>
-      </c>
-      <c r="H22" s="9">
-        <v>44968</v>
       </c>
       <c r="I22" s="5">
         <v>10</v>
       </c>
+      <c r="K22" s="16"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="9">
+        <v>44967</v>
+      </c>
       <c r="B23" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="5">
+        <v>1600</v>
+      </c>
+      <c r="D23" s="6">
+        <f t="shared" ref="D23:D30" si="1">D22+C23</f>
+        <v>4490</v>
+      </c>
+      <c r="H23" s="9">
+        <v>44968</v>
+      </c>
+      <c r="I23" s="5">
+        <v>10</v>
+      </c>
+      <c r="K23" s="16"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C24" s="5">
         <v>3000</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D24" s="6">
         <f t="shared" si="1"/>
         <v>7490</v>
       </c>
-      <c r="H23" s="9">
+      <c r="H24" s="9">
         <v>44969</v>
       </c>
-      <c r="I23" s="5">
+      <c r="I24" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B25" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C25" s="5">
         <v>2000</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D25" s="6">
         <f t="shared" si="1"/>
         <v>9490</v>
       </c>
-      <c r="H24" s="9">
+      <c r="H25" s="9">
         <v>45334</v>
       </c>
-      <c r="I24" s="5">
+      <c r="I25" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B26" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C26" s="5">
         <v>3000</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D26" s="6">
         <f t="shared" si="1"/>
         <v>12490</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="4" t="s">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C27" s="5">
         <v>-10000</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D27" s="6">
         <f t="shared" si="1"/>
         <v>2490</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B28" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C28" s="5">
         <v>4960</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D28" s="6">
         <f t="shared" si="1"/>
         <v>7450</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B29" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C29" s="5">
         <v>4000</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D29" s="6">
         <f t="shared" si="1"/>
         <v>11450</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="4" t="s">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C30" s="5">
         <v>-10000</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D30" s="6">
         <f t="shared" si="1"/>
         <v>1450</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B30" s="4" t="s">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C31" s="5">
         <v>7640</v>
       </c>
-      <c r="D30" s="6">
-        <f t="shared" ref="D30:D35" si="2">D29+C30</f>
+      <c r="D31" s="6">
+        <f t="shared" ref="D31:D36" si="2">D30+C31</f>
         <v>9090</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="9">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="9">
         <v>44968</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B32" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C32" s="5">
         <v>3000</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D32" s="6">
         <f t="shared" si="2"/>
         <v>12090</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B32" s="4" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C33" s="5">
         <v>-10000</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D33" s="6">
         <f t="shared" si="2"/>
         <v>2090</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="9">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="9">
         <v>44996</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B34" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C34" s="5">
         <v>800</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D34" s="6">
         <f t="shared" si="2"/>
         <v>2890</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B35" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C35" s="5">
         <v>2000</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D35" s="6">
         <f t="shared" si="2"/>
         <v>4890</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B36" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C35" s="5">
+      <c r="C36" s="5">
         <v>4000</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D36" s="6">
         <f t="shared" si="2"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="9" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B37" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C36" s="5">
+      <c r="C37" s="5">
         <v>4000</v>
       </c>
-      <c r="D36" s="6">
-        <f t="shared" ref="D36:D41" si="3">D35+C36</f>
+      <c r="D37" s="6">
+        <f t="shared" ref="D37:D42" si="3">D36+C37</f>
         <v>12890</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="4" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C37" s="5">
+      <c r="C38" s="5">
         <v>5000</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D38" s="6">
         <f t="shared" si="3"/>
         <v>17890</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B38" s="4" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C38" s="5">
+      <c r="C39" s="5">
         <v>-10000</v>
       </c>
-      <c r="D38" s="6">
+      <c r="D39" s="6">
         <f t="shared" si="3"/>
         <v>7890</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="9">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="9">
         <v>44969</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B40" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C39" s="5">
+      <c r="C40" s="5">
         <v>900</v>
       </c>
-      <c r="D39" s="6">
+      <c r="D40" s="6">
         <f t="shared" si="3"/>
         <v>8790</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="4" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C40" s="5">
+      <c r="C41" s="5">
         <v>4000</v>
       </c>
-      <c r="D40" s="6">
+      <c r="D41" s="6">
         <f t="shared" si="3"/>
         <v>12790</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B41" s="4" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C41" s="5">
+      <c r="C42" s="5">
         <v>-10000</v>
       </c>
-      <c r="D41" s="6">
+      <c r="D42" s="6">
         <f t="shared" si="3"/>
         <v>2790</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C42" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D42" s="6">
-        <f t="shared" ref="D42:D49" si="4">D41+C42</f>
-        <v>4790</v>
-      </c>
-    </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C43" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D43" s="6">
+        <f t="shared" ref="D43:D50" si="4">D42+C43</f>
+        <v>4790</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B44" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C43" s="5">
+      <c r="C44" s="5">
         <v>700</v>
       </c>
-      <c r="D43" s="6">
+      <c r="D44" s="6">
         <f t="shared" si="4"/>
         <v>5490</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B44" s="4" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C45" s="5">
         <v>4000</v>
       </c>
-      <c r="D44" s="6">
+      <c r="D45" s="6">
         <f t="shared" si="4"/>
         <v>9490</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="9" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B46" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C45" s="5">
+      <c r="C46" s="5">
         <v>600</v>
       </c>
-      <c r="D45" s="6">
+      <c r="D46" s="6">
         <f t="shared" si="4"/>
         <v>10090</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B46" s="4" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B47" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C46" s="5">
+      <c r="C47" s="5">
         <v>-10000</v>
       </c>
-      <c r="D46" s="6">
+      <c r="D47" s="6">
         <f t="shared" si="4"/>
         <v>90</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="9" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B48" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C48" s="5">
         <f>700+5000+300+600+400+1000+800</f>
         <v>8800</v>
       </c>
-      <c r="D47" s="6">
+      <c r="D48" s="6">
         <f t="shared" si="4"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B48" s="4" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C48" s="5">
+      <c r="C49" s="5">
         <v>6000</v>
       </c>
-      <c r="D48" s="6">
+      <c r="D49" s="6">
         <f t="shared" si="4"/>
         <v>14890</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B49" s="4" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B50" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C49" s="5">
+      <c r="C50" s="5">
         <v>-10000</v>
       </c>
-      <c r="D49" s="6">
+      <c r="D50" s="6">
         <f t="shared" si="4"/>
         <v>4890</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="9" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B51" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C50" s="5">
+      <c r="C51" s="5">
         <v>500</v>
       </c>
-      <c r="D50" s="6">
-        <f t="shared" ref="D50:D55" si="5">D49+C50</f>
+      <c r="D51" s="6">
+        <f t="shared" ref="D51:D56" si="5">D50+C51</f>
         <v>5390</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="9">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="9">
         <v>45323</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B52" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C51" s="5">
+      <c r="C52" s="5">
         <v>700</v>
       </c>
-      <c r="D51" s="6">
+      <c r="D52" s="6">
         <f t="shared" si="5"/>
         <v>6090</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B52" s="4" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B53" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C52" s="5">
+      <c r="C53" s="5">
         <v>1500</v>
       </c>
-      <c r="D52" s="6">
+      <c r="D53" s="6">
         <f t="shared" si="5"/>
         <v>7590</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B53" s="4" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B54" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C53" s="5">
+      <c r="C54" s="5">
         <v>5000</v>
       </c>
-      <c r="D53" s="6">
+      <c r="D54" s="6">
         <f t="shared" si="5"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B54" s="4" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B55" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C54" s="5">
+      <c r="C55" s="5">
         <v>-10000</v>
       </c>
-      <c r="D54" s="6">
+      <c r="D55" s="6">
         <f t="shared" si="5"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="9" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B56" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C55" s="5">
+      <c r="C56" s="5">
         <v>2000</v>
       </c>
-      <c r="D55" s="6">
+      <c r="D56" s="6">
         <f t="shared" si="5"/>
         <v>4590</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="9">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="9">
         <v>45474</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C56" s="5">
-        <v>700</v>
-      </c>
-      <c r="D56" s="6">
-        <f t="shared" ref="D56:D61" si="6">D55+C56</f>
-        <v>5290</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="9" t="s">
-        <v>82</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>77</v>
@@ -1651,203 +1652,245 @@
         <v>700</v>
       </c>
       <c r="D57" s="6">
+        <f t="shared" ref="D57:D62" si="6">D56+C57</f>
+        <v>5290</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C58" s="5">
+        <v>700</v>
+      </c>
+      <c r="D58" s="6">
         <f t="shared" si="6"/>
         <v>5990</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="9" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B59" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C58" s="5">
+      <c r="C59" s="5">
         <v>700</v>
       </c>
-      <c r="D58" s="6">
+      <c r="D59" s="6">
         <f t="shared" si="6"/>
         <v>6690</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="9" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B60" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C59" s="5">
+      <c r="C60" s="5">
         <v>4000</v>
       </c>
-      <c r="D59" s="6">
+      <c r="D60" s="6">
         <f t="shared" si="6"/>
         <v>10690</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B60" s="4" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B61" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C60" s="5">
+      <c r="C61" s="5">
         <v>-10000</v>
       </c>
-      <c r="D60" s="6">
+      <c r="D61" s="6">
         <f t="shared" si="6"/>
         <v>690</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="9" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B62" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C61" s="5">
+      <c r="C62" s="5">
         <v>1000</v>
       </c>
-      <c r="D61" s="6">
+      <c r="D62" s="6">
         <f t="shared" si="6"/>
         <v>1690</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="9" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B63" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C62" s="5">
+      <c r="C63" s="5">
         <v>7000</v>
       </c>
-      <c r="D62" s="6">
-        <f t="shared" ref="D62:D67" si="7">D61+C62</f>
+      <c r="D63" s="6">
+        <f t="shared" ref="D63:D68" si="7">D62+C63</f>
         <v>8690</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B63" s="4" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B64" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C63" s="5">
+      <c r="C64" s="5">
         <v>10000</v>
       </c>
-      <c r="D63" s="6">
+      <c r="D64" s="6">
         <f t="shared" si="7"/>
         <v>18690</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B64" s="4" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B65" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C64" s="5">
+      <c r="C65" s="5">
         <v>-10000</v>
       </c>
-      <c r="D64" s="6">
+      <c r="D65" s="6">
         <f t="shared" si="7"/>
         <v>8690</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="9">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="9">
         <v>45293</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B66" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C65" s="5">
+      <c r="C66" s="5">
         <v>1700</v>
       </c>
-      <c r="D65" s="6">
+      <c r="D66" s="6">
         <f t="shared" si="7"/>
         <v>10390</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B66" s="4" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B67" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C66" s="5">
+      <c r="C67" s="5">
         <v>-10000</v>
       </c>
-      <c r="D66" s="6">
+      <c r="D67" s="6">
         <f t="shared" si="7"/>
         <v>390</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="9">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="9">
         <v>45324</v>
       </c>
-      <c r="B67" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C67" s="5">
+      <c r="B68" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C68" s="5">
         <v>6000</v>
       </c>
-      <c r="D67" s="6">
+      <c r="D68" s="6">
         <f t="shared" si="7"/>
         <v>6390</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C68" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D68" s="6">
-        <f>D67+C68</f>
-        <v>8390</v>
-      </c>
-    </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C69" s="5">
-        <v>5000</v>
+        <v>2000</v>
       </c>
       <c r="D69" s="6">
         <f>D68+C69</f>
-        <v>13390</v>
+        <v>8390</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="9" t="s">
+        <v>105</v>
+      </c>
       <c r="B70" s="4" t="s">
-        <v>20</v>
+        <v>106</v>
       </c>
       <c r="C70" s="5">
-        <v>-10000</v>
+        <v>5000</v>
       </c>
       <c r="D70" s="6">
         <f>D69+C70</f>
-        <v>3390</v>
+        <v>13390</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="9" t="s">
-        <v>108</v>
-      </c>
       <c r="B71" s="4" t="s">
-        <v>109</v>
+        <v>20</v>
       </c>
       <c r="C71" s="5">
-        <v>1000</v>
+        <v>-10000</v>
       </c>
       <c r="D71" s="6">
         <f>D70+C71</f>
+        <v>3390</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C72" s="5">
+        <v>1000</v>
+      </c>
+      <c r="D72" s="6">
+        <f>D71+C72</f>
         <v>4390</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="9">
+        <v>45294</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C73" s="5">
+        <v>9000</v>
+      </c>
+      <c r="D73" s="6">
+        <f>D72+C73</f>
+        <v>13390</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C74" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D74" s="6">
+        <f>D73+C74</f>
+        <v>3390</v>
       </c>
     </row>
   </sheetData>
@@ -1898,10 +1941,10 @@
       <c r="E1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="16"/>
+      <c r="I1" s="15"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
@@ -2037,10 +2080,10 @@
       <c r="E1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="16"/>
+      <c r="I1" s="15"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -2173,10 +2216,10 @@
       <c r="E1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="16"/>
+      <c r="I1" s="15"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">

</xml_diff>

<commit_message>
duy gui cho co diem vay 2tr
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="111">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -348,6 +348,9 @@
   </si>
   <si>
     <t>Duy lấy tiền lời 9tr</t>
+  </si>
+  <si>
+    <t>Duy chuyển cho co Diễm 2tr</t>
   </si>
 </sst>
 </file>
@@ -496,13 +499,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -809,11 +812,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K74"/>
+  <dimension ref="A1:K75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K13" sqref="K13"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -843,11 +846,11 @@
       <c r="D1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="15"/>
-      <c r="J1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="16"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -962,7 +965,7 @@
       <c r="I8" s="5">
         <v>10</v>
       </c>
-      <c r="K8" s="16"/>
+      <c r="K8" s="15"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H9" s="9" t="s">
@@ -971,7 +974,7 @@
       <c r="I9" s="5">
         <v>10</v>
       </c>
-      <c r="K9" s="16"/>
+      <c r="K9" s="15"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H10" s="9" t="s">
@@ -980,7 +983,7 @@
       <c r="I10" s="5">
         <v>10</v>
       </c>
-      <c r="K10" s="16"/>
+      <c r="K10" s="15"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
@@ -999,7 +1002,7 @@
       <c r="I11" s="5">
         <v>10</v>
       </c>
-      <c r="K11" s="16"/>
+      <c r="K11" s="15"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
@@ -1021,7 +1024,7 @@
       <c r="I12" s="5">
         <v>10</v>
       </c>
-      <c r="K12" s="16"/>
+      <c r="K12" s="15"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
@@ -1043,7 +1046,7 @@
       <c r="I13" s="5">
         <v>10</v>
       </c>
-      <c r="K13" s="16"/>
+      <c r="K13" s="15"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H14" s="9" t="s">
@@ -1052,7 +1055,7 @@
       <c r="I14" s="5">
         <v>10</v>
       </c>
-      <c r="K14" s="16"/>
+      <c r="K14" s="15"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H15" s="9" t="s">
@@ -1061,7 +1064,7 @@
       <c r="I15" s="5">
         <v>10</v>
       </c>
-      <c r="K15" s="16"/>
+      <c r="K15" s="15"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H16" s="9" t="s">
@@ -1070,7 +1073,7 @@
       <c r="I16" s="5">
         <v>10</v>
       </c>
-      <c r="K16" s="16"/>
+      <c r="K16" s="15"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
@@ -1092,7 +1095,7 @@
       <c r="I17" s="5">
         <v>10</v>
       </c>
-      <c r="K17" s="16"/>
+      <c r="K17" s="15"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H18" s="9" t="s">
@@ -1101,7 +1104,7 @@
       <c r="I18" s="5">
         <v>10</v>
       </c>
-      <c r="K18" s="16"/>
+      <c r="K18" s="15"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H19" s="9">
@@ -1110,7 +1113,7 @@
       <c r="I19" s="5">
         <v>10</v>
       </c>
-      <c r="K19" s="16"/>
+      <c r="K19" s="15"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H20" s="9">
@@ -1119,7 +1122,7 @@
       <c r="I20" s="5">
         <v>10</v>
       </c>
-      <c r="K20" s="16"/>
+      <c r="K20" s="15"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
@@ -1138,7 +1141,7 @@
       <c r="I21" s="5">
         <v>20</v>
       </c>
-      <c r="K21" s="16"/>
+      <c r="K21" s="15"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
@@ -1157,7 +1160,7 @@
       <c r="I22" s="5">
         <v>10</v>
       </c>
-      <c r="K22" s="16"/>
+      <c r="K22" s="15"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
@@ -1179,7 +1182,7 @@
       <c r="I23" s="5">
         <v>10</v>
       </c>
-      <c r="K23" s="16"/>
+      <c r="K23" s="15"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
@@ -1820,7 +1823,7 @@
         <v>2000</v>
       </c>
       <c r="D69" s="6">
-        <f>D68+C69</f>
+        <f t="shared" ref="D69:D74" si="8">D68+C69</f>
         <v>8390</v>
       </c>
     </row>
@@ -1835,7 +1838,7 @@
         <v>5000</v>
       </c>
       <c r="D70" s="6">
-        <f>D69+C70</f>
+        <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
@@ -1847,7 +1850,7 @@
         <v>-10000</v>
       </c>
       <c r="D71" s="6">
-        <f>D70+C71</f>
+        <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
@@ -1862,7 +1865,7 @@
         <v>1000</v>
       </c>
       <c r="D72" s="6">
-        <f>D71+C72</f>
+        <f t="shared" si="8"/>
         <v>4390</v>
       </c>
     </row>
@@ -1877,7 +1880,7 @@
         <v>9000</v>
       </c>
       <c r="D73" s="6">
-        <f>D72+C73</f>
+        <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
@@ -1889,8 +1892,20 @@
         <v>-10000</v>
       </c>
       <c r="D74" s="6">
-        <f>D73+C74</f>
+        <f t="shared" si="8"/>
         <v>3390</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B75" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C75" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D75" s="6">
+        <f>D74+C75</f>
+        <v>5390</v>
       </c>
     </row>
   </sheetData>
@@ -1941,10 +1956,10 @@
       <c r="E1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="15"/>
+      <c r="I1" s="17"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
@@ -2043,11 +2058,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2080,10 +2095,10 @@
       <c r="E1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="15"/>
+      <c r="I1" s="17"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -2166,6 +2181,21 @@
       <c r="D6" s="4">
         <f>D5+C6</f>
         <v>7500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>45294</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="5">
+        <v>-500</v>
+      </c>
+      <c r="D7" s="4">
+        <f>D6+C7</f>
+        <v>7000</v>
       </c>
     </row>
   </sheetData>
@@ -2216,10 +2246,10 @@
       <c r="E1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="15"/>
+      <c r="I1" s="17"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">

</xml_diff>

<commit_message>
duy lay tien loi ngay 02
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="113">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -351,6 +351,12 @@
   </si>
   <si>
     <t>Duy chuyển cho co Diễm 2tr</t>
+  </si>
+  <si>
+    <t>Duy lấy tiền lời 6tr</t>
+  </si>
+  <si>
+    <t>chưa làm giấy</t>
   </si>
 </sst>
 </file>
@@ -377,7 +383,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -393,6 +399,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -457,7 +469,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -506,6 +518,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -812,11 +827,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K75"/>
+  <dimension ref="A1:K77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D76" sqref="D76"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -890,7 +905,7 @@
       </c>
       <c r="J3" s="4">
         <f>SUM(I3:I46)</f>
-        <v>250</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1237,6 +1252,15 @@
         <f t="shared" si="1"/>
         <v>12490</v>
       </c>
+      <c r="H26" s="9">
+        <v>45325</v>
+      </c>
+      <c r="I26" s="5">
+        <v>10</v>
+      </c>
+      <c r="K26" s="18" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
@@ -1906,6 +1930,33 @@
       <c r="D75" s="6">
         <f>D74+C75</f>
         <v>5390</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="9">
+        <v>44960</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C76" s="5">
+        <v>6000</v>
+      </c>
+      <c r="D76" s="6">
+        <f>D75+C76</f>
+        <v>11390</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B77" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C77" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D77" s="6">
+        <f>D76+C77</f>
+        <v>1390</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Duy lay tien loi ngay 21
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="CÔ DIỄM" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="106">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -284,39 +284,12 @@
     <t>Duy lấy tiền lời 1tr</t>
   </si>
   <si>
-    <t xml:space="preserve">nguyen tien dinh </t>
-  </si>
-  <si>
-    <t>lam van khoi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tổng = </t>
-  </si>
-  <si>
-    <t>dang minh nhat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hoang thi ngoc linh </t>
-  </si>
-  <si>
-    <t>ha thi dao</t>
-  </si>
-  <si>
-    <t>vo thi dang nga</t>
-  </si>
-  <si>
-    <t>phan chi cuong</t>
-  </si>
-  <si>
     <t>30/01/2024</t>
   </si>
   <si>
     <t>Duy lấy tiền lời ngày 30-31 - 7tr</t>
   </si>
   <si>
-    <t>Còn</t>
-  </si>
-  <si>
     <t>Duy chuyển cho cô Diễm 10tr</t>
   </si>
   <si>
@@ -360,6 +333,9 @@
   </si>
   <si>
     <t>13/03/24</t>
+  </si>
+  <si>
+    <t>21/03/24</t>
   </si>
 </sst>
 </file>
@@ -821,11 +797,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K79"/>
+  <dimension ref="A1:K80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K47" sqref="K47"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -978,7 +954,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H9" s="9" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I9" s="5">
         <v>10</v>
@@ -1077,7 +1053,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H16" s="9" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="I16" s="5">
         <v>10</v>
@@ -1749,10 +1725,10 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C63" s="5">
         <v>7000</v>
@@ -1764,7 +1740,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B64" s="4" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="C64" s="5">
         <v>10000</v>
@@ -1791,7 +1767,7 @@
         <v>45293</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C66" s="5">
         <v>1700</v>
@@ -1818,7 +1794,7 @@
         <v>45324</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C68" s="5">
         <v>6000</v>
@@ -1830,10 +1806,10 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="C69" s="5">
         <v>2000</v>
@@ -1845,10 +1821,10 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C70" s="5">
         <v>5000</v>
@@ -1872,10 +1848,10 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C72" s="5">
         <v>1000</v>
@@ -1890,7 +1866,7 @@
         <v>45294</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C73" s="5">
         <v>9000</v>
@@ -1914,7 +1890,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B75" s="4" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C75" s="5">
         <v>2000</v>
@@ -1929,7 +1905,7 @@
         <v>45325</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="C76" s="5">
         <v>6000</v>
@@ -1956,7 +1932,7 @@
         <v>45507</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C78" s="5">
         <v>400</v>
@@ -1968,7 +1944,7 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="B79" s="4" t="s">
         <v>65</v>
@@ -1979,6 +1955,21 @@
       <c r="D79" s="6">
         <f>D78+C79</f>
         <v>3790</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C80" s="5">
+        <v>6000</v>
+      </c>
+      <c r="D80" s="6">
+        <f>D79+C80</f>
+        <v>9790</v>
       </c>
     </row>
   </sheetData>
@@ -2373,10 +2364,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="D1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2385,75 +2376,9 @@
     <col min="5" max="5" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B1">
-        <v>310</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="E1" s="14">
-        <f>SUM(B:B)</f>
-        <v>5660</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B2">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B3">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B4">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B5">
-        <v>600</v>
-      </c>
-      <c r="E5" t="s">
-        <v>98</v>
-      </c>
-      <c r="F5">
-        <f>10000-E1</f>
-        <v>4340</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B6">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>95</v>
-      </c>
-      <c r="B7">
-        <v>500</v>
-      </c>
+    <row r="1" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
duy lay tien loi ngay 23
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="CÔ DIỄM" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="109">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -336,6 +336,15 @@
   </si>
   <si>
     <t>21/03/24</t>
+  </si>
+  <si>
+    <t>23/03/24</t>
+  </si>
+  <si>
+    <t>23/03/2024</t>
+  </si>
+  <si>
+    <t>chưa làm giấy</t>
   </si>
 </sst>
 </file>
@@ -362,7 +371,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -378,6 +387,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -442,7 +457,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -491,6 +506,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -797,11 +815,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K80"/>
+  <dimension ref="A1:K83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D81" sqref="D81"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,8 +892,8 @@
         <v>20</v>
       </c>
       <c r="J3" s="4">
-        <f>SUM(I3:I46)</f>
-        <v>260</v>
+        <f>SUM(I3:I47)</f>
+        <v>270</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -904,7 +922,7 @@
         <v>-10000</v>
       </c>
       <c r="D5" s="6">
-        <f t="shared" ref="D5:D13" si="0">D4+C5</f>
+        <f t="shared" ref="D5:D14" si="0">D4+C5</f>
         <v>8490</v>
       </c>
       <c r="H5" s="9" t="s">
@@ -971,71 +989,73 @@
       <c r="K10" s="15"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="5">
-        <v>-10000</v>
-      </c>
-      <c r="D11" s="6">
-        <f>D6+C11</f>
-        <v>490</v>
-      </c>
       <c r="H11" s="9" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="I11" s="5">
         <v>10</v>
       </c>
-      <c r="K11" s="15"/>
+      <c r="K11" s="18" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="B12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D12" s="6">
+        <f>D6+C12</f>
+        <v>490</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="5">
+        <v>10</v>
+      </c>
+      <c r="K12" s="15"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B13" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C13" s="5">
         <v>2000</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D13" s="6">
         <f t="shared" si="0"/>
         <v>2490</v>
       </c>
-      <c r="H12" s="9" t="s">
+      <c r="H13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="I12" s="5">
+      <c r="I13" s="5">
         <v>10</v>
       </c>
-      <c r="K12" s="15"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="K13" s="15"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C14" s="5">
         <v>3000</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D14" s="6">
         <f t="shared" si="0"/>
         <v>5490</v>
       </c>
-      <c r="H13" s="9" t="s">
+      <c r="H14" s="9" t="s">
         <v>24</v>
-      </c>
-      <c r="I13" s="5">
-        <v>10</v>
-      </c>
-      <c r="K13" s="15"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H14" s="9" t="s">
-        <v>59</v>
       </c>
       <c r="I14" s="5">
         <v>10</v>
@@ -1044,7 +1064,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H15" s="9" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="I15" s="5">
         <v>10</v>
@@ -1053,7 +1073,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H16" s="9" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="I16" s="5">
         <v>10</v>
@@ -1061,21 +1081,8 @@
       <c r="K16" s="15"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="5">
-        <v>3000</v>
-      </c>
-      <c r="D17" s="6">
-        <f>D13+C17</f>
-        <v>8490</v>
-      </c>
       <c r="H17" s="9" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="I17" s="5">
         <v>10</v>
@@ -1083,8 +1090,21 @@
       <c r="K17" s="15"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="5">
+        <v>3000</v>
+      </c>
+      <c r="D18" s="6">
+        <f>D14+C18</f>
+        <v>8490</v>
+      </c>
       <c r="H18" s="9" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="I18" s="5">
         <v>10</v>
@@ -1092,8 +1112,8 @@
       <c r="K18" s="15"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H19" s="9">
-        <v>45293</v>
+      <c r="H19" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="I19" s="5">
         <v>10</v>
@@ -1102,7 +1122,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H20" s="9">
-        <v>45294</v>
+        <v>45293</v>
       </c>
       <c r="I20" s="5">
         <v>10</v>
@@ -1110,59 +1130,46 @@
       <c r="K20" s="15"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="5">
-        <v>4400</v>
-      </c>
-      <c r="D21" s="6">
-        <f>D17+C21</f>
-        <v>12890</v>
-      </c>
       <c r="H21" s="9">
-        <v>44964</v>
+        <v>45294</v>
       </c>
       <c r="I21" s="5">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K21" s="15"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="5">
+        <v>4400</v>
+      </c>
+      <c r="D22" s="6">
+        <f>D18+C22</f>
+        <v>12890</v>
+      </c>
+      <c r="H22" s="9">
+        <v>44964</v>
+      </c>
+      <c r="I22" s="5">
+        <v>20</v>
+      </c>
+      <c r="K22" s="15"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C23" s="5">
         <v>-10000</v>
       </c>
-      <c r="D22" s="6">
-        <f>D21+C22</f>
+      <c r="D23" s="6">
+        <f>D22+C23</f>
         <v>2890</v>
       </c>
-      <c r="H22" s="9">
+      <c r="H23" s="9">
         <v>44966</v>
-      </c>
-      <c r="I22" s="5">
-        <v>10</v>
-      </c>
-      <c r="K22" s="15"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="9">
-        <v>44967</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" s="5">
-        <v>1600</v>
-      </c>
-      <c r="D23" s="6">
-        <f t="shared" ref="D23:D30" si="1">D22+C23</f>
-        <v>4490</v>
-      </c>
-      <c r="H23" s="9">
-        <v>44968</v>
       </c>
       <c r="I23" s="5">
         <v>10</v>
@@ -1170,490 +1177,497 @@
       <c r="K23" s="15"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="9">
+        <v>44967</v>
+      </c>
       <c r="B24" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="5">
+        <v>1600</v>
+      </c>
+      <c r="D24" s="6">
+        <f t="shared" ref="D24:D31" si="1">D23+C24</f>
+        <v>4490</v>
+      </c>
+      <c r="H24" s="9">
+        <v>44968</v>
+      </c>
+      <c r="I24" s="5">
+        <v>10</v>
+      </c>
+      <c r="K24" s="15"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C25" s="5">
         <v>3000</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D25" s="6">
         <f t="shared" si="1"/>
         <v>7490</v>
       </c>
-      <c r="H24" s="9">
+      <c r="H25" s="9">
         <v>44969</v>
       </c>
-      <c r="I24" s="5">
+      <c r="I25" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B26" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C26" s="5">
         <v>2000</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D26" s="6">
         <f t="shared" si="1"/>
         <v>9490</v>
       </c>
-      <c r="H25" s="9">
+      <c r="H26" s="9">
         <v>45334</v>
       </c>
-      <c r="I25" s="5">
+      <c r="I26" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B27" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C27" s="5">
         <v>3000</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D27" s="6">
         <f t="shared" si="1"/>
         <v>12490</v>
       </c>
-      <c r="H26" s="9">
+      <c r="H27" s="9">
         <v>45325</v>
       </c>
-      <c r="I26" s="5">
+      <c r="I27" s="5">
         <v>10</v>
       </c>
-      <c r="K26" s="15"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="4" t="s">
+      <c r="K27" s="15"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C28" s="5">
         <v>-10000</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D28" s="6">
         <f t="shared" si="1"/>
         <v>2490</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B29" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C29" s="5">
         <v>4960</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D29" s="6">
         <f t="shared" si="1"/>
         <v>7450</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B30" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C30" s="5">
         <v>4000</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D30" s="6">
         <f t="shared" si="1"/>
         <v>11450</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B30" s="4" t="s">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C31" s="5">
         <v>-10000</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D31" s="6">
         <f t="shared" si="1"/>
         <v>1450</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B31" s="4" t="s">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C32" s="5">
         <v>7640</v>
       </c>
-      <c r="D31" s="6">
-        <f t="shared" ref="D31:D36" si="2">D30+C31</f>
+      <c r="D32" s="6">
+        <f t="shared" ref="D32:D37" si="2">D31+C32</f>
         <v>9090</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="9">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="9">
         <v>44968</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B33" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C33" s="5">
         <v>3000</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D33" s="6">
         <f t="shared" si="2"/>
         <v>12090</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="4" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C34" s="5">
         <v>-10000</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D34" s="6">
         <f t="shared" si="2"/>
         <v>2090</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="9">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="9">
         <v>44996</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B35" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C35" s="5">
         <v>800</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D35" s="6">
         <f t="shared" si="2"/>
         <v>2890</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B36" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C35" s="5">
+      <c r="C36" s="5">
         <v>2000</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D36" s="6">
         <f t="shared" si="2"/>
         <v>4890</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="9" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B37" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C36" s="5">
+      <c r="C37" s="5">
         <v>4000</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D37" s="6">
         <f t="shared" si="2"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="9" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B38" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C37" s="5">
+      <c r="C38" s="5">
         <v>4000</v>
       </c>
-      <c r="D37" s="6">
-        <f t="shared" ref="D37:D42" si="3">D36+C37</f>
+      <c r="D38" s="6">
+        <f t="shared" ref="D38:D43" si="3">D37+C38</f>
         <v>12890</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B38" s="4" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C38" s="5">
+      <c r="C39" s="5">
         <v>5000</v>
       </c>
-      <c r="D38" s="6">
+      <c r="D39" s="6">
         <f t="shared" si="3"/>
         <v>17890</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B39" s="4" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C39" s="5">
+      <c r="C40" s="5">
         <v>-10000</v>
       </c>
-      <c r="D39" s="6">
+      <c r="D40" s="6">
         <f t="shared" si="3"/>
         <v>7890</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="9">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="9">
         <v>44969</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B41" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C40" s="5">
+      <c r="C41" s="5">
         <v>900</v>
       </c>
-      <c r="D40" s="6">
+      <c r="D41" s="6">
         <f t="shared" si="3"/>
         <v>8790</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B41" s="4" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C41" s="5">
+      <c r="C42" s="5">
         <v>4000</v>
       </c>
-      <c r="D41" s="6">
+      <c r="D42" s="6">
         <f t="shared" si="3"/>
         <v>12790</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B42" s="4" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C43" s="5">
         <v>-10000</v>
       </c>
-      <c r="D42" s="6">
+      <c r="D43" s="6">
         <f t="shared" si="3"/>
         <v>2790</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C43" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D43" s="6">
-        <f t="shared" ref="D43:D50" si="4">D42+C43</f>
-        <v>4790</v>
-      </c>
-    </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C44" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D44" s="6">
+        <f t="shared" ref="D44:D51" si="4">D43+C44</f>
+        <v>4790</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B45" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C45" s="5">
         <v>700</v>
       </c>
-      <c r="D44" s="6">
+      <c r="D45" s="6">
         <f t="shared" si="4"/>
         <v>5490</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B45" s="4" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C45" s="5">
+      <c r="C46" s="5">
         <v>4000</v>
       </c>
-      <c r="D45" s="6">
+      <c r="D46" s="6">
         <f t="shared" si="4"/>
         <v>9490</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="9" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B47" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C46" s="5">
+      <c r="C47" s="5">
         <v>600</v>
       </c>
-      <c r="D46" s="6">
+      <c r="D47" s="6">
         <f t="shared" si="4"/>
         <v>10090</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B47" s="4" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B48" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C48" s="5">
         <v>-10000</v>
       </c>
-      <c r="D47" s="6">
+      <c r="D48" s="6">
         <f t="shared" si="4"/>
         <v>90</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="9" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B49" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C48" s="5">
+      <c r="C49" s="5">
         <f>700+5000+300+600+400+1000+800</f>
         <v>8800</v>
       </c>
-      <c r="D48" s="6">
+      <c r="D49" s="6">
         <f t="shared" si="4"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B49" s="4" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B50" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C49" s="5">
+      <c r="C50" s="5">
         <v>6000</v>
       </c>
-      <c r="D49" s="6">
+      <c r="D50" s="6">
         <f t="shared" si="4"/>
         <v>14890</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B50" s="4" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B51" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C50" s="5">
+      <c r="C51" s="5">
         <v>-10000</v>
       </c>
-      <c r="D50" s="6">
+      <c r="D51" s="6">
         <f t="shared" si="4"/>
         <v>4890</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="9" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B52" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C51" s="5">
+      <c r="C52" s="5">
         <v>500</v>
       </c>
-      <c r="D51" s="6">
-        <f t="shared" ref="D51:D56" si="5">D50+C51</f>
+      <c r="D52" s="6">
+        <f t="shared" ref="D52:D57" si="5">D51+C52</f>
         <v>5390</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="9">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="9">
         <v>45323</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B53" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C52" s="5">
+      <c r="C53" s="5">
         <v>700</v>
       </c>
-      <c r="D52" s="6">
+      <c r="D53" s="6">
         <f t="shared" si="5"/>
         <v>6090</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B53" s="4" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B54" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C53" s="5">
+      <c r="C54" s="5">
         <v>1500</v>
       </c>
-      <c r="D53" s="6">
+      <c r="D54" s="6">
         <f t="shared" si="5"/>
         <v>7590</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B54" s="4" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B55" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C54" s="5">
+      <c r="C55" s="5">
         <v>5000</v>
       </c>
-      <c r="D54" s="6">
+      <c r="D55" s="6">
         <f t="shared" si="5"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="4" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B56" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C55" s="5">
+      <c r="C56" s="5">
         <v>-10000</v>
       </c>
-      <c r="D55" s="6">
+      <c r="D56" s="6">
         <f t="shared" si="5"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="9" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B57" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C56" s="5">
+      <c r="C57" s="5">
         <v>2000</v>
       </c>
-      <c r="D56" s="6">
+      <c r="D57" s="6">
         <f t="shared" si="5"/>
         <v>4590</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="9">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="9">
         <v>45474</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C57" s="5">
-        <v>700</v>
-      </c>
-      <c r="D57" s="6">
-        <f t="shared" ref="D57:D62" si="6">D56+C57</f>
-        <v>5290</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="9" t="s">
-        <v>82</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>77</v>
@@ -1662,314 +1676,352 @@
         <v>700</v>
       </c>
       <c r="D58" s="6">
+        <f t="shared" ref="D58:D63" si="6">D57+C58</f>
+        <v>5290</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C59" s="5">
+        <v>700</v>
+      </c>
+      <c r="D59" s="6">
         <f t="shared" si="6"/>
         <v>5990</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="9" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B60" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C59" s="5">
+      <c r="C60" s="5">
         <v>700</v>
       </c>
-      <c r="D59" s="6">
+      <c r="D60" s="6">
         <f t="shared" si="6"/>
         <v>6690</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="9" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B61" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C60" s="5">
+      <c r="C61" s="5">
         <v>4000</v>
       </c>
-      <c r="D60" s="6">
+      <c r="D61" s="6">
         <f t="shared" si="6"/>
         <v>10690</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B61" s="4" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B62" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C61" s="5">
+      <c r="C62" s="5">
         <v>-10000</v>
       </c>
-      <c r="D61" s="6">
+      <c r="D62" s="6">
         <f t="shared" si="6"/>
         <v>690</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="9" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B63" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C62" s="5">
+      <c r="C63" s="5">
         <v>1000</v>
       </c>
-      <c r="D62" s="6">
+      <c r="D63" s="6">
         <f t="shared" si="6"/>
         <v>1690</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="9" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B64" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C63" s="5">
+      <c r="C64" s="5">
         <v>7000</v>
       </c>
-      <c r="D63" s="6">
-        <f t="shared" ref="D63:D68" si="7">D62+C63</f>
+      <c r="D64" s="6">
+        <f t="shared" ref="D64:D69" si="7">D63+C64</f>
         <v>8690</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B64" s="4" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B65" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C64" s="5">
+      <c r="C65" s="5">
         <v>10000</v>
       </c>
-      <c r="D64" s="6">
+      <c r="D65" s="6">
         <f t="shared" si="7"/>
         <v>18690</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B65" s="4" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C65" s="5">
+      <c r="C66" s="5">
         <v>-10000</v>
       </c>
-      <c r="D65" s="6">
+      <c r="D66" s="6">
         <f t="shared" si="7"/>
         <v>8690</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="9">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="9">
         <v>45293</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B67" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C66" s="5">
+      <c r="C67" s="5">
         <v>1700</v>
       </c>
-      <c r="D66" s="6">
+      <c r="D67" s="6">
         <f t="shared" si="7"/>
         <v>10390</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B67" s="4" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B68" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C67" s="5">
+      <c r="C68" s="5">
         <v>-10000</v>
       </c>
-      <c r="D67" s="6">
+      <c r="D68" s="6">
         <f t="shared" si="7"/>
         <v>390</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="9">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="9">
         <v>45324</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B69" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C68" s="5">
+      <c r="C69" s="5">
         <v>6000</v>
       </c>
-      <c r="D68" s="6">
+      <c r="D69" s="6">
         <f t="shared" si="7"/>
         <v>6390</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C69" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D69" s="6">
-        <f t="shared" ref="D69:D74" si="8">D68+C69</f>
-        <v>8390</v>
-      </c>
-    </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C70" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D70" s="6">
+        <f t="shared" ref="D70:D75" si="8">D69+C70</f>
+        <v>8390</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B71" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C70" s="5">
+      <c r="C71" s="5">
         <v>5000</v>
       </c>
-      <c r="D70" s="6">
+      <c r="D71" s="6">
         <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B71" s="4" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B72" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C71" s="5">
+      <c r="C72" s="5">
         <v>-10000</v>
       </c>
-      <c r="D71" s="6">
+      <c r="D72" s="6">
         <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="9" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B73" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C72" s="5">
+      <c r="C73" s="5">
         <v>1000</v>
       </c>
-      <c r="D72" s="6">
+      <c r="D73" s="6">
         <f t="shared" si="8"/>
         <v>4390</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="9">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="9">
         <v>45294</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B74" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C73" s="5">
+      <c r="C74" s="5">
         <v>9000</v>
       </c>
-      <c r="D73" s="6">
+      <c r="D74" s="6">
         <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B74" s="4" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B75" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C74" s="5">
+      <c r="C75" s="5">
         <v>-10000</v>
       </c>
-      <c r="D74" s="6">
+      <c r="D75" s="6">
         <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B75" s="4" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B76" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C75" s="5">
+      <c r="C76" s="5">
         <v>2000</v>
       </c>
-      <c r="D75" s="6">
-        <f>D74+C75</f>
+      <c r="D76" s="6">
+        <f t="shared" ref="D76:D81" si="9">D75+C76</f>
         <v>5390</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="9">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="9">
         <v>45325</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B77" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C76" s="5">
+      <c r="C77" s="5">
         <v>6000</v>
       </c>
-      <c r="D76" s="6">
-        <f>D75+C76</f>
+      <c r="D77" s="6">
+        <f t="shared" si="9"/>
         <v>11390</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B77" s="4" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B78" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C77" s="5">
+      <c r="C78" s="5">
         <v>-10000</v>
       </c>
-      <c r="D77" s="6">
-        <f>D76+C77</f>
+      <c r="D78" s="6">
+        <f t="shared" si="9"/>
         <v>1390</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="9">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="9">
         <v>45507</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B79" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C78" s="5">
+      <c r="C79" s="5">
         <v>400</v>
       </c>
-      <c r="D78" s="6">
-        <f>D77+C78</f>
+      <c r="D79" s="6">
+        <f t="shared" si="9"/>
         <v>1790</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="B79" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C79" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D79" s="6">
-        <f>D78+C79</f>
-        <v>3790</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C80" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D80" s="6">
+        <f t="shared" si="9"/>
+        <v>3790</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B81" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C80" s="5">
+      <c r="C81" s="5">
         <v>6000</v>
       </c>
-      <c r="D80" s="6">
-        <f>D79+C80</f>
+      <c r="D81" s="6">
+        <f t="shared" si="9"/>
         <v>9790</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C82" s="5">
+        <v>1000</v>
+      </c>
+      <c r="D82" s="6">
+        <f>D81+C82</f>
+        <v>10790</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B83" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C83" s="5">
+        <v>-10000</v>
       </c>
     </row>
   </sheetData>
@@ -2366,7 +2418,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add tong ket sheet
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -4,21 +4,21 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="CÔ DIỄM" sheetId="1" r:id="rId1"/>
     <sheet name="CHÂU" sheetId="3" r:id="rId2"/>
     <sheet name="HÀ" sheetId="4" r:id="rId3"/>
     <sheet name="GIANG" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId5"/>
+    <sheet name="Tổng Kết" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="117">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -345,6 +345,30 @@
   </si>
   <si>
     <t>chưa làm giấy</t>
+  </si>
+  <si>
+    <t>Cô Diễm</t>
+  </si>
+  <si>
+    <t>Cô Yến</t>
+  </si>
+  <si>
+    <t>Chị Diệu</t>
+  </si>
+  <si>
+    <t>Tí</t>
+  </si>
+  <si>
+    <t>anh Tô</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hà </t>
+  </si>
+  <si>
+    <t>Giang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quốc </t>
   </si>
 </sst>
 </file>
@@ -505,10 +529,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -817,7 +841,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L18" sqref="L18"/>
     </sheetView>
@@ -849,10 +873,10 @@
       <c r="D1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="17"/>
+      <c r="I1" s="18"/>
       <c r="J1" s="16"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -995,7 +1019,7 @@
       <c r="I11" s="5">
         <v>10</v>
       </c>
-      <c r="K11" s="18" t="s">
+      <c r="K11" s="17" t="s">
         <v>108</v>
       </c>
     </row>
@@ -2072,10 +2096,10 @@
       <c r="E1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="17"/>
+      <c r="I1" s="18"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
@@ -2211,10 +2235,10 @@
       <c r="E1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="17"/>
+      <c r="I1" s="18"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -2362,10 +2386,10 @@
       <c r="E1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="17"/>
+      <c r="I1" s="18"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -2416,21 +2440,92 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D1:E1"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>110</v>
+      </c>
+      <c r="B11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>112</v>
+      </c>
+      <c r="B13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>114</v>
+      </c>
+      <c r="B15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>115</v>
+      </c>
+      <c r="B16">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>116</v>
+      </c>
+      <c r="B17">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32">
+        <f>SUM(B10:B29)</f>
+        <v>352.7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
duy chuyen cho co diem 800k
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="CÔ DIỄM" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="118">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -344,9 +344,6 @@
     <t>23/03/2024</t>
   </si>
   <si>
-    <t>chưa làm giấy</t>
-  </si>
-  <si>
     <t>Cô Diễm</t>
   </si>
   <si>
@@ -369,6 +366,12 @@
   </si>
   <si>
     <t xml:space="preserve">Quốc </t>
+  </si>
+  <si>
+    <t>27/03/2024</t>
+  </si>
+  <si>
+    <t>Duy chuyển cho cô Diễm 800k</t>
   </si>
 </sst>
 </file>
@@ -395,7 +398,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -411,12 +414,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -481,7 +478,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -527,9 +524,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -839,11 +833,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K83"/>
+  <dimension ref="A1:K84"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L18" sqref="L18"/>
+      <selection pane="bottomLeft" activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,10 +867,10 @@
       <c r="D1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="18"/>
+      <c r="I1" s="17"/>
       <c r="J1" s="16"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1019,9 +1013,7 @@
       <c r="I11" s="5">
         <v>10</v>
       </c>
-      <c r="K11" s="17" t="s">
-        <v>108</v>
-      </c>
+      <c r="K11" s="15"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
@@ -2046,6 +2038,25 @@
       </c>
       <c r="C83" s="5">
         <v>-10000</v>
+      </c>
+      <c r="D83" s="6">
+        <f>D82+C83</f>
+        <v>790</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C84" s="5">
+        <v>800</v>
+      </c>
+      <c r="D84" s="6">
+        <f>D83+C84</f>
+        <v>1590</v>
       </c>
     </row>
   </sheetData>
@@ -2096,10 +2107,10 @@
       <c r="E1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="18"/>
+      <c r="I1" s="17"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
@@ -2235,10 +2246,10 @@
       <c r="E1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="18"/>
+      <c r="I1" s="17"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -2386,10 +2397,10 @@
       <c r="E1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="18"/>
+      <c r="I1" s="17"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -2442,7 +2453,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
@@ -2459,7 +2470,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B10">
         <v>270</v>
@@ -2467,7 +2478,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B11">
         <v>30</v>
@@ -2475,7 +2486,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B12">
         <v>20</v>
@@ -2483,7 +2494,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B13">
         <v>15</v>
@@ -2491,12 +2502,12 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B15">
         <v>7</v>
@@ -2504,7 +2515,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B16">
         <v>8.5</v>
@@ -2512,7 +2523,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B17">
         <v>2.2000000000000002</v>

</xml_diff>

<commit_message>
duy chuyen cho co diem 1.5tr
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="120">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -372,6 +372,12 @@
   </si>
   <si>
     <t>Duy chuyển cho cô Diễm 800k</t>
+  </si>
+  <si>
+    <t>29/03/2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duy chuyển cho cô Diễm 1tr5 </t>
   </si>
 </sst>
 </file>
@@ -833,11 +839,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K84"/>
+  <dimension ref="A1:K85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K20" sqref="K20"/>
+      <selection pane="bottomLeft" activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2057,6 +2063,21 @@
       <c r="D84" s="6">
         <f>D83+C84</f>
         <v>1590</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C85" s="5">
+        <v>1500</v>
+      </c>
+      <c r="D85" s="6">
+        <f>D84+C85</f>
+        <v>3090</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
duy update chuyen co diem 5tr
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -12,13 +12,14 @@
     <sheet name="HÀ" sheetId="4" r:id="rId3"/>
     <sheet name="GIANG" sheetId="5" r:id="rId4"/>
     <sheet name="Tổng Kết" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="125">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -377,7 +378,22 @@
     <t>29/03/2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Duy chuyển cho cô Diễm 1tr5 </t>
+    <t>vu van cu</t>
+  </si>
+  <si>
+    <t>lam van khoi</t>
+  </si>
+  <si>
+    <t>ha thi dao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tổng </t>
+  </si>
+  <si>
+    <t>nguyen hoang kim oanh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duy chuyển cho cô Diễm 5tr </t>
   </si>
 </sst>
 </file>
@@ -387,7 +403,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -398,6 +414,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -484,7 +508,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -535,6 +559,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -843,7 +868,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D86" sqref="D86"/>
+      <selection pane="bottomLeft" activeCell="D89" sqref="D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2070,14 +2095,14 @@
         <v>118</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="C85" s="5">
-        <v>1500</v>
+        <v>5000</v>
       </c>
       <c r="D85" s="6">
         <f>D84+C85</f>
-        <v>3090</v>
+        <v>6590</v>
       </c>
     </row>
   </sheetData>
@@ -2563,4 +2588,64 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="B15" s="18">
+        <f>SUM(B2:B5)</f>
+        <v>5000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
duy lay tien loi ngay 30
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="128">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -394,6 +394,15 @@
   </si>
   <si>
     <t xml:space="preserve">Duy chuyển cho cô Diễm 5tr </t>
+  </si>
+  <si>
+    <t>30/03/2024</t>
+  </si>
+  <si>
+    <t>chưa làm giấy</t>
+  </si>
+  <si>
+    <t>GHI CHÚ</t>
   </si>
 </sst>
 </file>
@@ -556,10 +565,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -864,11 +873,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K85"/>
+  <dimension ref="A1:K88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D89" sqref="D89"/>
+      <selection pane="bottomLeft" activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,10 +907,10 @@
       <c r="D1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="17"/>
+      <c r="I1" s="18"/>
       <c r="J1" s="16"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -923,6 +932,9 @@
       <c r="J2" s="12" t="s">
         <v>5</v>
       </c>
+      <c r="K2" s="1" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
@@ -941,8 +953,8 @@
         <v>20</v>
       </c>
       <c r="J3" s="4">
-        <f>SUM(I3:I47)</f>
-        <v>270</v>
+        <f>SUM(I3:I48)</f>
+        <v>280</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1137,39 +1149,40 @@
       <c r="K17" s="15"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="5">
-        <v>3000</v>
-      </c>
-      <c r="D18" s="6">
-        <f>D14+C18</f>
-        <v>8490</v>
-      </c>
       <c r="H18" s="9" t="s">
-        <v>12</v>
+        <v>125</v>
       </c>
       <c r="I18" s="5">
         <v>10</v>
       </c>
-      <c r="K18" s="15"/>
+      <c r="K18" s="15" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="5">
+        <v>3000</v>
+      </c>
+      <c r="D19" s="6">
+        <f>D14+C19</f>
+        <v>8490</v>
+      </c>
       <c r="H19" s="9" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="I19" s="5">
         <v>10</v>
       </c>
-      <c r="K19" s="15"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H20" s="9">
-        <v>45293</v>
+      <c r="H20" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="I20" s="5">
         <v>10</v>
@@ -1178,7 +1191,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H21" s="9">
-        <v>45294</v>
+        <v>45293</v>
       </c>
       <c r="I21" s="5">
         <v>10</v>
@@ -1186,59 +1199,46 @@
       <c r="K21" s="15"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="5">
-        <v>4400</v>
-      </c>
-      <c r="D22" s="6">
-        <f>D18+C22</f>
-        <v>12890</v>
-      </c>
       <c r="H22" s="9">
-        <v>44964</v>
+        <v>45294</v>
       </c>
       <c r="I22" s="5">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K22" s="15"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="5">
+        <v>4400</v>
+      </c>
+      <c r="D23" s="6">
+        <f>D19+C23</f>
+        <v>12890</v>
+      </c>
+      <c r="H23" s="9">
+        <v>44964</v>
+      </c>
+      <c r="I23" s="5">
+        <v>20</v>
+      </c>
+      <c r="K23" s="15"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C24" s="5">
         <v>-10000</v>
       </c>
-      <c r="D23" s="6">
-        <f>D22+C23</f>
+      <c r="D24" s="6">
+        <f>D23+C24</f>
         <v>2890</v>
       </c>
-      <c r="H23" s="9">
+      <c r="H24" s="9">
         <v>44966</v>
-      </c>
-      <c r="I23" s="5">
-        <v>10</v>
-      </c>
-      <c r="K23" s="15"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="9">
-        <v>44967</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="5">
-        <v>1600</v>
-      </c>
-      <c r="D24" s="6">
-        <f t="shared" ref="D24:D31" si="1">D23+C24</f>
-        <v>4490</v>
-      </c>
-      <c r="H24" s="9">
-        <v>44968</v>
       </c>
       <c r="I24" s="5">
         <v>10</v>
@@ -1246,490 +1246,497 @@
       <c r="K24" s="15"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="9">
+        <v>44967</v>
+      </c>
       <c r="B25" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="5">
+        <v>1600</v>
+      </c>
+      <c r="D25" s="6">
+        <f t="shared" ref="D25:D32" si="1">D24+C25</f>
+        <v>4490</v>
+      </c>
+      <c r="H25" s="9">
+        <v>44968</v>
+      </c>
+      <c r="I25" s="5">
+        <v>10</v>
+      </c>
+      <c r="K25" s="15"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C26" s="5">
         <v>3000</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D26" s="6">
         <f t="shared" si="1"/>
         <v>7490</v>
       </c>
-      <c r="H25" s="9">
+      <c r="H26" s="9">
         <v>44969</v>
       </c>
-      <c r="I25" s="5">
+      <c r="I26" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B27" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C27" s="5">
         <v>2000</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D27" s="6">
         <f t="shared" si="1"/>
         <v>9490</v>
       </c>
-      <c r="H26" s="9">
+      <c r="H27" s="9">
         <v>45334</v>
       </c>
-      <c r="I26" s="5">
+      <c r="I27" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B28" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C28" s="5">
         <v>3000</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D28" s="6">
         <f t="shared" si="1"/>
         <v>12490</v>
       </c>
-      <c r="H27" s="9">
+      <c r="H28" s="9">
         <v>45325</v>
       </c>
-      <c r="I27" s="5">
+      <c r="I28" s="5">
         <v>10</v>
       </c>
-      <c r="K27" s="15"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="4" t="s">
+      <c r="K28" s="15"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C29" s="5">
         <v>-10000</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D29" s="6">
         <f t="shared" si="1"/>
         <v>2490</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B30" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C30" s="5">
         <v>4960</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D30" s="6">
         <f t="shared" si="1"/>
         <v>7450</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B31" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C31" s="5">
         <v>4000</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D31" s="6">
         <f t="shared" si="1"/>
         <v>11450</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B31" s="4" t="s">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C32" s="5">
         <v>-10000</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D32" s="6">
         <f t="shared" si="1"/>
         <v>1450</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B32" s="4" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C33" s="5">
         <v>7640</v>
       </c>
-      <c r="D32" s="6">
-        <f t="shared" ref="D32:D37" si="2">D31+C32</f>
+      <c r="D33" s="6">
+        <f t="shared" ref="D33:D38" si="2">D32+C33</f>
         <v>9090</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="9">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="9">
         <v>44968</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B34" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C34" s="5">
         <v>3000</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D34" s="6">
         <f t="shared" si="2"/>
         <v>12090</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="4" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C35" s="5">
         <v>-10000</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D35" s="6">
         <f t="shared" si="2"/>
         <v>2090</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="9">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="9">
         <v>44996</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B36" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="5">
+      <c r="C36" s="5">
         <v>800</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D36" s="6">
         <f t="shared" si="2"/>
         <v>2890</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="9" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B37" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C36" s="5">
+      <c r="C37" s="5">
         <v>2000</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D37" s="6">
         <f t="shared" si="2"/>
         <v>4890</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="9" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B38" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C37" s="5">
+      <c r="C38" s="5">
         <v>4000</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D38" s="6">
         <f t="shared" si="2"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="9" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B39" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C38" s="5">
+      <c r="C39" s="5">
         <v>4000</v>
       </c>
-      <c r="D38" s="6">
-        <f t="shared" ref="D38:D43" si="3">D37+C38</f>
+      <c r="D39" s="6">
+        <f t="shared" ref="D39:D44" si="3">D38+C39</f>
         <v>12890</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B39" s="4" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C39" s="5">
+      <c r="C40" s="5">
         <v>5000</v>
       </c>
-      <c r="D39" s="6">
+      <c r="D40" s="6">
         <f t="shared" si="3"/>
         <v>17890</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="4" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C40" s="5">
+      <c r="C41" s="5">
         <v>-10000</v>
       </c>
-      <c r="D40" s="6">
+      <c r="D41" s="6">
         <f t="shared" si="3"/>
         <v>7890</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="9">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="9">
         <v>44969</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B42" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C41" s="5">
+      <c r="C42" s="5">
         <v>900</v>
       </c>
-      <c r="D41" s="6">
+      <c r="D42" s="6">
         <f t="shared" si="3"/>
         <v>8790</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B42" s="4" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C43" s="5">
         <v>4000</v>
       </c>
-      <c r="D42" s="6">
+      <c r="D43" s="6">
         <f t="shared" si="3"/>
         <v>12790</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B43" s="4" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C43" s="5">
+      <c r="C44" s="5">
         <v>-10000</v>
       </c>
-      <c r="D43" s="6">
+      <c r="D44" s="6">
         <f t="shared" si="3"/>
         <v>2790</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C44" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D44" s="6">
-        <f t="shared" ref="D44:D51" si="4">D43+C44</f>
-        <v>4790</v>
-      </c>
-    </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C45" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D45" s="6">
+        <f t="shared" ref="D45:D52" si="4">D44+C45</f>
+        <v>4790</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B46" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C45" s="5">
+      <c r="C46" s="5">
         <v>700</v>
       </c>
-      <c r="D45" s="6">
+      <c r="D46" s="6">
         <f t="shared" si="4"/>
         <v>5490</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B46" s="4" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B47" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C46" s="5">
+      <c r="C47" s="5">
         <v>4000</v>
       </c>
-      <c r="D46" s="6">
+      <c r="D47" s="6">
         <f t="shared" si="4"/>
         <v>9490</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="9" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B48" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C48" s="5">
         <v>600</v>
       </c>
-      <c r="D47" s="6">
+      <c r="D48" s="6">
         <f t="shared" si="4"/>
         <v>10090</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B48" s="4" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C48" s="5">
+      <c r="C49" s="5">
         <v>-10000</v>
       </c>
-      <c r="D48" s="6">
+      <c r="D49" s="6">
         <f t="shared" si="4"/>
         <v>90</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="9" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B50" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C49" s="5">
+      <c r="C50" s="5">
         <f>700+5000+300+600+400+1000+800</f>
         <v>8800</v>
       </c>
-      <c r="D49" s="6">
+      <c r="D50" s="6">
         <f t="shared" si="4"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B50" s="4" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B51" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C50" s="5">
+      <c r="C51" s="5">
         <v>6000</v>
       </c>
-      <c r="D50" s="6">
+      <c r="D51" s="6">
         <f t="shared" si="4"/>
         <v>14890</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B51" s="4" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C51" s="5">
+      <c r="C52" s="5">
         <v>-10000</v>
       </c>
-      <c r="D51" s="6">
+      <c r="D52" s="6">
         <f t="shared" si="4"/>
         <v>4890</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="9" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B53" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C52" s="5">
+      <c r="C53" s="5">
         <v>500</v>
       </c>
-      <c r="D52" s="6">
-        <f t="shared" ref="D52:D57" si="5">D51+C52</f>
+      <c r="D53" s="6">
+        <f t="shared" ref="D53:D58" si="5">D52+C53</f>
         <v>5390</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="9">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="9">
         <v>45323</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B54" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C53" s="5">
+      <c r="C54" s="5">
         <v>700</v>
       </c>
-      <c r="D53" s="6">
+      <c r="D54" s="6">
         <f t="shared" si="5"/>
         <v>6090</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B54" s="4" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B55" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C54" s="5">
+      <c r="C55" s="5">
         <v>1500</v>
       </c>
-      <c r="D54" s="6">
+      <c r="D55" s="6">
         <f t="shared" si="5"/>
         <v>7590</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="4" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B56" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C55" s="5">
+      <c r="C56" s="5">
         <v>5000</v>
       </c>
-      <c r="D55" s="6">
+      <c r="D56" s="6">
         <f t="shared" si="5"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B56" s="4" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B57" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C56" s="5">
+      <c r="C57" s="5">
         <v>-10000</v>
       </c>
-      <c r="D56" s="6">
+      <c r="D57" s="6">
         <f t="shared" si="5"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="9" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B58" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C57" s="5">
+      <c r="C58" s="5">
         <v>2000</v>
       </c>
-      <c r="D57" s="6">
+      <c r="D58" s="6">
         <f t="shared" si="5"/>
         <v>4590</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="9">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="9">
         <v>45474</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C58" s="5">
-        <v>700</v>
-      </c>
-      <c r="D58" s="6">
-        <f t="shared" ref="D58:D63" si="6">D57+C58</f>
-        <v>5290</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="9" t="s">
-        <v>82</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>77</v>
@@ -1738,371 +1745,413 @@
         <v>700</v>
       </c>
       <c r="D59" s="6">
+        <f t="shared" ref="D59:D64" si="6">D58+C59</f>
+        <v>5290</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C60" s="5">
+        <v>700</v>
+      </c>
+      <c r="D60" s="6">
         <f t="shared" si="6"/>
         <v>5990</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="9" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B61" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C60" s="5">
+      <c r="C61" s="5">
         <v>700</v>
       </c>
-      <c r="D60" s="6">
+      <c r="D61" s="6">
         <f t="shared" si="6"/>
         <v>6690</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="9" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B62" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C61" s="5">
+      <c r="C62" s="5">
         <v>4000</v>
       </c>
-      <c r="D61" s="6">
+      <c r="D62" s="6">
         <f t="shared" si="6"/>
         <v>10690</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B62" s="4" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B63" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C62" s="5">
+      <c r="C63" s="5">
         <v>-10000</v>
       </c>
-      <c r="D62" s="6">
+      <c r="D63" s="6">
         <f t="shared" si="6"/>
         <v>690</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="9" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B64" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C63" s="5">
+      <c r="C64" s="5">
         <v>1000</v>
       </c>
-      <c r="D63" s="6">
+      <c r="D64" s="6">
         <f t="shared" si="6"/>
         <v>1690</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="9" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B65" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C64" s="5">
+      <c r="C65" s="5">
         <v>7000</v>
       </c>
-      <c r="D64" s="6">
-        <f t="shared" ref="D64:D69" si="7">D63+C64</f>
+      <c r="D65" s="6">
+        <f t="shared" ref="D65:D70" si="7">D64+C65</f>
         <v>8690</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B65" s="4" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C65" s="5">
+      <c r="C66" s="5">
         <v>10000</v>
       </c>
-      <c r="D65" s="6">
+      <c r="D66" s="6">
         <f t="shared" si="7"/>
         <v>18690</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B66" s="4" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B67" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C66" s="5">
+      <c r="C67" s="5">
         <v>-10000</v>
       </c>
-      <c r="D66" s="6">
+      <c r="D67" s="6">
         <f t="shared" si="7"/>
         <v>8690</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="9">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="9">
         <v>45293</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B68" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C67" s="5">
+      <c r="C68" s="5">
         <v>1700</v>
       </c>
-      <c r="D67" s="6">
+      <c r="D68" s="6">
         <f t="shared" si="7"/>
         <v>10390</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B68" s="4" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B69" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C68" s="5">
+      <c r="C69" s="5">
         <v>-10000</v>
       </c>
-      <c r="D68" s="6">
+      <c r="D69" s="6">
         <f t="shared" si="7"/>
         <v>390</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="9">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="9">
         <v>45324</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B70" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C69" s="5">
+      <c r="C70" s="5">
         <v>6000</v>
       </c>
-      <c r="D69" s="6">
+      <c r="D70" s="6">
         <f t="shared" si="7"/>
         <v>6390</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C70" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D70" s="6">
-        <f t="shared" ref="D70:D75" si="8">D69+C70</f>
-        <v>8390</v>
-      </c>
-    </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C71" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D71" s="6">
+        <f t="shared" ref="D71:D76" si="8">D70+C71</f>
+        <v>8390</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B72" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C71" s="5">
+      <c r="C72" s="5">
         <v>5000</v>
       </c>
-      <c r="D71" s="6">
+      <c r="D72" s="6">
         <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B72" s="4" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B73" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C72" s="5">
+      <c r="C73" s="5">
         <v>-10000</v>
       </c>
-      <c r="D72" s="6">
+      <c r="D73" s="6">
         <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="9" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B74" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C73" s="5">
+      <c r="C74" s="5">
         <v>1000</v>
       </c>
-      <c r="D73" s="6">
+      <c r="D74" s="6">
         <f t="shared" si="8"/>
         <v>4390</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="9">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="9">
         <v>45294</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B75" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C74" s="5">
+      <c r="C75" s="5">
         <v>9000</v>
       </c>
-      <c r="D74" s="6">
+      <c r="D75" s="6">
         <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B75" s="4" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B76" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C75" s="5">
+      <c r="C76" s="5">
         <v>-10000</v>
       </c>
-      <c r="D75" s="6">
+      <c r="D76" s="6">
         <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B76" s="4" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B77" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C76" s="5">
+      <c r="C77" s="5">
         <v>2000</v>
       </c>
-      <c r="D76" s="6">
-        <f t="shared" ref="D76:D81" si="9">D75+C76</f>
+      <c r="D77" s="6">
+        <f t="shared" ref="D77:D82" si="9">D76+C77</f>
         <v>5390</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="9">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="9">
         <v>45325</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="B78" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C77" s="5">
+      <c r="C78" s="5">
         <v>6000</v>
       </c>
-      <c r="D77" s="6">
+      <c r="D78" s="6">
         <f t="shared" si="9"/>
         <v>11390</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B78" s="4" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B79" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C78" s="5">
+      <c r="C79" s="5">
         <v>-10000</v>
       </c>
-      <c r="D78" s="6">
+      <c r="D79" s="6">
         <f t="shared" si="9"/>
         <v>1390</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="9">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="9">
         <v>45507</v>
       </c>
-      <c r="B79" s="4" t="s">
+      <c r="B80" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C79" s="5">
+      <c r="C80" s="5">
         <v>400</v>
       </c>
-      <c r="D79" s="6">
+      <c r="D80" s="6">
         <f t="shared" si="9"/>
         <v>1790</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="9" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B81" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C80" s="5">
+      <c r="C81" s="5">
         <v>2000</v>
       </c>
-      <c r="D80" s="6">
+      <c r="D81" s="6">
         <f t="shared" si="9"/>
         <v>3790</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="9" t="s">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="B81" s="4" t="s">
+      <c r="B82" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C81" s="5">
+      <c r="C82" s="5">
         <v>6000</v>
       </c>
-      <c r="D81" s="6">
+      <c r="D82" s="6">
         <f t="shared" si="9"/>
         <v>9790</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="9" t="s">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="B82" s="4" t="s">
+      <c r="B83" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C82" s="5">
+      <c r="C83" s="5">
         <v>1000</v>
-      </c>
-      <c r="D82" s="6">
-        <f>D81+C82</f>
-        <v>10790</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B83" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C83" s="5">
-        <v>-10000</v>
       </c>
       <c r="D83" s="6">
         <f>D82+C83</f>
-        <v>790</v>
+        <v>10790</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="9" t="s">
-        <v>116</v>
-      </c>
       <c r="B84" s="4" t="s">
-        <v>117</v>
+        <v>20</v>
       </c>
       <c r="C84" s="5">
-        <v>800</v>
+        <v>-10000</v>
       </c>
       <c r="D84" s="6">
         <f>D83+C84</f>
-        <v>1590</v>
+        <v>790</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C85" s="5">
-        <v>5000</v>
+        <v>800</v>
       </c>
       <c r="D85" s="6">
         <f>D84+C85</f>
+        <v>1590</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C86" s="5">
+        <v>5000</v>
+      </c>
+      <c r="D86" s="6">
+        <f>D85+C86</f>
         <v>6590</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C87" s="5">
+        <v>6000</v>
+      </c>
+      <c r="D87" s="6">
+        <f>D86+C87</f>
+        <v>12590</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B88" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C88" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D88" s="6">
+        <f>D87+C88</f>
+        <v>2590</v>
       </c>
     </row>
   </sheetData>
@@ -2153,10 +2202,10 @@
       <c r="E1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="17"/>
+      <c r="I1" s="18"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
@@ -2292,10 +2341,10 @@
       <c r="E1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="17"/>
+      <c r="I1" s="18"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -2443,10 +2492,10 @@
       <c r="E1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="17"/>
+      <c r="I1" s="18"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -2636,10 +2685,10 @@
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="B15" s="18">
+      <c r="B15" s="17">
         <f>SUM(B2:B5)</f>
         <v>5000</v>
       </c>

</xml_diff>

<commit_message>
duy lay tien loi ngay 31
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="130">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -403,6 +403,12 @@
   </si>
   <si>
     <t>GHI CHÚ</t>
+  </si>
+  <si>
+    <t>31/03/2023</t>
+  </si>
+  <si>
+    <t>31/03/2024</t>
   </si>
 </sst>
 </file>
@@ -437,7 +443,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -453,6 +459,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -517,7 +529,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -567,6 +579,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -873,11 +888,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K88"/>
+  <dimension ref="A1:K89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K35" sqref="K35"/>
+      <selection pane="bottomLeft" activeCell="I94" sqref="I94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1155,7 +1170,7 @@
       <c r="I18" s="5">
         <v>10</v>
       </c>
-      <c r="K18" s="15" t="s">
+      <c r="K18" s="19" t="s">
         <v>126</v>
       </c>
     </row>
@@ -2081,7 +2096,7 @@
         <v>1000</v>
       </c>
       <c r="D83" s="6">
-        <f>D82+C83</f>
+        <f t="shared" ref="D83:D88" si="10">D82+C83</f>
         <v>10790</v>
       </c>
     </row>
@@ -2093,7 +2108,7 @@
         <v>-10000</v>
       </c>
       <c r="D84" s="6">
-        <f>D83+C84</f>
+        <f t="shared" si="10"/>
         <v>790</v>
       </c>
     </row>
@@ -2108,7 +2123,7 @@
         <v>800</v>
       </c>
       <c r="D85" s="6">
-        <f>D84+C85</f>
+        <f t="shared" si="10"/>
         <v>1590</v>
       </c>
     </row>
@@ -2123,7 +2138,7 @@
         <v>5000</v>
       </c>
       <c r="D86" s="6">
-        <f>D85+C86</f>
+        <f t="shared" si="10"/>
         <v>6590</v>
       </c>
     </row>
@@ -2138,7 +2153,7 @@
         <v>6000</v>
       </c>
       <c r="D87" s="6">
-        <f>D86+C87</f>
+        <f t="shared" si="10"/>
         <v>12590</v>
       </c>
     </row>
@@ -2150,8 +2165,23 @@
         <v>-10000</v>
       </c>
       <c r="D88" s="6">
-        <f>D87+C88</f>
+        <f t="shared" si="10"/>
         <v>2590</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C89" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D89" s="6">
+        <f>D88+C89</f>
+        <v>4590</v>
       </c>
     </row>
   </sheetData>
@@ -2455,11 +2485,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2533,6 +2563,21 @@
       <c r="D3" s="4">
         <f>D2+C3</f>
         <v>8500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="5">
+        <v>1000</v>
+      </c>
+      <c r="D4" s="4">
+        <f>D3+C4</f>
+        <v>9500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
duy lay tien loi ngay 02/04
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="131">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -399,9 +399,6 @@
     <t>30/03/2024</t>
   </si>
   <si>
-    <t>chưa làm giấy</t>
-  </si>
-  <si>
     <t>GHI CHÚ</t>
   </si>
   <si>
@@ -409,6 +406,12 @@
   </si>
   <si>
     <t>31/03/2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Đông </t>
+  </si>
+  <si>
+    <t>Duy lấy tiền lời 7tr</t>
   </si>
 </sst>
 </file>
@@ -443,7 +446,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -459,12 +462,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -529,7 +526,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -579,9 +576,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -888,11 +882,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K89"/>
+  <dimension ref="A1:K92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I94" sqref="I94"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -948,7 +942,7 @@
         <v>5</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -969,7 +963,7 @@
       </c>
       <c r="J3" s="4">
         <f>SUM(I3:I48)</f>
-        <v>280</v>
+        <v>290</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1170,9 +1164,7 @@
       <c r="I18" s="5">
         <v>10</v>
       </c>
-      <c r="K18" s="19" t="s">
-        <v>126</v>
-      </c>
+      <c r="K18" s="15"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
@@ -1354,6 +1346,13 @@
         <f t="shared" si="1"/>
         <v>2490</v>
       </c>
+      <c r="H29" s="9">
+        <v>45326</v>
+      </c>
+      <c r="I29" s="5">
+        <v>10</v>
+      </c>
+      <c r="K29" s="15"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
@@ -2171,7 +2170,7 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B89" s="4" t="s">
         <v>65</v>
@@ -2182,6 +2181,48 @@
       <c r="D89" s="6">
         <f>D88+C89</f>
         <v>4590</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="9">
+        <v>45295</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C90" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D90" s="6">
+        <f>D89+C90</f>
+        <v>6590</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="9">
+        <v>45326</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C91" s="5">
+        <v>7000</v>
+      </c>
+      <c r="D91" s="6">
+        <f>D90+C91</f>
+        <v>13590</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B92" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C92" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D92" s="6">
+        <f>D91+C92</f>
+        <v>3590</v>
       </c>
     </row>
   </sheetData>
@@ -2567,7 +2608,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>56</v>
@@ -2594,7 +2635,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2613,7 +2654,7 @@
         <v>108</v>
       </c>
       <c r="B10">
-        <v>270</v>
+        <v>280000</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -2644,13 +2685,16 @@
       <c r="A14" t="s">
         <v>112</v>
       </c>
+      <c r="B14">
+        <v>9580</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>113</v>
       </c>
       <c r="B15">
-        <v>7</v>
+        <v>7000</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2658,7 +2702,7 @@
         <v>114</v>
       </c>
       <c r="B16">
-        <v>8.5</v>
+        <v>9500</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2666,7 +2710,15 @@
         <v>115</v>
       </c>
       <c r="B17">
-        <v>2.2000000000000002</v>
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>129</v>
+      </c>
+      <c r="B18">
+        <v>11000</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -2675,7 +2727,7 @@
       </c>
       <c r="B32">
         <f>SUM(B10:B29)</f>
-        <v>352.7</v>
+        <v>319345</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Duy lay tien loi ngay 30/04
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="134">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -415,6 +415,12 @@
   </si>
   <si>
     <t>23/04/2024</t>
+  </si>
+  <si>
+    <t>30/04/2024</t>
+  </si>
+  <si>
+    <t>Chưa làm giấy</t>
   </si>
 </sst>
 </file>
@@ -449,7 +455,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -465,6 +471,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -529,7 +541,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -579,6 +591,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -885,11 +900,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K97"/>
+  <dimension ref="A1:K100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D98" sqref="D98"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -965,8 +980,8 @@
         <v>20</v>
       </c>
       <c r="J3" s="4">
-        <f>SUM(I3:I49)</f>
-        <v>300</v>
+        <f>SUM(I3:I50)</f>
+        <v>310</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1179,38 +1194,40 @@
       <c r="K19" s="15"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" s="5">
-        <v>3000</v>
-      </c>
-      <c r="D20" s="6">
-        <f>D15+C20</f>
-        <v>8490</v>
-      </c>
       <c r="H20" s="9" t="s">
-        <v>12</v>
+        <v>132</v>
       </c>
       <c r="I20" s="5">
         <v>10</v>
       </c>
+      <c r="K20" s="19" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="5">
+        <v>3000</v>
+      </c>
+      <c r="D21" s="6">
+        <f>D15+C21</f>
+        <v>8490</v>
+      </c>
       <c r="H21" s="9" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="I21" s="5">
         <v>10</v>
       </c>
-      <c r="K21" s="15"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H22" s="9">
-        <v>45293</v>
+      <c r="H22" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="I22" s="5">
         <v>10</v>
@@ -1219,7 +1236,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H23" s="9">
-        <v>45294</v>
+        <v>45293</v>
       </c>
       <c r="I23" s="5">
         <v>10</v>
@@ -1227,59 +1244,46 @@
       <c r="K23" s="15"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="5">
-        <v>4400</v>
-      </c>
-      <c r="D24" s="6">
-        <f>D20+C24</f>
-        <v>12890</v>
-      </c>
       <c r="H24" s="9">
-        <v>44964</v>
+        <v>45294</v>
       </c>
       <c r="I24" s="5">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K24" s="15"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="5">
+        <v>4400</v>
+      </c>
+      <c r="D25" s="6">
+        <f>D21+C25</f>
+        <v>12890</v>
+      </c>
+      <c r="H25" s="9">
+        <v>44964</v>
+      </c>
+      <c r="I25" s="5">
+        <v>20</v>
+      </c>
+      <c r="K25" s="15"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C26" s="5">
         <v>-10000</v>
       </c>
-      <c r="D25" s="6">
-        <f>D24+C25</f>
+      <c r="D26" s="6">
+        <f>D25+C26</f>
         <v>2890</v>
       </c>
-      <c r="H25" s="9">
+      <c r="H26" s="9">
         <v>44966</v>
-      </c>
-      <c r="I25" s="5">
-        <v>10</v>
-      </c>
-      <c r="K25" s="15"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="9">
-        <v>44967</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="5">
-        <v>1600</v>
-      </c>
-      <c r="D26" s="6">
-        <f t="shared" ref="D26:D33" si="1">D25+C26</f>
-        <v>4490</v>
-      </c>
-      <c r="H26" s="9">
-        <v>44968</v>
       </c>
       <c r="I26" s="5">
         <v>10</v>
@@ -1287,497 +1291,504 @@
       <c r="K26" s="15"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="9">
+        <v>44967</v>
+      </c>
       <c r="B27" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="5">
+        <v>1600</v>
+      </c>
+      <c r="D27" s="6">
+        <f t="shared" ref="D27:D34" si="1">D26+C27</f>
+        <v>4490</v>
+      </c>
+      <c r="H27" s="9">
+        <v>44968</v>
+      </c>
+      <c r="I27" s="5">
+        <v>10</v>
+      </c>
+      <c r="K27" s="15"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C28" s="5">
         <v>3000</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D28" s="6">
         <f t="shared" si="1"/>
         <v>7490</v>
       </c>
-      <c r="H27" s="9">
+      <c r="H28" s="9">
         <v>44969</v>
       </c>
-      <c r="I27" s="5">
+      <c r="I28" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B29" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C29" s="5">
         <v>2000</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D29" s="6">
         <f t="shared" si="1"/>
         <v>9490</v>
       </c>
-      <c r="H28" s="9">
+      <c r="H29" s="9">
         <v>45334</v>
       </c>
-      <c r="I28" s="5">
+      <c r="I29" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B30" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C30" s="5">
         <v>3000</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D30" s="6">
         <f t="shared" si="1"/>
         <v>12490</v>
       </c>
-      <c r="H29" s="9">
+      <c r="H30" s="9">
         <v>45325</v>
       </c>
-      <c r="I29" s="5">
+      <c r="I30" s="5">
         <v>10</v>
       </c>
-      <c r="K29" s="15"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B30" s="4" t="s">
+      <c r="K30" s="15"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C31" s="5">
         <v>-10000</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D31" s="6">
         <f t="shared" si="1"/>
         <v>2490</v>
       </c>
-      <c r="H30" s="9">
+      <c r="H31" s="9">
         <v>45326</v>
       </c>
-      <c r="I30" s="5">
+      <c r="I31" s="5">
         <v>10</v>
       </c>
-      <c r="K30" s="15"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
+      <c r="K31" s="15"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B32" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C32" s="5">
         <v>4960</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D32" s="6">
         <f t="shared" si="1"/>
         <v>7450</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B33" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C33" s="5">
         <v>4000</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D33" s="6">
         <f t="shared" si="1"/>
         <v>11450</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="4" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C34" s="5">
         <v>-10000</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D34" s="6">
         <f t="shared" si="1"/>
         <v>1450</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="4" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C35" s="5">
         <v>7640</v>
       </c>
-      <c r="D34" s="6">
-        <f t="shared" ref="D34:D39" si="2">D33+C34</f>
+      <c r="D35" s="6">
+        <f t="shared" ref="D35:D40" si="2">D34+C35</f>
         <v>9090</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="9">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="9">
         <v>44968</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B36" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="5">
+      <c r="C36" s="5">
         <v>3000</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D36" s="6">
         <f t="shared" si="2"/>
         <v>12090</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="4" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C36" s="5">
+      <c r="C37" s="5">
         <v>-10000</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D37" s="6">
         <f t="shared" si="2"/>
         <v>2090</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="9">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="9">
         <v>44996</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B38" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C37" s="5">
+      <c r="C38" s="5">
         <v>800</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D38" s="6">
         <f t="shared" si="2"/>
         <v>2890</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="9" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B39" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="5">
+      <c r="C39" s="5">
         <v>2000</v>
       </c>
-      <c r="D38" s="6">
+      <c r="D39" s="6">
         <f t="shared" si="2"/>
         <v>4890</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B40" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C39" s="5">
+      <c r="C40" s="5">
         <v>4000</v>
       </c>
-      <c r="D39" s="6">
+      <c r="D40" s="6">
         <f t="shared" si="2"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="9" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B41" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C40" s="5">
+      <c r="C41" s="5">
         <v>4000</v>
       </c>
-      <c r="D40" s="6">
-        <f t="shared" ref="D40:D45" si="3">D39+C40</f>
+      <c r="D41" s="6">
+        <f t="shared" ref="D41:D46" si="3">D40+C41</f>
         <v>12890</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B41" s="4" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C41" s="5">
+      <c r="C42" s="5">
         <v>5000</v>
       </c>
-      <c r="D41" s="6">
+      <c r="D42" s="6">
         <f t="shared" si="3"/>
         <v>17890</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B42" s="4" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C43" s="5">
         <v>-10000</v>
       </c>
-      <c r="D42" s="6">
+      <c r="D43" s="6">
         <f t="shared" si="3"/>
         <v>7890</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="9">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="9">
         <v>44969</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B44" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C43" s="5">
+      <c r="C44" s="5">
         <v>900</v>
       </c>
-      <c r="D43" s="6">
+      <c r="D44" s="6">
         <f t="shared" si="3"/>
         <v>8790</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B44" s="4" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C45" s="5">
         <v>4000</v>
       </c>
-      <c r="D44" s="6">
+      <c r="D45" s="6">
         <f t="shared" si="3"/>
         <v>12790</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B45" s="4" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C45" s="5">
+      <c r="C46" s="5">
         <v>-10000</v>
       </c>
-      <c r="D45" s="6">
+      <c r="D46" s="6">
         <f t="shared" si="3"/>
         <v>2790</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C46" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D46" s="6">
-        <f t="shared" ref="D46:D53" si="4">D45+C46</f>
-        <v>4790</v>
-      </c>
-    </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C47" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D47" s="6">
+        <f t="shared" ref="D47:D54" si="4">D46+C47</f>
+        <v>4790</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B48" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C48" s="5">
         <v>700</v>
       </c>
-      <c r="D47" s="6">
+      <c r="D48" s="6">
         <f t="shared" si="4"/>
         <v>5490</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B48" s="4" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C48" s="5">
+      <c r="C49" s="5">
         <v>4000</v>
       </c>
-      <c r="D48" s="6">
+      <c r="D49" s="6">
         <f t="shared" si="4"/>
         <v>9490</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="9" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B50" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C49" s="5">
+      <c r="C50" s="5">
         <v>600</v>
       </c>
-      <c r="D49" s="6">
+      <c r="D50" s="6">
         <f t="shared" si="4"/>
         <v>10090</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B50" s="4" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B51" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C50" s="5">
+      <c r="C51" s="5">
         <v>-10000</v>
       </c>
-      <c r="D50" s="6">
+      <c r="D51" s="6">
         <f t="shared" si="4"/>
         <v>90</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="9" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B52" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C51" s="5">
+      <c r="C52" s="5">
         <f>700+5000+300+600+400+1000+800</f>
         <v>8800</v>
       </c>
-      <c r="D51" s="6">
+      <c r="D52" s="6">
         <f t="shared" si="4"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B52" s="4" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B53" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C52" s="5">
+      <c r="C53" s="5">
         <v>6000</v>
       </c>
-      <c r="D52" s="6">
+      <c r="D53" s="6">
         <f t="shared" si="4"/>
         <v>14890</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B53" s="4" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B54" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="5">
+      <c r="C54" s="5">
         <v>-10000</v>
       </c>
-      <c r="D53" s="6">
+      <c r="D54" s="6">
         <f t="shared" si="4"/>
         <v>4890</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="9" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B55" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C54" s="5">
+      <c r="C55" s="5">
         <v>500</v>
       </c>
-      <c r="D54" s="6">
-        <f t="shared" ref="D54:D59" si="5">D53+C54</f>
+      <c r="D55" s="6">
+        <f t="shared" ref="D55:D60" si="5">D54+C55</f>
         <v>5390</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="9">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="9">
         <v>45323</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B56" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C55" s="5">
+      <c r="C56" s="5">
         <v>700</v>
       </c>
-      <c r="D55" s="6">
+      <c r="D56" s="6">
         <f t="shared" si="5"/>
         <v>6090</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B56" s="4" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B57" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C56" s="5">
+      <c r="C57" s="5">
         <v>1500</v>
       </c>
-      <c r="D56" s="6">
+      <c r="D57" s="6">
         <f t="shared" si="5"/>
         <v>7590</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B57" s="4" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B58" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C57" s="5">
+      <c r="C58" s="5">
         <v>5000</v>
       </c>
-      <c r="D57" s="6">
+      <c r="D58" s="6">
         <f t="shared" si="5"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B58" s="4" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B59" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C58" s="5">
+      <c r="C59" s="5">
         <v>-10000</v>
       </c>
-      <c r="D58" s="6">
+      <c r="D59" s="6">
         <f t="shared" si="5"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="9" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B60" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C59" s="5">
+      <c r="C60" s="5">
         <v>2000</v>
       </c>
-      <c r="D59" s="6">
+      <c r="D60" s="6">
         <f t="shared" si="5"/>
         <v>4590</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="9">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="9">
         <v>45474</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C60" s="5">
-        <v>700</v>
-      </c>
-      <c r="D60" s="6">
-        <f t="shared" ref="D60:D65" si="6">D59+C60</f>
-        <v>5290</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="9" t="s">
-        <v>82</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>77</v>
@@ -1786,418 +1797,418 @@
         <v>700</v>
       </c>
       <c r="D61" s="6">
+        <f t="shared" ref="D61:D66" si="6">D60+C61</f>
+        <v>5290</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C62" s="5">
+        <v>700</v>
+      </c>
+      <c r="D62" s="6">
         <f t="shared" si="6"/>
         <v>5990</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="9" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B63" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C62" s="5">
+      <c r="C63" s="5">
         <v>700</v>
       </c>
-      <c r="D62" s="6">
+      <c r="D63" s="6">
         <f t="shared" si="6"/>
         <v>6690</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="9" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B64" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C63" s="5">
+      <c r="C64" s="5">
         <v>4000</v>
       </c>
-      <c r="D63" s="6">
+      <c r="D64" s="6">
         <f t="shared" si="6"/>
         <v>10690</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B64" s="4" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B65" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C64" s="5">
+      <c r="C65" s="5">
         <v>-10000</v>
       </c>
-      <c r="D64" s="6">
+      <c r="D65" s="6">
         <f t="shared" si="6"/>
         <v>690</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="9" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B66" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C65" s="5">
+      <c r="C66" s="5">
         <v>1000</v>
       </c>
-      <c r="D65" s="6">
+      <c r="D66" s="6">
         <f t="shared" si="6"/>
         <v>1690</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="9" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B67" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C66" s="5">
+      <c r="C67" s="5">
         <v>7000</v>
       </c>
-      <c r="D66" s="6">
-        <f t="shared" ref="D66:D71" si="7">D65+C66</f>
+      <c r="D67" s="6">
+        <f t="shared" ref="D67:D72" si="7">D66+C67</f>
         <v>8690</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B67" s="4" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B68" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C67" s="5">
+      <c r="C68" s="5">
         <v>10000</v>
       </c>
-      <c r="D67" s="6">
+      <c r="D68" s="6">
         <f t="shared" si="7"/>
         <v>18690</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B68" s="4" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B69" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C68" s="5">
+      <c r="C69" s="5">
         <v>-10000</v>
       </c>
-      <c r="D68" s="6">
+      <c r="D69" s="6">
         <f t="shared" si="7"/>
         <v>8690</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="9">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="9">
         <v>45293</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B70" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C69" s="5">
+      <c r="C70" s="5">
         <v>1700</v>
       </c>
-      <c r="D69" s="6">
+      <c r="D70" s="6">
         <f t="shared" si="7"/>
         <v>10390</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B70" s="4" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B71" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C70" s="5">
+      <c r="C71" s="5">
         <v>-10000</v>
       </c>
-      <c r="D70" s="6">
+      <c r="D71" s="6">
         <f t="shared" si="7"/>
         <v>390</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="9">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="9">
         <v>45324</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B72" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C71" s="5">
+      <c r="C72" s="5">
         <v>6000</v>
       </c>
-      <c r="D71" s="6">
+      <c r="D72" s="6">
         <f t="shared" si="7"/>
         <v>6390</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="B72" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C72" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D72" s="6">
-        <f t="shared" ref="D72:D77" si="8">D71+C72</f>
-        <v>8390</v>
-      </c>
-    </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C73" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D73" s="6">
+        <f t="shared" ref="D73:D78" si="8">D72+C73</f>
+        <v>8390</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B74" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C73" s="5">
+      <c r="C74" s="5">
         <v>5000</v>
       </c>
-      <c r="D73" s="6">
+      <c r="D74" s="6">
         <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B74" s="4" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B75" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C74" s="5">
+      <c r="C75" s="5">
         <v>-10000</v>
       </c>
-      <c r="D74" s="6">
+      <c r="D75" s="6">
         <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="9" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="B76" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C75" s="5">
+      <c r="C76" s="5">
         <v>1000</v>
       </c>
-      <c r="D75" s="6">
+      <c r="D76" s="6">
         <f t="shared" si="8"/>
         <v>4390</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="9">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="9">
         <v>45294</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B77" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C76" s="5">
+      <c r="C77" s="5">
         <v>9000</v>
       </c>
-      <c r="D76" s="6">
+      <c r="D77" s="6">
         <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B77" s="4" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B78" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C77" s="5">
+      <c r="C78" s="5">
         <v>-10000</v>
       </c>
-      <c r="D77" s="6">
+      <c r="D78" s="6">
         <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B78" s="4" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B79" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C78" s="5">
+      <c r="C79" s="5">
         <v>2000</v>
       </c>
-      <c r="D78" s="6">
-        <f t="shared" ref="D78:D83" si="9">D77+C78</f>
+      <c r="D79" s="6">
+        <f t="shared" ref="D79:D84" si="9">D78+C79</f>
         <v>5390</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="9">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="9">
         <v>45325</v>
       </c>
-      <c r="B79" s="4" t="s">
+      <c r="B80" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C79" s="5">
+      <c r="C80" s="5">
         <v>6000</v>
       </c>
-      <c r="D79" s="6">
+      <c r="D80" s="6">
         <f t="shared" si="9"/>
         <v>11390</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B80" s="4" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B81" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C80" s="5">
+      <c r="C81" s="5">
         <v>-10000</v>
       </c>
-      <c r="D80" s="6">
+      <c r="D81" s="6">
         <f t="shared" si="9"/>
         <v>1390</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="9">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="9">
         <v>45507</v>
       </c>
-      <c r="B81" s="4" t="s">
+      <c r="B82" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C81" s="5">
+      <c r="C82" s="5">
         <v>400</v>
       </c>
-      <c r="D81" s="6">
+      <c r="D82" s="6">
         <f t="shared" si="9"/>
         <v>1790</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="9" t="s">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="B82" s="4" t="s">
+      <c r="B83" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C82" s="5">
+      <c r="C83" s="5">
         <v>2000</v>
       </c>
-      <c r="D82" s="6">
+      <c r="D83" s="6">
         <f t="shared" si="9"/>
         <v>3790</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="9" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="B84" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C83" s="5">
+      <c r="C84" s="5">
         <v>6000</v>
       </c>
-      <c r="D83" s="6">
+      <c r="D84" s="6">
         <f t="shared" si="9"/>
         <v>9790</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="9" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="B84" s="4" t="s">
+      <c r="B85" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C84" s="5">
+      <c r="C85" s="5">
         <v>1000</v>
       </c>
-      <c r="D84" s="6">
-        <f t="shared" ref="D84:D89" si="10">D83+C84</f>
+      <c r="D85" s="6">
+        <f t="shared" ref="D85:D90" si="10">D84+C85</f>
         <v>10790</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B85" s="4" t="s">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B86" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C85" s="5">
+      <c r="C86" s="5">
         <v>-10000</v>
       </c>
-      <c r="D85" s="6">
+      <c r="D86" s="6">
         <f t="shared" si="10"/>
         <v>790</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="9" t="s">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="B87" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C86" s="5">
+      <c r="C87" s="5">
         <v>800</v>
       </c>
-      <c r="D86" s="6">
+      <c r="D87" s="6">
         <f t="shared" si="10"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="9" t="s">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="B87" s="4" t="s">
+      <c r="B88" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C87" s="5">
+      <c r="C88" s="5">
         <v>5000</v>
       </c>
-      <c r="D87" s="6">
+      <c r="D88" s="6">
         <f t="shared" si="10"/>
         <v>6590</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="9" t="s">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="B88" s="4" t="s">
+      <c r="B89" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C88" s="5">
+      <c r="C89" s="5">
         <v>6000</v>
       </c>
-      <c r="D88" s="6">
+      <c r="D89" s="6">
         <f t="shared" si="10"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B89" s="4" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B90" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C89" s="5">
+      <c r="C90" s="5">
         <v>-10000</v>
       </c>
-      <c r="D89" s="6">
+      <c r="D90" s="6">
         <f t="shared" si="10"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="9" t="s">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="9" t="s">
         <v>124</v>
-      </c>
-      <c r="B90" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C90" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D90" s="6">
-        <f t="shared" ref="D90:D96" si="11">D89+C90</f>
-        <v>4590</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="9">
-        <v>45295</v>
       </c>
       <c r="B91" s="4" t="s">
         <v>65</v>
@@ -2206,92 +2217,134 @@
         <v>2000</v>
       </c>
       <c r="D91" s="6">
+        <f t="shared" ref="D91:D97" si="11">D90+C91</f>
+        <v>4590</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="9">
+        <v>45295</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C92" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D92" s="6">
         <f t="shared" si="11"/>
         <v>6590</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="9">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="9">
         <v>45326</v>
       </c>
-      <c r="B92" s="4" t="s">
+      <c r="B93" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C92" s="5">
+      <c r="C93" s="5">
         <v>7000</v>
       </c>
-      <c r="D92" s="6">
+      <c r="D93" s="6">
         <f t="shared" si="11"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B93" s="4" t="s">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B94" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C93" s="5">
+      <c r="C94" s="5">
         <v>-10000</v>
       </c>
-      <c r="D93" s="6">
+      <c r="D94" s="6">
         <f t="shared" si="11"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="9" t="s">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="B94" s="4" t="s">
+      <c r="B95" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C94" s="5">
+      <c r="C95" s="5">
         <v>2000</v>
       </c>
-      <c r="D94" s="6">
+      <c r="D95" s="6">
         <f t="shared" si="11"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="9" t="s">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="B95" s="4" t="s">
+      <c r="B96" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C95" s="5">
+      <c r="C96" s="5">
         <v>6000</v>
       </c>
-      <c r="D95" s="6">
+      <c r="D96" s="6">
         <f t="shared" si="11"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B96" s="4" t="s">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B97" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C96" s="5">
+      <c r="C97" s="5">
         <v>-10000</v>
       </c>
-      <c r="D96" s="6">
+      <c r="D97" s="6">
         <f t="shared" si="11"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="9" t="s">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="B97" s="4" t="s">
+      <c r="B98" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C97" s="5">
+      <c r="C98" s="5">
         <v>2000</v>
       </c>
-      <c r="D97" s="6">
-        <f>D96+C97</f>
+      <c r="D98" s="6">
+        <f>D97+C98</f>
         <v>3590</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B99" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C99" s="5">
+        <v>7000</v>
+      </c>
+      <c r="D99" s="6">
+        <f>D98+C99</f>
+        <v>10590</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B100" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C100" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D100" s="6">
+        <f>D99+C100</f>
+        <v>590</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
duy lay tien loi ngay 2
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="136">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -421,6 +421,12 @@
   </si>
   <si>
     <t>Chưa làm giấy</t>
+  </si>
+  <si>
+    <t>Duy lấy tiền lời ngày 31,01,02</t>
+  </si>
+  <si>
+    <t>Duy chuyển cho cô Diễm 2tr</t>
   </si>
 </sst>
 </file>
@@ -590,10 +596,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -900,11 +906,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K100"/>
+  <dimension ref="A1:K103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D104" sqref="D104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -934,10 +940,10 @@
       <c r="D1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="18"/>
+      <c r="I1" s="19"/>
       <c r="J1" s="16"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -981,7 +987,7 @@
       </c>
       <c r="J3" s="4">
         <f>SUM(I3:I50)</f>
-        <v>310</v>
+        <v>320</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1200,7 +1206,7 @@
       <c r="I20" s="5">
         <v>10</v>
       </c>
-      <c r="K20" s="19" t="s">
+      <c r="K20" s="18" t="s">
         <v>133</v>
       </c>
     </row>
@@ -1406,6 +1412,15 @@
         <f t="shared" si="1"/>
         <v>7450</v>
       </c>
+      <c r="H32" s="9">
+        <v>45327</v>
+      </c>
+      <c r="I32" s="5">
+        <v>10</v>
+      </c>
+      <c r="K32" s="18" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
@@ -2345,6 +2360,45 @@
       <c r="D100" s="6">
         <f>D99+C100</f>
         <v>590</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="9">
+        <v>45327</v>
+      </c>
+      <c r="B101" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C101" s="5">
+        <v>12000</v>
+      </c>
+      <c r="D101" s="6">
+        <f>D100+C101</f>
+        <v>12590</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B102" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C102" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D102" s="6">
+        <f>D101+C102</f>
+        <v>2590</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B103" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C103" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D103" s="6">
+        <f>D102+C103</f>
+        <v>4590</v>
       </c>
     </row>
   </sheetData>
@@ -2395,10 +2449,10 @@
       <c r="E1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="18"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
@@ -2534,10 +2588,10 @@
       <c r="E1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="18"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -2700,10 +2754,10 @@
       <c r="E1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="18"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">

</xml_diff>

<commit_message>
duy cho co diem vay 5tr
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="147">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -442,6 +442,24 @@
   </si>
   <si>
     <t>31/05/2024</t>
+  </si>
+  <si>
+    <t>tran ngoc quang</t>
+  </si>
+  <si>
+    <t>nguyen khanh duy</t>
+  </si>
+  <si>
+    <t>co diem no</t>
+  </si>
+  <si>
+    <t>vo thi dang nga</t>
+  </si>
+  <si>
+    <t>Duy chyển cho cô Diễm 5tr</t>
+  </si>
+  <si>
+    <t>31/05/2023</t>
   </si>
 </sst>
 </file>
@@ -912,11 +930,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K112"/>
+  <dimension ref="A1:K115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D113" sqref="D113"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -992,8 +1010,8 @@
         <v>20</v>
       </c>
       <c r="J3" s="4">
-        <f>SUM(I3:I52)</f>
-        <v>340</v>
+        <f>SUM(I3:I53)</f>
+        <v>350</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1263,8 +1281,8 @@
       <c r="K24" s="15"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H25" s="9">
-        <v>45293</v>
+      <c r="H25" s="9" t="s">
+        <v>146</v>
       </c>
       <c r="I25" s="5">
         <v>10</v>
@@ -1273,7 +1291,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H26" s="9">
-        <v>45294</v>
+        <v>45293</v>
       </c>
       <c r="I26" s="5">
         <v>10</v>
@@ -1281,59 +1299,46 @@
       <c r="K26" s="15"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C27" s="5">
-        <v>4400</v>
-      </c>
-      <c r="D27" s="6">
-        <f>D23+C27</f>
-        <v>12890</v>
-      </c>
       <c r="H27" s="9">
-        <v>44964</v>
+        <v>45294</v>
       </c>
       <c r="I27" s="5">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K27" s="15"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="5">
+        <v>4400</v>
+      </c>
+      <c r="D28" s="6">
+        <f>D23+C28</f>
+        <v>12890</v>
+      </c>
+      <c r="H28" s="9">
+        <v>44964</v>
+      </c>
+      <c r="I28" s="5">
+        <v>20</v>
+      </c>
+      <c r="K28" s="15"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C29" s="5">
         <v>-10000</v>
       </c>
-      <c r="D28" s="6">
-        <f>D27+C28</f>
+      <c r="D29" s="6">
+        <f>D28+C29</f>
         <v>2890</v>
       </c>
-      <c r="H28" s="9">
+      <c r="H29" s="9">
         <v>44966</v>
-      </c>
-      <c r="I28" s="5">
-        <v>10</v>
-      </c>
-      <c r="K28" s="15"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="9">
-        <v>44967</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C29" s="5">
-        <v>1600</v>
-      </c>
-      <c r="D29" s="6">
-        <f t="shared" ref="D29:D36" si="1">D28+C29</f>
-        <v>4490</v>
-      </c>
-      <c r="H29" s="9">
-        <v>44968</v>
       </c>
       <c r="I29" s="5">
         <v>10</v>
@@ -1341,504 +1346,511 @@
       <c r="K29" s="15"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="9">
+        <v>44967</v>
+      </c>
       <c r="B30" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="5">
+        <v>1600</v>
+      </c>
+      <c r="D30" s="6">
+        <f t="shared" ref="D30:D37" si="1">D29+C30</f>
+        <v>4490</v>
+      </c>
+      <c r="H30" s="9">
+        <v>44968</v>
+      </c>
+      <c r="I30" s="5">
+        <v>10</v>
+      </c>
+      <c r="K30" s="15"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C31" s="5">
         <v>3000</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D31" s="6">
         <f t="shared" si="1"/>
         <v>7490</v>
       </c>
-      <c r="H30" s="9">
+      <c r="H31" s="9">
         <v>44969</v>
       </c>
-      <c r="I30" s="5">
+      <c r="I31" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B32" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C32" s="5">
         <v>2000</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D32" s="6">
         <f t="shared" si="1"/>
         <v>9490</v>
       </c>
-      <c r="H31" s="9">
+      <c r="H32" s="9">
         <v>45334</v>
       </c>
-      <c r="I31" s="5">
+      <c r="I32" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B33" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C33" s="5">
         <v>3000</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D33" s="6">
         <f t="shared" si="1"/>
         <v>12490</v>
       </c>
-      <c r="H32" s="9">
+      <c r="H33" s="9">
         <v>45325</v>
       </c>
-      <c r="I32" s="5">
+      <c r="I33" s="5">
         <v>10</v>
       </c>
-      <c r="K32" s="15"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B33" s="4" t="s">
+      <c r="K33" s="15"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B34" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C34" s="5">
         <v>-10000</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D34" s="6">
         <f t="shared" si="1"/>
         <v>2490</v>
       </c>
-      <c r="H33" s="9">
+      <c r="H34" s="9">
         <v>45326</v>
       </c>
-      <c r="I33" s="5">
+      <c r="I34" s="5">
         <v>10</v>
       </c>
-      <c r="K33" s="15"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
+      <c r="K34" s="15"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B35" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C35" s="5">
         <v>4960</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D35" s="6">
         <f t="shared" si="1"/>
         <v>7450</v>
       </c>
-      <c r="H34" s="9">
+      <c r="H35" s="9">
         <v>45327</v>
       </c>
-      <c r="I34" s="5">
+      <c r="I35" s="5">
         <v>10</v>
       </c>
-      <c r="K34" s="15"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
+      <c r="K35" s="15"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B36" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="5">
+      <c r="C36" s="5">
         <v>4000</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D36" s="6">
         <f t="shared" si="1"/>
         <v>11450</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B36" s="4" t="s">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B37" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C36" s="5">
+      <c r="C37" s="5">
         <v>-10000</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D37" s="6">
         <f t="shared" si="1"/>
         <v>1450</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B37" s="4" t="s">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B38" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C37" s="5">
+      <c r="C38" s="5">
         <v>7640</v>
       </c>
-      <c r="D37" s="6">
-        <f t="shared" ref="D37:D42" si="2">D36+C37</f>
+      <c r="D38" s="6">
+        <f t="shared" ref="D38:D43" si="2">D37+C38</f>
         <v>9090</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="9">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="9">
         <v>44968</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B39" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C38" s="5">
+      <c r="C39" s="5">
         <v>3000</v>
       </c>
-      <c r="D38" s="6">
+      <c r="D39" s="6">
         <f t="shared" si="2"/>
         <v>12090</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B39" s="4" t="s">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C39" s="5">
+      <c r="C40" s="5">
         <v>-10000</v>
       </c>
-      <c r="D39" s="6">
+      <c r="D40" s="6">
         <f t="shared" si="2"/>
         <v>2090</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="9">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="9">
         <v>44996</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B41" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C40" s="5">
+      <c r="C41" s="5">
         <v>800</v>
       </c>
-      <c r="D40" s="6">
+      <c r="D41" s="6">
         <f t="shared" si="2"/>
         <v>2890</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B42" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C41" s="5">
+      <c r="C42" s="5">
         <v>2000</v>
       </c>
-      <c r="D41" s="6">
+      <c r="D42" s="6">
         <f t="shared" si="2"/>
         <v>4890</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="9" t="s">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B43" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C43" s="5">
         <v>4000</v>
       </c>
-      <c r="D42" s="6">
+      <c r="D43" s="6">
         <f t="shared" si="2"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="9" t="s">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B44" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C43" s="5">
+      <c r="C44" s="5">
         <v>4000</v>
       </c>
-      <c r="D43" s="6">
-        <f t="shared" ref="D43:D48" si="3">D42+C43</f>
+      <c r="D44" s="6">
+        <f t="shared" ref="D44:D49" si="3">D43+C44</f>
         <v>12890</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B44" s="4" t="s">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B45" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C45" s="5">
         <v>5000</v>
       </c>
-      <c r="D44" s="6">
+      <c r="D45" s="6">
         <f t="shared" si="3"/>
         <v>17890</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B45" s="4" t="s">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B46" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C45" s="5">
+      <c r="C46" s="5">
         <v>-10000</v>
       </c>
-      <c r="D45" s="6">
+      <c r="D46" s="6">
         <f t="shared" si="3"/>
         <v>7890</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="9">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="9">
         <v>44969</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B47" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C46" s="5">
+      <c r="C47" s="5">
         <v>900</v>
       </c>
-      <c r="D46" s="6">
+      <c r="D47" s="6">
         <f t="shared" si="3"/>
         <v>8790</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B47" s="4" t="s">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B48" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C48" s="5">
         <v>4000</v>
       </c>
-      <c r="D47" s="6">
+      <c r="D48" s="6">
         <f t="shared" si="3"/>
         <v>12790</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B48" s="4" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C48" s="5">
+      <c r="C49" s="5">
         <v>-10000</v>
       </c>
-      <c r="D48" s="6">
+      <c r="D49" s="6">
         <f t="shared" si="3"/>
         <v>2790</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C49" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D49" s="6">
-        <f t="shared" ref="D49:D56" si="4">D48+C49</f>
-        <v>4790</v>
-      </c>
-    </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C50" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D50" s="6">
+        <f t="shared" ref="D50:D57" si="4">D49+C50</f>
+        <v>4790</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B51" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C50" s="5">
+      <c r="C51" s="5">
         <v>700</v>
       </c>
-      <c r="D50" s="6">
+      <c r="D51" s="6">
         <f t="shared" si="4"/>
         <v>5490</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B51" s="4" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C51" s="5">
+      <c r="C52" s="5">
         <v>4000</v>
       </c>
-      <c r="D51" s="6">
+      <c r="D52" s="6">
         <f t="shared" si="4"/>
         <v>9490</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="9" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B53" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C52" s="5">
+      <c r="C53" s="5">
         <v>600</v>
       </c>
-      <c r="D52" s="6">
+      <c r="D53" s="6">
         <f t="shared" si="4"/>
         <v>10090</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B53" s="4" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B54" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="5">
+      <c r="C54" s="5">
         <v>-10000</v>
       </c>
-      <c r="D53" s="6">
+      <c r="D54" s="6">
         <f t="shared" si="4"/>
         <v>90</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="9" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B55" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C54" s="5">
+      <c r="C55" s="5">
         <f>700+5000+300+600+400+1000+800</f>
         <v>8800</v>
       </c>
-      <c r="D54" s="6">
+      <c r="D55" s="6">
         <f t="shared" si="4"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="4" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B56" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C55" s="5">
+      <c r="C56" s="5">
         <v>6000</v>
       </c>
-      <c r="D55" s="6">
+      <c r="D56" s="6">
         <f t="shared" si="4"/>
         <v>14890</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B56" s="4" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B57" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C56" s="5">
+      <c r="C57" s="5">
         <v>-10000</v>
       </c>
-      <c r="D56" s="6">
+      <c r="D57" s="6">
         <f t="shared" si="4"/>
         <v>4890</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="9" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B58" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C57" s="5">
+      <c r="C58" s="5">
         <v>500</v>
       </c>
-      <c r="D57" s="6">
-        <f t="shared" ref="D57:D62" si="5">D56+C57</f>
+      <c r="D58" s="6">
+        <f t="shared" ref="D58:D63" si="5">D57+C58</f>
         <v>5390</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="9">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="9">
         <v>45323</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B59" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C58" s="5">
+      <c r="C59" s="5">
         <v>700</v>
       </c>
-      <c r="D58" s="6">
+      <c r="D59" s="6">
         <f t="shared" si="5"/>
         <v>6090</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B59" s="4" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B60" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C59" s="5">
+      <c r="C60" s="5">
         <v>1500</v>
       </c>
-      <c r="D59" s="6">
+      <c r="D60" s="6">
         <f t="shared" si="5"/>
         <v>7590</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B60" s="4" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B61" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C60" s="5">
+      <c r="C61" s="5">
         <v>5000</v>
       </c>
-      <c r="D60" s="6">
+      <c r="D61" s="6">
         <f t="shared" si="5"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B61" s="4" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B62" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C61" s="5">
+      <c r="C62" s="5">
         <v>-10000</v>
       </c>
-      <c r="D61" s="6">
+      <c r="D62" s="6">
         <f t="shared" si="5"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="9" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B63" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C62" s="5">
+      <c r="C63" s="5">
         <v>2000</v>
       </c>
-      <c r="D62" s="6">
+      <c r="D63" s="6">
         <f t="shared" si="5"/>
         <v>4590</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="9">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="9">
         <v>45474</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C63" s="5">
-        <v>700</v>
-      </c>
-      <c r="D63" s="6">
-        <f t="shared" ref="D63:D68" si="6">D62+C63</f>
-        <v>5290</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="9" t="s">
-        <v>82</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>77</v>
@@ -1847,418 +1859,418 @@
         <v>700</v>
       </c>
       <c r="D64" s="6">
+        <f t="shared" ref="D64:D69" si="6">D63+C64</f>
+        <v>5290</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C65" s="5">
+        <v>700</v>
+      </c>
+      <c r="D65" s="6">
         <f t="shared" si="6"/>
         <v>5990</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="9" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B66" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C65" s="5">
+      <c r="C66" s="5">
         <v>700</v>
       </c>
-      <c r="D65" s="6">
+      <c r="D66" s="6">
         <f t="shared" si="6"/>
         <v>6690</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="9" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B67" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C66" s="5">
+      <c r="C67" s="5">
         <v>4000</v>
       </c>
-      <c r="D66" s="6">
+      <c r="D67" s="6">
         <f t="shared" si="6"/>
         <v>10690</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B67" s="4" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B68" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C67" s="5">
+      <c r="C68" s="5">
         <v>-10000</v>
       </c>
-      <c r="D67" s="6">
+      <c r="D68" s="6">
         <f t="shared" si="6"/>
         <v>690</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="9" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B69" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C68" s="5">
+      <c r="C69" s="5">
         <v>1000</v>
       </c>
-      <c r="D68" s="6">
+      <c r="D69" s="6">
         <f t="shared" si="6"/>
         <v>1690</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="9" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B70" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C69" s="5">
+      <c r="C70" s="5">
         <v>7000</v>
       </c>
-      <c r="D69" s="6">
-        <f t="shared" ref="D69:D74" si="7">D68+C69</f>
+      <c r="D70" s="6">
+        <f t="shared" ref="D70:D75" si="7">D69+C70</f>
         <v>8690</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B70" s="4" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B71" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C70" s="5">
+      <c r="C71" s="5">
         <v>10000</v>
       </c>
-      <c r="D70" s="6">
+      <c r="D71" s="6">
         <f t="shared" si="7"/>
         <v>18690</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B71" s="4" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B72" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C71" s="5">
+      <c r="C72" s="5">
         <v>-10000</v>
       </c>
-      <c r="D71" s="6">
+      <c r="D72" s="6">
         <f t="shared" si="7"/>
         <v>8690</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="9">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="9">
         <v>45293</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B73" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C72" s="5">
+      <c r="C73" s="5">
         <v>1700</v>
       </c>
-      <c r="D72" s="6">
+      <c r="D73" s="6">
         <f t="shared" si="7"/>
         <v>10390</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B73" s="4" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C73" s="5">
+      <c r="C74" s="5">
         <v>-10000</v>
       </c>
-      <c r="D73" s="6">
+      <c r="D74" s="6">
         <f t="shared" si="7"/>
         <v>390</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="9">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="9">
         <v>45324</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B75" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C74" s="5">
+      <c r="C75" s="5">
         <v>6000</v>
       </c>
-      <c r="D74" s="6">
+      <c r="D75" s="6">
         <f t="shared" si="7"/>
         <v>6390</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C75" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D75" s="6">
-        <f t="shared" ref="D75:D80" si="8">D74+C75</f>
-        <v>8390</v>
-      </c>
-    </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C76" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D76" s="6">
+        <f t="shared" ref="D76:D81" si="8">D75+C76</f>
+        <v>8390</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B77" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C76" s="5">
+      <c r="C77" s="5">
         <v>5000</v>
       </c>
-      <c r="D76" s="6">
+      <c r="D77" s="6">
         <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B77" s="4" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B78" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C77" s="5">
+      <c r="C78" s="5">
         <v>-10000</v>
       </c>
-      <c r="D77" s="6">
+      <c r="D78" s="6">
         <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="9" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B79" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C78" s="5">
+      <c r="C79" s="5">
         <v>1000</v>
       </c>
-      <c r="D78" s="6">
+      <c r="D79" s="6">
         <f t="shared" si="8"/>
         <v>4390</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="9">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="9">
         <v>45294</v>
       </c>
-      <c r="B79" s="4" t="s">
+      <c r="B80" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C79" s="5">
+      <c r="C80" s="5">
         <v>9000</v>
       </c>
-      <c r="D79" s="6">
+      <c r="D80" s="6">
         <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B80" s="4" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B81" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C80" s="5">
+      <c r="C81" s="5">
         <v>-10000</v>
       </c>
-      <c r="D80" s="6">
+      <c r="D81" s="6">
         <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B81" s="4" t="s">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B82" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C81" s="5">
+      <c r="C82" s="5">
         <v>2000</v>
       </c>
-      <c r="D81" s="6">
-        <f t="shared" ref="D81:D86" si="9">D80+C81</f>
+      <c r="D82" s="6">
+        <f t="shared" ref="D82:D87" si="9">D81+C82</f>
         <v>5390</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="9">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="9">
         <v>45325</v>
       </c>
-      <c r="B82" s="4" t="s">
+      <c r="B83" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C82" s="5">
+      <c r="C83" s="5">
         <v>6000</v>
       </c>
-      <c r="D82" s="6">
+      <c r="D83" s="6">
         <f t="shared" si="9"/>
         <v>11390</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B83" s="4" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B84" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C83" s="5">
+      <c r="C84" s="5">
         <v>-10000</v>
       </c>
-      <c r="D83" s="6">
+      <c r="D84" s="6">
         <f t="shared" si="9"/>
         <v>1390</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="9">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="9">
         <v>45507</v>
       </c>
-      <c r="B84" s="4" t="s">
+      <c r="B85" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C84" s="5">
+      <c r="C85" s="5">
         <v>400</v>
       </c>
-      <c r="D84" s="6">
+      <c r="D85" s="6">
         <f t="shared" si="9"/>
         <v>1790</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="9" t="s">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="B85" s="4" t="s">
+      <c r="B86" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C85" s="5">
+      <c r="C86" s="5">
         <v>2000</v>
       </c>
-      <c r="D85" s="6">
+      <c r="D86" s="6">
         <f t="shared" si="9"/>
         <v>3790</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="9" t="s">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="B87" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C86" s="5">
+      <c r="C87" s="5">
         <v>6000</v>
       </c>
-      <c r="D86" s="6">
+      <c r="D87" s="6">
         <f t="shared" si="9"/>
         <v>9790</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="9" t="s">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="B87" s="4" t="s">
+      <c r="B88" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C87" s="5">
+      <c r="C88" s="5">
         <v>1000</v>
       </c>
-      <c r="D87" s="6">
-        <f t="shared" ref="D87:D92" si="10">D86+C87</f>
+      <c r="D88" s="6">
+        <f t="shared" ref="D88:D93" si="10">D87+C88</f>
         <v>10790</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B88" s="4" t="s">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B89" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C88" s="5">
+      <c r="C89" s="5">
         <v>-10000</v>
       </c>
-      <c r="D88" s="6">
+      <c r="D89" s="6">
         <f t="shared" si="10"/>
         <v>790</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="9" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="B89" s="4" t="s">
+      <c r="B90" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C89" s="5">
+      <c r="C90" s="5">
         <v>800</v>
       </c>
-      <c r="D89" s="6">
+      <c r="D90" s="6">
         <f t="shared" si="10"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="9" t="s">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="B90" s="4" t="s">
+      <c r="B91" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C90" s="5">
+      <c r="C91" s="5">
         <v>5000</v>
       </c>
-      <c r="D90" s="6">
+      <c r="D91" s="6">
         <f t="shared" si="10"/>
         <v>6590</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="9" t="s">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="B91" s="4" t="s">
+      <c r="B92" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C91" s="5">
+      <c r="C92" s="5">
         <v>6000</v>
       </c>
-      <c r="D91" s="6">
+      <c r="D92" s="6">
         <f t="shared" si="10"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B92" s="4" t="s">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B93" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C92" s="5">
+      <c r="C93" s="5">
         <v>-10000</v>
       </c>
-      <c r="D92" s="6">
+      <c r="D93" s="6">
         <f t="shared" si="10"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="9" t="s">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="9" t="s">
         <v>124</v>
-      </c>
-      <c r="B93" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C93" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D93" s="6">
-        <f t="shared" ref="D93:D99" si="11">D92+C93</f>
-        <v>4590</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="9">
-        <v>45295</v>
       </c>
       <c r="B94" s="4" t="s">
         <v>65</v>
@@ -2267,257 +2279,296 @@
         <v>2000</v>
       </c>
       <c r="D94" s="6">
+        <f t="shared" ref="D94:D100" si="11">D93+C94</f>
+        <v>4590</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="9">
+        <v>45295</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C95" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D95" s="6">
         <f t="shared" si="11"/>
         <v>6590</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="9">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="9">
         <v>45326</v>
       </c>
-      <c r="B95" s="4" t="s">
+      <c r="B96" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C95" s="5">
+      <c r="C96" s="5">
         <v>7000</v>
       </c>
-      <c r="D95" s="6">
+      <c r="D96" s="6">
         <f t="shared" si="11"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B96" s="4" t="s">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B97" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C96" s="5">
+      <c r="C97" s="5">
         <v>-10000</v>
       </c>
-      <c r="D96" s="6">
+      <c r="D97" s="6">
         <f t="shared" si="11"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="9" t="s">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="B97" s="4" t="s">
+      <c r="B98" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C97" s="5">
+      <c r="C98" s="5">
         <v>2000</v>
       </c>
-      <c r="D97" s="6">
+      <c r="D98" s="6">
         <f t="shared" si="11"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="9" t="s">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="B98" s="4" t="s">
+      <c r="B99" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C98" s="5">
+      <c r="C99" s="5">
         <v>6000</v>
       </c>
-      <c r="D98" s="6">
+      <c r="D99" s="6">
         <f t="shared" si="11"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B99" s="4" t="s">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B100" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C99" s="5">
+      <c r="C100" s="5">
         <v>-10000</v>
       </c>
-      <c r="D99" s="6">
+      <c r="D100" s="6">
         <f t="shared" si="11"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="B100" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C100" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D100" s="6">
-        <f t="shared" ref="D100:D105" si="12">D99+C100</f>
-        <v>3590</v>
-      </c>
-    </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="B101" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C101" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D101" s="6">
+        <f t="shared" ref="D101:D106" si="12">D100+C101</f>
+        <v>3590</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="B101" s="4" t="s">
+      <c r="B102" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C101" s="5">
+      <c r="C102" s="5">
         <v>7000</v>
       </c>
-      <c r="D101" s="6">
+      <c r="D102" s="6">
         <f t="shared" si="12"/>
         <v>10590</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B102" s="4" t="s">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B103" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C102" s="5">
+      <c r="C103" s="5">
         <v>-10000</v>
       </c>
-      <c r="D102" s="6">
+      <c r="D103" s="6">
         <f t="shared" si="12"/>
         <v>590</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="9">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="9">
         <v>45327</v>
       </c>
-      <c r="B103" s="4" t="s">
+      <c r="B104" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C103" s="5">
+      <c r="C104" s="5">
         <v>12000</v>
       </c>
-      <c r="D103" s="6">
+      <c r="D104" s="6">
         <f t="shared" si="12"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B104" s="4" t="s">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B105" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C104" s="5">
+      <c r="C105" s="5">
         <v>-10000</v>
       </c>
-      <c r="D104" s="6">
+      <c r="D105" s="6">
         <f t="shared" si="12"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B105" s="4" t="s">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B106" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C105" s="5">
+      <c r="C106" s="5">
         <v>2000</v>
       </c>
-      <c r="D105" s="6">
+      <c r="D106" s="6">
         <f t="shared" si="12"/>
         <v>4590</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="B106" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C106" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D106" s="6">
-        <f t="shared" ref="D106:D111" si="13">D105+C106</f>
-        <v>6590</v>
-      </c>
-    </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="B107" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C107" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D107" s="6">
+        <f t="shared" ref="D107:D112" si="13">D106+C107</f>
+        <v>6590</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="B107" s="4" t="s">
+      <c r="B108" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C107" s="5">
+      <c r="C108" s="5">
         <v>7000</v>
       </c>
-      <c r="D107" s="6">
+      <c r="D108" s="6">
         <f t="shared" si="13"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B108" s="4" t="s">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B109" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C108" s="5">
+      <c r="C109" s="5">
         <v>-10000</v>
       </c>
-      <c r="D108" s="6">
+      <c r="D109" s="6">
         <f t="shared" si="13"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="9" t="s">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="B109" s="4" t="s">
+      <c r="B110" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C109" s="5">
+      <c r="C110" s="5">
         <v>2000</v>
       </c>
-      <c r="D109" s="6">
+      <c r="D110" s="6">
         <f t="shared" si="13"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="9" t="s">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="B110" s="4" t="s">
+      <c r="B111" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C110" s="5">
+      <c r="C111" s="5">
         <v>8000</v>
       </c>
-      <c r="D110" s="6">
+      <c r="D111" s="6">
         <f t="shared" si="13"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B111" s="4" t="s">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B112" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C111" s="5">
+      <c r="C112" s="5">
         <v>-10000</v>
       </c>
-      <c r="D111" s="6">
+      <c r="D112" s="6">
         <f t="shared" si="13"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="9" t="s">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="B112" s="4" t="s">
+      <c r="B113" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C112" s="5">
+      <c r="C113" s="5">
         <v>2000</v>
       </c>
-      <c r="D112" s="6">
-        <f>D111+C112</f>
+      <c r="D113" s="6">
+        <f>D112+C113</f>
         <v>5590</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B114" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C114" s="5">
+        <v>5000</v>
+      </c>
+      <c r="D114" s="6">
+        <f>D113+C114</f>
+        <v>10590</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B115" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C115" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D115" s="6">
+        <f>D114+C115</f>
+        <v>590</v>
       </c>
     </row>
   </sheetData>
@@ -3078,10 +3129,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A15:B17"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3089,18 +3140,50 @@
     <col min="1" max="1" width="40" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B3">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B4">
+        <v>400</v>
+      </c>
+    </row>
     <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>119</v>
       </c>
       <c r="B15" s="17">
-        <f>SUM(B2:B5)</f>
-        <v>0</v>
+        <f>SUM(B1:B13)</f>
+        <v>2500</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16">
-        <v>0</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -3109,7 +3192,7 @@
       </c>
       <c r="B17">
         <f>B16-B15</f>
-        <v>0</v>
+        <v>2500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
duy lay tien loi ngay 01
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="147">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -930,11 +930,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K115"/>
+  <dimension ref="A1:K116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I26" sqref="I26"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2569,6 +2569,21 @@
       <c r="D115" s="6">
         <f>D114+C115</f>
         <v>590</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="9">
+        <v>45296</v>
+      </c>
+      <c r="B116" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C116" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D116" s="6">
+        <f>D115+C116</f>
+        <v>2590</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ha tra no 500k
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CÔ DIỄM" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="148">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -2772,11 +2772,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2940,6 +2940,21 @@
       <c r="D9" s="4">
         <f>D8+C9</f>
         <v>6000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>45632</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="5">
+        <v>-500</v>
+      </c>
+      <c r="D10" s="4">
+        <f>D9+C10</f>
+        <v>5500</v>
       </c>
     </row>
   </sheetData>
@@ -3190,7 +3205,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Duy lay tien loi co diem
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="149">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -463,6 +463,9 @@
   </si>
   <si>
     <t>Lì</t>
+  </si>
+  <si>
+    <t>13/06/2024</t>
   </si>
 </sst>
 </file>
@@ -933,11 +936,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K118"/>
+  <dimension ref="A1:K119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I37" sqref="I37"/>
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D120" sqref="D120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2620,6 +2623,21 @@
       <c r="D118" s="6">
         <f t="shared" si="14"/>
         <v>1590</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B119" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C119" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D119" s="6">
+        <f>D118+C119</f>
+        <v>3590</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
duy lay tien loi co diem ngay 30,31
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="CÔ DIỄM" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="155">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -478,6 +478,12 @@
   </si>
   <si>
     <t>Thạch</t>
+  </si>
+  <si>
+    <t>30/06/2024</t>
+  </si>
+  <si>
+    <t>Duy lấy tiền lời ngày 30,31 = 12tr</t>
   </si>
 </sst>
 </file>
@@ -948,11 +954,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K123"/>
+  <dimension ref="A1:K126"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D124" sqref="D124"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1028,8 +1034,8 @@
         <v>20</v>
       </c>
       <c r="J3" s="4">
-        <f>SUM(I3:I54)</f>
-        <v>370</v>
+        <f>SUM(I3:I55)</f>
+        <v>380</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1280,38 +1286,40 @@
       <c r="K23" s="15"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="5">
-        <v>3000</v>
-      </c>
-      <c r="D24" s="6">
-        <f>D17+C24</f>
-        <v>8490</v>
-      </c>
       <c r="H24" s="9" t="s">
-        <v>12</v>
+        <v>153</v>
       </c>
       <c r="I24" s="5">
         <v>10</v>
       </c>
+      <c r="K24" s="15" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="5">
+        <v>3000</v>
+      </c>
+      <c r="D25" s="6">
+        <f>D17+C25</f>
+        <v>8490</v>
+      </c>
       <c r="H25" s="9" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="I25" s="5">
         <v>10</v>
       </c>
-      <c r="K25" s="15"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H26" s="9" t="s">
-        <v>146</v>
+        <v>43</v>
       </c>
       <c r="I26" s="5">
         <v>10</v>
@@ -1319,8 +1327,8 @@
       <c r="K26" s="15"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H27" s="9">
-        <v>45293</v>
+      <c r="H27" s="9" t="s">
+        <v>146</v>
       </c>
       <c r="I27" s="5">
         <v>10</v>
@@ -1329,7 +1337,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H28" s="9">
-        <v>45294</v>
+        <v>45293</v>
       </c>
       <c r="I28" s="5">
         <v>10</v>
@@ -1337,59 +1345,46 @@
       <c r="K28" s="15"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C29" s="5">
-        <v>4400</v>
-      </c>
-      <c r="D29" s="6">
-        <f>D24+C29</f>
-        <v>12890</v>
-      </c>
       <c r="H29" s="9">
-        <v>44964</v>
+        <v>45294</v>
       </c>
       <c r="I29" s="5">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K29" s="15"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="5">
+        <v>4400</v>
+      </c>
+      <c r="D30" s="6">
+        <f>D25+C30</f>
+        <v>12890</v>
+      </c>
+      <c r="H30" s="9">
+        <v>44964</v>
+      </c>
+      <c r="I30" s="5">
+        <v>20</v>
+      </c>
+      <c r="K30" s="15"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C31" s="5">
         <v>-10000</v>
       </c>
-      <c r="D30" s="6">
-        <f>D29+C30</f>
+      <c r="D31" s="6">
+        <f>D30+C31</f>
         <v>2890</v>
       </c>
-      <c r="H30" s="9">
+      <c r="H31" s="9">
         <v>44966</v>
-      </c>
-      <c r="I30" s="5">
-        <v>10</v>
-      </c>
-      <c r="K30" s="15"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="9">
-        <v>44967</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C31" s="5">
-        <v>1600</v>
-      </c>
-      <c r="D31" s="6">
-        <f t="shared" ref="D31:D38" si="1">D30+C31</f>
-        <v>4490</v>
-      </c>
-      <c r="H31" s="9">
-        <v>44968</v>
       </c>
       <c r="I31" s="5">
         <v>10</v>
@@ -1397,510 +1392,517 @@
       <c r="K31" s="15"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="9">
+        <v>44967</v>
+      </c>
       <c r="B32" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" s="5">
+        <v>1600</v>
+      </c>
+      <c r="D32" s="6">
+        <f t="shared" ref="D32:D39" si="1">D31+C32</f>
+        <v>4490</v>
+      </c>
+      <c r="H32" s="9">
+        <v>44968</v>
+      </c>
+      <c r="I32" s="5">
+        <v>10</v>
+      </c>
+      <c r="K32" s="15"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C33" s="5">
         <v>3000</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D33" s="6">
         <f t="shared" si="1"/>
         <v>7490</v>
       </c>
-      <c r="H32" s="9">
+      <c r="H33" s="9">
         <v>44969</v>
       </c>
-      <c r="I32" s="5">
+      <c r="I33" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B34" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C34" s="5">
         <v>2000</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D34" s="6">
         <f t="shared" si="1"/>
         <v>9490</v>
       </c>
-      <c r="H33" s="9">
+      <c r="H34" s="9">
         <v>45334</v>
       </c>
-      <c r="I33" s="5">
+      <c r="I34" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B35" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C35" s="5">
         <v>3000</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D35" s="6">
         <f t="shared" si="1"/>
         <v>12490</v>
       </c>
-      <c r="H34" s="9">
+      <c r="H35" s="9">
         <v>45325</v>
       </c>
-      <c r="I34" s="5">
+      <c r="I35" s="5">
         <v>10</v>
       </c>
-      <c r="K34" s="15"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B35" s="4" t="s">
+      <c r="K35" s="15"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C35" s="5">
+      <c r="C36" s="5">
         <v>-10000</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D36" s="6">
         <f t="shared" si="1"/>
         <v>2490</v>
       </c>
-      <c r="H35" s="9">
+      <c r="H36" s="9">
         <v>45326</v>
       </c>
-      <c r="I35" s="5">
+      <c r="I36" s="5">
         <v>10</v>
       </c>
-      <c r="K35" s="15"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="9" t="s">
+      <c r="K36" s="15"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B37" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C36" s="5">
+      <c r="C37" s="5">
         <v>4960</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D37" s="6">
         <f t="shared" si="1"/>
         <v>7450</v>
       </c>
-      <c r="H36" s="9">
+      <c r="H37" s="9">
         <v>45327</v>
       </c>
-      <c r="I36" s="5">
+      <c r="I37" s="5">
         <v>10</v>
       </c>
-      <c r="K36" s="15"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="9" t="s">
+      <c r="K37" s="15"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B38" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C37" s="5">
+      <c r="C38" s="5">
         <v>4000</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D38" s="6">
         <f t="shared" si="1"/>
         <v>11450</v>
       </c>
-      <c r="H37" s="9">
+      <c r="H38" s="9">
         <v>45328</v>
       </c>
-      <c r="I37" s="5">
+      <c r="I38" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B38" s="4" t="s">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B39" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C38" s="5">
+      <c r="C39" s="5">
         <v>-10000</v>
       </c>
-      <c r="D38" s="6">
+      <c r="D39" s="6">
         <f t="shared" si="1"/>
         <v>1450</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B39" s="4" t="s">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C39" s="5">
+      <c r="C40" s="5">
         <v>7640</v>
       </c>
-      <c r="D39" s="6">
-        <f t="shared" ref="D39:D44" si="2">D38+C39</f>
+      <c r="D40" s="6">
+        <f t="shared" ref="D40:D45" si="2">D39+C40</f>
         <v>9090</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="9">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="9">
         <v>44968</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B41" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="5">
+      <c r="C41" s="5">
         <v>3000</v>
       </c>
-      <c r="D40" s="6">
+      <c r="D41" s="6">
         <f t="shared" si="2"/>
         <v>12090</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B41" s="4" t="s">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B42" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C41" s="5">
+      <c r="C42" s="5">
         <v>-10000</v>
       </c>
-      <c r="D41" s="6">
+      <c r="D42" s="6">
         <f t="shared" si="2"/>
         <v>2090</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="9">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="9">
         <v>44996</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B43" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C43" s="5">
         <v>800</v>
       </c>
-      <c r="D42" s="6">
+      <c r="D43" s="6">
         <f t="shared" si="2"/>
         <v>2890</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="9" t="s">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B44" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C43" s="5">
+      <c r="C44" s="5">
         <v>2000</v>
       </c>
-      <c r="D43" s="6">
+      <c r="D44" s="6">
         <f t="shared" si="2"/>
         <v>4890</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="9" t="s">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B45" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C45" s="5">
         <v>4000</v>
       </c>
-      <c r="D44" s="6">
+      <c r="D45" s="6">
         <f t="shared" si="2"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="9" t="s">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B46" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C45" s="5">
+      <c r="C46" s="5">
         <v>4000</v>
       </c>
-      <c r="D45" s="6">
-        <f t="shared" ref="D45:D50" si="3">D44+C45</f>
+      <c r="D46" s="6">
+        <f t="shared" ref="D46:D51" si="3">D45+C46</f>
         <v>12890</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B46" s="4" t="s">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B47" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C46" s="5">
+      <c r="C47" s="5">
         <v>5000</v>
       </c>
-      <c r="D46" s="6">
+      <c r="D47" s="6">
         <f t="shared" si="3"/>
         <v>17890</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B47" s="4" t="s">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B48" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C48" s="5">
         <v>-10000</v>
       </c>
-      <c r="D47" s="6">
+      <c r="D48" s="6">
         <f t="shared" si="3"/>
         <v>7890</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="9">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="9">
         <v>44969</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B49" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C48" s="5">
+      <c r="C49" s="5">
         <v>900</v>
       </c>
-      <c r="D48" s="6">
+      <c r="D49" s="6">
         <f t="shared" si="3"/>
         <v>8790</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B49" s="4" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B50" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C49" s="5">
+      <c r="C50" s="5">
         <v>4000</v>
       </c>
-      <c r="D49" s="6">
+      <c r="D50" s="6">
         <f t="shared" si="3"/>
         <v>12790</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B50" s="4" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B51" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C50" s="5">
+      <c r="C51" s="5">
         <v>-10000</v>
       </c>
-      <c r="D50" s="6">
+      <c r="D51" s="6">
         <f t="shared" si="3"/>
         <v>2790</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C51" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D51" s="6">
-        <f t="shared" ref="D51:D58" si="4">D50+C51</f>
-        <v>4790</v>
-      </c>
-    </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C52" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D52" s="6">
+        <f t="shared" ref="D52:D59" si="4">D51+C52</f>
+        <v>4790</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B53" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C52" s="5">
+      <c r="C53" s="5">
         <v>700</v>
       </c>
-      <c r="D52" s="6">
+      <c r="D53" s="6">
         <f t="shared" si="4"/>
         <v>5490</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B53" s="4" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B54" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C53" s="5">
+      <c r="C54" s="5">
         <v>4000</v>
       </c>
-      <c r="D53" s="6">
+      <c r="D54" s="6">
         <f t="shared" si="4"/>
         <v>9490</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="9" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B55" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C54" s="5">
+      <c r="C55" s="5">
         <v>600</v>
       </c>
-      <c r="D54" s="6">
+      <c r="D55" s="6">
         <f t="shared" si="4"/>
         <v>10090</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="4" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B56" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C55" s="5">
+      <c r="C56" s="5">
         <v>-10000</v>
       </c>
-      <c r="D55" s="6">
+      <c r="D56" s="6">
         <f t="shared" si="4"/>
         <v>90</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="9" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B57" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C56" s="5">
+      <c r="C57" s="5">
         <f>700+5000+300+600+400+1000+800</f>
         <v>8800</v>
       </c>
-      <c r="D56" s="6">
+      <c r="D57" s="6">
         <f t="shared" si="4"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B57" s="4" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B58" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C57" s="5">
+      <c r="C58" s="5">
         <v>6000</v>
       </c>
-      <c r="D57" s="6">
+      <c r="D58" s="6">
         <f t="shared" si="4"/>
         <v>14890</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B58" s="4" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B59" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C58" s="5">
+      <c r="C59" s="5">
         <v>-10000</v>
       </c>
-      <c r="D58" s="6">
+      <c r="D59" s="6">
         <f t="shared" si="4"/>
         <v>4890</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="9" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B60" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C59" s="5">
+      <c r="C60" s="5">
         <v>500</v>
       </c>
-      <c r="D59" s="6">
-        <f t="shared" ref="D59:D64" si="5">D58+C59</f>
+      <c r="D60" s="6">
+        <f t="shared" ref="D60:D65" si="5">D59+C60</f>
         <v>5390</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="9">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="9">
         <v>45323</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B61" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C60" s="5">
+      <c r="C61" s="5">
         <v>700</v>
       </c>
-      <c r="D60" s="6">
+      <c r="D61" s="6">
         <f t="shared" si="5"/>
         <v>6090</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B61" s="4" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B62" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C61" s="5">
+      <c r="C62" s="5">
         <v>1500</v>
       </c>
-      <c r="D61" s="6">
+      <c r="D62" s="6">
         <f t="shared" si="5"/>
         <v>7590</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B62" s="4" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B63" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C62" s="5">
+      <c r="C63" s="5">
         <v>5000</v>
       </c>
-      <c r="D62" s="6">
+      <c r="D63" s="6">
         <f t="shared" si="5"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B63" s="4" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B64" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C63" s="5">
+      <c r="C64" s="5">
         <v>-10000</v>
       </c>
-      <c r="D63" s="6">
+      <c r="D64" s="6">
         <f t="shared" si="5"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="9" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B65" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C64" s="5">
+      <c r="C65" s="5">
         <v>2000</v>
       </c>
-      <c r="D64" s="6">
+      <c r="D65" s="6">
         <f t="shared" si="5"/>
         <v>4590</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="9">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="9">
         <v>45474</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C65" s="5">
-        <v>700</v>
-      </c>
-      <c r="D65" s="6">
-        <f t="shared" ref="D65:D70" si="6">D64+C65</f>
-        <v>5290</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="9" t="s">
-        <v>82</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>77</v>
@@ -1909,418 +1911,418 @@
         <v>700</v>
       </c>
       <c r="D66" s="6">
+        <f t="shared" ref="D66:D71" si="6">D65+C66</f>
+        <v>5290</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C67" s="5">
+        <v>700</v>
+      </c>
+      <c r="D67" s="6">
         <f t="shared" si="6"/>
         <v>5990</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="9" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B68" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C67" s="5">
+      <c r="C68" s="5">
         <v>700</v>
       </c>
-      <c r="D67" s="6">
+      <c r="D68" s="6">
         <f t="shared" si="6"/>
         <v>6690</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="9" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B69" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C68" s="5">
+      <c r="C69" s="5">
         <v>4000</v>
       </c>
-      <c r="D68" s="6">
+      <c r="D69" s="6">
         <f t="shared" si="6"/>
         <v>10690</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B69" s="4" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B70" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C69" s="5">
+      <c r="C70" s="5">
         <v>-10000</v>
       </c>
-      <c r="D69" s="6">
+      <c r="D70" s="6">
         <f t="shared" si="6"/>
         <v>690</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="9" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B71" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C70" s="5">
+      <c r="C71" s="5">
         <v>1000</v>
       </c>
-      <c r="D70" s="6">
+      <c r="D71" s="6">
         <f t="shared" si="6"/>
         <v>1690</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="9" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B72" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C71" s="5">
+      <c r="C72" s="5">
         <v>7000</v>
       </c>
-      <c r="D71" s="6">
-        <f t="shared" ref="D71:D76" si="7">D70+C71</f>
+      <c r="D72" s="6">
+        <f t="shared" ref="D72:D77" si="7">D71+C72</f>
         <v>8690</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B72" s="4" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B73" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C72" s="5">
+      <c r="C73" s="5">
         <v>10000</v>
       </c>
-      <c r="D72" s="6">
+      <c r="D73" s="6">
         <f t="shared" si="7"/>
         <v>18690</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B73" s="4" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C73" s="5">
+      <c r="C74" s="5">
         <v>-10000</v>
       </c>
-      <c r="D73" s="6">
+      <c r="D74" s="6">
         <f t="shared" si="7"/>
         <v>8690</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="9">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="9">
         <v>45293</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B75" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C74" s="5">
+      <c r="C75" s="5">
         <v>1700</v>
       </c>
-      <c r="D74" s="6">
+      <c r="D75" s="6">
         <f t="shared" si="7"/>
         <v>10390</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B75" s="4" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B76" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C75" s="5">
+      <c r="C76" s="5">
         <v>-10000</v>
       </c>
-      <c r="D75" s="6">
+      <c r="D76" s="6">
         <f t="shared" si="7"/>
         <v>390</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="9">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="9">
         <v>45324</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B77" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C76" s="5">
+      <c r="C77" s="5">
         <v>6000</v>
       </c>
-      <c r="D76" s="6">
+      <c r="D77" s="6">
         <f t="shared" si="7"/>
         <v>6390</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="B77" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C77" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D77" s="6">
-        <f t="shared" ref="D77:D82" si="8">D76+C77</f>
-        <v>8390</v>
-      </c>
-    </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C78" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D78" s="6">
+        <f t="shared" ref="D78:D83" si="8">D77+C78</f>
+        <v>8390</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B79" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C78" s="5">
+      <c r="C79" s="5">
         <v>5000</v>
       </c>
-      <c r="D78" s="6">
+      <c r="D79" s="6">
         <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B79" s="4" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B80" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C79" s="5">
+      <c r="C80" s="5">
         <v>-10000</v>
       </c>
-      <c r="D79" s="6">
+      <c r="D80" s="6">
         <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="9" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B81" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C80" s="5">
+      <c r="C81" s="5">
         <v>1000</v>
       </c>
-      <c r="D80" s="6">
+      <c r="D81" s="6">
         <f t="shared" si="8"/>
         <v>4390</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="9">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="9">
         <v>45294</v>
       </c>
-      <c r="B81" s="4" t="s">
+      <c r="B82" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C81" s="5">
+      <c r="C82" s="5">
         <v>9000</v>
       </c>
-      <c r="D81" s="6">
+      <c r="D82" s="6">
         <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B82" s="4" t="s">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B83" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C82" s="5">
+      <c r="C83" s="5">
         <v>-10000</v>
       </c>
-      <c r="D82" s="6">
+      <c r="D83" s="6">
         <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B83" s="4" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B84" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C83" s="5">
+      <c r="C84" s="5">
         <v>2000</v>
       </c>
-      <c r="D83" s="6">
-        <f t="shared" ref="D83:D88" si="9">D82+C83</f>
+      <c r="D84" s="6">
+        <f t="shared" ref="D84:D89" si="9">D83+C84</f>
         <v>5390</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="9">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="9">
         <v>45325</v>
       </c>
-      <c r="B84" s="4" t="s">
+      <c r="B85" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C84" s="5">
+      <c r="C85" s="5">
         <v>6000</v>
       </c>
-      <c r="D84" s="6">
+      <c r="D85" s="6">
         <f t="shared" si="9"/>
         <v>11390</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B85" s="4" t="s">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B86" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C85" s="5">
+      <c r="C86" s="5">
         <v>-10000</v>
       </c>
-      <c r="D85" s="6">
+      <c r="D86" s="6">
         <f t="shared" si="9"/>
         <v>1390</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="9">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="9">
         <v>45507</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="B87" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C86" s="5">
+      <c r="C87" s="5">
         <v>400</v>
       </c>
-      <c r="D86" s="6">
+      <c r="D87" s="6">
         <f t="shared" si="9"/>
         <v>1790</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="9" t="s">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="B87" s="4" t="s">
+      <c r="B88" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C87" s="5">
+      <c r="C88" s="5">
         <v>2000</v>
       </c>
-      <c r="D87" s="6">
+      <c r="D88" s="6">
         <f t="shared" si="9"/>
         <v>3790</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="9" t="s">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="B88" s="4" t="s">
+      <c r="B89" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C88" s="5">
+      <c r="C89" s="5">
         <v>6000</v>
       </c>
-      <c r="D88" s="6">
+      <c r="D89" s="6">
         <f t="shared" si="9"/>
         <v>9790</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="9" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="B89" s="4" t="s">
+      <c r="B90" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C89" s="5">
+      <c r="C90" s="5">
         <v>1000</v>
       </c>
-      <c r="D89" s="6">
-        <f t="shared" ref="D89:D94" si="10">D88+C89</f>
+      <c r="D90" s="6">
+        <f t="shared" ref="D90:D95" si="10">D89+C90</f>
         <v>10790</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B90" s="4" t="s">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B91" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C90" s="5">
+      <c r="C91" s="5">
         <v>-10000</v>
       </c>
-      <c r="D90" s="6">
+      <c r="D91" s="6">
         <f t="shared" si="10"/>
         <v>790</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="9" t="s">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="B91" s="4" t="s">
+      <c r="B92" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C91" s="5">
+      <c r="C92" s="5">
         <v>800</v>
       </c>
-      <c r="D91" s="6">
+      <c r="D92" s="6">
         <f t="shared" si="10"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="9" t="s">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="B92" s="4" t="s">
+      <c r="B93" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C92" s="5">
+      <c r="C93" s="5">
         <v>5000</v>
       </c>
-      <c r="D92" s="6">
+      <c r="D93" s="6">
         <f t="shared" si="10"/>
         <v>6590</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="9" t="s">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="B93" s="4" t="s">
+      <c r="B94" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C93" s="5">
+      <c r="C94" s="5">
         <v>6000</v>
       </c>
-      <c r="D93" s="6">
+      <c r="D94" s="6">
         <f t="shared" si="10"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B94" s="4" t="s">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B95" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C94" s="5">
+      <c r="C95" s="5">
         <v>-10000</v>
       </c>
-      <c r="D94" s="6">
+      <c r="D95" s="6">
         <f t="shared" si="10"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="9" t="s">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="9" t="s">
         <v>124</v>
-      </c>
-      <c r="B95" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C95" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D95" s="6">
-        <f t="shared" ref="D95:D101" si="11">D94+C95</f>
-        <v>4590</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="9">
-        <v>45295</v>
       </c>
       <c r="B96" s="4" t="s">
         <v>65</v>
@@ -2329,380 +2331,422 @@
         <v>2000</v>
       </c>
       <c r="D96" s="6">
+        <f t="shared" ref="D96:D102" si="11">D95+C96</f>
+        <v>4590</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="9">
+        <v>45295</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C97" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D97" s="6">
         <f t="shared" si="11"/>
         <v>6590</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="9">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="9">
         <v>45326</v>
       </c>
-      <c r="B97" s="4" t="s">
+      <c r="B98" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C97" s="5">
+      <c r="C98" s="5">
         <v>7000</v>
       </c>
-      <c r="D97" s="6">
+      <c r="D98" s="6">
         <f t="shared" si="11"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B98" s="4" t="s">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B99" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C98" s="5">
+      <c r="C99" s="5">
         <v>-10000</v>
       </c>
-      <c r="D98" s="6">
+      <c r="D99" s="6">
         <f t="shared" si="11"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="9" t="s">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="B99" s="4" t="s">
+      <c r="B100" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C99" s="5">
+      <c r="C100" s="5">
         <v>2000</v>
       </c>
-      <c r="D99" s="6">
+      <c r="D100" s="6">
         <f t="shared" si="11"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="9" t="s">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="B100" s="4" t="s">
+      <c r="B101" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C100" s="5">
+      <c r="C101" s="5">
         <v>6000</v>
       </c>
-      <c r="D100" s="6">
+      <c r="D101" s="6">
         <f t="shared" si="11"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B101" s="4" t="s">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B102" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C101" s="5">
+      <c r="C102" s="5">
         <v>-10000</v>
       </c>
-      <c r="D101" s="6">
+      <c r="D102" s="6">
         <f t="shared" si="11"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="B102" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C102" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D102" s="6">
-        <f t="shared" ref="D102:D107" si="12">D101+C102</f>
-        <v>3590</v>
-      </c>
-    </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C103" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D103" s="6">
+        <f t="shared" ref="D103:D108" si="12">D102+C103</f>
+        <v>3590</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="B103" s="4" t="s">
+      <c r="B104" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C103" s="5">
+      <c r="C104" s="5">
         <v>7000</v>
       </c>
-      <c r="D103" s="6">
+      <c r="D104" s="6">
         <f t="shared" si="12"/>
         <v>10590</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B104" s="4" t="s">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B105" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C104" s="5">
+      <c r="C105" s="5">
         <v>-10000</v>
       </c>
-      <c r="D104" s="6">
+      <c r="D105" s="6">
         <f t="shared" si="12"/>
         <v>590</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="9">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="9">
         <v>45327</v>
       </c>
-      <c r="B105" s="4" t="s">
+      <c r="B106" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C105" s="5">
+      <c r="C106" s="5">
         <v>12000</v>
       </c>
-      <c r="D105" s="6">
+      <c r="D106" s="6">
         <f t="shared" si="12"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B106" s="4" t="s">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B107" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C106" s="5">
+      <c r="C107" s="5">
         <v>-10000</v>
       </c>
-      <c r="D106" s="6">
+      <c r="D107" s="6">
         <f t="shared" si="12"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B107" s="4" t="s">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B108" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C107" s="5">
+      <c r="C108" s="5">
         <v>2000</v>
       </c>
-      <c r="D107" s="6">
+      <c r="D108" s="6">
         <f t="shared" si="12"/>
         <v>4590</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="B108" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C108" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D108" s="6">
-        <f t="shared" ref="D108:D113" si="13">D107+C108</f>
-        <v>6590</v>
-      </c>
-    </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C109" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D109" s="6">
+        <f t="shared" ref="D109:D114" si="13">D108+C109</f>
+        <v>6590</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="B109" s="4" t="s">
+      <c r="B110" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C109" s="5">
+      <c r="C110" s="5">
         <v>7000</v>
       </c>
-      <c r="D109" s="6">
+      <c r="D110" s="6">
         <f t="shared" si="13"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B110" s="4" t="s">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B111" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C110" s="5">
+      <c r="C111" s="5">
         <v>-10000</v>
       </c>
-      <c r="D110" s="6">
+      <c r="D111" s="6">
         <f t="shared" si="13"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="9" t="s">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="B111" s="4" t="s">
+      <c r="B112" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C111" s="5">
+      <c r="C112" s="5">
         <v>2000</v>
       </c>
-      <c r="D111" s="6">
+      <c r="D112" s="6">
         <f t="shared" si="13"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="9" t="s">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="B112" s="4" t="s">
+      <c r="B113" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C112" s="5">
+      <c r="C113" s="5">
         <v>8000</v>
       </c>
-      <c r="D112" s="6">
+      <c r="D113" s="6">
         <f t="shared" si="13"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B113" s="4" t="s">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B114" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C113" s="5">
+      <c r="C114" s="5">
         <v>-10000</v>
       </c>
-      <c r="D113" s="6">
+      <c r="D114" s="6">
         <f t="shared" si="13"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="9" t="s">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="B114" s="4" t="s">
+      <c r="B115" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C114" s="5">
+      <c r="C115" s="5">
         <v>2000</v>
       </c>
-      <c r="D114" s="6">
-        <f t="shared" ref="D114:D119" si="14">D113+C114</f>
+      <c r="D115" s="6">
+        <f t="shared" ref="D115:D120" si="14">D114+C115</f>
         <v>5590</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B115" s="4" t="s">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B116" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C115" s="5">
+      <c r="C116" s="5">
         <v>5000</v>
       </c>
-      <c r="D115" s="6">
+      <c r="D116" s="6">
         <f t="shared" si="14"/>
         <v>10590</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B116" s="4" t="s">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B117" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C116" s="5">
+      <c r="C117" s="5">
         <v>-10000</v>
       </c>
-      <c r="D116" s="6">
+      <c r="D117" s="6">
         <f t="shared" si="14"/>
         <v>590</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="9">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="9">
         <v>45297</v>
       </c>
-      <c r="B117" s="4" t="s">
+      <c r="B118" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C117" s="5">
+      <c r="C118" s="5">
         <v>2000</v>
       </c>
-      <c r="D117" s="6">
+      <c r="D118" s="6">
         <f t="shared" si="14"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="9">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="9">
         <v>45328</v>
       </c>
-      <c r="B118" s="4" t="s">
+      <c r="B119" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C118" s="5">
+      <c r="C119" s="5">
         <v>9000</v>
       </c>
-      <c r="D118" s="6">
+      <c r="D119" s="6">
         <f t="shared" si="14"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B119" s="4" t="s">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B120" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C119" s="5">
+      <c r="C120" s="5">
         <v>-10000</v>
       </c>
-      <c r="D119" s="6">
+      <c r="D120" s="6">
         <f t="shared" si="14"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="B120" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C120" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D120" s="6">
-        <f>D119+C120</f>
-        <v>3590</v>
-      </c>
-    </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>139</v>
+        <v>65</v>
       </c>
       <c r="C121" s="5">
-        <v>8000</v>
+        <v>2000</v>
       </c>
       <c r="D121" s="6">
         <f>D120+C121</f>
-        <v>11590</v>
+        <v>3590</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="9" t="s">
+        <v>149</v>
+      </c>
       <c r="B122" s="4" t="s">
-        <v>20</v>
+        <v>139</v>
       </c>
       <c r="C122" s="5">
-        <v>-10000</v>
+        <v>8000</v>
       </c>
       <c r="D122" s="6">
         <f>D121+C122</f>
-        <v>1590</v>
+        <v>11590</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="9" t="s">
-        <v>151</v>
-      </c>
       <c r="B123" s="4" t="s">
-        <v>65</v>
+        <v>20</v>
       </c>
       <c r="C123" s="5">
-        <v>2000</v>
+        <v>-10000</v>
       </c>
       <c r="D123" s="6">
         <f>D122+C123</f>
+        <v>1590</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="B124" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C124" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D124" s="6">
+        <f>D123+C124</f>
         <v>3590</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="B125" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C125" s="5">
+        <v>12000</v>
+      </c>
+      <c r="D125" s="6">
+        <f>D124+C125</f>
+        <v>15590</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B126" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C126" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D126" s="6">
+        <f>D125+C126</f>
+        <v>5590</v>
       </c>
     </row>
   </sheetData>
@@ -3174,7 +3218,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
duy chuyen cho co diem 1tr
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="156">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -484,6 +484,9 @@
   </si>
   <si>
     <t>Duy lấy tiền lời ngày 30,31 = 12tr</t>
+  </si>
+  <si>
+    <t>Duy chuyển cho cô diễm 1tr</t>
   </si>
 </sst>
 </file>
@@ -954,11 +957,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K126"/>
+  <dimension ref="A1:K127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K24" sqref="K24"/>
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H133" sqref="H133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2676,7 +2679,7 @@
         <v>2000</v>
       </c>
       <c r="D121" s="6">
-        <f>D120+C121</f>
+        <f t="shared" ref="D121:D126" si="15">D120+C121</f>
         <v>3590</v>
       </c>
     </row>
@@ -2691,7 +2694,7 @@
         <v>8000</v>
       </c>
       <c r="D122" s="6">
-        <f>D121+C122</f>
+        <f t="shared" si="15"/>
         <v>11590</v>
       </c>
     </row>
@@ -2703,7 +2706,7 @@
         <v>-10000</v>
       </c>
       <c r="D123" s="6">
-        <f>D122+C123</f>
+        <f t="shared" si="15"/>
         <v>1590</v>
       </c>
     </row>
@@ -2718,7 +2721,7 @@
         <v>2000</v>
       </c>
       <c r="D124" s="6">
-        <f>D123+C124</f>
+        <f t="shared" si="15"/>
         <v>3590</v>
       </c>
     </row>
@@ -2733,7 +2736,7 @@
         <v>12000</v>
       </c>
       <c r="D125" s="6">
-        <f>D124+C125</f>
+        <f t="shared" si="15"/>
         <v>15590</v>
       </c>
     </row>
@@ -2745,8 +2748,23 @@
         <v>-10000</v>
       </c>
       <c r="D126" s="6">
-        <f>D125+C126</f>
+        <f t="shared" si="15"/>
         <v>5590</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="9">
+        <v>45298</v>
+      </c>
+      <c r="B127" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C127" s="5">
+        <v>1000</v>
+      </c>
+      <c r="D127" s="6">
+        <f>D126+C127</f>
+        <v>6590</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
duy chuyen them cho co diem 1tr
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -486,7 +486,7 @@
     <t>Duy lấy tiền lời ngày 30,31 = 12tr</t>
   </si>
   <si>
-    <t>Duy chuyển cho cô diễm 1tr</t>
+    <t>Duy chuyển cho cô diễm 2tr</t>
   </si>
 </sst>
 </file>
@@ -960,8 +960,8 @@
   <dimension ref="A1:K127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H133" sqref="H133"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C128" sqref="C128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2760,11 +2760,11 @@
         <v>155</v>
       </c>
       <c r="C127" s="5">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="D127" s="6">
         <f>D126+C127</f>
-        <v>6590</v>
+        <v>7590</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
duy chuyen cho co diem them 1tr
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="CÔ DIỄM" sheetId="1" r:id="rId1"/>
@@ -959,7 +959,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K127"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C128" sqref="C128"/>
     </sheetView>
@@ -3236,8 +3236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3256,7 +3256,7 @@
         <v>108</v>
       </c>
       <c r="B10">
-        <v>360000</v>
+        <v>380000</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -3345,7 +3345,7 @@
       </c>
       <c r="B32">
         <f>SUM(B10:B29)</f>
-        <v>471580</v>
+        <v>491580</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
duy chuyen them cho co diem 500k
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -492,7 +492,7 @@
     <t>Duy lấy tiền lời 10tr</t>
   </si>
   <si>
-    <t>Duy chuyển cho co Diem 1.5tr</t>
+    <t>Duy chuyển cho co Diem 2tr</t>
   </si>
 </sst>
 </file>
@@ -966,8 +966,8 @@
   <dimension ref="A1:K130"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D131" sqref="D131"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H133" sqref="H133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2814,11 +2814,11 @@
         <v>157</v>
       </c>
       <c r="C130" s="5">
-        <v>1500</v>
+        <v>2000</v>
       </c>
       <c r="D130" s="6">
         <f>D129+C130</f>
-        <v>9090</v>
+        <v>9590</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
duy thanh toan thue kho + chuyen cho co diem 500k
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="173">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -529,6 +529,15 @@
   </si>
   <si>
     <t>01/07/2024</t>
+  </si>
+  <si>
+    <t>07/07/2024</t>
+  </si>
+  <si>
+    <t>Duy thanh toán tiền thuê kho đến hết tháng 12</t>
+  </si>
+  <si>
+    <t>Duy chuyển cho cô diễm 500k</t>
   </si>
 </sst>
 </file>
@@ -692,13 +701,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1005,11 +1014,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K159"/>
+  <dimension ref="A1:K164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K39" sqref="K39"/>
+      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D133" sqref="D133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1019,7 +1028,7 @@
     <col min="3" max="3" width="20.5703125" style="5" customWidth="1"/>
     <col min="4" max="4" width="25.5703125" style="6" customWidth="1"/>
     <col min="5" max="7" width="9.140625" style="6"/>
-    <col min="8" max="8" width="12.7109375" style="19" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="18" customWidth="1"/>
     <col min="9" max="9" width="29.5703125" style="5" customWidth="1"/>
     <col min="10" max="10" width="14.28515625" style="4" customWidth="1"/>
     <col min="11" max="11" width="26" style="6" customWidth="1"/>
@@ -1039,10 +1048,10 @@
       <c r="D1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="18"/>
+      <c r="I1" s="20"/>
       <c r="J1" s="16"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1055,7 +1064,7 @@
       <c r="C2" s="5">
         <v>1930</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="19" t="s">
         <v>2</v>
       </c>
       <c r="I2" s="3" t="s">
@@ -1078,7 +1087,7 @@
       <c r="D3" s="6">
         <v>3930</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="H3" s="18" t="s">
         <v>6</v>
       </c>
       <c r="I3" s="5">
@@ -1100,7 +1109,7 @@
         <f>C4+D3</f>
         <v>18490</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="18" t="s">
         <v>7</v>
       </c>
       <c r="I4" s="5">
@@ -1118,7 +1127,7 @@
         <f t="shared" ref="D5:D17" si="0">D4+C5</f>
         <v>8490</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="18" t="s">
         <v>8</v>
       </c>
       <c r="I5" s="5">
@@ -1139,7 +1148,7 @@
         <f t="shared" si="0"/>
         <v>10490</v>
       </c>
-      <c r="H6" s="19" t="s">
+      <c r="H6" s="18" t="s">
         <v>9</v>
       </c>
       <c r="I6" s="5">
@@ -1147,7 +1156,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H7" s="19" t="s">
+      <c r="H7" s="18" t="s">
         <v>41</v>
       </c>
       <c r="I7" s="5">
@@ -1155,7 +1164,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H8" s="19" t="s">
+      <c r="H8" s="18" t="s">
         <v>84</v>
       </c>
       <c r="I8" s="5">
@@ -1164,7 +1173,7 @@
       <c r="K8" s="15"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H9" s="19" t="s">
+      <c r="H9" s="18" t="s">
         <v>96</v>
       </c>
       <c r="I9" s="5">
@@ -1173,7 +1182,7 @@
       <c r="K9" s="15"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H10" s="19" t="s">
+      <c r="H10" s="18" t="s">
         <v>130</v>
       </c>
       <c r="I10" s="5">
@@ -1182,7 +1191,7 @@
       <c r="K10" s="15"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H11" s="19" t="s">
+      <c r="H11" s="18" t="s">
         <v>136</v>
       </c>
       <c r="I11" s="5">
@@ -1191,7 +1200,7 @@
       <c r="K11" s="15"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H12" s="19" t="s">
+      <c r="H12" s="18" t="s">
         <v>149</v>
       </c>
       <c r="I12" s="5">
@@ -1200,7 +1209,7 @@
       <c r="K12" s="15"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H13" s="19" t="s">
+      <c r="H13" s="18" t="s">
         <v>70</v>
       </c>
       <c r="I13" s="5">
@@ -1208,7 +1217,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H14" s="19" t="s">
+      <c r="H14" s="18" t="s">
         <v>107</v>
       </c>
       <c r="I14" s="5">
@@ -1227,7 +1236,7 @@
         <f>D6+C15</f>
         <v>490</v>
       </c>
-      <c r="H15" s="19" t="s">
+      <c r="H15" s="18" t="s">
         <v>10</v>
       </c>
       <c r="I15" s="5">
@@ -1249,7 +1258,7 @@
         <f t="shared" si="0"/>
         <v>2490</v>
       </c>
-      <c r="H16" s="19" t="s">
+      <c r="H16" s="18" t="s">
         <v>11</v>
       </c>
       <c r="I16" s="5">
@@ -1271,7 +1280,7 @@
         <f t="shared" si="0"/>
         <v>5490</v>
       </c>
-      <c r="H17" s="19" t="s">
+      <c r="H17" s="18" t="s">
         <v>24</v>
       </c>
       <c r="I17" s="5">
@@ -1280,7 +1289,7 @@
       <c r="K17" s="15"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H18" s="19" t="s">
+      <c r="H18" s="18" t="s">
         <v>59</v>
       </c>
       <c r="I18" s="5">
@@ -1289,7 +1298,7 @@
       <c r="K18" s="15"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H19" s="19" t="s">
+      <c r="H19" s="18" t="s">
         <v>73</v>
       </c>
       <c r="I19" s="5">
@@ -1298,7 +1307,7 @@
       <c r="K19" s="15"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H20" s="19" t="s">
+      <c r="H20" s="18" t="s">
         <v>91</v>
       </c>
       <c r="I20" s="5">
@@ -1307,7 +1316,7 @@
       <c r="K20" s="15"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H21" s="19" t="s">
+      <c r="H21" s="18" t="s">
         <v>121</v>
       </c>
       <c r="I21" s="5">
@@ -1316,7 +1325,7 @@
       <c r="K21" s="15"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H22" s="19" t="s">
+      <c r="H22" s="18" t="s">
         <v>132</v>
       </c>
       <c r="I22" s="5">
@@ -1325,7 +1334,7 @@
       <c r="K22" s="15"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H23" s="19" t="s">
+      <c r="H23" s="18" t="s">
         <v>138</v>
       </c>
       <c r="I23" s="5">
@@ -1334,7 +1343,7 @@
       <c r="K23" s="15"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H24" s="19" t="s">
+      <c r="H24" s="18" t="s">
         <v>152</v>
       </c>
       <c r="I24" s="5">
@@ -1356,7 +1365,7 @@
         <f>D17+C25</f>
         <v>8490</v>
       </c>
-      <c r="H25" s="19" t="s">
+      <c r="H25" s="18" t="s">
         <v>12</v>
       </c>
       <c r="I25" s="5">
@@ -1364,7 +1373,7 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H26" s="19" t="s">
+      <c r="H26" s="18" t="s">
         <v>43</v>
       </c>
       <c r="I26" s="5">
@@ -1373,7 +1382,7 @@
       <c r="K26" s="15"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H27" s="19" t="s">
+      <c r="H27" s="18" t="s">
         <v>146</v>
       </c>
       <c r="I27" s="5">
@@ -1382,7 +1391,7 @@
       <c r="K27" s="15"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H28" s="19" t="s">
+      <c r="H28" s="18" t="s">
         <v>163</v>
       </c>
       <c r="I28" s="5">
@@ -1391,7 +1400,7 @@
       <c r="K28" s="15"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H29" s="19" t="s">
+      <c r="H29" s="18" t="s">
         <v>164</v>
       </c>
       <c r="I29" s="5">
@@ -1410,7 +1419,7 @@
         <f>D25+C30</f>
         <v>12890</v>
       </c>
-      <c r="H30" s="19" t="s">
+      <c r="H30" s="18" t="s">
         <v>165</v>
       </c>
       <c r="I30" s="5">
@@ -1429,7 +1438,7 @@
         <f>D30+C31</f>
         <v>2890</v>
       </c>
-      <c r="H31" s="19" t="s">
+      <c r="H31" s="18" t="s">
         <v>166</v>
       </c>
       <c r="I31" s="5">
@@ -1451,7 +1460,7 @@
         <f t="shared" ref="D32:D39" si="1">D31+C32</f>
         <v>4490</v>
       </c>
-      <c r="H32" s="19" t="s">
+      <c r="H32" s="18" t="s">
         <v>167</v>
       </c>
       <c r="I32" s="5">
@@ -1470,7 +1479,7 @@
         <f t="shared" si="1"/>
         <v>7490</v>
       </c>
-      <c r="H33" s="19" t="s">
+      <c r="H33" s="18" t="s">
         <v>168</v>
       </c>
       <c r="I33" s="5">
@@ -1491,7 +1500,7 @@
         <f t="shared" si="1"/>
         <v>9490</v>
       </c>
-      <c r="H34" s="19" t="s">
+      <c r="H34" s="18" t="s">
         <v>162</v>
       </c>
       <c r="I34" s="5">
@@ -1512,7 +1521,7 @@
         <f t="shared" si="1"/>
         <v>12490</v>
       </c>
-      <c r="H35" s="19" t="s">
+      <c r="H35" s="18" t="s">
         <v>161</v>
       </c>
       <c r="I35" s="5">
@@ -1531,7 +1540,7 @@
         <f t="shared" si="1"/>
         <v>2490</v>
       </c>
-      <c r="H36" s="19" t="s">
+      <c r="H36" s="18" t="s">
         <v>160</v>
       </c>
       <c r="I36" s="5">
@@ -1553,7 +1562,7 @@
         <f t="shared" si="1"/>
         <v>7450</v>
       </c>
-      <c r="H37" s="19" t="s">
+      <c r="H37" s="18" t="s">
         <v>159</v>
       </c>
       <c r="I37" s="5">
@@ -1575,7 +1584,7 @@
         <f t="shared" si="1"/>
         <v>11450</v>
       </c>
-      <c r="H38" s="19" t="s">
+      <c r="H38" s="18" t="s">
         <v>158</v>
       </c>
       <c r="I38" s="5">
@@ -1593,7 +1602,7 @@
         <f t="shared" si="1"/>
         <v>1450</v>
       </c>
-      <c r="H39" s="19" t="s">
+      <c r="H39" s="18" t="s">
         <v>157</v>
       </c>
       <c r="I39" s="5">
@@ -2665,7 +2674,7 @@
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="19"/>
+      <c r="A117" s="18"/>
       <c r="B117" s="4" t="s">
         <v>20</v>
       </c>
@@ -2678,7 +2687,7 @@
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="19">
+      <c r="A118" s="18">
         <v>45297</v>
       </c>
       <c r="B118" s="4" t="s">
@@ -2693,7 +2702,7 @@
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="19">
+      <c r="A119" s="18">
         <v>45328</v>
       </c>
       <c r="B119" s="4" t="s">
@@ -2708,7 +2717,7 @@
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="19"/>
+      <c r="A120" s="18"/>
       <c r="B120" s="4" t="s">
         <v>20</v>
       </c>
@@ -2721,7 +2730,7 @@
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="19" t="s">
+      <c r="A121" s="18" t="s">
         <v>148</v>
       </c>
       <c r="B121" s="4" t="s">
@@ -2736,7 +2745,7 @@
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="19" t="s">
+      <c r="A122" s="18" t="s">
         <v>149</v>
       </c>
       <c r="B122" s="4" t="s">
@@ -2751,7 +2760,7 @@
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="19"/>
+      <c r="A123" s="18"/>
       <c r="B123" s="4" t="s">
         <v>20</v>
       </c>
@@ -2764,7 +2773,7 @@
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="19" t="s">
+      <c r="A124" s="18" t="s">
         <v>150</v>
       </c>
       <c r="B124" s="4" t="s">
@@ -2779,7 +2788,7 @@
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="19" t="s">
+      <c r="A125" s="18" t="s">
         <v>152</v>
       </c>
       <c r="B125" s="4" t="s">
@@ -2794,7 +2803,7 @@
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="19"/>
+      <c r="A126" s="18"/>
       <c r="B126" s="4" t="s">
         <v>20</v>
       </c>
@@ -2807,7 +2816,7 @@
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="19" t="s">
+      <c r="A127" s="18" t="s">
         <v>169</v>
       </c>
       <c r="B127" s="4" t="s">
@@ -2822,7 +2831,7 @@
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="19" t="s">
+      <c r="A128" s="18" t="s">
         <v>157</v>
       </c>
       <c r="B128" s="4" t="s">
@@ -2837,7 +2846,7 @@
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="19"/>
+      <c r="A129" s="18"/>
       <c r="B129" s="4" t="s">
         <v>20</v>
       </c>
@@ -2850,7 +2859,7 @@
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="19"/>
+      <c r="A130" s="18"/>
       <c r="B130" s="4" t="s">
         <v>156</v>
       </c>
@@ -2863,91 +2872,128 @@
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="19"/>
+      <c r="A131" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="B131" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C131" s="5">
+        <v>-1200</v>
+      </c>
+      <c r="D131" s="6">
+        <f>D130+C131</f>
+        <v>8390</v>
+      </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="19"/>
+      <c r="A132" s="18"/>
+      <c r="B132" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C132" s="5">
+        <v>500</v>
+      </c>
+      <c r="D132" s="6">
+        <f>D131+C132</f>
+        <v>8890</v>
+      </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="19"/>
+      <c r="A133" s="18"/>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="19"/>
+      <c r="A134" s="18"/>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="19"/>
+      <c r="A135" s="18"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="19"/>
+      <c r="A136" s="18"/>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="19"/>
+      <c r="A137" s="18"/>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="19"/>
+      <c r="A138" s="18"/>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="19"/>
+      <c r="A139" s="18"/>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="19"/>
+      <c r="A140" s="18"/>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="19"/>
+      <c r="A141" s="18"/>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="19"/>
+      <c r="A142" s="18"/>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="19"/>
+      <c r="A143" s="18"/>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="19"/>
+      <c r="A144" s="18"/>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" s="19"/>
+      <c r="A145" s="18"/>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" s="19"/>
+      <c r="A146" s="18"/>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" s="19"/>
+      <c r="A147" s="18"/>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148" s="19"/>
+      <c r="A148" s="18"/>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A149" s="19"/>
+      <c r="A149" s="18"/>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" s="19"/>
+      <c r="A150" s="18"/>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151" s="19"/>
+      <c r="A151" s="18"/>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152" s="19"/>
+      <c r="A152" s="18"/>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" s="19"/>
+      <c r="A153" s="18"/>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154" s="19"/>
+      <c r="A154" s="18"/>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155" s="19"/>
+      <c r="A155" s="18"/>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A156" s="19"/>
+      <c r="A156" s="18"/>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A157" s="19"/>
+      <c r="A157" s="18"/>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158" s="19"/>
+      <c r="A158" s="18"/>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A159" s="19"/>
+      <c r="A159" s="18"/>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" s="18"/>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" s="18"/>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" s="18"/>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" s="18"/>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2997,10 +3043,10 @@
       <c r="E1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="18"/>
+      <c r="I1" s="20"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
@@ -3136,10 +3182,10 @@
       <c r="E1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="18"/>
+      <c r="I1" s="20"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -3332,10 +3378,10 @@
       <c r="E1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="18"/>
+      <c r="I1" s="20"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">

</xml_diff>

<commit_message>
Duy chuyen cho co diem 350k
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="175">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -538,6 +538,12 @@
   </si>
   <si>
     <t>Duy chuyển cho cô diễm 500k</t>
+  </si>
+  <si>
+    <t>08/07/2024</t>
+  </si>
+  <si>
+    <t>Duy chuyển cho cô diễm 350k</t>
   </si>
 </sst>
 </file>
@@ -1017,8 +1023,8 @@
   <dimension ref="A1:K164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D133" sqref="D133"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D134" sqref="D134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2826,7 +2832,7 @@
         <v>2000</v>
       </c>
       <c r="D127" s="6">
-        <f>D126+C127</f>
+        <f t="shared" ref="D127:D132" si="16">D126+C127</f>
         <v>7590</v>
       </c>
     </row>
@@ -2841,7 +2847,7 @@
         <v>10000</v>
       </c>
       <c r="D128" s="6">
-        <f>D127+C128</f>
+        <f t="shared" si="16"/>
         <v>17590</v>
       </c>
     </row>
@@ -2854,7 +2860,7 @@
         <v>-10000</v>
       </c>
       <c r="D129" s="6">
-        <f>D128+C129</f>
+        <f t="shared" si="16"/>
         <v>7590</v>
       </c>
     </row>
@@ -2867,7 +2873,7 @@
         <v>2000</v>
       </c>
       <c r="D130" s="6">
-        <f>D129+C130</f>
+        <f t="shared" si="16"/>
         <v>9590</v>
       </c>
     </row>
@@ -2882,7 +2888,7 @@
         <v>-1200</v>
       </c>
       <c r="D131" s="6">
-        <f>D130+C131</f>
+        <f t="shared" si="16"/>
         <v>8390</v>
       </c>
     </row>
@@ -2895,12 +2901,24 @@
         <v>500</v>
       </c>
       <c r="D132" s="6">
-        <f>D131+C132</f>
+        <f t="shared" si="16"/>
         <v>8890</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="18"/>
+      <c r="A133" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="B133" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C133" s="5">
+        <v>350</v>
+      </c>
+      <c r="D133" s="6">
+        <f>D132+C133</f>
+        <v>9240</v>
+      </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="18"/>

</xml_diff>

<commit_message>
duy chuyen cho co diem 750k
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -543,7 +543,7 @@
     <t>08/07/2024</t>
   </si>
   <si>
-    <t>Duy chuyển cho cô diễm 350k</t>
+    <t>Duy chuyển cho cô diễm 750k</t>
   </si>
 </sst>
 </file>
@@ -1023,8 +1023,8 @@
   <dimension ref="A1:K164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D134" sqref="D134"/>
+      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D137" sqref="D137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2913,11 +2913,11 @@
         <v>174</v>
       </c>
       <c r="C133" s="5">
-        <v>350</v>
+        <v>750</v>
       </c>
       <c r="D133" s="6">
         <f>D132+C133</f>
-        <v>9240</v>
+        <v>9640</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
duy chuyen cho co diem 2tr,  lay tien loi ngay 13 2tr
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="177">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -544,6 +544,12 @@
   </si>
   <si>
     <t>Duy chuyển cho cô diễm 750k</t>
+  </si>
+  <si>
+    <t>13/072024</t>
+  </si>
+  <si>
+    <t>13/07/2024</t>
   </si>
 </sst>
 </file>
@@ -1020,11 +1026,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K164"/>
+  <dimension ref="A1:K165"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D137" sqref="D137"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1100,23 +1106,13 @@
         <v>20</v>
       </c>
       <c r="J3" s="4">
-        <f>SUM(I3:I55)</f>
-        <v>390</v>
+        <f>SUM(I3:I56)</f>
+        <v>400</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="5">
-        <v>14560</v>
-      </c>
-      <c r="D4" s="6">
-        <f>C4+D3</f>
-        <v>18490</v>
-      </c>
       <c r="H4" s="18" t="s">
-        <v>7</v>
+        <v>176</v>
       </c>
       <c r="I4" s="5">
         <v>10</v>
@@ -1124,46 +1120,56 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5" s="5">
-        <v>-10000</v>
+        <v>14560</v>
       </c>
       <c r="D5" s="6">
-        <f t="shared" ref="D5:D17" si="0">D4+C5</f>
-        <v>8490</v>
+        <f>C5+D3</f>
+        <v>18490</v>
       </c>
       <c r="H5" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I5" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="B6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D6" s="6">
+        <f t="shared" ref="D6:D18" si="0">D5+C6</f>
+        <v>8490</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
         <v>44966</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C7" s="5">
         <v>2000</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D7" s="6">
         <f t="shared" si="0"/>
         <v>10490</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="H7" s="18" t="s">
         <v>9</v>
-      </c>
-      <c r="I6" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H7" s="18" t="s">
-        <v>41</v>
       </c>
       <c r="I7" s="5">
         <v>10</v>
@@ -1171,16 +1177,15 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H8" s="18" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="I8" s="5">
         <v>10</v>
       </c>
-      <c r="K8" s="15"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H9" s="18" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="I9" s="5">
         <v>10</v>
@@ -1189,7 +1194,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H10" s="18" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="I10" s="5">
         <v>10</v>
@@ -1198,7 +1203,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H11" s="18" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="I11" s="5">
         <v>10</v>
@@ -1207,7 +1212,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H12" s="18" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="I12" s="5">
         <v>10</v>
@@ -1216,34 +1221,24 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H13" s="18" t="s">
-        <v>70</v>
+        <v>149</v>
       </c>
       <c r="I13" s="5">
         <v>10</v>
       </c>
+      <c r="K13" s="15"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H14" s="18" t="s">
-        <v>107</v>
+        <v>70</v>
       </c>
       <c r="I14" s="5">
         <v>10</v>
       </c>
-      <c r="K14" s="15"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="5">
-        <v>-10000</v>
-      </c>
-      <c r="D15" s="6">
-        <f>D6+C15</f>
-        <v>490</v>
-      </c>
       <c r="H15" s="18" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="I15" s="5">
         <v>10</v>
@@ -1251,52 +1246,62 @@
       <c r="K15" s="15"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="B16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D16" s="6">
+        <f>D7+C16</f>
+        <v>490</v>
+      </c>
+      <c r="H16" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" s="5">
+        <v>10</v>
+      </c>
+      <c r="K16" s="15"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C17" s="5">
         <v>2000</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D17" s="6">
         <f t="shared" si="0"/>
         <v>2490</v>
       </c>
-      <c r="H16" s="18" t="s">
+      <c r="H17" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="I16" s="5">
+      <c r="I17" s="5">
         <v>10</v>
       </c>
-      <c r="K16" s="15"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="K17" s="15"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B18" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C18" s="5">
         <v>3000</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D18" s="6">
         <f t="shared" si="0"/>
         <v>5490</v>
       </c>
-      <c r="H17" s="18" t="s">
+      <c r="H18" s="18" t="s">
         <v>24</v>
-      </c>
-      <c r="I17" s="5">
-        <v>10</v>
-      </c>
-      <c r="K17" s="15"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H18" s="18" t="s">
-        <v>59</v>
       </c>
       <c r="I18" s="5">
         <v>10</v>
@@ -1305,7 +1310,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H19" s="18" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="I19" s="5">
         <v>10</v>
@@ -1314,7 +1319,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H20" s="18" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="I20" s="5">
         <v>10</v>
@@ -1323,7 +1328,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H21" s="18" t="s">
-        <v>121</v>
+        <v>91</v>
       </c>
       <c r="I21" s="5">
         <v>10</v>
@@ -1332,7 +1337,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H22" s="18" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="I22" s="5">
         <v>10</v>
@@ -1341,7 +1346,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H23" s="18" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="I23" s="5">
         <v>10</v>
@@ -1350,7 +1355,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H24" s="18" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="I24" s="5">
         <v>10</v>
@@ -1358,38 +1363,38 @@
       <c r="K24" s="15"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" s="5">
-        <v>3000</v>
-      </c>
-      <c r="D25" s="6">
-        <f>D17+C25</f>
-        <v>8490</v>
-      </c>
       <c r="H25" s="18" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="I25" s="5">
         <v>10</v>
       </c>
+      <c r="K25" s="15"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="5">
+        <v>3000</v>
+      </c>
+      <c r="D26" s="6">
+        <f>D18+C26</f>
+        <v>8490</v>
+      </c>
       <c r="H26" s="18" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="I26" s="5">
         <v>10</v>
       </c>
-      <c r="K26" s="15"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H27" s="18" t="s">
-        <v>146</v>
+        <v>43</v>
       </c>
       <c r="I27" s="5">
         <v>10</v>
@@ -1398,7 +1403,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H28" s="18" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="I28" s="5">
         <v>10</v>
@@ -1407,7 +1412,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H29" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I29" s="5">
         <v>10</v>
@@ -1415,59 +1420,46 @@
       <c r="K29" s="15"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B30" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" s="5">
-        <v>4400</v>
-      </c>
-      <c r="D30" s="6">
-        <f>D25+C30</f>
-        <v>12890</v>
-      </c>
       <c r="H30" s="18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I30" s="5">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K30" s="15"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="5">
+        <v>4400</v>
+      </c>
+      <c r="D31" s="6">
+        <f>D26+C31</f>
+        <v>12890</v>
+      </c>
+      <c r="H31" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="I31" s="5">
+        <v>20</v>
+      </c>
+      <c r="K31" s="15"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C32" s="5">
         <v>-10000</v>
       </c>
-      <c r="D31" s="6">
-        <f>D30+C31</f>
+      <c r="D32" s="6">
+        <f>D31+C32</f>
         <v>2890</v>
       </c>
-      <c r="H31" s="18" t="s">
+      <c r="H32" s="18" t="s">
         <v>166</v>
-      </c>
-      <c r="I31" s="5">
-        <v>10</v>
-      </c>
-      <c r="K31" s="15"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="9">
-        <v>44967</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C32" s="5">
-        <v>1600</v>
-      </c>
-      <c r="D32" s="6">
-        <f t="shared" ref="D32:D39" si="1">D31+C32</f>
-        <v>4490</v>
-      </c>
-      <c r="H32" s="18" t="s">
-        <v>167</v>
       </c>
       <c r="I32" s="5">
         <v>10</v>
@@ -1475,517 +1467,524 @@
       <c r="K32" s="15"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="9">
+        <v>44967</v>
+      </c>
       <c r="B33" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="5">
+        <v>1600</v>
+      </c>
+      <c r="D33" s="6">
+        <f t="shared" ref="D33:D40" si="1">D32+C33</f>
+        <v>4490</v>
+      </c>
+      <c r="H33" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="I33" s="5">
+        <v>10</v>
+      </c>
+      <c r="K33" s="15"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B34" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C34" s="5">
         <v>3000</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D34" s="6">
         <f t="shared" si="1"/>
         <v>7490</v>
       </c>
-      <c r="H33" s="18" t="s">
+      <c r="H34" s="18" t="s">
         <v>168</v>
       </c>
-      <c r="I33" s="5">
+      <c r="I34" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B35" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C35" s="5">
         <v>2000</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D35" s="6">
         <f t="shared" si="1"/>
         <v>9490</v>
       </c>
-      <c r="H34" s="18" t="s">
+      <c r="H35" s="18" t="s">
         <v>162</v>
       </c>
-      <c r="I34" s="5">
+      <c r="I35" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B36" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="5">
+      <c r="C36" s="5">
         <v>3000</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D36" s="6">
         <f t="shared" si="1"/>
         <v>12490</v>
       </c>
-      <c r="H35" s="18" t="s">
+      <c r="H36" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="I35" s="5">
+      <c r="I36" s="5">
         <v>10</v>
       </c>
-      <c r="K35" s="15"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B36" s="4" t="s">
+      <c r="K36" s="15"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B37" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C36" s="5">
+      <c r="C37" s="5">
         <v>-10000</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D37" s="6">
         <f t="shared" si="1"/>
         <v>2490</v>
       </c>
-      <c r="H36" s="18" t="s">
+      <c r="H37" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="I36" s="5">
+      <c r="I37" s="5">
         <v>10</v>
       </c>
-      <c r="K36" s="15"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="9" t="s">
+      <c r="K37" s="15"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B38" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C37" s="5">
+      <c r="C38" s="5">
         <v>4960</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D38" s="6">
         <f t="shared" si="1"/>
         <v>7450</v>
       </c>
-      <c r="H37" s="18" t="s">
+      <c r="H38" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="I37" s="5">
+      <c r="I38" s="5">
         <v>10</v>
       </c>
-      <c r="K37" s="15"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="9" t="s">
+      <c r="K38" s="15"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B39" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C38" s="5">
+      <c r="C39" s="5">
         <v>4000</v>
       </c>
-      <c r="D38" s="6">
+      <c r="D39" s="6">
         <f t="shared" si="1"/>
         <v>11450</v>
       </c>
-      <c r="H38" s="18" t="s">
+      <c r="H39" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="I38" s="5">
+      <c r="I39" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B39" s="4" t="s">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C39" s="5">
+      <c r="C40" s="5">
         <v>-10000</v>
       </c>
-      <c r="D39" s="6">
+      <c r="D40" s="6">
         <f t="shared" si="1"/>
         <v>1450</v>
       </c>
-      <c r="H39" s="18" t="s">
+      <c r="H40" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="I39" s="5">
+      <c r="I40" s="5">
         <v>10</v>
       </c>
-      <c r="K39" s="15"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B40" s="4" t="s">
+      <c r="K40" s="15"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B41" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C40" s="5">
+      <c r="C41" s="5">
         <v>7640</v>
       </c>
-      <c r="D40" s="6">
-        <f t="shared" ref="D40:D45" si="2">D39+C40</f>
+      <c r="D41" s="6">
+        <f t="shared" ref="D41:D46" si="2">D40+C41</f>
         <v>9090</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="9">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="9">
         <v>44968</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B42" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="5">
+      <c r="C42" s="5">
         <v>3000</v>
       </c>
-      <c r="D41" s="6">
+      <c r="D42" s="6">
         <f t="shared" si="2"/>
         <v>12090</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B42" s="4" t="s">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B43" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C43" s="5">
         <v>-10000</v>
       </c>
-      <c r="D42" s="6">
+      <c r="D43" s="6">
         <f t="shared" si="2"/>
         <v>2090</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="9">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="9">
         <v>44996</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B44" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C43" s="5">
+      <c r="C44" s="5">
         <v>800</v>
       </c>
-      <c r="D43" s="6">
+      <c r="D44" s="6">
         <f t="shared" si="2"/>
         <v>2890</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="9" t="s">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B45" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C45" s="5">
         <v>2000</v>
       </c>
-      <c r="D44" s="6">
+      <c r="D45" s="6">
         <f t="shared" si="2"/>
         <v>4890</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="9" t="s">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B46" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C45" s="5">
+      <c r="C46" s="5">
         <v>4000</v>
       </c>
-      <c r="D45" s="6">
+      <c r="D46" s="6">
         <f t="shared" si="2"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="9" t="s">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B47" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C46" s="5">
+      <c r="C47" s="5">
         <v>4000</v>
       </c>
-      <c r="D46" s="6">
-        <f t="shared" ref="D46:D51" si="3">D45+C46</f>
+      <c r="D47" s="6">
+        <f t="shared" ref="D47:D52" si="3">D46+C47</f>
         <v>12890</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B47" s="4" t="s">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B48" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C48" s="5">
         <v>5000</v>
       </c>
-      <c r="D47" s="6">
+      <c r="D48" s="6">
         <f t="shared" si="3"/>
         <v>17890</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B48" s="4" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C48" s="5">
+      <c r="C49" s="5">
         <v>-10000</v>
       </c>
-      <c r="D48" s="6">
+      <c r="D49" s="6">
         <f t="shared" si="3"/>
         <v>7890</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="9">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="9">
         <v>44969</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B50" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C49" s="5">
+      <c r="C50" s="5">
         <v>900</v>
       </c>
-      <c r="D49" s="6">
+      <c r="D50" s="6">
         <f t="shared" si="3"/>
         <v>8790</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B50" s="4" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B51" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C50" s="5">
+      <c r="C51" s="5">
         <v>4000</v>
       </c>
-      <c r="D50" s="6">
+      <c r="D51" s="6">
         <f t="shared" si="3"/>
         <v>12790</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B51" s="4" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C51" s="5">
+      <c r="C52" s="5">
         <v>-10000</v>
       </c>
-      <c r="D51" s="6">
+      <c r="D52" s="6">
         <f t="shared" si="3"/>
         <v>2790</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C52" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D52" s="6">
-        <f t="shared" ref="D52:D59" si="4">D51+C52</f>
-        <v>4790</v>
-      </c>
-    </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C53" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D53" s="6">
+        <f t="shared" ref="D53:D60" si="4">D52+C53</f>
+        <v>4790</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B54" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C53" s="5">
+      <c r="C54" s="5">
         <v>700</v>
       </c>
-      <c r="D53" s="6">
+      <c r="D54" s="6">
         <f t="shared" si="4"/>
         <v>5490</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B54" s="4" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B55" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C54" s="5">
+      <c r="C55" s="5">
         <v>4000</v>
       </c>
-      <c r="D54" s="6">
+      <c r="D55" s="6">
         <f t="shared" si="4"/>
         <v>9490</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="9" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B56" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C55" s="5">
+      <c r="C56" s="5">
         <v>600</v>
       </c>
-      <c r="D55" s="6">
+      <c r="D56" s="6">
         <f t="shared" si="4"/>
         <v>10090</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B56" s="4" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B57" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C56" s="5">
+      <c r="C57" s="5">
         <v>-10000</v>
       </c>
-      <c r="D56" s="6">
+      <c r="D57" s="6">
         <f t="shared" si="4"/>
         <v>90</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="9" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B58" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C57" s="5">
+      <c r="C58" s="5">
         <f>700+5000+300+600+400+1000+800</f>
         <v>8800</v>
       </c>
-      <c r="D57" s="6">
+      <c r="D58" s="6">
         <f t="shared" si="4"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B58" s="4" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B59" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C58" s="5">
+      <c r="C59" s="5">
         <v>6000</v>
       </c>
-      <c r="D58" s="6">
+      <c r="D59" s="6">
         <f t="shared" si="4"/>
         <v>14890</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B59" s="4" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B60" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C59" s="5">
+      <c r="C60" s="5">
         <v>-10000</v>
       </c>
-      <c r="D59" s="6">
+      <c r="D60" s="6">
         <f t="shared" si="4"/>
         <v>4890</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="9" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B61" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C60" s="5">
+      <c r="C61" s="5">
         <v>500</v>
       </c>
-      <c r="D60" s="6">
-        <f t="shared" ref="D60:D65" si="5">D59+C60</f>
+      <c r="D61" s="6">
+        <f t="shared" ref="D61:D66" si="5">D60+C61</f>
         <v>5390</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="9">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="9">
         <v>45323</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B62" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C61" s="5">
+      <c r="C62" s="5">
         <v>700</v>
       </c>
-      <c r="D61" s="6">
+      <c r="D62" s="6">
         <f t="shared" si="5"/>
         <v>6090</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B62" s="4" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B63" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C62" s="5">
+      <c r="C63" s="5">
         <v>1500</v>
       </c>
-      <c r="D62" s="6">
+      <c r="D63" s="6">
         <f t="shared" si="5"/>
         <v>7590</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B63" s="4" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B64" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C63" s="5">
+      <c r="C64" s="5">
         <v>5000</v>
       </c>
-      <c r="D63" s="6">
+      <c r="D64" s="6">
         <f t="shared" si="5"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B64" s="4" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B65" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C64" s="5">
+      <c r="C65" s="5">
         <v>-10000</v>
       </c>
-      <c r="D64" s="6">
+      <c r="D65" s="6">
         <f t="shared" si="5"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="9" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B66" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C65" s="5">
+      <c r="C66" s="5">
         <v>2000</v>
       </c>
-      <c r="D65" s="6">
+      <c r="D66" s="6">
         <f t="shared" si="5"/>
         <v>4590</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="9">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="9">
         <v>45474</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C66" s="5">
-        <v>700</v>
-      </c>
-      <c r="D66" s="6">
-        <f t="shared" ref="D66:D71" si="6">D65+C66</f>
-        <v>5290</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="9" t="s">
-        <v>82</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>77</v>
@@ -1994,418 +1993,418 @@
         <v>700</v>
       </c>
       <c r="D67" s="6">
+        <f t="shared" ref="D67:D72" si="6">D66+C67</f>
+        <v>5290</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C68" s="5">
+        <v>700</v>
+      </c>
+      <c r="D68" s="6">
         <f t="shared" si="6"/>
         <v>5990</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="9" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B69" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C68" s="5">
+      <c r="C69" s="5">
         <v>700</v>
       </c>
-      <c r="D68" s="6">
+      <c r="D69" s="6">
         <f t="shared" si="6"/>
         <v>6690</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="9" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B70" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C69" s="5">
+      <c r="C70" s="5">
         <v>4000</v>
       </c>
-      <c r="D69" s="6">
+      <c r="D70" s="6">
         <f t="shared" si="6"/>
         <v>10690</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B70" s="4" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B71" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C70" s="5">
+      <c r="C71" s="5">
         <v>-10000</v>
       </c>
-      <c r="D70" s="6">
+      <c r="D71" s="6">
         <f t="shared" si="6"/>
         <v>690</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="9" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B72" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C71" s="5">
+      <c r="C72" s="5">
         <v>1000</v>
       </c>
-      <c r="D71" s="6">
+      <c r="D72" s="6">
         <f t="shared" si="6"/>
         <v>1690</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="9" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B73" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C72" s="5">
+      <c r="C73" s="5">
         <v>7000</v>
       </c>
-      <c r="D72" s="6">
-        <f t="shared" ref="D72:D77" si="7">D71+C72</f>
+      <c r="D73" s="6">
+        <f t="shared" ref="D73:D78" si="7">D72+C73</f>
         <v>8690</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B73" s="4" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C73" s="5">
+      <c r="C74" s="5">
         <v>10000</v>
       </c>
-      <c r="D73" s="6">
+      <c r="D74" s="6">
         <f t="shared" si="7"/>
         <v>18690</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B74" s="4" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B75" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C74" s="5">
+      <c r="C75" s="5">
         <v>-10000</v>
       </c>
-      <c r="D74" s="6">
+      <c r="D75" s="6">
         <f t="shared" si="7"/>
         <v>8690</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="9">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="9">
         <v>45293</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="B76" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C75" s="5">
+      <c r="C76" s="5">
         <v>1700</v>
       </c>
-      <c r="D75" s="6">
+      <c r="D76" s="6">
         <f t="shared" si="7"/>
         <v>10390</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B76" s="4" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B77" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C76" s="5">
+      <c r="C77" s="5">
         <v>-10000</v>
       </c>
-      <c r="D76" s="6">
+      <c r="D77" s="6">
         <f t="shared" si="7"/>
         <v>390</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="9">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="9">
         <v>45324</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="B78" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C77" s="5">
+      <c r="C78" s="5">
         <v>6000</v>
       </c>
-      <c r="D77" s="6">
+      <c r="D78" s="6">
         <f t="shared" si="7"/>
         <v>6390</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="B78" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C78" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D78" s="6">
-        <f t="shared" ref="D78:D83" si="8">D77+C78</f>
-        <v>8390</v>
-      </c>
-    </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C79" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D79" s="6">
+        <f t="shared" ref="D79:D84" si="8">D78+C79</f>
+        <v>8390</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B79" s="4" t="s">
+      <c r="B80" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C79" s="5">
+      <c r="C80" s="5">
         <v>5000</v>
       </c>
-      <c r="D79" s="6">
+      <c r="D80" s="6">
         <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B80" s="4" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B81" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C80" s="5">
+      <c r="C81" s="5">
         <v>-10000</v>
       </c>
-      <c r="D80" s="6">
+      <c r="D81" s="6">
         <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="9" t="s">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="B81" s="4" t="s">
+      <c r="B82" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C81" s="5">
+      <c r="C82" s="5">
         <v>1000</v>
       </c>
-      <c r="D81" s="6">
+      <c r="D82" s="6">
         <f t="shared" si="8"/>
         <v>4390</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="9">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="9">
         <v>45294</v>
       </c>
-      <c r="B82" s="4" t="s">
+      <c r="B83" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C82" s="5">
+      <c r="C83" s="5">
         <v>9000</v>
       </c>
-      <c r="D82" s="6">
+      <c r="D83" s="6">
         <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B83" s="4" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B84" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C83" s="5">
+      <c r="C84" s="5">
         <v>-10000</v>
       </c>
-      <c r="D83" s="6">
+      <c r="D84" s="6">
         <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B84" s="4" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B85" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C84" s="5">
+      <c r="C85" s="5">
         <v>2000</v>
       </c>
-      <c r="D84" s="6">
-        <f t="shared" ref="D84:D89" si="9">D83+C84</f>
+      <c r="D85" s="6">
+        <f t="shared" ref="D85:D90" si="9">D84+C85</f>
         <v>5390</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="9">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="9">
         <v>45325</v>
       </c>
-      <c r="B85" s="4" t="s">
+      <c r="B86" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C85" s="5">
+      <c r="C86" s="5">
         <v>6000</v>
       </c>
-      <c r="D85" s="6">
+      <c r="D86" s="6">
         <f t="shared" si="9"/>
         <v>11390</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B86" s="4" t="s">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B87" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C86" s="5">
+      <c r="C87" s="5">
         <v>-10000</v>
       </c>
-      <c r="D86" s="6">
+      <c r="D87" s="6">
         <f t="shared" si="9"/>
         <v>1390</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="9">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="9">
         <v>45507</v>
       </c>
-      <c r="B87" s="4" t="s">
+      <c r="B88" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C87" s="5">
+      <c r="C88" s="5">
         <v>400</v>
       </c>
-      <c r="D87" s="6">
+      <c r="D88" s="6">
         <f t="shared" si="9"/>
         <v>1790</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="9" t="s">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="B88" s="4" t="s">
+      <c r="B89" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C88" s="5">
+      <c r="C89" s="5">
         <v>2000</v>
       </c>
-      <c r="D88" s="6">
+      <c r="D89" s="6">
         <f t="shared" si="9"/>
         <v>3790</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="9" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="B89" s="4" t="s">
+      <c r="B90" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C89" s="5">
+      <c r="C90" s="5">
         <v>6000</v>
       </c>
-      <c r="D89" s="6">
+      <c r="D90" s="6">
         <f t="shared" si="9"/>
         <v>9790</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="9" t="s">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="B90" s="4" t="s">
+      <c r="B91" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C90" s="5">
+      <c r="C91" s="5">
         <v>1000</v>
       </c>
-      <c r="D90" s="6">
-        <f t="shared" ref="D90:D95" si="10">D89+C90</f>
+      <c r="D91" s="6">
+        <f t="shared" ref="D91:D96" si="10">D90+C91</f>
         <v>10790</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B91" s="4" t="s">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B92" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C91" s="5">
+      <c r="C92" s="5">
         <v>-10000</v>
       </c>
-      <c r="D91" s="6">
+      <c r="D92" s="6">
         <f t="shared" si="10"/>
         <v>790</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="9" t="s">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="B92" s="4" t="s">
+      <c r="B93" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C92" s="5">
+      <c r="C93" s="5">
         <v>800</v>
       </c>
-      <c r="D92" s="6">
+      <c r="D93" s="6">
         <f t="shared" si="10"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="9" t="s">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="B93" s="4" t="s">
+      <c r="B94" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C93" s="5">
+      <c r="C94" s="5">
         <v>5000</v>
       </c>
-      <c r="D93" s="6">
+      <c r="D94" s="6">
         <f t="shared" si="10"/>
         <v>6590</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="9" t="s">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="B94" s="4" t="s">
+      <c r="B95" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C94" s="5">
+      <c r="C95" s="5">
         <v>6000</v>
       </c>
-      <c r="D94" s="6">
+      <c r="D95" s="6">
         <f t="shared" si="10"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B95" s="4" t="s">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B96" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C95" s="5">
+      <c r="C96" s="5">
         <v>-10000</v>
       </c>
-      <c r="D95" s="6">
+      <c r="D96" s="6">
         <f t="shared" si="10"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="9" t="s">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="9" t="s">
         <v>124</v>
-      </c>
-      <c r="B96" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C96" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D96" s="6">
-        <f t="shared" ref="D96:D102" si="11">D95+C96</f>
-        <v>4590</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="9">
-        <v>45295</v>
       </c>
       <c r="B97" s="4" t="s">
         <v>65</v>
@@ -2414,523 +2413,567 @@
         <v>2000</v>
       </c>
       <c r="D97" s="6">
+        <f t="shared" ref="D97:D103" si="11">D96+C97</f>
+        <v>4590</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="9">
+        <v>45295</v>
+      </c>
+      <c r="B98" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C98" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D98" s="6">
         <f t="shared" si="11"/>
         <v>6590</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="9">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="9">
         <v>45326</v>
       </c>
-      <c r="B98" s="4" t="s">
+      <c r="B99" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C98" s="5">
+      <c r="C99" s="5">
         <v>7000</v>
       </c>
-      <c r="D98" s="6">
+      <c r="D99" s="6">
         <f t="shared" si="11"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B99" s="4" t="s">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B100" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C99" s="5">
+      <c r="C100" s="5">
         <v>-10000</v>
       </c>
-      <c r="D99" s="6">
+      <c r="D100" s="6">
         <f t="shared" si="11"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="9" t="s">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="B100" s="4" t="s">
+      <c r="B101" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C100" s="5">
+      <c r="C101" s="5">
         <v>2000</v>
       </c>
-      <c r="D100" s="6">
+      <c r="D101" s="6">
         <f t="shared" si="11"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="9" t="s">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="B101" s="4" t="s">
+      <c r="B102" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C101" s="5">
+      <c r="C102" s="5">
         <v>6000</v>
       </c>
-      <c r="D101" s="6">
+      <c r="D102" s="6">
         <f t="shared" si="11"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B102" s="4" t="s">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B103" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C102" s="5">
+      <c r="C103" s="5">
         <v>-10000</v>
       </c>
-      <c r="D102" s="6">
+      <c r="D103" s="6">
         <f t="shared" si="11"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="B103" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C103" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D103" s="6">
-        <f t="shared" ref="D103:D108" si="12">D102+C103</f>
-        <v>3590</v>
-      </c>
-    </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C104" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D104" s="6">
+        <f t="shared" ref="D104:D109" si="12">D103+C104</f>
+        <v>3590</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="B104" s="4" t="s">
+      <c r="B105" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C104" s="5">
+      <c r="C105" s="5">
         <v>7000</v>
       </c>
-      <c r="D104" s="6">
+      <c r="D105" s="6">
         <f t="shared" si="12"/>
         <v>10590</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B105" s="4" t="s">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B106" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C105" s="5">
+      <c r="C106" s="5">
         <v>-10000</v>
       </c>
-      <c r="D105" s="6">
+      <c r="D106" s="6">
         <f t="shared" si="12"/>
         <v>590</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="9">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="9">
         <v>45327</v>
       </c>
-      <c r="B106" s="4" t="s">
+      <c r="B107" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C106" s="5">
+      <c r="C107" s="5">
         <v>12000</v>
       </c>
-      <c r="D106" s="6">
+      <c r="D107" s="6">
         <f t="shared" si="12"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B107" s="4" t="s">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B108" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C107" s="5">
+      <c r="C108" s="5">
         <v>-10000</v>
       </c>
-      <c r="D107" s="6">
+      <c r="D108" s="6">
         <f t="shared" si="12"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B108" s="4" t="s">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B109" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C108" s="5">
+      <c r="C109" s="5">
         <v>2000</v>
       </c>
-      <c r="D108" s="6">
+      <c r="D109" s="6">
         <f t="shared" si="12"/>
         <v>4590</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="B109" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C109" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D109" s="6">
-        <f t="shared" ref="D109:D114" si="13">D108+C109</f>
-        <v>6590</v>
-      </c>
-    </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="B110" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C110" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D110" s="6">
+        <f t="shared" ref="D110:D115" si="13">D109+C110</f>
+        <v>6590</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="B110" s="4" t="s">
+      <c r="B111" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C110" s="5">
+      <c r="C111" s="5">
         <v>7000</v>
       </c>
-      <c r="D110" s="6">
+      <c r="D111" s="6">
         <f t="shared" si="13"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B111" s="4" t="s">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B112" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C111" s="5">
+      <c r="C112" s="5">
         <v>-10000</v>
       </c>
-      <c r="D111" s="6">
+      <c r="D112" s="6">
         <f t="shared" si="13"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="9" t="s">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="B112" s="4" t="s">
+      <c r="B113" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C112" s="5">
+      <c r="C113" s="5">
         <v>2000</v>
       </c>
-      <c r="D112" s="6">
+      <c r="D113" s="6">
         <f t="shared" si="13"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="9" t="s">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="B113" s="4" t="s">
+      <c r="B114" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C113" s="5">
+      <c r="C114" s="5">
         <v>8000</v>
       </c>
-      <c r="D113" s="6">
+      <c r="D114" s="6">
         <f t="shared" si="13"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B114" s="4" t="s">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B115" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C114" s="5">
+      <c r="C115" s="5">
         <v>-10000</v>
       </c>
-      <c r="D114" s="6">
+      <c r="D115" s="6">
         <f t="shared" si="13"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="9" t="s">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="B115" s="4" t="s">
+      <c r="B116" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C115" s="5">
+      <c r="C116" s="5">
         <v>2000</v>
       </c>
-      <c r="D115" s="6">
-        <f t="shared" ref="D115:D120" si="14">D114+C115</f>
+      <c r="D116" s="6">
+        <f t="shared" ref="D116:D121" si="14">D115+C116</f>
         <v>5590</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B116" s="4" t="s">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B117" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C116" s="5">
+      <c r="C117" s="5">
         <v>5000</v>
       </c>
-      <c r="D116" s="6">
+      <c r="D117" s="6">
         <f t="shared" si="14"/>
         <v>10590</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="18"/>
-      <c r="B117" s="4" t="s">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="18"/>
+      <c r="B118" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C117" s="5">
+      <c r="C118" s="5">
         <v>-10000</v>
       </c>
-      <c r="D117" s="6">
+      <c r="D118" s="6">
         <f t="shared" si="14"/>
         <v>590</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="18">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="18">
         <v>45297</v>
       </c>
-      <c r="B118" s="4" t="s">
+      <c r="B119" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C118" s="5">
+      <c r="C119" s="5">
         <v>2000</v>
       </c>
-      <c r="D118" s="6">
+      <c r="D119" s="6">
         <f t="shared" si="14"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="18">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="18">
         <v>45328</v>
       </c>
-      <c r="B119" s="4" t="s">
+      <c r="B120" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C119" s="5">
+      <c r="C120" s="5">
         <v>9000</v>
       </c>
-      <c r="D119" s="6">
+      <c r="D120" s="6">
         <f t="shared" si="14"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="18"/>
-      <c r="B120" s="4" t="s">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="18"/>
+      <c r="B121" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C120" s="5">
+      <c r="C121" s="5">
         <v>-10000</v>
       </c>
-      <c r="D120" s="6">
+      <c r="D121" s="6">
         <f t="shared" si="14"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="B121" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C121" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D121" s="6">
-        <f t="shared" ref="D121:D126" si="15">D120+C121</f>
-        <v>3590</v>
-      </c>
-    </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B122" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C122" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D122" s="6">
+        <f t="shared" ref="D122:D127" si="15">D121+C122</f>
+        <v>3590</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="B122" s="4" t="s">
+      <c r="B123" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C122" s="5">
+      <c r="C123" s="5">
         <v>8000</v>
       </c>
-      <c r="D122" s="6">
+      <c r="D123" s="6">
         <f t="shared" si="15"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="18"/>
-      <c r="B123" s="4" t="s">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="18"/>
+      <c r="B124" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C123" s="5">
+      <c r="C124" s="5">
         <v>-10000</v>
       </c>
-      <c r="D123" s="6">
+      <c r="D124" s="6">
         <f t="shared" si="15"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="18" t="s">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="B124" s="4" t="s">
+      <c r="B125" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C124" s="5">
+      <c r="C125" s="5">
         <v>2000</v>
       </c>
-      <c r="D124" s="6">
+      <c r="D125" s="6">
         <f t="shared" si="15"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="18" t="s">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="B125" s="4" t="s">
+      <c r="B126" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="C125" s="5">
+      <c r="C126" s="5">
         <v>12000</v>
       </c>
-      <c r="D125" s="6">
+      <c r="D126" s="6">
         <f t="shared" si="15"/>
         <v>15590</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="18"/>
-      <c r="B126" s="4" t="s">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="18"/>
+      <c r="B127" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C126" s="5">
+      <c r="C127" s="5">
         <v>-10000</v>
       </c>
-      <c r="D126" s="6">
+      <c r="D127" s="6">
         <f t="shared" si="15"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="18" t="s">
-        <v>169</v>
-      </c>
-      <c r="B127" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="C127" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D127" s="6">
-        <f t="shared" ref="D127:D132" si="16">D126+C127</f>
-        <v>7590</v>
-      </c>
-    </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="B128" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C128" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D128" s="6">
+        <f t="shared" ref="D128:D133" si="16">D127+C128</f>
+        <v>7590</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="B128" s="4" t="s">
+      <c r="B129" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="C128" s="5">
+      <c r="C129" s="5">
         <v>10000</v>
       </c>
-      <c r="D128" s="6">
+      <c r="D129" s="6">
         <f t="shared" si="16"/>
         <v>17590</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="18"/>
-      <c r="B129" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C129" s="5">
-        <v>-10000</v>
-      </c>
-      <c r="D129" s="6">
-        <f t="shared" si="16"/>
-        <v>7590</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="18"/>
       <c r="B130" s="4" t="s">
-        <v>156</v>
+        <v>20</v>
       </c>
       <c r="C130" s="5">
-        <v>2000</v>
+        <v>-10000</v>
       </c>
       <c r="D130" s="6">
         <f t="shared" si="16"/>
-        <v>9590</v>
+        <v>7590</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="18" t="s">
-        <v>170</v>
-      </c>
+      <c r="A131" s="18"/>
       <c r="B131" s="4" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="C131" s="5">
-        <v>-1200</v>
+        <v>2000</v>
       </c>
       <c r="D131" s="6">
         <f t="shared" si="16"/>
-        <v>8390</v>
+        <v>9590</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="18"/>
+      <c r="A132" s="18" t="s">
+        <v>170</v>
+      </c>
       <c r="B132" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C132" s="5">
-        <v>500</v>
+        <v>-1200</v>
       </c>
       <c r="D132" s="6">
         <f t="shared" si="16"/>
+        <v>8390</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="18"/>
+      <c r="B133" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C133" s="5">
+        <v>500</v>
+      </c>
+      <c r="D133" s="6">
+        <f t="shared" si="16"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="18" t="s">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" s="18" t="s">
         <v>173</v>
       </c>
-      <c r="B133" s="4" t="s">
+      <c r="B134" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="C133" s="5">
+      <c r="C134" s="5">
         <v>750</v>
       </c>
-      <c r="D133" s="6">
-        <f>D132+C133</f>
+      <c r="D134" s="6">
+        <f>D133+C134</f>
         <v>9640</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="18"/>
-    </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="18"/>
+      <c r="A135" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="B135" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C135" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D135" s="6">
+        <f>D134+C135</f>
+        <v>11640</v>
+      </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="18"/>
+      <c r="B136" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C136" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D136" s="6">
+        <f>D135+C136</f>
+        <v>13640</v>
+      </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="18"/>
+      <c r="B137" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C137" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D137" s="6">
+        <f>D136+C137</f>
+        <v>3640</v>
+      </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="18"/>
@@ -3012,6 +3055,9 @@
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" s="18"/>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
duy them ghi chu + tong ket
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="CÔ DIỄM" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="181">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -550,6 +550,18 @@
   </si>
   <si>
     <t>13/07/2024</t>
+  </si>
+  <si>
+    <t>chua lam giay</t>
+  </si>
+  <si>
+    <t>dau thang 8/2024 tra</t>
+  </si>
+  <si>
+    <t>12/08/2024 trả</t>
+  </si>
+  <si>
+    <t>đầu tháng 07 trả</t>
   </si>
 </sst>
 </file>
@@ -664,7 +676,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -721,6 +733,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1028,9 +1043,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K24" sqref="K24"/>
+      <selection pane="bottomLeft" activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1116,6 +1131,9 @@
       </c>
       <c r="I4" s="5">
         <v>10</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -3528,14 +3546,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.28515625" customWidth="1"/>
     <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="35" style="21" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3548,7 +3567,7 @@
         <v>108</v>
       </c>
       <c r="B10">
-        <v>390000</v>
+        <v>400000</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -3599,15 +3618,18 @@
         <v>8300</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>115</v>
       </c>
       <c r="B17">
         <v>2200</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" s="21" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>125</v>
       </c>
@@ -3615,29 +3637,35 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>147</v>
       </c>
       <c r="B19">
         <v>5000</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" s="21" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>151</v>
       </c>
       <c r="B20">
         <v>7000</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" s="21" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>5</v>
       </c>
       <c r="B32">
         <f>SUM(B10:B29)</f>
-        <v>521580</v>
+        <v>531580</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Duy chuyen cho co diem 350 + 300
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="CÔ DIỄM" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="183">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -552,9 +552,6 @@
     <t>13/07/2024</t>
   </si>
   <si>
-    <t>chua lam giay</t>
-  </si>
-  <si>
     <t>dau thang 8/2024 tra</t>
   </si>
   <si>
@@ -562,6 +559,15 @@
   </si>
   <si>
     <t>đầu tháng 07 trả</t>
+  </si>
+  <si>
+    <t>Chuyển cho cô Diễm 350k</t>
+  </si>
+  <si>
+    <t>14/07/2024</t>
+  </si>
+  <si>
+    <t>Chuyển cho cô Diễm 300k</t>
   </si>
 </sst>
 </file>
@@ -731,11 +737,11 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1041,16 +1047,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K165"/>
+  <dimension ref="A1:K139"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" style="18" customWidth="1"/>
     <col min="2" max="2" width="54.28515625" style="4" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" style="5" customWidth="1"/>
     <col min="4" max="4" width="25.5703125" style="6" customWidth="1"/>
@@ -1063,7 +1069,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -1075,14 +1081,14 @@
       <c r="D1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="20"/>
+      <c r="I1" s="21"/>
       <c r="J1" s="16"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="18" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1132,9 +1138,6 @@
       <c r="I4" s="5">
         <v>10</v>
       </c>
-      <c r="K4" s="6" t="s">
-        <v>177</v>
-      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -1173,9 +1176,6 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
-        <v>44966</v>
-      </c>
       <c r="B7" s="4" t="s">
         <v>19</v>
       </c>
@@ -1283,7 +1283,7 @@
       <c r="K16" s="15"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="18" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -1305,7 +1305,7 @@
       <c r="K17" s="15"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="18" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="4" t="s">
@@ -1390,7 +1390,7 @@
       <c r="K25" s="15"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="18" t="s">
         <v>24</v>
       </c>
       <c r="B26" s="4" t="s">
@@ -1485,9 +1485,6 @@
       <c r="K32" s="15"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="9">
-        <v>44967</v>
-      </c>
       <c r="B33" s="4" t="s">
         <v>26</v>
       </c>
@@ -1525,7 +1522,7 @@
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
+      <c r="A35" s="18" t="s">
         <v>39</v>
       </c>
       <c r="B35" s="4" t="s">
@@ -1546,7 +1543,7 @@
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="9" t="s">
+      <c r="A36" s="18" t="s">
         <v>41</v>
       </c>
       <c r="B36" s="4" t="s">
@@ -1587,7 +1584,7 @@
       <c r="K37" s="15"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="9" t="s">
+      <c r="A38" s="18" t="s">
         <v>42</v>
       </c>
       <c r="B38" s="4" t="s">
@@ -1609,7 +1606,7 @@
       <c r="K38" s="15"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
+      <c r="A39" s="18" t="s">
         <v>43</v>
       </c>
       <c r="B39" s="4" t="s">
@@ -1661,9 +1658,6 @@
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="9">
-        <v>44968</v>
-      </c>
       <c r="B42" s="4" t="s">
         <v>28</v>
       </c>
@@ -1688,9 +1682,6 @@
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="9">
-        <v>44996</v>
-      </c>
       <c r="B44" s="4" t="s">
         <v>52</v>
       </c>
@@ -1703,7 +1694,7 @@
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="9" t="s">
+      <c r="A45" s="18" t="s">
         <v>53</v>
       </c>
       <c r="B45" s="4" t="s">
@@ -1718,7 +1709,7 @@
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="9" t="s">
+      <c r="A46" s="18" t="s">
         <v>57</v>
       </c>
       <c r="B46" s="4" t="s">
@@ -1733,7 +1724,7 @@
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="9" t="s">
+      <c r="A47" s="18" t="s">
         <v>59</v>
       </c>
       <c r="B47" s="4" t="s">
@@ -1772,7 +1763,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="9">
+      <c r="A50" s="18">
         <v>44969</v>
       </c>
       <c r="B50" s="4" t="s">
@@ -1811,7 +1802,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="9" t="s">
+      <c r="A53" s="18" t="s">
         <v>64</v>
       </c>
       <c r="B53" s="4" t="s">
@@ -1826,7 +1817,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="9" t="s">
+      <c r="A54" s="18" t="s">
         <v>66</v>
       </c>
       <c r="B54" s="4" t="s">
@@ -1853,7 +1844,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="9" t="s">
+      <c r="A56" s="18" t="s">
         <v>68</v>
       </c>
       <c r="B56" s="4" t="s">
@@ -1880,7 +1871,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="9" t="s">
+      <c r="A58" s="18" t="s">
         <v>71</v>
       </c>
       <c r="B58" s="4" t="s">
@@ -1920,7 +1911,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="9" t="s">
+      <c r="A61" s="18" t="s">
         <v>75</v>
       </c>
       <c r="B61" s="4" t="s">
@@ -1935,9 +1926,6 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="9">
-        <v>45323</v>
-      </c>
       <c r="B62" s="4" t="s">
         <v>77</v>
       </c>
@@ -1986,7 +1974,7 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="9" t="s">
+      <c r="A66" s="18" t="s">
         <v>81</v>
       </c>
       <c r="B66" s="4" t="s">
@@ -2001,9 +1989,6 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="9">
-        <v>45474</v>
-      </c>
       <c r="B67" s="4" t="s">
         <v>77</v>
       </c>
@@ -2016,7 +2001,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="9" t="s">
+      <c r="A68" s="18" t="s">
         <v>82</v>
       </c>
       <c r="B68" s="4" t="s">
@@ -2031,7 +2016,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="9" t="s">
+      <c r="A69" s="18" t="s">
         <v>83</v>
       </c>
       <c r="B69" s="4" t="s">
@@ -2046,7 +2031,7 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="9" t="s">
+      <c r="A70" s="18" t="s">
         <v>84</v>
       </c>
       <c r="B70" s="4" t="s">
@@ -2073,7 +2058,7 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="9" t="s">
+      <c r="A72" s="18" t="s">
         <v>86</v>
       </c>
       <c r="B72" s="4" t="s">
@@ -2088,7 +2073,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="9" t="s">
+      <c r="A73" s="18" t="s">
         <v>88</v>
       </c>
       <c r="B73" s="4" t="s">
@@ -2127,9 +2112,6 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="9">
-        <v>45293</v>
-      </c>
       <c r="B76" s="4" t="s">
         <v>92</v>
       </c>
@@ -2154,9 +2136,6 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="9">
-        <v>45324</v>
-      </c>
       <c r="B78" s="4" t="s">
         <v>93</v>
       </c>
@@ -2169,7 +2148,7 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="9" t="s">
+      <c r="A79" s="18" t="s">
         <v>94</v>
       </c>
       <c r="B79" s="4" t="s">
@@ -2184,7 +2163,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="9" t="s">
+      <c r="A80" s="18" t="s">
         <v>96</v>
       </c>
       <c r="B80" s="4" t="s">
@@ -2211,7 +2190,7 @@
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="9" t="s">
+      <c r="A82" s="18" t="s">
         <v>98</v>
       </c>
       <c r="B82" s="4" t="s">
@@ -2226,9 +2205,6 @@
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="9">
-        <v>45294</v>
-      </c>
       <c r="B83" s="4" t="s">
         <v>100</v>
       </c>
@@ -2265,9 +2241,6 @@
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="9">
-        <v>45325</v>
-      </c>
       <c r="B86" s="4" t="s">
         <v>102</v>
       </c>
@@ -2292,9 +2265,6 @@
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="9">
-        <v>45507</v>
-      </c>
       <c r="B88" s="4" t="s">
         <v>103</v>
       </c>
@@ -2307,7 +2277,7 @@
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="9" t="s">
+      <c r="A89" s="18" t="s">
         <v>104</v>
       </c>
       <c r="B89" s="4" t="s">
@@ -2322,7 +2292,7 @@
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="9" t="s">
+      <c r="A90" s="18" t="s">
         <v>105</v>
       </c>
       <c r="B90" s="4" t="s">
@@ -2337,7 +2307,7 @@
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="9" t="s">
+      <c r="A91" s="18" t="s">
         <v>106</v>
       </c>
       <c r="B91" s="4" t="s">
@@ -2364,7 +2334,7 @@
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="9" t="s">
+      <c r="A93" s="18" t="s">
         <v>116</v>
       </c>
       <c r="B93" s="4" t="s">
@@ -2379,7 +2349,7 @@
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="9" t="s">
+      <c r="A94" s="18" t="s">
         <v>118</v>
       </c>
       <c r="B94" s="4" t="s">
@@ -2394,7 +2364,7 @@
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="9" t="s">
+      <c r="A95" s="18" t="s">
         <v>121</v>
       </c>
       <c r="B95" s="4" t="s">
@@ -2421,7 +2391,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="9" t="s">
+      <c r="A97" s="18" t="s">
         <v>124</v>
       </c>
       <c r="B97" s="4" t="s">
@@ -2436,9 +2406,6 @@
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="9">
-        <v>45295</v>
-      </c>
       <c r="B98" s="4" t="s">
         <v>65</v>
       </c>
@@ -2451,9 +2418,6 @@
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="9">
-        <v>45326</v>
-      </c>
       <c r="B99" s="4" t="s">
         <v>126</v>
       </c>
@@ -2478,7 +2442,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="9" t="s">
+      <c r="A101" s="18" t="s">
         <v>128</v>
       </c>
       <c r="B101" s="4" t="s">
@@ -2493,7 +2457,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="9" t="s">
+      <c r="A102" s="18" t="s">
         <v>130</v>
       </c>
       <c r="B102" s="4" t="s">
@@ -2520,7 +2484,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="9" t="s">
+      <c r="A104" s="18" t="s">
         <v>131</v>
       </c>
       <c r="B104" s="4" t="s">
@@ -2535,7 +2499,7 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="9" t="s">
+      <c r="A105" s="18" t="s">
         <v>132</v>
       </c>
       <c r="B105" s="4" t="s">
@@ -2562,9 +2526,6 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="9">
-        <v>45327</v>
-      </c>
       <c r="B107" s="4" t="s">
         <v>133</v>
       </c>
@@ -2601,7 +2562,7 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="9" t="s">
+      <c r="A110" s="18" t="s">
         <v>135</v>
       </c>
       <c r="B110" s="4" t="s">
@@ -2616,7 +2577,7 @@
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="9" t="s">
+      <c r="A111" s="18" t="s">
         <v>136</v>
       </c>
       <c r="B111" s="4" t="s">
@@ -2643,7 +2604,7 @@
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="9" t="s">
+      <c r="A113" s="18" t="s">
         <v>137</v>
       </c>
       <c r="B113" s="4" t="s">
@@ -2658,7 +2619,7 @@
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="9" t="s">
+      <c r="A114" s="18" t="s">
         <v>138</v>
       </c>
       <c r="B114" s="4" t="s">
@@ -2685,7 +2646,7 @@
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="9" t="s">
+      <c r="A116" s="18" t="s">
         <v>140</v>
       </c>
       <c r="B116" s="4" t="s">
@@ -2712,7 +2673,6 @@
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="18"/>
       <c r="B118" s="4" t="s">
         <v>20</v>
       </c>
@@ -2725,9 +2685,6 @@
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="18">
-        <v>45297</v>
-      </c>
       <c r="B119" s="4" t="s">
         <v>65</v>
       </c>
@@ -2740,9 +2697,6 @@
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="18">
-        <v>45328</v>
-      </c>
       <c r="B120" s="4" t="s">
         <v>100</v>
       </c>
@@ -2755,7 +2709,6 @@
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="18"/>
       <c r="B121" s="4" t="s">
         <v>20</v>
       </c>
@@ -2798,7 +2751,6 @@
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="18"/>
       <c r="B124" s="4" t="s">
         <v>20</v>
       </c>
@@ -2841,7 +2793,6 @@
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="18"/>
       <c r="B127" s="4" t="s">
         <v>20</v>
       </c>
@@ -2884,7 +2835,6 @@
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="18"/>
       <c r="B130" s="4" t="s">
         <v>20</v>
       </c>
@@ -2897,7 +2847,6 @@
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="18"/>
       <c r="B131" s="4" t="s">
         <v>156</v>
       </c>
@@ -2925,7 +2874,6 @@
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="18"/>
       <c r="B133" s="4" t="s">
         <v>172</v>
       </c>
@@ -2968,7 +2916,6 @@
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="18"/>
       <c r="B136" s="4" t="s">
         <v>65</v>
       </c>
@@ -2981,7 +2928,6 @@
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="18"/>
       <c r="B137" s="4" t="s">
         <v>20</v>
       </c>
@@ -2994,88 +2940,31 @@
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="18"/>
+      <c r="B138" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C138" s="5">
+        <v>350</v>
+      </c>
+      <c r="D138" s="6">
+        <f>D137+C138</f>
+        <v>3990</v>
+      </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="18"/>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="18"/>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="18"/>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="18"/>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="18"/>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="18"/>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" s="18"/>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" s="18"/>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" s="18"/>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148" s="18"/>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A149" s="18"/>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" s="18"/>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151" s="18"/>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152" s="18"/>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" s="18"/>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154" s="18"/>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155" s="18"/>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A156" s="18"/>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A157" s="18"/>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158" s="18"/>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A159" s="18"/>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A160" s="18"/>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161" s="18"/>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A162" s="18"/>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A163" s="18"/>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164" s="18"/>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A165" s="18"/>
+      <c r="A139" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="B139" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C139" s="5">
+        <v>300</v>
+      </c>
+      <c r="D139" s="6">
+        <f>D138+C139</f>
+        <v>4290</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3125,10 +3014,10 @@
       <c r="E1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="20"/>
+      <c r="I1" s="21"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
@@ -3264,10 +3153,10 @@
       <c r="E1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="20"/>
+      <c r="I1" s="21"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -3460,10 +3349,10 @@
       <c r="E1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="20"/>
+      <c r="I1" s="21"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -3546,7 +3435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
@@ -3554,7 +3443,7 @@
   <cols>
     <col min="1" max="1" width="37.28515625" customWidth="1"/>
     <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="35" style="21" customWidth="1"/>
+    <col min="3" max="3" width="35" style="20" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3625,8 +3514,8 @@
       <c r="B17">
         <v>2200</v>
       </c>
-      <c r="C17" s="21" t="s">
-        <v>179</v>
+      <c r="C17" s="20" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -3644,8 +3533,8 @@
       <c r="B19">
         <v>5000</v>
       </c>
-      <c r="C19" s="21" t="s">
-        <v>178</v>
+      <c r="C19" s="20" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -3655,8 +3544,8 @@
       <c r="B20">
         <v>7000</v>
       </c>
-      <c r="C20" s="21" t="s">
-        <v>180</v>
+      <c r="C20" s="20" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Thach tra no 7tr
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="181">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -474,9 +474,6 @@
     <t>23/06/2024</t>
   </si>
   <si>
-    <t>Thạch</t>
-  </si>
-  <si>
     <t>30/06/2024</t>
   </si>
   <si>
@@ -556,9 +553,6 @@
   </si>
   <si>
     <t>12/08/2024 trả</t>
-  </si>
-  <si>
-    <t>đầu tháng 07 trả</t>
   </si>
   <si>
     <t>Chuyển cho cô Diễm 350k</t>
@@ -682,7 +676,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -723,7 +717,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1050,18 +1043,18 @@
   <dimension ref="A1:K139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K4" sqref="K4"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" style="18" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" style="17" customWidth="1"/>
     <col min="2" max="2" width="54.28515625" style="4" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" style="5" customWidth="1"/>
     <col min="4" max="4" width="25.5703125" style="6" customWidth="1"/>
     <col min="5" max="7" width="9.140625" style="6"/>
-    <col min="8" max="8" width="12.7109375" style="18" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="17" customWidth="1"/>
     <col min="9" max="9" width="29.5703125" style="5" customWidth="1"/>
     <col min="10" max="10" width="14.28515625" style="4" customWidth="1"/>
     <col min="11" max="11" width="26" style="6" customWidth="1"/>
@@ -1069,7 +1062,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -1081,14 +1074,14 @@
       <c r="D1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="21"/>
-      <c r="J1" s="16"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="15"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1097,7 +1090,7 @@
       <c r="C2" s="5">
         <v>1930</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="18" t="s">
         <v>2</v>
       </c>
       <c r="I2" s="3" t="s">
@@ -1120,7 +1113,7 @@
       <c r="D3" s="6">
         <v>3930</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="17" t="s">
         <v>6</v>
       </c>
       <c r="I3" s="5">
@@ -1132,8 +1125,8 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H4" s="18" t="s">
-        <v>176</v>
+      <c r="H4" s="17" t="s">
+        <v>175</v>
       </c>
       <c r="I4" s="5">
         <v>10</v>
@@ -1150,7 +1143,7 @@
         <f>C5+D3</f>
         <v>18490</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="17" t="s">
         <v>7</v>
       </c>
       <c r="I5" s="5">
@@ -1168,7 +1161,7 @@
         <f t="shared" ref="D6:D18" si="0">D5+C6</f>
         <v>8490</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="H6" s="17" t="s">
         <v>8</v>
       </c>
       <c r="I6" s="5">
@@ -1186,7 +1179,7 @@
         <f t="shared" si="0"/>
         <v>10490</v>
       </c>
-      <c r="H7" s="18" t="s">
+      <c r="H7" s="17" t="s">
         <v>9</v>
       </c>
       <c r="I7" s="5">
@@ -1194,7 +1187,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H8" s="18" t="s">
+      <c r="H8" s="17" t="s">
         <v>41</v>
       </c>
       <c r="I8" s="5">
@@ -1202,52 +1195,52 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H9" s="18" t="s">
+      <c r="H9" s="17" t="s">
         <v>84</v>
       </c>
       <c r="I9" s="5">
         <v>10</v>
       </c>
-      <c r="K9" s="15"/>
+      <c r="K9" s="14"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H10" s="18" t="s">
+      <c r="H10" s="17" t="s">
         <v>96</v>
       </c>
       <c r="I10" s="5">
         <v>10</v>
       </c>
-      <c r="K10" s="15"/>
+      <c r="K10" s="14"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H11" s="18" t="s">
+      <c r="H11" s="17" t="s">
         <v>130</v>
       </c>
       <c r="I11" s="5">
         <v>10</v>
       </c>
-      <c r="K11" s="15"/>
+      <c r="K11" s="14"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H12" s="18" t="s">
+      <c r="H12" s="17" t="s">
         <v>136</v>
       </c>
       <c r="I12" s="5">
         <v>10</v>
       </c>
-      <c r="K12" s="15"/>
+      <c r="K12" s="14"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H13" s="18" t="s">
+      <c r="H13" s="17" t="s">
         <v>149</v>
       </c>
       <c r="I13" s="5">
         <v>10</v>
       </c>
-      <c r="K13" s="15"/>
+      <c r="K13" s="14"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H14" s="18" t="s">
+      <c r="H14" s="17" t="s">
         <v>70</v>
       </c>
       <c r="I14" s="5">
@@ -1255,13 +1248,13 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H15" s="18" t="s">
+      <c r="H15" s="17" t="s">
         <v>107</v>
       </c>
       <c r="I15" s="5">
         <v>10</v>
       </c>
-      <c r="K15" s="15"/>
+      <c r="K15" s="14"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
@@ -1274,16 +1267,16 @@
         <f>D7+C16</f>
         <v>490</v>
       </c>
-      <c r="H16" s="18" t="s">
+      <c r="H16" s="17" t="s">
         <v>10</v>
       </c>
       <c r="I16" s="5">
         <v>10</v>
       </c>
-      <c r="K16" s="15"/>
+      <c r="K16" s="14"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="17" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -1296,16 +1289,16 @@
         <f t="shared" si="0"/>
         <v>2490</v>
       </c>
-      <c r="H17" s="18" t="s">
+      <c r="H17" s="17" t="s">
         <v>11</v>
       </c>
       <c r="I17" s="5">
         <v>10</v>
       </c>
-      <c r="K17" s="15"/>
+      <c r="K17" s="14"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="17" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="4" t="s">
@@ -1318,79 +1311,79 @@
         <f t="shared" si="0"/>
         <v>5490</v>
       </c>
-      <c r="H18" s="18" t="s">
+      <c r="H18" s="17" t="s">
         <v>24</v>
       </c>
       <c r="I18" s="5">
         <v>10</v>
       </c>
-      <c r="K18" s="15"/>
+      <c r="K18" s="14"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H19" s="18" t="s">
+      <c r="H19" s="17" t="s">
         <v>59</v>
       </c>
       <c r="I19" s="5">
         <v>10</v>
       </c>
-      <c r="K19" s="15"/>
+      <c r="K19" s="14"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H20" s="18" t="s">
+      <c r="H20" s="17" t="s">
         <v>73</v>
       </c>
       <c r="I20" s="5">
         <v>10</v>
       </c>
-      <c r="K20" s="15"/>
+      <c r="K20" s="14"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H21" s="18" t="s">
+      <c r="H21" s="17" t="s">
         <v>91</v>
       </c>
       <c r="I21" s="5">
         <v>10</v>
       </c>
-      <c r="K21" s="15"/>
+      <c r="K21" s="14"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H22" s="18" t="s">
+      <c r="H22" s="17" t="s">
         <v>121</v>
       </c>
       <c r="I22" s="5">
         <v>10</v>
       </c>
-      <c r="K22" s="15"/>
+      <c r="K22" s="14"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H23" s="18" t="s">
+      <c r="H23" s="17" t="s">
         <v>132</v>
       </c>
       <c r="I23" s="5">
         <v>10</v>
       </c>
-      <c r="K23" s="15"/>
+      <c r="K23" s="14"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H24" s="18" t="s">
+      <c r="H24" s="17" t="s">
         <v>138</v>
       </c>
       <c r="I24" s="5">
         <v>10</v>
       </c>
-      <c r="K24" s="15"/>
+      <c r="K24" s="14"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H25" s="18" t="s">
-        <v>152</v>
+      <c r="H25" s="17" t="s">
+        <v>151</v>
       </c>
       <c r="I25" s="5">
         <v>10</v>
       </c>
-      <c r="K25" s="15"/>
+      <c r="K25" s="14"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="18" t="s">
+      <c r="A26" s="17" t="s">
         <v>24</v>
       </c>
       <c r="B26" s="4" t="s">
@@ -1403,7 +1396,7 @@
         <f>D18+C26</f>
         <v>8490</v>
       </c>
-      <c r="H26" s="18" t="s">
+      <c r="H26" s="17" t="s">
         <v>12</v>
       </c>
       <c r="I26" s="5">
@@ -1411,40 +1404,40 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H27" s="18" t="s">
+      <c r="H27" s="17" t="s">
         <v>43</v>
       </c>
       <c r="I27" s="5">
         <v>10</v>
       </c>
-      <c r="K27" s="15"/>
+      <c r="K27" s="14"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H28" s="18" t="s">
+      <c r="H28" s="17" t="s">
         <v>146</v>
       </c>
       <c r="I28" s="5">
         <v>10</v>
       </c>
-      <c r="K28" s="15"/>
+      <c r="K28" s="14"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H29" s="18" t="s">
-        <v>163</v>
+      <c r="H29" s="17" t="s">
+        <v>162</v>
       </c>
       <c r="I29" s="5">
         <v>10</v>
       </c>
-      <c r="K29" s="15"/>
+      <c r="K29" s="14"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H30" s="18" t="s">
-        <v>164</v>
+      <c r="H30" s="17" t="s">
+        <v>163</v>
       </c>
       <c r="I30" s="5">
         <v>10</v>
       </c>
-      <c r="K30" s="15"/>
+      <c r="K30" s="14"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
@@ -1457,13 +1450,13 @@
         <f>D26+C31</f>
         <v>12890</v>
       </c>
-      <c r="H31" s="18" t="s">
-        <v>165</v>
+      <c r="H31" s="17" t="s">
+        <v>164</v>
       </c>
       <c r="I31" s="5">
         <v>20</v>
       </c>
-      <c r="K31" s="15"/>
+      <c r="K31" s="14"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
@@ -1476,13 +1469,13 @@
         <f>D31+C32</f>
         <v>2890</v>
       </c>
-      <c r="H32" s="18" t="s">
-        <v>166</v>
+      <c r="H32" s="17" t="s">
+        <v>165</v>
       </c>
       <c r="I32" s="5">
         <v>10</v>
       </c>
-      <c r="K32" s="15"/>
+      <c r="K32" s="14"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
@@ -1495,13 +1488,13 @@
         <f t="shared" ref="D33:D40" si="1">D32+C33</f>
         <v>4490</v>
       </c>
-      <c r="H33" s="18" t="s">
-        <v>167</v>
+      <c r="H33" s="17" t="s">
+        <v>166</v>
       </c>
       <c r="I33" s="5">
         <v>10</v>
       </c>
-      <c r="K33" s="15"/>
+      <c r="K33" s="14"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
@@ -1514,15 +1507,15 @@
         <f t="shared" si="1"/>
         <v>7490</v>
       </c>
-      <c r="H34" s="18" t="s">
-        <v>168</v>
+      <c r="H34" s="17" t="s">
+        <v>167</v>
       </c>
       <c r="I34" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="18" t="s">
+      <c r="A35" s="17" t="s">
         <v>39</v>
       </c>
       <c r="B35" s="4" t="s">
@@ -1535,15 +1528,15 @@
         <f t="shared" si="1"/>
         <v>9490</v>
       </c>
-      <c r="H35" s="18" t="s">
-        <v>162</v>
+      <c r="H35" s="17" t="s">
+        <v>161</v>
       </c>
       <c r="I35" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="18" t="s">
+      <c r="A36" s="17" t="s">
         <v>41</v>
       </c>
       <c r="B36" s="4" t="s">
@@ -1556,13 +1549,13 @@
         <f t="shared" si="1"/>
         <v>12490</v>
       </c>
-      <c r="H36" s="18" t="s">
-        <v>161</v>
+      <c r="H36" s="17" t="s">
+        <v>160</v>
       </c>
       <c r="I36" s="5">
         <v>10</v>
       </c>
-      <c r="K36" s="15"/>
+      <c r="K36" s="14"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
@@ -1575,16 +1568,16 @@
         <f t="shared" si="1"/>
         <v>2490</v>
       </c>
-      <c r="H37" s="18" t="s">
-        <v>160</v>
+      <c r="H37" s="17" t="s">
+        <v>159</v>
       </c>
       <c r="I37" s="5">
         <v>10</v>
       </c>
-      <c r="K37" s="15"/>
+      <c r="K37" s="14"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="18" t="s">
+      <c r="A38" s="17" t="s">
         <v>42</v>
       </c>
       <c r="B38" s="4" t="s">
@@ -1597,16 +1590,16 @@
         <f t="shared" si="1"/>
         <v>7450</v>
       </c>
-      <c r="H38" s="18" t="s">
-        <v>159</v>
+      <c r="H38" s="17" t="s">
+        <v>158</v>
       </c>
       <c r="I38" s="5">
         <v>10</v>
       </c>
-      <c r="K38" s="15"/>
+      <c r="K38" s="14"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="18" t="s">
+      <c r="A39" s="17" t="s">
         <v>43</v>
       </c>
       <c r="B39" s="4" t="s">
@@ -1619,8 +1612,8 @@
         <f t="shared" si="1"/>
         <v>11450</v>
       </c>
-      <c r="H39" s="18" t="s">
-        <v>158</v>
+      <c r="H39" s="17" t="s">
+        <v>157</v>
       </c>
       <c r="I39" s="5">
         <v>10</v>
@@ -1637,13 +1630,13 @@
         <f t="shared" si="1"/>
         <v>1450</v>
       </c>
-      <c r="H40" s="18" t="s">
-        <v>157</v>
+      <c r="H40" s="17" t="s">
+        <v>156</v>
       </c>
       <c r="I40" s="5">
         <v>10</v>
       </c>
-      <c r="K40" s="15"/>
+      <c r="K40" s="14"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
@@ -1694,7 +1687,7 @@
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="18" t="s">
+      <c r="A45" s="17" t="s">
         <v>53</v>
       </c>
       <c r="B45" s="4" t="s">
@@ -1709,7 +1702,7 @@
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="18" t="s">
+      <c r="A46" s="17" t="s">
         <v>57</v>
       </c>
       <c r="B46" s="4" t="s">
@@ -1724,7 +1717,7 @@
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="18" t="s">
+      <c r="A47" s="17" t="s">
         <v>59</v>
       </c>
       <c r="B47" s="4" t="s">
@@ -1763,7 +1756,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="18">
+      <c r="A50" s="17">
         <v>44969</v>
       </c>
       <c r="B50" s="4" t="s">
@@ -1802,7 +1795,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="18" t="s">
+      <c r="A53" s="17" t="s">
         <v>64</v>
       </c>
       <c r="B53" s="4" t="s">
@@ -1817,7 +1810,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="18" t="s">
+      <c r="A54" s="17" t="s">
         <v>66</v>
       </c>
       <c r="B54" s="4" t="s">
@@ -1844,7 +1837,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="18" t="s">
+      <c r="A56" s="17" t="s">
         <v>68</v>
       </c>
       <c r="B56" s="4" t="s">
@@ -1871,7 +1864,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="18" t="s">
+      <c r="A58" s="17" t="s">
         <v>71</v>
       </c>
       <c r="B58" s="4" t="s">
@@ -1911,7 +1904,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="18" t="s">
+      <c r="A61" s="17" t="s">
         <v>75</v>
       </c>
       <c r="B61" s="4" t="s">
@@ -1974,7 +1967,7 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="18" t="s">
+      <c r="A66" s="17" t="s">
         <v>81</v>
       </c>
       <c r="B66" s="4" t="s">
@@ -2001,7 +1994,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="18" t="s">
+      <c r="A68" s="17" t="s">
         <v>82</v>
       </c>
       <c r="B68" s="4" t="s">
@@ -2016,7 +2009,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="18" t="s">
+      <c r="A69" s="17" t="s">
         <v>83</v>
       </c>
       <c r="B69" s="4" t="s">
@@ -2031,7 +2024,7 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="18" t="s">
+      <c r="A70" s="17" t="s">
         <v>84</v>
       </c>
       <c r="B70" s="4" t="s">
@@ -2058,7 +2051,7 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="18" t="s">
+      <c r="A72" s="17" t="s">
         <v>86</v>
       </c>
       <c r="B72" s="4" t="s">
@@ -2073,7 +2066,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="18" t="s">
+      <c r="A73" s="17" t="s">
         <v>88</v>
       </c>
       <c r="B73" s="4" t="s">
@@ -2148,7 +2141,7 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="18" t="s">
+      <c r="A79" s="17" t="s">
         <v>94</v>
       </c>
       <c r="B79" s="4" t="s">
@@ -2163,7 +2156,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="18" t="s">
+      <c r="A80" s="17" t="s">
         <v>96</v>
       </c>
       <c r="B80" s="4" t="s">
@@ -2190,7 +2183,7 @@
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="18" t="s">
+      <c r="A82" s="17" t="s">
         <v>98</v>
       </c>
       <c r="B82" s="4" t="s">
@@ -2277,7 +2270,7 @@
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="18" t="s">
+      <c r="A89" s="17" t="s">
         <v>104</v>
       </c>
       <c r="B89" s="4" t="s">
@@ -2292,7 +2285,7 @@
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="18" t="s">
+      <c r="A90" s="17" t="s">
         <v>105</v>
       </c>
       <c r="B90" s="4" t="s">
@@ -2307,7 +2300,7 @@
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="18" t="s">
+      <c r="A91" s="17" t="s">
         <v>106</v>
       </c>
       <c r="B91" s="4" t="s">
@@ -2334,7 +2327,7 @@
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="18" t="s">
+      <c r="A93" s="17" t="s">
         <v>116</v>
       </c>
       <c r="B93" s="4" t="s">
@@ -2349,7 +2342,7 @@
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="18" t="s">
+      <c r="A94" s="17" t="s">
         <v>118</v>
       </c>
       <c r="B94" s="4" t="s">
@@ -2364,7 +2357,7 @@
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="18" t="s">
+      <c r="A95" s="17" t="s">
         <v>121</v>
       </c>
       <c r="B95" s="4" t="s">
@@ -2391,7 +2384,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="18" t="s">
+      <c r="A97" s="17" t="s">
         <v>124</v>
       </c>
       <c r="B97" s="4" t="s">
@@ -2442,7 +2435,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="18" t="s">
+      <c r="A101" s="17" t="s">
         <v>128</v>
       </c>
       <c r="B101" s="4" t="s">
@@ -2457,7 +2450,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="18" t="s">
+      <c r="A102" s="17" t="s">
         <v>130</v>
       </c>
       <c r="B102" s="4" t="s">
@@ -2484,7 +2477,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="18" t="s">
+      <c r="A104" s="17" t="s">
         <v>131</v>
       </c>
       <c r="B104" s="4" t="s">
@@ -2499,7 +2492,7 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="18" t="s">
+      <c r="A105" s="17" t="s">
         <v>132</v>
       </c>
       <c r="B105" s="4" t="s">
@@ -2562,7 +2555,7 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="18" t="s">
+      <c r="A110" s="17" t="s">
         <v>135</v>
       </c>
       <c r="B110" s="4" t="s">
@@ -2577,7 +2570,7 @@
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="18" t="s">
+      <c r="A111" s="17" t="s">
         <v>136</v>
       </c>
       <c r="B111" s="4" t="s">
@@ -2604,7 +2597,7 @@
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="18" t="s">
+      <c r="A113" s="17" t="s">
         <v>137</v>
       </c>
       <c r="B113" s="4" t="s">
@@ -2619,7 +2612,7 @@
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="18" t="s">
+      <c r="A114" s="17" t="s">
         <v>138</v>
       </c>
       <c r="B114" s="4" t="s">
@@ -2646,7 +2639,7 @@
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="18" t="s">
+      <c r="A116" s="17" t="s">
         <v>140</v>
       </c>
       <c r="B116" s="4" t="s">
@@ -2721,7 +2714,7 @@
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="18" t="s">
+      <c r="A122" s="17" t="s">
         <v>148</v>
       </c>
       <c r="B122" s="4" t="s">
@@ -2736,7 +2729,7 @@
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="18" t="s">
+      <c r="A123" s="17" t="s">
         <v>149</v>
       </c>
       <c r="B123" s="4" t="s">
@@ -2763,7 +2756,7 @@
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="18" t="s">
+      <c r="A125" s="17" t="s">
         <v>150</v>
       </c>
       <c r="B125" s="4" t="s">
@@ -2778,11 +2771,11 @@
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="18" t="s">
+      <c r="A126" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="B126" s="4" t="s">
         <v>152</v>
-      </c>
-      <c r="B126" s="4" t="s">
-        <v>153</v>
       </c>
       <c r="C126" s="5">
         <v>12000</v>
@@ -2805,11 +2798,11 @@
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="18" t="s">
-        <v>169</v>
+      <c r="A128" s="17" t="s">
+        <v>168</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C128" s="5">
         <v>2000</v>
@@ -2820,11 +2813,11 @@
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="18" t="s">
-        <v>157</v>
+      <c r="A129" s="17" t="s">
+        <v>156</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C129" s="5">
         <v>10000</v>
@@ -2848,7 +2841,7 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B131" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C131" s="5">
         <v>2000</v>
@@ -2859,11 +2852,11 @@
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="18" t="s">
+      <c r="A132" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="B132" s="4" t="s">
         <v>170</v>
-      </c>
-      <c r="B132" s="4" t="s">
-        <v>171</v>
       </c>
       <c r="C132" s="5">
         <v>-1200</v>
@@ -2875,7 +2868,7 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B133" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C133" s="5">
         <v>500</v>
@@ -2886,23 +2879,23 @@
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="18" t="s">
+      <c r="A134" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="B134" s="4" t="s">
         <v>173</v>
-      </c>
-      <c r="B134" s="4" t="s">
-        <v>174</v>
       </c>
       <c r="C134" s="5">
         <v>750</v>
       </c>
       <c r="D134" s="6">
-        <f>D133+C134</f>
+        <f t="shared" ref="D134:D139" si="17">D133+C134</f>
         <v>9640</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="18" t="s">
-        <v>175</v>
+      <c r="A135" s="17" t="s">
+        <v>174</v>
       </c>
       <c r="B135" s="4" t="s">
         <v>134</v>
@@ -2911,7 +2904,7 @@
         <v>2000</v>
       </c>
       <c r="D135" s="6">
-        <f>D134+C135</f>
+        <f t="shared" si="17"/>
         <v>11640</v>
       </c>
     </row>
@@ -2923,7 +2916,7 @@
         <v>2000</v>
       </c>
       <c r="D136" s="6">
-        <f>D135+C136</f>
+        <f t="shared" si="17"/>
         <v>13640</v>
       </c>
     </row>
@@ -2935,34 +2928,34 @@
         <v>-10000</v>
       </c>
       <c r="D137" s="6">
-        <f>D136+C137</f>
+        <f t="shared" si="17"/>
         <v>3640</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B138" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C138" s="5">
         <v>350</v>
       </c>
       <c r="D138" s="6">
-        <f>D137+C138</f>
+        <f t="shared" si="17"/>
         <v>3990</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="18" t="s">
-        <v>181</v>
+      <c r="A139" s="17" t="s">
+        <v>179</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C139" s="5">
         <v>300</v>
       </c>
       <c r="D139" s="6">
-        <f>D138+C139</f>
+        <f t="shared" si="17"/>
         <v>4290</v>
       </c>
     </row>
@@ -3014,10 +3007,10 @@
       <c r="E1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="21"/>
+      <c r="I1" s="20"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
@@ -3153,10 +3146,10 @@
       <c r="E1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="21"/>
+      <c r="I1" s="20"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -3349,10 +3342,10 @@
       <c r="E1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="21"/>
+      <c r="I1" s="20"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -3433,128 +3426,113 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.28515625" customWidth="1"/>
     <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="35" style="20" customWidth="1"/>
+    <col min="3" max="3" width="35" style="19" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5">
+        <v>7580</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B6">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7">
+        <v>8300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8">
+        <v>2200</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B9">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>108</v>
+        <v>147</v>
       </c>
       <c r="B10">
-        <v>400000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>109</v>
-      </c>
-      <c r="B11">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>110</v>
-      </c>
-      <c r="B12">
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>111</v>
-      </c>
-      <c r="B13">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>112</v>
-      </c>
-      <c r="B14">
-        <v>7580</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>113</v>
-      </c>
-      <c r="B15">
-        <v>5500</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>114</v>
-      </c>
-      <c r="B16">
-        <v>8300</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>115</v>
-      </c>
-      <c r="B17">
-        <v>2200</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>125</v>
-      </c>
-      <c r="B18">
-        <v>11000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>147</v>
-      </c>
-      <c r="B19">
         <v>5000</v>
       </c>
-      <c r="C19" s="20" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>151</v>
-      </c>
-      <c r="B20">
-        <v>7000</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="C10" s="19" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>5</v>
       </c>
-      <c r="B32">
-        <f>SUM(B10:B29)</f>
-        <v>531580</v>
+      <c r="B23">
+        <f>SUM(B1:B20)</f>
+        <v>524580</v>
       </c>
     </row>
   </sheetData>
@@ -3609,10 +3587,10 @@
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="B15" s="17">
+      <c r="B15" s="16">
         <f>SUM(B1:B13)</f>
         <v>2500</v>
       </c>

</xml_diff>

<commit_message>
duy chuyen cho co diem 3800k
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="183">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -562,6 +562,12 @@
   </si>
   <si>
     <t>Chuyển cho cô Diễm 300k</t>
+  </si>
+  <si>
+    <t>18/07/2024</t>
+  </si>
+  <si>
+    <t>Chuyển cho cô Diễm 3tr</t>
   </si>
 </sst>
 </file>
@@ -1040,11 +1046,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K139"/>
+  <dimension ref="A1:K140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K40" sqref="K40"/>
+      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F143" sqref="F143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2957,6 +2963,21 @@
       <c r="D139" s="6">
         <f t="shared" si="17"/>
         <v>4290</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="B140" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C140" s="5">
+        <v>3800</v>
+      </c>
+      <c r="D140" s="6">
+        <f>D139+C140</f>
+        <v>8090</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Duy chuyen cho co diem them 500k
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="183">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -567,7 +567,7 @@
     <t>18/07/2024</t>
   </si>
   <si>
-    <t>Chuyển cho cô Diễm 3tr</t>
+    <t>Chuyển cho cô Diễm 3.8tr</t>
   </si>
 </sst>
 </file>
@@ -1046,11 +1046,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K140"/>
+  <dimension ref="A1:K141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F143" sqref="F143"/>
+      <selection pane="bottomLeft" activeCell="D142" sqref="D142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2978,6 +2978,18 @@
       <c r="D140" s="6">
         <f>D139+C140</f>
         <v>8090</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B141" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C141" s="5">
+        <v>500</v>
+      </c>
+      <c r="D141" s="6">
+        <f>D140+C141</f>
+        <v>8590</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
duy chuyen cho co diem 1300
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="185">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -568,6 +568,12 @@
   </si>
   <si>
     <t>Chuyển cho cô Diễm 3.8tr</t>
+  </si>
+  <si>
+    <t>20/07/2024</t>
+  </si>
+  <si>
+    <t>Duy chyển cho cô Diễm 1300k</t>
   </si>
 </sst>
 </file>
@@ -1046,11 +1052,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K141"/>
+  <dimension ref="A1:K142"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D142" sqref="D142"/>
+      <selection pane="bottomLeft" activeCell="E146" sqref="E146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2990,6 +2996,21 @@
       <c r="D141" s="6">
         <f>D140+C141</f>
         <v>8590</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="B142" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C142" s="5">
+        <v>1300</v>
+      </c>
+      <c r="D142" s="6">
+        <f>D141+C142</f>
+        <v>9890</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Duy lay tien loi ngay 2107
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="186">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -574,6 +574,9 @@
   </si>
   <si>
     <t>Duy chyển cho cô Diễm 1300k</t>
+  </si>
+  <si>
+    <t>21/07/2024</t>
   </si>
 </sst>
 </file>
@@ -1052,11 +1055,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K142"/>
+  <dimension ref="A1:K145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E146" sqref="E146"/>
+      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,7 +1067,7 @@
     <col min="1" max="1" width="16.140625" style="17" customWidth="1"/>
     <col min="2" max="2" width="54.28515625" style="4" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="25.5703125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" style="4" customWidth="1"/>
     <col min="5" max="7" width="9.140625" style="6"/>
     <col min="8" max="8" width="12.7109375" style="17" customWidth="1"/>
     <col min="9" max="9" width="29.5703125" style="5" customWidth="1"/>
@@ -1083,7 +1086,7 @@
       <c r="C1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="12" t="s">
         <v>15</v>
       </c>
       <c r="H1" s="20" t="s">
@@ -1122,7 +1125,7 @@
       <c r="C3" s="5">
         <v>2000</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="4">
         <v>3930</v>
       </c>
       <c r="H3" s="17" t="s">
@@ -1132,8 +1135,8 @@
         <v>20</v>
       </c>
       <c r="J3" s="4">
-        <f>SUM(I3:I56)</f>
-        <v>400</v>
+        <f>SUM(I3:I57)</f>
+        <v>410</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1151,7 +1154,7 @@
       <c r="C5" s="5">
         <v>14560</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="4">
         <f>C5+D3</f>
         <v>18490</v>
       </c>
@@ -1169,8 +1172,8 @@
       <c r="C6" s="5">
         <v>-10000</v>
       </c>
-      <c r="D6" s="6">
-        <f t="shared" ref="D6:D18" si="0">D5+C6</f>
+      <c r="D6" s="4">
+        <f t="shared" ref="D6:D19" si="0">D5+C6</f>
         <v>8490</v>
       </c>
       <c r="H6" s="17" t="s">
@@ -1187,7 +1190,7 @@
       <c r="C7" s="5">
         <v>2000</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="4">
         <f t="shared" si="0"/>
         <v>10490</v>
       </c>
@@ -1253,34 +1256,24 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H14" s="17" t="s">
-        <v>70</v>
+        <v>185</v>
       </c>
       <c r="I14" s="5">
         <v>10</v>
       </c>
+      <c r="K14" s="14"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H15" s="17" t="s">
-        <v>107</v>
+        <v>70</v>
       </c>
       <c r="I15" s="5">
         <v>10</v>
       </c>
-      <c r="K15" s="14"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="5">
-        <v>-10000</v>
-      </c>
-      <c r="D16" s="6">
-        <f>D7+C16</f>
-        <v>490</v>
-      </c>
       <c r="H16" s="17" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="I16" s="5">
         <v>10</v>
@@ -1288,52 +1281,62 @@
       <c r="K16" s="14"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
+      <c r="B17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D17" s="4">
+        <f>D7+C17</f>
+        <v>490</v>
+      </c>
+      <c r="H17" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I17" s="5">
+        <v>10</v>
+      </c>
+      <c r="K17" s="14"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B18" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C18" s="5">
         <v>2000</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D18" s="4">
         <f t="shared" si="0"/>
         <v>2490</v>
       </c>
-      <c r="H17" s="17" t="s">
+      <c r="H18" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I17" s="5">
+      <c r="I18" s="5">
         <v>10</v>
       </c>
-      <c r="K17" s="14"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
+      <c r="K18" s="14"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B19" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C19" s="5">
         <v>3000</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D19" s="4">
         <f t="shared" si="0"/>
         <v>5490</v>
       </c>
-      <c r="H18" s="17" t="s">
+      <c r="H19" s="17" t="s">
         <v>24</v>
-      </c>
-      <c r="I18" s="5">
-        <v>10</v>
-      </c>
-      <c r="K18" s="14"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H19" s="17" t="s">
-        <v>59</v>
       </c>
       <c r="I19" s="5">
         <v>10</v>
@@ -1342,7 +1345,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H20" s="17" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="I20" s="5">
         <v>10</v>
@@ -1351,7 +1354,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H21" s="17" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="I21" s="5">
         <v>10</v>
@@ -1360,7 +1363,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H22" s="17" t="s">
-        <v>121</v>
+        <v>91</v>
       </c>
       <c r="I22" s="5">
         <v>10</v>
@@ -1369,7 +1372,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H23" s="17" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="I23" s="5">
         <v>10</v>
@@ -1378,7 +1381,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H24" s="17" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="I24" s="5">
         <v>10</v>
@@ -1387,7 +1390,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H25" s="17" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="I25" s="5">
         <v>10</v>
@@ -1395,38 +1398,38 @@
       <c r="K25" s="14"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" s="5">
-        <v>3000</v>
-      </c>
-      <c r="D26" s="6">
-        <f>D18+C26</f>
-        <v>8490</v>
-      </c>
       <c r="H26" s="17" t="s">
-        <v>12</v>
+        <v>151</v>
       </c>
       <c r="I26" s="5">
         <v>10</v>
       </c>
+      <c r="K26" s="14"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="5">
+        <v>3000</v>
+      </c>
+      <c r="D27" s="4">
+        <f>D19+C27</f>
+        <v>8490</v>
+      </c>
       <c r="H27" s="17" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="I27" s="5">
         <v>10</v>
       </c>
-      <c r="K27" s="14"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H28" s="17" t="s">
-        <v>146</v>
+        <v>43</v>
       </c>
       <c r="I28" s="5">
         <v>10</v>
@@ -1435,7 +1438,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H29" s="17" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="I29" s="5">
         <v>10</v>
@@ -1444,7 +1447,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H30" s="17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I30" s="5">
         <v>10</v>
@@ -1452,56 +1455,46 @@
       <c r="K30" s="14"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B31" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C31" s="5">
-        <v>4400</v>
-      </c>
-      <c r="D31" s="6">
-        <f>D26+C31</f>
-        <v>12890</v>
-      </c>
       <c r="H31" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I31" s="5">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K31" s="14"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C32" s="5">
-        <v>-10000</v>
-      </c>
-      <c r="D32" s="6">
-        <f>D31+C32</f>
-        <v>2890</v>
+        <v>4400</v>
+      </c>
+      <c r="D32" s="4">
+        <f>D27+C32</f>
+        <v>12890</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I32" s="5">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="K32" s="14"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C33" s="5">
-        <v>1600</v>
-      </c>
-      <c r="D33" s="6">
-        <f t="shared" ref="D33:D40" si="1">D32+C33</f>
-        <v>4490</v>
+        <v>-10000</v>
+      </c>
+      <c r="D33" s="4">
+        <f>D32+C33</f>
+        <v>2890</v>
       </c>
       <c r="H33" s="17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I33" s="5">
         <v>10</v>
@@ -1510,1507 +1503,1553 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" s="5">
+        <v>1600</v>
+      </c>
+      <c r="D34" s="4">
+        <f t="shared" ref="D34:D41" si="1">D33+C34</f>
+        <v>4490</v>
+      </c>
+      <c r="H34" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="I34" s="5">
+        <v>10</v>
+      </c>
+      <c r="K34" s="14"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B35" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C35" s="5">
         <v>3000</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D35" s="4">
         <f t="shared" si="1"/>
         <v>7490</v>
       </c>
-      <c r="H34" s="17" t="s">
+      <c r="H35" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="I34" s="5">
+      <c r="I35" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="17" t="s">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B36" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C35" s="5">
+      <c r="C36" s="5">
         <v>2000</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D36" s="4">
         <f t="shared" si="1"/>
         <v>9490</v>
       </c>
-      <c r="H35" s="17" t="s">
+      <c r="H36" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="I35" s="5">
+      <c r="I36" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="17" t="s">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B37" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C36" s="5">
+      <c r="C37" s="5">
         <v>3000</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D37" s="4">
         <f t="shared" si="1"/>
         <v>12490</v>
       </c>
-      <c r="H36" s="17" t="s">
+      <c r="H37" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="I36" s="5">
+      <c r="I37" s="5">
         <v>10</v>
       </c>
-      <c r="K36" s="14"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B37" s="4" t="s">
+      <c r="K37" s="14"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B38" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="5">
+      <c r="C38" s="5">
         <v>-10000</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D38" s="4">
         <f t="shared" si="1"/>
         <v>2490</v>
       </c>
-      <c r="H37" s="17" t="s">
+      <c r="H38" s="17" t="s">
         <v>159</v>
       </c>
-      <c r="I37" s="5">
+      <c r="I38" s="5">
         <v>10</v>
       </c>
-      <c r="K37" s="14"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="17" t="s">
+      <c r="K38" s="14"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B39" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C38" s="5">
+      <c r="C39" s="5">
         <v>4960</v>
       </c>
-      <c r="D38" s="6">
+      <c r="D39" s="4">
         <f t="shared" si="1"/>
         <v>7450</v>
       </c>
-      <c r="H38" s="17" t="s">
+      <c r="H39" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="I38" s="5">
+      <c r="I39" s="5">
         <v>10</v>
       </c>
-      <c r="K38" s="14"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="17" t="s">
+      <c r="K39" s="14"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B40" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C39" s="5">
+      <c r="C40" s="5">
         <v>4000</v>
       </c>
-      <c r="D39" s="6">
+      <c r="D40" s="4">
         <f t="shared" si="1"/>
         <v>11450</v>
       </c>
-      <c r="H39" s="17" t="s">
+      <c r="H40" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="I39" s="5">
+      <c r="I40" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B40" s="4" t="s">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B41" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C40" s="5">
+      <c r="C41" s="5">
         <v>-10000</v>
       </c>
-      <c r="D40" s="6">
+      <c r="D41" s="4">
         <f t="shared" si="1"/>
         <v>1450</v>
       </c>
-      <c r="H40" s="17" t="s">
+      <c r="H41" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="I40" s="5">
+      <c r="I41" s="5">
         <v>10</v>
       </c>
-      <c r="K40" s="14"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B41" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C41" s="5">
-        <v>7640</v>
-      </c>
-      <c r="D41" s="6">
-        <f t="shared" ref="D41:D46" si="2">D40+C41</f>
-        <v>9090</v>
-      </c>
+      <c r="K41" s="14"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C42" s="5">
+        <v>7640</v>
+      </c>
+      <c r="D42" s="4">
+        <f t="shared" ref="D42:D47" si="2">D41+C42</f>
+        <v>9090</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B43" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C43" s="5">
         <v>3000</v>
       </c>
-      <c r="D42" s="6">
+      <c r="D43" s="4">
         <f t="shared" si="2"/>
         <v>12090</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B43" s="4" t="s">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B44" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C43" s="5">
+      <c r="C44" s="5">
         <v>-10000</v>
       </c>
-      <c r="D43" s="6">
+      <c r="D44" s="4">
         <f t="shared" si="2"/>
         <v>2090</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B44" s="4" t="s">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B45" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C45" s="5">
         <v>800</v>
       </c>
-      <c r="D44" s="6">
+      <c r="D45" s="4">
         <f t="shared" si="2"/>
         <v>2890</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="17" t="s">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B46" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C45" s="5">
+      <c r="C46" s="5">
         <v>2000</v>
       </c>
-      <c r="D45" s="6">
+      <c r="D46" s="4">
         <f t="shared" si="2"/>
         <v>4890</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="17" t="s">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B47" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="5">
+      <c r="C47" s="5">
         <v>4000</v>
       </c>
-      <c r="D46" s="6">
+      <c r="D47" s="4">
         <f t="shared" si="2"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="17" t="s">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B48" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C48" s="5">
         <v>4000</v>
       </c>
-      <c r="D47" s="6">
-        <f t="shared" ref="D47:D52" si="3">D46+C47</f>
+      <c r="D48" s="4">
+        <f t="shared" ref="D48:D53" si="3">D47+C48</f>
         <v>12890</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B48" s="4" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C48" s="5">
+      <c r="C49" s="5">
         <v>5000</v>
       </c>
-      <c r="D48" s="6">
+      <c r="D49" s="4">
         <f t="shared" si="3"/>
         <v>17890</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B49" s="4" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B50" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C49" s="5">
+      <c r="C50" s="5">
         <v>-10000</v>
       </c>
-      <c r="D49" s="6">
+      <c r="D50" s="4">
         <f t="shared" si="3"/>
         <v>7890</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="17">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="17">
         <v>44969</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B51" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C50" s="5">
+      <c r="C51" s="5">
         <v>900</v>
       </c>
-      <c r="D50" s="6">
+      <c r="D51" s="4">
         <f t="shared" si="3"/>
         <v>8790</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B51" s="4" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C51" s="5">
+      <c r="C52" s="5">
         <v>4000</v>
       </c>
-      <c r="D51" s="6">
+      <c r="D52" s="4">
         <f t="shared" si="3"/>
         <v>12790</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B52" s="4" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B53" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C52" s="5">
+      <c r="C53" s="5">
         <v>-10000</v>
       </c>
-      <c r="D52" s="6">
+      <c r="D53" s="4">
         <f t="shared" si="3"/>
         <v>2790</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C53" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D53" s="6">
-        <f t="shared" ref="D53:D60" si="4">D52+C53</f>
-        <v>4790</v>
-      </c>
-    </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C54" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D54" s="4">
+        <f t="shared" ref="D54:D61" si="4">D53+C54</f>
+        <v>4790</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B55" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C54" s="5">
+      <c r="C55" s="5">
         <v>700</v>
       </c>
-      <c r="D54" s="6">
+      <c r="D55" s="4">
         <f t="shared" si="4"/>
         <v>5490</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="4" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B56" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C55" s="5">
+      <c r="C56" s="5">
         <v>4000</v>
       </c>
-      <c r="D55" s="6">
+      <c r="D56" s="4">
         <f t="shared" si="4"/>
         <v>9490</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="17" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B57" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C56" s="5">
+      <c r="C57" s="5">
         <v>600</v>
       </c>
-      <c r="D56" s="6">
+      <c r="D57" s="4">
         <f t="shared" si="4"/>
         <v>10090</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B57" s="4" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B58" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C57" s="5">
+      <c r="C58" s="5">
         <v>-10000</v>
       </c>
-      <c r="D57" s="6">
+      <c r="D58" s="4">
         <f t="shared" si="4"/>
         <v>90</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="17" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B59" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C58" s="5">
+      <c r="C59" s="5">
         <f>700+5000+300+600+400+1000+800</f>
         <v>8800</v>
       </c>
-      <c r="D58" s="6">
+      <c r="D59" s="4">
         <f t="shared" si="4"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B59" s="4" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B60" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C59" s="5">
+      <c r="C60" s="5">
         <v>6000</v>
       </c>
-      <c r="D59" s="6">
+      <c r="D60" s="4">
         <f t="shared" si="4"/>
         <v>14890</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B60" s="4" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B61" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C60" s="5">
+      <c r="C61" s="5">
         <v>-10000</v>
       </c>
-      <c r="D60" s="6">
+      <c r="D61" s="4">
         <f t="shared" si="4"/>
         <v>4890</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="17" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B62" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C61" s="5">
+      <c r="C62" s="5">
         <v>500</v>
       </c>
-      <c r="D61" s="6">
-        <f t="shared" ref="D61:D66" si="5">D60+C61</f>
+      <c r="D62" s="4">
+        <f t="shared" ref="D62:D67" si="5">D61+C62</f>
         <v>5390</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B62" s="4" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B63" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C62" s="5">
+      <c r="C63" s="5">
         <v>700</v>
       </c>
-      <c r="D62" s="6">
+      <c r="D63" s="4">
         <f t="shared" si="5"/>
         <v>6090</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B63" s="4" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B64" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C63" s="5">
+      <c r="C64" s="5">
         <v>1500</v>
       </c>
-      <c r="D63" s="6">
+      <c r="D64" s="4">
         <f t="shared" si="5"/>
         <v>7590</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B64" s="4" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B65" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C64" s="5">
+      <c r="C65" s="5">
         <v>5000</v>
       </c>
-      <c r="D64" s="6">
+      <c r="D65" s="4">
         <f t="shared" si="5"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B65" s="4" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C65" s="5">
+      <c r="C66" s="5">
         <v>-10000</v>
       </c>
-      <c r="D65" s="6">
+      <c r="D66" s="4">
         <f t="shared" si="5"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="17" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B67" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C66" s="5">
+      <c r="C67" s="5">
         <v>2000</v>
       </c>
-      <c r="D66" s="6">
+      <c r="D67" s="4">
         <f t="shared" si="5"/>
         <v>4590</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B67" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C67" s="5">
-        <v>700</v>
-      </c>
-      <c r="D67" s="6">
-        <f t="shared" ref="D67:D72" si="6">D66+C67</f>
-        <v>5290</v>
-      </c>
-    </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="17" t="s">
-        <v>82</v>
-      </c>
       <c r="B68" s="4" t="s">
         <v>77</v>
       </c>
       <c r="C68" s="5">
         <v>700</v>
       </c>
-      <c r="D68" s="6">
+      <c r="D68" s="4">
+        <f t="shared" ref="D68:D73" si="6">D67+C68</f>
+        <v>5290</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C69" s="5">
+        <v>700</v>
+      </c>
+      <c r="D69" s="4">
         <f t="shared" si="6"/>
         <v>5990</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="17" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B70" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C69" s="5">
+      <c r="C70" s="5">
         <v>700</v>
       </c>
-      <c r="D69" s="6">
+      <c r="D70" s="4">
         <f t="shared" si="6"/>
         <v>6690</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="17" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B71" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C70" s="5">
+      <c r="C71" s="5">
         <v>4000</v>
       </c>
-      <c r="D70" s="6">
+      <c r="D71" s="4">
         <f t="shared" si="6"/>
         <v>10690</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B71" s="4" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B72" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C71" s="5">
+      <c r="C72" s="5">
         <v>-10000</v>
       </c>
-      <c r="D71" s="6">
+      <c r="D72" s="4">
         <f t="shared" si="6"/>
         <v>690</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="17" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B73" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C72" s="5">
+      <c r="C73" s="5">
         <v>1000</v>
       </c>
-      <c r="D72" s="6">
+      <c r="D73" s="4">
         <f t="shared" si="6"/>
         <v>1690</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="17" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B74" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C73" s="5">
+      <c r="C74" s="5">
         <v>7000</v>
       </c>
-      <c r="D73" s="6">
-        <f t="shared" ref="D73:D78" si="7">D72+C73</f>
+      <c r="D74" s="4">
+        <f t="shared" ref="D74:D79" si="7">D73+C74</f>
         <v>8690</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B74" s="4" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B75" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C74" s="5">
+      <c r="C75" s="5">
         <v>10000</v>
       </c>
-      <c r="D74" s="6">
+      <c r="D75" s="4">
         <f t="shared" si="7"/>
         <v>18690</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B75" s="4" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B76" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C75" s="5">
+      <c r="C76" s="5">
         <v>-10000</v>
       </c>
-      <c r="D75" s="6">
+      <c r="D76" s="4">
         <f t="shared" si="7"/>
         <v>8690</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B76" s="4" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B77" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C76" s="5">
+      <c r="C77" s="5">
         <v>1700</v>
       </c>
-      <c r="D76" s="6">
+      <c r="D77" s="4">
         <f t="shared" si="7"/>
         <v>10390</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B77" s="4" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B78" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C77" s="5">
+      <c r="C78" s="5">
         <v>-10000</v>
       </c>
-      <c r="D77" s="6">
+      <c r="D78" s="4">
         <f t="shared" si="7"/>
         <v>390</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B78" s="4" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B79" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C78" s="5">
+      <c r="C79" s="5">
         <v>6000</v>
       </c>
-      <c r="D78" s="6">
+      <c r="D79" s="4">
         <f t="shared" si="7"/>
         <v>6390</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="B79" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C79" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D79" s="6">
-        <f t="shared" ref="D79:D84" si="8">D78+C79</f>
-        <v>8390</v>
-      </c>
-    </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C80" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D80" s="4">
+        <f t="shared" ref="D80:D85" si="8">D79+C80</f>
+        <v>8390</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B81" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C80" s="5">
+      <c r="C81" s="5">
         <v>5000</v>
       </c>
-      <c r="D80" s="6">
+      <c r="D81" s="4">
         <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B81" s="4" t="s">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B82" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C81" s="5">
+      <c r="C82" s="5">
         <v>-10000</v>
       </c>
-      <c r="D81" s="6">
+      <c r="D82" s="4">
         <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="17" t="s">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="B82" s="4" t="s">
+      <c r="B83" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C82" s="5">
+      <c r="C83" s="5">
         <v>1000</v>
       </c>
-      <c r="D82" s="6">
+      <c r="D83" s="4">
         <f t="shared" si="8"/>
         <v>4390</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B83" s="4" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B84" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C83" s="5">
+      <c r="C84" s="5">
         <v>9000</v>
       </c>
-      <c r="D83" s="6">
+      <c r="D84" s="4">
         <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B84" s="4" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B85" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C84" s="5">
+      <c r="C85" s="5">
         <v>-10000</v>
       </c>
-      <c r="D84" s="6">
+      <c r="D85" s="4">
         <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B85" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C85" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D85" s="6">
-        <f t="shared" ref="D85:D90" si="9">D84+C85</f>
-        <v>5390</v>
-      </c>
-    </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B86" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C86" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D86" s="4">
+        <f t="shared" ref="D86:D91" si="9">D85+C86</f>
+        <v>5390</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B87" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C86" s="5">
+      <c r="C87" s="5">
         <v>6000</v>
       </c>
-      <c r="D86" s="6">
+      <c r="D87" s="4">
         <f t="shared" si="9"/>
         <v>11390</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B87" s="4" t="s">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B88" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C87" s="5">
+      <c r="C88" s="5">
         <v>-10000</v>
       </c>
-      <c r="D87" s="6">
+      <c r="D88" s="4">
         <f t="shared" si="9"/>
         <v>1390</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B88" s="4" t="s">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B89" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C88" s="5">
+      <c r="C89" s="5">
         <v>400</v>
       </c>
-      <c r="D88" s="6">
+      <c r="D89" s="4">
         <f t="shared" si="9"/>
         <v>1790</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="17" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="B89" s="4" t="s">
+      <c r="B90" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C89" s="5">
+      <c r="C90" s="5">
         <v>2000</v>
       </c>
-      <c r="D89" s="6">
+      <c r="D90" s="4">
         <f t="shared" si="9"/>
         <v>3790</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="17" t="s">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="B90" s="4" t="s">
+      <c r="B91" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C90" s="5">
+      <c r="C91" s="5">
         <v>6000</v>
       </c>
-      <c r="D90" s="6">
+      <c r="D91" s="4">
         <f t="shared" si="9"/>
         <v>9790</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="17" t="s">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="B91" s="4" t="s">
+      <c r="B92" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C91" s="5">
+      <c r="C92" s="5">
         <v>1000</v>
       </c>
-      <c r="D91" s="6">
-        <f t="shared" ref="D91:D96" si="10">D90+C91</f>
+      <c r="D92" s="4">
+        <f t="shared" ref="D92:D97" si="10">D91+C92</f>
         <v>10790</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B92" s="4" t="s">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B93" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C92" s="5">
+      <c r="C93" s="5">
         <v>-10000</v>
       </c>
-      <c r="D92" s="6">
+      <c r="D93" s="4">
         <f t="shared" si="10"/>
         <v>790</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="17" t="s">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="B93" s="4" t="s">
+      <c r="B94" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C93" s="5">
+      <c r="C94" s="5">
         <v>800</v>
       </c>
-      <c r="D93" s="6">
+      <c r="D94" s="4">
         <f t="shared" si="10"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="17" t="s">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="B94" s="4" t="s">
+      <c r="B95" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C94" s="5">
+      <c r="C95" s="5">
         <v>5000</v>
       </c>
-      <c r="D94" s="6">
+      <c r="D95" s="4">
         <f t="shared" si="10"/>
         <v>6590</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="17" t="s">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="B95" s="4" t="s">
+      <c r="B96" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C95" s="5">
+      <c r="C96" s="5">
         <v>6000</v>
       </c>
-      <c r="D95" s="6">
+      <c r="D96" s="4">
         <f t="shared" si="10"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B96" s="4" t="s">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B97" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C96" s="5">
+      <c r="C97" s="5">
         <v>-10000</v>
       </c>
-      <c r="D96" s="6">
+      <c r="D97" s="4">
         <f t="shared" si="10"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="17" t="s">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="B97" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C97" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D97" s="6">
-        <f t="shared" ref="D97:D103" si="11">D96+C97</f>
-        <v>4590</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B98" s="4" t="s">
         <v>65</v>
       </c>
       <c r="C98" s="5">
         <v>2000</v>
       </c>
-      <c r="D98" s="6">
+      <c r="D98" s="4">
+        <f t="shared" ref="D98:D104" si="11">D97+C98</f>
+        <v>4590</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B99" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C99" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D99" s="4">
         <f t="shared" si="11"/>
         <v>6590</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B99" s="4" t="s">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B100" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C99" s="5">
+      <c r="C100" s="5">
         <v>7000</v>
       </c>
-      <c r="D99" s="6">
+      <c r="D100" s="4">
         <f t="shared" si="11"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B100" s="4" t="s">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B101" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C100" s="5">
+      <c r="C101" s="5">
         <v>-10000</v>
       </c>
-      <c r="D100" s="6">
+      <c r="D101" s="4">
         <f t="shared" si="11"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="17" t="s">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="B101" s="4" t="s">
+      <c r="B102" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C101" s="5">
+      <c r="C102" s="5">
         <v>2000</v>
       </c>
-      <c r="D101" s="6">
+      <c r="D102" s="4">
         <f t="shared" si="11"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="17" t="s">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="B102" s="4" t="s">
+      <c r="B103" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C102" s="5">
+      <c r="C103" s="5">
         <v>6000</v>
       </c>
-      <c r="D102" s="6">
+      <c r="D103" s="4">
         <f t="shared" si="11"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B103" s="4" t="s">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B104" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C103" s="5">
+      <c r="C104" s="5">
         <v>-10000</v>
       </c>
-      <c r="D103" s="6">
+      <c r="D104" s="4">
         <f t="shared" si="11"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="B104" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C104" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D104" s="6">
-        <f t="shared" ref="D104:D109" si="12">D103+C104</f>
-        <v>3590</v>
-      </c>
-    </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C105" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D105" s="4">
+        <f t="shared" ref="D105:D110" si="12">D104+C105</f>
+        <v>3590</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="B105" s="4" t="s">
+      <c r="B106" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C105" s="5">
+      <c r="C106" s="5">
         <v>7000</v>
       </c>
-      <c r="D105" s="6">
+      <c r="D106" s="4">
         <f t="shared" si="12"/>
         <v>10590</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B106" s="4" t="s">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B107" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C106" s="5">
+      <c r="C107" s="5">
         <v>-10000</v>
       </c>
-      <c r="D106" s="6">
+      <c r="D107" s="4">
         <f t="shared" si="12"/>
         <v>590</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B107" s="4" t="s">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B108" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C107" s="5">
+      <c r="C108" s="5">
         <v>12000</v>
       </c>
-      <c r="D107" s="6">
+      <c r="D108" s="4">
         <f t="shared" si="12"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B108" s="4" t="s">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B109" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C108" s="5">
+      <c r="C109" s="5">
         <v>-10000</v>
       </c>
-      <c r="D108" s="6">
+      <c r="D109" s="4">
         <f t="shared" si="12"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B109" s="4" t="s">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B110" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C109" s="5">
+      <c r="C110" s="5">
         <v>2000</v>
       </c>
-      <c r="D109" s="6">
+      <c r="D110" s="4">
         <f t="shared" si="12"/>
         <v>4590</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="B110" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C110" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D110" s="6">
-        <f t="shared" ref="D110:D115" si="13">D109+C110</f>
-        <v>6590</v>
-      </c>
-    </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="B111" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C111" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D111" s="4">
+        <f t="shared" ref="D111:D116" si="13">D110+C111</f>
+        <v>6590</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="B111" s="4" t="s">
+      <c r="B112" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C111" s="5">
+      <c r="C112" s="5">
         <v>7000</v>
       </c>
-      <c r="D111" s="6">
+      <c r="D112" s="4">
         <f t="shared" si="13"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B112" s="4" t="s">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B113" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C112" s="5">
+      <c r="C113" s="5">
         <v>-10000</v>
       </c>
-      <c r="D112" s="6">
+      <c r="D113" s="4">
         <f t="shared" si="13"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="17" t="s">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="B113" s="4" t="s">
+      <c r="B114" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C113" s="5">
+      <c r="C114" s="5">
         <v>2000</v>
       </c>
-      <c r="D113" s="6">
+      <c r="D114" s="4">
         <f t="shared" si="13"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="17" t="s">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="B114" s="4" t="s">
+      <c r="B115" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C114" s="5">
+      <c r="C115" s="5">
         <v>8000</v>
       </c>
-      <c r="D114" s="6">
+      <c r="D115" s="4">
         <f t="shared" si="13"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B115" s="4" t="s">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B116" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C115" s="5">
+      <c r="C116" s="5">
         <v>-10000</v>
       </c>
-      <c r="D115" s="6">
+      <c r="D116" s="4">
         <f t="shared" si="13"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="17" t="s">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="B116" s="4" t="s">
+      <c r="B117" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C116" s="5">
+      <c r="C117" s="5">
         <v>2000</v>
       </c>
-      <c r="D116" s="6">
-        <f t="shared" ref="D116:D121" si="14">D115+C116</f>
+      <c r="D117" s="4">
+        <f t="shared" ref="D117:D122" si="14">D116+C117</f>
         <v>5590</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B117" s="4" t="s">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B118" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C117" s="5">
+      <c r="C118" s="5">
         <v>5000</v>
       </c>
-      <c r="D117" s="6">
+      <c r="D118" s="4">
         <f t="shared" si="14"/>
         <v>10590</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B118" s="4" t="s">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B119" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C118" s="5">
+      <c r="C119" s="5">
         <v>-10000</v>
       </c>
-      <c r="D118" s="6">
+      <c r="D119" s="4">
         <f t="shared" si="14"/>
         <v>590</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B119" s="4" t="s">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B120" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C119" s="5">
+      <c r="C120" s="5">
         <v>2000</v>
       </c>
-      <c r="D119" s="6">
+      <c r="D120" s="4">
         <f t="shared" si="14"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B120" s="4" t="s">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B121" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C120" s="5">
+      <c r="C121" s="5">
         <v>9000</v>
       </c>
-      <c r="D120" s="6">
+      <c r="D121" s="4">
         <f t="shared" si="14"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B121" s="4" t="s">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B122" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C121" s="5">
+      <c r="C122" s="5">
         <v>-10000</v>
       </c>
-      <c r="D121" s="6">
+      <c r="D122" s="4">
         <f t="shared" si="14"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="B122" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C122" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D122" s="6">
-        <f t="shared" ref="D122:D127" si="15">D121+C122</f>
-        <v>3590</v>
-      </c>
-    </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="B123" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C123" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D123" s="4">
+        <f t="shared" ref="D123:D128" si="15">D122+C123</f>
+        <v>3590</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="B123" s="4" t="s">
+      <c r="B124" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C123" s="5">
+      <c r="C124" s="5">
         <v>8000</v>
       </c>
-      <c r="D123" s="6">
+      <c r="D124" s="4">
         <f t="shared" si="15"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B124" s="4" t="s">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B125" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C124" s="5">
+      <c r="C125" s="5">
         <v>-10000</v>
       </c>
-      <c r="D124" s="6">
+      <c r="D125" s="4">
         <f t="shared" si="15"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="17" t="s">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="B125" s="4" t="s">
+      <c r="B126" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C125" s="5">
+      <c r="C126" s="5">
         <v>2000</v>
       </c>
-      <c r="D125" s="6">
+      <c r="D126" s="4">
         <f t="shared" si="15"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="17" t="s">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="B126" s="4" t="s">
+      <c r="B127" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="C126" s="5">
+      <c r="C127" s="5">
         <v>12000</v>
       </c>
-      <c r="D126" s="6">
+      <c r="D127" s="4">
         <f t="shared" si="15"/>
         <v>15590</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B127" s="4" t="s">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B128" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C127" s="5">
+      <c r="C128" s="5">
         <v>-10000</v>
       </c>
-      <c r="D127" s="6">
+      <c r="D128" s="4">
         <f t="shared" si="15"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="17" t="s">
-        <v>168</v>
-      </c>
-      <c r="B128" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="C128" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D128" s="6">
-        <f t="shared" ref="D128:D133" si="16">D127+C128</f>
-        <v>7590</v>
-      </c>
-    </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="B129" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C129" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D129" s="4">
+        <f t="shared" ref="D129:D134" si="16">D128+C129</f>
+        <v>7590</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="B129" s="4" t="s">
+      <c r="B130" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="C129" s="5">
+      <c r="C130" s="5">
         <v>10000</v>
       </c>
-      <c r="D129" s="6">
+      <c r="D130" s="4">
         <f t="shared" si="16"/>
         <v>17590</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B130" s="4" t="s">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B131" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C130" s="5">
+      <c r="C131" s="5">
         <v>-10000</v>
       </c>
-      <c r="D130" s="6">
+      <c r="D131" s="4">
         <f t="shared" si="16"/>
         <v>7590</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B131" s="4" t="s">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B132" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="C131" s="5">
+      <c r="C132" s="5">
         <v>2000</v>
       </c>
-      <c r="D131" s="6">
+      <c r="D132" s="4">
         <f t="shared" si="16"/>
         <v>9590</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="17" t="s">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="B132" s="4" t="s">
+      <c r="B133" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="C132" s="5">
+      <c r="C133" s="5">
         <v>-1200</v>
       </c>
-      <c r="D132" s="6">
+      <c r="D133" s="4">
         <f t="shared" si="16"/>
         <v>8390</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B133" s="4" t="s">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B134" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="C133" s="5">
+      <c r="C134" s="5">
         <v>500</v>
       </c>
-      <c r="D133" s="6">
+      <c r="D134" s="4">
         <f t="shared" si="16"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="B134" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C134" s="5">
-        <v>750</v>
-      </c>
-      <c r="D134" s="6">
-        <f t="shared" ref="D134:D139" si="17">D133+C134</f>
-        <v>9640</v>
-      </c>
-    </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="B135" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C135" s="5">
+        <v>750</v>
+      </c>
+      <c r="D135" s="4">
+        <f t="shared" ref="D135:D140" si="17">D134+C135</f>
+        <v>9640</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="B135" s="4" t="s">
+      <c r="B136" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C135" s="5">
+      <c r="C136" s="5">
         <v>2000</v>
       </c>
-      <c r="D135" s="6">
+      <c r="D136" s="4">
         <f t="shared" si="17"/>
         <v>11640</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B136" s="4" t="s">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B137" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C136" s="5">
+      <c r="C137" s="5">
         <v>2000</v>
       </c>
-      <c r="D136" s="6">
+      <c r="D137" s="4">
         <f t="shared" si="17"/>
         <v>13640</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B137" s="4" t="s">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B138" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C137" s="5">
+      <c r="C138" s="5">
         <v>-10000</v>
       </c>
-      <c r="D137" s="6">
+      <c r="D138" s="4">
         <f t="shared" si="17"/>
         <v>3640</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B138" s="4" t="s">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B139" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="C138" s="5">
+      <c r="C139" s="5">
         <v>350</v>
       </c>
-      <c r="D138" s="6">
+      <c r="D139" s="4">
         <f t="shared" si="17"/>
         <v>3990</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="17" t="s">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="B139" s="4" t="s">
+      <c r="B140" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="C139" s="5">
+      <c r="C140" s="5">
         <v>300</v>
       </c>
-      <c r="D139" s="6">
+      <c r="D140" s="4">
         <f t="shared" si="17"/>
         <v>4290</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="17" t="s">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" s="17" t="s">
         <v>181</v>
       </c>
-      <c r="B140" s="4" t="s">
+      <c r="B141" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="C140" s="5">
+      <c r="C141" s="5">
         <v>3800</v>
       </c>
-      <c r="D140" s="6">
-        <f>D139+C140</f>
+      <c r="D141" s="4">
+        <f>D140+C141</f>
         <v>8090</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B141" s="4" t="s">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B142" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C141" s="5">
+      <c r="C142" s="5">
         <v>500</v>
       </c>
-      <c r="D141" s="6">
-        <f>D140+C141</f>
+      <c r="D142" s="4">
+        <f>D141+C142</f>
         <v>8590</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="17" t="s">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="B142" s="4" t="s">
+      <c r="B143" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="C142" s="5">
+      <c r="C143" s="5">
         <v>1300</v>
       </c>
-      <c r="D142" s="6">
-        <f>D141+C142</f>
+      <c r="D143" s="4">
+        <f>D142+C143</f>
         <v>9890</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="B144" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C144" s="5">
+        <v>9000</v>
+      </c>
+      <c r="D144" s="4">
+        <f>D143+C144</f>
+        <v>18890</v>
+      </c>
+    </row>
+    <row r="145" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B145" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C145" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D145" s="4">
+        <f>D144+C145</f>
+        <v>8890</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
duy chuyen cho co diem 500
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="190">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -583,6 +583,12 @@
   </si>
   <si>
     <t>chua lam giay</t>
+  </si>
+  <si>
+    <t>25/07/2024</t>
+  </si>
+  <si>
+    <t>Duy chuyển cho cô 500k</t>
   </si>
 </sst>
 </file>
@@ -1061,11 +1067,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K148"/>
+  <dimension ref="A1:K149"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L21" sqref="L21"/>
+      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D150" sqref="D150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3011,7 +3017,7 @@
         <v>3800</v>
       </c>
       <c r="D142" s="4">
-        <f>D141+C142</f>
+        <f t="shared" ref="D142:D148" si="18">D141+C142</f>
         <v>8090</v>
       </c>
     </row>
@@ -3023,7 +3029,7 @@
         <v>500</v>
       </c>
       <c r="D143" s="4">
-        <f>D142+C143</f>
+        <f t="shared" si="18"/>
         <v>8590</v>
       </c>
     </row>
@@ -3038,7 +3044,7 @@
         <v>1300</v>
       </c>
       <c r="D144" s="4">
-        <f>D143+C144</f>
+        <f t="shared" si="18"/>
         <v>9890</v>
       </c>
     </row>
@@ -3053,7 +3059,7 @@
         <v>9000</v>
       </c>
       <c r="D145" s="4">
-        <f>D144+C145</f>
+        <f t="shared" si="18"/>
         <v>18890</v>
       </c>
     </row>
@@ -3065,7 +3071,7 @@
         <v>-10000</v>
       </c>
       <c r="D146" s="4">
-        <f>D145+C146</f>
+        <f t="shared" si="18"/>
         <v>8890</v>
       </c>
     </row>
@@ -3080,7 +3086,7 @@
         <v>2000</v>
       </c>
       <c r="D147" s="4">
-        <f>D146+C147</f>
+        <f t="shared" si="18"/>
         <v>10890</v>
       </c>
     </row>
@@ -3092,8 +3098,23 @@
         <v>-10000</v>
       </c>
       <c r="D148" s="4">
-        <f>D147+C148</f>
+        <f t="shared" si="18"/>
         <v>890</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="B149" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C149" s="5">
+        <v>500</v>
+      </c>
+      <c r="D149" s="4">
+        <f>D148+C149</f>
+        <v>1390</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
duy lay tien loi ngay 30 co diem
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="192">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -589,6 +589,12 @@
   </si>
   <si>
     <t>Duy chuyển cho cô 500k</t>
+  </si>
+  <si>
+    <t>30/07/2024</t>
+  </si>
+  <si>
+    <t>Duy lấy tiền lời ngày 30</t>
   </si>
 </sst>
 </file>
@@ -1067,11 +1073,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K149"/>
+  <dimension ref="A1:K152"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D150" sqref="D150"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1147,8 +1153,8 @@
         <v>20</v>
       </c>
       <c r="J3" s="4">
-        <f>SUM(I3:I58)</f>
-        <v>420</v>
+        <f>SUM(I3:I59)</f>
+        <v>430</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1430,38 +1436,40 @@
       <c r="K27" s="14"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="17" t="s">
+      <c r="H28" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="I28" s="5">
+        <v>10</v>
+      </c>
+      <c r="K28" s="14" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B29" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C29" s="5">
         <v>3000</v>
       </c>
-      <c r="D28" s="4">
-        <f>D20+C28</f>
+      <c r="D29" s="4">
+        <f>D20+C29</f>
         <v>8490</v>
       </c>
-      <c r="H28" s="17" t="s">
+      <c r="H29" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="I28" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H29" s="17" t="s">
-        <v>43</v>
-      </c>
       <c r="I29" s="5">
         <v>10</v>
       </c>
-      <c r="K29" s="14"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H30" s="17" t="s">
-        <v>146</v>
+        <v>43</v>
       </c>
       <c r="I30" s="5">
         <v>10</v>
@@ -1470,7 +1478,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H31" s="17" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="I31" s="5">
         <v>10</v>
@@ -1479,64 +1487,54 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H32" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="I32" s="5">
+        <v>10</v>
+      </c>
+      <c r="K32" s="14"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H33" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="I32" s="5">
-        <v>10</v>
-      </c>
-      <c r="K32" s="14"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B33" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C33" s="5">
-        <v>4400</v>
-      </c>
-      <c r="D33" s="4">
-        <f>D28+C33</f>
-        <v>12890</v>
-      </c>
-      <c r="H33" s="17" t="s">
-        <v>164</v>
-      </c>
       <c r="I33" s="5">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K33" s="14"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C34" s="5">
-        <v>-10000</v>
+        <v>4400</v>
       </c>
       <c r="D34" s="4">
-        <f>D33+C34</f>
-        <v>2890</v>
+        <f>D29+C34</f>
+        <v>12890</v>
       </c>
       <c r="H34" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I34" s="5">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="K34" s="14"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C35" s="5">
-        <v>1600</v>
+        <v>-10000</v>
       </c>
       <c r="D35" s="4">
-        <f t="shared" ref="D35:D42" si="1">D34+C35</f>
-        <v>4490</v>
+        <f>D34+C35</f>
+        <v>2890</v>
       </c>
       <c r="H35" s="17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I35" s="5">
         <v>10</v>
@@ -1545,505 +1543,509 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36" s="5">
+        <v>1600</v>
+      </c>
+      <c r="D36" s="4">
+        <f t="shared" ref="D36:D43" si="1">D35+C36</f>
+        <v>4490</v>
+      </c>
+      <c r="H36" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="I36" s="5">
+        <v>10</v>
+      </c>
+      <c r="K36" s="14"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B37" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C36" s="5">
+      <c r="C37" s="5">
         <v>3000</v>
       </c>
-      <c r="D36" s="4">
+      <c r="D37" s="4">
         <f t="shared" si="1"/>
         <v>7490</v>
       </c>
-      <c r="H36" s="17" t="s">
+      <c r="H37" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="I36" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="17" t="s">
+      <c r="I37" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B38" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="5">
+      <c r="C38" s="5">
         <v>2000</v>
       </c>
-      <c r="D37" s="4">
+      <c r="D38" s="4">
         <f t="shared" si="1"/>
         <v>9490</v>
       </c>
-      <c r="H37" s="17" t="s">
+      <c r="H38" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="I37" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="17" t="s">
+      <c r="I38" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B39" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C38" s="5">
+      <c r="C39" s="5">
         <v>3000</v>
       </c>
-      <c r="D38" s="4">
+      <c r="D39" s="4">
         <f t="shared" si="1"/>
         <v>12490</v>
       </c>
-      <c r="H38" s="17" t="s">
+      <c r="H39" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="I38" s="5">
-        <v>10</v>
-      </c>
-      <c r="K38" s="14"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B39" s="4" t="s">
+      <c r="I39" s="5">
+        <v>10</v>
+      </c>
+      <c r="K39" s="14"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C39" s="5">
+      <c r="C40" s="5">
         <v>-10000</v>
       </c>
-      <c r="D39" s="4">
+      <c r="D40" s="4">
         <f t="shared" si="1"/>
         <v>2490</v>
       </c>
-      <c r="H39" s="17" t="s">
+      <c r="H40" s="17" t="s">
         <v>159</v>
       </c>
-      <c r="I39" s="5">
-        <v>10</v>
-      </c>
-      <c r="K39" s="14"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="17" t="s">
+      <c r="I40" s="5">
+        <v>10</v>
+      </c>
+      <c r="K40" s="14"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B41" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C40" s="5">
+      <c r="C41" s="5">
         <v>4960</v>
       </c>
-      <c r="D40" s="4">
+      <c r="D41" s="4">
         <f t="shared" si="1"/>
         <v>7450</v>
       </c>
-      <c r="H40" s="17" t="s">
+      <c r="H41" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="I40" s="5">
-        <v>10</v>
-      </c>
-      <c r="K40" s="14"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="17" t="s">
+      <c r="I41" s="5">
+        <v>10</v>
+      </c>
+      <c r="K41" s="14"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B42" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C41" s="5">
+      <c r="C42" s="5">
         <v>4000</v>
       </c>
-      <c r="D41" s="4">
+      <c r="D42" s="4">
         <f t="shared" si="1"/>
         <v>11450</v>
       </c>
-      <c r="H41" s="17" t="s">
+      <c r="H42" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="I41" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B42" s="4" t="s">
+      <c r="I42" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B43" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C43" s="5">
         <v>-10000</v>
       </c>
-      <c r="D42" s="4">
+      <c r="D43" s="4">
         <f t="shared" si="1"/>
         <v>1450</v>
       </c>
-      <c r="H42" s="17" t="s">
+      <c r="H43" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="I42" s="5">
-        <v>10</v>
-      </c>
-      <c r="K42" s="14"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B43" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C43" s="5">
-        <v>7640</v>
-      </c>
-      <c r="D43" s="4">
-        <f t="shared" ref="D43:D48" si="2">D42+C43</f>
-        <v>9090</v>
-      </c>
+      <c r="I43" s="5">
+        <v>10</v>
+      </c>
+      <c r="K43" s="14"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C44" s="5">
+        <v>7640</v>
+      </c>
+      <c r="D44" s="4">
+        <f t="shared" ref="D44:D49" si="2">D43+C44</f>
+        <v>9090</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B45" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C45" s="5">
         <v>3000</v>
       </c>
-      <c r="D44" s="4">
+      <c r="D45" s="4">
         <f t="shared" si="2"/>
         <v>12090</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B45" s="4" t="s">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B46" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C45" s="5">
+      <c r="C46" s="5">
         <v>-10000</v>
       </c>
-      <c r="D45" s="4">
+      <c r="D46" s="4">
         <f t="shared" si="2"/>
         <v>2090</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B46" s="4" t="s">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B47" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C46" s="5">
+      <c r="C47" s="5">
         <v>800</v>
       </c>
-      <c r="D46" s="4">
+      <c r="D47" s="4">
         <f t="shared" si="2"/>
         <v>2890</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="17" t="s">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B48" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C48" s="5">
         <v>2000</v>
       </c>
-      <c r="D47" s="4">
+      <c r="D48" s="4">
         <f t="shared" si="2"/>
         <v>4890</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="17" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B49" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C48" s="5">
+      <c r="C49" s="5">
         <v>4000</v>
       </c>
-      <c r="D48" s="4">
+      <c r="D49" s="4">
         <f t="shared" si="2"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="17" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B50" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C49" s="5">
+      <c r="C50" s="5">
         <v>4000</v>
       </c>
-      <c r="D49" s="4">
-        <f t="shared" ref="D49:D54" si="3">D48+C49</f>
+      <c r="D50" s="4">
+        <f t="shared" ref="D50:D55" si="3">D49+C50</f>
         <v>12890</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B50" s="4" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B51" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C50" s="5">
+      <c r="C51" s="5">
         <v>5000</v>
       </c>
-      <c r="D50" s="4">
+      <c r="D51" s="4">
         <f t="shared" si="3"/>
         <v>17890</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B51" s="4" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C51" s="5">
+      <c r="C52" s="5">
         <v>-10000</v>
       </c>
-      <c r="D51" s="4">
+      <c r="D52" s="4">
         <f t="shared" si="3"/>
         <v>7890</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="17">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="17">
         <v>44969</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B53" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C52" s="5">
+      <c r="C53" s="5">
         <v>900</v>
       </c>
-      <c r="D52" s="4">
+      <c r="D53" s="4">
         <f t="shared" si="3"/>
         <v>8790</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B53" s="4" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B54" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C53" s="5">
+      <c r="C54" s="5">
         <v>4000</v>
       </c>
-      <c r="D53" s="4">
+      <c r="D54" s="4">
         <f t="shared" si="3"/>
         <v>12790</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B54" s="4" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B55" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C54" s="5">
+      <c r="C55" s="5">
         <v>-10000</v>
       </c>
-      <c r="D54" s="4">
+      <c r="D55" s="4">
         <f t="shared" si="3"/>
         <v>2790</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C55" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D55" s="4">
-        <f t="shared" ref="D55:D62" si="4">D54+C55</f>
-        <v>4790</v>
-      </c>
-    </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C56" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D56" s="4">
+        <f t="shared" ref="D56:D63" si="4">D55+C56</f>
+        <v>4790</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B57" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C56" s="5">
+      <c r="C57" s="5">
         <v>700</v>
       </c>
-      <c r="D56" s="4">
+      <c r="D57" s="4">
         <f t="shared" si="4"/>
         <v>5490</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B57" s="4" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B58" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C57" s="5">
+      <c r="C58" s="5">
         <v>4000</v>
       </c>
-      <c r="D57" s="4">
+      <c r="D58" s="4">
         <f t="shared" si="4"/>
         <v>9490</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="17" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B59" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C58" s="5">
+      <c r="C59" s="5">
         <v>600</v>
       </c>
-      <c r="D58" s="4">
+      <c r="D59" s="4">
         <f t="shared" si="4"/>
         <v>10090</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B59" s="4" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B60" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C59" s="5">
+      <c r="C60" s="5">
         <v>-10000</v>
       </c>
-      <c r="D59" s="4">
+      <c r="D60" s="4">
         <f t="shared" si="4"/>
         <v>90</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="17" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B61" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C60" s="5">
+      <c r="C61" s="5">
         <f>700+5000+300+600+400+1000+800</f>
         <v>8800</v>
       </c>
-      <c r="D60" s="4">
+      <c r="D61" s="4">
         <f t="shared" si="4"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B61" s="4" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B62" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C61" s="5">
+      <c r="C62" s="5">
         <v>6000</v>
       </c>
-      <c r="D61" s="4">
+      <c r="D62" s="4">
         <f t="shared" si="4"/>
         <v>14890</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B62" s="4" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B63" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C62" s="5">
+      <c r="C63" s="5">
         <v>-10000</v>
       </c>
-      <c r="D62" s="4">
+      <c r="D63" s="4">
         <f t="shared" si="4"/>
         <v>4890</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="17" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B64" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C63" s="5">
+      <c r="C64" s="5">
         <v>500</v>
       </c>
-      <c r="D63" s="4">
-        <f t="shared" ref="D63:D68" si="5">D62+C63</f>
+      <c r="D64" s="4">
+        <f t="shared" ref="D64:D69" si="5">D63+C64</f>
         <v>5390</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B64" s="4" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B65" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C64" s="5">
+      <c r="C65" s="5">
         <v>700</v>
       </c>
-      <c r="D64" s="4">
+      <c r="D65" s="4">
         <f t="shared" si="5"/>
         <v>6090</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B65" s="4" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C65" s="5">
+      <c r="C66" s="5">
         <v>1500</v>
       </c>
-      <c r="D65" s="4">
+      <c r="D66" s="4">
         <f t="shared" si="5"/>
         <v>7590</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B66" s="4" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B67" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C66" s="5">
+      <c r="C67" s="5">
         <v>5000</v>
       </c>
-      <c r="D66" s="4">
+      <c r="D67" s="4">
         <f t="shared" si="5"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B67" s="4" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B68" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C67" s="5">
+      <c r="C68" s="5">
         <v>-10000</v>
       </c>
-      <c r="D67" s="4">
+      <c r="D68" s="4">
         <f t="shared" si="5"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="17" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B69" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C68" s="5">
+      <c r="C69" s="5">
         <v>2000</v>
       </c>
-      <c r="D68" s="4">
+      <c r="D69" s="4">
         <f t="shared" si="5"/>
         <v>4590</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B69" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C69" s="5">
-        <v>700</v>
-      </c>
-      <c r="D69" s="4">
-        <f t="shared" ref="D69:D74" si="6">D68+C69</f>
-        <v>5290</v>
-      </c>
-    </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="17" t="s">
-        <v>82</v>
-      </c>
       <c r="B70" s="4" t="s">
         <v>77</v>
       </c>
@@ -2051,401 +2053,404 @@
         <v>700</v>
       </c>
       <c r="D70" s="4">
+        <f t="shared" ref="D70:D75" si="6">D69+C70</f>
+        <v>5290</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C71" s="5">
+        <v>700</v>
+      </c>
+      <c r="D71" s="4">
         <f t="shared" si="6"/>
         <v>5990</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="17" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B72" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C71" s="5">
+      <c r="C72" s="5">
         <v>700</v>
       </c>
-      <c r="D71" s="4">
+      <c r="D72" s="4">
         <f t="shared" si="6"/>
         <v>6690</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="17" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B73" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C72" s="5">
+      <c r="C73" s="5">
         <v>4000</v>
       </c>
-      <c r="D72" s="4">
+      <c r="D73" s="4">
         <f t="shared" si="6"/>
         <v>10690</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B73" s="4" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C73" s="5">
+      <c r="C74" s="5">
         <v>-10000</v>
       </c>
-      <c r="D73" s="4">
+      <c r="D74" s="4">
         <f t="shared" si="6"/>
         <v>690</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="17" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B75" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C74" s="5">
+      <c r="C75" s="5">
         <v>1000</v>
       </c>
-      <c r="D74" s="4">
+      <c r="D75" s="4">
         <f t="shared" si="6"/>
         <v>1690</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="17" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="B76" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C75" s="5">
+      <c r="C76" s="5">
         <v>7000</v>
       </c>
-      <c r="D75" s="4">
-        <f t="shared" ref="D75:D80" si="7">D74+C75</f>
+      <c r="D76" s="4">
+        <f t="shared" ref="D76:D81" si="7">D75+C76</f>
         <v>8690</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B76" s="4" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B77" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C76" s="5">
+      <c r="C77" s="5">
         <v>10000</v>
       </c>
-      <c r="D76" s="4">
+      <c r="D77" s="4">
         <f t="shared" si="7"/>
         <v>18690</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B77" s="4" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B78" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C77" s="5">
+      <c r="C78" s="5">
         <v>-10000</v>
       </c>
-      <c r="D77" s="4">
+      <c r="D78" s="4">
         <f t="shared" si="7"/>
         <v>8690</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B78" s="4" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B79" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C78" s="5">
+      <c r="C79" s="5">
         <v>1700</v>
       </c>
-      <c r="D78" s="4">
+      <c r="D79" s="4">
         <f t="shared" si="7"/>
         <v>10390</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B79" s="4" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B80" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C79" s="5">
+      <c r="C80" s="5">
         <v>-10000</v>
       </c>
-      <c r="D79" s="4">
+      <c r="D80" s="4">
         <f t="shared" si="7"/>
         <v>390</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B80" s="4" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B81" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C80" s="5">
+      <c r="C81" s="5">
         <v>6000</v>
       </c>
-      <c r="D80" s="4">
+      <c r="D81" s="4">
         <f t="shared" si="7"/>
         <v>6390</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="B81" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C81" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D81" s="4">
-        <f t="shared" ref="D81:D86" si="8">D80+C81</f>
-        <v>8390</v>
-      </c>
-    </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C82" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D82" s="4">
+        <f t="shared" ref="D82:D87" si="8">D81+C82</f>
+        <v>8390</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="B82" s="4" t="s">
+      <c r="B83" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C82" s="5">
+      <c r="C83" s="5">
         <v>5000</v>
       </c>
-      <c r="D82" s="4">
+      <c r="D83" s="4">
         <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B83" s="4" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B84" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C83" s="5">
+      <c r="C84" s="5">
         <v>-10000</v>
       </c>
-      <c r="D83" s="4">
+      <c r="D84" s="4">
         <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="17" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="B84" s="4" t="s">
+      <c r="B85" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C84" s="5">
+      <c r="C85" s="5">
         <v>1000</v>
       </c>
-      <c r="D84" s="4">
+      <c r="D85" s="4">
         <f t="shared" si="8"/>
         <v>4390</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B85" s="4" t="s">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B86" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C85" s="5">
+      <c r="C86" s="5">
         <v>9000</v>
       </c>
-      <c r="D85" s="4">
+      <c r="D86" s="4">
         <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B86" s="4" t="s">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B87" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C86" s="5">
+      <c r="C87" s="5">
         <v>-10000</v>
       </c>
-      <c r="D86" s="4">
+      <c r="D87" s="4">
         <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B87" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C87" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D87" s="4">
-        <f t="shared" ref="D87:D92" si="9">D86+C87</f>
-        <v>5390</v>
-      </c>
-    </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B88" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C88" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D88" s="4">
+        <f t="shared" ref="D88:D93" si="9">D87+C88</f>
+        <v>5390</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B89" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C88" s="5">
+      <c r="C89" s="5">
         <v>6000</v>
       </c>
-      <c r="D88" s="4">
+      <c r="D89" s="4">
         <f t="shared" si="9"/>
         <v>11390</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B89" s="4" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B90" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C89" s="5">
+      <c r="C90" s="5">
         <v>-10000</v>
       </c>
-      <c r="D89" s="4">
+      <c r="D90" s="4">
         <f t="shared" si="9"/>
         <v>1390</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B90" s="4" t="s">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B91" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C90" s="5">
+      <c r="C91" s="5">
         <v>400</v>
       </c>
-      <c r="D90" s="4">
+      <c r="D91" s="4">
         <f t="shared" si="9"/>
         <v>1790</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="17" t="s">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="B91" s="4" t="s">
+      <c r="B92" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C91" s="5">
+      <c r="C92" s="5">
         <v>2000</v>
       </c>
-      <c r="D91" s="4">
+      <c r="D92" s="4">
         <f t="shared" si="9"/>
         <v>3790</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="17" t="s">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="B92" s="4" t="s">
+      <c r="B93" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C92" s="5">
+      <c r="C93" s="5">
         <v>6000</v>
       </c>
-      <c r="D92" s="4">
+      <c r="D93" s="4">
         <f t="shared" si="9"/>
         <v>9790</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="17" t="s">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="B93" s="4" t="s">
+      <c r="B94" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C93" s="5">
+      <c r="C94" s="5">
         <v>1000</v>
       </c>
-      <c r="D93" s="4">
-        <f t="shared" ref="D93:D98" si="10">D92+C93</f>
+      <c r="D94" s="4">
+        <f t="shared" ref="D94:D99" si="10">D93+C94</f>
         <v>10790</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B94" s="4" t="s">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B95" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C94" s="5">
+      <c r="C95" s="5">
         <v>-10000</v>
       </c>
-      <c r="D94" s="4">
+      <c r="D95" s="4">
         <f t="shared" si="10"/>
         <v>790</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="17" t="s">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="B95" s="4" t="s">
+      <c r="B96" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C95" s="5">
+      <c r="C96" s="5">
         <v>800</v>
       </c>
-      <c r="D95" s="4">
+      <c r="D96" s="4">
         <f t="shared" si="10"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="17" t="s">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="B96" s="4" t="s">
+      <c r="B97" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C96" s="5">
+      <c r="C97" s="5">
         <v>5000</v>
       </c>
-      <c r="D96" s="4">
+      <c r="D97" s="4">
         <f t="shared" si="10"/>
         <v>6590</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="17" t="s">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="B97" s="4" t="s">
+      <c r="B98" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C97" s="5">
+      <c r="C98" s="5">
         <v>6000</v>
       </c>
-      <c r="D97" s="4">
+      <c r="D98" s="4">
         <f t="shared" si="10"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B98" s="4" t="s">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B99" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C98" s="5">
+      <c r="C99" s="5">
         <v>-10000</v>
       </c>
-      <c r="D98" s="4">
+      <c r="D99" s="4">
         <f t="shared" si="10"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="17" t="s">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="B99" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C99" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D99" s="4">
-        <f t="shared" ref="D99:D105" si="11">D98+C99</f>
-        <v>4590</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B100" s="4" t="s">
         <v>65</v>
       </c>
@@ -2453,667 +2458,706 @@
         <v>2000</v>
       </c>
       <c r="D100" s="4">
+        <f t="shared" ref="D100:D106" si="11">D99+C100</f>
+        <v>4590</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B101" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C101" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D101" s="4">
         <f t="shared" si="11"/>
         <v>6590</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B101" s="4" t="s">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B102" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C101" s="5">
+      <c r="C102" s="5">
         <v>7000</v>
       </c>
-      <c r="D101" s="4">
+      <c r="D102" s="4">
         <f t="shared" si="11"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B102" s="4" t="s">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B103" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C102" s="5">
+      <c r="C103" s="5">
         <v>-10000</v>
       </c>
-      <c r="D102" s="4">
+      <c r="D103" s="4">
         <f t="shared" si="11"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="17" t="s">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="B103" s="4" t="s">
+      <c r="B104" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C103" s="5">
+      <c r="C104" s="5">
         <v>2000</v>
       </c>
-      <c r="D103" s="4">
+      <c r="D104" s="4">
         <f t="shared" si="11"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="17" t="s">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="B104" s="4" t="s">
+      <c r="B105" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C104" s="5">
+      <c r="C105" s="5">
         <v>6000</v>
       </c>
-      <c r="D104" s="4">
+      <c r="D105" s="4">
         <f t="shared" si="11"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B105" s="4" t="s">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B106" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C105" s="5">
+      <c r="C106" s="5">
         <v>-10000</v>
       </c>
-      <c r="D105" s="4">
+      <c r="D106" s="4">
         <f t="shared" si="11"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="B106" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C106" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D106" s="4">
-        <f t="shared" ref="D106:D111" si="12">D105+C106</f>
-        <v>3590</v>
-      </c>
-    </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="B107" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C107" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D107" s="4">
+        <f t="shared" ref="D107:D112" si="12">D106+C107</f>
+        <v>3590</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="B107" s="4" t="s">
+      <c r="B108" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C107" s="5">
+      <c r="C108" s="5">
         <v>7000</v>
       </c>
-      <c r="D107" s="4">
+      <c r="D108" s="4">
         <f t="shared" si="12"/>
         <v>10590</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B108" s="4" t="s">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B109" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C108" s="5">
+      <c r="C109" s="5">
         <v>-10000</v>
       </c>
-      <c r="D108" s="4">
+      <c r="D109" s="4">
         <f t="shared" si="12"/>
         <v>590</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B109" s="4" t="s">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B110" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C109" s="5">
+      <c r="C110" s="5">
         <v>12000</v>
       </c>
-      <c r="D109" s="4">
+      <c r="D110" s="4">
         <f t="shared" si="12"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B110" s="4" t="s">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B111" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C110" s="5">
+      <c r="C111" s="5">
         <v>-10000</v>
       </c>
-      <c r="D110" s="4">
+      <c r="D111" s="4">
         <f t="shared" si="12"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B111" s="4" t="s">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B112" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C111" s="5">
+      <c r="C112" s="5">
         <v>2000</v>
       </c>
-      <c r="D111" s="4">
+      <c r="D112" s="4">
         <f t="shared" si="12"/>
         <v>4590</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="B112" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C112" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D112" s="4">
-        <f t="shared" ref="D112:D117" si="13">D111+C112</f>
-        <v>6590</v>
-      </c>
-    </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="B113" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C113" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D113" s="4">
+        <f t="shared" ref="D113:D118" si="13">D112+C113</f>
+        <v>6590</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="B113" s="4" t="s">
+      <c r="B114" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C113" s="5">
+      <c r="C114" s="5">
         <v>7000</v>
       </c>
-      <c r="D113" s="4">
+      <c r="D114" s="4">
         <f t="shared" si="13"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B114" s="4" t="s">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B115" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C114" s="5">
+      <c r="C115" s="5">
         <v>-10000</v>
       </c>
-      <c r="D114" s="4">
+      <c r="D115" s="4">
         <f t="shared" si="13"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="17" t="s">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="B115" s="4" t="s">
+      <c r="B116" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C115" s="5">
+      <c r="C116" s="5">
         <v>2000</v>
       </c>
-      <c r="D115" s="4">
+      <c r="D116" s="4">
         <f t="shared" si="13"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="17" t="s">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="B116" s="4" t="s">
+      <c r="B117" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C116" s="5">
+      <c r="C117" s="5">
         <v>8000</v>
       </c>
-      <c r="D116" s="4">
+      <c r="D117" s="4">
         <f t="shared" si="13"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B117" s="4" t="s">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B118" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C117" s="5">
+      <c r="C118" s="5">
         <v>-10000</v>
       </c>
-      <c r="D117" s="4">
+      <c r="D118" s="4">
         <f t="shared" si="13"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="17" t="s">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="B118" s="4" t="s">
+      <c r="B119" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C118" s="5">
+      <c r="C119" s="5">
         <v>2000</v>
       </c>
-      <c r="D118" s="4">
-        <f t="shared" ref="D118:D123" si="14">D117+C118</f>
+      <c r="D119" s="4">
+        <f t="shared" ref="D119:D124" si="14">D118+C119</f>
         <v>5590</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B119" s="4" t="s">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B120" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C119" s="5">
+      <c r="C120" s="5">
         <v>5000</v>
       </c>
-      <c r="D119" s="4">
+      <c r="D120" s="4">
         <f t="shared" si="14"/>
         <v>10590</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B120" s="4" t="s">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B121" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C120" s="5">
+      <c r="C121" s="5">
         <v>-10000</v>
       </c>
-      <c r="D120" s="4">
+      <c r="D121" s="4">
         <f t="shared" si="14"/>
         <v>590</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B121" s="4" t="s">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B122" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C121" s="5">
+      <c r="C122" s="5">
         <v>2000</v>
       </c>
-      <c r="D121" s="4">
+      <c r="D122" s="4">
         <f t="shared" si="14"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B122" s="4" t="s">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B123" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C122" s="5">
+      <c r="C123" s="5">
         <v>9000</v>
       </c>
-      <c r="D122" s="4">
+      <c r="D123" s="4">
         <f t="shared" si="14"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B123" s="4" t="s">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B124" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C123" s="5">
+      <c r="C124" s="5">
         <v>-10000</v>
       </c>
-      <c r="D123" s="4">
+      <c r="D124" s="4">
         <f t="shared" si="14"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="B124" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C124" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D124" s="4">
-        <f t="shared" ref="D124:D129" si="15">D123+C124</f>
-        <v>3590</v>
-      </c>
-    </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="B125" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C125" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D125" s="4">
+        <f t="shared" ref="D125:D130" si="15">D124+C125</f>
+        <v>3590</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="B125" s="4" t="s">
+      <c r="B126" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C125" s="5">
+      <c r="C126" s="5">
         <v>8000</v>
       </c>
-      <c r="D125" s="4">
+      <c r="D126" s="4">
         <f t="shared" si="15"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B126" s="4" t="s">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B127" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C126" s="5">
+      <c r="C127" s="5">
         <v>-10000</v>
       </c>
-      <c r="D126" s="4">
+      <c r="D127" s="4">
         <f t="shared" si="15"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="17" t="s">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="B127" s="4" t="s">
+      <c r="B128" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C127" s="5">
+      <c r="C128" s="5">
         <v>2000</v>
       </c>
-      <c r="D127" s="4">
+      <c r="D128" s="4">
         <f t="shared" si="15"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="17" t="s">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="B128" s="4" t="s">
+      <c r="B129" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="C128" s="5">
+      <c r="C129" s="5">
         <v>12000</v>
       </c>
-      <c r="D128" s="4">
+      <c r="D129" s="4">
         <f t="shared" si="15"/>
         <v>15590</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B129" s="4" t="s">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B130" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C129" s="5">
+      <c r="C130" s="5">
         <v>-10000</v>
       </c>
-      <c r="D129" s="4">
+      <c r="D130" s="4">
         <f t="shared" si="15"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="17" t="s">
-        <v>168</v>
-      </c>
-      <c r="B130" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="C130" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D130" s="4">
-        <f t="shared" ref="D130:D135" si="16">D129+C130</f>
-        <v>7590</v>
-      </c>
-    </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="B131" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C131" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D131" s="4">
+        <f t="shared" ref="D131:D136" si="16">D130+C131</f>
+        <v>7590</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="B131" s="4" t="s">
+      <c r="B132" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="C131" s="5">
+      <c r="C132" s="5">
         <v>10000</v>
       </c>
-      <c r="D131" s="4">
+      <c r="D132" s="4">
         <f t="shared" si="16"/>
         <v>17590</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B132" s="4" t="s">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B133" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C132" s="5">
+      <c r="C133" s="5">
         <v>-10000</v>
       </c>
-      <c r="D132" s="4">
+      <c r="D133" s="4">
         <f t="shared" si="16"/>
         <v>7590</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B133" s="4" t="s">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B134" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="C133" s="5">
+      <c r="C134" s="5">
         <v>2000</v>
       </c>
-      <c r="D133" s="4">
+      <c r="D134" s="4">
         <f t="shared" si="16"/>
         <v>9590</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="17" t="s">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="B134" s="4" t="s">
+      <c r="B135" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="C134" s="5">
+      <c r="C135" s="5">
         <v>-1200</v>
       </c>
-      <c r="D134" s="4">
+      <c r="D135" s="4">
         <f t="shared" si="16"/>
         <v>8390</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B135" s="4" t="s">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B136" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="C135" s="5">
+      <c r="C136" s="5">
         <v>500</v>
       </c>
-      <c r="D135" s="4">
+      <c r="D136" s="4">
         <f t="shared" si="16"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="B136" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C136" s="5">
-        <v>750</v>
-      </c>
-      <c r="D136" s="4">
-        <f t="shared" ref="D136:D141" si="17">D135+C136</f>
-        <v>9640</v>
-      </c>
-    </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="B137" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C137" s="5">
+        <v>750</v>
+      </c>
+      <c r="D137" s="4">
+        <f t="shared" ref="D137:D142" si="17">D136+C137</f>
+        <v>9640</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="B137" s="4" t="s">
+      <c r="B138" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C137" s="5">
+      <c r="C138" s="5">
         <v>2000</v>
       </c>
-      <c r="D137" s="4">
+      <c r="D138" s="4">
         <f t="shared" si="17"/>
         <v>11640</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B138" s="4" t="s">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B139" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C138" s="5">
+      <c r="C139" s="5">
         <v>2000</v>
       </c>
-      <c r="D138" s="4">
+      <c r="D139" s="4">
         <f t="shared" si="17"/>
         <v>13640</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B139" s="4" t="s">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B140" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C139" s="5">
+      <c r="C140" s="5">
         <v>-10000</v>
       </c>
-      <c r="D139" s="4">
+      <c r="D140" s="4">
         <f t="shared" si="17"/>
         <v>3640</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B140" s="4" t="s">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B141" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="C140" s="5">
+      <c r="C141" s="5">
         <v>350</v>
       </c>
-      <c r="D140" s="4">
+      <c r="D141" s="4">
         <f t="shared" si="17"/>
         <v>3990</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="17" t="s">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="B141" s="4" t="s">
+      <c r="B142" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="C141" s="5">
+      <c r="C142" s="5">
         <v>300</v>
       </c>
-      <c r="D141" s="4">
+      <c r="D142" s="4">
         <f t="shared" si="17"/>
         <v>4290</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="17" t="s">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" s="17" t="s">
         <v>181</v>
       </c>
-      <c r="B142" s="4" t="s">
+      <c r="B143" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="C142" s="5">
+      <c r="C143" s="5">
         <v>3800</v>
       </c>
-      <c r="D142" s="4">
-        <f t="shared" ref="D142:D148" si="18">D141+C142</f>
+      <c r="D143" s="4">
+        <f t="shared" ref="D143:D149" si="18">D142+C143</f>
         <v>8090</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B143" s="4" t="s">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B144" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C143" s="5">
+      <c r="C144" s="5">
         <v>500</v>
       </c>
-      <c r="D143" s="4">
+      <c r="D144" s="4">
         <f t="shared" si="18"/>
         <v>8590</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="17" t="s">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="B144" s="4" t="s">
+      <c r="B145" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="C144" s="5">
+      <c r="C145" s="5">
         <v>1300</v>
       </c>
-      <c r="D144" s="4">
+      <c r="D145" s="4">
         <f t="shared" si="18"/>
         <v>9890</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="17" t="s">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" s="17" t="s">
         <v>185</v>
       </c>
-      <c r="B145" s="4" t="s">
+      <c r="B146" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C145" s="5">
+      <c r="C146" s="5">
         <v>9000</v>
       </c>
-      <c r="D145" s="4">
+      <c r="D146" s="4">
         <f t="shared" si="18"/>
         <v>18890</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B146" s="4" t="s">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B147" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C146" s="5">
+      <c r="C147" s="5">
         <v>-10000</v>
       </c>
-      <c r="D146" s="4">
+      <c r="D147" s="4">
         <f t="shared" si="18"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="17" t="s">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="B147" s="4" t="s">
+      <c r="B148" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C147" s="5">
+      <c r="C148" s="5">
         <v>2000</v>
       </c>
-      <c r="D147" s="4">
+      <c r="D148" s="4">
         <f t="shared" si="18"/>
         <v>10890</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B148" s="4" t="s">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B149" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C148" s="5">
+      <c r="C149" s="5">
         <v>-10000</v>
       </c>
-      <c r="D148" s="4">
+      <c r="D149" s="4">
         <f t="shared" si="18"/>
         <v>890</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="17" t="s">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="B149" s="4" t="s">
+      <c r="B150" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="C149" s="5">
+      <c r="C150" s="5">
         <v>500</v>
       </c>
-      <c r="D149" s="4">
-        <f>D148+C149</f>
+      <c r="D150" s="4">
+        <f>D149+C150</f>
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="B151" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C151" s="5">
+        <v>10000</v>
+      </c>
+      <c r="D151" s="4">
+        <f>D150+C151</f>
+        <v>11390</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B152" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C152" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D152" s="4">
+        <f>D151+C152</f>
         <v>1390</v>
       </c>
     </row>

</xml_diff>

<commit_message>
duy lay tien loi ngay 0108
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="194">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -598,6 +598,9 @@
   </si>
   <si>
     <t>31/07/2024</t>
+  </si>
+  <si>
+    <t>01/08/2024</t>
   </si>
 </sst>
 </file>
@@ -1076,11 +1079,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K153"/>
+  <dimension ref="A1:K154"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D154" sqref="D154"/>
+      <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D155" sqref="D155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3177,6 +3180,21 @@
       <c r="D153" s="4">
         <f>D152+C153</f>
         <v>4390</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="B154" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C154" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D154" s="4">
+        <f>D153+C154</f>
+        <v>6390</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Duy chuyen cho co diem 2tr
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="CÔ DIỄM" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="194">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -1079,11 +1079,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K154"/>
+  <dimension ref="A1:K155"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D155" sqref="D155"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D165" sqref="D165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3195,6 +3195,18 @@
       <c r="D154" s="4">
         <f>D153+C154</f>
         <v>6390</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B155" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C155" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D155" s="4">
+        <f>D154+C155</f>
+        <v>8390</v>
       </c>
     </row>
   </sheetData>
@@ -3666,8 +3678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3683,7 +3695,7 @@
         <v>108</v>
       </c>
       <c r="B1">
-        <v>400000</v>
+        <v>430000</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3770,7 +3782,7 @@
       </c>
       <c r="B23">
         <f>SUM(B1:B20)</f>
-        <v>524580</v>
+        <v>554580</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
duy update ghi chu co diem
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="CÔ DIỄM" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="193">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -580,9 +580,6 @@
   </si>
   <si>
     <t>23/07/2024</t>
-  </si>
-  <si>
-    <t>chua lam giay</t>
   </si>
   <si>
     <t>25/07/2024</t>
@@ -1081,9 +1078,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K155"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D165" sqref="D165"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1311,9 +1308,7 @@
       <c r="I17" s="5">
         <v>10</v>
       </c>
-      <c r="K17" s="14" t="s">
-        <v>187</v>
-      </c>
+      <c r="K17" s="14"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
@@ -1443,14 +1438,12 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H28" s="17" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I28" s="5">
         <v>10</v>
       </c>
-      <c r="K28" s="14" t="s">
-        <v>187</v>
-      </c>
+      <c r="K28" s="14"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
@@ -3127,31 +3120,31 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="B150" s="4" t="s">
         <v>188</v>
-      </c>
-      <c r="B150" s="4" t="s">
-        <v>189</v>
       </c>
       <c r="C150" s="5">
         <v>500</v>
       </c>
       <c r="D150" s="4">
-        <f>D149+C150</f>
+        <f t="shared" ref="D150:D155" si="19">D149+C150</f>
         <v>1390</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="B151" s="4" t="s">
         <v>190</v>
-      </c>
-      <c r="B151" s="4" t="s">
-        <v>191</v>
       </c>
       <c r="C151" s="5">
         <v>10000</v>
       </c>
       <c r="D151" s="4">
-        <f>D150+C151</f>
+        <f t="shared" si="19"/>
         <v>11390</v>
       </c>
     </row>
@@ -3163,13 +3156,13 @@
         <v>-10000</v>
       </c>
       <c r="D152" s="4">
-        <f>D151+C152</f>
+        <f t="shared" si="19"/>
         <v>1390</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="17" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B153" s="4" t="s">
         <v>25</v>
@@ -3178,13 +3171,13 @@
         <v>3000</v>
       </c>
       <c r="D153" s="4">
-        <f>D152+C153</f>
+        <f t="shared" si="19"/>
         <v>4390</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B154" s="4" t="s">
         <v>65</v>
@@ -3193,7 +3186,7 @@
         <v>2000</v>
       </c>
       <c r="D154" s="4">
-        <f>D153+C154</f>
+        <f t="shared" si="19"/>
         <v>6390</v>
       </c>
     </row>
@@ -3205,7 +3198,7 @@
         <v>2000</v>
       </c>
       <c r="D155" s="4">
-        <f>D154+C155</f>
+        <f t="shared" si="19"/>
         <v>8390</v>
       </c>
     </row>
@@ -3678,7 +3671,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
duy lay tien loi ngay 0208 co diem
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="195">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -598,6 +598,12 @@
   </si>
   <si>
     <t>01/08/2024</t>
+  </si>
+  <si>
+    <t>02/08/2024</t>
+  </si>
+  <si>
+    <t>Duy lấy tiền lời 11tr</t>
   </si>
 </sst>
 </file>
@@ -1076,11 +1082,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K155"/>
+  <dimension ref="A1:K157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K28" sqref="K28"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1157,7 +1163,7 @@
       </c>
       <c r="J3" s="4">
         <f>SUM(I3:I59)</f>
-        <v>430</v>
+        <v>440</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1712,6 +1718,12 @@
         <f t="shared" ref="D44:D49" si="2">D43+C44</f>
         <v>9090</v>
       </c>
+      <c r="H44" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="I44" s="5">
+        <v>10</v>
+      </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="s">
@@ -3200,6 +3212,33 @@
       <c r="D155" s="4">
         <f t="shared" si="19"/>
         <v>8390</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="B156" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C156" s="5">
+        <v>11000</v>
+      </c>
+      <c r="D156" s="4">
+        <f>D155+C156</f>
+        <v>19390</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B157" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C157" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D157" s="4">
+        <f>D156+C157</f>
+        <v>9390</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
duy chuyen cho co diem 3tr
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="197">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -604,6 +604,12 @@
   </si>
   <si>
     <t>Duy lấy tiền lời 11tr</t>
+  </si>
+  <si>
+    <t>06/08/2024</t>
+  </si>
+  <si>
+    <t>Duy chuyển cho cô Diễm 3tr</t>
   </si>
 </sst>
 </file>
@@ -1082,11 +1088,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K157"/>
+  <dimension ref="A1:K159"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I45" sqref="I45"/>
+      <selection pane="bottomLeft" activeCell="K155" sqref="K155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1163,7 +1169,7 @@
       </c>
       <c r="J3" s="4">
         <f>SUM(I3:I59)</f>
-        <v>440</v>
+        <v>450</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1736,6 +1742,12 @@
         <f t="shared" si="2"/>
         <v>12090</v>
       </c>
+      <c r="H45" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="I45" s="5">
+        <v>10</v>
+      </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B46" s="4" t="s">
@@ -3239,6 +3251,33 @@
       <c r="D157" s="4">
         <f>D156+C157</f>
         <v>9390</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="B158" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="C158" s="5">
+        <v>3000</v>
+      </c>
+      <c r="D158" s="4">
+        <f>D157+C158</f>
+        <v>12390</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B159" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C159" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D159" s="4">
+        <f>D158+C159</f>
+        <v>2390</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
duy chuyen cho co diem 5tr600
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="199">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -610,6 +610,12 @@
   </si>
   <si>
     <t>Duy chuyển cho cô Diễm 3tr</t>
+  </si>
+  <si>
+    <t>07/08/2024</t>
+  </si>
+  <si>
+    <t>Duy chuyển cho cô Diễm 5.600k</t>
   </si>
 </sst>
 </file>
@@ -1088,11 +1094,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K160"/>
+  <dimension ref="A1:K161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A145" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D161" sqref="D161"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D173" sqref="D173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3290,6 +3296,21 @@
       <c r="D160" s="4">
         <f>D159+C160</f>
         <v>2890</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="B161" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="C161" s="5">
+        <v>5600</v>
+      </c>
+      <c r="D161" s="4">
+        <f>D160+C161</f>
+        <v>8490</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
duy chuyen cho co diem 4tr700
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="CÔ DIỄM" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="200">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -616,6 +616,9 @@
   </si>
   <si>
     <t>Duy chuyển cho cô Diễm 5.600k</t>
+  </si>
+  <si>
+    <t>Duy chuyển cho cô Diễm 4.700k</t>
   </si>
 </sst>
 </file>
@@ -1094,11 +1097,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K161"/>
+  <dimension ref="A1:K162"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D173" sqref="D173"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A135" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D163" sqref="D163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3243,7 +3246,7 @@
         <v>11000</v>
       </c>
       <c r="D156" s="4">
-        <f>D155+C156</f>
+        <f t="shared" ref="D156:D161" si="20">D155+C156</f>
         <v>19390</v>
       </c>
     </row>
@@ -3255,7 +3258,7 @@
         <v>-10000</v>
       </c>
       <c r="D157" s="4">
-        <f>D156+C157</f>
+        <f t="shared" si="20"/>
         <v>9390</v>
       </c>
     </row>
@@ -3270,7 +3273,7 @@
         <v>3000</v>
       </c>
       <c r="D158" s="4">
-        <f>D157+C158</f>
+        <f t="shared" si="20"/>
         <v>12390</v>
       </c>
     </row>
@@ -3282,7 +3285,7 @@
         <v>-10000</v>
       </c>
       <c r="D159" s="4">
-        <f>D158+C159</f>
+        <f t="shared" si="20"/>
         <v>2390</v>
       </c>
     </row>
@@ -3294,7 +3297,7 @@
         <v>500</v>
       </c>
       <c r="D160" s="4">
-        <f>D159+C160</f>
+        <f t="shared" si="20"/>
         <v>2890</v>
       </c>
     </row>
@@ -3309,8 +3312,20 @@
         <v>5600</v>
       </c>
       <c r="D161" s="4">
-        <f>D160+C161</f>
+        <f t="shared" si="20"/>
         <v>8490</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B162" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="C162" s="5">
+        <v>4700</v>
+      </c>
+      <c r="D162" s="4">
+        <f>D161+C162</f>
+        <v>13190</v>
       </c>
     </row>
   </sheetData>
@@ -3782,7 +3797,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -3799,7 +3814,7 @@
         <v>108</v>
       </c>
       <c r="B1">
-        <v>430000</v>
+        <v>450000</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3815,7 +3830,7 @@
         <v>110</v>
       </c>
       <c r="B3">
-        <v>40000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Duy chuyen cho co diem 1tr500
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="CÔ DIỄM" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="201">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -619,6 +619,9 @@
   </si>
   <si>
     <t>Duy chuyển cho cô Diễm 4.700k</t>
+  </si>
+  <si>
+    <t>08/08/2024</t>
   </si>
 </sst>
 </file>
@@ -1097,11 +1100,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K162"/>
+  <dimension ref="A1:K163"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A135" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D163" sqref="D163"/>
+      <selection pane="bottomLeft" activeCell="D164" sqref="D164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3326,6 +3329,21 @@
       <c r="D162" s="4">
         <f>D161+C162</f>
         <v>13190</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="B163" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C163" s="5">
+        <v>1500</v>
+      </c>
+      <c r="D163" s="4">
+        <f>D162+C163</f>
+        <v>14690</v>
       </c>
     </row>
   </sheetData>
@@ -3797,7 +3815,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
duy chuyen cho co diem 500k
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CÔ DIỄM" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="201">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -1100,11 +1100,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K163"/>
+  <dimension ref="A1:K164"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A135" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D164" sqref="D164"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A138" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K165" sqref="K165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3344,6 +3344,18 @@
       <c r="D163" s="4">
         <f>D162+C163</f>
         <v>14690</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B164" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C164" s="5">
+        <v>500</v>
+      </c>
+      <c r="D164" s="4">
+        <f>D163+C164</f>
+        <v>15190</v>
       </c>
     </row>
   </sheetData>
@@ -3498,7 +3510,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K29" sqref="K29"/>
     </sheetView>

</xml_diff>

<commit_message>
Duy lay tien loi ngay 13, cho co diem vay 20tr
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="CÔ DIỄM" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="207">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -634,6 +634,12 @@
   </si>
   <si>
     <t>Duy chuyển cho cô Diễm 1tr</t>
+  </si>
+  <si>
+    <t>13/08/2024</t>
+  </si>
+  <si>
+    <t>Duy cho cô Diễm vay 20tr</t>
   </si>
 </sst>
 </file>
@@ -1112,11 +1118,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K166"/>
+  <dimension ref="A1:K169"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D167" sqref="D167"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1192,8 +1198,8 @@
         <v>20</v>
       </c>
       <c r="J3" s="4">
-        <f>SUM(I3:I59)</f>
-        <v>450</v>
+        <f>SUM(I3:I60)</f>
+        <v>470</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1205,36 +1211,26 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="5">
-        <v>14560</v>
-      </c>
-      <c r="D5" s="4">
-        <f>C5+D3</f>
-        <v>18490</v>
-      </c>
       <c r="H5" s="17" t="s">
-        <v>7</v>
+        <v>205</v>
       </c>
       <c r="I5" s="5">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" s="5">
-        <v>-10000</v>
+        <v>14560</v>
       </c>
       <c r="D6" s="4">
-        <f t="shared" ref="D6:D20" si="0">D5+C6</f>
-        <v>8490</v>
+        <f>C6+D3</f>
+        <v>18490</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I6" s="5">
         <v>10</v>
@@ -1242,25 +1238,35 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D7" s="4">
+        <f t="shared" ref="D7:D21" si="0">D6+C7</f>
+        <v>8490</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C8" s="5">
         <v>2000</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D8" s="4">
         <f t="shared" si="0"/>
         <v>10490</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H8" s="17" t="s">
         <v>9</v>
-      </c>
-      <c r="I7" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H8" s="17" t="s">
-        <v>41</v>
       </c>
       <c r="I8" s="5">
         <v>10</v>
@@ -1268,16 +1274,15 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H9" s="17" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="I9" s="5">
         <v>10</v>
       </c>
-      <c r="K9" s="14"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H10" s="17" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="I10" s="5">
         <v>10</v>
@@ -1286,7 +1291,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H11" s="17" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="I11" s="5">
         <v>10</v>
@@ -1295,7 +1300,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H12" s="17" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="I12" s="5">
         <v>10</v>
@@ -1304,7 +1309,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H13" s="17" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="I13" s="5">
         <v>10</v>
@@ -1313,7 +1318,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H14" s="17" t="s">
-        <v>185</v>
+        <v>149</v>
       </c>
       <c r="I14" s="5">
         <v>10</v>
@@ -1322,24 +1327,24 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H15" s="17" t="s">
-        <v>70</v>
+        <v>185</v>
       </c>
       <c r="I15" s="5">
         <v>10</v>
       </c>
+      <c r="K15" s="14"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H16" s="17" t="s">
-        <v>107</v>
+        <v>70</v>
       </c>
       <c r="I16" s="5">
         <v>10</v>
       </c>
-      <c r="K16" s="14"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H17" s="17" t="s">
-        <v>186</v>
+        <v>107</v>
       </c>
       <c r="I17" s="5">
         <v>10</v>
@@ -1347,18 +1352,8 @@
       <c r="K17" s="14"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="5">
-        <v>-10000</v>
-      </c>
-      <c r="D18" s="4">
-        <f>D7+C18</f>
-        <v>490</v>
-      </c>
       <c r="H18" s="17" t="s">
-        <v>10</v>
+        <v>186</v>
       </c>
       <c r="I18" s="5">
         <v>10</v>
@@ -1366,52 +1361,62 @@
       <c r="K18" s="14"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
+      <c r="B19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D19" s="4">
+        <f>D8+C19</f>
+        <v>490</v>
+      </c>
+      <c r="H19" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I19" s="5">
+        <v>10</v>
+      </c>
+      <c r="K19" s="14"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B20" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C20" s="5">
         <v>2000</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D20" s="4">
         <f t="shared" si="0"/>
         <v>2490</v>
       </c>
-      <c r="H19" s="17" t="s">
+      <c r="H20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I19" s="5">
+      <c r="I20" s="5">
         <v>10</v>
       </c>
-      <c r="K19" s="14"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
+      <c r="K20" s="14"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B21" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C21" s="5">
         <v>3000</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D21" s="4">
         <f t="shared" si="0"/>
         <v>5490</v>
       </c>
-      <c r="H20" s="17" t="s">
+      <c r="H21" s="17" t="s">
         <v>24</v>
-      </c>
-      <c r="I20" s="5">
-        <v>10</v>
-      </c>
-      <c r="K20" s="14"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H21" s="17" t="s">
-        <v>59</v>
       </c>
       <c r="I21" s="5">
         <v>10</v>
@@ -1420,7 +1425,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H22" s="17" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="I22" s="5">
         <v>10</v>
@@ -1429,7 +1434,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H23" s="17" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="I23" s="5">
         <v>10</v>
@@ -1438,7 +1443,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H24" s="17" t="s">
-        <v>121</v>
+        <v>91</v>
       </c>
       <c r="I24" s="5">
         <v>10</v>
@@ -1447,7 +1452,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H25" s="17" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="I25" s="5">
         <v>10</v>
@@ -1456,7 +1461,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H26" s="17" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="I26" s="5">
         <v>10</v>
@@ -1465,7 +1470,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H27" s="17" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="I27" s="5">
         <v>10</v>
@@ -1474,7 +1479,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H28" s="17" t="s">
-        <v>189</v>
+        <v>151</v>
       </c>
       <c r="I28" s="5">
         <v>10</v>
@@ -1482,38 +1487,38 @@
       <c r="K28" s="14"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C29" s="5">
-        <v>3000</v>
-      </c>
-      <c r="D29" s="4">
-        <f>D20+C29</f>
-        <v>8490</v>
-      </c>
       <c r="H29" s="17" t="s">
-        <v>12</v>
+        <v>189</v>
       </c>
       <c r="I29" s="5">
         <v>10</v>
       </c>
+      <c r="K29" s="14"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="5">
+        <v>3000</v>
+      </c>
+      <c r="D30" s="4">
+        <f>D21+C30</f>
+        <v>8490</v>
+      </c>
       <c r="H30" s="17" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="I30" s="5">
         <v>10</v>
       </c>
-      <c r="K30" s="14"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H31" s="17" t="s">
-        <v>146</v>
+        <v>43</v>
       </c>
       <c r="I31" s="5">
         <v>10</v>
@@ -1522,7 +1527,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H32" s="17" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="I32" s="5">
         <v>10</v>
@@ -1531,7 +1536,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H33" s="17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I33" s="5">
         <v>10</v>
@@ -1539,56 +1544,46 @@
       <c r="K33" s="14"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B34" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C34" s="5">
-        <v>4400</v>
-      </c>
-      <c r="D34" s="4">
-        <f>D29+C34</f>
-        <v>12890</v>
-      </c>
       <c r="H34" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I34" s="5">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K34" s="14"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C35" s="5">
-        <v>-10000</v>
+        <v>4400</v>
       </c>
       <c r="D35" s="4">
-        <f>D34+C35</f>
-        <v>2890</v>
+        <f>D30+C35</f>
+        <v>12890</v>
       </c>
       <c r="H35" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I35" s="5">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="K35" s="14"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C36" s="5">
-        <v>1600</v>
+        <v>-10000</v>
       </c>
       <c r="D36" s="4">
-        <f t="shared" ref="D36:D43" si="1">D35+C36</f>
-        <v>4490</v>
+        <f>D35+C36</f>
+        <v>2890</v>
       </c>
       <c r="H36" s="17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I36" s="5">
         <v>10</v>
@@ -1597,517 +1592,521 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" s="5">
+        <v>1600</v>
+      </c>
+      <c r="D37" s="4">
+        <f t="shared" ref="D37:D44" si="1">D36+C37</f>
+        <v>4490</v>
+      </c>
+      <c r="H37" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="I37" s="5">
+        <v>10</v>
+      </c>
+      <c r="K37" s="14"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B38" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C37" s="5">
+      <c r="C38" s="5">
         <v>3000</v>
       </c>
-      <c r="D37" s="4">
+      <c r="D38" s="4">
         <f t="shared" si="1"/>
         <v>7490</v>
       </c>
-      <c r="H37" s="17" t="s">
+      <c r="H38" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="I37" s="5">
+      <c r="I38" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="17" t="s">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B39" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C38" s="5">
+      <c r="C39" s="5">
         <v>2000</v>
       </c>
-      <c r="D38" s="4">
+      <c r="D39" s="4">
         <f t="shared" si="1"/>
         <v>9490</v>
       </c>
-      <c r="H38" s="17" t="s">
+      <c r="H39" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="I38" s="5">
+      <c r="I39" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="17" t="s">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B40" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C39" s="5">
+      <c r="C40" s="5">
         <v>3000</v>
       </c>
-      <c r="D39" s="4">
+      <c r="D40" s="4">
         <f t="shared" si="1"/>
         <v>12490</v>
       </c>
-      <c r="H39" s="17" t="s">
+      <c r="H40" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="I39" s="5">
+      <c r="I40" s="5">
         <v>10</v>
       </c>
-      <c r="K39" s="14"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B40" s="4" t="s">
+      <c r="K40" s="14"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B41" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C40" s="5">
+      <c r="C41" s="5">
         <v>-10000</v>
       </c>
-      <c r="D40" s="4">
+      <c r="D41" s="4">
         <f t="shared" si="1"/>
         <v>2490</v>
       </c>
-      <c r="H40" s="17" t="s">
+      <c r="H41" s="17" t="s">
         <v>159</v>
       </c>
-      <c r="I40" s="5">
+      <c r="I41" s="5">
         <v>10</v>
       </c>
-      <c r="K40" s="14"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="17" t="s">
+      <c r="K41" s="14"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B42" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C41" s="5">
+      <c r="C42" s="5">
         <v>4960</v>
       </c>
-      <c r="D41" s="4">
+      <c r="D42" s="4">
         <f t="shared" si="1"/>
         <v>7450</v>
       </c>
-      <c r="H41" s="17" t="s">
+      <c r="H42" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="I41" s="5">
+      <c r="I42" s="5">
         <v>10</v>
       </c>
-      <c r="K41" s="14"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="17" t="s">
+      <c r="K42" s="14"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B43" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C43" s="5">
         <v>4000</v>
       </c>
-      <c r="D42" s="4">
+      <c r="D43" s="4">
         <f t="shared" si="1"/>
         <v>11450</v>
       </c>
-      <c r="H42" s="17" t="s">
+      <c r="H43" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="I42" s="5">
+      <c r="I43" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B43" s="4" t="s">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B44" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C43" s="5">
+      <c r="C44" s="5">
         <v>-10000</v>
       </c>
-      <c r="D43" s="4">
+      <c r="D44" s="4">
         <f t="shared" si="1"/>
         <v>1450</v>
       </c>
-      <c r="H43" s="17" t="s">
+      <c r="H44" s="17" t="s">
         <v>156</v>
-      </c>
-      <c r="I43" s="5">
-        <v>10</v>
-      </c>
-      <c r="K43" s="14"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B44" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C44" s="5">
-        <v>7640</v>
-      </c>
-      <c r="D44" s="4">
-        <f t="shared" ref="D44:D49" si="2">D43+C44</f>
-        <v>9090</v>
-      </c>
-      <c r="H44" s="17" t="s">
-        <v>193</v>
       </c>
       <c r="I44" s="5">
         <v>10</v>
       </c>
+      <c r="K44" s="14"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C45" s="5">
+        <v>7640</v>
+      </c>
+      <c r="D45" s="4">
+        <f t="shared" ref="D45:D50" si="2">D44+C45</f>
+        <v>9090</v>
+      </c>
+      <c r="H45" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="I45" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B46" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C45" s="5">
+      <c r="C46" s="5">
         <v>3000</v>
       </c>
-      <c r="D45" s="4">
+      <c r="D46" s="4">
         <f t="shared" si="2"/>
         <v>12090</v>
       </c>
-      <c r="H45" s="17" t="s">
+      <c r="H46" s="17" t="s">
         <v>195</v>
       </c>
-      <c r="I45" s="5">
+      <c r="I46" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B46" s="4" t="s">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B47" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C46" s="5">
+      <c r="C47" s="5">
         <v>-10000</v>
       </c>
-      <c r="D46" s="4">
+      <c r="D47" s="4">
         <f t="shared" si="2"/>
         <v>2090</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B47" s="4" t="s">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B48" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C48" s="5">
         <v>800</v>
       </c>
-      <c r="D47" s="4">
+      <c r="D48" s="4">
         <f t="shared" si="2"/>
         <v>2890</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="17" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B49" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C48" s="5">
+      <c r="C49" s="5">
         <v>2000</v>
       </c>
-      <c r="D48" s="4">
+      <c r="D49" s="4">
         <f t="shared" si="2"/>
         <v>4890</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="17" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B50" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C49" s="5">
+      <c r="C50" s="5">
         <v>4000</v>
       </c>
-      <c r="D49" s="4">
+      <c r="D50" s="4">
         <f t="shared" si="2"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="17" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B51" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C50" s="5">
+      <c r="C51" s="5">
         <v>4000</v>
       </c>
-      <c r="D50" s="4">
-        <f t="shared" ref="D50:D55" si="3">D49+C50</f>
+      <c r="D51" s="4">
+        <f t="shared" ref="D51:D56" si="3">D50+C51</f>
         <v>12890</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B51" s="4" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C51" s="5">
+      <c r="C52" s="5">
         <v>5000</v>
       </c>
-      <c r="D51" s="4">
+      <c r="D52" s="4">
         <f t="shared" si="3"/>
         <v>17890</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B52" s="4" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B53" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C52" s="5">
+      <c r="C53" s="5">
         <v>-10000</v>
       </c>
-      <c r="D52" s="4">
+      <c r="D53" s="4">
         <f t="shared" si="3"/>
         <v>7890</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="17">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="17">
         <v>44969</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B54" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C53" s="5">
+      <c r="C54" s="5">
         <v>900</v>
       </c>
-      <c r="D53" s="4">
+      <c r="D54" s="4">
         <f t="shared" si="3"/>
         <v>8790</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B54" s="4" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B55" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C54" s="5">
+      <c r="C55" s="5">
         <v>4000</v>
       </c>
-      <c r="D54" s="4">
+      <c r="D55" s="4">
         <f t="shared" si="3"/>
         <v>12790</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="4" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B56" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C55" s="5">
+      <c r="C56" s="5">
         <v>-10000</v>
       </c>
-      <c r="D55" s="4">
+      <c r="D56" s="4">
         <f t="shared" si="3"/>
         <v>2790</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C56" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D56" s="4">
-        <f t="shared" ref="D56:D63" si="4">D55+C56</f>
-        <v>4790</v>
-      </c>
-    </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C57" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D57" s="4">
+        <f t="shared" ref="D57:D64" si="4">D56+C57</f>
+        <v>4790</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B58" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C57" s="5">
+      <c r="C58" s="5">
         <v>700</v>
       </c>
-      <c r="D57" s="4">
+      <c r="D58" s="4">
         <f t="shared" si="4"/>
         <v>5490</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B58" s="4" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B59" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C58" s="5">
+      <c r="C59" s="5">
         <v>4000</v>
       </c>
-      <c r="D58" s="4">
+      <c r="D59" s="4">
         <f t="shared" si="4"/>
         <v>9490</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="17" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B60" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C59" s="5">
+      <c r="C60" s="5">
         <v>600</v>
       </c>
-      <c r="D59" s="4">
+      <c r="D60" s="4">
         <f t="shared" si="4"/>
         <v>10090</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B60" s="4" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B61" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C60" s="5">
+      <c r="C61" s="5">
         <v>-10000</v>
       </c>
-      <c r="D60" s="4">
+      <c r="D61" s="4">
         <f t="shared" si="4"/>
         <v>90</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="17" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B62" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C61" s="5">
+      <c r="C62" s="5">
         <f>700+5000+300+600+400+1000+800</f>
         <v>8800</v>
       </c>
-      <c r="D61" s="4">
+      <c r="D62" s="4">
         <f t="shared" si="4"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B62" s="4" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B63" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C62" s="5">
+      <c r="C63" s="5">
         <v>6000</v>
       </c>
-      <c r="D62" s="4">
+      <c r="D63" s="4">
         <f t="shared" si="4"/>
         <v>14890</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B63" s="4" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B64" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C63" s="5">
+      <c r="C64" s="5">
         <v>-10000</v>
       </c>
-      <c r="D63" s="4">
+      <c r="D64" s="4">
         <f t="shared" si="4"/>
         <v>4890</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="17" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B65" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C64" s="5">
+      <c r="C65" s="5">
         <v>500</v>
       </c>
-      <c r="D64" s="4">
-        <f t="shared" ref="D64:D69" si="5">D63+C64</f>
+      <c r="D65" s="4">
+        <f t="shared" ref="D65:D70" si="5">D64+C65</f>
         <v>5390</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B65" s="4" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C65" s="5">
+      <c r="C66" s="5">
         <v>700</v>
       </c>
-      <c r="D65" s="4">
+      <c r="D66" s="4">
         <f t="shared" si="5"/>
         <v>6090</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B66" s="4" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B67" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C66" s="5">
+      <c r="C67" s="5">
         <v>1500</v>
       </c>
-      <c r="D66" s="4">
+      <c r="D67" s="4">
         <f t="shared" si="5"/>
         <v>7590</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B67" s="4" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B68" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C67" s="5">
+      <c r="C68" s="5">
         <v>5000</v>
       </c>
-      <c r="D67" s="4">
+      <c r="D68" s="4">
         <f t="shared" si="5"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B68" s="4" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B69" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C68" s="5">
+      <c r="C69" s="5">
         <v>-10000</v>
       </c>
-      <c r="D68" s="4">
+      <c r="D69" s="4">
         <f t="shared" si="5"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="17" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B70" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C69" s="5">
+      <c r="C70" s="5">
         <v>2000</v>
       </c>
-      <c r="D69" s="4">
+      <c r="D70" s="4">
         <f t="shared" si="5"/>
         <v>4590</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B70" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C70" s="5">
-        <v>700</v>
-      </c>
-      <c r="D70" s="4">
-        <f t="shared" ref="D70:D75" si="6">D69+C70</f>
-        <v>5290</v>
-      </c>
-    </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="17" t="s">
-        <v>82</v>
-      </c>
       <c r="B71" s="4" t="s">
         <v>77</v>
       </c>
@@ -2115,401 +2114,404 @@
         <v>700</v>
       </c>
       <c r="D71" s="4">
+        <f t="shared" ref="D71:D76" si="6">D70+C71</f>
+        <v>5290</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C72" s="5">
+        <v>700</v>
+      </c>
+      <c r="D72" s="4">
         <f t="shared" si="6"/>
         <v>5990</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="17" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B73" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C72" s="5">
+      <c r="C73" s="5">
         <v>700</v>
       </c>
-      <c r="D72" s="4">
+      <c r="D73" s="4">
         <f t="shared" si="6"/>
         <v>6690</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="17" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B74" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C73" s="5">
+      <c r="C74" s="5">
         <v>4000</v>
       </c>
-      <c r="D73" s="4">
+      <c r="D74" s="4">
         <f t="shared" si="6"/>
         <v>10690</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B74" s="4" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B75" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C74" s="5">
+      <c r="C75" s="5">
         <v>-10000</v>
       </c>
-      <c r="D74" s="4">
+      <c r="D75" s="4">
         <f t="shared" si="6"/>
         <v>690</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="17" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="B76" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C75" s="5">
+      <c r="C76" s="5">
         <v>1000</v>
       </c>
-      <c r="D75" s="4">
+      <c r="D76" s="4">
         <f t="shared" si="6"/>
         <v>1690</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="17" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B77" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C76" s="5">
+      <c r="C77" s="5">
         <v>7000</v>
       </c>
-      <c r="D76" s="4">
-        <f t="shared" ref="D76:D81" si="7">D75+C76</f>
+      <c r="D77" s="4">
+        <f t="shared" ref="D77:D82" si="7">D76+C77</f>
         <v>8690</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B77" s="4" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B78" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C77" s="5">
+      <c r="C78" s="5">
         <v>10000</v>
       </c>
-      <c r="D77" s="4">
+      <c r="D78" s="4">
         <f t="shared" si="7"/>
         <v>18690</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B78" s="4" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B79" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C78" s="5">
+      <c r="C79" s="5">
         <v>-10000</v>
       </c>
-      <c r="D78" s="4">
+      <c r="D79" s="4">
         <f t="shared" si="7"/>
         <v>8690</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B79" s="4" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B80" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C79" s="5">
+      <c r="C80" s="5">
         <v>1700</v>
       </c>
-      <c r="D79" s="4">
+      <c r="D80" s="4">
         <f t="shared" si="7"/>
         <v>10390</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B80" s="4" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B81" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C80" s="5">
+      <c r="C81" s="5">
         <v>-10000</v>
       </c>
-      <c r="D80" s="4">
+      <c r="D81" s="4">
         <f t="shared" si="7"/>
         <v>390</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B81" s="4" t="s">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B82" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C81" s="5">
+      <c r="C82" s="5">
         <v>6000</v>
       </c>
-      <c r="D81" s="4">
+      <c r="D82" s="4">
         <f t="shared" si="7"/>
         <v>6390</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C82" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D82" s="4">
-        <f t="shared" ref="D82:D87" si="8">D81+C82</f>
-        <v>8390</v>
-      </c>
-    </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C83" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D83" s="4">
+        <f t="shared" ref="D83:D88" si="8">D82+C83</f>
+        <v>8390</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="B84" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C83" s="5">
+      <c r="C84" s="5">
         <v>5000</v>
       </c>
-      <c r="D83" s="4">
+      <c r="D84" s="4">
         <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B84" s="4" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B85" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C84" s="5">
+      <c r="C85" s="5">
         <v>-10000</v>
       </c>
-      <c r="D84" s="4">
+      <c r="D85" s="4">
         <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="17" t="s">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="B85" s="4" t="s">
+      <c r="B86" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C85" s="5">
+      <c r="C86" s="5">
         <v>1000</v>
       </c>
-      <c r="D85" s="4">
+      <c r="D86" s="4">
         <f t="shared" si="8"/>
         <v>4390</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B86" s="4" t="s">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B87" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C86" s="5">
+      <c r="C87" s="5">
         <v>9000</v>
       </c>
-      <c r="D86" s="4">
+      <c r="D87" s="4">
         <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B87" s="4" t="s">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B88" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C87" s="5">
+      <c r="C88" s="5">
         <v>-10000</v>
       </c>
-      <c r="D87" s="4">
+      <c r="D88" s="4">
         <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B88" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C88" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D88" s="4">
-        <f t="shared" ref="D88:D93" si="9">D87+C88</f>
-        <v>5390</v>
-      </c>
-    </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B89" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C89" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D89" s="4">
+        <f t="shared" ref="D89:D94" si="9">D88+C89</f>
+        <v>5390</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B90" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C89" s="5">
+      <c r="C90" s="5">
         <v>6000</v>
       </c>
-      <c r="D89" s="4">
+      <c r="D90" s="4">
         <f t="shared" si="9"/>
         <v>11390</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B90" s="4" t="s">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B91" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C90" s="5">
+      <c r="C91" s="5">
         <v>-10000</v>
       </c>
-      <c r="D90" s="4">
+      <c r="D91" s="4">
         <f t="shared" si="9"/>
         <v>1390</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B91" s="4" t="s">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B92" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C91" s="5">
+      <c r="C92" s="5">
         <v>400</v>
       </c>
-      <c r="D91" s="4">
+      <c r="D92" s="4">
         <f t="shared" si="9"/>
         <v>1790</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="17" t="s">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="B92" s="4" t="s">
+      <c r="B93" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C92" s="5">
+      <c r="C93" s="5">
         <v>2000</v>
       </c>
-      <c r="D92" s="4">
+      <c r="D93" s="4">
         <f t="shared" si="9"/>
         <v>3790</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="17" t="s">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="B93" s="4" t="s">
+      <c r="B94" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C93" s="5">
+      <c r="C94" s="5">
         <v>6000</v>
       </c>
-      <c r="D93" s="4">
+      <c r="D94" s="4">
         <f t="shared" si="9"/>
         <v>9790</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="17" t="s">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="B94" s="4" t="s">
+      <c r="B95" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C94" s="5">
+      <c r="C95" s="5">
         <v>1000</v>
       </c>
-      <c r="D94" s="4">
-        <f t="shared" ref="D94:D99" si="10">D93+C94</f>
+      <c r="D95" s="4">
+        <f t="shared" ref="D95:D100" si="10">D94+C95</f>
         <v>10790</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B95" s="4" t="s">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B96" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C95" s="5">
+      <c r="C96" s="5">
         <v>-10000</v>
       </c>
-      <c r="D95" s="4">
+      <c r="D96" s="4">
         <f t="shared" si="10"/>
         <v>790</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="17" t="s">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="B96" s="4" t="s">
+      <c r="B97" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C96" s="5">
+      <c r="C97" s="5">
         <v>800</v>
       </c>
-      <c r="D96" s="4">
+      <c r="D97" s="4">
         <f t="shared" si="10"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="17" t="s">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="B97" s="4" t="s">
+      <c r="B98" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C97" s="5">
+      <c r="C98" s="5">
         <v>5000</v>
       </c>
-      <c r="D97" s="4">
+      <c r="D98" s="4">
         <f t="shared" si="10"/>
         <v>6590</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="17" t="s">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="B98" s="4" t="s">
+      <c r="B99" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C98" s="5">
+      <c r="C99" s="5">
         <v>6000</v>
       </c>
-      <c r="D98" s="4">
+      <c r="D99" s="4">
         <f t="shared" si="10"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B99" s="4" t="s">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B100" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C99" s="5">
+      <c r="C100" s="5">
         <v>-10000</v>
       </c>
-      <c r="D99" s="4">
+      <c r="D100" s="4">
         <f t="shared" si="10"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="17" t="s">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="B100" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C100" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D100" s="4">
-        <f t="shared" ref="D100:D106" si="11">D99+C100</f>
-        <v>4590</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B101" s="4" t="s">
         <v>65</v>
       </c>
@@ -2517,887 +2519,926 @@
         <v>2000</v>
       </c>
       <c r="D101" s="4">
+        <f t="shared" ref="D101:D107" si="11">D100+C101</f>
+        <v>4590</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B102" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C102" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D102" s="4">
         <f t="shared" si="11"/>
         <v>6590</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B102" s="4" t="s">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B103" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C102" s="5">
+      <c r="C103" s="5">
         <v>7000</v>
       </c>
-      <c r="D102" s="4">
+      <c r="D103" s="4">
         <f t="shared" si="11"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B103" s="4" t="s">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B104" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C103" s="5">
+      <c r="C104" s="5">
         <v>-10000</v>
       </c>
-      <c r="D103" s="4">
+      <c r="D104" s="4">
         <f t="shared" si="11"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="17" t="s">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="B104" s="4" t="s">
+      <c r="B105" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C104" s="5">
+      <c r="C105" s="5">
         <v>2000</v>
       </c>
-      <c r="D104" s="4">
+      <c r="D105" s="4">
         <f t="shared" si="11"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="17" t="s">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="B105" s="4" t="s">
+      <c r="B106" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C105" s="5">
+      <c r="C106" s="5">
         <v>6000</v>
       </c>
-      <c r="D105" s="4">
+      <c r="D106" s="4">
         <f t="shared" si="11"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B106" s="4" t="s">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B107" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C106" s="5">
+      <c r="C107" s="5">
         <v>-10000</v>
       </c>
-      <c r="D106" s="4">
+      <c r="D107" s="4">
         <f t="shared" si="11"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="B107" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C107" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D107" s="4">
-        <f t="shared" ref="D107:D112" si="12">D106+C107</f>
-        <v>3590</v>
-      </c>
-    </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C108" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D108" s="4">
+        <f t="shared" ref="D108:D113" si="12">D107+C108</f>
+        <v>3590</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="B108" s="4" t="s">
+      <c r="B109" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C108" s="5">
+      <c r="C109" s="5">
         <v>7000</v>
       </c>
-      <c r="D108" s="4">
+      <c r="D109" s="4">
         <f t="shared" si="12"/>
         <v>10590</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B109" s="4" t="s">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B110" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C109" s="5">
+      <c r="C110" s="5">
         <v>-10000</v>
       </c>
-      <c r="D109" s="4">
+      <c r="D110" s="4">
         <f t="shared" si="12"/>
         <v>590</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B110" s="4" t="s">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B111" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C110" s="5">
+      <c r="C111" s="5">
         <v>12000</v>
       </c>
-      <c r="D110" s="4">
+      <c r="D111" s="4">
         <f t="shared" si="12"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B111" s="4" t="s">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B112" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C111" s="5">
+      <c r="C112" s="5">
         <v>-10000</v>
       </c>
-      <c r="D111" s="4">
+      <c r="D112" s="4">
         <f t="shared" si="12"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B112" s="4" t="s">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B113" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C112" s="5">
+      <c r="C113" s="5">
         <v>2000</v>
       </c>
-      <c r="D112" s="4">
+      <c r="D113" s="4">
         <f t="shared" si="12"/>
         <v>4590</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="B113" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C113" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D113" s="4">
-        <f t="shared" ref="D113:D118" si="13">D112+C113</f>
-        <v>6590</v>
-      </c>
-    </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="B114" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C114" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D114" s="4">
+        <f t="shared" ref="D114:D119" si="13">D113+C114</f>
+        <v>6590</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="B114" s="4" t="s">
+      <c r="B115" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C114" s="5">
+      <c r="C115" s="5">
         <v>7000</v>
       </c>
-      <c r="D114" s="4">
+      <c r="D115" s="4">
         <f t="shared" si="13"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B115" s="4" t="s">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B116" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C115" s="5">
+      <c r="C116" s="5">
         <v>-10000</v>
       </c>
-      <c r="D115" s="4">
+      <c r="D116" s="4">
         <f t="shared" si="13"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="17" t="s">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="B116" s="4" t="s">
+      <c r="B117" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C116" s="5">
+      <c r="C117" s="5">
         <v>2000</v>
       </c>
-      <c r="D116" s="4">
+      <c r="D117" s="4">
         <f t="shared" si="13"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="17" t="s">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="B117" s="4" t="s">
+      <c r="B118" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C117" s="5">
+      <c r="C118" s="5">
         <v>8000</v>
       </c>
-      <c r="D117" s="4">
+      <c r="D118" s="4">
         <f t="shared" si="13"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B118" s="4" t="s">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B119" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C118" s="5">
+      <c r="C119" s="5">
         <v>-10000</v>
       </c>
-      <c r="D118" s="4">
+      <c r="D119" s="4">
         <f t="shared" si="13"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="17" t="s">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="B119" s="4" t="s">
+      <c r="B120" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C119" s="5">
+      <c r="C120" s="5">
         <v>2000</v>
       </c>
-      <c r="D119" s="4">
-        <f t="shared" ref="D119:D124" si="14">D118+C119</f>
+      <c r="D120" s="4">
+        <f t="shared" ref="D120:D125" si="14">D119+C120</f>
         <v>5590</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B120" s="4" t="s">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B121" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C120" s="5">
+      <c r="C121" s="5">
         <v>5000</v>
       </c>
-      <c r="D120" s="4">
+      <c r="D121" s="4">
         <f t="shared" si="14"/>
         <v>10590</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B121" s="4" t="s">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B122" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C121" s="5">
+      <c r="C122" s="5">
         <v>-10000</v>
       </c>
-      <c r="D121" s="4">
+      <c r="D122" s="4">
         <f t="shared" si="14"/>
         <v>590</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B122" s="4" t="s">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B123" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C122" s="5">
+      <c r="C123" s="5">
         <v>2000</v>
       </c>
-      <c r="D122" s="4">
+      <c r="D123" s="4">
         <f t="shared" si="14"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B123" s="4" t="s">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B124" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C123" s="5">
+      <c r="C124" s="5">
         <v>9000</v>
       </c>
-      <c r="D123" s="4">
+      <c r="D124" s="4">
         <f t="shared" si="14"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B124" s="4" t="s">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B125" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C124" s="5">
+      <c r="C125" s="5">
         <v>-10000</v>
       </c>
-      <c r="D124" s="4">
+      <c r="D125" s="4">
         <f t="shared" si="14"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="B125" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C125" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D125" s="4">
-        <f t="shared" ref="D125:D130" si="15">D124+C125</f>
-        <v>3590</v>
-      </c>
-    </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="B126" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C126" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D126" s="4">
+        <f t="shared" ref="D126:D131" si="15">D125+C126</f>
+        <v>3590</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="B126" s="4" t="s">
+      <c r="B127" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C126" s="5">
+      <c r="C127" s="5">
         <v>8000</v>
       </c>
-      <c r="D126" s="4">
+      <c r="D127" s="4">
         <f t="shared" si="15"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B127" s="4" t="s">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B128" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C127" s="5">
+      <c r="C128" s="5">
         <v>-10000</v>
       </c>
-      <c r="D127" s="4">
+      <c r="D128" s="4">
         <f t="shared" si="15"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="17" t="s">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="B128" s="4" t="s">
+      <c r="B129" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C128" s="5">
+      <c r="C129" s="5">
         <v>2000</v>
       </c>
-      <c r="D128" s="4">
+      <c r="D129" s="4">
         <f t="shared" si="15"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="17" t="s">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="B129" s="4" t="s">
+      <c r="B130" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="C129" s="5">
+      <c r="C130" s="5">
         <v>12000</v>
       </c>
-      <c r="D129" s="4">
+      <c r="D130" s="4">
         <f t="shared" si="15"/>
         <v>15590</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B130" s="4" t="s">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B131" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C130" s="5">
+      <c r="C131" s="5">
         <v>-10000</v>
       </c>
-      <c r="D130" s="4">
+      <c r="D131" s="4">
         <f t="shared" si="15"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="17" t="s">
-        <v>168</v>
-      </c>
-      <c r="B131" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="C131" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D131" s="4">
-        <f t="shared" ref="D131:D136" si="16">D130+C131</f>
-        <v>7590</v>
-      </c>
-    </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="B132" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C132" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D132" s="4">
+        <f t="shared" ref="D132:D137" si="16">D131+C132</f>
+        <v>7590</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="B132" s="4" t="s">
+      <c r="B133" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="C132" s="5">
+      <c r="C133" s="5">
         <v>10000</v>
       </c>
-      <c r="D132" s="4">
+      <c r="D133" s="4">
         <f t="shared" si="16"/>
         <v>17590</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B133" s="4" t="s">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B134" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C133" s="5">
+      <c r="C134" s="5">
         <v>-10000</v>
       </c>
-      <c r="D133" s="4">
+      <c r="D134" s="4">
         <f t="shared" si="16"/>
         <v>7590</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B134" s="4" t="s">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B135" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="C134" s="5">
+      <c r="C135" s="5">
         <v>2000</v>
       </c>
-      <c r="D134" s="4">
+      <c r="D135" s="4">
         <f t="shared" si="16"/>
         <v>9590</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="17" t="s">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="B135" s="4" t="s">
+      <c r="B136" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="C135" s="5">
+      <c r="C136" s="5">
         <v>-1200</v>
       </c>
-      <c r="D135" s="4">
+      <c r="D136" s="4">
         <f t="shared" si="16"/>
         <v>8390</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B136" s="4" t="s">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B137" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="C136" s="5">
+      <c r="C137" s="5">
         <v>500</v>
       </c>
-      <c r="D136" s="4">
+      <c r="D137" s="4">
         <f t="shared" si="16"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="B137" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C137" s="5">
-        <v>750</v>
-      </c>
-      <c r="D137" s="4">
-        <f t="shared" ref="D137:D142" si="17">D136+C137</f>
-        <v>9640</v>
-      </c>
-    </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="B138" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C138" s="5">
+        <v>750</v>
+      </c>
+      <c r="D138" s="4">
+        <f t="shared" ref="D138:D143" si="17">D137+C138</f>
+        <v>9640</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="B138" s="4" t="s">
+      <c r="B139" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C138" s="5">
+      <c r="C139" s="5">
         <v>2000</v>
       </c>
-      <c r="D138" s="4">
+      <c r="D139" s="4">
         <f t="shared" si="17"/>
         <v>11640</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B139" s="4" t="s">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B140" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C139" s="5">
+      <c r="C140" s="5">
         <v>2000</v>
       </c>
-      <c r="D139" s="4">
+      <c r="D140" s="4">
         <f t="shared" si="17"/>
         <v>13640</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B140" s="4" t="s">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B141" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C140" s="5">
+      <c r="C141" s="5">
         <v>-10000</v>
       </c>
-      <c r="D140" s="4">
+      <c r="D141" s="4">
         <f t="shared" si="17"/>
         <v>3640</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B141" s="4" t="s">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B142" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="C141" s="5">
+      <c r="C142" s="5">
         <v>350</v>
       </c>
-      <c r="D141" s="4">
+      <c r="D142" s="4">
         <f t="shared" si="17"/>
         <v>3990</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="17" t="s">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="B142" s="4" t="s">
+      <c r="B143" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="C142" s="5">
+      <c r="C143" s="5">
         <v>300</v>
       </c>
-      <c r="D142" s="4">
+      <c r="D143" s="4">
         <f t="shared" si="17"/>
         <v>4290</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="17" t="s">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" s="17" t="s">
         <v>181</v>
       </c>
-      <c r="B143" s="4" t="s">
+      <c r="B144" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="C143" s="5">
+      <c r="C144" s="5">
         <v>3800</v>
       </c>
-      <c r="D143" s="4">
-        <f t="shared" ref="D143:D149" si="18">D142+C143</f>
+      <c r="D144" s="4">
+        <f t="shared" ref="D144:D150" si="18">D143+C144</f>
         <v>8090</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B144" s="4" t="s">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B145" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C144" s="5">
+      <c r="C145" s="5">
         <v>500</v>
       </c>
-      <c r="D144" s="4">
+      <c r="D145" s="4">
         <f t="shared" si="18"/>
         <v>8590</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="17" t="s">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="B145" s="4" t="s">
+      <c r="B146" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="C145" s="5">
+      <c r="C146" s="5">
         <v>1300</v>
       </c>
-      <c r="D145" s="4">
+      <c r="D146" s="4">
         <f t="shared" si="18"/>
         <v>9890</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="17" t="s">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" s="17" t="s">
         <v>185</v>
       </c>
-      <c r="B146" s="4" t="s">
+      <c r="B147" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C146" s="5">
+      <c r="C147" s="5">
         <v>9000</v>
       </c>
-      <c r="D146" s="4">
+      <c r="D147" s="4">
         <f t="shared" si="18"/>
         <v>18890</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B147" s="4" t="s">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B148" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C147" s="5">
+      <c r="C148" s="5">
         <v>-10000</v>
       </c>
-      <c r="D147" s="4">
+      <c r="D148" s="4">
         <f t="shared" si="18"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="17" t="s">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="B148" s="4" t="s">
+      <c r="B149" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C148" s="5">
+      <c r="C149" s="5">
         <v>2000</v>
       </c>
-      <c r="D148" s="4">
+      <c r="D149" s="4">
         <f t="shared" si="18"/>
         <v>10890</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B149" s="4" t="s">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B150" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C149" s="5">
+      <c r="C150" s="5">
         <v>-10000</v>
       </c>
-      <c r="D149" s="4">
+      <c r="D150" s="4">
         <f t="shared" si="18"/>
         <v>890</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="17" t="s">
-        <v>187</v>
-      </c>
-      <c r="B150" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="C150" s="5">
-        <v>500</v>
-      </c>
-      <c r="D150" s="4">
-        <f t="shared" ref="D150:D155" si="19">D149+C150</f>
-        <v>1390</v>
-      </c>
-    </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="B151" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="C151" s="5">
+        <v>500</v>
+      </c>
+      <c r="D151" s="4">
+        <f t="shared" ref="D151:D156" si="19">D150+C151</f>
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" s="17" t="s">
         <v>189</v>
       </c>
-      <c r="B151" s="4" t="s">
+      <c r="B152" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C151" s="5">
+      <c r="C152" s="5">
         <v>10000</v>
       </c>
-      <c r="D151" s="4">
+      <c r="D152" s="4">
         <f t="shared" si="19"/>
         <v>11390</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B152" s="4" t="s">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B153" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C152" s="5">
+      <c r="C153" s="5">
         <v>-10000</v>
       </c>
-      <c r="D152" s="4">
+      <c r="D153" s="4">
         <f t="shared" si="19"/>
         <v>1390</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" s="17" t="s">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="B153" s="4" t="s">
+      <c r="B154" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C153" s="5">
+      <c r="C154" s="5">
         <v>3000</v>
       </c>
-      <c r="D153" s="4">
+      <c r="D154" s="4">
         <f t="shared" si="19"/>
         <v>4390</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="17" t="s">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="B154" s="4" t="s">
+      <c r="B155" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C154" s="5">
+      <c r="C155" s="5">
         <v>2000</v>
       </c>
-      <c r="D154" s="4">
+      <c r="D155" s="4">
         <f t="shared" si="19"/>
         <v>6390</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B155" s="4" t="s">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B156" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C155" s="5">
+      <c r="C156" s="5">
         <v>2000</v>
       </c>
-      <c r="D155" s="4">
+      <c r="D156" s="4">
         <f t="shared" si="19"/>
         <v>8390</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="17" t="s">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" s="17" t="s">
         <v>193</v>
       </c>
-      <c r="B156" s="4" t="s">
+      <c r="B157" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="C156" s="5">
+      <c r="C157" s="5">
         <v>11000</v>
       </c>
-      <c r="D156" s="4">
-        <f t="shared" ref="D156:D161" si="20">D155+C156</f>
+      <c r="D157" s="4">
+        <f t="shared" ref="D157:D162" si="20">D156+C157</f>
         <v>19390</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B157" s="4" t="s">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B158" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C157" s="5">
+      <c r="C158" s="5">
         <v>-10000</v>
       </c>
-      <c r="D157" s="4">
+      <c r="D158" s="4">
         <f t="shared" si="20"/>
         <v>9390</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="17" t="s">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" s="17" t="s">
         <v>195</v>
       </c>
-      <c r="B158" s="4" t="s">
+      <c r="B159" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="C158" s="5">
+      <c r="C159" s="5">
         <v>3000</v>
       </c>
-      <c r="D158" s="4">
+      <c r="D159" s="4">
         <f t="shared" si="20"/>
         <v>12390</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B159" s="4" t="s">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B160" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C159" s="5">
+      <c r="C160" s="5">
         <v>-10000</v>
       </c>
-      <c r="D159" s="4">
+      <c r="D160" s="4">
         <f t="shared" si="20"/>
         <v>2390</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B160" s="4" t="s">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B161" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C160" s="5">
+      <c r="C161" s="5">
         <v>500</v>
       </c>
-      <c r="D160" s="4">
+      <c r="D161" s="4">
         <f t="shared" si="20"/>
         <v>2890</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" s="17" t="s">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="B161" s="4" t="s">
+      <c r="B162" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C161" s="5">
+      <c r="C162" s="5">
         <v>5600</v>
       </c>
-      <c r="D161" s="4">
+      <c r="D162" s="4">
         <f t="shared" si="20"/>
         <v>8490</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B162" s="4" t="s">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B163" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="C162" s="5">
+      <c r="C163" s="5">
         <v>4700</v>
-      </c>
-      <c r="D162" s="4">
-        <f>D161+C162</f>
-        <v>13190</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163" s="17" t="s">
-        <v>200</v>
-      </c>
-      <c r="B163" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C163" s="5">
-        <v>1500</v>
       </c>
       <c r="D163" s="4">
         <f>D162+C163</f>
-        <v>14690</v>
+        <v>13190</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" s="17" t="s">
+        <v>200</v>
+      </c>
       <c r="B164" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C164" s="5">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="D164" s="4">
         <f>D163+C164</f>
-        <v>15190</v>
+        <v>14690</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" s="17" t="s">
-        <v>201</v>
-      </c>
       <c r="B165" s="4" t="s">
-        <v>202</v>
+        <v>76</v>
       </c>
       <c r="C165" s="5">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="D165" s="4">
         <f>D164+C165</f>
-        <v>16190</v>
+        <v>15190</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="17" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B166" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C166" s="5">
         <v>1000</v>
       </c>
       <c r="D166" s="4">
         <f>D165+C166</f>
+        <v>16190</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="B167" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C167" s="5">
+        <v>1000</v>
+      </c>
+      <c r="D167" s="4">
+        <f>D166+C167</f>
         <v>17190</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="B168" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C168" s="5">
+        <v>3000</v>
+      </c>
+      <c r="D168" s="4">
+        <f>D167+C168</f>
+        <v>20190</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B169" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="C169" s="5">
+        <v>-20000</v>
+      </c>
+      <c r="D169" s="4">
+        <f>D168+C169</f>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -3552,7 +3593,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
     </sheetView>

</xml_diff>

<commit_message>
duy lay tien loi ngay 21 co diem
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="CÔ DIỄM" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="211">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -643,6 +643,15 @@
   </si>
   <si>
     <t>15/08/2024</t>
+  </si>
+  <si>
+    <t>21/08/2024</t>
+  </si>
+  <si>
+    <t>Duy lấy tiên lời 10tr</t>
+  </si>
+  <si>
+    <t>Duy cho cô diễm vay 10tr</t>
   </si>
 </sst>
 </file>
@@ -1121,11 +1130,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K171"/>
+  <dimension ref="A1:K174"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A141" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D172" sqref="D172"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1201,8 +1210,8 @@
         <v>20</v>
       </c>
       <c r="J3" s="4">
-        <f>SUM(I3:I60)</f>
-        <v>470</v>
+        <f>SUM(I3:I61)</f>
+        <v>480</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1247,7 +1256,7 @@
         <v>-10000</v>
       </c>
       <c r="D7" s="4">
-        <f t="shared" ref="D7:D21" si="0">D6+C7</f>
+        <f t="shared" ref="D7:D22" si="0">D6+C7</f>
         <v>8490</v>
       </c>
       <c r="H7" s="17" t="s">
@@ -1339,24 +1348,24 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H16" s="17" t="s">
-        <v>70</v>
+        <v>208</v>
       </c>
       <c r="I16" s="5">
         <v>10</v>
       </c>
+      <c r="K16" s="14"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H17" s="17" t="s">
-        <v>107</v>
+        <v>70</v>
       </c>
       <c r="I17" s="5">
         <v>10</v>
       </c>
-      <c r="K17" s="14"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H18" s="17" t="s">
-        <v>186</v>
+        <v>107</v>
       </c>
       <c r="I18" s="5">
         <v>10</v>
@@ -1364,18 +1373,8 @@
       <c r="K18" s="14"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="5">
-        <v>-10000</v>
-      </c>
-      <c r="D19" s="4">
-        <f>D8+C19</f>
-        <v>490</v>
-      </c>
       <c r="H19" s="17" t="s">
-        <v>10</v>
+        <v>186</v>
       </c>
       <c r="I19" s="5">
         <v>10</v>
@@ -1383,52 +1382,62 @@
       <c r="K19" s="14"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
+      <c r="B20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D20" s="4">
+        <f>D8+C20</f>
+        <v>490</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" s="5">
+        <v>10</v>
+      </c>
+      <c r="K20" s="14"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B21" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C21" s="5">
         <v>2000</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D21" s="4">
         <f t="shared" si="0"/>
         <v>2490</v>
       </c>
-      <c r="H20" s="17" t="s">
+      <c r="H21" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="5">
+      <c r="I21" s="5">
         <v>10</v>
       </c>
-      <c r="K20" s="14"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
+      <c r="K21" s="14"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B22" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C22" s="5">
         <v>3000</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D22" s="4">
         <f t="shared" si="0"/>
         <v>5490</v>
       </c>
-      <c r="H21" s="17" t="s">
+      <c r="H22" s="17" t="s">
         <v>24</v>
-      </c>
-      <c r="I21" s="5">
-        <v>10</v>
-      </c>
-      <c r="K21" s="14"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H22" s="17" t="s">
-        <v>59</v>
       </c>
       <c r="I22" s="5">
         <v>10</v>
@@ -1437,7 +1446,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H23" s="17" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="I23" s="5">
         <v>10</v>
@@ -1446,7 +1455,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H24" s="17" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="I24" s="5">
         <v>10</v>
@@ -1455,7 +1464,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H25" s="17" t="s">
-        <v>121</v>
+        <v>91</v>
       </c>
       <c r="I25" s="5">
         <v>10</v>
@@ -1464,7 +1473,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H26" s="17" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="I26" s="5">
         <v>10</v>
@@ -1473,7 +1482,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H27" s="17" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="I27" s="5">
         <v>10</v>
@@ -1482,7 +1491,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H28" s="17" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="I28" s="5">
         <v>10</v>
@@ -1491,7 +1500,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H29" s="17" t="s">
-        <v>189</v>
+        <v>151</v>
       </c>
       <c r="I29" s="5">
         <v>10</v>
@@ -1499,38 +1508,38 @@
       <c r="K29" s="14"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C30" s="5">
-        <v>3000</v>
-      </c>
-      <c r="D30" s="4">
-        <f>D21+C30</f>
-        <v>8490</v>
-      </c>
       <c r="H30" s="17" t="s">
-        <v>12</v>
+        <v>189</v>
       </c>
       <c r="I30" s="5">
         <v>10</v>
       </c>
+      <c r="K30" s="14"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" s="5">
+        <v>3000</v>
+      </c>
+      <c r="D31" s="4">
+        <f>D22+C31</f>
+        <v>8490</v>
+      </c>
       <c r="H31" s="17" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="I31" s="5">
         <v>10</v>
       </c>
-      <c r="K31" s="14"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H32" s="17" t="s">
-        <v>146</v>
+        <v>43</v>
       </c>
       <c r="I32" s="5">
         <v>10</v>
@@ -1539,7 +1548,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H33" s="17" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="I33" s="5">
         <v>10</v>
@@ -1548,7 +1557,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H34" s="17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I34" s="5">
         <v>10</v>
@@ -1556,56 +1565,46 @@
       <c r="K34" s="14"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B35" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C35" s="5">
-        <v>4400</v>
-      </c>
-      <c r="D35" s="4">
-        <f>D30+C35</f>
-        <v>12890</v>
-      </c>
       <c r="H35" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I35" s="5">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K35" s="14"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C36" s="5">
-        <v>-10000</v>
+        <v>4400</v>
       </c>
       <c r="D36" s="4">
-        <f>D35+C36</f>
-        <v>2890</v>
+        <f>D31+C36</f>
+        <v>12890</v>
       </c>
       <c r="H36" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I36" s="5">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="K36" s="14"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C37" s="5">
-        <v>1600</v>
+        <v>-10000</v>
       </c>
       <c r="D37" s="4">
-        <f t="shared" ref="D37:D44" si="1">D36+C37</f>
-        <v>4490</v>
+        <f>D36+C37</f>
+        <v>2890</v>
       </c>
       <c r="H37" s="17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I37" s="5">
         <v>10</v>
@@ -1614,517 +1613,521 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C38" s="5">
+        <v>1600</v>
+      </c>
+      <c r="D38" s="4">
+        <f t="shared" ref="D38:D45" si="1">D37+C38</f>
+        <v>4490</v>
+      </c>
+      <c r="H38" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="I38" s="5">
+        <v>10</v>
+      </c>
+      <c r="K38" s="14"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B39" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C38" s="5">
+      <c r="C39" s="5">
         <v>3000</v>
       </c>
-      <c r="D38" s="4">
+      <c r="D39" s="4">
         <f t="shared" si="1"/>
         <v>7490</v>
       </c>
-      <c r="H38" s="17" t="s">
+      <c r="H39" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="I38" s="5">
+      <c r="I39" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="17" t="s">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B40" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C39" s="5">
+      <c r="C40" s="5">
         <v>2000</v>
       </c>
-      <c r="D39" s="4">
+      <c r="D40" s="4">
         <f t="shared" si="1"/>
         <v>9490</v>
       </c>
-      <c r="H39" s="17" t="s">
+      <c r="H40" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="I39" s="5">
+      <c r="I40" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="17" t="s">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B41" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="5">
+      <c r="C41" s="5">
         <v>3000</v>
       </c>
-      <c r="D40" s="4">
+      <c r="D41" s="4">
         <f t="shared" si="1"/>
         <v>12490</v>
       </c>
-      <c r="H40" s="17" t="s">
+      <c r="H41" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="I40" s="5">
+      <c r="I41" s="5">
         <v>10</v>
       </c>
-      <c r="K40" s="14"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B41" s="4" t="s">
+      <c r="K41" s="14"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B42" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C41" s="5">
+      <c r="C42" s="5">
         <v>-10000</v>
       </c>
-      <c r="D41" s="4">
+      <c r="D42" s="4">
         <f t="shared" si="1"/>
         <v>2490</v>
       </c>
-      <c r="H41" s="17" t="s">
+      <c r="H42" s="17" t="s">
         <v>159</v>
       </c>
-      <c r="I41" s="5">
+      <c r="I42" s="5">
         <v>10</v>
       </c>
-      <c r="K41" s="14"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="17" t="s">
+      <c r="K42" s="14"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B43" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C43" s="5">
         <v>4960</v>
       </c>
-      <c r="D42" s="4">
+      <c r="D43" s="4">
         <f t="shared" si="1"/>
         <v>7450</v>
       </c>
-      <c r="H42" s="17" t="s">
+      <c r="H43" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="I42" s="5">
+      <c r="I43" s="5">
         <v>10</v>
       </c>
-      <c r="K42" s="14"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="17" t="s">
+      <c r="K43" s="14"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B44" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C43" s="5">
+      <c r="C44" s="5">
         <v>4000</v>
       </c>
-      <c r="D43" s="4">
+      <c r="D44" s="4">
         <f t="shared" si="1"/>
         <v>11450</v>
       </c>
-      <c r="H43" s="17" t="s">
+      <c r="H44" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="I43" s="5">
+      <c r="I44" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B44" s="4" t="s">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B45" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C45" s="5">
         <v>-10000</v>
       </c>
-      <c r="D44" s="4">
+      <c r="D45" s="4">
         <f t="shared" si="1"/>
         <v>1450</v>
       </c>
-      <c r="H44" s="17" t="s">
+      <c r="H45" s="17" t="s">
         <v>156</v>
-      </c>
-      <c r="I44" s="5">
-        <v>10</v>
-      </c>
-      <c r="K44" s="14"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B45" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C45" s="5">
-        <v>7640</v>
-      </c>
-      <c r="D45" s="4">
-        <f t="shared" ref="D45:D50" si="2">D44+C45</f>
-        <v>9090</v>
-      </c>
-      <c r="H45" s="17" t="s">
-        <v>193</v>
       </c>
       <c r="I45" s="5">
         <v>10</v>
       </c>
+      <c r="K45" s="14"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B46" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C46" s="5">
+        <v>7640</v>
+      </c>
+      <c r="D46" s="4">
+        <f t="shared" ref="D46:D51" si="2">D45+C46</f>
+        <v>9090</v>
+      </c>
+      <c r="H46" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="I46" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B47" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C46" s="5">
+      <c r="C47" s="5">
         <v>3000</v>
       </c>
-      <c r="D46" s="4">
+      <c r="D47" s="4">
         <f t="shared" si="2"/>
         <v>12090</v>
       </c>
-      <c r="H46" s="17" t="s">
+      <c r="H47" s="17" t="s">
         <v>195</v>
       </c>
-      <c r="I46" s="5">
+      <c r="I47" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B47" s="4" t="s">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B48" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C48" s="5">
         <v>-10000</v>
       </c>
-      <c r="D47" s="4">
+      <c r="D48" s="4">
         <f t="shared" si="2"/>
         <v>2090</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B48" s="4" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C48" s="5">
+      <c r="C49" s="5">
         <v>800</v>
       </c>
-      <c r="D48" s="4">
+      <c r="D49" s="4">
         <f t="shared" si="2"/>
         <v>2890</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="17" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B50" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C49" s="5">
+      <c r="C50" s="5">
         <v>2000</v>
       </c>
-      <c r="D49" s="4">
+      <c r="D50" s="4">
         <f t="shared" si="2"/>
         <v>4890</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="17" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B51" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C50" s="5">
+      <c r="C51" s="5">
         <v>4000</v>
       </c>
-      <c r="D50" s="4">
+      <c r="D51" s="4">
         <f t="shared" si="2"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="17" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B52" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C51" s="5">
+      <c r="C52" s="5">
         <v>4000</v>
       </c>
-      <c r="D51" s="4">
-        <f t="shared" ref="D51:D56" si="3">D50+C51</f>
+      <c r="D52" s="4">
+        <f t="shared" ref="D52:D57" si="3">D51+C52</f>
         <v>12890</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B52" s="4" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B53" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C52" s="5">
+      <c r="C53" s="5">
         <v>5000</v>
       </c>
-      <c r="D52" s="4">
+      <c r="D53" s="4">
         <f t="shared" si="3"/>
         <v>17890</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B53" s="4" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B54" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="5">
+      <c r="C54" s="5">
         <v>-10000</v>
       </c>
-      <c r="D53" s="4">
+      <c r="D54" s="4">
         <f t="shared" si="3"/>
         <v>7890</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="17">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="17">
         <v>44969</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B55" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C54" s="5">
+      <c r="C55" s="5">
         <v>900</v>
       </c>
-      <c r="D54" s="4">
+      <c r="D55" s="4">
         <f t="shared" si="3"/>
         <v>8790</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="4" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B56" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C55" s="5">
+      <c r="C56" s="5">
         <v>4000</v>
       </c>
-      <c r="D55" s="4">
+      <c r="D56" s="4">
         <f t="shared" si="3"/>
         <v>12790</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B56" s="4" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B57" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C56" s="5">
+      <c r="C57" s="5">
         <v>-10000</v>
       </c>
-      <c r="D56" s="4">
+      <c r="D57" s="4">
         <f t="shared" si="3"/>
         <v>2790</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C57" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D57" s="4">
-        <f t="shared" ref="D57:D64" si="4">D56+C57</f>
-        <v>4790</v>
-      </c>
-    </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C58" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D58" s="4">
+        <f t="shared" ref="D58:D65" si="4">D57+C58</f>
+        <v>4790</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B59" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C58" s="5">
+      <c r="C59" s="5">
         <v>700</v>
       </c>
-      <c r="D58" s="4">
+      <c r="D59" s="4">
         <f t="shared" si="4"/>
         <v>5490</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B59" s="4" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B60" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C59" s="5">
+      <c r="C60" s="5">
         <v>4000</v>
       </c>
-      <c r="D59" s="4">
+      <c r="D60" s="4">
         <f t="shared" si="4"/>
         <v>9490</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="17" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B61" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C60" s="5">
+      <c r="C61" s="5">
         <v>600</v>
       </c>
-      <c r="D60" s="4">
+      <c r="D61" s="4">
         <f t="shared" si="4"/>
         <v>10090</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B61" s="4" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B62" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C61" s="5">
+      <c r="C62" s="5">
         <v>-10000</v>
       </c>
-      <c r="D61" s="4">
+      <c r="D62" s="4">
         <f t="shared" si="4"/>
         <v>90</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="17" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B63" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C62" s="5">
+      <c r="C63" s="5">
         <f>700+5000+300+600+400+1000+800</f>
         <v>8800</v>
       </c>
-      <c r="D62" s="4">
+      <c r="D63" s="4">
         <f t="shared" si="4"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B63" s="4" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B64" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C63" s="5">
+      <c r="C64" s="5">
         <v>6000</v>
       </c>
-      <c r="D63" s="4">
+      <c r="D64" s="4">
         <f t="shared" si="4"/>
         <v>14890</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B64" s="4" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B65" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C64" s="5">
+      <c r="C65" s="5">
         <v>-10000</v>
       </c>
-      <c r="D64" s="4">
+      <c r="D65" s="4">
         <f t="shared" si="4"/>
         <v>4890</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="17" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B66" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C65" s="5">
+      <c r="C66" s="5">
         <v>500</v>
       </c>
-      <c r="D65" s="4">
-        <f t="shared" ref="D65:D70" si="5">D64+C65</f>
+      <c r="D66" s="4">
+        <f t="shared" ref="D66:D71" si="5">D65+C66</f>
         <v>5390</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B66" s="4" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B67" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C66" s="5">
+      <c r="C67" s="5">
         <v>700</v>
       </c>
-      <c r="D66" s="4">
+      <c r="D67" s="4">
         <f t="shared" si="5"/>
         <v>6090</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B67" s="4" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B68" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C67" s="5">
+      <c r="C68" s="5">
         <v>1500</v>
       </c>
-      <c r="D67" s="4">
+      <c r="D68" s="4">
         <f t="shared" si="5"/>
         <v>7590</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B68" s="4" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B69" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C68" s="5">
+      <c r="C69" s="5">
         <v>5000</v>
       </c>
-      <c r="D68" s="4">
+      <c r="D69" s="4">
         <f t="shared" si="5"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B69" s="4" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B70" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C69" s="5">
+      <c r="C70" s="5">
         <v>-10000</v>
       </c>
-      <c r="D69" s="4">
+      <c r="D70" s="4">
         <f t="shared" si="5"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="17" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B71" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C70" s="5">
+      <c r="C71" s="5">
         <v>2000</v>
       </c>
-      <c r="D70" s="4">
+      <c r="D71" s="4">
         <f t="shared" si="5"/>
         <v>4590</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B71" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C71" s="5">
-        <v>700</v>
-      </c>
-      <c r="D71" s="4">
-        <f t="shared" ref="D71:D76" si="6">D70+C71</f>
-        <v>5290</v>
-      </c>
-    </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="17" t="s">
-        <v>82</v>
-      </c>
       <c r="B72" s="4" t="s">
         <v>77</v>
       </c>
@@ -2132,401 +2135,404 @@
         <v>700</v>
       </c>
       <c r="D72" s="4">
+        <f t="shared" ref="D72:D77" si="6">D71+C72</f>
+        <v>5290</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C73" s="5">
+        <v>700</v>
+      </c>
+      <c r="D73" s="4">
         <f t="shared" si="6"/>
         <v>5990</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="17" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B74" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C73" s="5">
+      <c r="C74" s="5">
         <v>700</v>
       </c>
-      <c r="D73" s="4">
+      <c r="D74" s="4">
         <f t="shared" si="6"/>
         <v>6690</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="17" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B75" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C74" s="5">
+      <c r="C75" s="5">
         <v>4000</v>
       </c>
-      <c r="D74" s="4">
+      <c r="D75" s="4">
         <f t="shared" si="6"/>
         <v>10690</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B75" s="4" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B76" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C75" s="5">
+      <c r="C76" s="5">
         <v>-10000</v>
       </c>
-      <c r="D75" s="4">
+      <c r="D76" s="4">
         <f t="shared" si="6"/>
         <v>690</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="17" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B77" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C76" s="5">
+      <c r="C77" s="5">
         <v>1000</v>
       </c>
-      <c r="D76" s="4">
+      <c r="D77" s="4">
         <f t="shared" si="6"/>
         <v>1690</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="17" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="B78" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C77" s="5">
+      <c r="C78" s="5">
         <v>7000</v>
       </c>
-      <c r="D77" s="4">
-        <f t="shared" ref="D77:D82" si="7">D76+C77</f>
+      <c r="D78" s="4">
+        <f t="shared" ref="D78:D83" si="7">D77+C78</f>
         <v>8690</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B78" s="4" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B79" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C78" s="5">
+      <c r="C79" s="5">
         <v>10000</v>
       </c>
-      <c r="D78" s="4">
+      <c r="D79" s="4">
         <f t="shared" si="7"/>
         <v>18690</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B79" s="4" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B80" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C79" s="5">
+      <c r="C80" s="5">
         <v>-10000</v>
       </c>
-      <c r="D79" s="4">
+      <c r="D80" s="4">
         <f t="shared" si="7"/>
         <v>8690</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B80" s="4" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B81" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C80" s="5">
+      <c r="C81" s="5">
         <v>1700</v>
       </c>
-      <c r="D80" s="4">
+      <c r="D81" s="4">
         <f t="shared" si="7"/>
         <v>10390</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B81" s="4" t="s">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B82" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C81" s="5">
+      <c r="C82" s="5">
         <v>-10000</v>
       </c>
-      <c r="D81" s="4">
+      <c r="D82" s="4">
         <f t="shared" si="7"/>
         <v>390</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B82" s="4" t="s">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B83" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C82" s="5">
+      <c r="C83" s="5">
         <v>6000</v>
       </c>
-      <c r="D82" s="4">
+      <c r="D83" s="4">
         <f t="shared" si="7"/>
         <v>6390</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="B83" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C83" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D83" s="4">
-        <f t="shared" ref="D83:D88" si="8">D82+C83</f>
-        <v>8390</v>
-      </c>
-    </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C84" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D84" s="4">
+        <f t="shared" ref="D84:D89" si="8">D83+C84</f>
+        <v>8390</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="B84" s="4" t="s">
+      <c r="B85" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C84" s="5">
+      <c r="C85" s="5">
         <v>5000</v>
       </c>
-      <c r="D84" s="4">
+      <c r="D85" s="4">
         <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B85" s="4" t="s">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B86" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C85" s="5">
+      <c r="C86" s="5">
         <v>-10000</v>
       </c>
-      <c r="D85" s="4">
+      <c r="D86" s="4">
         <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="17" t="s">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="B87" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C86" s="5">
+      <c r="C87" s="5">
         <v>1000</v>
       </c>
-      <c r="D86" s="4">
+      <c r="D87" s="4">
         <f t="shared" si="8"/>
         <v>4390</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B87" s="4" t="s">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B88" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C87" s="5">
+      <c r="C88" s="5">
         <v>9000</v>
       </c>
-      <c r="D87" s="4">
+      <c r="D88" s="4">
         <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B88" s="4" t="s">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B89" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C88" s="5">
+      <c r="C89" s="5">
         <v>-10000</v>
       </c>
-      <c r="D88" s="4">
+      <c r="D89" s="4">
         <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B89" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C89" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D89" s="4">
-        <f t="shared" ref="D89:D94" si="9">D88+C89</f>
-        <v>5390</v>
-      </c>
-    </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B90" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C90" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D90" s="4">
+        <f t="shared" ref="D90:D95" si="9">D89+C90</f>
+        <v>5390</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B91" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C90" s="5">
+      <c r="C91" s="5">
         <v>6000</v>
       </c>
-      <c r="D90" s="4">
+      <c r="D91" s="4">
         <f t="shared" si="9"/>
         <v>11390</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B91" s="4" t="s">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B92" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C91" s="5">
+      <c r="C92" s="5">
         <v>-10000</v>
       </c>
-      <c r="D91" s="4">
+      <c r="D92" s="4">
         <f t="shared" si="9"/>
         <v>1390</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B92" s="4" t="s">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B93" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C92" s="5">
+      <c r="C93" s="5">
         <v>400</v>
       </c>
-      <c r="D92" s="4">
+      <c r="D93" s="4">
         <f t="shared" si="9"/>
         <v>1790</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="17" t="s">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="B93" s="4" t="s">
+      <c r="B94" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C93" s="5">
+      <c r="C94" s="5">
         <v>2000</v>
       </c>
-      <c r="D93" s="4">
+      <c r="D94" s="4">
         <f t="shared" si="9"/>
         <v>3790</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="17" t="s">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="B94" s="4" t="s">
+      <c r="B95" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C94" s="5">
+      <c r="C95" s="5">
         <v>6000</v>
       </c>
-      <c r="D94" s="4">
+      <c r="D95" s="4">
         <f t="shared" si="9"/>
         <v>9790</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="17" t="s">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="B95" s="4" t="s">
+      <c r="B96" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C95" s="5">
+      <c r="C96" s="5">
         <v>1000</v>
       </c>
-      <c r="D95" s="4">
-        <f t="shared" ref="D95:D100" si="10">D94+C95</f>
+      <c r="D96" s="4">
+        <f t="shared" ref="D96:D101" si="10">D95+C96</f>
         <v>10790</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B96" s="4" t="s">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B97" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C96" s="5">
+      <c r="C97" s="5">
         <v>-10000</v>
       </c>
-      <c r="D96" s="4">
+      <c r="D97" s="4">
         <f t="shared" si="10"/>
         <v>790</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="17" t="s">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="B97" s="4" t="s">
+      <c r="B98" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C97" s="5">
+      <c r="C98" s="5">
         <v>800</v>
       </c>
-      <c r="D97" s="4">
+      <c r="D98" s="4">
         <f t="shared" si="10"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="17" t="s">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="B98" s="4" t="s">
+      <c r="B99" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C98" s="5">
+      <c r="C99" s="5">
         <v>5000</v>
       </c>
-      <c r="D98" s="4">
+      <c r="D99" s="4">
         <f t="shared" si="10"/>
         <v>6590</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="17" t="s">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="B99" s="4" t="s">
+      <c r="B100" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C99" s="5">
+      <c r="C100" s="5">
         <v>6000</v>
       </c>
-      <c r="D99" s="4">
+      <c r="D100" s="4">
         <f t="shared" si="10"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B100" s="4" t="s">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B101" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C100" s="5">
+      <c r="C101" s="5">
         <v>-10000</v>
       </c>
-      <c r="D100" s="4">
+      <c r="D101" s="4">
         <f t="shared" si="10"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="17" t="s">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="B101" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C101" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D101" s="4">
-        <f t="shared" ref="D101:D107" si="11">D100+C101</f>
-        <v>4590</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B102" s="4" t="s">
         <v>65</v>
       </c>
@@ -2534,926 +2540,926 @@
         <v>2000</v>
       </c>
       <c r="D102" s="4">
+        <f t="shared" ref="D102:D108" si="11">D101+C102</f>
+        <v>4590</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B103" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C103" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D103" s="4">
         <f t="shared" si="11"/>
         <v>6590</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B103" s="4" t="s">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B104" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C103" s="5">
+      <c r="C104" s="5">
         <v>7000</v>
       </c>
-      <c r="D103" s="4">
+      <c r="D104" s="4">
         <f t="shared" si="11"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B104" s="4" t="s">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B105" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C104" s="5">
+      <c r="C105" s="5">
         <v>-10000</v>
       </c>
-      <c r="D104" s="4">
+      <c r="D105" s="4">
         <f t="shared" si="11"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="17" t="s">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="B105" s="4" t="s">
+      <c r="B106" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C105" s="5">
+      <c r="C106" s="5">
         <v>2000</v>
       </c>
-      <c r="D105" s="4">
+      <c r="D106" s="4">
         <f t="shared" si="11"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="17" t="s">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="B106" s="4" t="s">
+      <c r="B107" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C106" s="5">
+      <c r="C107" s="5">
         <v>6000</v>
       </c>
-      <c r="D106" s="4">
+      <c r="D107" s="4">
         <f t="shared" si="11"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B107" s="4" t="s">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B108" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C107" s="5">
+      <c r="C108" s="5">
         <v>-10000</v>
       </c>
-      <c r="D107" s="4">
+      <c r="D108" s="4">
         <f t="shared" si="11"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="B108" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C108" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D108" s="4">
-        <f t="shared" ref="D108:D113" si="12">D107+C108</f>
-        <v>3590</v>
-      </c>
-    </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C109" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D109" s="4">
+        <f t="shared" ref="D109:D114" si="12">D108+C109</f>
+        <v>3590</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="B109" s="4" t="s">
+      <c r="B110" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C109" s="5">
+      <c r="C110" s="5">
         <v>7000</v>
       </c>
-      <c r="D109" s="4">
+      <c r="D110" s="4">
         <f t="shared" si="12"/>
         <v>10590</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B110" s="4" t="s">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B111" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C110" s="5">
+      <c r="C111" s="5">
         <v>-10000</v>
       </c>
-      <c r="D110" s="4">
+      <c r="D111" s="4">
         <f t="shared" si="12"/>
         <v>590</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B111" s="4" t="s">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B112" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C111" s="5">
+      <c r="C112" s="5">
         <v>12000</v>
       </c>
-      <c r="D111" s="4">
+      <c r="D112" s="4">
         <f t="shared" si="12"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B112" s="4" t="s">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B113" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C112" s="5">
+      <c r="C113" s="5">
         <v>-10000</v>
       </c>
-      <c r="D112" s="4">
+      <c r="D113" s="4">
         <f t="shared" si="12"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B113" s="4" t="s">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B114" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C113" s="5">
+      <c r="C114" s="5">
         <v>2000</v>
       </c>
-      <c r="D113" s="4">
+      <c r="D114" s="4">
         <f t="shared" si="12"/>
         <v>4590</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="B114" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C114" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D114" s="4">
-        <f t="shared" ref="D114:D119" si="13">D113+C114</f>
-        <v>6590</v>
-      </c>
-    </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="B115" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C115" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D115" s="4">
+        <f t="shared" ref="D115:D120" si="13">D114+C115</f>
+        <v>6590</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="B115" s="4" t="s">
+      <c r="B116" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C115" s="5">
+      <c r="C116" s="5">
         <v>7000</v>
       </c>
-      <c r="D115" s="4">
+      <c r="D116" s="4">
         <f t="shared" si="13"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B116" s="4" t="s">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B117" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C116" s="5">
+      <c r="C117" s="5">
         <v>-10000</v>
       </c>
-      <c r="D116" s="4">
+      <c r="D117" s="4">
         <f t="shared" si="13"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="17" t="s">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="B117" s="4" t="s">
+      <c r="B118" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C117" s="5">
+      <c r="C118" s="5">
         <v>2000</v>
       </c>
-      <c r="D117" s="4">
+      <c r="D118" s="4">
         <f t="shared" si="13"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="17" t="s">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="B118" s="4" t="s">
+      <c r="B119" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C118" s="5">
+      <c r="C119" s="5">
         <v>8000</v>
       </c>
-      <c r="D118" s="4">
+      <c r="D119" s="4">
         <f t="shared" si="13"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B119" s="4" t="s">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B120" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C119" s="5">
+      <c r="C120" s="5">
         <v>-10000</v>
       </c>
-      <c r="D119" s="4">
+      <c r="D120" s="4">
         <f t="shared" si="13"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="17" t="s">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="B120" s="4" t="s">
+      <c r="B121" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C120" s="5">
+      <c r="C121" s="5">
         <v>2000</v>
       </c>
-      <c r="D120" s="4">
-        <f t="shared" ref="D120:D125" si="14">D119+C120</f>
+      <c r="D121" s="4">
+        <f t="shared" ref="D121:D126" si="14">D120+C121</f>
         <v>5590</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B121" s="4" t="s">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B122" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C121" s="5">
+      <c r="C122" s="5">
         <v>5000</v>
       </c>
-      <c r="D121" s="4">
+      <c r="D122" s="4">
         <f t="shared" si="14"/>
         <v>10590</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B122" s="4" t="s">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B123" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C122" s="5">
+      <c r="C123" s="5">
         <v>-10000</v>
       </c>
-      <c r="D122" s="4">
+      <c r="D123" s="4">
         <f t="shared" si="14"/>
         <v>590</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B123" s="4" t="s">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B124" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C123" s="5">
+      <c r="C124" s="5">
         <v>2000</v>
       </c>
-      <c r="D123" s="4">
+      <c r="D124" s="4">
         <f t="shared" si="14"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B124" s="4" t="s">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B125" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C124" s="5">
+      <c r="C125" s="5">
         <v>9000</v>
       </c>
-      <c r="D124" s="4">
+      <c r="D125" s="4">
         <f t="shared" si="14"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B125" s="4" t="s">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B126" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C125" s="5">
+      <c r="C126" s="5">
         <v>-10000</v>
       </c>
-      <c r="D125" s="4">
+      <c r="D126" s="4">
         <f t="shared" si="14"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="B126" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C126" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D126" s="4">
-        <f t="shared" ref="D126:D131" si="15">D125+C126</f>
-        <v>3590</v>
-      </c>
-    </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="B127" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C127" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D127" s="4">
+        <f t="shared" ref="D127:D132" si="15">D126+C127</f>
+        <v>3590</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="B127" s="4" t="s">
+      <c r="B128" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C127" s="5">
+      <c r="C128" s="5">
         <v>8000</v>
       </c>
-      <c r="D127" s="4">
+      <c r="D128" s="4">
         <f t="shared" si="15"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B128" s="4" t="s">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B129" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C128" s="5">
+      <c r="C129" s="5">
         <v>-10000</v>
       </c>
-      <c r="D128" s="4">
+      <c r="D129" s="4">
         <f t="shared" si="15"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="17" t="s">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="B129" s="4" t="s">
+      <c r="B130" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C129" s="5">
+      <c r="C130" s="5">
         <v>2000</v>
       </c>
-      <c r="D129" s="4">
+      <c r="D130" s="4">
         <f t="shared" si="15"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="17" t="s">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="B130" s="4" t="s">
+      <c r="B131" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="C130" s="5">
+      <c r="C131" s="5">
         <v>12000</v>
       </c>
-      <c r="D130" s="4">
+      <c r="D131" s="4">
         <f t="shared" si="15"/>
         <v>15590</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B131" s="4" t="s">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B132" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C131" s="5">
+      <c r="C132" s="5">
         <v>-10000</v>
       </c>
-      <c r="D131" s="4">
+      <c r="D132" s="4">
         <f t="shared" si="15"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="17" t="s">
-        <v>168</v>
-      </c>
-      <c r="B132" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="C132" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D132" s="4">
-        <f t="shared" ref="D132:D137" si="16">D131+C132</f>
-        <v>7590</v>
-      </c>
-    </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="B133" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C133" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D133" s="4">
+        <f t="shared" ref="D133:D138" si="16">D132+C133</f>
+        <v>7590</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="B133" s="4" t="s">
+      <c r="B134" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="C133" s="5">
+      <c r="C134" s="5">
         <v>10000</v>
       </c>
-      <c r="D133" s="4">
+      <c r="D134" s="4">
         <f t="shared" si="16"/>
         <v>17590</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B134" s="4" t="s">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B135" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C134" s="5">
+      <c r="C135" s="5">
         <v>-10000</v>
       </c>
-      <c r="D134" s="4">
+      <c r="D135" s="4">
         <f t="shared" si="16"/>
         <v>7590</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B135" s="4" t="s">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B136" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="C135" s="5">
+      <c r="C136" s="5">
         <v>2000</v>
       </c>
-      <c r="D135" s="4">
+      <c r="D136" s="4">
         <f t="shared" si="16"/>
         <v>9590</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="17" t="s">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="B136" s="4" t="s">
+      <c r="B137" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="C136" s="5">
+      <c r="C137" s="5">
         <v>-1200</v>
       </c>
-      <c r="D136" s="4">
+      <c r="D137" s="4">
         <f t="shared" si="16"/>
         <v>8390</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B137" s="4" t="s">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B138" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="C137" s="5">
+      <c r="C138" s="5">
         <v>500</v>
       </c>
-      <c r="D137" s="4">
+      <c r="D138" s="4">
         <f t="shared" si="16"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="B138" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C138" s="5">
-        <v>750</v>
-      </c>
-      <c r="D138" s="4">
-        <f t="shared" ref="D138:D143" si="17">D137+C138</f>
-        <v>9640</v>
-      </c>
-    </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="B139" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C139" s="5">
+        <v>750</v>
+      </c>
+      <c r="D139" s="4">
+        <f t="shared" ref="D139:D144" si="17">D138+C139</f>
+        <v>9640</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="B139" s="4" t="s">
+      <c r="B140" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C139" s="5">
+      <c r="C140" s="5">
         <v>2000</v>
       </c>
-      <c r="D139" s="4">
+      <c r="D140" s="4">
         <f t="shared" si="17"/>
         <v>11640</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B140" s="4" t="s">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B141" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C140" s="5">
+      <c r="C141" s="5">
         <v>2000</v>
       </c>
-      <c r="D140" s="4">
+      <c r="D141" s="4">
         <f t="shared" si="17"/>
         <v>13640</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B141" s="4" t="s">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B142" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C141" s="5">
+      <c r="C142" s="5">
         <v>-10000</v>
       </c>
-      <c r="D141" s="4">
+      <c r="D142" s="4">
         <f t="shared" si="17"/>
         <v>3640</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B142" s="4" t="s">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B143" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="C142" s="5">
+      <c r="C143" s="5">
         <v>350</v>
       </c>
-      <c r="D142" s="4">
+      <c r="D143" s="4">
         <f t="shared" si="17"/>
         <v>3990</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="17" t="s">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="B143" s="4" t="s">
+      <c r="B144" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="C143" s="5">
+      <c r="C144" s="5">
         <v>300</v>
       </c>
-      <c r="D143" s="4">
+      <c r="D144" s="4">
         <f t="shared" si="17"/>
         <v>4290</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="17" t="s">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" s="17" t="s">
         <v>181</v>
       </c>
-      <c r="B144" s="4" t="s">
+      <c r="B145" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="C144" s="5">
+      <c r="C145" s="5">
         <v>3800</v>
       </c>
-      <c r="D144" s="4">
-        <f t="shared" ref="D144:D150" si="18">D143+C144</f>
+      <c r="D145" s="4">
+        <f t="shared" ref="D145:D151" si="18">D144+C145</f>
         <v>8090</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B145" s="4" t="s">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B146" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C145" s="5">
+      <c r="C146" s="5">
         <v>500</v>
       </c>
-      <c r="D145" s="4">
+      <c r="D146" s="4">
         <f t="shared" si="18"/>
         <v>8590</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="17" t="s">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="B146" s="4" t="s">
+      <c r="B147" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="C146" s="5">
+      <c r="C147" s="5">
         <v>1300</v>
       </c>
-      <c r="D146" s="4">
+      <c r="D147" s="4">
         <f t="shared" si="18"/>
         <v>9890</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="17" t="s">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" s="17" t="s">
         <v>185</v>
       </c>
-      <c r="B147" s="4" t="s">
+      <c r="B148" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C147" s="5">
+      <c r="C148" s="5">
         <v>9000</v>
       </c>
-      <c r="D147" s="4">
+      <c r="D148" s="4">
         <f t="shared" si="18"/>
         <v>18890</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B148" s="4" t="s">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B149" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C148" s="5">
+      <c r="C149" s="5">
         <v>-10000</v>
       </c>
-      <c r="D148" s="4">
+      <c r="D149" s="4">
         <f t="shared" si="18"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="17" t="s">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="B149" s="4" t="s">
+      <c r="B150" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C149" s="5">
+      <c r="C150" s="5">
         <v>2000</v>
       </c>
-      <c r="D149" s="4">
+      <c r="D150" s="4">
         <f t="shared" si="18"/>
         <v>10890</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B150" s="4" t="s">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B151" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C150" s="5">
+      <c r="C151" s="5">
         <v>-10000</v>
       </c>
-      <c r="D150" s="4">
+      <c r="D151" s="4">
         <f t="shared" si="18"/>
         <v>890</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="17" t="s">
-        <v>187</v>
-      </c>
-      <c r="B151" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="C151" s="5">
-        <v>500</v>
-      </c>
-      <c r="D151" s="4">
-        <f t="shared" ref="D151:D156" si="19">D150+C151</f>
-        <v>1390</v>
-      </c>
-    </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="B152" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="C152" s="5">
+        <v>500</v>
+      </c>
+      <c r="D152" s="4">
+        <f t="shared" ref="D152:D157" si="19">D151+C152</f>
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" s="17" t="s">
         <v>189</v>
       </c>
-      <c r="B152" s="4" t="s">
+      <c r="B153" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C152" s="5">
+      <c r="C153" s="5">
         <v>10000</v>
       </c>
-      <c r="D152" s="4">
+      <c r="D153" s="4">
         <f t="shared" si="19"/>
         <v>11390</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B153" s="4" t="s">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B154" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C153" s="5">
+      <c r="C154" s="5">
         <v>-10000</v>
       </c>
-      <c r="D153" s="4">
+      <c r="D154" s="4">
         <f t="shared" si="19"/>
         <v>1390</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="17" t="s">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="B154" s="4" t="s">
+      <c r="B155" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C154" s="5">
+      <c r="C155" s="5">
         <v>3000</v>
       </c>
-      <c r="D154" s="4">
+      <c r="D155" s="4">
         <f t="shared" si="19"/>
         <v>4390</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="17" t="s">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="B155" s="4" t="s">
+      <c r="B156" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C155" s="5">
+      <c r="C156" s="5">
         <v>2000</v>
       </c>
-      <c r="D155" s="4">
+      <c r="D156" s="4">
         <f t="shared" si="19"/>
         <v>6390</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B156" s="4" t="s">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B157" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C156" s="5">
+      <c r="C157" s="5">
         <v>2000</v>
       </c>
-      <c r="D156" s="4">
+      <c r="D157" s="4">
         <f t="shared" si="19"/>
         <v>8390</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="17" t="s">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" s="17" t="s">
         <v>193</v>
       </c>
-      <c r="B157" s="4" t="s">
+      <c r="B158" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="C157" s="5">
+      <c r="C158" s="5">
         <v>11000</v>
       </c>
-      <c r="D157" s="4">
-        <f t="shared" ref="D157:D162" si="20">D156+C157</f>
+      <c r="D158" s="4">
+        <f t="shared" ref="D158:D163" si="20">D157+C158</f>
         <v>19390</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B158" s="4" t="s">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B159" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C158" s="5">
+      <c r="C159" s="5">
         <v>-10000</v>
       </c>
-      <c r="D158" s="4">
+      <c r="D159" s="4">
         <f t="shared" si="20"/>
         <v>9390</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="17" t="s">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" s="17" t="s">
         <v>195</v>
       </c>
-      <c r="B159" s="4" t="s">
+      <c r="B160" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="C159" s="5">
+      <c r="C160" s="5">
         <v>3000</v>
       </c>
-      <c r="D159" s="4">
+      <c r="D160" s="4">
         <f t="shared" si="20"/>
         <v>12390</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B160" s="4" t="s">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B161" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C160" s="5">
+      <c r="C161" s="5">
         <v>-10000</v>
       </c>
-      <c r="D160" s="4">
+      <c r="D161" s="4">
         <f t="shared" si="20"/>
         <v>2390</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B161" s="4" t="s">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B162" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C161" s="5">
+      <c r="C162" s="5">
         <v>500</v>
       </c>
-      <c r="D161" s="4">
+      <c r="D162" s="4">
         <f t="shared" si="20"/>
         <v>2890</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" s="17" t="s">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="B162" s="4" t="s">
+      <c r="B163" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C162" s="5">
+      <c r="C163" s="5">
         <v>5600</v>
       </c>
-      <c r="D162" s="4">
+      <c r="D163" s="4">
         <f t="shared" si="20"/>
         <v>8490</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B163" s="4" t="s">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B164" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="C163" s="5">
+      <c r="C164" s="5">
         <v>4700</v>
       </c>
-      <c r="D163" s="4">
-        <f t="shared" ref="D163:D169" si="21">D162+C163</f>
+      <c r="D164" s="4">
+        <f t="shared" ref="D164:D170" si="21">D163+C164</f>
         <v>13190</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164" s="17" t="s">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" s="17" t="s">
         <v>200</v>
       </c>
-      <c r="B164" s="4" t="s">
+      <c r="B165" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C164" s="5">
+      <c r="C165" s="5">
         <v>1500</v>
       </c>
-      <c r="D164" s="4">
+      <c r="D165" s="4">
         <f t="shared" si="21"/>
         <v>14690</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B165" s="4" t="s">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B166" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C165" s="5">
+      <c r="C166" s="5">
         <v>500</v>
       </c>
-      <c r="D165" s="4">
+      <c r="D166" s="4">
         <f t="shared" si="21"/>
         <v>15190</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A166" s="17" t="s">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" s="17" t="s">
         <v>201</v>
       </c>
-      <c r="B166" s="4" t="s">
+      <c r="B167" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C166" s="5">
+      <c r="C167" s="5">
         <v>1000</v>
       </c>
-      <c r="D166" s="4">
+      <c r="D167" s="4">
         <f t="shared" si="21"/>
         <v>16190</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A167" s="17" t="s">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="B167" s="4" t="s">
+      <c r="B168" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="C167" s="5">
+      <c r="C168" s="5">
         <v>1000</v>
       </c>
-      <c r="D167" s="4">
+      <c r="D168" s="4">
         <f t="shared" si="21"/>
         <v>17190</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A168" s="17" t="s">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="B168" s="4" t="s">
+      <c r="B169" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C168" s="5">
+      <c r="C169" s="5">
         <v>3000</v>
       </c>
-      <c r="D168" s="4">
+      <c r="D169" s="4">
         <f t="shared" si="21"/>
         <v>20190</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B169" s="4" t="s">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B170" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="C169" s="5">
+      <c r="C170" s="5">
         <v>-20000</v>
       </c>
-      <c r="D169" s="4">
+      <c r="D170" s="4">
         <f t="shared" si="21"/>
         <v>190</v>
-      </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B170" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C170" s="5">
-        <v>500</v>
-      </c>
-      <c r="D170" s="4">
-        <f>D169+C170</f>
-        <v>690</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -3465,6 +3471,45 @@
       </c>
       <c r="D171" s="4">
         <f>D170+C171</f>
+        <v>690</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B172" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C172" s="5">
+        <v>500</v>
+      </c>
+      <c r="D172" s="4">
+        <f>D171+C172</f>
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="B173" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="C173" s="5">
+        <v>10000</v>
+      </c>
+      <c r="D173" s="4">
+        <f>D172+C173</f>
+        <v>11190</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B174" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="C174" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D174" s="4">
+        <f>D173+C174</f>
         <v>1190</v>
       </c>
     </row>
@@ -3831,7 +3876,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>

</xml_diff>

<commit_message>
duy lay tien loi ngay 2308
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="CÔ DIỄM" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="212">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -652,6 +652,9 @@
   </si>
   <si>
     <t>cuối năm trả</t>
+  </si>
+  <si>
+    <t>23/08/2024</t>
   </si>
 </sst>
 </file>
@@ -1130,11 +1133,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K174"/>
+  <dimension ref="A1:K175"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D176" sqref="D176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3511,6 +3514,21 @@
       <c r="D174" s="4">
         <f>D173+C174</f>
         <v>1190</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="B175" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C175" s="5">
+        <v>3000</v>
+      </c>
+      <c r="D175" s="4">
+        <f>D174+C175</f>
+        <v>4190</v>
       </c>
     </row>
   </sheetData>
@@ -4012,7 +4030,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Duy layy tien loi co diem ngay 3008
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="213">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -655,6 +655,9 @@
   </si>
   <si>
     <t>23/08/2024</t>
+  </si>
+  <si>
+    <t>30/08/2024</t>
   </si>
 </sst>
 </file>
@@ -1133,11 +1136,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K175"/>
+  <dimension ref="A1:K178"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D176" sqref="D176"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1213,8 +1216,8 @@
         <v>20</v>
       </c>
       <c r="J3" s="4">
-        <f>SUM(I3:I61)</f>
-        <v>480</v>
+        <f>SUM(I3:I62)</f>
+        <v>490</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1520,38 +1523,38 @@
       <c r="K30" s="14"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="17" t="s">
+      <c r="H31" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="I31" s="5">
+        <v>10</v>
+      </c>
+      <c r="K31" s="14"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B32" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C32" s="5">
         <v>3000</v>
       </c>
-      <c r="D31" s="4">
-        <f>D22+C31</f>
+      <c r="D32" s="4">
+        <f>D22+C32</f>
         <v>8490</v>
       </c>
-      <c r="H31" s="17" t="s">
+      <c r="H32" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="I31" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H32" s="17" t="s">
-        <v>43</v>
-      </c>
       <c r="I32" s="5">
         <v>10</v>
       </c>
-      <c r="K32" s="14"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H33" s="17" t="s">
-        <v>146</v>
+        <v>43</v>
       </c>
       <c r="I33" s="5">
         <v>10</v>
@@ -1560,7 +1563,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H34" s="17" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="I34" s="5">
         <v>10</v>
@@ -1569,64 +1572,54 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H35" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="I35" s="5">
+        <v>10</v>
+      </c>
+      <c r="K35" s="14"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H36" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="I35" s="5">
-        <v>10</v>
-      </c>
-      <c r="K35" s="14"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B36" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C36" s="5">
-        <v>4400</v>
-      </c>
-      <c r="D36" s="4">
-        <f>D31+C36</f>
-        <v>12890</v>
-      </c>
-      <c r="H36" s="17" t="s">
-        <v>164</v>
-      </c>
       <c r="I36" s="5">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K36" s="14"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C37" s="5">
-        <v>-10000</v>
+        <v>4400</v>
       </c>
       <c r="D37" s="4">
-        <f>D36+C37</f>
-        <v>2890</v>
+        <f>D32+C37</f>
+        <v>12890</v>
       </c>
       <c r="H37" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I37" s="5">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="K37" s="14"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C38" s="5">
-        <v>1600</v>
+        <v>-10000</v>
       </c>
       <c r="D38" s="4">
-        <f t="shared" ref="D38:D45" si="1">D37+C38</f>
-        <v>4490</v>
+        <f>D37+C38</f>
+        <v>2890</v>
       </c>
       <c r="H38" s="17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I38" s="5">
         <v>10</v>
@@ -1635,517 +1628,521 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C39" s="5">
+        <v>1600</v>
+      </c>
+      <c r="D39" s="4">
+        <f t="shared" ref="D39:D46" si="1">D38+C39</f>
+        <v>4490</v>
+      </c>
+      <c r="H39" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="I39" s="5">
+        <v>10</v>
+      </c>
+      <c r="K39" s="14"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C39" s="5">
+      <c r="C40" s="5">
         <v>3000</v>
       </c>
-      <c r="D39" s="4">
+      <c r="D40" s="4">
         <f t="shared" si="1"/>
         <v>7490</v>
       </c>
-      <c r="H39" s="17" t="s">
+      <c r="H40" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="I39" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="17" t="s">
+      <c r="I40" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B41" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C40" s="5">
+      <c r="C41" s="5">
         <v>2000</v>
       </c>
-      <c r="D40" s="4">
+      <c r="D41" s="4">
         <f t="shared" si="1"/>
         <v>9490</v>
       </c>
-      <c r="H40" s="17" t="s">
+      <c r="H41" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="I40" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="17" t="s">
+      <c r="I41" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B42" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="5">
+      <c r="C42" s="5">
         <v>3000</v>
       </c>
-      <c r="D41" s="4">
+      <c r="D42" s="4">
         <f t="shared" si="1"/>
         <v>12490</v>
       </c>
-      <c r="H41" s="17" t="s">
+      <c r="H42" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="I41" s="5">
-        <v>10</v>
-      </c>
-      <c r="K41" s="14"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B42" s="4" t="s">
+      <c r="I42" s="5">
+        <v>10</v>
+      </c>
+      <c r="K42" s="14"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B43" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C43" s="5">
         <v>-10000</v>
       </c>
-      <c r="D42" s="4">
+      <c r="D43" s="4">
         <f t="shared" si="1"/>
         <v>2490</v>
       </c>
-      <c r="H42" s="17" t="s">
+      <c r="H43" s="17" t="s">
         <v>159</v>
       </c>
-      <c r="I42" s="5">
-        <v>10</v>
-      </c>
-      <c r="K42" s="14"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="17" t="s">
+      <c r="I43" s="5">
+        <v>10</v>
+      </c>
+      <c r="K43" s="14"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B44" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C43" s="5">
+      <c r="C44" s="5">
         <v>4960</v>
       </c>
-      <c r="D43" s="4">
+      <c r="D44" s="4">
         <f t="shared" si="1"/>
         <v>7450</v>
       </c>
-      <c r="H43" s="17" t="s">
+      <c r="H44" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="I43" s="5">
-        <v>10</v>
-      </c>
-      <c r="K43" s="14"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="17" t="s">
+      <c r="I44" s="5">
+        <v>10</v>
+      </c>
+      <c r="K44" s="14"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B45" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C45" s="5">
         <v>4000</v>
       </c>
-      <c r="D44" s="4">
+      <c r="D45" s="4">
         <f t="shared" si="1"/>
         <v>11450</v>
       </c>
-      <c r="H44" s="17" t="s">
+      <c r="H45" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="I44" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B45" s="4" t="s">
+      <c r="I45" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B46" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C45" s="5">
+      <c r="C46" s="5">
         <v>-10000</v>
       </c>
-      <c r="D45" s="4">
+      <c r="D46" s="4">
         <f t="shared" si="1"/>
         <v>1450</v>
       </c>
-      <c r="H45" s="17" t="s">
+      <c r="H46" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="I45" s="5">
-        <v>10</v>
-      </c>
-      <c r="K45" s="14"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B46" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C46" s="5">
-        <v>7640</v>
-      </c>
-      <c r="D46" s="4">
-        <f t="shared" ref="D46:D51" si="2">D45+C46</f>
-        <v>9090</v>
-      </c>
-      <c r="H46" s="17" t="s">
-        <v>192</v>
-      </c>
       <c r="I46" s="5">
         <v>10</v>
       </c>
+      <c r="K46" s="14"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B47" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C47" s="5">
+        <v>7640</v>
+      </c>
+      <c r="D47" s="4">
+        <f t="shared" ref="D47:D52" si="2">D46+C47</f>
+        <v>9090</v>
+      </c>
+      <c r="H47" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="I47" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B48" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C48" s="5">
         <v>3000</v>
       </c>
-      <c r="D47" s="4">
+      <c r="D48" s="4">
         <f t="shared" si="2"/>
         <v>12090</v>
       </c>
-      <c r="H47" s="17" t="s">
+      <c r="H48" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="I47" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B48" s="4" t="s">
+      <c r="I48" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C48" s="5">
+      <c r="C49" s="5">
         <v>-10000</v>
       </c>
-      <c r="D48" s="4">
+      <c r="D49" s="4">
         <f t="shared" si="2"/>
         <v>2090</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B49" s="4" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B50" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C49" s="5">
+      <c r="C50" s="5">
         <v>800</v>
       </c>
-      <c r="D49" s="4">
+      <c r="D50" s="4">
         <f t="shared" si="2"/>
         <v>2890</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="17" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B51" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C50" s="5">
+      <c r="C51" s="5">
         <v>2000</v>
       </c>
-      <c r="D50" s="4">
+      <c r="D51" s="4">
         <f t="shared" si="2"/>
         <v>4890</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="17" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B52" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C51" s="5">
+      <c r="C52" s="5">
         <v>4000</v>
       </c>
-      <c r="D51" s="4">
+      <c r="D52" s="4">
         <f t="shared" si="2"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="17" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B53" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C52" s="5">
+      <c r="C53" s="5">
         <v>4000</v>
       </c>
-      <c r="D52" s="4">
-        <f t="shared" ref="D52:D57" si="3">D51+C52</f>
+      <c r="D53" s="4">
+        <f t="shared" ref="D53:D58" si="3">D52+C53</f>
         <v>12890</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B53" s="4" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B54" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C53" s="5">
+      <c r="C54" s="5">
         <v>5000</v>
       </c>
-      <c r="D53" s="4">
+      <c r="D54" s="4">
         <f t="shared" si="3"/>
         <v>17890</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B54" s="4" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B55" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C54" s="5">
+      <c r="C55" s="5">
         <v>-10000</v>
       </c>
-      <c r="D54" s="4">
+      <c r="D55" s="4">
         <f t="shared" si="3"/>
         <v>7890</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="17">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="17">
         <v>44969</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B56" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C55" s="5">
+      <c r="C56" s="5">
         <v>900</v>
       </c>
-      <c r="D55" s="4">
+      <c r="D56" s="4">
         <f t="shared" si="3"/>
         <v>8790</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B56" s="4" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B57" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C56" s="5">
+      <c r="C57" s="5">
         <v>4000</v>
       </c>
-      <c r="D56" s="4">
+      <c r="D57" s="4">
         <f t="shared" si="3"/>
         <v>12790</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B57" s="4" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B58" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C57" s="5">
+      <c r="C58" s="5">
         <v>-10000</v>
       </c>
-      <c r="D57" s="4">
+      <c r="D58" s="4">
         <f t="shared" si="3"/>
         <v>2790</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C58" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D58" s="4">
-        <f t="shared" ref="D58:D65" si="4">D57+C58</f>
-        <v>4790</v>
-      </c>
-    </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C59" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D59" s="4">
+        <f t="shared" ref="D59:D66" si="4">D58+C59</f>
+        <v>4790</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B60" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C59" s="5">
+      <c r="C60" s="5">
         <v>700</v>
       </c>
-      <c r="D59" s="4">
+      <c r="D60" s="4">
         <f t="shared" si="4"/>
         <v>5490</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B60" s="4" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B61" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C60" s="5">
+      <c r="C61" s="5">
         <v>4000</v>
       </c>
-      <c r="D60" s="4">
+      <c r="D61" s="4">
         <f t="shared" si="4"/>
         <v>9490</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="17" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B62" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C61" s="5">
+      <c r="C62" s="5">
         <v>600</v>
       </c>
-      <c r="D61" s="4">
+      <c r="D62" s="4">
         <f t="shared" si="4"/>
         <v>10090</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B62" s="4" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B63" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C62" s="5">
+      <c r="C63" s="5">
         <v>-10000</v>
       </c>
-      <c r="D62" s="4">
+      <c r="D63" s="4">
         <f t="shared" si="4"/>
         <v>90</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="17" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B64" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C63" s="5">
+      <c r="C64" s="5">
         <f>700+5000+300+600+400+1000+800</f>
         <v>8800</v>
       </c>
-      <c r="D63" s="4">
+      <c r="D64" s="4">
         <f t="shared" si="4"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B64" s="4" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B65" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C64" s="5">
+      <c r="C65" s="5">
         <v>6000</v>
       </c>
-      <c r="D64" s="4">
+      <c r="D65" s="4">
         <f t="shared" si="4"/>
         <v>14890</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B65" s="4" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C65" s="5">
+      <c r="C66" s="5">
         <v>-10000</v>
       </c>
-      <c r="D65" s="4">
+      <c r="D66" s="4">
         <f t="shared" si="4"/>
         <v>4890</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="17" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B67" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C66" s="5">
+      <c r="C67" s="5">
         <v>500</v>
       </c>
-      <c r="D66" s="4">
-        <f t="shared" ref="D66:D71" si="5">D65+C66</f>
+      <c r="D67" s="4">
+        <f t="shared" ref="D67:D72" si="5">D66+C67</f>
         <v>5390</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B67" s="4" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B68" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C67" s="5">
+      <c r="C68" s="5">
         <v>700</v>
       </c>
-      <c r="D67" s="4">
+      <c r="D68" s="4">
         <f t="shared" si="5"/>
         <v>6090</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B68" s="4" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B69" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C68" s="5">
+      <c r="C69" s="5">
         <v>1500</v>
       </c>
-      <c r="D68" s="4">
+      <c r="D69" s="4">
         <f t="shared" si="5"/>
         <v>7590</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B69" s="4" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B70" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C69" s="5">
+      <c r="C70" s="5">
         <v>5000</v>
       </c>
-      <c r="D69" s="4">
+      <c r="D70" s="4">
         <f t="shared" si="5"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B70" s="4" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B71" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C70" s="5">
+      <c r="C71" s="5">
         <v>-10000</v>
       </c>
-      <c r="D70" s="4">
+      <c r="D71" s="4">
         <f t="shared" si="5"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="17" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B72" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C71" s="5">
+      <c r="C72" s="5">
         <v>2000</v>
       </c>
-      <c r="D71" s="4">
+      <c r="D72" s="4">
         <f t="shared" si="5"/>
         <v>4590</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B72" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C72" s="5">
-        <v>700</v>
-      </c>
-      <c r="D72" s="4">
-        <f t="shared" ref="D72:D77" si="6">D71+C72</f>
-        <v>5290</v>
-      </c>
-    </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="17" t="s">
-        <v>82</v>
-      </c>
       <c r="B73" s="4" t="s">
         <v>77</v>
       </c>
@@ -2153,401 +2150,404 @@
         <v>700</v>
       </c>
       <c r="D73" s="4">
+        <f t="shared" ref="D73:D78" si="6">D72+C73</f>
+        <v>5290</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C74" s="5">
+        <v>700</v>
+      </c>
+      <c r="D74" s="4">
         <f t="shared" si="6"/>
         <v>5990</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="17" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B75" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C74" s="5">
+      <c r="C75" s="5">
         <v>700</v>
       </c>
-      <c r="D74" s="4">
+      <c r="D75" s="4">
         <f t="shared" si="6"/>
         <v>6690</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="17" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="B76" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C75" s="5">
+      <c r="C76" s="5">
         <v>4000</v>
       </c>
-      <c r="D75" s="4">
+      <c r="D76" s="4">
         <f t="shared" si="6"/>
         <v>10690</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B76" s="4" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B77" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C76" s="5">
+      <c r="C77" s="5">
         <v>-10000</v>
       </c>
-      <c r="D76" s="4">
+      <c r="D77" s="4">
         <f t="shared" si="6"/>
         <v>690</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="17" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="B78" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C77" s="5">
+      <c r="C78" s="5">
         <v>1000</v>
       </c>
-      <c r="D77" s="4">
+      <c r="D78" s="4">
         <f t="shared" si="6"/>
         <v>1690</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="17" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B79" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C78" s="5">
+      <c r="C79" s="5">
         <v>7000</v>
       </c>
-      <c r="D78" s="4">
-        <f t="shared" ref="D78:D83" si="7">D77+C78</f>
+      <c r="D79" s="4">
+        <f t="shared" ref="D79:D84" si="7">D78+C79</f>
         <v>8690</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B79" s="4" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B80" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C79" s="5">
+      <c r="C80" s="5">
         <v>10000</v>
       </c>
-      <c r="D79" s="4">
+      <c r="D80" s="4">
         <f t="shared" si="7"/>
         <v>18690</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B80" s="4" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B81" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C80" s="5">
+      <c r="C81" s="5">
         <v>-10000</v>
       </c>
-      <c r="D80" s="4">
+      <c r="D81" s="4">
         <f t="shared" si="7"/>
         <v>8690</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B81" s="4" t="s">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B82" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C81" s="5">
+      <c r="C82" s="5">
         <v>1700</v>
       </c>
-      <c r="D81" s="4">
+      <c r="D82" s="4">
         <f t="shared" si="7"/>
         <v>10390</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B82" s="4" t="s">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B83" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C82" s="5">
+      <c r="C83" s="5">
         <v>-10000</v>
       </c>
-      <c r="D82" s="4">
+      <c r="D83" s="4">
         <f t="shared" si="7"/>
         <v>390</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B83" s="4" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B84" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C83" s="5">
+      <c r="C84" s="5">
         <v>6000</v>
       </c>
-      <c r="D83" s="4">
+      <c r="D84" s="4">
         <f t="shared" si="7"/>
         <v>6390</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="B84" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C84" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D84" s="4">
-        <f t="shared" ref="D84:D89" si="8">D83+C84</f>
-        <v>8390</v>
-      </c>
-    </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C85" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D85" s="4">
+        <f t="shared" ref="D85:D90" si="8">D84+C85</f>
+        <v>8390</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="B85" s="4" t="s">
+      <c r="B86" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C85" s="5">
+      <c r="C86" s="5">
         <v>5000</v>
       </c>
-      <c r="D85" s="4">
+      <c r="D86" s="4">
         <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B86" s="4" t="s">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B87" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C86" s="5">
+      <c r="C87" s="5">
         <v>-10000</v>
       </c>
-      <c r="D86" s="4">
+      <c r="D87" s="4">
         <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="17" t="s">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="B87" s="4" t="s">
+      <c r="B88" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C87" s="5">
+      <c r="C88" s="5">
         <v>1000</v>
       </c>
-      <c r="D87" s="4">
+      <c r="D88" s="4">
         <f t="shared" si="8"/>
         <v>4390</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B88" s="4" t="s">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B89" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C88" s="5">
+      <c r="C89" s="5">
         <v>9000</v>
       </c>
-      <c r="D88" s="4">
+      <c r="D89" s="4">
         <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B89" s="4" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B90" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C89" s="5">
+      <c r="C90" s="5">
         <v>-10000</v>
       </c>
-      <c r="D89" s="4">
+      <c r="D90" s="4">
         <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B90" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C90" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D90" s="4">
-        <f t="shared" ref="D90:D95" si="9">D89+C90</f>
-        <v>5390</v>
-      </c>
-    </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B91" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C91" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D91" s="4">
+        <f t="shared" ref="D91:D96" si="9">D90+C91</f>
+        <v>5390</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B92" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C91" s="5">
+      <c r="C92" s="5">
         <v>6000</v>
       </c>
-      <c r="D91" s="4">
+      <c r="D92" s="4">
         <f t="shared" si="9"/>
         <v>11390</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B92" s="4" t="s">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B93" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C92" s="5">
+      <c r="C93" s="5">
         <v>-10000</v>
       </c>
-      <c r="D92" s="4">
+      <c r="D93" s="4">
         <f t="shared" si="9"/>
         <v>1390</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B93" s="4" t="s">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B94" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C93" s="5">
+      <c r="C94" s="5">
         <v>400</v>
       </c>
-      <c r="D93" s="4">
+      <c r="D94" s="4">
         <f t="shared" si="9"/>
         <v>1790</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="17" t="s">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="B94" s="4" t="s">
+      <c r="B95" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C94" s="5">
+      <c r="C95" s="5">
         <v>2000</v>
       </c>
-      <c r="D94" s="4">
+      <c r="D95" s="4">
         <f t="shared" si="9"/>
         <v>3790</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="17" t="s">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="B95" s="4" t="s">
+      <c r="B96" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C95" s="5">
+      <c r="C96" s="5">
         <v>6000</v>
       </c>
-      <c r="D95" s="4">
+      <c r="D96" s="4">
         <f t="shared" si="9"/>
         <v>9790</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="17" t="s">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="B96" s="4" t="s">
+      <c r="B97" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C96" s="5">
+      <c r="C97" s="5">
         <v>1000</v>
       </c>
-      <c r="D96" s="4">
-        <f t="shared" ref="D96:D101" si="10">D95+C96</f>
+      <c r="D97" s="4">
+        <f t="shared" ref="D97:D102" si="10">D96+C97</f>
         <v>10790</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B97" s="4" t="s">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B98" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C97" s="5">
+      <c r="C98" s="5">
         <v>-10000</v>
       </c>
-      <c r="D97" s="4">
+      <c r="D98" s="4">
         <f t="shared" si="10"/>
         <v>790</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="17" t="s">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="B98" s="4" t="s">
+      <c r="B99" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C98" s="5">
+      <c r="C99" s="5">
         <v>800</v>
       </c>
-      <c r="D98" s="4">
+      <c r="D99" s="4">
         <f t="shared" si="10"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="17" t="s">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="B99" s="4" t="s">
+      <c r="B100" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C99" s="5">
+      <c r="C100" s="5">
         <v>5000</v>
       </c>
-      <c r="D99" s="4">
+      <c r="D100" s="4">
         <f t="shared" si="10"/>
         <v>6590</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="17" t="s">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="B100" s="4" t="s">
+      <c r="B101" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C100" s="5">
+      <c r="C101" s="5">
         <v>6000</v>
       </c>
-      <c r="D100" s="4">
+      <c r="D101" s="4">
         <f t="shared" si="10"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B101" s="4" t="s">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B102" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C101" s="5">
+      <c r="C102" s="5">
         <v>-10000</v>
       </c>
-      <c r="D101" s="4">
+      <c r="D102" s="4">
         <f t="shared" si="10"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="17" t="s">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="B102" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C102" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D102" s="4">
-        <f t="shared" ref="D102:D108" si="11">D101+C102</f>
-        <v>4590</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B103" s="4" t="s">
         <v>65</v>
       </c>
@@ -2555,926 +2555,926 @@
         <v>2000</v>
       </c>
       <c r="D103" s="4">
+        <f t="shared" ref="D103:D109" si="11">D102+C103</f>
+        <v>4590</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B104" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C104" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D104" s="4">
         <f t="shared" si="11"/>
         <v>6590</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B104" s="4" t="s">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B105" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C104" s="5">
+      <c r="C105" s="5">
         <v>7000</v>
       </c>
-      <c r="D104" s="4">
+      <c r="D105" s="4">
         <f t="shared" si="11"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B105" s="4" t="s">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B106" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C105" s="5">
+      <c r="C106" s="5">
         <v>-10000</v>
       </c>
-      <c r="D105" s="4">
+      <c r="D106" s="4">
         <f t="shared" si="11"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="17" t="s">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="B106" s="4" t="s">
+      <c r="B107" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C106" s="5">
+      <c r="C107" s="5">
         <v>2000</v>
       </c>
-      <c r="D106" s="4">
+      <c r="D107" s="4">
         <f t="shared" si="11"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="17" t="s">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="B107" s="4" t="s">
+      <c r="B108" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C107" s="5">
+      <c r="C108" s="5">
         <v>6000</v>
       </c>
-      <c r="D107" s="4">
+      <c r="D108" s="4">
         <f t="shared" si="11"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B108" s="4" t="s">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B109" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C108" s="5">
+      <c r="C109" s="5">
         <v>-10000</v>
       </c>
-      <c r="D108" s="4">
+      <c r="D109" s="4">
         <f t="shared" si="11"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="B109" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C109" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D109" s="4">
-        <f t="shared" ref="D109:D114" si="12">D108+C109</f>
-        <v>3590</v>
-      </c>
-    </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="B110" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C110" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D110" s="4">
+        <f t="shared" ref="D110:D115" si="12">D109+C110</f>
+        <v>3590</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="B110" s="4" t="s">
+      <c r="B111" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C110" s="5">
+      <c r="C111" s="5">
         <v>7000</v>
       </c>
-      <c r="D110" s="4">
+      <c r="D111" s="4">
         <f t="shared" si="12"/>
         <v>10590</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B111" s="4" t="s">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B112" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C111" s="5">
+      <c r="C112" s="5">
         <v>-10000</v>
       </c>
-      <c r="D111" s="4">
+      <c r="D112" s="4">
         <f t="shared" si="12"/>
         <v>590</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B112" s="4" t="s">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B113" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C112" s="5">
+      <c r="C113" s="5">
         <v>12000</v>
       </c>
-      <c r="D112" s="4">
+      <c r="D113" s="4">
         <f t="shared" si="12"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B113" s="4" t="s">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B114" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C113" s="5">
+      <c r="C114" s="5">
         <v>-10000</v>
       </c>
-      <c r="D113" s="4">
+      <c r="D114" s="4">
         <f t="shared" si="12"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B114" s="4" t="s">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B115" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C114" s="5">
+      <c r="C115" s="5">
         <v>2000</v>
       </c>
-      <c r="D114" s="4">
+      <c r="D115" s="4">
         <f t="shared" si="12"/>
         <v>4590</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="B115" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C115" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D115" s="4">
-        <f t="shared" ref="D115:D120" si="13">D114+C115</f>
-        <v>6590</v>
-      </c>
-    </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="B116" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C116" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D116" s="4">
+        <f t="shared" ref="D116:D121" si="13">D115+C116</f>
+        <v>6590</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="B116" s="4" t="s">
+      <c r="B117" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C116" s="5">
+      <c r="C117" s="5">
         <v>7000</v>
       </c>
-      <c r="D116" s="4">
+      <c r="D117" s="4">
         <f t="shared" si="13"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B117" s="4" t="s">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B118" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C117" s="5">
+      <c r="C118" s="5">
         <v>-10000</v>
       </c>
-      <c r="D117" s="4">
+      <c r="D118" s="4">
         <f t="shared" si="13"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="17" t="s">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="B118" s="4" t="s">
+      <c r="B119" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C118" s="5">
+      <c r="C119" s="5">
         <v>2000</v>
       </c>
-      <c r="D118" s="4">
+      <c r="D119" s="4">
         <f t="shared" si="13"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="17" t="s">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="B119" s="4" t="s">
+      <c r="B120" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C119" s="5">
+      <c r="C120" s="5">
         <v>8000</v>
       </c>
-      <c r="D119" s="4">
+      <c r="D120" s="4">
         <f t="shared" si="13"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B120" s="4" t="s">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B121" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C120" s="5">
+      <c r="C121" s="5">
         <v>-10000</v>
       </c>
-      <c r="D120" s="4">
+      <c r="D121" s="4">
         <f t="shared" si="13"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="17" t="s">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="B121" s="4" t="s">
+      <c r="B122" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C121" s="5">
+      <c r="C122" s="5">
         <v>2000</v>
       </c>
-      <c r="D121" s="4">
-        <f t="shared" ref="D121:D126" si="14">D120+C121</f>
+      <c r="D122" s="4">
+        <f t="shared" ref="D122:D127" si="14">D121+C122</f>
         <v>5590</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B122" s="4" t="s">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B123" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C122" s="5">
+      <c r="C123" s="5">
         <v>5000</v>
       </c>
-      <c r="D122" s="4">
+      <c r="D123" s="4">
         <f t="shared" si="14"/>
         <v>10590</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B123" s="4" t="s">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B124" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C123" s="5">
+      <c r="C124" s="5">
         <v>-10000</v>
       </c>
-      <c r="D123" s="4">
+      <c r="D124" s="4">
         <f t="shared" si="14"/>
         <v>590</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B124" s="4" t="s">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B125" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C124" s="5">
+      <c r="C125" s="5">
         <v>2000</v>
       </c>
-      <c r="D124" s="4">
+      <c r="D125" s="4">
         <f t="shared" si="14"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B125" s="4" t="s">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B126" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C125" s="5">
+      <c r="C126" s="5">
         <v>9000</v>
       </c>
-      <c r="D125" s="4">
+      <c r="D126" s="4">
         <f t="shared" si="14"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B126" s="4" t="s">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B127" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C126" s="5">
+      <c r="C127" s="5">
         <v>-10000</v>
       </c>
-      <c r="D126" s="4">
+      <c r="D127" s="4">
         <f t="shared" si="14"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="B127" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C127" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D127" s="4">
-        <f t="shared" ref="D127:D132" si="15">D126+C127</f>
-        <v>3590</v>
-      </c>
-    </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="B128" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C128" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D128" s="4">
+        <f t="shared" ref="D128:D133" si="15">D127+C128</f>
+        <v>3590</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="B128" s="4" t="s">
+      <c r="B129" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C128" s="5">
+      <c r="C129" s="5">
         <v>8000</v>
       </c>
-      <c r="D128" s="4">
+      <c r="D129" s="4">
         <f t="shared" si="15"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B129" s="4" t="s">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B130" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C129" s="5">
+      <c r="C130" s="5">
         <v>-10000</v>
       </c>
-      <c r="D129" s="4">
+      <c r="D130" s="4">
         <f t="shared" si="15"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="17" t="s">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="B130" s="4" t="s">
+      <c r="B131" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C130" s="5">
+      <c r="C131" s="5">
         <v>2000</v>
       </c>
-      <c r="D130" s="4">
+      <c r="D131" s="4">
         <f t="shared" si="15"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="17" t="s">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="B131" s="4" t="s">
+      <c r="B132" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="C131" s="5">
+      <c r="C132" s="5">
         <v>12000</v>
       </c>
-      <c r="D131" s="4">
+      <c r="D132" s="4">
         <f t="shared" si="15"/>
         <v>15590</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B132" s="4" t="s">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B133" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C132" s="5">
+      <c r="C133" s="5">
         <v>-10000</v>
       </c>
-      <c r="D132" s="4">
+      <c r="D133" s="4">
         <f t="shared" si="15"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="17" t="s">
-        <v>168</v>
-      </c>
-      <c r="B133" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="C133" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D133" s="4">
-        <f t="shared" ref="D133:D138" si="16">D132+C133</f>
-        <v>7590</v>
-      </c>
-    </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="B134" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C134" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D134" s="4">
+        <f t="shared" ref="D134:D139" si="16">D133+C134</f>
+        <v>7590</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="B134" s="4" t="s">
+      <c r="B135" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="C134" s="5">
+      <c r="C135" s="5">
         <v>10000</v>
       </c>
-      <c r="D134" s="4">
+      <c r="D135" s="4">
         <f t="shared" si="16"/>
         <v>17590</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B135" s="4" t="s">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B136" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C135" s="5">
+      <c r="C136" s="5">
         <v>-10000</v>
       </c>
-      <c r="D135" s="4">
+      <c r="D136" s="4">
         <f t="shared" si="16"/>
         <v>7590</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B136" s="4" t="s">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B137" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="C136" s="5">
+      <c r="C137" s="5">
         <v>2000</v>
       </c>
-      <c r="D136" s="4">
+      <c r="D137" s="4">
         <f t="shared" si="16"/>
         <v>9590</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="17" t="s">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="B137" s="4" t="s">
+      <c r="B138" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="C137" s="5">
+      <c r="C138" s="5">
         <v>-1200</v>
       </c>
-      <c r="D137" s="4">
+      <c r="D138" s="4">
         <f t="shared" si="16"/>
         <v>8390</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B138" s="4" t="s">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B139" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="C138" s="5">
+      <c r="C139" s="5">
         <v>500</v>
       </c>
-      <c r="D138" s="4">
+      <c r="D139" s="4">
         <f t="shared" si="16"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="B139" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C139" s="5">
-        <v>750</v>
-      </c>
-      <c r="D139" s="4">
-        <f t="shared" ref="D139:D144" si="17">D138+C139</f>
-        <v>9640</v>
-      </c>
-    </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="B140" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C140" s="5">
+        <v>750</v>
+      </c>
+      <c r="D140" s="4">
+        <f t="shared" ref="D140:D145" si="17">D139+C140</f>
+        <v>9640</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="B140" s="4" t="s">
+      <c r="B141" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C140" s="5">
+      <c r="C141" s="5">
         <v>2000</v>
       </c>
-      <c r="D140" s="4">
+      <c r="D141" s="4">
         <f t="shared" si="17"/>
         <v>11640</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B141" s="4" t="s">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B142" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C141" s="5">
+      <c r="C142" s="5">
         <v>2000</v>
       </c>
-      <c r="D141" s="4">
+      <c r="D142" s="4">
         <f t="shared" si="17"/>
         <v>13640</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B142" s="4" t="s">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B143" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C142" s="5">
+      <c r="C143" s="5">
         <v>-10000</v>
       </c>
-      <c r="D142" s="4">
+      <c r="D143" s="4">
         <f t="shared" si="17"/>
         <v>3640</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B143" s="4" t="s">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B144" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="C143" s="5">
+      <c r="C144" s="5">
         <v>350</v>
       </c>
-      <c r="D143" s="4">
+      <c r="D144" s="4">
         <f t="shared" si="17"/>
         <v>3990</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="17" t="s">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="B144" s="4" t="s">
+      <c r="B145" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="C144" s="5">
+      <c r="C145" s="5">
         <v>300</v>
       </c>
-      <c r="D144" s="4">
+      <c r="D145" s="4">
         <f t="shared" si="17"/>
         <v>4290</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="17" t="s">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="B145" s="4" t="s">
+      <c r="B146" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="C145" s="5">
+      <c r="C146" s="5">
         <v>3800</v>
       </c>
-      <c r="D145" s="4">
-        <f t="shared" ref="D145:D151" si="18">D144+C145</f>
+      <c r="D146" s="4">
+        <f t="shared" ref="D146:D152" si="18">D145+C146</f>
         <v>8090</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B146" s="4" t="s">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B147" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C146" s="5">
+      <c r="C147" s="5">
         <v>500</v>
       </c>
-      <c r="D146" s="4">
+      <c r="D147" s="4">
         <f t="shared" si="18"/>
         <v>8590</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="17" t="s">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" s="17" t="s">
         <v>182</v>
       </c>
-      <c r="B147" s="4" t="s">
+      <c r="B148" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="C147" s="5">
+      <c r="C148" s="5">
         <v>1300</v>
       </c>
-      <c r="D147" s="4">
+      <c r="D148" s="4">
         <f t="shared" si="18"/>
         <v>9890</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="17" t="s">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" s="17" t="s">
         <v>184</v>
       </c>
-      <c r="B148" s="4" t="s">
+      <c r="B149" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C148" s="5">
+      <c r="C149" s="5">
         <v>9000</v>
       </c>
-      <c r="D148" s="4">
+      <c r="D149" s="4">
         <f t="shared" si="18"/>
         <v>18890</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B149" s="4" t="s">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B150" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C149" s="5">
+      <c r="C150" s="5">
         <v>-10000</v>
       </c>
-      <c r="D149" s="4">
+      <c r="D150" s="4">
         <f t="shared" si="18"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="17" t="s">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" s="17" t="s">
         <v>185</v>
       </c>
-      <c r="B150" s="4" t="s">
+      <c r="B151" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C150" s="5">
+      <c r="C151" s="5">
         <v>2000</v>
       </c>
-      <c r="D150" s="4">
+      <c r="D151" s="4">
         <f t="shared" si="18"/>
         <v>10890</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B151" s="4" t="s">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B152" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C151" s="5">
+      <c r="C152" s="5">
         <v>-10000</v>
       </c>
-      <c r="D151" s="4">
+      <c r="D152" s="4">
         <f t="shared" si="18"/>
         <v>890</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="B152" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="C152" s="5">
-        <v>500</v>
-      </c>
-      <c r="D152" s="4">
-        <f t="shared" ref="D152:D157" si="19">D151+C152</f>
-        <v>1390</v>
-      </c>
-    </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="B153" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C153" s="5">
+        <v>500</v>
+      </c>
+      <c r="D153" s="4">
+        <f t="shared" ref="D153:D158" si="19">D152+C153</f>
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="B153" s="4" t="s">
+      <c r="B154" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="C153" s="5">
+      <c r="C154" s="5">
         <v>10000</v>
       </c>
-      <c r="D153" s="4">
+      <c r="D154" s="4">
         <f t="shared" si="19"/>
         <v>11390</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B154" s="4" t="s">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B155" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C154" s="5">
+      <c r="C155" s="5">
         <v>-10000</v>
       </c>
-      <c r="D154" s="4">
+      <c r="D155" s="4">
         <f t="shared" si="19"/>
         <v>1390</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="17" t="s">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="B155" s="4" t="s">
+      <c r="B156" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C155" s="5">
+      <c r="C156" s="5">
         <v>3000</v>
       </c>
-      <c r="D155" s="4">
+      <c r="D156" s="4">
         <f t="shared" si="19"/>
         <v>4390</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="17" t="s">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="B156" s="4" t="s">
+      <c r="B157" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C156" s="5">
+      <c r="C157" s="5">
         <v>2000</v>
       </c>
-      <c r="D156" s="4">
+      <c r="D157" s="4">
         <f t="shared" si="19"/>
         <v>6390</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B157" s="4" t="s">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B158" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C157" s="5">
+      <c r="C158" s="5">
         <v>2000</v>
       </c>
-      <c r="D157" s="4">
+      <c r="D158" s="4">
         <f t="shared" si="19"/>
         <v>8390</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="17" t="s">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="B158" s="4" t="s">
+      <c r="B159" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="C158" s="5">
+      <c r="C159" s="5">
         <v>11000</v>
       </c>
-      <c r="D158" s="4">
-        <f t="shared" ref="D158:D163" si="20">D157+C158</f>
+      <c r="D159" s="4">
+        <f t="shared" ref="D159:D164" si="20">D158+C159</f>
         <v>19390</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B159" s="4" t="s">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B160" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C159" s="5">
+      <c r="C160" s="5">
         <v>-10000</v>
       </c>
-      <c r="D159" s="4">
+      <c r="D160" s="4">
         <f t="shared" si="20"/>
         <v>9390</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="17" t="s">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="B160" s="4" t="s">
+      <c r="B161" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="C160" s="5">
+      <c r="C161" s="5">
         <v>3000</v>
       </c>
-      <c r="D160" s="4">
+      <c r="D161" s="4">
         <f t="shared" si="20"/>
         <v>12390</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B161" s="4" t="s">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B162" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C161" s="5">
+      <c r="C162" s="5">
         <v>-10000</v>
       </c>
-      <c r="D161" s="4">
+      <c r="D162" s="4">
         <f t="shared" si="20"/>
         <v>2390</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B162" s="4" t="s">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B163" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C162" s="5">
+      <c r="C163" s="5">
         <v>500</v>
       </c>
-      <c r="D162" s="4">
+      <c r="D163" s="4">
         <f t="shared" si="20"/>
         <v>2890</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163" s="17" t="s">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="B163" s="4" t="s">
+      <c r="B164" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="C163" s="5">
+      <c r="C164" s="5">
         <v>5600</v>
       </c>
-      <c r="D163" s="4">
+      <c r="D164" s="4">
         <f t="shared" si="20"/>
         <v>8490</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B164" s="4" t="s">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B165" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C164" s="5">
+      <c r="C165" s="5">
         <v>4700</v>
       </c>
-      <c r="D164" s="4">
-        <f t="shared" ref="D164:D170" si="21">D163+C164</f>
+      <c r="D165" s="4">
+        <f t="shared" ref="D165:D171" si="21">D164+C165</f>
         <v>13190</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" s="17" t="s">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="B165" s="4" t="s">
+      <c r="B166" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C165" s="5">
+      <c r="C166" s="5">
         <v>1500</v>
       </c>
-      <c r="D165" s="4">
+      <c r="D166" s="4">
         <f t="shared" si="21"/>
         <v>14690</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B166" s="4" t="s">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B167" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C166" s="5">
+      <c r="C167" s="5">
         <v>500</v>
       </c>
-      <c r="D166" s="4">
+      <c r="D167" s="4">
         <f t="shared" si="21"/>
         <v>15190</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A167" s="17" t="s">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" s="17" t="s">
         <v>200</v>
       </c>
-      <c r="B167" s="4" t="s">
+      <c r="B168" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="C167" s="5">
+      <c r="C168" s="5">
         <v>1000</v>
       </c>
-      <c r="D167" s="4">
+      <c r="D168" s="4">
         <f t="shared" si="21"/>
         <v>16190</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A168" s="17" t="s">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="B168" s="4" t="s">
+      <c r="B169" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="C168" s="5">
+      <c r="C169" s="5">
         <v>1000</v>
       </c>
-      <c r="D168" s="4">
+      <c r="D169" s="4">
         <f t="shared" si="21"/>
         <v>17190</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A169" s="17" t="s">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" s="17" t="s">
         <v>204</v>
       </c>
-      <c r="B169" s="4" t="s">
+      <c r="B170" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C169" s="5">
+      <c r="C170" s="5">
         <v>3000</v>
       </c>
-      <c r="D169" s="4">
+      <c r="D170" s="4">
         <f t="shared" si="21"/>
         <v>20190</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B170" s="4" t="s">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B171" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="C170" s="5">
+      <c r="C171" s="5">
         <v>-20000</v>
       </c>
-      <c r="D170" s="4">
+      <c r="D171" s="4">
         <f t="shared" si="21"/>
         <v>190</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B171" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C171" s="5">
-        <v>500</v>
-      </c>
-      <c r="D171" s="4">
-        <f>D170+C171</f>
-        <v>690</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -3486,49 +3486,88 @@
       </c>
       <c r="D172" s="4">
         <f>D171+C172</f>
-        <v>1190</v>
+        <v>690</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173" s="17" t="s">
-        <v>207</v>
-      </c>
       <c r="B173" s="4" t="s">
-        <v>208</v>
+        <v>76</v>
       </c>
       <c r="C173" s="5">
-        <v>10000</v>
+        <v>500</v>
       </c>
       <c r="D173" s="4">
         <f>D172+C173</f>
-        <v>11190</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174" s="17" t="s">
+        <v>207</v>
+      </c>
       <c r="B174" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C174" s="5">
-        <v>-10000</v>
+        <v>10000</v>
       </c>
       <c r="D174" s="4">
         <f>D173+C174</f>
-        <v>1190</v>
+        <v>11190</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A175" s="17" t="s">
-        <v>211</v>
-      </c>
       <c r="B175" s="4" t="s">
-        <v>28</v>
+        <v>209</v>
       </c>
       <c r="C175" s="5">
-        <v>3000</v>
+        <v>-10000</v>
       </c>
       <c r="D175" s="4">
         <f>D174+C175</f>
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="B176" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C176" s="5">
+        <v>3000</v>
+      </c>
+      <c r="D176" s="4">
+        <f>D175+C176</f>
         <v>4190</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="B177" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C177" s="5">
+        <v>11000</v>
+      </c>
+      <c r="D177" s="4">
+        <f>D176+C177</f>
+        <v>15190</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B178" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C178" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D178" s="4">
+        <f>D177+C178</f>
+        <v>5190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Duy lay 3tr tien loi co diem ngay 31
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="214">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -658,6 +658,9 @@
   </si>
   <si>
     <t>30/08/2024</t>
+  </si>
+  <si>
+    <t>31/08/2024</t>
   </si>
 </sst>
 </file>
@@ -1136,11 +1139,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K178"/>
+  <dimension ref="A1:K179"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I32" sqref="I32"/>
+      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D180" sqref="D180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3485,7 +3488,7 @@
         <v>500</v>
       </c>
       <c r="D172" s="4">
-        <f>D171+C172</f>
+        <f t="shared" ref="D172:D178" si="22">D171+C172</f>
         <v>690</v>
       </c>
     </row>
@@ -3497,7 +3500,7 @@
         <v>500</v>
       </c>
       <c r="D173" s="4">
-        <f>D172+C173</f>
+        <f t="shared" si="22"/>
         <v>1190</v>
       </c>
     </row>
@@ -3512,7 +3515,7 @@
         <v>10000</v>
       </c>
       <c r="D174" s="4">
-        <f>D173+C174</f>
+        <f t="shared" si="22"/>
         <v>11190</v>
       </c>
     </row>
@@ -3524,7 +3527,7 @@
         <v>-10000</v>
       </c>
       <c r="D175" s="4">
-        <f>D174+C175</f>
+        <f t="shared" si="22"/>
         <v>1190</v>
       </c>
     </row>
@@ -3539,7 +3542,7 @@
         <v>3000</v>
       </c>
       <c r="D176" s="4">
-        <f>D175+C176</f>
+        <f t="shared" si="22"/>
         <v>4190</v>
       </c>
     </row>
@@ -3554,7 +3557,7 @@
         <v>11000</v>
       </c>
       <c r="D177" s="4">
-        <f>D176+C177</f>
+        <f t="shared" si="22"/>
         <v>15190</v>
       </c>
     </row>
@@ -3566,8 +3569,23 @@
         <v>-10000</v>
       </c>
       <c r="D178" s="4">
-        <f>D177+C178</f>
+        <f t="shared" si="22"/>
         <v>5190</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A179" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="B179" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C179" s="5">
+        <v>3000</v>
+      </c>
+      <c r="D179" s="4">
+        <f>D178+C179</f>
+        <v>8190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Duy lay tien loi ngay 01,02 co diem
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="217">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -661,6 +661,15 @@
   </si>
   <si>
     <t>31/08/2024</t>
+  </si>
+  <si>
+    <t>03/08/2024</t>
+  </si>
+  <si>
+    <t>Duy lấy 14tr tiền lời</t>
+  </si>
+  <si>
+    <t>Duy cho cô diễm vay 20tr</t>
   </si>
 </sst>
 </file>
@@ -1139,11 +1148,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K179"/>
+  <dimension ref="A1:K182"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D180" sqref="D180"/>
+      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1219,8 +1228,8 @@
         <v>20</v>
       </c>
       <c r="J3" s="4">
-        <f>SUM(I3:I62)</f>
-        <v>490</v>
+        <f>SUM(I3:I63)</f>
+        <v>510</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1798,7 +1807,7 @@
         <v>7640</v>
       </c>
       <c r="D47" s="4">
-        <f t="shared" ref="D47:D52" si="2">D46+C47</f>
+        <f t="shared" ref="D47:D53" si="2">D46+C47</f>
         <v>9090</v>
       </c>
       <c r="H47" s="17" t="s">
@@ -1809,358 +1818,351 @@
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B48" s="4" t="s">
+      <c r="H48" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="I48" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B49" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C48" s="5">
+      <c r="C49" s="5">
         <v>3000</v>
       </c>
-      <c r="D48" s="4">
-        <f t="shared" si="2"/>
+      <c r="D49" s="4">
+        <f>D47+C49</f>
         <v>12090</v>
       </c>
-      <c r="H48" s="17" t="s">
+      <c r="H49" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="I48" s="5">
+      <c r="I49" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B49" s="4" t="s">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B50" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C49" s="5">
+      <c r="C50" s="5">
         <v>-10000</v>
       </c>
-      <c r="D49" s="4">
+      <c r="D50" s="4">
         <f t="shared" si="2"/>
         <v>2090</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B50" s="4" t="s">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B51" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C50" s="5">
+      <c r="C51" s="5">
         <v>800</v>
       </c>
-      <c r="D50" s="4">
+      <c r="D51" s="4">
         <f t="shared" si="2"/>
         <v>2890</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="17" t="s">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B52" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C51" s="5">
+      <c r="C52" s="5">
         <v>2000</v>
       </c>
-      <c r="D51" s="4">
+      <c r="D52" s="4">
         <f t="shared" si="2"/>
         <v>4890</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="17" t="s">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B53" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C52" s="5">
+      <c r="C53" s="5">
         <v>4000</v>
       </c>
-      <c r="D52" s="4">
+      <c r="D53" s="4">
         <f t="shared" si="2"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="17" t="s">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B54" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C53" s="5">
+      <c r="C54" s="5">
         <v>4000</v>
       </c>
-      <c r="D53" s="4">
-        <f t="shared" ref="D53:D58" si="3">D52+C53</f>
+      <c r="D54" s="4">
+        <f t="shared" ref="D54:D59" si="3">D53+C54</f>
         <v>12890</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B54" s="4" t="s">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B55" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C54" s="5">
+      <c r="C55" s="5">
         <v>5000</v>
       </c>
-      <c r="D54" s="4">
+      <c r="D55" s="4">
         <f t="shared" si="3"/>
         <v>17890</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="4" t="s">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B56" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C55" s="5">
+      <c r="C56" s="5">
         <v>-10000</v>
       </c>
-      <c r="D55" s="4">
+      <c r="D56" s="4">
         <f t="shared" si="3"/>
         <v>7890</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="17">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="17">
         <v>44969</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B57" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C56" s="5">
+      <c r="C57" s="5">
         <v>900</v>
       </c>
-      <c r="D56" s="4">
+      <c r="D57" s="4">
         <f t="shared" si="3"/>
         <v>8790</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B57" s="4" t="s">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B58" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C57" s="5">
+      <c r="C58" s="5">
         <v>4000</v>
       </c>
-      <c r="D57" s="4">
+      <c r="D58" s="4">
         <f t="shared" si="3"/>
         <v>12790</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B58" s="4" t="s">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B59" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C58" s="5">
+      <c r="C59" s="5">
         <v>-10000</v>
       </c>
-      <c r="D58" s="4">
+      <c r="D59" s="4">
         <f t="shared" si="3"/>
         <v>2790</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="17" t="s">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B60" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C59" s="5">
+      <c r="C60" s="5">
         <v>2000</v>
       </c>
-      <c r="D59" s="4">
-        <f t="shared" ref="D59:D66" si="4">D58+C59</f>
+      <c r="D60" s="4">
+        <f t="shared" ref="D60:D67" si="4">D59+C60</f>
         <v>4790</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="17" t="s">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B61" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C60" s="5">
+      <c r="C61" s="5">
         <v>700</v>
       </c>
-      <c r="D60" s="4">
+      <c r="D61" s="4">
         <f t="shared" si="4"/>
         <v>5490</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B61" s="4" t="s">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B62" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C61" s="5">
+      <c r="C62" s="5">
         <v>4000</v>
       </c>
-      <c r="D61" s="4">
+      <c r="D62" s="4">
         <f t="shared" si="4"/>
         <v>9490</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="17" t="s">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B63" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C62" s="5">
+      <c r="C63" s="5">
         <v>600</v>
       </c>
-      <c r="D62" s="4">
+      <c r="D63" s="4">
         <f t="shared" si="4"/>
         <v>10090</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B63" s="4" t="s">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B64" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C63" s="5">
+      <c r="C64" s="5">
         <v>-10000</v>
       </c>
-      <c r="D63" s="4">
+      <c r="D64" s="4">
         <f t="shared" si="4"/>
         <v>90</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="17" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B65" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C64" s="5">
+      <c r="C65" s="5">
         <f>700+5000+300+600+400+1000+800</f>
         <v>8800</v>
       </c>
-      <c r="D64" s="4">
+      <c r="D65" s="4">
         <f t="shared" si="4"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B65" s="4" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C65" s="5">
+      <c r="C66" s="5">
         <v>6000</v>
       </c>
-      <c r="D65" s="4">
+      <c r="D66" s="4">
         <f t="shared" si="4"/>
         <v>14890</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B66" s="4" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B67" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C66" s="5">
+      <c r="C67" s="5">
         <v>-10000</v>
       </c>
-      <c r="D66" s="4">
+      <c r="D67" s="4">
         <f t="shared" si="4"/>
         <v>4890</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="17" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B68" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C67" s="5">
+      <c r="C68" s="5">
         <v>500</v>
       </c>
-      <c r="D67" s="4">
-        <f t="shared" ref="D67:D72" si="5">D66+C67</f>
+      <c r="D68" s="4">
+        <f t="shared" ref="D68:D73" si="5">D67+C68</f>
         <v>5390</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B68" s="4" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B69" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C68" s="5">
+      <c r="C69" s="5">
         <v>700</v>
       </c>
-      <c r="D68" s="4">
+      <c r="D69" s="4">
         <f t="shared" si="5"/>
         <v>6090</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B69" s="4" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B70" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C69" s="5">
+      <c r="C70" s="5">
         <v>1500</v>
       </c>
-      <c r="D69" s="4">
+      <c r="D70" s="4">
         <f t="shared" si="5"/>
         <v>7590</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B70" s="4" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B71" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C70" s="5">
+      <c r="C71" s="5">
         <v>5000</v>
       </c>
-      <c r="D70" s="4">
+      <c r="D71" s="4">
         <f t="shared" si="5"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B71" s="4" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B72" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C71" s="5">
+      <c r="C72" s="5">
         <v>-10000</v>
       </c>
-      <c r="D71" s="4">
+      <c r="D72" s="4">
         <f t="shared" si="5"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="17" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B73" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C72" s="5">
+      <c r="C73" s="5">
         <v>2000</v>
       </c>
-      <c r="D72" s="4">
+      <c r="D73" s="4">
         <f t="shared" si="5"/>
         <v>4590</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B73" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C73" s="5">
-        <v>700</v>
-      </c>
-      <c r="D73" s="4">
-        <f t="shared" ref="D73:D78" si="6">D72+C73</f>
-        <v>5290</v>
-      </c>
-    </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="17" t="s">
-        <v>82</v>
-      </c>
       <c r="B74" s="4" t="s">
         <v>77</v>
       </c>
@@ -2168,401 +2170,404 @@
         <v>700</v>
       </c>
       <c r="D74" s="4">
+        <f t="shared" ref="D74:D79" si="6">D73+C74</f>
+        <v>5290</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C75" s="5">
+        <v>700</v>
+      </c>
+      <c r="D75" s="4">
         <f t="shared" si="6"/>
         <v>5990</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="17" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="B76" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C75" s="5">
+      <c r="C76" s="5">
         <v>700</v>
       </c>
-      <c r="D75" s="4">
+      <c r="D76" s="4">
         <f t="shared" si="6"/>
         <v>6690</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="17" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B77" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C76" s="5">
+      <c r="C77" s="5">
         <v>4000</v>
       </c>
-      <c r="D76" s="4">
+      <c r="D77" s="4">
         <f t="shared" si="6"/>
         <v>10690</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B77" s="4" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B78" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C77" s="5">
+      <c r="C78" s="5">
         <v>-10000</v>
       </c>
-      <c r="D77" s="4">
+      <c r="D78" s="4">
         <f t="shared" si="6"/>
         <v>690</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="17" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B79" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C78" s="5">
+      <c r="C79" s="5">
         <v>1000</v>
       </c>
-      <c r="D78" s="4">
+      <c r="D79" s="4">
         <f t="shared" si="6"/>
         <v>1690</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="17" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="B79" s="4" t="s">
+      <c r="B80" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C79" s="5">
+      <c r="C80" s="5">
         <v>7000</v>
       </c>
-      <c r="D79" s="4">
-        <f t="shared" ref="D79:D84" si="7">D78+C79</f>
+      <c r="D80" s="4">
+        <f t="shared" ref="D80:D85" si="7">D79+C80</f>
         <v>8690</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B80" s="4" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B81" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C80" s="5">
+      <c r="C81" s="5">
         <v>10000</v>
       </c>
-      <c r="D80" s="4">
+      <c r="D81" s="4">
         <f t="shared" si="7"/>
         <v>18690</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B81" s="4" t="s">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B82" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C81" s="5">
+      <c r="C82" s="5">
         <v>-10000</v>
       </c>
-      <c r="D81" s="4">
+      <c r="D82" s="4">
         <f t="shared" si="7"/>
         <v>8690</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B82" s="4" t="s">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B83" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C82" s="5">
+      <c r="C83" s="5">
         <v>1700</v>
       </c>
-      <c r="D82" s="4">
+      <c r="D83" s="4">
         <f t="shared" si="7"/>
         <v>10390</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B83" s="4" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B84" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C83" s="5">
+      <c r="C84" s="5">
         <v>-10000</v>
       </c>
-      <c r="D83" s="4">
+      <c r="D84" s="4">
         <f t="shared" si="7"/>
         <v>390</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B84" s="4" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B85" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C84" s="5">
+      <c r="C85" s="5">
         <v>6000</v>
       </c>
-      <c r="D84" s="4">
+      <c r="D85" s="4">
         <f t="shared" si="7"/>
         <v>6390</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="B85" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C85" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D85" s="4">
-        <f t="shared" ref="D85:D90" si="8">D84+C85</f>
-        <v>8390</v>
-      </c>
-    </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C86" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D86" s="4">
+        <f t="shared" ref="D86:D91" si="8">D85+C86</f>
+        <v>8390</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="B87" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C86" s="5">
+      <c r="C87" s="5">
         <v>5000</v>
       </c>
-      <c r="D86" s="4">
+      <c r="D87" s="4">
         <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B87" s="4" t="s">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B88" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C87" s="5">
+      <c r="C88" s="5">
         <v>-10000</v>
       </c>
-      <c r="D87" s="4">
+      <c r="D88" s="4">
         <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="17" t="s">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="B88" s="4" t="s">
+      <c r="B89" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C88" s="5">
+      <c r="C89" s="5">
         <v>1000</v>
       </c>
-      <c r="D88" s="4">
+      <c r="D89" s="4">
         <f t="shared" si="8"/>
         <v>4390</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B89" s="4" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B90" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C89" s="5">
+      <c r="C90" s="5">
         <v>9000</v>
       </c>
-      <c r="D89" s="4">
+      <c r="D90" s="4">
         <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B90" s="4" t="s">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B91" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C90" s="5">
+      <c r="C91" s="5">
         <v>-10000</v>
       </c>
-      <c r="D90" s="4">
+      <c r="D91" s="4">
         <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B91" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C91" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D91" s="4">
-        <f t="shared" ref="D91:D96" si="9">D90+C91</f>
-        <v>5390</v>
-      </c>
-    </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B92" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C92" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D92" s="4">
+        <f t="shared" ref="D92:D97" si="9">D91+C92</f>
+        <v>5390</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B93" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C92" s="5">
+      <c r="C93" s="5">
         <v>6000</v>
       </c>
-      <c r="D92" s="4">
+      <c r="D93" s="4">
         <f t="shared" si="9"/>
         <v>11390</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B93" s="4" t="s">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B94" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C93" s="5">
+      <c r="C94" s="5">
         <v>-10000</v>
       </c>
-      <c r="D93" s="4">
+      <c r="D94" s="4">
         <f t="shared" si="9"/>
         <v>1390</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B94" s="4" t="s">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B95" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C94" s="5">
+      <c r="C95" s="5">
         <v>400</v>
       </c>
-      <c r="D94" s="4">
+      <c r="D95" s="4">
         <f t="shared" si="9"/>
         <v>1790</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="17" t="s">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="B95" s="4" t="s">
+      <c r="B96" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C95" s="5">
+      <c r="C96" s="5">
         <v>2000</v>
       </c>
-      <c r="D95" s="4">
+      <c r="D96" s="4">
         <f t="shared" si="9"/>
         <v>3790</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="17" t="s">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="B96" s="4" t="s">
+      <c r="B97" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C96" s="5">
+      <c r="C97" s="5">
         <v>6000</v>
       </c>
-      <c r="D96" s="4">
+      <c r="D97" s="4">
         <f t="shared" si="9"/>
         <v>9790</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="17" t="s">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="B97" s="4" t="s">
+      <c r="B98" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C97" s="5">
+      <c r="C98" s="5">
         <v>1000</v>
       </c>
-      <c r="D97" s="4">
-        <f t="shared" ref="D97:D102" si="10">D96+C97</f>
+      <c r="D98" s="4">
+        <f t="shared" ref="D98:D103" si="10">D97+C98</f>
         <v>10790</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B98" s="4" t="s">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B99" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C98" s="5">
+      <c r="C99" s="5">
         <v>-10000</v>
       </c>
-      <c r="D98" s="4">
+      <c r="D99" s="4">
         <f t="shared" si="10"/>
         <v>790</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="17" t="s">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="B99" s="4" t="s">
+      <c r="B100" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C99" s="5">
+      <c r="C100" s="5">
         <v>800</v>
       </c>
-      <c r="D99" s="4">
+      <c r="D100" s="4">
         <f t="shared" si="10"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="17" t="s">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="B100" s="4" t="s">
+      <c r="B101" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C100" s="5">
+      <c r="C101" s="5">
         <v>5000</v>
       </c>
-      <c r="D100" s="4">
+      <c r="D101" s="4">
         <f t="shared" si="10"/>
         <v>6590</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="17" t="s">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="B101" s="4" t="s">
+      <c r="B102" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C101" s="5">
+      <c r="C102" s="5">
         <v>6000</v>
       </c>
-      <c r="D101" s="4">
+      <c r="D102" s="4">
         <f t="shared" si="10"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B102" s="4" t="s">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B103" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C102" s="5">
+      <c r="C103" s="5">
         <v>-10000</v>
       </c>
-      <c r="D102" s="4">
+      <c r="D103" s="4">
         <f t="shared" si="10"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="17" t="s">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="B103" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C103" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D103" s="4">
-        <f t="shared" ref="D103:D109" si="11">D102+C103</f>
-        <v>4590</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B104" s="4" t="s">
         <v>65</v>
       </c>
@@ -2570,926 +2575,926 @@
         <v>2000</v>
       </c>
       <c r="D104" s="4">
+        <f t="shared" ref="D104:D110" si="11">D103+C104</f>
+        <v>4590</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B105" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C105" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D105" s="4">
         <f t="shared" si="11"/>
         <v>6590</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B105" s="4" t="s">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B106" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C105" s="5">
+      <c r="C106" s="5">
         <v>7000</v>
       </c>
-      <c r="D105" s="4">
+      <c r="D106" s="4">
         <f t="shared" si="11"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B106" s="4" t="s">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B107" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C106" s="5">
+      <c r="C107" s="5">
         <v>-10000</v>
       </c>
-      <c r="D106" s="4">
+      <c r="D107" s="4">
         <f t="shared" si="11"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="17" t="s">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="B107" s="4" t="s">
+      <c r="B108" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C107" s="5">
+      <c r="C108" s="5">
         <v>2000</v>
       </c>
-      <c r="D107" s="4">
+      <c r="D108" s="4">
         <f t="shared" si="11"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="17" t="s">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="B108" s="4" t="s">
+      <c r="B109" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C108" s="5">
+      <c r="C109" s="5">
         <v>6000</v>
       </c>
-      <c r="D108" s="4">
+      <c r="D109" s="4">
         <f t="shared" si="11"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B109" s="4" t="s">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B110" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C109" s="5">
+      <c r="C110" s="5">
         <v>-10000</v>
       </c>
-      <c r="D109" s="4">
+      <c r="D110" s="4">
         <f t="shared" si="11"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="B110" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C110" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D110" s="4">
-        <f t="shared" ref="D110:D115" si="12">D109+C110</f>
-        <v>3590</v>
-      </c>
-    </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="B111" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C111" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D111" s="4">
+        <f t="shared" ref="D111:D116" si="12">D110+C111</f>
+        <v>3590</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="B111" s="4" t="s">
+      <c r="B112" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C111" s="5">
+      <c r="C112" s="5">
         <v>7000</v>
       </c>
-      <c r="D111" s="4">
+      <c r="D112" s="4">
         <f t="shared" si="12"/>
         <v>10590</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B112" s="4" t="s">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B113" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C112" s="5">
+      <c r="C113" s="5">
         <v>-10000</v>
       </c>
-      <c r="D112" s="4">
+      <c r="D113" s="4">
         <f t="shared" si="12"/>
         <v>590</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B113" s="4" t="s">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B114" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C113" s="5">
+      <c r="C114" s="5">
         <v>12000</v>
       </c>
-      <c r="D113" s="4">
+      <c r="D114" s="4">
         <f t="shared" si="12"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B114" s="4" t="s">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B115" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C114" s="5">
+      <c r="C115" s="5">
         <v>-10000</v>
       </c>
-      <c r="D114" s="4">
+      <c r="D115" s="4">
         <f t="shared" si="12"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B115" s="4" t="s">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B116" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C115" s="5">
+      <c r="C116" s="5">
         <v>2000</v>
       </c>
-      <c r="D115" s="4">
+      <c r="D116" s="4">
         <f t="shared" si="12"/>
         <v>4590</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="B116" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C116" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D116" s="4">
-        <f t="shared" ref="D116:D121" si="13">D115+C116</f>
-        <v>6590</v>
-      </c>
-    </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="B117" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C117" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D117" s="4">
+        <f t="shared" ref="D117:D122" si="13">D116+C117</f>
+        <v>6590</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="B117" s="4" t="s">
+      <c r="B118" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C117" s="5">
+      <c r="C118" s="5">
         <v>7000</v>
       </c>
-      <c r="D117" s="4">
+      <c r="D118" s="4">
         <f t="shared" si="13"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B118" s="4" t="s">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B119" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C118" s="5">
+      <c r="C119" s="5">
         <v>-10000</v>
       </c>
-      <c r="D118" s="4">
+      <c r="D119" s="4">
         <f t="shared" si="13"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="17" t="s">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="B119" s="4" t="s">
+      <c r="B120" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C119" s="5">
+      <c r="C120" s="5">
         <v>2000</v>
       </c>
-      <c r="D119" s="4">
+      <c r="D120" s="4">
         <f t="shared" si="13"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="17" t="s">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="B120" s="4" t="s">
+      <c r="B121" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C120" s="5">
+      <c r="C121" s="5">
         <v>8000</v>
       </c>
-      <c r="D120" s="4">
+      <c r="D121" s="4">
         <f t="shared" si="13"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B121" s="4" t="s">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B122" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C121" s="5">
+      <c r="C122" s="5">
         <v>-10000</v>
       </c>
-      <c r="D121" s="4">
+      <c r="D122" s="4">
         <f t="shared" si="13"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="17" t="s">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="B122" s="4" t="s">
+      <c r="B123" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C122" s="5">
+      <c r="C123" s="5">
         <v>2000</v>
       </c>
-      <c r="D122" s="4">
-        <f t="shared" ref="D122:D127" si="14">D121+C122</f>
+      <c r="D123" s="4">
+        <f t="shared" ref="D123:D128" si="14">D122+C123</f>
         <v>5590</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B123" s="4" t="s">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B124" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C123" s="5">
+      <c r="C124" s="5">
         <v>5000</v>
       </c>
-      <c r="D123" s="4">
+      <c r="D124" s="4">
         <f t="shared" si="14"/>
         <v>10590</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B124" s="4" t="s">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B125" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C124" s="5">
+      <c r="C125" s="5">
         <v>-10000</v>
       </c>
-      <c r="D124" s="4">
+      <c r="D125" s="4">
         <f t="shared" si="14"/>
         <v>590</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B125" s="4" t="s">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B126" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C125" s="5">
+      <c r="C126" s="5">
         <v>2000</v>
       </c>
-      <c r="D125" s="4">
+      <c r="D126" s="4">
         <f t="shared" si="14"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B126" s="4" t="s">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B127" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C126" s="5">
+      <c r="C127" s="5">
         <v>9000</v>
       </c>
-      <c r="D126" s="4">
+      <c r="D127" s="4">
         <f t="shared" si="14"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B127" s="4" t="s">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B128" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C127" s="5">
+      <c r="C128" s="5">
         <v>-10000</v>
       </c>
-      <c r="D127" s="4">
+      <c r="D128" s="4">
         <f t="shared" si="14"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="B128" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C128" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D128" s="4">
-        <f t="shared" ref="D128:D133" si="15">D127+C128</f>
-        <v>3590</v>
-      </c>
-    </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="B129" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C129" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D129" s="4">
+        <f t="shared" ref="D129:D134" si="15">D128+C129</f>
+        <v>3590</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="B129" s="4" t="s">
+      <c r="B130" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C129" s="5">
+      <c r="C130" s="5">
         <v>8000</v>
       </c>
-      <c r="D129" s="4">
+      <c r="D130" s="4">
         <f t="shared" si="15"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B130" s="4" t="s">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B131" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C130" s="5">
+      <c r="C131" s="5">
         <v>-10000</v>
       </c>
-      <c r="D130" s="4">
+      <c r="D131" s="4">
         <f t="shared" si="15"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="17" t="s">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="B131" s="4" t="s">
+      <c r="B132" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C131" s="5">
+      <c r="C132" s="5">
         <v>2000</v>
       </c>
-      <c r="D131" s="4">
+      <c r="D132" s="4">
         <f t="shared" si="15"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="17" t="s">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="B132" s="4" t="s">
+      <c r="B133" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="C132" s="5">
+      <c r="C133" s="5">
         <v>12000</v>
       </c>
-      <c r="D132" s="4">
+      <c r="D133" s="4">
         <f t="shared" si="15"/>
         <v>15590</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B133" s="4" t="s">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B134" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C133" s="5">
+      <c r="C134" s="5">
         <v>-10000</v>
       </c>
-      <c r="D133" s="4">
+      <c r="D134" s="4">
         <f t="shared" si="15"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="17" t="s">
-        <v>168</v>
-      </c>
-      <c r="B134" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="C134" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D134" s="4">
-        <f t="shared" ref="D134:D139" si="16">D133+C134</f>
-        <v>7590</v>
-      </c>
-    </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="B135" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C135" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D135" s="4">
+        <f t="shared" ref="D135:D140" si="16">D134+C135</f>
+        <v>7590</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="B135" s="4" t="s">
+      <c r="B136" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="C135" s="5">
+      <c r="C136" s="5">
         <v>10000</v>
       </c>
-      <c r="D135" s="4">
+      <c r="D136" s="4">
         <f t="shared" si="16"/>
         <v>17590</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B136" s="4" t="s">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B137" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C136" s="5">
+      <c r="C137" s="5">
         <v>-10000</v>
       </c>
-      <c r="D136" s="4">
+      <c r="D137" s="4">
         <f t="shared" si="16"/>
         <v>7590</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B137" s="4" t="s">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B138" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="C137" s="5">
+      <c r="C138" s="5">
         <v>2000</v>
       </c>
-      <c r="D137" s="4">
+      <c r="D138" s="4">
         <f t="shared" si="16"/>
         <v>9590</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="17" t="s">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="B138" s="4" t="s">
+      <c r="B139" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="C138" s="5">
+      <c r="C139" s="5">
         <v>-1200</v>
       </c>
-      <c r="D138" s="4">
+      <c r="D139" s="4">
         <f t="shared" si="16"/>
         <v>8390</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B139" s="4" t="s">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B140" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="C139" s="5">
+      <c r="C140" s="5">
         <v>500</v>
       </c>
-      <c r="D139" s="4">
+      <c r="D140" s="4">
         <f t="shared" si="16"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="B140" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C140" s="5">
-        <v>750</v>
-      </c>
-      <c r="D140" s="4">
-        <f t="shared" ref="D140:D145" si="17">D139+C140</f>
-        <v>9640</v>
-      </c>
-    </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="B141" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C141" s="5">
+        <v>750</v>
+      </c>
+      <c r="D141" s="4">
+        <f t="shared" ref="D141:D146" si="17">D140+C141</f>
+        <v>9640</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="B141" s="4" t="s">
+      <c r="B142" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C141" s="5">
+      <c r="C142" s="5">
         <v>2000</v>
       </c>
-      <c r="D141" s="4">
+      <c r="D142" s="4">
         <f t="shared" si="17"/>
         <v>11640</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B142" s="4" t="s">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B143" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C142" s="5">
+      <c r="C143" s="5">
         <v>2000</v>
       </c>
-      <c r="D142" s="4">
+      <c r="D143" s="4">
         <f t="shared" si="17"/>
         <v>13640</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B143" s="4" t="s">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B144" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C143" s="5">
+      <c r="C144" s="5">
         <v>-10000</v>
       </c>
-      <c r="D143" s="4">
+      <c r="D144" s="4">
         <f t="shared" si="17"/>
         <v>3640</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B144" s="4" t="s">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B145" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="C144" s="5">
+      <c r="C145" s="5">
         <v>350</v>
       </c>
-      <c r="D144" s="4">
+      <c r="D145" s="4">
         <f t="shared" si="17"/>
         <v>3990</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="17" t="s">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="B145" s="4" t="s">
+      <c r="B146" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="C145" s="5">
+      <c r="C146" s="5">
         <v>300</v>
       </c>
-      <c r="D145" s="4">
+      <c r="D146" s="4">
         <f t="shared" si="17"/>
         <v>4290</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="17" t="s">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="B146" s="4" t="s">
+      <c r="B147" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="C146" s="5">
+      <c r="C147" s="5">
         <v>3800</v>
       </c>
-      <c r="D146" s="4">
-        <f t="shared" ref="D146:D152" si="18">D145+C146</f>
+      <c r="D147" s="4">
+        <f t="shared" ref="D147:D153" si="18">D146+C147</f>
         <v>8090</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B147" s="4" t="s">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B148" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C147" s="5">
+      <c r="C148" s="5">
         <v>500</v>
       </c>
-      <c r="D147" s="4">
+      <c r="D148" s="4">
         <f t="shared" si="18"/>
         <v>8590</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="17" t="s">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" s="17" t="s">
         <v>182</v>
       </c>
-      <c r="B148" s="4" t="s">
+      <c r="B149" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="C148" s="5">
+      <c r="C149" s="5">
         <v>1300</v>
       </c>
-      <c r="D148" s="4">
+      <c r="D149" s="4">
         <f t="shared" si="18"/>
         <v>9890</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="17" t="s">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" s="17" t="s">
         <v>184</v>
       </c>
-      <c r="B149" s="4" t="s">
+      <c r="B150" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C149" s="5">
+      <c r="C150" s="5">
         <v>9000</v>
       </c>
-      <c r="D149" s="4">
+      <c r="D150" s="4">
         <f t="shared" si="18"/>
         <v>18890</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B150" s="4" t="s">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B151" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C150" s="5">
+      <c r="C151" s="5">
         <v>-10000</v>
       </c>
-      <c r="D150" s="4">
+      <c r="D151" s="4">
         <f t="shared" si="18"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="17" t="s">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" s="17" t="s">
         <v>185</v>
       </c>
-      <c r="B151" s="4" t="s">
+      <c r="B152" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C151" s="5">
+      <c r="C152" s="5">
         <v>2000</v>
       </c>
-      <c r="D151" s="4">
+      <c r="D152" s="4">
         <f t="shared" si="18"/>
         <v>10890</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B152" s="4" t="s">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B153" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C152" s="5">
+      <c r="C153" s="5">
         <v>-10000</v>
       </c>
-      <c r="D152" s="4">
+      <c r="D153" s="4">
         <f t="shared" si="18"/>
         <v>890</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="B153" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="C153" s="5">
-        <v>500</v>
-      </c>
-      <c r="D153" s="4">
-        <f t="shared" ref="D153:D158" si="19">D152+C153</f>
-        <v>1390</v>
-      </c>
-    </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="B154" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C154" s="5">
+        <v>500</v>
+      </c>
+      <c r="D154" s="4">
+        <f t="shared" ref="D154:D159" si="19">D153+C154</f>
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="B154" s="4" t="s">
+      <c r="B155" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="C154" s="5">
+      <c r="C155" s="5">
         <v>10000</v>
       </c>
-      <c r="D154" s="4">
+      <c r="D155" s="4">
         <f t="shared" si="19"/>
         <v>11390</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B155" s="4" t="s">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B156" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C155" s="5">
+      <c r="C156" s="5">
         <v>-10000</v>
       </c>
-      <c r="D155" s="4">
+      <c r="D156" s="4">
         <f t="shared" si="19"/>
         <v>1390</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="17" t="s">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="B156" s="4" t="s">
+      <c r="B157" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C156" s="5">
+      <c r="C157" s="5">
         <v>3000</v>
       </c>
-      <c r="D156" s="4">
+      <c r="D157" s="4">
         <f t="shared" si="19"/>
         <v>4390</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="17" t="s">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="B157" s="4" t="s">
+      <c r="B158" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C157" s="5">
+      <c r="C158" s="5">
         <v>2000</v>
       </c>
-      <c r="D157" s="4">
+      <c r="D158" s="4">
         <f t="shared" si="19"/>
         <v>6390</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B158" s="4" t="s">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B159" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C158" s="5">
+      <c r="C159" s="5">
         <v>2000</v>
       </c>
-      <c r="D158" s="4">
+      <c r="D159" s="4">
         <f t="shared" si="19"/>
         <v>8390</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="17" t="s">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="B159" s="4" t="s">
+      <c r="B160" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="C159" s="5">
+      <c r="C160" s="5">
         <v>11000</v>
       </c>
-      <c r="D159" s="4">
-        <f t="shared" ref="D159:D164" si="20">D158+C159</f>
+      <c r="D160" s="4">
+        <f t="shared" ref="D160:D165" si="20">D159+C160</f>
         <v>19390</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B160" s="4" t="s">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B161" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C160" s="5">
+      <c r="C161" s="5">
         <v>-10000</v>
       </c>
-      <c r="D160" s="4">
+      <c r="D161" s="4">
         <f t="shared" si="20"/>
         <v>9390</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" s="17" t="s">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="B161" s="4" t="s">
+      <c r="B162" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="C161" s="5">
+      <c r="C162" s="5">
         <v>3000</v>
       </c>
-      <c r="D161" s="4">
+      <c r="D162" s="4">
         <f t="shared" si="20"/>
         <v>12390</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B162" s="4" t="s">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B163" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C162" s="5">
+      <c r="C163" s="5">
         <v>-10000</v>
       </c>
-      <c r="D162" s="4">
+      <c r="D163" s="4">
         <f t="shared" si="20"/>
         <v>2390</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B163" s="4" t="s">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B164" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C163" s="5">
+      <c r="C164" s="5">
         <v>500</v>
       </c>
-      <c r="D163" s="4">
+      <c r="D164" s="4">
         <f t="shared" si="20"/>
         <v>2890</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164" s="17" t="s">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="B164" s="4" t="s">
+      <c r="B165" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="C164" s="5">
+      <c r="C165" s="5">
         <v>5600</v>
       </c>
-      <c r="D164" s="4">
+      <c r="D165" s="4">
         <f t="shared" si="20"/>
         <v>8490</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B165" s="4" t="s">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B166" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C165" s="5">
+      <c r="C166" s="5">
         <v>4700</v>
       </c>
-      <c r="D165" s="4">
-        <f t="shared" ref="D165:D171" si="21">D164+C165</f>
+      <c r="D166" s="4">
+        <f t="shared" ref="D166:D172" si="21">D165+C166</f>
         <v>13190</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A166" s="17" t="s">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="B166" s="4" t="s">
+      <c r="B167" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C166" s="5">
+      <c r="C167" s="5">
         <v>1500</v>
       </c>
-      <c r="D166" s="4">
+      <c r="D167" s="4">
         <f t="shared" si="21"/>
         <v>14690</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B167" s="4" t="s">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B168" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C167" s="5">
+      <c r="C168" s="5">
         <v>500</v>
       </c>
-      <c r="D167" s="4">
+      <c r="D168" s="4">
         <f t="shared" si="21"/>
         <v>15190</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A168" s="17" t="s">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" s="17" t="s">
         <v>200</v>
       </c>
-      <c r="B168" s="4" t="s">
+      <c r="B169" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="C168" s="5">
+      <c r="C169" s="5">
         <v>1000</v>
       </c>
-      <c r="D168" s="4">
+      <c r="D169" s="4">
         <f t="shared" si="21"/>
         <v>16190</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A169" s="17" t="s">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="B169" s="4" t="s">
+      <c r="B170" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="C169" s="5">
+      <c r="C170" s="5">
         <v>1000</v>
       </c>
-      <c r="D169" s="4">
+      <c r="D170" s="4">
         <f t="shared" si="21"/>
         <v>17190</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" s="17" t="s">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" s="17" t="s">
         <v>204</v>
       </c>
-      <c r="B170" s="4" t="s">
+      <c r="B171" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C170" s="5">
+      <c r="C171" s="5">
         <v>3000</v>
       </c>
-      <c r="D170" s="4">
+      <c r="D171" s="4">
         <f t="shared" si="21"/>
         <v>20190</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B171" s="4" t="s">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B172" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="C171" s="5">
+      <c r="C172" s="5">
         <v>-20000</v>
       </c>
-      <c r="D171" s="4">
+      <c r="D172" s="4">
         <f t="shared" si="21"/>
         <v>190</v>
-      </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B172" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C172" s="5">
-        <v>500</v>
-      </c>
-      <c r="D172" s="4">
-        <f t="shared" ref="D172:D178" si="22">D171+C172</f>
-        <v>690</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -3500,92 +3505,131 @@
         <v>500</v>
       </c>
       <c r="D173" s="4">
+        <f t="shared" ref="D173:D179" si="22">D172+C173</f>
+        <v>690</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B174" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C174" s="5">
+        <v>500</v>
+      </c>
+      <c r="D174" s="4">
         <f t="shared" si="22"/>
         <v>1190</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174" s="17" t="s">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175" s="17" t="s">
         <v>207</v>
       </c>
-      <c r="B174" s="4" t="s">
+      <c r="B175" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="C174" s="5">
+      <c r="C175" s="5">
         <v>10000</v>
       </c>
-      <c r="D174" s="4">
+      <c r="D175" s="4">
         <f t="shared" si="22"/>
         <v>11190</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B175" s="4" t="s">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B176" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="C175" s="5">
+      <c r="C176" s="5">
         <v>-10000</v>
       </c>
-      <c r="D175" s="4">
+      <c r="D176" s="4">
         <f t="shared" si="22"/>
         <v>1190</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176" s="17" t="s">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177" s="17" t="s">
         <v>211</v>
       </c>
-      <c r="B176" s="4" t="s">
+      <c r="B177" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C176" s="5">
+      <c r="C177" s="5">
         <v>3000</v>
       </c>
-      <c r="D176" s="4">
+      <c r="D177" s="4">
         <f t="shared" si="22"/>
         <v>4190</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A177" s="17" t="s">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A178" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="B177" s="4" t="s">
+      <c r="B178" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="C177" s="5">
+      <c r="C178" s="5">
         <v>11000</v>
       </c>
-      <c r="D177" s="4">
+      <c r="D178" s="4">
         <f t="shared" si="22"/>
         <v>15190</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B178" s="4" t="s">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B179" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C178" s="5">
+      <c r="C179" s="5">
         <v>-10000</v>
       </c>
-      <c r="D178" s="4">
+      <c r="D179" s="4">
         <f t="shared" si="22"/>
         <v>5190</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A179" s="17" t="s">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180" s="17" t="s">
         <v>213</v>
       </c>
-      <c r="B179" s="4" t="s">
+      <c r="B180" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C179" s="5">
+      <c r="C180" s="5">
         <v>3000</v>
       </c>
-      <c r="D179" s="4">
-        <f>D178+C179</f>
+      <c r="D180" s="4">
+        <f>D179+C180</f>
         <v>8190</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A181" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="B181" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="C181" s="5">
+        <v>14000</v>
+      </c>
+      <c r="D181" s="4">
+        <f>D180+C181</f>
+        <v>22190</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B182" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="C182" s="5">
+        <v>-20000</v>
+      </c>
+      <c r="D182" s="4">
+        <f>D181+C182</f>
+        <v>2190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
duy note chua lam giay
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="218">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -670,6 +670,9 @@
   </si>
   <si>
     <t>Duy cho cô diễm vay 20tr</t>
+  </si>
+  <si>
+    <t>chưa làm giấy</t>
   </si>
 </sst>
 </file>
@@ -704,7 +707,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -720,6 +723,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -784,7 +793,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -842,6 +851,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1151,8 +1163,8 @@
   <dimension ref="A1:K182"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N24" sqref="N24"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S25" sqref="S25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1371,7 +1383,9 @@
       <c r="I16" s="5">
         <v>10</v>
       </c>
-      <c r="K16" s="14"/>
+      <c r="K16" s="21" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H17" s="17" t="s">
@@ -1438,7 +1452,9 @@
       <c r="I21" s="5">
         <v>10</v>
       </c>
-      <c r="K21" s="14"/>
+      <c r="K21" s="21" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
@@ -1823,6 +1839,9 @@
       </c>
       <c r="I48" s="5">
         <v>20</v>
+      </c>
+      <c r="K48" s="21" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
chi dieu tra 20tr
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="CÔ DIỄM" sheetId="1" r:id="rId1"/>
@@ -12,14 +12,13 @@
     <sheet name="HÀ" sheetId="4" r:id="rId3"/>
     <sheet name="GIANG" sheetId="5" r:id="rId4"/>
     <sheet name="Tổng Kết" sheetId="6" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="211">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -351,9 +350,6 @@
     <t>Cô Yến</t>
   </si>
   <si>
-    <t>Chị Diệu</t>
-  </si>
-  <si>
     <t>Tí</t>
   </si>
   <si>
@@ -378,9 +374,6 @@
     <t>29/03/2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Tổng </t>
-  </si>
-  <si>
     <t xml:space="preserve">Duy chuyển cho cô Diễm 5tr </t>
   </si>
   <si>
@@ -408,9 +401,6 @@
     <t>13/04/24</t>
   </si>
   <si>
-    <t xml:space="preserve">Còn </t>
-  </si>
-  <si>
     <t>21/04/2024</t>
   </si>
   <si>
@@ -442,18 +432,6 @@
   </si>
   <si>
     <t>31/05/2024</t>
-  </si>
-  <si>
-    <t>tran ngoc quang</t>
-  </si>
-  <si>
-    <t>nguyen khanh duy</t>
-  </si>
-  <si>
-    <t>co diem no</t>
-  </si>
-  <si>
-    <t>vo thi dang nga</t>
   </si>
   <si>
     <t>Duy chyển cho cô Diễm 5tr</t>
@@ -682,7 +660,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -693,14 +671,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -793,7 +763,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -840,7 +810,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -850,10 +819,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1162,19 +1131,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K182"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="S25" sqref="S25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" style="17" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" style="16" customWidth="1"/>
     <col min="2" max="2" width="54.28515625" style="4" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" style="5" customWidth="1"/>
     <col min="4" max="4" width="25.5703125" style="4" customWidth="1"/>
     <col min="5" max="7" width="9.140625" style="6"/>
-    <col min="8" max="8" width="12.7109375" style="17" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="16" customWidth="1"/>
     <col min="9" max="9" width="29.5703125" style="5" customWidth="1"/>
     <col min="10" max="10" width="14.28515625" style="4" customWidth="1"/>
     <col min="11" max="11" width="26" style="6" customWidth="1"/>
@@ -1182,7 +1151,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -1201,7 +1170,7 @@
       <c r="J1" s="15"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1210,7 +1179,7 @@
       <c r="C2" s="5">
         <v>1930</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="17" t="s">
         <v>2</v>
       </c>
       <c r="I2" s="3" t="s">
@@ -1220,7 +1189,7 @@
         <v>5</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1233,7 +1202,7 @@
       <c r="D3" s="4">
         <v>3930</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="16" t="s">
         <v>6</v>
       </c>
       <c r="I3" s="5">
@@ -1245,16 +1214,16 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H4" s="17" t="s">
-        <v>175</v>
+      <c r="H4" s="16" t="s">
+        <v>168</v>
       </c>
       <c r="I4" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H5" s="17" t="s">
-        <v>204</v>
+      <c r="H5" s="16" t="s">
+        <v>197</v>
       </c>
       <c r="I5" s="5">
         <v>20</v>
@@ -1271,7 +1240,7 @@
         <f>C6+D3</f>
         <v>18490</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="H6" s="16" t="s">
         <v>7</v>
       </c>
       <c r="I6" s="5">
@@ -1289,7 +1258,7 @@
         <f t="shared" ref="D7:D22" si="0">D6+C7</f>
         <v>8490</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H7" s="16" t="s">
         <v>8</v>
       </c>
       <c r="I7" s="5">
@@ -1307,7 +1276,7 @@
         <f t="shared" si="0"/>
         <v>10490</v>
       </c>
-      <c r="H8" s="17" t="s">
+      <c r="H8" s="16" t="s">
         <v>9</v>
       </c>
       <c r="I8" s="5">
@@ -1315,7 +1284,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H9" s="17" t="s">
+      <c r="H9" s="16" t="s">
         <v>41</v>
       </c>
       <c r="I9" s="5">
@@ -1323,7 +1292,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H10" s="17" t="s">
+      <c r="H10" s="16" t="s">
         <v>84</v>
       </c>
       <c r="I10" s="5">
@@ -1332,7 +1301,7 @@
       <c r="K10" s="14"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H11" s="17" t="s">
+      <c r="H11" s="16" t="s">
         <v>96</v>
       </c>
       <c r="I11" s="5">
@@ -1341,8 +1310,8 @@
       <c r="K11" s="14"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H12" s="17" t="s">
-        <v>130</v>
+      <c r="H12" s="16" t="s">
+        <v>127</v>
       </c>
       <c r="I12" s="5">
         <v>10</v>
@@ -1350,8 +1319,8 @@
       <c r="K12" s="14"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H13" s="17" t="s">
-        <v>136</v>
+      <c r="H13" s="16" t="s">
+        <v>133</v>
       </c>
       <c r="I13" s="5">
         <v>10</v>
@@ -1359,8 +1328,8 @@
       <c r="K13" s="14"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H14" s="17" t="s">
-        <v>149</v>
+      <c r="H14" s="16" t="s">
+        <v>142</v>
       </c>
       <c r="I14" s="5">
         <v>10</v>
@@ -1368,8 +1337,8 @@
       <c r="K14" s="14"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H15" s="17" t="s">
-        <v>184</v>
+      <c r="H15" s="16" t="s">
+        <v>177</v>
       </c>
       <c r="I15" s="5">
         <v>10</v>
@@ -1377,18 +1346,18 @@
       <c r="K15" s="14"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H16" s="17" t="s">
-        <v>207</v>
+      <c r="H16" s="16" t="s">
+        <v>200</v>
       </c>
       <c r="I16" s="5">
         <v>10</v>
       </c>
-      <c r="K16" s="21" t="s">
-        <v>217</v>
+      <c r="K16" s="19" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H17" s="17" t="s">
+      <c r="H17" s="16" t="s">
         <v>70</v>
       </c>
       <c r="I17" s="5">
@@ -1396,7 +1365,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H18" s="17" t="s">
+      <c r="H18" s="16" t="s">
         <v>107</v>
       </c>
       <c r="I18" s="5">
@@ -1405,8 +1374,8 @@
       <c r="K18" s="14"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H19" s="17" t="s">
-        <v>185</v>
+      <c r="H19" s="16" t="s">
+        <v>178</v>
       </c>
       <c r="I19" s="5">
         <v>10</v>
@@ -1424,7 +1393,7 @@
         <f>D8+C20</f>
         <v>490</v>
       </c>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="16" t="s">
         <v>10</v>
       </c>
       <c r="I20" s="5">
@@ -1433,7 +1402,7 @@
       <c r="K20" s="14"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="16" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="4" t="s">
@@ -1446,18 +1415,18 @@
         <f t="shared" si="0"/>
         <v>2490</v>
       </c>
-      <c r="H21" s="17" t="s">
+      <c r="H21" s="16" t="s">
         <v>11</v>
       </c>
       <c r="I21" s="5">
         <v>10</v>
       </c>
-      <c r="K21" s="21" t="s">
-        <v>217</v>
+      <c r="K21" s="19" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="17" t="s">
+      <c r="A22" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -1470,7 +1439,7 @@
         <f t="shared" si="0"/>
         <v>5490</v>
       </c>
-      <c r="H22" s="17" t="s">
+      <c r="H22" s="16" t="s">
         <v>24</v>
       </c>
       <c r="I22" s="5">
@@ -1479,7 +1448,7 @@
       <c r="K22" s="14"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H23" s="17" t="s">
+      <c r="H23" s="16" t="s">
         <v>59</v>
       </c>
       <c r="I23" s="5">
@@ -1488,7 +1457,7 @@
       <c r="K23" s="14"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H24" s="17" t="s">
+      <c r="H24" s="16" t="s">
         <v>73</v>
       </c>
       <c r="I24" s="5">
@@ -1497,7 +1466,7 @@
       <c r="K24" s="14"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H25" s="17" t="s">
+      <c r="H25" s="16" t="s">
         <v>91</v>
       </c>
       <c r="I25" s="5">
@@ -1506,8 +1475,8 @@
       <c r="K25" s="14"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H26" s="17" t="s">
-        <v>121</v>
+      <c r="H26" s="16" t="s">
+        <v>119</v>
       </c>
       <c r="I26" s="5">
         <v>10</v>
@@ -1515,8 +1484,8 @@
       <c r="K26" s="14"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H27" s="17" t="s">
-        <v>132</v>
+      <c r="H27" s="16" t="s">
+        <v>129</v>
       </c>
       <c r="I27" s="5">
         <v>10</v>
@@ -1524,8 +1493,8 @@
       <c r="K27" s="14"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H28" s="17" t="s">
-        <v>138</v>
+      <c r="H28" s="16" t="s">
+        <v>135</v>
       </c>
       <c r="I28" s="5">
         <v>10</v>
@@ -1533,8 +1502,8 @@
       <c r="K28" s="14"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H29" s="17" t="s">
-        <v>151</v>
+      <c r="H29" s="16" t="s">
+        <v>144</v>
       </c>
       <c r="I29" s="5">
         <v>10</v>
@@ -1542,8 +1511,8 @@
       <c r="K29" s="14"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H30" s="17" t="s">
-        <v>188</v>
+      <c r="H30" s="16" t="s">
+        <v>181</v>
       </c>
       <c r="I30" s="5">
         <v>10</v>
@@ -1551,8 +1520,8 @@
       <c r="K30" s="14"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H31" s="17" t="s">
-        <v>212</v>
+      <c r="H31" s="16" t="s">
+        <v>205</v>
       </c>
       <c r="I31" s="5">
         <v>10</v>
@@ -1560,7 +1529,7 @@
       <c r="K31" s="14"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="17" t="s">
+      <c r="A32" s="16" t="s">
         <v>24</v>
       </c>
       <c r="B32" s="4" t="s">
@@ -1573,7 +1542,7 @@
         <f>D22+C32</f>
         <v>8490</v>
       </c>
-      <c r="H32" s="17" t="s">
+      <c r="H32" s="16" t="s">
         <v>12</v>
       </c>
       <c r="I32" s="5">
@@ -1581,7 +1550,7 @@
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H33" s="17" t="s">
+      <c r="H33" s="16" t="s">
         <v>43</v>
       </c>
       <c r="I33" s="5">
@@ -1590,8 +1559,8 @@
       <c r="K33" s="14"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H34" s="17" t="s">
-        <v>146</v>
+      <c r="H34" s="16" t="s">
+        <v>139</v>
       </c>
       <c r="I34" s="5">
         <v>10</v>
@@ -1599,8 +1568,8 @@
       <c r="K34" s="14"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H35" s="17" t="s">
-        <v>162</v>
+      <c r="H35" s="16" t="s">
+        <v>155</v>
       </c>
       <c r="I35" s="5">
         <v>10</v>
@@ -1608,8 +1577,8 @@
       <c r="K35" s="14"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H36" s="17" t="s">
-        <v>163</v>
+      <c r="H36" s="16" t="s">
+        <v>156</v>
       </c>
       <c r="I36" s="5">
         <v>10</v>
@@ -1627,8 +1596,8 @@
         <f>D32+C37</f>
         <v>12890</v>
       </c>
-      <c r="H37" s="17" t="s">
-        <v>164</v>
+      <c r="H37" s="16" t="s">
+        <v>157</v>
       </c>
       <c r="I37" s="5">
         <v>20</v>
@@ -1646,8 +1615,8 @@
         <f>D37+C38</f>
         <v>2890</v>
       </c>
-      <c r="H38" s="17" t="s">
-        <v>165</v>
+      <c r="H38" s="16" t="s">
+        <v>158</v>
       </c>
       <c r="I38" s="5">
         <v>10</v>
@@ -1665,8 +1634,8 @@
         <f t="shared" ref="D39:D46" si="1">D38+C39</f>
         <v>4490</v>
       </c>
-      <c r="H39" s="17" t="s">
-        <v>166</v>
+      <c r="H39" s="16" t="s">
+        <v>159</v>
       </c>
       <c r="I39" s="5">
         <v>10</v>
@@ -1684,15 +1653,15 @@
         <f t="shared" si="1"/>
         <v>7490</v>
       </c>
-      <c r="H40" s="17" t="s">
-        <v>167</v>
+      <c r="H40" s="16" t="s">
+        <v>160</v>
       </c>
       <c r="I40" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="17" t="s">
+      <c r="A41" s="16" t="s">
         <v>39</v>
       </c>
       <c r="B41" s="4" t="s">
@@ -1705,15 +1674,15 @@
         <f t="shared" si="1"/>
         <v>9490</v>
       </c>
-      <c r="H41" s="17" t="s">
-        <v>161</v>
+      <c r="H41" s="16" t="s">
+        <v>154</v>
       </c>
       <c r="I41" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="17" t="s">
+      <c r="A42" s="16" t="s">
         <v>41</v>
       </c>
       <c r="B42" s="4" t="s">
@@ -1726,8 +1695,8 @@
         <f t="shared" si="1"/>
         <v>12490</v>
       </c>
-      <c r="H42" s="17" t="s">
-        <v>160</v>
+      <c r="H42" s="16" t="s">
+        <v>153</v>
       </c>
       <c r="I42" s="5">
         <v>10</v>
@@ -1745,8 +1714,8 @@
         <f t="shared" si="1"/>
         <v>2490</v>
       </c>
-      <c r="H43" s="17" t="s">
-        <v>159</v>
+      <c r="H43" s="16" t="s">
+        <v>152</v>
       </c>
       <c r="I43" s="5">
         <v>10</v>
@@ -1754,7 +1723,7 @@
       <c r="K43" s="14"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="17" t="s">
+      <c r="A44" s="16" t="s">
         <v>42</v>
       </c>
       <c r="B44" s="4" t="s">
@@ -1767,8 +1736,8 @@
         <f t="shared" si="1"/>
         <v>7450</v>
       </c>
-      <c r="H44" s="17" t="s">
-        <v>158</v>
+      <c r="H44" s="16" t="s">
+        <v>151</v>
       </c>
       <c r="I44" s="5">
         <v>10</v>
@@ -1776,7 +1745,7 @@
       <c r="K44" s="14"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="17" t="s">
+      <c r="A45" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B45" s="4" t="s">
@@ -1789,8 +1758,8 @@
         <f t="shared" si="1"/>
         <v>11450</v>
       </c>
-      <c r="H45" s="17" t="s">
-        <v>157</v>
+      <c r="H45" s="16" t="s">
+        <v>150</v>
       </c>
       <c r="I45" s="5">
         <v>10</v>
@@ -1807,8 +1776,8 @@
         <f t="shared" si="1"/>
         <v>1450</v>
       </c>
-      <c r="H46" s="17" t="s">
-        <v>156</v>
+      <c r="H46" s="16" t="s">
+        <v>149</v>
       </c>
       <c r="I46" s="5">
         <v>10</v>
@@ -1826,22 +1795,22 @@
         <f t="shared" ref="D47:D53" si="2">D46+C47</f>
         <v>9090</v>
       </c>
-      <c r="H47" s="17" t="s">
-        <v>192</v>
+      <c r="H47" s="16" t="s">
+        <v>185</v>
       </c>
       <c r="I47" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H48" s="17" t="s">
-        <v>214</v>
+      <c r="H48" s="16" t="s">
+        <v>207</v>
       </c>
       <c r="I48" s="5">
         <v>20</v>
       </c>
-      <c r="K48" s="21" t="s">
-        <v>217</v>
+      <c r="K48" s="19" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -1855,8 +1824,8 @@
         <f>D47+C49</f>
         <v>12090</v>
       </c>
-      <c r="H49" s="17" t="s">
-        <v>194</v>
+      <c r="H49" s="16" t="s">
+        <v>187</v>
       </c>
       <c r="I49" s="5">
         <v>10</v>
@@ -1887,7 +1856,7 @@
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="17" t="s">
+      <c r="A52" s="16" t="s">
         <v>53</v>
       </c>
       <c r="B52" s="4" t="s">
@@ -1902,7 +1871,7 @@
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="17" t="s">
+      <c r="A53" s="16" t="s">
         <v>57</v>
       </c>
       <c r="B53" s="4" t="s">
@@ -1917,7 +1886,7 @@
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="17" t="s">
+      <c r="A54" s="16" t="s">
         <v>59</v>
       </c>
       <c r="B54" s="4" t="s">
@@ -1956,7 +1925,7 @@
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="17">
+      <c r="A57" s="16">
         <v>44969</v>
       </c>
       <c r="B57" s="4" t="s">
@@ -1995,7 +1964,7 @@
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="17" t="s">
+      <c r="A60" s="16" t="s">
         <v>64</v>
       </c>
       <c r="B60" s="4" t="s">
@@ -2010,7 +1979,7 @@
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="17" t="s">
+      <c r="A61" s="16" t="s">
         <v>66</v>
       </c>
       <c r="B61" s="4" t="s">
@@ -2037,7 +2006,7 @@
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="17" t="s">
+      <c r="A63" s="16" t="s">
         <v>68</v>
       </c>
       <c r="B63" s="4" t="s">
@@ -2064,7 +2033,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="17" t="s">
+      <c r="A65" s="16" t="s">
         <v>71</v>
       </c>
       <c r="B65" s="4" t="s">
@@ -2104,7 +2073,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="17" t="s">
+      <c r="A68" s="16" t="s">
         <v>75</v>
       </c>
       <c r="B68" s="4" t="s">
@@ -2167,7 +2136,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="17" t="s">
+      <c r="A73" s="16" t="s">
         <v>81</v>
       </c>
       <c r="B73" s="4" t="s">
@@ -2194,7 +2163,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="17" t="s">
+      <c r="A75" s="16" t="s">
         <v>82</v>
       </c>
       <c r="B75" s="4" t="s">
@@ -2209,7 +2178,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="17" t="s">
+      <c r="A76" s="16" t="s">
         <v>83</v>
       </c>
       <c r="B76" s="4" t="s">
@@ -2224,7 +2193,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="17" t="s">
+      <c r="A77" s="16" t="s">
         <v>84</v>
       </c>
       <c r="B77" s="4" t="s">
@@ -2251,7 +2220,7 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="17" t="s">
+      <c r="A79" s="16" t="s">
         <v>86</v>
       </c>
       <c r="B79" s="4" t="s">
@@ -2266,7 +2235,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="17" t="s">
+      <c r="A80" s="16" t="s">
         <v>88</v>
       </c>
       <c r="B80" s="4" t="s">
@@ -2341,7 +2310,7 @@
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="17" t="s">
+      <c r="A86" s="16" t="s">
         <v>94</v>
       </c>
       <c r="B86" s="4" t="s">
@@ -2356,7 +2325,7 @@
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="17" t="s">
+      <c r="A87" s="16" t="s">
         <v>96</v>
       </c>
       <c r="B87" s="4" t="s">
@@ -2383,7 +2352,7 @@
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="17" t="s">
+      <c r="A89" s="16" t="s">
         <v>98</v>
       </c>
       <c r="B89" s="4" t="s">
@@ -2470,7 +2439,7 @@
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="17" t="s">
+      <c r="A96" s="16" t="s">
         <v>104</v>
       </c>
       <c r="B96" s="4" t="s">
@@ -2485,7 +2454,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="17" t="s">
+      <c r="A97" s="16" t="s">
         <v>105</v>
       </c>
       <c r="B97" s="4" t="s">
@@ -2500,7 +2469,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="17" t="s">
+      <c r="A98" s="16" t="s">
         <v>106</v>
       </c>
       <c r="B98" s="4" t="s">
@@ -2527,11 +2496,11 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="17" t="s">
+      <c r="A100" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="B100" s="4" t="s">
         <v>116</v>
-      </c>
-      <c r="B100" s="4" t="s">
-        <v>117</v>
       </c>
       <c r="C100" s="5">
         <v>800</v>
@@ -2542,11 +2511,11 @@
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="17" t="s">
+      <c r="A101" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="B101" s="4" t="s">
         <v>118</v>
-      </c>
-      <c r="B101" s="4" t="s">
-        <v>120</v>
       </c>
       <c r="C101" s="5">
         <v>5000</v>
@@ -2557,8 +2526,8 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="17" t="s">
-        <v>121</v>
+      <c r="A102" s="16" t="s">
+        <v>119</v>
       </c>
       <c r="B102" s="4" t="s">
         <v>102</v>
@@ -2584,8 +2553,8 @@
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="17" t="s">
-        <v>124</v>
+      <c r="A104" s="16" t="s">
+        <v>122</v>
       </c>
       <c r="B104" s="4" t="s">
         <v>65</v>
@@ -2612,7 +2581,7 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B106" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C106" s="5">
         <v>7000</v>
@@ -2635,8 +2604,8 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="17" t="s">
-        <v>128</v>
+      <c r="A108" s="16" t="s">
+        <v>126</v>
       </c>
       <c r="B108" s="4" t="s">
         <v>65</v>
@@ -2650,8 +2619,8 @@
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="17" t="s">
-        <v>130</v>
+      <c r="A109" s="16" t="s">
+        <v>127</v>
       </c>
       <c r="B109" s="4" t="s">
         <v>102</v>
@@ -2677,8 +2646,8 @@
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="17" t="s">
-        <v>131</v>
+      <c r="A111" s="16" t="s">
+        <v>128</v>
       </c>
       <c r="B111" s="4" t="s">
         <v>65</v>
@@ -2692,11 +2661,11 @@
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="17" t="s">
-        <v>132</v>
+      <c r="A112" s="16" t="s">
+        <v>129</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C112" s="5">
         <v>7000</v>
@@ -2720,7 +2689,7 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B114" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C114" s="5">
         <v>12000</v>
@@ -2744,7 +2713,7 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B116" s="4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C116" s="5">
         <v>2000</v>
@@ -2755,8 +2724,8 @@
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="17" t="s">
-        <v>135</v>
+      <c r="A117" s="16" t="s">
+        <v>132</v>
       </c>
       <c r="B117" s="4" t="s">
         <v>65</v>
@@ -2770,11 +2739,11 @@
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="17" t="s">
-        <v>136</v>
+      <c r="A118" s="16" t="s">
+        <v>133</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C118" s="5">
         <v>7000</v>
@@ -2797,8 +2766,8 @@
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="17" t="s">
-        <v>137</v>
+      <c r="A120" s="16" t="s">
+        <v>134</v>
       </c>
       <c r="B120" s="4" t="s">
         <v>65</v>
@@ -2812,11 +2781,11 @@
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="17" t="s">
-        <v>138</v>
+      <c r="A121" s="16" t="s">
+        <v>135</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C121" s="5">
         <v>8000</v>
@@ -2839,8 +2808,8 @@
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="17" t="s">
-        <v>140</v>
+      <c r="A123" s="16" t="s">
+        <v>137</v>
       </c>
       <c r="B123" s="4" t="s">
         <v>65</v>
@@ -2855,7 +2824,7 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B124" s="4" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="C124" s="5">
         <v>5000</v>
@@ -2914,8 +2883,8 @@
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="17" t="s">
-        <v>148</v>
+      <c r="A129" s="16" t="s">
+        <v>141</v>
       </c>
       <c r="B129" s="4" t="s">
         <v>65</v>
@@ -2929,11 +2898,11 @@
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="17" t="s">
-        <v>149</v>
+      <c r="A130" s="16" t="s">
+        <v>142</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C130" s="5">
         <v>8000</v>
@@ -2956,8 +2925,8 @@
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="17" t="s">
-        <v>150</v>
+      <c r="A132" s="16" t="s">
+        <v>143</v>
       </c>
       <c r="B132" s="4" t="s">
         <v>65</v>
@@ -2971,11 +2940,11 @@
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="17" t="s">
-        <v>151</v>
+      <c r="A133" s="16" t="s">
+        <v>144</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C133" s="5">
         <v>12000</v>
@@ -2998,11 +2967,11 @@
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="17" t="s">
-        <v>168</v>
+      <c r="A135" s="16" t="s">
+        <v>161</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="C135" s="5">
         <v>2000</v>
@@ -3013,11 +2982,11 @@
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="17" t="s">
-        <v>156</v>
+      <c r="A136" s="16" t="s">
+        <v>149</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="C136" s="5">
         <v>10000</v>
@@ -3041,7 +3010,7 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B138" s="4" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="C138" s="5">
         <v>2000</v>
@@ -3052,11 +3021,11 @@
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="17" t="s">
-        <v>169</v>
+      <c r="A139" s="16" t="s">
+        <v>162</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C139" s="5">
         <v>-1200</v>
@@ -3068,7 +3037,7 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B140" s="4" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="C140" s="5">
         <v>500</v>
@@ -3079,11 +3048,11 @@
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="17" t="s">
-        <v>172</v>
+      <c r="A141" s="16" t="s">
+        <v>165</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C141" s="5">
         <v>750</v>
@@ -3094,11 +3063,11 @@
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="17" t="s">
-        <v>174</v>
+      <c r="A142" s="16" t="s">
+        <v>167</v>
       </c>
       <c r="B142" s="4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C142" s="5">
         <v>2000</v>
@@ -3134,7 +3103,7 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B145" s="4" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C145" s="5">
         <v>350</v>
@@ -3145,11 +3114,11 @@
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="17" t="s">
-        <v>178</v>
+      <c r="A146" s="16" t="s">
+        <v>171</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="C146" s="5">
         <v>300</v>
@@ -3160,11 +3129,11 @@
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="17" t="s">
-        <v>180</v>
+      <c r="A147" s="16" t="s">
+        <v>173</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="C147" s="5">
         <v>3800</v>
@@ -3187,11 +3156,11 @@
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="17" t="s">
-        <v>182</v>
+      <c r="A149" s="16" t="s">
+        <v>175</v>
       </c>
       <c r="B149" s="4" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="C149" s="5">
         <v>1300</v>
@@ -3202,8 +3171,8 @@
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="17" t="s">
-        <v>184</v>
+      <c r="A150" s="16" t="s">
+        <v>177</v>
       </c>
       <c r="B150" s="4" t="s">
         <v>100</v>
@@ -3229,8 +3198,8 @@
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="17" t="s">
-        <v>185</v>
+      <c r="A152" s="16" t="s">
+        <v>178</v>
       </c>
       <c r="B152" s="4" t="s">
         <v>65</v>
@@ -3256,11 +3225,11 @@
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="17" t="s">
-        <v>186</v>
+      <c r="A154" s="16" t="s">
+        <v>179</v>
       </c>
       <c r="B154" s="4" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="C154" s="5">
         <v>500</v>
@@ -3271,11 +3240,11 @@
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="17" t="s">
-        <v>188</v>
+      <c r="A155" s="16" t="s">
+        <v>181</v>
       </c>
       <c r="B155" s="4" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="C155" s="5">
         <v>10000</v>
@@ -3298,8 +3267,8 @@
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="17" t="s">
-        <v>190</v>
+      <c r="A157" s="16" t="s">
+        <v>183</v>
       </c>
       <c r="B157" s="4" t="s">
         <v>25</v>
@@ -3313,8 +3282,8 @@
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="17" t="s">
-        <v>191</v>
+      <c r="A158" s="16" t="s">
+        <v>184</v>
       </c>
       <c r="B158" s="4" t="s">
         <v>65</v>
@@ -3329,7 +3298,7 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B159" s="4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C159" s="5">
         <v>2000</v>
@@ -3340,11 +3309,11 @@
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="17" t="s">
-        <v>192</v>
+      <c r="A160" s="16" t="s">
+        <v>185</v>
       </c>
       <c r="B160" s="4" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="C160" s="5">
         <v>11000</v>
@@ -3367,11 +3336,11 @@
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" s="17" t="s">
-        <v>194</v>
+      <c r="A162" s="16" t="s">
+        <v>187</v>
       </c>
       <c r="B162" s="4" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="C162" s="5">
         <v>3000</v>
@@ -3406,11 +3375,11 @@
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" s="17" t="s">
-        <v>196</v>
+      <c r="A165" s="16" t="s">
+        <v>189</v>
       </c>
       <c r="B165" s="4" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C165" s="5">
         <v>5600</v>
@@ -3422,7 +3391,7 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B166" s="4" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="C166" s="5">
         <v>4700</v>
@@ -3433,8 +3402,8 @@
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A167" s="17" t="s">
-        <v>199</v>
+      <c r="A167" s="16" t="s">
+        <v>192</v>
       </c>
       <c r="B167" s="4" t="s">
         <v>78</v>
@@ -3460,11 +3429,11 @@
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A169" s="17" t="s">
-        <v>200</v>
+      <c r="A169" s="16" t="s">
+        <v>193</v>
       </c>
       <c r="B169" s="4" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="C169" s="5">
         <v>1000</v>
@@ -3475,11 +3444,11 @@
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" s="17" t="s">
-        <v>202</v>
+      <c r="A170" s="16" t="s">
+        <v>195</v>
       </c>
       <c r="B170" s="4" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C170" s="5">
         <v>1000</v>
@@ -3490,8 +3459,8 @@
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" s="17" t="s">
-        <v>204</v>
+      <c r="A171" s="16" t="s">
+        <v>197</v>
       </c>
       <c r="B171" s="4" t="s">
         <v>28</v>
@@ -3506,7 +3475,7 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B172" s="4" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="C172" s="5">
         <v>-20000</v>
@@ -3541,11 +3510,11 @@
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A175" s="17" t="s">
-        <v>207</v>
+      <c r="A175" s="16" t="s">
+        <v>200</v>
       </c>
       <c r="B175" s="4" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="C175" s="5">
         <v>10000</v>
@@ -3557,7 +3526,7 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B176" s="4" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="C176" s="5">
         <v>-10000</v>
@@ -3568,8 +3537,8 @@
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A177" s="17" t="s">
-        <v>211</v>
+      <c r="A177" s="16" t="s">
+        <v>204</v>
       </c>
       <c r="B177" s="4" t="s">
         <v>28</v>
@@ -3583,11 +3552,11 @@
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A178" s="17" t="s">
-        <v>212</v>
+      <c r="A178" s="16" t="s">
+        <v>205</v>
       </c>
       <c r="B178" s="4" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="C178" s="5">
         <v>11000</v>
@@ -3610,8 +3579,8 @@
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" s="17" t="s">
-        <v>213</v>
+      <c r="A180" s="16" t="s">
+        <v>206</v>
       </c>
       <c r="B180" s="4" t="s">
         <v>28</v>
@@ -3625,11 +3594,11 @@
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="17" t="s">
-        <v>214</v>
+      <c r="A181" s="16" t="s">
+        <v>207</v>
       </c>
       <c r="B181" s="4" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="C181" s="5">
         <v>14000</v>
@@ -3641,7 +3610,7 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B182" s="4" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="C182" s="5">
         <v>-20000</v>
@@ -4014,7 +3983,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
@@ -4094,7 +4063,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>56</v>
@@ -4112,7 +4081,7 @@
         <v>45508</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C5" s="5">
         <v>-1200</v>
@@ -4124,7 +4093,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>56</v>
@@ -4148,17 +4117,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.28515625" customWidth="1"/>
     <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="35" style="19" customWidth="1"/>
+    <col min="3" max="3" width="35" style="18" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4167,7 +4136,7 @@
         <v>108</v>
       </c>
       <c r="B1">
-        <v>480000</v>
+        <v>510000</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -4183,7 +4152,7 @@
         <v>110</v>
       </c>
       <c r="B3">
-        <v>20000</v>
+        <v>15000</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -4191,7 +4160,7 @@
         <v>111</v>
       </c>
       <c r="B4">
-        <v>15000</v>
+        <v>6580</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -4199,7 +4168,7 @@
         <v>112</v>
       </c>
       <c r="B5">
-        <v>6580</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -4207,7 +4176,7 @@
         <v>113</v>
       </c>
       <c r="B6">
-        <v>5000</v>
+        <v>9300</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -4215,120 +4184,38 @@
         <v>114</v>
       </c>
       <c r="B7">
-        <v>9300</v>
+        <v>2200</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="B8">
-        <v>2200</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>210</v>
+        <v>11000</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="B9">
-        <v>11000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>147</v>
-      </c>
-      <c r="B10">
         <v>5000</v>
       </c>
-      <c r="C10" s="19" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="C9" s="18" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>5</v>
       </c>
-      <c r="B23">
-        <f>SUM(B1:B20)</f>
-        <v>584080</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="40" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>141</v>
-      </c>
-      <c r="B1">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>142</v>
-      </c>
-      <c r="B2">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>143</v>
-      </c>
-      <c r="B3">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>144</v>
-      </c>
-      <c r="B4">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="B15" s="16">
-        <f>SUM(B1:B13)</f>
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B16">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>129</v>
-      </c>
-      <c r="B17">
-        <f>B16-B15</f>
-        <v>2500</v>
+      <c r="B22">
+        <f>SUM(B1:B19)</f>
+        <v>594080</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
duy lam giay cho co diem 03,21,30/08
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="CÔ DIỄM" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="211">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -650,7 +650,7 @@
     <t>Duy cho cô diễm vay 20tr</t>
   </si>
   <si>
-    <t>chưa làm giấy</t>
+    <t>03/09/2024</t>
   </si>
 </sst>
 </file>
@@ -677,7 +677,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -693,12 +693,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -763,7 +757,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -818,9 +812,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1131,9 +1122,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K182"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S25" sqref="S25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A162" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I179" sqref="I179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1163,10 +1154,10 @@
       <c r="D1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="20"/>
+      <c r="I1" s="19"/>
       <c r="J1" s="15"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1352,9 +1343,7 @@
       <c r="I16" s="5">
         <v>10</v>
       </c>
-      <c r="K16" s="19" t="s">
-        <v>210</v>
-      </c>
+      <c r="K16" s="14"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H17" s="16" t="s">
@@ -1363,6 +1352,7 @@
       <c r="I17" s="5">
         <v>10</v>
       </c>
+      <c r="K17" s="14"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H18" s="16" t="s">
@@ -1421,9 +1411,7 @@
       <c r="I21" s="5">
         <v>10</v>
       </c>
-      <c r="K21" s="19" t="s">
-        <v>210</v>
-      </c>
+      <c r="K21" s="14"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
@@ -1548,6 +1536,7 @@
       <c r="I32" s="5">
         <v>10</v>
       </c>
+      <c r="K32" s="14"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H33" s="16" t="s">
@@ -1659,6 +1648,7 @@
       <c r="I40" s="5">
         <v>10</v>
       </c>
+      <c r="K40" s="14"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
@@ -1680,6 +1670,7 @@
       <c r="I41" s="5">
         <v>10</v>
       </c>
+      <c r="K41" s="14"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
@@ -1764,6 +1755,7 @@
       <c r="I45" s="5">
         <v>10</v>
       </c>
+      <c r="K45" s="14"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B46" s="4" t="s">
@@ -1801,6 +1793,7 @@
       <c r="I47" s="5">
         <v>10</v>
       </c>
+      <c r="K47" s="14"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H48" s="16" t="s">
@@ -1809,9 +1802,7 @@
       <c r="I48" s="5">
         <v>20</v>
       </c>
-      <c r="K48" s="19" t="s">
-        <v>210</v>
-      </c>
+      <c r="K48" s="14"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B49" s="4" t="s">
@@ -3595,7 +3586,7 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="16" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="B181" s="4" t="s">
         <v>208</v>
@@ -3668,10 +3659,10 @@
       <c r="E1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="20"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
@@ -3772,7 +3763,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
@@ -3807,10 +3798,10 @@
       <c r="E1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="20"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -4033,10 +4024,10 @@
       <c r="E1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="20"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">

</xml_diff>

<commit_message>
Duy lay 5tr tien loi co diem
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="213">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -651,6 +651,12 @@
   </si>
   <si>
     <t>03/09/2024</t>
+  </si>
+  <si>
+    <t>13/09/2024</t>
+  </si>
+  <si>
+    <t>Duy lấy 5tr tiền lời</t>
   </si>
 </sst>
 </file>
@@ -1120,11 +1126,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K182"/>
+  <dimension ref="A1:K183"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A162" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I179" sqref="I179"/>
+      <pane ySplit="1" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D184" sqref="D184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3609,6 +3615,21 @@
       <c r="D182" s="4">
         <f>D181+C182</f>
         <v>2190</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A183" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="B183" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="C183" s="5">
+        <v>5000</v>
+      </c>
+      <c r="D183" s="4">
+        <f>D182+C183</f>
+        <v>7190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
co diem tra tien xe 5tr
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="215">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -657,6 +657,12 @@
   </si>
   <si>
     <t>Duy lấy 5tr tiền lời</t>
+  </si>
+  <si>
+    <t>14/09/2024</t>
+  </si>
+  <si>
+    <t>Cô Diễm trả tiền xe 5tr</t>
   </si>
 </sst>
 </file>
@@ -1126,11 +1132,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K183"/>
+  <dimension ref="A1:K184"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D184" sqref="D184"/>
+      <pane ySplit="1" topLeftCell="A169" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C193" sqref="C193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3630,6 +3636,21 @@
       <c r="D183" s="4">
         <f>D182+C183</f>
         <v>7190</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A184" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="B184" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="C184" s="5">
+        <v>5000</v>
+      </c>
+      <c r="D184" s="4">
+        <f>D183+C184</f>
+        <v>12190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Duy lay tien loi ngay 21 - cho co diem vay 20tr
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="216">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -663,6 +663,9 @@
   </si>
   <si>
     <t>Cô Diễm trả tiền xe 5tr</t>
+  </si>
+  <si>
+    <t>21/09/2024</t>
   </si>
 </sst>
 </file>
@@ -1132,11 +1135,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K184"/>
+  <dimension ref="A1:K187"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A169" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C193" sqref="C193"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1212,8 +1215,8 @@
         <v>20</v>
       </c>
       <c r="J3" s="4">
-        <f>SUM(I3:I63)</f>
-        <v>510</v>
+        <f>SUM(I3:I64)</f>
+        <v>530</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1258,7 +1261,7 @@
         <v>-10000</v>
       </c>
       <c r="D7" s="4">
-        <f t="shared" ref="D7:D22" si="0">D6+C7</f>
+        <f t="shared" ref="D7:D23" si="0">D6+C7</f>
         <v>8490</v>
       </c>
       <c r="H7" s="16" t="s">
@@ -1359,16 +1362,16 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H17" s="16" t="s">
-        <v>70</v>
+        <v>215</v>
       </c>
       <c r="I17" s="5">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="K17" s="14"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H18" s="16" t="s">
-        <v>107</v>
+        <v>70</v>
       </c>
       <c r="I18" s="5">
         <v>10</v>
@@ -1377,7 +1380,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H19" s="16" t="s">
-        <v>178</v>
+        <v>107</v>
       </c>
       <c r="I19" s="5">
         <v>10</v>
@@ -1385,18 +1388,8 @@
       <c r="K19" s="14"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="5">
-        <v>-10000</v>
-      </c>
-      <c r="D20" s="4">
-        <f>D8+C20</f>
-        <v>490</v>
-      </c>
       <c r="H20" s="16" t="s">
-        <v>10</v>
+        <v>178</v>
       </c>
       <c r="I20" s="5">
         <v>10</v>
@@ -1404,52 +1397,62 @@
       <c r="K20" s="14"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="16" t="s">
+      <c r="B21" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D21" s="4">
+        <f>D8+C21</f>
+        <v>490</v>
+      </c>
+      <c r="H21" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" s="5">
+        <v>10</v>
+      </c>
+      <c r="K21" s="14"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B22" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C22" s="5">
         <v>2000</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D22" s="4">
         <f t="shared" si="0"/>
         <v>2490</v>
       </c>
-      <c r="H21" s="16" t="s">
+      <c r="H22" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="I21" s="5">
+      <c r="I22" s="5">
         <v>10</v>
       </c>
-      <c r="K21" s="14"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="16" t="s">
+      <c r="K22" s="14"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B23" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C23" s="5">
         <v>3000</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D23" s="4">
         <f t="shared" si="0"/>
         <v>5490</v>
       </c>
-      <c r="H22" s="16" t="s">
+      <c r="H23" s="16" t="s">
         <v>24</v>
-      </c>
-      <c r="I22" s="5">
-        <v>10</v>
-      </c>
-      <c r="K22" s="14"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H23" s="16" t="s">
-        <v>59</v>
       </c>
       <c r="I23" s="5">
         <v>10</v>
@@ -1458,7 +1461,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H24" s="16" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="I24" s="5">
         <v>10</v>
@@ -1467,7 +1470,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H25" s="16" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="I25" s="5">
         <v>10</v>
@@ -1476,7 +1479,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H26" s="16" t="s">
-        <v>119</v>
+        <v>91</v>
       </c>
       <c r="I26" s="5">
         <v>10</v>
@@ -1485,7 +1488,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H27" s="16" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="I27" s="5">
         <v>10</v>
@@ -1494,7 +1497,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H28" s="16" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="I28" s="5">
         <v>10</v>
@@ -1503,7 +1506,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H29" s="16" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="I29" s="5">
         <v>10</v>
@@ -1512,7 +1515,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H30" s="16" t="s">
-        <v>181</v>
+        <v>144</v>
       </c>
       <c r="I30" s="5">
         <v>10</v>
@@ -1521,7 +1524,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H31" s="16" t="s">
-        <v>205</v>
+        <v>181</v>
       </c>
       <c r="I31" s="5">
         <v>10</v>
@@ -1529,21 +1532,8 @@
       <c r="K31" s="14"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C32" s="5">
-        <v>3000</v>
-      </c>
-      <c r="D32" s="4">
-        <f>D22+C32</f>
-        <v>8490</v>
-      </c>
       <c r="H32" s="16" t="s">
-        <v>12</v>
+        <v>205</v>
       </c>
       <c r="I32" s="5">
         <v>10</v>
@@ -1551,8 +1541,21 @@
       <c r="K32" s="14"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="5">
+        <v>3000</v>
+      </c>
+      <c r="D33" s="4">
+        <f>D23+C33</f>
+        <v>8490</v>
+      </c>
       <c r="H33" s="16" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="I33" s="5">
         <v>10</v>
@@ -1561,7 +1564,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H34" s="16" t="s">
-        <v>139</v>
+        <v>43</v>
       </c>
       <c r="I34" s="5">
         <v>10</v>
@@ -1570,7 +1573,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H35" s="16" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="I35" s="5">
         <v>10</v>
@@ -1579,7 +1582,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H36" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I36" s="5">
         <v>10</v>
@@ -1587,56 +1590,46 @@
       <c r="K36" s="14"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B37" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C37" s="5">
-        <v>4400</v>
-      </c>
-      <c r="D37" s="4">
-        <f>D32+C37</f>
-        <v>12890</v>
-      </c>
       <c r="H37" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I37" s="5">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K37" s="14"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C38" s="5">
-        <v>-10000</v>
+        <v>4400</v>
       </c>
       <c r="D38" s="4">
-        <f>D37+C38</f>
-        <v>2890</v>
+        <f>D33+C38</f>
+        <v>12890</v>
       </c>
       <c r="H38" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I38" s="5">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="K38" s="14"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C39" s="5">
-        <v>1600</v>
+        <v>-10000</v>
       </c>
       <c r="D39" s="4">
-        <f t="shared" ref="D39:D46" si="1">D38+C39</f>
-        <v>4490</v>
+        <f>D38+C39</f>
+        <v>2890</v>
       </c>
       <c r="H39" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I39" s="5">
         <v>10</v>
@@ -1645,162 +1638,162 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" s="5">
+        <v>1600</v>
+      </c>
+      <c r="D40" s="4">
+        <f t="shared" ref="D40:D47" si="1">D39+C40</f>
+        <v>4490</v>
+      </c>
+      <c r="H40" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="I40" s="5">
+        <v>10</v>
+      </c>
+      <c r="K40" s="14"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B41" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="5">
+      <c r="C41" s="5">
         <v>3000</v>
       </c>
-      <c r="D40" s="4">
+      <c r="D41" s="4">
         <f t="shared" si="1"/>
         <v>7490</v>
       </c>
-      <c r="H40" s="16" t="s">
+      <c r="H41" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="I40" s="5">
+      <c r="I41" s="5">
         <v>10</v>
       </c>
-      <c r="K40" s="14"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="16" t="s">
+      <c r="K41" s="14"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B42" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C41" s="5">
+      <c r="C42" s="5">
         <v>2000</v>
       </c>
-      <c r="D41" s="4">
+      <c r="D42" s="4">
         <f t="shared" si="1"/>
         <v>9490</v>
       </c>
-      <c r="H41" s="16" t="s">
+      <c r="H42" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="I41" s="5">
+      <c r="I42" s="5">
         <v>10</v>
       </c>
-      <c r="K41" s="14"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="16" t="s">
+      <c r="K42" s="14"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B43" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C43" s="5">
         <v>3000</v>
       </c>
-      <c r="D42" s="4">
+      <c r="D43" s="4">
         <f t="shared" si="1"/>
         <v>12490</v>
       </c>
-      <c r="H42" s="16" t="s">
+      <c r="H43" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="I42" s="5">
+      <c r="I43" s="5">
         <v>10</v>
       </c>
-      <c r="K42" s="14"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B43" s="4" t="s">
+      <c r="K43" s="14"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B44" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C43" s="5">
+      <c r="C44" s="5">
         <v>-10000</v>
       </c>
-      <c r="D43" s="4">
+      <c r="D44" s="4">
         <f t="shared" si="1"/>
         <v>2490</v>
       </c>
-      <c r="H43" s="16" t="s">
+      <c r="H44" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="I43" s="5">
+      <c r="I44" s="5">
         <v>10</v>
       </c>
-      <c r="K43" s="14"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="16" t="s">
+      <c r="K44" s="14"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B45" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C45" s="5">
         <v>4960</v>
       </c>
-      <c r="D44" s="4">
+      <c r="D45" s="4">
         <f t="shared" si="1"/>
         <v>7450</v>
       </c>
-      <c r="H44" s="16" t="s">
+      <c r="H45" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="I44" s="5">
+      <c r="I45" s="5">
         <v>10</v>
       </c>
-      <c r="K44" s="14"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="16" t="s">
+      <c r="K45" s="14"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B46" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C45" s="5">
+      <c r="C46" s="5">
         <v>4000</v>
       </c>
-      <c r="D45" s="4">
+      <c r="D46" s="4">
         <f t="shared" si="1"/>
         <v>11450</v>
       </c>
-      <c r="H45" s="16" t="s">
+      <c r="H46" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="I45" s="5">
+      <c r="I46" s="5">
         <v>10</v>
       </c>
-      <c r="K45" s="14"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B46" s="4" t="s">
+      <c r="K46" s="14"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B47" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C46" s="5">
+      <c r="C47" s="5">
         <v>-10000</v>
       </c>
-      <c r="D46" s="4">
+      <c r="D47" s="4">
         <f t="shared" si="1"/>
         <v>1450</v>
       </c>
-      <c r="H46" s="16" t="s">
+      <c r="H47" s="16" t="s">
         <v>149</v>
-      </c>
-      <c r="I46" s="5">
-        <v>10</v>
-      </c>
-      <c r="K46" s="14"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B47" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C47" s="5">
-        <v>7640</v>
-      </c>
-      <c r="D47" s="4">
-        <f t="shared" ref="D47:D53" si="2">D46+C47</f>
-        <v>9090</v>
-      </c>
-      <c r="H47" s="16" t="s">
-        <v>185</v>
       </c>
       <c r="I47" s="5">
         <v>10</v>
@@ -1808,367 +1801,371 @@
       <c r="K47" s="14"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B48" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C48" s="5">
+        <v>7640</v>
+      </c>
+      <c r="D48" s="4">
+        <f t="shared" ref="D48:D54" si="2">D47+C48</f>
+        <v>9090</v>
+      </c>
       <c r="H48" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="I48" s="5">
+        <v>10</v>
+      </c>
+      <c r="K48" s="14"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H49" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="I48" s="5">
+      <c r="I49" s="5">
         <v>20</v>
       </c>
-      <c r="K48" s="14"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B49" s="4" t="s">
+      <c r="K49" s="14"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B50" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C49" s="5">
+      <c r="C50" s="5">
         <v>3000</v>
       </c>
-      <c r="D49" s="4">
-        <f>D47+C49</f>
+      <c r="D50" s="4">
+        <f>D48+C50</f>
         <v>12090</v>
       </c>
-      <c r="H49" s="16" t="s">
+      <c r="H50" s="16" t="s">
         <v>187</v>
       </c>
-      <c r="I49" s="5">
+      <c r="I50" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B50" s="4" t="s">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B51" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C50" s="5">
+      <c r="C51" s="5">
         <v>-10000</v>
       </c>
-      <c r="D50" s="4">
+      <c r="D51" s="4">
         <f t="shared" si="2"/>
         <v>2090</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B51" s="4" t="s">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B52" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C51" s="5">
+      <c r="C52" s="5">
         <v>800</v>
       </c>
-      <c r="D51" s="4">
+      <c r="D52" s="4">
         <f t="shared" si="2"/>
         <v>2890</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="16" t="s">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B53" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C52" s="5">
+      <c r="C53" s="5">
         <v>2000</v>
       </c>
-      <c r="D52" s="4">
+      <c r="D53" s="4">
         <f t="shared" si="2"/>
         <v>4890</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="16" t="s">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B54" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C53" s="5">
+      <c r="C54" s="5">
         <v>4000</v>
       </c>
-      <c r="D53" s="4">
+      <c r="D54" s="4">
         <f t="shared" si="2"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="16" t="s">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B55" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C54" s="5">
+      <c r="C55" s="5">
         <v>4000</v>
       </c>
-      <c r="D54" s="4">
-        <f t="shared" ref="D54:D59" si="3">D53+C54</f>
+      <c r="D55" s="4">
+        <f t="shared" ref="D55:D60" si="3">D54+C55</f>
         <v>12890</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B55" s="4" t="s">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B56" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C55" s="5">
+      <c r="C56" s="5">
         <v>5000</v>
       </c>
-      <c r="D55" s="4">
+      <c r="D56" s="4">
         <f t="shared" si="3"/>
         <v>17890</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B56" s="4" t="s">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B57" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C56" s="5">
+      <c r="C57" s="5">
         <v>-10000</v>
       </c>
-      <c r="D56" s="4">
+      <c r="D57" s="4">
         <f t="shared" si="3"/>
         <v>7890</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="16">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="16">
         <v>44969</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B58" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C57" s="5">
+      <c r="C58" s="5">
         <v>900</v>
       </c>
-      <c r="D57" s="4">
+      <c r="D58" s="4">
         <f t="shared" si="3"/>
         <v>8790</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B58" s="4" t="s">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B59" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C58" s="5">
+      <c r="C59" s="5">
         <v>4000</v>
       </c>
-      <c r="D58" s="4">
+      <c r="D59" s="4">
         <f t="shared" si="3"/>
         <v>12790</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B59" s="4" t="s">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B60" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C59" s="5">
+      <c r="C60" s="5">
         <v>-10000</v>
       </c>
-      <c r="D59" s="4">
+      <c r="D60" s="4">
         <f t="shared" si="3"/>
         <v>2790</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="16" t="s">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B61" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C60" s="5">
+      <c r="C61" s="5">
         <v>2000</v>
       </c>
-      <c r="D60" s="4">
-        <f t="shared" ref="D60:D67" si="4">D59+C60</f>
+      <c r="D61" s="4">
+        <f t="shared" ref="D61:D68" si="4">D60+C61</f>
         <v>4790</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="16" t="s">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B62" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C61" s="5">
+      <c r="C62" s="5">
         <v>700</v>
       </c>
-      <c r="D61" s="4">
+      <c r="D62" s="4">
         <f t="shared" si="4"/>
         <v>5490</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B62" s="4" t="s">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B63" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C62" s="5">
+      <c r="C63" s="5">
         <v>4000</v>
       </c>
-      <c r="D62" s="4">
+      <c r="D63" s="4">
         <f t="shared" si="4"/>
         <v>9490</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="16" t="s">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B64" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C63" s="5">
+      <c r="C64" s="5">
         <v>600</v>
       </c>
-      <c r="D63" s="4">
+      <c r="D64" s="4">
         <f t="shared" si="4"/>
         <v>10090</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B64" s="4" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B65" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C64" s="5">
+      <c r="C65" s="5">
         <v>-10000</v>
       </c>
-      <c r="D64" s="4">
+      <c r="D65" s="4">
         <f t="shared" si="4"/>
         <v>90</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="16" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B66" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C65" s="5">
+      <c r="C66" s="5">
         <f>700+5000+300+600+400+1000+800</f>
         <v>8800</v>
       </c>
-      <c r="D65" s="4">
+      <c r="D66" s="4">
         <f t="shared" si="4"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B66" s="4" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B67" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C66" s="5">
+      <c r="C67" s="5">
         <v>6000</v>
       </c>
-      <c r="D66" s="4">
+      <c r="D67" s="4">
         <f t="shared" si="4"/>
         <v>14890</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B67" s="4" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B68" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C67" s="5">
+      <c r="C68" s="5">
         <v>-10000</v>
       </c>
-      <c r="D67" s="4">
+      <c r="D68" s="4">
         <f t="shared" si="4"/>
         <v>4890</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="16" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B69" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C68" s="5">
+      <c r="C69" s="5">
         <v>500</v>
       </c>
-      <c r="D68" s="4">
-        <f t="shared" ref="D68:D73" si="5">D67+C68</f>
+      <c r="D69" s="4">
+        <f t="shared" ref="D69:D74" si="5">D68+C69</f>
         <v>5390</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B69" s="4" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B70" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C69" s="5">
+      <c r="C70" s="5">
         <v>700</v>
       </c>
-      <c r="D69" s="4">
+      <c r="D70" s="4">
         <f t="shared" si="5"/>
         <v>6090</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B70" s="4" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B71" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C70" s="5">
+      <c r="C71" s="5">
         <v>1500</v>
       </c>
-      <c r="D70" s="4">
+      <c r="D71" s="4">
         <f t="shared" si="5"/>
         <v>7590</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B71" s="4" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B72" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C71" s="5">
+      <c r="C72" s="5">
         <v>5000</v>
       </c>
-      <c r="D71" s="4">
+      <c r="D72" s="4">
         <f t="shared" si="5"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B72" s="4" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B73" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C72" s="5">
+      <c r="C73" s="5">
         <v>-10000</v>
       </c>
-      <c r="D72" s="4">
+      <c r="D73" s="4">
         <f t="shared" si="5"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="16" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B74" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C73" s="5">
+      <c r="C74" s="5">
         <v>2000</v>
       </c>
-      <c r="D73" s="4">
+      <c r="D74" s="4">
         <f t="shared" si="5"/>
         <v>4590</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B74" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C74" s="5">
-        <v>700</v>
-      </c>
-      <c r="D74" s="4">
-        <f t="shared" ref="D74:D79" si="6">D73+C74</f>
-        <v>5290</v>
-      </c>
-    </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="16" t="s">
-        <v>82</v>
-      </c>
       <c r="B75" s="4" t="s">
         <v>77</v>
       </c>
@@ -2176,401 +2173,404 @@
         <v>700</v>
       </c>
       <c r="D75" s="4">
+        <f t="shared" ref="D75:D80" si="6">D74+C75</f>
+        <v>5290</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C76" s="5">
+        <v>700</v>
+      </c>
+      <c r="D76" s="4">
         <f t="shared" si="6"/>
         <v>5990</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="16" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B77" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C76" s="5">
+      <c r="C77" s="5">
         <v>700</v>
       </c>
-      <c r="D76" s="4">
+      <c r="D77" s="4">
         <f t="shared" si="6"/>
         <v>6690</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="16" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="B78" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C77" s="5">
+      <c r="C78" s="5">
         <v>4000</v>
       </c>
-      <c r="D77" s="4">
+      <c r="D78" s="4">
         <f t="shared" si="6"/>
         <v>10690</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B78" s="4" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B79" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C78" s="5">
+      <c r="C79" s="5">
         <v>-10000</v>
       </c>
-      <c r="D78" s="4">
+      <c r="D79" s="4">
         <f t="shared" si="6"/>
         <v>690</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="16" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="B79" s="4" t="s">
+      <c r="B80" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C79" s="5">
+      <c r="C80" s="5">
         <v>1000</v>
       </c>
-      <c r="D79" s="4">
+      <c r="D80" s="4">
         <f t="shared" si="6"/>
         <v>1690</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="16" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B81" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C80" s="5">
+      <c r="C81" s="5">
         <v>7000</v>
       </c>
-      <c r="D80" s="4">
-        <f t="shared" ref="D80:D85" si="7">D79+C80</f>
+      <c r="D81" s="4">
+        <f t="shared" ref="D81:D86" si="7">D80+C81</f>
         <v>8690</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B81" s="4" t="s">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B82" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C81" s="5">
+      <c r="C82" s="5">
         <v>10000</v>
       </c>
-      <c r="D81" s="4">
+      <c r="D82" s="4">
         <f t="shared" si="7"/>
         <v>18690</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B82" s="4" t="s">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B83" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C82" s="5">
+      <c r="C83" s="5">
         <v>-10000</v>
       </c>
-      <c r="D82" s="4">
+      <c r="D83" s="4">
         <f t="shared" si="7"/>
         <v>8690</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B83" s="4" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B84" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C83" s="5">
+      <c r="C84" s="5">
         <v>1700</v>
       </c>
-      <c r="D83" s="4">
+      <c r="D84" s="4">
         <f t="shared" si="7"/>
         <v>10390</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B84" s="4" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B85" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C84" s="5">
+      <c r="C85" s="5">
         <v>-10000</v>
       </c>
-      <c r="D84" s="4">
+      <c r="D85" s="4">
         <f t="shared" si="7"/>
         <v>390</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B85" s="4" t="s">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B86" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C85" s="5">
+      <c r="C86" s="5">
         <v>6000</v>
       </c>
-      <c r="D85" s="4">
+      <c r="D86" s="4">
         <f t="shared" si="7"/>
         <v>6390</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="B86" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C86" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D86" s="4">
-        <f t="shared" ref="D86:D91" si="8">D85+C86</f>
-        <v>8390</v>
-      </c>
-    </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C87" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D87" s="4">
+        <f t="shared" ref="D87:D92" si="8">D86+C87</f>
+        <v>8390</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="B87" s="4" t="s">
+      <c r="B88" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C87" s="5">
+      <c r="C88" s="5">
         <v>5000</v>
       </c>
-      <c r="D87" s="4">
+      <c r="D88" s="4">
         <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B88" s="4" t="s">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B89" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C88" s="5">
+      <c r="C89" s="5">
         <v>-10000</v>
       </c>
-      <c r="D88" s="4">
+      <c r="D89" s="4">
         <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="16" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="B89" s="4" t="s">
+      <c r="B90" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C89" s="5">
+      <c r="C90" s="5">
         <v>1000</v>
       </c>
-      <c r="D89" s="4">
+      <c r="D90" s="4">
         <f t="shared" si="8"/>
         <v>4390</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B90" s="4" t="s">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B91" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C90" s="5">
+      <c r="C91" s="5">
         <v>9000</v>
       </c>
-      <c r="D90" s="4">
+      <c r="D91" s="4">
         <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B91" s="4" t="s">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B92" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C91" s="5">
+      <c r="C92" s="5">
         <v>-10000</v>
       </c>
-      <c r="D91" s="4">
+      <c r="D92" s="4">
         <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B92" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C92" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D92" s="4">
-        <f t="shared" ref="D92:D97" si="9">D91+C92</f>
-        <v>5390</v>
-      </c>
-    </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B93" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C93" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D93" s="4">
+        <f t="shared" ref="D93:D98" si="9">D92+C93</f>
+        <v>5390</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B94" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C93" s="5">
+      <c r="C94" s="5">
         <v>6000</v>
       </c>
-      <c r="D93" s="4">
+      <c r="D94" s="4">
         <f t="shared" si="9"/>
         <v>11390</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B94" s="4" t="s">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B95" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C94" s="5">
+      <c r="C95" s="5">
         <v>-10000</v>
       </c>
-      <c r="D94" s="4">
+      <c r="D95" s="4">
         <f t="shared" si="9"/>
         <v>1390</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B95" s="4" t="s">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B96" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C95" s="5">
+      <c r="C96" s="5">
         <v>400</v>
       </c>
-      <c r="D95" s="4">
+      <c r="D96" s="4">
         <f t="shared" si="9"/>
         <v>1790</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="16" t="s">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="B96" s="4" t="s">
+      <c r="B97" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C96" s="5">
+      <c r="C97" s="5">
         <v>2000</v>
       </c>
-      <c r="D96" s="4">
+      <c r="D97" s="4">
         <f t="shared" si="9"/>
         <v>3790</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="16" t="s">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="B97" s="4" t="s">
+      <c r="B98" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C97" s="5">
+      <c r="C98" s="5">
         <v>6000</v>
       </c>
-      <c r="D97" s="4">
+      <c r="D98" s="4">
         <f t="shared" si="9"/>
         <v>9790</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="16" t="s">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="B98" s="4" t="s">
+      <c r="B99" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C98" s="5">
+      <c r="C99" s="5">
         <v>1000</v>
       </c>
-      <c r="D98" s="4">
-        <f t="shared" ref="D98:D103" si="10">D97+C98</f>
+      <c r="D99" s="4">
+        <f t="shared" ref="D99:D104" si="10">D98+C99</f>
         <v>10790</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B99" s="4" t="s">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B100" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C99" s="5">
+      <c r="C100" s="5">
         <v>-10000</v>
       </c>
-      <c r="D99" s="4">
+      <c r="D100" s="4">
         <f t="shared" si="10"/>
         <v>790</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="16" t="s">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="B100" s="4" t="s">
+      <c r="B101" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C100" s="5">
+      <c r="C101" s="5">
         <v>800</v>
       </c>
-      <c r="D100" s="4">
+      <c r="D101" s="4">
         <f t="shared" si="10"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="16" t="s">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="B101" s="4" t="s">
+      <c r="B102" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C101" s="5">
+      <c r="C102" s="5">
         <v>5000</v>
       </c>
-      <c r="D101" s="4">
+      <c r="D102" s="4">
         <f t="shared" si="10"/>
         <v>6590</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="16" t="s">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="B102" s="4" t="s">
+      <c r="B103" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C102" s="5">
+      <c r="C103" s="5">
         <v>6000</v>
       </c>
-      <c r="D102" s="4">
+      <c r="D103" s="4">
         <f t="shared" si="10"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B103" s="4" t="s">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B104" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C103" s="5">
+      <c r="C104" s="5">
         <v>-10000</v>
       </c>
-      <c r="D103" s="4">
+      <c r="D104" s="4">
         <f t="shared" si="10"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="16" t="s">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="B104" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C104" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D104" s="4">
-        <f t="shared" ref="D104:D110" si="11">D103+C104</f>
-        <v>4590</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B105" s="4" t="s">
         <v>65</v>
       </c>
@@ -2578,926 +2578,926 @@
         <v>2000</v>
       </c>
       <c r="D105" s="4">
+        <f t="shared" ref="D105:D111" si="11">D104+C105</f>
+        <v>4590</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B106" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C106" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D106" s="4">
         <f t="shared" si="11"/>
         <v>6590</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B106" s="4" t="s">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B107" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C106" s="5">
+      <c r="C107" s="5">
         <v>7000</v>
       </c>
-      <c r="D106" s="4">
+      <c r="D107" s="4">
         <f t="shared" si="11"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B107" s="4" t="s">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B108" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C107" s="5">
+      <c r="C108" s="5">
         <v>-10000</v>
       </c>
-      <c r="D107" s="4">
+      <c r="D108" s="4">
         <f t="shared" si="11"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="16" t="s">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="B108" s="4" t="s">
+      <c r="B109" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C108" s="5">
+      <c r="C109" s="5">
         <v>2000</v>
       </c>
-      <c r="D108" s="4">
+      <c r="D109" s="4">
         <f t="shared" si="11"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="16" t="s">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="B109" s="4" t="s">
+      <c r="B110" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C109" s="5">
+      <c r="C110" s="5">
         <v>6000</v>
       </c>
-      <c r="D109" s="4">
+      <c r="D110" s="4">
         <f t="shared" si="11"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B110" s="4" t="s">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B111" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C110" s="5">
+      <c r="C111" s="5">
         <v>-10000</v>
       </c>
-      <c r="D110" s="4">
+      <c r="D111" s="4">
         <f t="shared" si="11"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="B111" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C111" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D111" s="4">
-        <f t="shared" ref="D111:D116" si="12">D110+C111</f>
-        <v>3590</v>
-      </c>
-    </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B112" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C112" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D112" s="4">
+        <f t="shared" ref="D112:D117" si="12">D111+C112</f>
+        <v>3590</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="B112" s="4" t="s">
+      <c r="B113" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C112" s="5">
+      <c r="C113" s="5">
         <v>7000</v>
       </c>
-      <c r="D112" s="4">
+      <c r="D113" s="4">
         <f t="shared" si="12"/>
         <v>10590</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B113" s="4" t="s">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B114" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C113" s="5">
+      <c r="C114" s="5">
         <v>-10000</v>
       </c>
-      <c r="D113" s="4">
+      <c r="D114" s="4">
         <f t="shared" si="12"/>
         <v>590</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B114" s="4" t="s">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B115" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C114" s="5">
+      <c r="C115" s="5">
         <v>12000</v>
       </c>
-      <c r="D114" s="4">
+      <c r="D115" s="4">
         <f t="shared" si="12"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B115" s="4" t="s">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B116" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C115" s="5">
+      <c r="C116" s="5">
         <v>-10000</v>
       </c>
-      <c r="D115" s="4">
+      <c r="D116" s="4">
         <f t="shared" si="12"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B116" s="4" t="s">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B117" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C116" s="5">
+      <c r="C117" s="5">
         <v>2000</v>
       </c>
-      <c r="D116" s="4">
+      <c r="D117" s="4">
         <f t="shared" si="12"/>
         <v>4590</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="B117" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C117" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D117" s="4">
-        <f t="shared" ref="D117:D122" si="13">D116+C117</f>
-        <v>6590</v>
-      </c>
-    </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="B118" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C118" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D118" s="4">
+        <f t="shared" ref="D118:D123" si="13">D117+C118</f>
+        <v>6590</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="B118" s="4" t="s">
+      <c r="B119" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C118" s="5">
+      <c r="C119" s="5">
         <v>7000</v>
       </c>
-      <c r="D118" s="4">
+      <c r="D119" s="4">
         <f t="shared" si="13"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B119" s="4" t="s">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B120" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C119" s="5">
+      <c r="C120" s="5">
         <v>-10000</v>
       </c>
-      <c r="D119" s="4">
+      <c r="D120" s="4">
         <f t="shared" si="13"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="16" t="s">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="B120" s="4" t="s">
+      <c r="B121" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C120" s="5">
+      <c r="C121" s="5">
         <v>2000</v>
       </c>
-      <c r="D120" s="4">
+      <c r="D121" s="4">
         <f t="shared" si="13"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="16" t="s">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="B121" s="4" t="s">
+      <c r="B122" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C121" s="5">
+      <c r="C122" s="5">
         <v>8000</v>
       </c>
-      <c r="D121" s="4">
+      <c r="D122" s="4">
         <f t="shared" si="13"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B122" s="4" t="s">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B123" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C122" s="5">
+      <c r="C123" s="5">
         <v>-10000</v>
       </c>
-      <c r="D122" s="4">
+      <c r="D123" s="4">
         <f t="shared" si="13"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="16" t="s">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="B123" s="4" t="s">
+      <c r="B124" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C123" s="5">
+      <c r="C124" s="5">
         <v>2000</v>
       </c>
-      <c r="D123" s="4">
-        <f t="shared" ref="D123:D128" si="14">D122+C123</f>
+      <c r="D124" s="4">
+        <f t="shared" ref="D124:D129" si="14">D123+C124</f>
         <v>5590</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B124" s="4" t="s">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B125" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C124" s="5">
+      <c r="C125" s="5">
         <v>5000</v>
       </c>
-      <c r="D124" s="4">
+      <c r="D125" s="4">
         <f t="shared" si="14"/>
         <v>10590</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B125" s="4" t="s">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B126" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C125" s="5">
+      <c r="C126" s="5">
         <v>-10000</v>
       </c>
-      <c r="D125" s="4">
+      <c r="D126" s="4">
         <f t="shared" si="14"/>
         <v>590</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B126" s="4" t="s">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B127" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C126" s="5">
+      <c r="C127" s="5">
         <v>2000</v>
       </c>
-      <c r="D126" s="4">
+      <c r="D127" s="4">
         <f t="shared" si="14"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B127" s="4" t="s">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B128" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C127" s="5">
+      <c r="C128" s="5">
         <v>9000</v>
       </c>
-      <c r="D127" s="4">
+      <c r="D128" s="4">
         <f t="shared" si="14"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B128" s="4" t="s">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B129" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C128" s="5">
+      <c r="C129" s="5">
         <v>-10000</v>
       </c>
-      <c r="D128" s="4">
+      <c r="D129" s="4">
         <f t="shared" si="14"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B129" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C129" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D129" s="4">
-        <f t="shared" ref="D129:D134" si="15">D128+C129</f>
-        <v>3590</v>
-      </c>
-    </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B130" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C130" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D130" s="4">
+        <f t="shared" ref="D130:D135" si="15">D129+C130</f>
+        <v>3590</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="B130" s="4" t="s">
+      <c r="B131" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C130" s="5">
+      <c r="C131" s="5">
         <v>8000</v>
       </c>
-      <c r="D130" s="4">
+      <c r="D131" s="4">
         <f t="shared" si="15"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B131" s="4" t="s">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B132" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C131" s="5">
+      <c r="C132" s="5">
         <v>-10000</v>
       </c>
-      <c r="D131" s="4">
+      <c r="D132" s="4">
         <f t="shared" si="15"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="16" t="s">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="B132" s="4" t="s">
+      <c r="B133" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C132" s="5">
+      <c r="C133" s="5">
         <v>2000</v>
       </c>
-      <c r="D132" s="4">
+      <c r="D133" s="4">
         <f t="shared" si="15"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="16" t="s">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="B133" s="4" t="s">
+      <c r="B134" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C133" s="5">
+      <c r="C134" s="5">
         <v>12000</v>
       </c>
-      <c r="D133" s="4">
+      <c r="D134" s="4">
         <f t="shared" si="15"/>
         <v>15590</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B134" s="4" t="s">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B135" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C134" s="5">
+      <c r="C135" s="5">
         <v>-10000</v>
       </c>
-      <c r="D134" s="4">
+      <c r="D135" s="4">
         <f t="shared" si="15"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="B135" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="C135" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D135" s="4">
-        <f t="shared" ref="D135:D140" si="16">D134+C135</f>
-        <v>7590</v>
-      </c>
-    </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="B136" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C136" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D136" s="4">
+        <f t="shared" ref="D136:D141" si="16">D135+C136</f>
+        <v>7590</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="B136" s="4" t="s">
+      <c r="B137" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="C136" s="5">
+      <c r="C137" s="5">
         <v>10000</v>
       </c>
-      <c r="D136" s="4">
+      <c r="D137" s="4">
         <f t="shared" si="16"/>
         <v>17590</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B137" s="4" t="s">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B138" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C137" s="5">
+      <c r="C138" s="5">
         <v>-10000</v>
       </c>
-      <c r="D137" s="4">
+      <c r="D138" s="4">
         <f t="shared" si="16"/>
         <v>7590</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B138" s="4" t="s">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B139" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="C138" s="5">
+      <c r="C139" s="5">
         <v>2000</v>
       </c>
-      <c r="D138" s="4">
+      <c r="D139" s="4">
         <f t="shared" si="16"/>
         <v>9590</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="16" t="s">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="B139" s="4" t="s">
+      <c r="B140" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="C139" s="5">
+      <c r="C140" s="5">
         <v>-1200</v>
       </c>
-      <c r="D139" s="4">
+      <c r="D140" s="4">
         <f t="shared" si="16"/>
         <v>8390</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B140" s="4" t="s">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B141" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="C140" s="5">
+      <c r="C141" s="5">
         <v>500</v>
       </c>
-      <c r="D140" s="4">
+      <c r="D141" s="4">
         <f t="shared" si="16"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="16" t="s">
-        <v>165</v>
-      </c>
-      <c r="B141" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="C141" s="5">
-        <v>750</v>
-      </c>
-      <c r="D141" s="4">
-        <f t="shared" ref="D141:D146" si="17">D140+C141</f>
-        <v>9640</v>
-      </c>
-    </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="B142" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C142" s="5">
+        <v>750</v>
+      </c>
+      <c r="D142" s="4">
+        <f t="shared" ref="D142:D147" si="17">D141+C142</f>
+        <v>9640</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="B142" s="4" t="s">
+      <c r="B143" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C142" s="5">
+      <c r="C143" s="5">
         <v>2000</v>
       </c>
-      <c r="D142" s="4">
+      <c r="D143" s="4">
         <f t="shared" si="17"/>
         <v>11640</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B143" s="4" t="s">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B144" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C143" s="5">
+      <c r="C144" s="5">
         <v>2000</v>
       </c>
-      <c r="D143" s="4">
+      <c r="D144" s="4">
         <f t="shared" si="17"/>
         <v>13640</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B144" s="4" t="s">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B145" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C144" s="5">
+      <c r="C145" s="5">
         <v>-10000</v>
       </c>
-      <c r="D144" s="4">
+      <c r="D145" s="4">
         <f t="shared" si="17"/>
         <v>3640</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B145" s="4" t="s">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B146" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="C145" s="5">
+      <c r="C146" s="5">
         <v>350</v>
       </c>
-      <c r="D145" s="4">
+      <c r="D146" s="4">
         <f t="shared" si="17"/>
         <v>3990</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="16" t="s">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="B146" s="4" t="s">
+      <c r="B147" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="C146" s="5">
+      <c r="C147" s="5">
         <v>300</v>
       </c>
-      <c r="D146" s="4">
+      <c r="D147" s="4">
         <f t="shared" si="17"/>
         <v>4290</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="16" t="s">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="B147" s="4" t="s">
+      <c r="B148" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="C147" s="5">
+      <c r="C148" s="5">
         <v>3800</v>
       </c>
-      <c r="D147" s="4">
-        <f t="shared" ref="D147:D153" si="18">D146+C147</f>
+      <c r="D148" s="4">
+        <f t="shared" ref="D148:D154" si="18">D147+C148</f>
         <v>8090</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B148" s="4" t="s">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B149" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C148" s="5">
+      <c r="C149" s="5">
         <v>500</v>
       </c>
-      <c r="D148" s="4">
+      <c r="D149" s="4">
         <f t="shared" si="18"/>
         <v>8590</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="16" t="s">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="B149" s="4" t="s">
+      <c r="B150" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="C149" s="5">
+      <c r="C150" s="5">
         <v>1300</v>
       </c>
-      <c r="D149" s="4">
+      <c r="D150" s="4">
         <f t="shared" si="18"/>
         <v>9890</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="16" t="s">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="B150" s="4" t="s">
+      <c r="B151" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C150" s="5">
+      <c r="C151" s="5">
         <v>9000</v>
       </c>
-      <c r="D150" s="4">
+      <c r="D151" s="4">
         <f t="shared" si="18"/>
         <v>18890</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B151" s="4" t="s">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B152" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C151" s="5">
+      <c r="C152" s="5">
         <v>-10000</v>
       </c>
-      <c r="D151" s="4">
+      <c r="D152" s="4">
         <f t="shared" si="18"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="16" t="s">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="B152" s="4" t="s">
+      <c r="B153" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C152" s="5">
+      <c r="C153" s="5">
         <v>2000</v>
       </c>
-      <c r="D152" s="4">
+      <c r="D153" s="4">
         <f t="shared" si="18"/>
         <v>10890</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B153" s="4" t="s">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B154" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C153" s="5">
+      <c r="C154" s="5">
         <v>-10000</v>
       </c>
-      <c r="D153" s="4">
+      <c r="D154" s="4">
         <f t="shared" si="18"/>
         <v>890</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="B154" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="C154" s="5">
-        <v>500</v>
-      </c>
-      <c r="D154" s="4">
-        <f t="shared" ref="D154:D159" si="19">D153+C154</f>
-        <v>1390</v>
-      </c>
-    </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="B155" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C155" s="5">
+        <v>500</v>
+      </c>
+      <c r="D155" s="4">
+        <f t="shared" ref="D155:D160" si="19">D154+C155</f>
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="B155" s="4" t="s">
+      <c r="B156" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="C155" s="5">
+      <c r="C156" s="5">
         <v>10000</v>
       </c>
-      <c r="D155" s="4">
+      <c r="D156" s="4">
         <f t="shared" si="19"/>
         <v>11390</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B156" s="4" t="s">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B157" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C156" s="5">
+      <c r="C157" s="5">
         <v>-10000</v>
       </c>
-      <c r="D156" s="4">
+      <c r="D157" s="4">
         <f t="shared" si="19"/>
         <v>1390</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="16" t="s">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="B157" s="4" t="s">
+      <c r="B158" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C157" s="5">
+      <c r="C158" s="5">
         <v>3000</v>
       </c>
-      <c r="D157" s="4">
+      <c r="D158" s="4">
         <f t="shared" si="19"/>
         <v>4390</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="16" t="s">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="B158" s="4" t="s">
+      <c r="B159" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C158" s="5">
+      <c r="C159" s="5">
         <v>2000</v>
       </c>
-      <c r="D158" s="4">
+      <c r="D159" s="4">
         <f t="shared" si="19"/>
         <v>6390</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B159" s="4" t="s">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B160" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C159" s="5">
+      <c r="C160" s="5">
         <v>2000</v>
       </c>
-      <c r="D159" s="4">
+      <c r="D160" s="4">
         <f t="shared" si="19"/>
         <v>8390</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="16" t="s">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="B160" s="4" t="s">
+      <c r="B161" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C160" s="5">
+      <c r="C161" s="5">
         <v>11000</v>
       </c>
-      <c r="D160" s="4">
-        <f t="shared" ref="D160:D165" si="20">D159+C160</f>
+      <c r="D161" s="4">
+        <f t="shared" ref="D161:D166" si="20">D160+C161</f>
         <v>19390</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B161" s="4" t="s">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B162" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C161" s="5">
+      <c r="C162" s="5">
         <v>-10000</v>
       </c>
-      <c r="D161" s="4">
+      <c r="D162" s="4">
         <f t="shared" si="20"/>
         <v>9390</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" s="16" t="s">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" s="16" t="s">
         <v>187</v>
       </c>
-      <c r="B162" s="4" t="s">
+      <c r="B163" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C162" s="5">
+      <c r="C163" s="5">
         <v>3000</v>
       </c>
-      <c r="D162" s="4">
+      <c r="D163" s="4">
         <f t="shared" si="20"/>
         <v>12390</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B163" s="4" t="s">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B164" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C163" s="5">
+      <c r="C164" s="5">
         <v>-10000</v>
       </c>
-      <c r="D163" s="4">
+      <c r="D164" s="4">
         <f t="shared" si="20"/>
         <v>2390</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B164" s="4" t="s">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B165" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C164" s="5">
+      <c r="C165" s="5">
         <v>500</v>
       </c>
-      <c r="D164" s="4">
+      <c r="D165" s="4">
         <f t="shared" si="20"/>
         <v>2890</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" s="16" t="s">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" s="16" t="s">
         <v>189</v>
       </c>
-      <c r="B165" s="4" t="s">
+      <c r="B166" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C165" s="5">
+      <c r="C166" s="5">
         <v>5600</v>
       </c>
-      <c r="D165" s="4">
+      <c r="D166" s="4">
         <f t="shared" si="20"/>
         <v>8490</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B166" s="4" t="s">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B167" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="C166" s="5">
+      <c r="C167" s="5">
         <v>4700</v>
       </c>
-      <c r="D166" s="4">
-        <f t="shared" ref="D166:D172" si="21">D165+C166</f>
+      <c r="D167" s="4">
+        <f t="shared" ref="D167:D173" si="21">D166+C167</f>
         <v>13190</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A167" s="16" t="s">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" s="16" t="s">
         <v>192</v>
       </c>
-      <c r="B167" s="4" t="s">
+      <c r="B168" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C167" s="5">
+      <c r="C168" s="5">
         <v>1500</v>
       </c>
-      <c r="D167" s="4">
+      <c r="D168" s="4">
         <f t="shared" si="21"/>
         <v>14690</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B168" s="4" t="s">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B169" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C168" s="5">
+      <c r="C169" s="5">
         <v>500</v>
       </c>
-      <c r="D168" s="4">
+      <c r="D169" s="4">
         <f t="shared" si="21"/>
         <v>15190</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A169" s="16" t="s">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="B169" s="4" t="s">
+      <c r="B170" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="C169" s="5">
+      <c r="C170" s="5">
         <v>1000</v>
       </c>
-      <c r="D169" s="4">
+      <c r="D170" s="4">
         <f t="shared" si="21"/>
         <v>16190</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" s="16" t="s">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="B170" s="4" t="s">
+      <c r="B171" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="C170" s="5">
+      <c r="C171" s="5">
         <v>1000</v>
       </c>
-      <c r="D170" s="4">
+      <c r="D171" s="4">
         <f t="shared" si="21"/>
         <v>17190</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" s="16" t="s">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="B171" s="4" t="s">
+      <c r="B172" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C171" s="5">
+      <c r="C172" s="5">
         <v>3000</v>
       </c>
-      <c r="D171" s="4">
+      <c r="D172" s="4">
         <f t="shared" si="21"/>
         <v>20190</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B172" s="4" t="s">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B173" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C172" s="5">
+      <c r="C173" s="5">
         <v>-20000</v>
       </c>
-      <c r="D172" s="4">
+      <c r="D173" s="4">
         <f t="shared" si="21"/>
         <v>190</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B173" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C173" s="5">
-        <v>500</v>
-      </c>
-      <c r="D173" s="4">
-        <f t="shared" ref="D173:D179" si="22">D172+C173</f>
-        <v>690</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -3508,149 +3508,188 @@
         <v>500</v>
       </c>
       <c r="D174" s="4">
+        <f t="shared" ref="D174:D180" si="22">D173+C174</f>
+        <v>690</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B175" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C175" s="5">
+        <v>500</v>
+      </c>
+      <c r="D175" s="4">
         <f t="shared" si="22"/>
         <v>1190</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A175" s="16" t="s">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="B175" s="4" t="s">
+      <c r="B176" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="C175" s="5">
+      <c r="C176" s="5">
         <v>10000</v>
       </c>
-      <c r="D175" s="4">
+      <c r="D176" s="4">
         <f t="shared" si="22"/>
         <v>11190</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B176" s="4" t="s">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B177" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C176" s="5">
+      <c r="C177" s="5">
         <v>-10000</v>
       </c>
-      <c r="D176" s="4">
+      <c r="D177" s="4">
         <f t="shared" si="22"/>
         <v>1190</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A177" s="16" t="s">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A178" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="B177" s="4" t="s">
+      <c r="B178" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C177" s="5">
+      <c r="C178" s="5">
         <v>3000</v>
       </c>
-      <c r="D177" s="4">
+      <c r="D178" s="4">
         <f t="shared" si="22"/>
         <v>4190</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A178" s="16" t="s">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A179" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="B178" s="4" t="s">
+      <c r="B179" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C178" s="5">
+      <c r="C179" s="5">
         <v>11000</v>
       </c>
-      <c r="D178" s="4">
+      <c r="D179" s="4">
         <f t="shared" si="22"/>
         <v>15190</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B179" s="4" t="s">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B180" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C179" s="5">
+      <c r="C180" s="5">
         <v>-10000</v>
       </c>
-      <c r="D179" s="4">
+      <c r="D180" s="4">
         <f t="shared" si="22"/>
         <v>5190</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="B180" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C180" s="5">
-        <v>3000</v>
-      </c>
-      <c r="D180" s="4">
-        <f>D179+C180</f>
-        <v>8190</v>
-      </c>
-    </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="16" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B181" s="4" t="s">
-        <v>208</v>
+        <v>28</v>
       </c>
       <c r="C181" s="5">
-        <v>14000</v>
+        <v>3000</v>
       </c>
       <c r="D181" s="4">
         <f>D180+C181</f>
-        <v>22190</v>
+        <v>8190</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182" s="16" t="s">
+        <v>210</v>
+      </c>
       <c r="B182" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C182" s="5">
-        <v>-20000</v>
+        <v>14000</v>
       </c>
       <c r="D182" s="4">
         <f>D181+C182</f>
-        <v>2190</v>
+        <v>22190</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183" s="16" t="s">
-        <v>211</v>
-      </c>
       <c r="B183" s="4" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C183" s="5">
-        <v>5000</v>
+        <v>-20000</v>
       </c>
       <c r="D183" s="4">
         <f>D182+C183</f>
-        <v>7190</v>
+        <v>2190</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="16" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B184" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C184" s="5">
         <v>5000</v>
       </c>
       <c r="D184" s="4">
         <f>D183+C184</f>
+        <v>7190</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A185" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="B185" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="C185" s="5">
+        <v>5000</v>
+      </c>
+      <c r="D185" s="4">
+        <f>D184+C185</f>
         <v>12190</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="B186" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C186" s="5">
+        <v>11000</v>
+      </c>
+      <c r="D186" s="4">
+        <f>D185+C186</f>
+        <v>23190</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B187" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="C187" s="5">
+        <v>-20000</v>
+      </c>
+      <c r="D187" s="4">
+        <f>D186+C187</f>
+        <v>3190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
co Yen tra 1tr
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="CÔ DIỄM" sheetId="1" r:id="rId1"/>
@@ -1140,7 +1140,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K189"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D190" sqref="D190"/>
     </sheetView>
@@ -4236,8 +4236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4288,7 +4288,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>113</v>
       </c>
@@ -4296,12 +4296,12 @@
         <v>9300</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>114</v>
       </c>
       <c r="B7">
-        <v>2200</v>
+        <v>2500</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>203</v>
@@ -4332,7 +4332,7 @@
       </c>
       <c r="B22">
         <f>SUM(B1:B19)</f>
-        <v>594080</v>
+        <v>594380</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
duy lay tien loi co diem ngay 30
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="CÔ DIỄM" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="219">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -669,6 +669,12 @@
   </si>
   <si>
     <t>23/09/2024</t>
+  </si>
+  <si>
+    <t>30/09/2024</t>
+  </si>
+  <si>
+    <t>Duy lấy 12tr tiền lời</t>
   </si>
 </sst>
 </file>
@@ -1138,11 +1144,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K189"/>
+  <dimension ref="A1:K192"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D190" sqref="D190"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P43" sqref="P43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1218,8 +1224,8 @@
         <v>20</v>
       </c>
       <c r="J3" s="4">
-        <f>SUM(I3:I64)</f>
-        <v>530</v>
+        <f>SUM(I3:I65)</f>
+        <v>540</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1544,30 +1550,30 @@
       <c r="K32" s="14"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="16" t="s">
+      <c r="H33" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="I33" s="5">
+        <v>10</v>
+      </c>
+      <c r="K33" s="14"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B34" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C34" s="5">
         <v>3000</v>
       </c>
-      <c r="D33" s="4">
-        <f>D23+C33</f>
+      <c r="D34" s="4">
+        <f>D23+C34</f>
         <v>8490</v>
       </c>
-      <c r="H33" s="16" t="s">
+      <c r="H34" s="16" t="s">
         <v>12</v>
-      </c>
-      <c r="I33" s="5">
-        <v>10</v>
-      </c>
-      <c r="K33" s="14"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H34" s="16" t="s">
-        <v>43</v>
       </c>
       <c r="I34" s="5">
         <v>10</v>
@@ -1576,7 +1582,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H35" s="16" t="s">
-        <v>139</v>
+        <v>43</v>
       </c>
       <c r="I35" s="5">
         <v>10</v>
@@ -1585,7 +1591,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H36" s="16" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="I36" s="5">
         <v>10</v>
@@ -1594,64 +1600,54 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H37" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="I37" s="5">
+        <v>10</v>
+      </c>
+      <c r="K37" s="14"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H38" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="I37" s="5">
-        <v>10</v>
-      </c>
-      <c r="K37" s="14"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B38" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C38" s="5">
-        <v>4400</v>
-      </c>
-      <c r="D38" s="4">
-        <f>D33+C38</f>
-        <v>12890</v>
-      </c>
-      <c r="H38" s="16" t="s">
-        <v>157</v>
-      </c>
       <c r="I38" s="5">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K38" s="14"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C39" s="5">
-        <v>-10000</v>
+        <v>4400</v>
       </c>
       <c r="D39" s="4">
-        <f>D38+C39</f>
-        <v>2890</v>
+        <f>D34+C39</f>
+        <v>12890</v>
       </c>
       <c r="H39" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I39" s="5">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="K39" s="14"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C40" s="5">
-        <v>1600</v>
+        <v>-10000</v>
       </c>
       <c r="D40" s="4">
-        <f t="shared" ref="D40:D47" si="1">D39+C40</f>
-        <v>4490</v>
+        <f>D39+C40</f>
+        <v>2890</v>
       </c>
       <c r="H40" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I40" s="5">
         <v>10</v>
@@ -1660,530 +1656,534 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C41" s="5">
+        <v>1600</v>
+      </c>
+      <c r="D41" s="4">
+        <f t="shared" ref="D41:D48" si="1">D40+C41</f>
+        <v>4490</v>
+      </c>
+      <c r="H41" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="I41" s="5">
+        <v>10</v>
+      </c>
+      <c r="K41" s="14"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B42" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="5">
+      <c r="C42" s="5">
         <v>3000</v>
       </c>
-      <c r="D41" s="4">
+      <c r="D42" s="4">
         <f t="shared" si="1"/>
         <v>7490</v>
       </c>
-      <c r="H41" s="16" t="s">
+      <c r="H42" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="I41" s="5">
-        <v>10</v>
-      </c>
-      <c r="K41" s="14"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="16" t="s">
+      <c r="I42" s="5">
+        <v>10</v>
+      </c>
+      <c r="K42" s="14"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B43" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C43" s="5">
         <v>2000</v>
       </c>
-      <c r="D42" s="4">
+      <c r="D43" s="4">
         <f t="shared" si="1"/>
         <v>9490</v>
       </c>
-      <c r="H42" s="16" t="s">
+      <c r="H43" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="I42" s="5">
-        <v>10</v>
-      </c>
-      <c r="K42" s="14"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="16" t="s">
+      <c r="I43" s="5">
+        <v>10</v>
+      </c>
+      <c r="K43" s="14"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B44" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C43" s="5">
+      <c r="C44" s="5">
         <v>3000</v>
       </c>
-      <c r="D43" s="4">
+      <c r="D44" s="4">
         <f t="shared" si="1"/>
         <v>12490</v>
       </c>
-      <c r="H43" s="16" t="s">
+      <c r="H44" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="I43" s="5">
-        <v>10</v>
-      </c>
-      <c r="K43" s="14"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B44" s="4" t="s">
+      <c r="I44" s="5">
+        <v>10</v>
+      </c>
+      <c r="K44" s="14"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B45" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C45" s="5">
         <v>-10000</v>
       </c>
-      <c r="D44" s="4">
+      <c r="D45" s="4">
         <f t="shared" si="1"/>
         <v>2490</v>
       </c>
-      <c r="H44" s="16" t="s">
+      <c r="H45" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="I44" s="5">
-        <v>10</v>
-      </c>
-      <c r="K44" s="14"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="16" t="s">
+      <c r="I45" s="5">
+        <v>10</v>
+      </c>
+      <c r="K45" s="14"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B46" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C45" s="5">
+      <c r="C46" s="5">
         <v>4960</v>
       </c>
-      <c r="D45" s="4">
+      <c r="D46" s="4">
         <f t="shared" si="1"/>
         <v>7450</v>
       </c>
-      <c r="H45" s="16" t="s">
+      <c r="H46" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="I45" s="5">
-        <v>10</v>
-      </c>
-      <c r="K45" s="14"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="16" t="s">
+      <c r="I46" s="5">
+        <v>10</v>
+      </c>
+      <c r="K46" s="14"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B47" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C46" s="5">
+      <c r="C47" s="5">
         <v>4000</v>
       </c>
-      <c r="D46" s="4">
+      <c r="D47" s="4">
         <f t="shared" si="1"/>
         <v>11450</v>
       </c>
-      <c r="H46" s="16" t="s">
+      <c r="H47" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="I46" s="5">
-        <v>10</v>
-      </c>
-      <c r="K46" s="14"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B47" s="4" t="s">
+      <c r="I47" s="5">
+        <v>10</v>
+      </c>
+      <c r="K47" s="14"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B48" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C48" s="5">
         <v>-10000</v>
       </c>
-      <c r="D47" s="4">
+      <c r="D48" s="4">
         <f t="shared" si="1"/>
         <v>1450</v>
       </c>
-      <c r="H47" s="16" t="s">
+      <c r="H48" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="I47" s="5">
-        <v>10</v>
-      </c>
-      <c r="K47" s="14"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B48" s="4" t="s">
+      <c r="I48" s="5">
+        <v>10</v>
+      </c>
+      <c r="K48" s="14"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B49" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C48" s="5">
+      <c r="C49" s="5">
         <v>7640</v>
       </c>
-      <c r="D48" s="4">
-        <f t="shared" ref="D48:D54" si="2">D47+C48</f>
+      <c r="D49" s="4">
+        <f t="shared" ref="D49:D55" si="2">D48+C49</f>
         <v>9090</v>
       </c>
-      <c r="H48" s="16" t="s">
+      <c r="H49" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="I48" s="5">
-        <v>10</v>
-      </c>
-      <c r="K48" s="14"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H49" s="16" t="s">
+      <c r="I49" s="5">
+        <v>10</v>
+      </c>
+      <c r="K49" s="14"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H50" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="I49" s="5">
+      <c r="I50" s="5">
         <v>20</v>
       </c>
-      <c r="K49" s="14"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B50" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C50" s="5">
-        <v>3000</v>
-      </c>
-      <c r="D50" s="4">
-        <f>D48+C50</f>
-        <v>12090</v>
-      </c>
-      <c r="H50" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="I50" s="5">
-        <v>10</v>
-      </c>
+      <c r="K50" s="14"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C51" s="5">
+        <v>3000</v>
+      </c>
+      <c r="D51" s="4">
+        <f>D49+C51</f>
+        <v>12090</v>
+      </c>
+      <c r="H51" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="I51" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B52" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C51" s="5">
+      <c r="C52" s="5">
         <v>-10000</v>
       </c>
-      <c r="D51" s="4">
+      <c r="D52" s="4">
         <f t="shared" si="2"/>
         <v>2090</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B52" s="4" t="s">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B53" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C52" s="5">
+      <c r="C53" s="5">
         <v>800</v>
       </c>
-      <c r="D52" s="4">
+      <c r="D53" s="4">
         <f t="shared" si="2"/>
         <v>2890</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="16" t="s">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B54" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C53" s="5">
+      <c r="C54" s="5">
         <v>2000</v>
       </c>
-      <c r="D53" s="4">
+      <c r="D54" s="4">
         <f t="shared" si="2"/>
         <v>4890</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="16" t="s">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B55" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C54" s="5">
+      <c r="C55" s="5">
         <v>4000</v>
       </c>
-      <c r="D54" s="4">
+      <c r="D55" s="4">
         <f t="shared" si="2"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="16" t="s">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B56" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C55" s="5">
+      <c r="C56" s="5">
         <v>4000</v>
       </c>
-      <c r="D55" s="4">
-        <f t="shared" ref="D55:D60" si="3">D54+C55</f>
+      <c r="D56" s="4">
+        <f t="shared" ref="D56:D61" si="3">D55+C56</f>
         <v>12890</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B56" s="4" t="s">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B57" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C56" s="5">
+      <c r="C57" s="5">
         <v>5000</v>
       </c>
-      <c r="D56" s="4">
+      <c r="D57" s="4">
         <f t="shared" si="3"/>
         <v>17890</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B57" s="4" t="s">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B58" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C57" s="5">
+      <c r="C58" s="5">
         <v>-10000</v>
       </c>
-      <c r="D57" s="4">
+      <c r="D58" s="4">
         <f t="shared" si="3"/>
         <v>7890</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="16">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="16">
         <v>44969</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B59" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C58" s="5">
+      <c r="C59" s="5">
         <v>900</v>
       </c>
-      <c r="D58" s="4">
+      <c r="D59" s="4">
         <f t="shared" si="3"/>
         <v>8790</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B59" s="4" t="s">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B60" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C59" s="5">
+      <c r="C60" s="5">
         <v>4000</v>
       </c>
-      <c r="D59" s="4">
+      <c r="D60" s="4">
         <f t="shared" si="3"/>
         <v>12790</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B60" s="4" t="s">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B61" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C60" s="5">
+      <c r="C61" s="5">
         <v>-10000</v>
       </c>
-      <c r="D60" s="4">
+      <c r="D61" s="4">
         <f t="shared" si="3"/>
         <v>2790</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C61" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D61" s="4">
-        <f t="shared" ref="D61:D68" si="4">D60+C61</f>
-        <v>4790</v>
-      </c>
-    </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D62" s="4">
+        <f t="shared" ref="D62:D69" si="4">D61+C62</f>
+        <v>4790</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B63" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C62" s="5">
+      <c r="C63" s="5">
         <v>700</v>
       </c>
-      <c r="D62" s="4">
+      <c r="D63" s="4">
         <f t="shared" si="4"/>
         <v>5490</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B63" s="4" t="s">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B64" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C63" s="5">
+      <c r="C64" s="5">
         <v>4000</v>
       </c>
-      <c r="D63" s="4">
+      <c r="D64" s="4">
         <f t="shared" si="4"/>
         <v>9490</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64" s="16" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B65" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C64" s="5">
+      <c r="C65" s="5">
         <v>600</v>
       </c>
-      <c r="D64" s="4">
+      <c r="D65" s="4">
         <f t="shared" si="4"/>
         <v>10090</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B65" s="4" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C65" s="5">
+      <c r="C66" s="5">
         <v>-10000</v>
       </c>
-      <c r="D65" s="4">
+      <c r="D66" s="4">
         <f t="shared" si="4"/>
         <v>90</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="16" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B67" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C66" s="5">
+      <c r="C67" s="5">
         <f>700+5000+300+600+400+1000+800</f>
         <v>8800</v>
       </c>
-      <c r="D66" s="4">
+      <c r="D67" s="4">
         <f t="shared" si="4"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B67" s="4" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B68" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C67" s="5">
+      <c r="C68" s="5">
         <v>6000</v>
       </c>
-      <c r="D67" s="4">
+      <c r="D68" s="4">
         <f t="shared" si="4"/>
         <v>14890</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B68" s="4" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B69" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C68" s="5">
+      <c r="C69" s="5">
         <v>-10000</v>
       </c>
-      <c r="D68" s="4">
+      <c r="D69" s="4">
         <f t="shared" si="4"/>
         <v>4890</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="16" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B70" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C69" s="5">
+      <c r="C70" s="5">
         <v>500</v>
       </c>
-      <c r="D69" s="4">
-        <f t="shared" ref="D69:D74" si="5">D68+C69</f>
+      <c r="D70" s="4">
+        <f t="shared" ref="D70:D75" si="5">D69+C70</f>
         <v>5390</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B70" s="4" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B71" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C70" s="5">
+      <c r="C71" s="5">
         <v>700</v>
       </c>
-      <c r="D70" s="4">
+      <c r="D71" s="4">
         <f t="shared" si="5"/>
         <v>6090</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B71" s="4" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B72" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C71" s="5">
+      <c r="C72" s="5">
         <v>1500</v>
       </c>
-      <c r="D71" s="4">
+      <c r="D72" s="4">
         <f t="shared" si="5"/>
         <v>7590</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B72" s="4" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B73" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C72" s="5">
+      <c r="C73" s="5">
         <v>5000</v>
       </c>
-      <c r="D72" s="4">
+      <c r="D73" s="4">
         <f t="shared" si="5"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B73" s="4" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C73" s="5">
+      <c r="C74" s="5">
         <v>-10000</v>
       </c>
-      <c r="D73" s="4">
+      <c r="D74" s="4">
         <f t="shared" si="5"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="16" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B75" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C74" s="5">
+      <c r="C75" s="5">
         <v>2000</v>
       </c>
-      <c r="D74" s="4">
+      <c r="D75" s="4">
         <f t="shared" si="5"/>
         <v>4590</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B75" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C75" s="5">
-        <v>700</v>
-      </c>
-      <c r="D75" s="4">
-        <f t="shared" ref="D75:D80" si="6">D74+C75</f>
-        <v>5290</v>
-      </c>
-    </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="16" t="s">
-        <v>82</v>
-      </c>
       <c r="B76" s="4" t="s">
         <v>77</v>
       </c>
@@ -2191,401 +2191,404 @@
         <v>700</v>
       </c>
       <c r="D76" s="4">
+        <f t="shared" ref="D76:D81" si="6">D75+C76</f>
+        <v>5290</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C77" s="5">
+        <v>700</v>
+      </c>
+      <c r="D77" s="4">
         <f t="shared" si="6"/>
         <v>5990</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="16" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="B78" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C77" s="5">
+      <c r="C78" s="5">
         <v>700</v>
       </c>
-      <c r="D77" s="4">
+      <c r="D78" s="4">
         <f t="shared" si="6"/>
         <v>6690</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="16" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B79" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C78" s="5">
+      <c r="C79" s="5">
         <v>4000</v>
       </c>
-      <c r="D78" s="4">
+      <c r="D79" s="4">
         <f t="shared" si="6"/>
         <v>10690</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B79" s="4" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B80" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C79" s="5">
+      <c r="C80" s="5">
         <v>-10000</v>
       </c>
-      <c r="D79" s="4">
+      <c r="D80" s="4">
         <f t="shared" si="6"/>
         <v>690</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="16" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B81" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C80" s="5">
+      <c r="C81" s="5">
         <v>1000</v>
       </c>
-      <c r="D80" s="4">
+      <c r="D81" s="4">
         <f t="shared" si="6"/>
         <v>1690</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="16" t="s">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="B81" s="4" t="s">
+      <c r="B82" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C81" s="5">
+      <c r="C82" s="5">
         <v>7000</v>
       </c>
-      <c r="D81" s="4">
-        <f t="shared" ref="D81:D86" si="7">D80+C81</f>
+      <c r="D82" s="4">
+        <f t="shared" ref="D82:D87" si="7">D81+C82</f>
         <v>8690</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B82" s="4" t="s">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B83" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C82" s="5">
+      <c r="C83" s="5">
         <v>10000</v>
       </c>
-      <c r="D82" s="4">
+      <c r="D83" s="4">
         <f t="shared" si="7"/>
         <v>18690</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B83" s="4" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B84" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C83" s="5">
+      <c r="C84" s="5">
         <v>-10000</v>
       </c>
-      <c r="D83" s="4">
+      <c r="D84" s="4">
         <f t="shared" si="7"/>
         <v>8690</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B84" s="4" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B85" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C84" s="5">
+      <c r="C85" s="5">
         <v>1700</v>
       </c>
-      <c r="D84" s="4">
+      <c r="D85" s="4">
         <f t="shared" si="7"/>
         <v>10390</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B85" s="4" t="s">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B86" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C85" s="5">
+      <c r="C86" s="5">
         <v>-10000</v>
       </c>
-      <c r="D85" s="4">
+      <c r="D86" s="4">
         <f t="shared" si="7"/>
         <v>390</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B86" s="4" t="s">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B87" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C86" s="5">
+      <c r="C87" s="5">
         <v>6000</v>
       </c>
-      <c r="D86" s="4">
+      <c r="D87" s="4">
         <f t="shared" si="7"/>
         <v>6390</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="B87" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C87" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D87" s="4">
-        <f t="shared" ref="D87:D92" si="8">D86+C87</f>
-        <v>8390</v>
-      </c>
-    </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C88" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D88" s="4">
+        <f t="shared" ref="D88:D93" si="8">D87+C88</f>
+        <v>8390</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="B88" s="4" t="s">
+      <c r="B89" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C88" s="5">
+      <c r="C89" s="5">
         <v>5000</v>
       </c>
-      <c r="D88" s="4">
+      <c r="D89" s="4">
         <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B89" s="4" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B90" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C89" s="5">
+      <c r="C90" s="5">
         <v>-10000</v>
       </c>
-      <c r="D89" s="4">
+      <c r="D90" s="4">
         <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="16" t="s">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="B90" s="4" t="s">
+      <c r="B91" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C90" s="5">
+      <c r="C91" s="5">
         <v>1000</v>
       </c>
-      <c r="D90" s="4">
+      <c r="D91" s="4">
         <f t="shared" si="8"/>
         <v>4390</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B91" s="4" t="s">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B92" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C91" s="5">
+      <c r="C92" s="5">
         <v>9000</v>
       </c>
-      <c r="D91" s="4">
+      <c r="D92" s="4">
         <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B92" s="4" t="s">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B93" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C92" s="5">
+      <c r="C93" s="5">
         <v>-10000</v>
       </c>
-      <c r="D92" s="4">
+      <c r="D93" s="4">
         <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B93" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C93" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D93" s="4">
-        <f t="shared" ref="D93:D98" si="9">D92+C93</f>
-        <v>5390</v>
-      </c>
-    </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B94" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C94" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D94" s="4">
+        <f t="shared" ref="D94:D99" si="9">D93+C94</f>
+        <v>5390</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B95" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C94" s="5">
+      <c r="C95" s="5">
         <v>6000</v>
       </c>
-      <c r="D94" s="4">
+      <c r="D95" s="4">
         <f t="shared" si="9"/>
         <v>11390</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B95" s="4" t="s">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B96" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C95" s="5">
+      <c r="C96" s="5">
         <v>-10000</v>
       </c>
-      <c r="D95" s="4">
+      <c r="D96" s="4">
         <f t="shared" si="9"/>
         <v>1390</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B96" s="4" t="s">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B97" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C96" s="5">
+      <c r="C97" s="5">
         <v>400</v>
       </c>
-      <c r="D96" s="4">
+      <c r="D97" s="4">
         <f t="shared" si="9"/>
         <v>1790</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="16" t="s">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="B97" s="4" t="s">
+      <c r="B98" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C97" s="5">
+      <c r="C98" s="5">
         <v>2000</v>
       </c>
-      <c r="D97" s="4">
+      <c r="D98" s="4">
         <f t="shared" si="9"/>
         <v>3790</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="16" t="s">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="B98" s="4" t="s">
+      <c r="B99" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C98" s="5">
+      <c r="C99" s="5">
         <v>6000</v>
       </c>
-      <c r="D98" s="4">
+      <c r="D99" s="4">
         <f t="shared" si="9"/>
         <v>9790</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="16" t="s">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="B99" s="4" t="s">
+      <c r="B100" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C99" s="5">
+      <c r="C100" s="5">
         <v>1000</v>
       </c>
-      <c r="D99" s="4">
-        <f t="shared" ref="D99:D104" si="10">D98+C99</f>
+      <c r="D100" s="4">
+        <f t="shared" ref="D100:D105" si="10">D99+C100</f>
         <v>10790</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B100" s="4" t="s">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B101" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C100" s="5">
+      <c r="C101" s="5">
         <v>-10000</v>
       </c>
-      <c r="D100" s="4">
+      <c r="D101" s="4">
         <f t="shared" si="10"/>
         <v>790</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="16" t="s">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="B101" s="4" t="s">
+      <c r="B102" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C101" s="5">
+      <c r="C102" s="5">
         <v>800</v>
       </c>
-      <c r="D101" s="4">
+      <c r="D102" s="4">
         <f t="shared" si="10"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="16" t="s">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="B102" s="4" t="s">
+      <c r="B103" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C102" s="5">
+      <c r="C103" s="5">
         <v>5000</v>
       </c>
-      <c r="D102" s="4">
+      <c r="D103" s="4">
         <f t="shared" si="10"/>
         <v>6590</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="16" t="s">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="B103" s="4" t="s">
+      <c r="B104" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C103" s="5">
+      <c r="C104" s="5">
         <v>6000</v>
       </c>
-      <c r="D103" s="4">
+      <c r="D104" s="4">
         <f t="shared" si="10"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B104" s="4" t="s">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B105" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C104" s="5">
+      <c r="C105" s="5">
         <v>-10000</v>
       </c>
-      <c r="D104" s="4">
+      <c r="D105" s="4">
         <f t="shared" si="10"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="16" t="s">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="B105" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C105" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D105" s="4">
-        <f t="shared" ref="D105:D111" si="11">D104+C105</f>
-        <v>4590</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B106" s="4" t="s">
         <v>65</v>
       </c>
@@ -2593,926 +2596,926 @@
         <v>2000</v>
       </c>
       <c r="D106" s="4">
+        <f t="shared" ref="D106:D112" si="11">D105+C106</f>
+        <v>4590</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B107" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C107" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D107" s="4">
         <f t="shared" si="11"/>
         <v>6590</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B107" s="4" t="s">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B108" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C107" s="5">
+      <c r="C108" s="5">
         <v>7000</v>
       </c>
-      <c r="D107" s="4">
+      <c r="D108" s="4">
         <f t="shared" si="11"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B108" s="4" t="s">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B109" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C108" s="5">
+      <c r="C109" s="5">
         <v>-10000</v>
       </c>
-      <c r="D108" s="4">
+      <c r="D109" s="4">
         <f t="shared" si="11"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="16" t="s">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="B109" s="4" t="s">
+      <c r="B110" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C109" s="5">
+      <c r="C110" s="5">
         <v>2000</v>
       </c>
-      <c r="D109" s="4">
+      <c r="D110" s="4">
         <f t="shared" si="11"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="16" t="s">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="B110" s="4" t="s">
+      <c r="B111" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C110" s="5">
+      <c r="C111" s="5">
         <v>6000</v>
       </c>
-      <c r="D110" s="4">
+      <c r="D111" s="4">
         <f t="shared" si="11"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B111" s="4" t="s">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B112" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C111" s="5">
+      <c r="C112" s="5">
         <v>-10000</v>
       </c>
-      <c r="D111" s="4">
+      <c r="D112" s="4">
         <f t="shared" si="11"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="B112" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C112" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D112" s="4">
-        <f t="shared" ref="D112:D117" si="12">D111+C112</f>
-        <v>3590</v>
-      </c>
-    </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B113" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C113" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D113" s="4">
+        <f t="shared" ref="D113:D118" si="12">D112+C113</f>
+        <v>3590</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="B113" s="4" t="s">
+      <c r="B114" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C113" s="5">
+      <c r="C114" s="5">
         <v>7000</v>
       </c>
-      <c r="D113" s="4">
+      <c r="D114" s="4">
         <f t="shared" si="12"/>
         <v>10590</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B114" s="4" t="s">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B115" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C114" s="5">
+      <c r="C115" s="5">
         <v>-10000</v>
       </c>
-      <c r="D114" s="4">
+      <c r="D115" s="4">
         <f t="shared" si="12"/>
         <v>590</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B115" s="4" t="s">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B116" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C115" s="5">
+      <c r="C116" s="5">
         <v>12000</v>
       </c>
-      <c r="D115" s="4">
+      <c r="D116" s="4">
         <f t="shared" si="12"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B116" s="4" t="s">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B117" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C116" s="5">
+      <c r="C117" s="5">
         <v>-10000</v>
       </c>
-      <c r="D116" s="4">
+      <c r="D117" s="4">
         <f t="shared" si="12"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B117" s="4" t="s">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B118" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C117" s="5">
+      <c r="C118" s="5">
         <v>2000</v>
       </c>
-      <c r="D117" s="4">
+      <c r="D118" s="4">
         <f t="shared" si="12"/>
         <v>4590</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="B118" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C118" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D118" s="4">
-        <f t="shared" ref="D118:D123" si="13">D117+C118</f>
-        <v>6590</v>
-      </c>
-    </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="B119" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C119" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D119" s="4">
+        <f t="shared" ref="D119:D124" si="13">D118+C119</f>
+        <v>6590</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="B119" s="4" t="s">
+      <c r="B120" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C119" s="5">
+      <c r="C120" s="5">
         <v>7000</v>
       </c>
-      <c r="D119" s="4">
+      <c r="D120" s="4">
         <f t="shared" si="13"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B120" s="4" t="s">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B121" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C120" s="5">
+      <c r="C121" s="5">
         <v>-10000</v>
       </c>
-      <c r="D120" s="4">
+      <c r="D121" s="4">
         <f t="shared" si="13"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="16" t="s">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="B121" s="4" t="s">
+      <c r="B122" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C121" s="5">
+      <c r="C122" s="5">
         <v>2000</v>
       </c>
-      <c r="D121" s="4">
+      <c r="D122" s="4">
         <f t="shared" si="13"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="16" t="s">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="B122" s="4" t="s">
+      <c r="B123" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C122" s="5">
+      <c r="C123" s="5">
         <v>8000</v>
       </c>
-      <c r="D122" s="4">
+      <c r="D123" s="4">
         <f t="shared" si="13"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B123" s="4" t="s">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B124" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C123" s="5">
+      <c r="C124" s="5">
         <v>-10000</v>
       </c>
-      <c r="D123" s="4">
+      <c r="D124" s="4">
         <f t="shared" si="13"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="16" t="s">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="B124" s="4" t="s">
+      <c r="B125" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C124" s="5">
+      <c r="C125" s="5">
         <v>2000</v>
       </c>
-      <c r="D124" s="4">
-        <f t="shared" ref="D124:D129" si="14">D123+C124</f>
+      <c r="D125" s="4">
+        <f t="shared" ref="D125:D130" si="14">D124+C125</f>
         <v>5590</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B125" s="4" t="s">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B126" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C125" s="5">
+      <c r="C126" s="5">
         <v>5000</v>
       </c>
-      <c r="D125" s="4">
+      <c r="D126" s="4">
         <f t="shared" si="14"/>
         <v>10590</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B126" s="4" t="s">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B127" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C126" s="5">
+      <c r="C127" s="5">
         <v>-10000</v>
       </c>
-      <c r="D126" s="4">
+      <c r="D127" s="4">
         <f t="shared" si="14"/>
         <v>590</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B127" s="4" t="s">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B128" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C127" s="5">
+      <c r="C128" s="5">
         <v>2000</v>
       </c>
-      <c r="D127" s="4">
+      <c r="D128" s="4">
         <f t="shared" si="14"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B128" s="4" t="s">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B129" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C128" s="5">
+      <c r="C129" s="5">
         <v>9000</v>
       </c>
-      <c r="D128" s="4">
+      <c r="D129" s="4">
         <f t="shared" si="14"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B129" s="4" t="s">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B130" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C129" s="5">
+      <c r="C130" s="5">
         <v>-10000</v>
       </c>
-      <c r="D129" s="4">
+      <c r="D130" s="4">
         <f t="shared" si="14"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B130" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C130" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D130" s="4">
-        <f t="shared" ref="D130:D135" si="15">D129+C130</f>
-        <v>3590</v>
-      </c>
-    </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B131" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C131" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D131" s="4">
+        <f t="shared" ref="D131:D136" si="15">D130+C131</f>
+        <v>3590</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="B131" s="4" t="s">
+      <c r="B132" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C131" s="5">
+      <c r="C132" s="5">
         <v>8000</v>
       </c>
-      <c r="D131" s="4">
+      <c r="D132" s="4">
         <f t="shared" si="15"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B132" s="4" t="s">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B133" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C132" s="5">
+      <c r="C133" s="5">
         <v>-10000</v>
       </c>
-      <c r="D132" s="4">
+      <c r="D133" s="4">
         <f t="shared" si="15"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="16" t="s">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="B133" s="4" t="s">
+      <c r="B134" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C133" s="5">
+      <c r="C134" s="5">
         <v>2000</v>
       </c>
-      <c r="D133" s="4">
+      <c r="D134" s="4">
         <f t="shared" si="15"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="16" t="s">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="B134" s="4" t="s">
+      <c r="B135" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C134" s="5">
+      <c r="C135" s="5">
         <v>12000</v>
       </c>
-      <c r="D134" s="4">
+      <c r="D135" s="4">
         <f t="shared" si="15"/>
         <v>15590</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B135" s="4" t="s">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B136" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C135" s="5">
+      <c r="C136" s="5">
         <v>-10000</v>
       </c>
-      <c r="D135" s="4">
+      <c r="D136" s="4">
         <f t="shared" si="15"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="B136" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="C136" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D136" s="4">
-        <f t="shared" ref="D136:D141" si="16">D135+C136</f>
-        <v>7590</v>
-      </c>
-    </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="B137" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C137" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D137" s="4">
+        <f t="shared" ref="D137:D142" si="16">D136+C137</f>
+        <v>7590</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="B137" s="4" t="s">
+      <c r="B138" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="C137" s="5">
+      <c r="C138" s="5">
         <v>10000</v>
       </c>
-      <c r="D137" s="4">
+      <c r="D138" s="4">
         <f t="shared" si="16"/>
         <v>17590</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B138" s="4" t="s">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B139" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C138" s="5">
+      <c r="C139" s="5">
         <v>-10000</v>
       </c>
-      <c r="D138" s="4">
+      <c r="D139" s="4">
         <f t="shared" si="16"/>
         <v>7590</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B139" s="4" t="s">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B140" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="C139" s="5">
+      <c r="C140" s="5">
         <v>2000</v>
       </c>
-      <c r="D139" s="4">
+      <c r="D140" s="4">
         <f t="shared" si="16"/>
         <v>9590</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="16" t="s">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="B140" s="4" t="s">
+      <c r="B141" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="C140" s="5">
+      <c r="C141" s="5">
         <v>-1200</v>
       </c>
-      <c r="D140" s="4">
+      <c r="D141" s="4">
         <f t="shared" si="16"/>
         <v>8390</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B141" s="4" t="s">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B142" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="C141" s="5">
+      <c r="C142" s="5">
         <v>500</v>
       </c>
-      <c r="D141" s="4">
+      <c r="D142" s="4">
         <f t="shared" si="16"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="16" t="s">
-        <v>165</v>
-      </c>
-      <c r="B142" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="C142" s="5">
-        <v>750</v>
-      </c>
-      <c r="D142" s="4">
-        <f t="shared" ref="D142:D147" si="17">D141+C142</f>
-        <v>9640</v>
-      </c>
-    </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="B143" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C143" s="5">
+        <v>750</v>
+      </c>
+      <c r="D143" s="4">
+        <f t="shared" ref="D143:D148" si="17">D142+C143</f>
+        <v>9640</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="B143" s="4" t="s">
+      <c r="B144" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C143" s="5">
+      <c r="C144" s="5">
         <v>2000</v>
       </c>
-      <c r="D143" s="4">
+      <c r="D144" s="4">
         <f t="shared" si="17"/>
         <v>11640</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B144" s="4" t="s">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B145" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C144" s="5">
+      <c r="C145" s="5">
         <v>2000</v>
       </c>
-      <c r="D144" s="4">
+      <c r="D145" s="4">
         <f t="shared" si="17"/>
         <v>13640</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B145" s="4" t="s">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B146" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C145" s="5">
+      <c r="C146" s="5">
         <v>-10000</v>
       </c>
-      <c r="D145" s="4">
+      <c r="D146" s="4">
         <f t="shared" si="17"/>
         <v>3640</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B146" s="4" t="s">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B147" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="C146" s="5">
+      <c r="C147" s="5">
         <v>350</v>
       </c>
-      <c r="D146" s="4">
+      <c r="D147" s="4">
         <f t="shared" si="17"/>
         <v>3990</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="16" t="s">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="B147" s="4" t="s">
+      <c r="B148" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="C147" s="5">
+      <c r="C148" s="5">
         <v>300</v>
       </c>
-      <c r="D147" s="4">
+      <c r="D148" s="4">
         <f t="shared" si="17"/>
         <v>4290</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="16" t="s">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="B148" s="4" t="s">
+      <c r="B149" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="C148" s="5">
+      <c r="C149" s="5">
         <v>3800</v>
       </c>
-      <c r="D148" s="4">
-        <f t="shared" ref="D148:D154" si="18">D147+C148</f>
+      <c r="D149" s="4">
+        <f t="shared" ref="D149:D155" si="18">D148+C149</f>
         <v>8090</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B149" s="4" t="s">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B150" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C149" s="5">
+      <c r="C150" s="5">
         <v>500</v>
       </c>
-      <c r="D149" s="4">
+      <c r="D150" s="4">
         <f t="shared" si="18"/>
         <v>8590</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="16" t="s">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="B150" s="4" t="s">
+      <c r="B151" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="C150" s="5">
+      <c r="C151" s="5">
         <v>1300</v>
       </c>
-      <c r="D150" s="4">
+      <c r="D151" s="4">
         <f t="shared" si="18"/>
         <v>9890</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="16" t="s">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="B151" s="4" t="s">
+      <c r="B152" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C151" s="5">
+      <c r="C152" s="5">
         <v>9000</v>
       </c>
-      <c r="D151" s="4">
+      <c r="D152" s="4">
         <f t="shared" si="18"/>
         <v>18890</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B152" s="4" t="s">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B153" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C152" s="5">
+      <c r="C153" s="5">
         <v>-10000</v>
       </c>
-      <c r="D152" s="4">
+      <c r="D153" s="4">
         <f t="shared" si="18"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" s="16" t="s">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="B153" s="4" t="s">
+      <c r="B154" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C153" s="5">
+      <c r="C154" s="5">
         <v>2000</v>
       </c>
-      <c r="D153" s="4">
+      <c r="D154" s="4">
         <f t="shared" si="18"/>
         <v>10890</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B154" s="4" t="s">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B155" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C154" s="5">
+      <c r="C155" s="5">
         <v>-10000</v>
       </c>
-      <c r="D154" s="4">
+      <c r="D155" s="4">
         <f t="shared" si="18"/>
         <v>890</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="B155" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="C155" s="5">
-        <v>500</v>
-      </c>
-      <c r="D155" s="4">
-        <f t="shared" ref="D155:D160" si="19">D154+C155</f>
-        <v>1390</v>
-      </c>
-    </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="B156" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C156" s="5">
+        <v>500</v>
+      </c>
+      <c r="D156" s="4">
+        <f t="shared" ref="D156:D161" si="19">D155+C156</f>
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="B156" s="4" t="s">
+      <c r="B157" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="C156" s="5">
+      <c r="C157" s="5">
         <v>10000</v>
       </c>
-      <c r="D156" s="4">
+      <c r="D157" s="4">
         <f t="shared" si="19"/>
         <v>11390</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B157" s="4" t="s">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B158" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C157" s="5">
+      <c r="C158" s="5">
         <v>-10000</v>
       </c>
-      <c r="D157" s="4">
+      <c r="D158" s="4">
         <f t="shared" si="19"/>
         <v>1390</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="16" t="s">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="B158" s="4" t="s">
+      <c r="B159" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C158" s="5">
+      <c r="C159" s="5">
         <v>3000</v>
       </c>
-      <c r="D158" s="4">
+      <c r="D159" s="4">
         <f t="shared" si="19"/>
         <v>4390</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="16" t="s">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="B159" s="4" t="s">
+      <c r="B160" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C159" s="5">
+      <c r="C160" s="5">
         <v>2000</v>
       </c>
-      <c r="D159" s="4">
+      <c r="D160" s="4">
         <f t="shared" si="19"/>
         <v>6390</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B160" s="4" t="s">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B161" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C160" s="5">
+      <c r="C161" s="5">
         <v>2000</v>
       </c>
-      <c r="D160" s="4">
+      <c r="D161" s="4">
         <f t="shared" si="19"/>
         <v>8390</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" s="16" t="s">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="B161" s="4" t="s">
+      <c r="B162" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C161" s="5">
+      <c r="C162" s="5">
         <v>11000</v>
       </c>
-      <c r="D161" s="4">
-        <f t="shared" ref="D161:D166" si="20">D160+C161</f>
+      <c r="D162" s="4">
+        <f t="shared" ref="D162:D167" si="20">D161+C162</f>
         <v>19390</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B162" s="4" t="s">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B163" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C162" s="5">
+      <c r="C163" s="5">
         <v>-10000</v>
       </c>
-      <c r="D162" s="4">
+      <c r="D163" s="4">
         <f t="shared" si="20"/>
         <v>9390</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163" s="16" t="s">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" s="16" t="s">
         <v>187</v>
       </c>
-      <c r="B163" s="4" t="s">
+      <c r="B164" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C163" s="5">
+      <c r="C164" s="5">
         <v>3000</v>
       </c>
-      <c r="D163" s="4">
+      <c r="D164" s="4">
         <f t="shared" si="20"/>
         <v>12390</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B164" s="4" t="s">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B165" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C164" s="5">
+      <c r="C165" s="5">
         <v>-10000</v>
       </c>
-      <c r="D164" s="4">
+      <c r="D165" s="4">
         <f t="shared" si="20"/>
         <v>2390</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B165" s="4" t="s">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B166" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C165" s="5">
+      <c r="C166" s="5">
         <v>500</v>
       </c>
-      <c r="D165" s="4">
+      <c r="D166" s="4">
         <f t="shared" si="20"/>
         <v>2890</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A166" s="16" t="s">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" s="16" t="s">
         <v>189</v>
       </c>
-      <c r="B166" s="4" t="s">
+      <c r="B167" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C166" s="5">
+      <c r="C167" s="5">
         <v>5600</v>
       </c>
-      <c r="D166" s="4">
+      <c r="D167" s="4">
         <f t="shared" si="20"/>
         <v>8490</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B167" s="4" t="s">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B168" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="C167" s="5">
+      <c r="C168" s="5">
         <v>4700</v>
       </c>
-      <c r="D167" s="4">
-        <f t="shared" ref="D167:D173" si="21">D166+C167</f>
+      <c r="D168" s="4">
+        <f t="shared" ref="D168:D174" si="21">D167+C168</f>
         <v>13190</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A168" s="16" t="s">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" s="16" t="s">
         <v>192</v>
       </c>
-      <c r="B168" s="4" t="s">
+      <c r="B169" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C168" s="5">
+      <c r="C169" s="5">
         <v>1500</v>
       </c>
-      <c r="D168" s="4">
+      <c r="D169" s="4">
         <f t="shared" si="21"/>
         <v>14690</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B169" s="4" t="s">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B170" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C169" s="5">
+      <c r="C170" s="5">
         <v>500</v>
       </c>
-      <c r="D169" s="4">
+      <c r="D170" s="4">
         <f t="shared" si="21"/>
         <v>15190</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" s="16" t="s">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="B170" s="4" t="s">
+      <c r="B171" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="C170" s="5">
+      <c r="C171" s="5">
         <v>1000</v>
       </c>
-      <c r="D170" s="4">
+      <c r="D171" s="4">
         <f t="shared" si="21"/>
         <v>16190</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" s="16" t="s">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="B171" s="4" t="s">
+      <c r="B172" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="C171" s="5">
+      <c r="C172" s="5">
         <v>1000</v>
       </c>
-      <c r="D171" s="4">
+      <c r="D172" s="4">
         <f t="shared" si="21"/>
         <v>17190</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A172" s="16" t="s">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="B172" s="4" t="s">
+      <c r="B173" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C172" s="5">
+      <c r="C173" s="5">
         <v>3000</v>
       </c>
-      <c r="D172" s="4">
+      <c r="D173" s="4">
         <f t="shared" si="21"/>
         <v>20190</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B173" s="4" t="s">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B174" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C173" s="5">
+      <c r="C174" s="5">
         <v>-20000</v>
       </c>
-      <c r="D173" s="4">
+      <c r="D174" s="4">
         <f t="shared" si="21"/>
         <v>190</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B174" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C174" s="5">
-        <v>500</v>
-      </c>
-      <c r="D174" s="4">
-        <f t="shared" ref="D174:D180" si="22">D173+C174</f>
-        <v>690</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -3523,203 +3526,242 @@
         <v>500</v>
       </c>
       <c r="D175" s="4">
+        <f t="shared" ref="D175:D181" si="22">D174+C175</f>
+        <v>690</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B176" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C176" s="5">
+        <v>500</v>
+      </c>
+      <c r="D176" s="4">
         <f t="shared" si="22"/>
         <v>1190</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176" s="16" t="s">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="B176" s="4" t="s">
+      <c r="B177" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="C176" s="5">
+      <c r="C177" s="5">
         <v>10000</v>
       </c>
-      <c r="D176" s="4">
+      <c r="D177" s="4">
         <f t="shared" si="22"/>
         <v>11190</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B177" s="4" t="s">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B178" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C177" s="5">
+      <c r="C178" s="5">
         <v>-10000</v>
       </c>
-      <c r="D177" s="4">
+      <c r="D178" s="4">
         <f t="shared" si="22"/>
         <v>1190</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A178" s="16" t="s">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A179" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="B178" s="4" t="s">
+      <c r="B179" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C178" s="5">
+      <c r="C179" s="5">
         <v>3000</v>
       </c>
-      <c r="D178" s="4">
+      <c r="D179" s="4">
         <f t="shared" si="22"/>
         <v>4190</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A179" s="16" t="s">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="B179" s="4" t="s">
+      <c r="B180" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C179" s="5">
+      <c r="C180" s="5">
         <v>11000</v>
       </c>
-      <c r="D179" s="4">
+      <c r="D180" s="4">
         <f t="shared" si="22"/>
         <v>15190</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B180" s="4" t="s">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B181" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C180" s="5">
+      <c r="C181" s="5">
         <v>-10000</v>
       </c>
-      <c r="D180" s="4">
+      <c r="D181" s="4">
         <f t="shared" si="22"/>
         <v>5190</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="B181" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C181" s="5">
-        <v>3000</v>
-      </c>
-      <c r="D181" s="4">
-        <f t="shared" ref="D181:D187" si="23">D180+C181</f>
-        <v>8190</v>
-      </c>
-    </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="B182" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C182" s="5">
+        <v>3000</v>
+      </c>
+      <c r="D182" s="4">
+        <f t="shared" ref="D182:D188" si="23">D181+C182</f>
+        <v>8190</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A183" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="B182" s="4" t="s">
+      <c r="B183" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="C182" s="5">
+      <c r="C183" s="5">
         <v>14000</v>
       </c>
-      <c r="D182" s="4">
+      <c r="D183" s="4">
         <f t="shared" si="23"/>
         <v>22190</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B183" s="4" t="s">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B184" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="C183" s="5">
+      <c r="C184" s="5">
         <v>-20000</v>
       </c>
-      <c r="D183" s="4">
+      <c r="D184" s="4">
         <f t="shared" si="23"/>
         <v>2190</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" s="16" t="s">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A185" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="B184" s="4" t="s">
+      <c r="B185" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="C184" s="5">
+      <c r="C185" s="5">
         <v>5000</v>
       </c>
-      <c r="D184" s="4">
+      <c r="D185" s="4">
         <f t="shared" si="23"/>
         <v>7190</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A185" s="16" t="s">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" s="16" t="s">
         <v>213</v>
       </c>
-      <c r="B185" s="4" t="s">
+      <c r="B186" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="C185" s="5">
+      <c r="C186" s="5">
         <v>5000</v>
       </c>
-      <c r="D185" s="4">
+      <c r="D186" s="4">
         <f t="shared" si="23"/>
         <v>12190</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A186" s="16" t="s">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A187" s="16" t="s">
         <v>215</v>
       </c>
-      <c r="B186" s="4" t="s">
+      <c r="B187" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C186" s="5">
+      <c r="C187" s="5">
         <v>11000</v>
       </c>
-      <c r="D186" s="4">
+      <c r="D187" s="4">
         <f t="shared" si="23"/>
         <v>23190</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B187" s="4" t="s">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B188" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C187" s="5">
+      <c r="C188" s="5">
         <v>-20000</v>
       </c>
-      <c r="D187" s="4">
+      <c r="D188" s="4">
         <f t="shared" si="23"/>
         <v>3190</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A188" s="16" t="s">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189" s="16" t="s">
         <v>216</v>
       </c>
-      <c r="B188" s="4" t="s">
+      <c r="B189" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C188" s="5">
+      <c r="C189" s="5">
         <v>500</v>
-      </c>
-      <c r="D188" s="4">
-        <f>D187+C188</f>
-        <v>3690</v>
-      </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B189" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C189" s="5">
-        <v>3000</v>
       </c>
       <c r="D189" s="4">
         <f>D188+C189</f>
+        <v>3690</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B190" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C190" s="5">
+        <v>3000</v>
+      </c>
+      <c r="D190" s="4">
+        <f>D189+C190</f>
         <v>6690</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A191" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="B191" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="C191" s="5">
+        <v>12000</v>
+      </c>
+      <c r="D191" s="4">
+        <f>D190+C191</f>
+        <v>18690</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B192" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="C192" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D192" s="4">
+        <f>D191+C192</f>
+        <v>8690</v>
       </c>
     </row>
   </sheetData>
@@ -4236,8 +4278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
lay tien loi co diem ngay 02
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="223">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -681,6 +681,12 @@
   </si>
   <si>
     <t>Duy lấy tiền lời ngày 31,01 là 5tr</t>
+  </si>
+  <si>
+    <t>02/10/2024</t>
+  </si>
+  <si>
+    <t>Duy lấy tiền lãi 12tr</t>
   </si>
 </sst>
 </file>
@@ -1150,11 +1156,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K195"/>
+  <dimension ref="A1:K198"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H40" sqref="H40"/>
+      <selection pane="bottomLeft" activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1230,8 +1236,8 @@
         <v>20</v>
       </c>
       <c r="J3" s="4">
-        <f>SUM(I3:I66)</f>
-        <v>550</v>
+        <f>SUM(I3:I67)</f>
+        <v>560</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1841,7 +1847,7 @@
         <v>7640</v>
       </c>
       <c r="D50" s="4">
-        <f t="shared" ref="D50:D56" si="2">D49+C50</f>
+        <f t="shared" ref="D50:D57" si="2">D49+C50</f>
         <v>9090</v>
       </c>
       <c r="H50" s="16" t="s">
@@ -1854,366 +1860,360 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H51" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="I51" s="5">
+        <v>10</v>
+      </c>
+      <c r="K51" s="14"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H52" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="I51" s="5">
+      <c r="I52" s="5">
         <v>20</v>
       </c>
-      <c r="K51" s="14"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B52" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C52" s="5">
-        <v>3000</v>
-      </c>
-      <c r="D52" s="4">
-        <f>D50+C52</f>
-        <v>12090</v>
-      </c>
-      <c r="H52" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="I52" s="5">
-        <v>10</v>
-      </c>
+      <c r="K52" s="14"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B53" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C53" s="5">
+        <v>3000</v>
+      </c>
+      <c r="D53" s="4">
+        <f>D50+C53</f>
+        <v>12090</v>
+      </c>
+      <c r="H53" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="I53" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B54" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="5">
+      <c r="C54" s="5">
         <v>-10000</v>
       </c>
-      <c r="D53" s="4">
+      <c r="D54" s="4">
         <f t="shared" si="2"/>
         <v>2090</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B54" s="4" t="s">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B55" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C54" s="5">
+      <c r="C55" s="5">
         <v>800</v>
       </c>
-      <c r="D54" s="4">
+      <c r="D55" s="4">
         <f t="shared" si="2"/>
         <v>2890</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="16" t="s">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B56" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C55" s="5">
+      <c r="C56" s="5">
         <v>2000</v>
       </c>
-      <c r="D55" s="4">
+      <c r="D56" s="4">
         <f t="shared" si="2"/>
         <v>4890</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="16" t="s">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B57" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C56" s="5">
+      <c r="C57" s="5">
         <v>4000</v>
       </c>
-      <c r="D56" s="4">
+      <c r="D57" s="4">
         <f t="shared" si="2"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="16" t="s">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B58" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C57" s="5">
+      <c r="C58" s="5">
         <v>4000</v>
       </c>
-      <c r="D57" s="4">
-        <f t="shared" ref="D57:D62" si="3">D56+C57</f>
+      <c r="D58" s="4">
+        <f t="shared" ref="D58:D63" si="3">D57+C58</f>
         <v>12890</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B58" s="4" t="s">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B59" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C58" s="5">
+      <c r="C59" s="5">
         <v>5000</v>
       </c>
-      <c r="D58" s="4">
+      <c r="D59" s="4">
         <f t="shared" si="3"/>
         <v>17890</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B59" s="4" t="s">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B60" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C59" s="5">
+      <c r="C60" s="5">
         <v>-10000</v>
       </c>
-      <c r="D59" s="4">
+      <c r="D60" s="4">
         <f t="shared" si="3"/>
         <v>7890</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" s="16">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" s="16">
         <v>44969</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B61" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C60" s="5">
+      <c r="C61" s="5">
         <v>900</v>
       </c>
-      <c r="D60" s="4">
+      <c r="D61" s="4">
         <f t="shared" si="3"/>
         <v>8790</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B61" s="4" t="s">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B62" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C61" s="5">
+      <c r="C62" s="5">
         <v>4000</v>
       </c>
-      <c r="D61" s="4">
+      <c r="D62" s="4">
         <f t="shared" si="3"/>
         <v>12790</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B62" s="4" t="s">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B63" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C62" s="5">
+      <c r="C63" s="5">
         <v>-10000</v>
       </c>
-      <c r="D62" s="4">
+      <c r="D63" s="4">
         <f t="shared" si="3"/>
         <v>2790</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C63" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D63" s="4">
-        <f t="shared" ref="D63:D70" si="4">D62+C63</f>
-        <v>4790</v>
-      </c>
-    </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C64" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D64" s="4">
+        <f t="shared" ref="D64:D71" si="4">D63+C64</f>
+        <v>4790</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B65" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C64" s="5">
+      <c r="C65" s="5">
         <v>700</v>
       </c>
-      <c r="D64" s="4">
+      <c r="D65" s="4">
         <f t="shared" si="4"/>
         <v>5490</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B65" s="4" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C65" s="5">
+      <c r="C66" s="5">
         <v>4000</v>
       </c>
-      <c r="D65" s="4">
+      <c r="D66" s="4">
         <f t="shared" si="4"/>
         <v>9490</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="16" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B67" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C66" s="5">
+      <c r="C67" s="5">
         <v>600</v>
       </c>
-      <c r="D66" s="4">
+      <c r="D67" s="4">
         <f t="shared" si="4"/>
         <v>10090</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B67" s="4" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B68" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C67" s="5">
+      <c r="C68" s="5">
         <v>-10000</v>
       </c>
-      <c r="D67" s="4">
+      <c r="D68" s="4">
         <f t="shared" si="4"/>
         <v>90</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="16" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B69" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C68" s="5">
+      <c r="C69" s="5">
         <f>700+5000+300+600+400+1000+800</f>
         <v>8800</v>
       </c>
-      <c r="D68" s="4">
+      <c r="D69" s="4">
         <f t="shared" si="4"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B69" s="4" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B70" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C69" s="5">
+      <c r="C70" s="5">
         <v>6000</v>
       </c>
-      <c r="D69" s="4">
+      <c r="D70" s="4">
         <f t="shared" si="4"/>
         <v>14890</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B70" s="4" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B71" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C70" s="5">
+      <c r="C71" s="5">
         <v>-10000</v>
       </c>
-      <c r="D70" s="4">
+      <c r="D71" s="4">
         <f t="shared" si="4"/>
         <v>4890</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="16" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B72" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C71" s="5">
+      <c r="C72" s="5">
         <v>500</v>
       </c>
-      <c r="D71" s="4">
-        <f t="shared" ref="D71:D76" si="5">D70+C71</f>
+      <c r="D72" s="4">
+        <f t="shared" ref="D72:D77" si="5">D71+C72</f>
         <v>5390</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B72" s="4" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B73" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C72" s="5">
+      <c r="C73" s="5">
         <v>700</v>
       </c>
-      <c r="D72" s="4">
+      <c r="D73" s="4">
         <f t="shared" si="5"/>
         <v>6090</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B73" s="4" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C73" s="5">
+      <c r="C74" s="5">
         <v>1500</v>
       </c>
-      <c r="D73" s="4">
+      <c r="D74" s="4">
         <f t="shared" si="5"/>
         <v>7590</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B74" s="4" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B75" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C74" s="5">
+      <c r="C75" s="5">
         <v>5000</v>
       </c>
-      <c r="D74" s="4">
+      <c r="D75" s="4">
         <f t="shared" si="5"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B75" s="4" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B76" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C75" s="5">
+      <c r="C76" s="5">
         <v>-10000</v>
       </c>
-      <c r="D75" s="4">
+      <c r="D76" s="4">
         <f t="shared" si="5"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="16" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B77" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C76" s="5">
+      <c r="C77" s="5">
         <v>2000</v>
       </c>
-      <c r="D76" s="4">
+      <c r="D77" s="4">
         <f t="shared" si="5"/>
         <v>4590</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B77" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C77" s="5">
-        <v>700</v>
-      </c>
-      <c r="D77" s="4">
-        <f t="shared" ref="D77:D82" si="6">D76+C77</f>
-        <v>5290</v>
-      </c>
-    </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="16" t="s">
-        <v>82</v>
-      </c>
       <c r="B78" s="4" t="s">
         <v>77</v>
       </c>
@@ -2221,401 +2221,404 @@
         <v>700</v>
       </c>
       <c r="D78" s="4">
+        <f t="shared" ref="D78:D83" si="6">D77+C78</f>
+        <v>5290</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C79" s="5">
+        <v>700</v>
+      </c>
+      <c r="D79" s="4">
         <f t="shared" si="6"/>
         <v>5990</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="16" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="B79" s="4" t="s">
+      <c r="B80" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C79" s="5">
+      <c r="C80" s="5">
         <v>700</v>
       </c>
-      <c r="D79" s="4">
+      <c r="D80" s="4">
         <f t="shared" si="6"/>
         <v>6690</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="16" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B81" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C80" s="5">
+      <c r="C81" s="5">
         <v>4000</v>
       </c>
-      <c r="D80" s="4">
+      <c r="D81" s="4">
         <f t="shared" si="6"/>
         <v>10690</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B81" s="4" t="s">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B82" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C81" s="5">
+      <c r="C82" s="5">
         <v>-10000</v>
       </c>
-      <c r="D81" s="4">
+      <c r="D82" s="4">
         <f t="shared" si="6"/>
         <v>690</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="16" t="s">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="B82" s="4" t="s">
+      <c r="B83" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C82" s="5">
+      <c r="C83" s="5">
         <v>1000</v>
       </c>
-      <c r="D82" s="4">
+      <c r="D83" s="4">
         <f t="shared" si="6"/>
         <v>1690</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="16" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="B84" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C83" s="5">
+      <c r="C84" s="5">
         <v>7000</v>
       </c>
-      <c r="D83" s="4">
-        <f t="shared" ref="D83:D88" si="7">D82+C83</f>
+      <c r="D84" s="4">
+        <f t="shared" ref="D84:D89" si="7">D83+C84</f>
         <v>8690</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B84" s="4" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B85" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C84" s="5">
+      <c r="C85" s="5">
         <v>10000</v>
       </c>
-      <c r="D84" s="4">
+      <c r="D85" s="4">
         <f t="shared" si="7"/>
         <v>18690</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B85" s="4" t="s">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B86" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C85" s="5">
+      <c r="C86" s="5">
         <v>-10000</v>
       </c>
-      <c r="D85" s="4">
+      <c r="D86" s="4">
         <f t="shared" si="7"/>
         <v>8690</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B86" s="4" t="s">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B87" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C86" s="5">
+      <c r="C87" s="5">
         <v>1700</v>
       </c>
-      <c r="D86" s="4">
+      <c r="D87" s="4">
         <f t="shared" si="7"/>
         <v>10390</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B87" s="4" t="s">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B88" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C87" s="5">
+      <c r="C88" s="5">
         <v>-10000</v>
       </c>
-      <c r="D87" s="4">
+      <c r="D88" s="4">
         <f t="shared" si="7"/>
         <v>390</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B88" s="4" t="s">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B89" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C88" s="5">
+      <c r="C89" s="5">
         <v>6000</v>
       </c>
-      <c r="D88" s="4">
+      <c r="D89" s="4">
         <f t="shared" si="7"/>
         <v>6390</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="B89" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C89" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D89" s="4">
-        <f t="shared" ref="D89:D94" si="8">D88+C89</f>
-        <v>8390</v>
-      </c>
-    </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C90" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D90" s="4">
+        <f t="shared" ref="D90:D95" si="8">D89+C90</f>
+        <v>8390</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="B90" s="4" t="s">
+      <c r="B91" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C90" s="5">
+      <c r="C91" s="5">
         <v>5000</v>
       </c>
-      <c r="D90" s="4">
+      <c r="D91" s="4">
         <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B91" s="4" t="s">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B92" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C91" s="5">
+      <c r="C92" s="5">
         <v>-10000</v>
       </c>
-      <c r="D91" s="4">
+      <c r="D92" s="4">
         <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="16" t="s">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="B92" s="4" t="s">
+      <c r="B93" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C92" s="5">
+      <c r="C93" s="5">
         <v>1000</v>
       </c>
-      <c r="D92" s="4">
+      <c r="D93" s="4">
         <f t="shared" si="8"/>
         <v>4390</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B93" s="4" t="s">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B94" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C93" s="5">
+      <c r="C94" s="5">
         <v>9000</v>
       </c>
-      <c r="D93" s="4">
+      <c r="D94" s="4">
         <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B94" s="4" t="s">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B95" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C94" s="5">
+      <c r="C95" s="5">
         <v>-10000</v>
       </c>
-      <c r="D94" s="4">
+      <c r="D95" s="4">
         <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B95" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C95" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D95" s="4">
-        <f t="shared" ref="D95:D100" si="9">D94+C95</f>
-        <v>5390</v>
-      </c>
-    </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B96" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C96" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D96" s="4">
+        <f t="shared" ref="D96:D101" si="9">D95+C96</f>
+        <v>5390</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B97" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C96" s="5">
+      <c r="C97" s="5">
         <v>6000</v>
       </c>
-      <c r="D96" s="4">
+      <c r="D97" s="4">
         <f t="shared" si="9"/>
         <v>11390</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B97" s="4" t="s">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B98" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C97" s="5">
+      <c r="C98" s="5">
         <v>-10000</v>
       </c>
-      <c r="D97" s="4">
+      <c r="D98" s="4">
         <f t="shared" si="9"/>
         <v>1390</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B98" s="4" t="s">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B99" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C98" s="5">
+      <c r="C99" s="5">
         <v>400</v>
       </c>
-      <c r="D98" s="4">
+      <c r="D99" s="4">
         <f t="shared" si="9"/>
         <v>1790</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="16" t="s">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="B99" s="4" t="s">
+      <c r="B100" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C99" s="5">
+      <c r="C100" s="5">
         <v>2000</v>
       </c>
-      <c r="D99" s="4">
+      <c r="D100" s="4">
         <f t="shared" si="9"/>
         <v>3790</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="16" t="s">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="B100" s="4" t="s">
+      <c r="B101" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C100" s="5">
+      <c r="C101" s="5">
         <v>6000</v>
       </c>
-      <c r="D100" s="4">
+      <c r="D101" s="4">
         <f t="shared" si="9"/>
         <v>9790</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="16" t="s">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="B101" s="4" t="s">
+      <c r="B102" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C101" s="5">
+      <c r="C102" s="5">
         <v>1000</v>
       </c>
-      <c r="D101" s="4">
-        <f t="shared" ref="D101:D106" si="10">D100+C101</f>
+      <c r="D102" s="4">
+        <f t="shared" ref="D102:D107" si="10">D101+C102</f>
         <v>10790</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B102" s="4" t="s">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B103" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C102" s="5">
+      <c r="C103" s="5">
         <v>-10000</v>
       </c>
-      <c r="D102" s="4">
+      <c r="D103" s="4">
         <f t="shared" si="10"/>
         <v>790</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="16" t="s">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="B103" s="4" t="s">
+      <c r="B104" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C103" s="5">
+      <c r="C104" s="5">
         <v>800</v>
       </c>
-      <c r="D103" s="4">
+      <c r="D104" s="4">
         <f t="shared" si="10"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="16" t="s">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="B104" s="4" t="s">
+      <c r="B105" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C104" s="5">
+      <c r="C105" s="5">
         <v>5000</v>
       </c>
-      <c r="D104" s="4">
+      <c r="D105" s="4">
         <f t="shared" si="10"/>
         <v>6590</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="16" t="s">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="B105" s="4" t="s">
+      <c r="B106" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C105" s="5">
+      <c r="C106" s="5">
         <v>6000</v>
       </c>
-      <c r="D105" s="4">
+      <c r="D106" s="4">
         <f t="shared" si="10"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B106" s="4" t="s">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B107" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C106" s="5">
+      <c r="C107" s="5">
         <v>-10000</v>
       </c>
-      <c r="D106" s="4">
+      <c r="D107" s="4">
         <f t="shared" si="10"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="16" t="s">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="B107" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C107" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D107" s="4">
-        <f t="shared" ref="D107:D113" si="11">D106+C107</f>
-        <v>4590</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B108" s="4" t="s">
         <v>65</v>
       </c>
@@ -2623,926 +2626,926 @@
         <v>2000</v>
       </c>
       <c r="D108" s="4">
+        <f t="shared" ref="D108:D114" si="11">D107+C108</f>
+        <v>4590</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B109" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C109" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D109" s="4">
         <f t="shared" si="11"/>
         <v>6590</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B109" s="4" t="s">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B110" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C109" s="5">
+      <c r="C110" s="5">
         <v>7000</v>
       </c>
-      <c r="D109" s="4">
+      <c r="D110" s="4">
         <f t="shared" si="11"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B110" s="4" t="s">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B111" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C110" s="5">
+      <c r="C111" s="5">
         <v>-10000</v>
       </c>
-      <c r="D110" s="4">
+      <c r="D111" s="4">
         <f t="shared" si="11"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="16" t="s">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="B111" s="4" t="s">
+      <c r="B112" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C111" s="5">
+      <c r="C112" s="5">
         <v>2000</v>
       </c>
-      <c r="D111" s="4">
+      <c r="D112" s="4">
         <f t="shared" si="11"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="16" t="s">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="B112" s="4" t="s">
+      <c r="B113" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C112" s="5">
+      <c r="C113" s="5">
         <v>6000</v>
       </c>
-      <c r="D112" s="4">
+      <c r="D113" s="4">
         <f t="shared" si="11"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B113" s="4" t="s">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B114" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C113" s="5">
+      <c r="C114" s="5">
         <v>-10000</v>
       </c>
-      <c r="D113" s="4">
+      <c r="D114" s="4">
         <f t="shared" si="11"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="B114" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C114" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D114" s="4">
-        <f t="shared" ref="D114:D119" si="12">D113+C114</f>
-        <v>3590</v>
-      </c>
-    </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B115" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C115" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D115" s="4">
+        <f t="shared" ref="D115:D120" si="12">D114+C115</f>
+        <v>3590</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="B115" s="4" t="s">
+      <c r="B116" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C115" s="5">
+      <c r="C116" s="5">
         <v>7000</v>
       </c>
-      <c r="D115" s="4">
+      <c r="D116" s="4">
         <f t="shared" si="12"/>
         <v>10590</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B116" s="4" t="s">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B117" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C116" s="5">
+      <c r="C117" s="5">
         <v>-10000</v>
       </c>
-      <c r="D116" s="4">
+      <c r="D117" s="4">
         <f t="shared" si="12"/>
         <v>590</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B117" s="4" t="s">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B118" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C117" s="5">
+      <c r="C118" s="5">
         <v>12000</v>
       </c>
-      <c r="D117" s="4">
+      <c r="D118" s="4">
         <f t="shared" si="12"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B118" s="4" t="s">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B119" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C118" s="5">
+      <c r="C119" s="5">
         <v>-10000</v>
       </c>
-      <c r="D118" s="4">
+      <c r="D119" s="4">
         <f t="shared" si="12"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B119" s="4" t="s">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B120" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C119" s="5">
+      <c r="C120" s="5">
         <v>2000</v>
       </c>
-      <c r="D119" s="4">
+      <c r="D120" s="4">
         <f t="shared" si="12"/>
         <v>4590</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="B120" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C120" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D120" s="4">
-        <f t="shared" ref="D120:D125" si="13">D119+C120</f>
-        <v>6590</v>
-      </c>
-    </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="B121" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C121" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D121" s="4">
+        <f t="shared" ref="D121:D126" si="13">D120+C121</f>
+        <v>6590</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="B121" s="4" t="s">
+      <c r="B122" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C121" s="5">
+      <c r="C122" s="5">
         <v>7000</v>
       </c>
-      <c r="D121" s="4">
+      <c r="D122" s="4">
         <f t="shared" si="13"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B122" s="4" t="s">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B123" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C122" s="5">
+      <c r="C123" s="5">
         <v>-10000</v>
       </c>
-      <c r="D122" s="4">
+      <c r="D123" s="4">
         <f t="shared" si="13"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="16" t="s">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="B123" s="4" t="s">
+      <c r="B124" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C123" s="5">
+      <c r="C124" s="5">
         <v>2000</v>
       </c>
-      <c r="D123" s="4">
+      <c r="D124" s="4">
         <f t="shared" si="13"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="16" t="s">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="B124" s="4" t="s">
+      <c r="B125" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C124" s="5">
+      <c r="C125" s="5">
         <v>8000</v>
       </c>
-      <c r="D124" s="4">
+      <c r="D125" s="4">
         <f t="shared" si="13"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B125" s="4" t="s">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B126" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C125" s="5">
+      <c r="C126" s="5">
         <v>-10000</v>
       </c>
-      <c r="D125" s="4">
+      <c r="D126" s="4">
         <f t="shared" si="13"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="16" t="s">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="B126" s="4" t="s">
+      <c r="B127" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C126" s="5">
+      <c r="C127" s="5">
         <v>2000</v>
       </c>
-      <c r="D126" s="4">
-        <f t="shared" ref="D126:D131" si="14">D125+C126</f>
+      <c r="D127" s="4">
+        <f t="shared" ref="D127:D132" si="14">D126+C127</f>
         <v>5590</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B127" s="4" t="s">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B128" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C127" s="5">
+      <c r="C128" s="5">
         <v>5000</v>
       </c>
-      <c r="D127" s="4">
+      <c r="D128" s="4">
         <f t="shared" si="14"/>
         <v>10590</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B128" s="4" t="s">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B129" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C128" s="5">
+      <c r="C129" s="5">
         <v>-10000</v>
       </c>
-      <c r="D128" s="4">
+      <c r="D129" s="4">
         <f t="shared" si="14"/>
         <v>590</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B129" s="4" t="s">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B130" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C129" s="5">
+      <c r="C130" s="5">
         <v>2000</v>
       </c>
-      <c r="D129" s="4">
+      <c r="D130" s="4">
         <f t="shared" si="14"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B130" s="4" t="s">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B131" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C130" s="5">
+      <c r="C131" s="5">
         <v>9000</v>
       </c>
-      <c r="D130" s="4">
+      <c r="D131" s="4">
         <f t="shared" si="14"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B131" s="4" t="s">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B132" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C131" s="5">
+      <c r="C132" s="5">
         <v>-10000</v>
       </c>
-      <c r="D131" s="4">
+      <c r="D132" s="4">
         <f t="shared" si="14"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B132" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C132" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D132" s="4">
-        <f t="shared" ref="D132:D137" si="15">D131+C132</f>
-        <v>3590</v>
-      </c>
-    </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B133" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C133" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D133" s="4">
+        <f t="shared" ref="D133:D138" si="15">D132+C133</f>
+        <v>3590</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="B133" s="4" t="s">
+      <c r="B134" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C133" s="5">
+      <c r="C134" s="5">
         <v>8000</v>
       </c>
-      <c r="D133" s="4">
+      <c r="D134" s="4">
         <f t="shared" si="15"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B134" s="4" t="s">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B135" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C134" s="5">
+      <c r="C135" s="5">
         <v>-10000</v>
       </c>
-      <c r="D134" s="4">
+      <c r="D135" s="4">
         <f t="shared" si="15"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="16" t="s">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="B135" s="4" t="s">
+      <c r="B136" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C135" s="5">
+      <c r="C136" s="5">
         <v>2000</v>
       </c>
-      <c r="D135" s="4">
+      <c r="D136" s="4">
         <f t="shared" si="15"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="16" t="s">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="B136" s="4" t="s">
+      <c r="B137" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C136" s="5">
+      <c r="C137" s="5">
         <v>12000</v>
       </c>
-      <c r="D136" s="4">
+      <c r="D137" s="4">
         <f t="shared" si="15"/>
         <v>15590</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B137" s="4" t="s">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B138" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C137" s="5">
+      <c r="C138" s="5">
         <v>-10000</v>
       </c>
-      <c r="D137" s="4">
+      <c r="D138" s="4">
         <f t="shared" si="15"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="B138" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="C138" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D138" s="4">
-        <f t="shared" ref="D138:D143" si="16">D137+C138</f>
-        <v>7590</v>
-      </c>
-    </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="B139" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C139" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D139" s="4">
+        <f t="shared" ref="D139:D144" si="16">D138+C139</f>
+        <v>7590</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="B139" s="4" t="s">
+      <c r="B140" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="C139" s="5">
+      <c r="C140" s="5">
         <v>10000</v>
       </c>
-      <c r="D139" s="4">
+      <c r="D140" s="4">
         <f t="shared" si="16"/>
         <v>17590</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B140" s="4" t="s">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B141" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C140" s="5">
+      <c r="C141" s="5">
         <v>-10000</v>
       </c>
-      <c r="D140" s="4">
+      <c r="D141" s="4">
         <f t="shared" si="16"/>
         <v>7590</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B141" s="4" t="s">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B142" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="C141" s="5">
+      <c r="C142" s="5">
         <v>2000</v>
       </c>
-      <c r="D141" s="4">
+      <c r="D142" s="4">
         <f t="shared" si="16"/>
         <v>9590</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="16" t="s">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="B142" s="4" t="s">
+      <c r="B143" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="C142" s="5">
+      <c r="C143" s="5">
         <v>-1200</v>
       </c>
-      <c r="D142" s="4">
+      <c r="D143" s="4">
         <f t="shared" si="16"/>
         <v>8390</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B143" s="4" t="s">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B144" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="C143" s="5">
+      <c r="C144" s="5">
         <v>500</v>
       </c>
-      <c r="D143" s="4">
+      <c r="D144" s="4">
         <f t="shared" si="16"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="16" t="s">
-        <v>165</v>
-      </c>
-      <c r="B144" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="C144" s="5">
-        <v>750</v>
-      </c>
-      <c r="D144" s="4">
-        <f t="shared" ref="D144:D149" si="17">D143+C144</f>
-        <v>9640</v>
-      </c>
-    </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="B145" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C145" s="5">
+        <v>750</v>
+      </c>
+      <c r="D145" s="4">
+        <f t="shared" ref="D145:D150" si="17">D144+C145</f>
+        <v>9640</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="B145" s="4" t="s">
+      <c r="B146" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C145" s="5">
+      <c r="C146" s="5">
         <v>2000</v>
       </c>
-      <c r="D145" s="4">
+      <c r="D146" s="4">
         <f t="shared" si="17"/>
         <v>11640</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B146" s="4" t="s">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B147" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C146" s="5">
+      <c r="C147" s="5">
         <v>2000</v>
       </c>
-      <c r="D146" s="4">
+      <c r="D147" s="4">
         <f t="shared" si="17"/>
         <v>13640</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B147" s="4" t="s">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B148" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C147" s="5">
+      <c r="C148" s="5">
         <v>-10000</v>
       </c>
-      <c r="D147" s="4">
+      <c r="D148" s="4">
         <f t="shared" si="17"/>
         <v>3640</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B148" s="4" t="s">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B149" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="C148" s="5">
+      <c r="C149" s="5">
         <v>350</v>
       </c>
-      <c r="D148" s="4">
+      <c r="D149" s="4">
         <f t="shared" si="17"/>
         <v>3990</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="16" t="s">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="B149" s="4" t="s">
+      <c r="B150" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="C149" s="5">
+      <c r="C150" s="5">
         <v>300</v>
       </c>
-      <c r="D149" s="4">
+      <c r="D150" s="4">
         <f t="shared" si="17"/>
         <v>4290</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="16" t="s">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="B150" s="4" t="s">
+      <c r="B151" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="C150" s="5">
+      <c r="C151" s="5">
         <v>3800</v>
       </c>
-      <c r="D150" s="4">
-        <f t="shared" ref="D150:D156" si="18">D149+C150</f>
+      <c r="D151" s="4">
+        <f t="shared" ref="D151:D157" si="18">D150+C151</f>
         <v>8090</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B151" s="4" t="s">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B152" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C151" s="5">
+      <c r="C152" s="5">
         <v>500</v>
       </c>
-      <c r="D151" s="4">
+      <c r="D152" s="4">
         <f t="shared" si="18"/>
         <v>8590</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="16" t="s">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="B152" s="4" t="s">
+      <c r="B153" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="C152" s="5">
+      <c r="C153" s="5">
         <v>1300</v>
       </c>
-      <c r="D152" s="4">
+      <c r="D153" s="4">
         <f t="shared" si="18"/>
         <v>9890</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" s="16" t="s">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="B153" s="4" t="s">
+      <c r="B154" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C153" s="5">
+      <c r="C154" s="5">
         <v>9000</v>
       </c>
-      <c r="D153" s="4">
+      <c r="D154" s="4">
         <f t="shared" si="18"/>
         <v>18890</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B154" s="4" t="s">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B155" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C154" s="5">
+      <c r="C155" s="5">
         <v>-10000</v>
       </c>
-      <c r="D154" s="4">
+      <c r="D155" s="4">
         <f t="shared" si="18"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="16" t="s">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="B155" s="4" t="s">
+      <c r="B156" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C155" s="5">
+      <c r="C156" s="5">
         <v>2000</v>
       </c>
-      <c r="D155" s="4">
+      <c r="D156" s="4">
         <f t="shared" si="18"/>
         <v>10890</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B156" s="4" t="s">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B157" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C156" s="5">
+      <c r="C157" s="5">
         <v>-10000</v>
       </c>
-      <c r="D156" s="4">
+      <c r="D157" s="4">
         <f t="shared" si="18"/>
         <v>890</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="B157" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="C157" s="5">
-        <v>500</v>
-      </c>
-      <c r="D157" s="4">
-        <f t="shared" ref="D157:D162" si="19">D156+C157</f>
-        <v>1390</v>
-      </c>
-    </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="B158" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C158" s="5">
+        <v>500</v>
+      </c>
+      <c r="D158" s="4">
+        <f t="shared" ref="D158:D163" si="19">D157+C158</f>
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="B158" s="4" t="s">
+      <c r="B159" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="C158" s="5">
+      <c r="C159" s="5">
         <v>10000</v>
       </c>
-      <c r="D158" s="4">
+      <c r="D159" s="4">
         <f t="shared" si="19"/>
         <v>11390</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B159" s="4" t="s">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B160" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C159" s="5">
+      <c r="C160" s="5">
         <v>-10000</v>
       </c>
-      <c r="D159" s="4">
+      <c r="D160" s="4">
         <f t="shared" si="19"/>
         <v>1390</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="16" t="s">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="B160" s="4" t="s">
+      <c r="B161" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C160" s="5">
+      <c r="C161" s="5">
         <v>3000</v>
       </c>
-      <c r="D160" s="4">
+      <c r="D161" s="4">
         <f t="shared" si="19"/>
         <v>4390</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" s="16" t="s">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="B161" s="4" t="s">
+      <c r="B162" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C161" s="5">
+      <c r="C162" s="5">
         <v>2000</v>
       </c>
-      <c r="D161" s="4">
+      <c r="D162" s="4">
         <f t="shared" si="19"/>
         <v>6390</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B162" s="4" t="s">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B163" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C162" s="5">
+      <c r="C163" s="5">
         <v>2000</v>
       </c>
-      <c r="D162" s="4">
+      <c r="D163" s="4">
         <f t="shared" si="19"/>
         <v>8390</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163" s="16" t="s">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="B163" s="4" t="s">
+      <c r="B164" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C163" s="5">
+      <c r="C164" s="5">
         <v>11000</v>
       </c>
-      <c r="D163" s="4">
-        <f t="shared" ref="D163:D168" si="20">D162+C163</f>
+      <c r="D164" s="4">
+        <f t="shared" ref="D164:D169" si="20">D163+C164</f>
         <v>19390</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B164" s="4" t="s">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B165" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C164" s="5">
+      <c r="C165" s="5">
         <v>-10000</v>
       </c>
-      <c r="D164" s="4">
+      <c r="D165" s="4">
         <f t="shared" si="20"/>
         <v>9390</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" s="16" t="s">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" s="16" t="s">
         <v>187</v>
       </c>
-      <c r="B165" s="4" t="s">
+      <c r="B166" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C165" s="5">
+      <c r="C166" s="5">
         <v>3000</v>
       </c>
-      <c r="D165" s="4">
+      <c r="D166" s="4">
         <f t="shared" si="20"/>
         <v>12390</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B166" s="4" t="s">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B167" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C166" s="5">
+      <c r="C167" s="5">
         <v>-10000</v>
       </c>
-      <c r="D166" s="4">
+      <c r="D167" s="4">
         <f t="shared" si="20"/>
         <v>2390</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B167" s="4" t="s">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B168" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C167" s="5">
+      <c r="C168" s="5">
         <v>500</v>
       </c>
-      <c r="D167" s="4">
+      <c r="D168" s="4">
         <f t="shared" si="20"/>
         <v>2890</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A168" s="16" t="s">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" s="16" t="s">
         <v>189</v>
       </c>
-      <c r="B168" s="4" t="s">
+      <c r="B169" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C168" s="5">
+      <c r="C169" s="5">
         <v>5600</v>
       </c>
-      <c r="D168" s="4">
+      <c r="D169" s="4">
         <f t="shared" si="20"/>
         <v>8490</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B169" s="4" t="s">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B170" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="C169" s="5">
+      <c r="C170" s="5">
         <v>4700</v>
       </c>
-      <c r="D169" s="4">
-        <f t="shared" ref="D169:D175" si="21">D168+C169</f>
+      <c r="D170" s="4">
+        <f t="shared" ref="D170:D176" si="21">D169+C170</f>
         <v>13190</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" s="16" t="s">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" s="16" t="s">
         <v>192</v>
       </c>
-      <c r="B170" s="4" t="s">
+      <c r="B171" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C170" s="5">
+      <c r="C171" s="5">
         <v>1500</v>
       </c>
-      <c r="D170" s="4">
+      <c r="D171" s="4">
         <f t="shared" si="21"/>
         <v>14690</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B171" s="4" t="s">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B172" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C171" s="5">
+      <c r="C172" s="5">
         <v>500</v>
       </c>
-      <c r="D171" s="4">
+      <c r="D172" s="4">
         <f t="shared" si="21"/>
         <v>15190</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A172" s="16" t="s">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="B172" s="4" t="s">
+      <c r="B173" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="C172" s="5">
+      <c r="C173" s="5">
         <v>1000</v>
       </c>
-      <c r="D172" s="4">
+      <c r="D173" s="4">
         <f t="shared" si="21"/>
         <v>16190</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173" s="16" t="s">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="B173" s="4" t="s">
+      <c r="B174" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="C173" s="5">
+      <c r="C174" s="5">
         <v>1000</v>
       </c>
-      <c r="D173" s="4">
+      <c r="D174" s="4">
         <f t="shared" si="21"/>
         <v>17190</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174" s="16" t="s">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="B174" s="4" t="s">
+      <c r="B175" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C174" s="5">
+      <c r="C175" s="5">
         <v>3000</v>
       </c>
-      <c r="D174" s="4">
+      <c r="D175" s="4">
         <f t="shared" si="21"/>
         <v>20190</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B175" s="4" t="s">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B176" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C175" s="5">
+      <c r="C176" s="5">
         <v>-20000</v>
       </c>
-      <c r="D175" s="4">
+      <c r="D176" s="4">
         <f t="shared" si="21"/>
         <v>190</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B176" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C176" s="5">
-        <v>500</v>
-      </c>
-      <c r="D176" s="4">
-        <f t="shared" ref="D176:D182" si="22">D175+C176</f>
-        <v>690</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -3553,257 +3556,296 @@
         <v>500</v>
       </c>
       <c r="D177" s="4">
+        <f t="shared" ref="D177:D183" si="22">D176+C177</f>
+        <v>690</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B178" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C178" s="5">
+        <v>500</v>
+      </c>
+      <c r="D178" s="4">
         <f t="shared" si="22"/>
         <v>1190</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A178" s="16" t="s">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A179" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="B178" s="4" t="s">
+      <c r="B179" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="C178" s="5">
+      <c r="C179" s="5">
         <v>10000</v>
       </c>
-      <c r="D178" s="4">
+      <c r="D179" s="4">
         <f t="shared" si="22"/>
         <v>11190</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B179" s="4" t="s">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B180" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C179" s="5">
+      <c r="C180" s="5">
         <v>-10000</v>
       </c>
-      <c r="D179" s="4">
+      <c r="D180" s="4">
         <f t="shared" si="22"/>
         <v>1190</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" s="16" t="s">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A181" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="B180" s="4" t="s">
+      <c r="B181" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C180" s="5">
+      <c r="C181" s="5">
         <v>3000</v>
       </c>
-      <c r="D180" s="4">
+      <c r="D181" s="4">
         <f t="shared" si="22"/>
         <v>4190</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="16" t="s">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="B181" s="4" t="s">
+      <c r="B182" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C181" s="5">
+      <c r="C182" s="5">
         <v>11000</v>
       </c>
-      <c r="D181" s="4">
+      <c r="D182" s="4">
         <f t="shared" si="22"/>
         <v>15190</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B182" s="4" t="s">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B183" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C182" s="5">
+      <c r="C183" s="5">
         <v>-10000</v>
       </c>
-      <c r="D182" s="4">
+      <c r="D183" s="4">
         <f t="shared" si="22"/>
         <v>5190</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="B183" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C183" s="5">
-        <v>3000</v>
-      </c>
-      <c r="D183" s="4">
-        <f t="shared" ref="D183:D189" si="23">D182+C183</f>
-        <v>8190</v>
-      </c>
-    </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="B184" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C184" s="5">
+        <v>3000</v>
+      </c>
+      <c r="D184" s="4">
+        <f t="shared" ref="D184:D190" si="23">D183+C184</f>
+        <v>8190</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A185" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="B184" s="4" t="s">
+      <c r="B185" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="C184" s="5">
+      <c r="C185" s="5">
         <v>14000</v>
       </c>
-      <c r="D184" s="4">
+      <c r="D185" s="4">
         <f t="shared" si="23"/>
         <v>22190</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B185" s="4" t="s">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B186" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="C185" s="5">
+      <c r="C186" s="5">
         <v>-20000</v>
       </c>
-      <c r="D185" s="4">
+      <c r="D186" s="4">
         <f t="shared" si="23"/>
         <v>2190</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A186" s="16" t="s">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A187" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="B186" s="4" t="s">
+      <c r="B187" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="C186" s="5">
+      <c r="C187" s="5">
         <v>5000</v>
       </c>
-      <c r="D186" s="4">
+      <c r="D187" s="4">
         <f t="shared" si="23"/>
         <v>7190</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A187" s="16" t="s">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A188" s="16" t="s">
         <v>213</v>
       </c>
-      <c r="B187" s="4" t="s">
+      <c r="B188" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="C187" s="5">
+      <c r="C188" s="5">
         <v>5000</v>
       </c>
-      <c r="D187" s="4">
+      <c r="D188" s="4">
         <f t="shared" si="23"/>
         <v>12190</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A188" s="16" t="s">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189" s="16" t="s">
         <v>215</v>
       </c>
-      <c r="B188" s="4" t="s">
+      <c r="B189" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C188" s="5">
+      <c r="C189" s="5">
         <v>11000</v>
       </c>
-      <c r="D188" s="4">
+      <c r="D189" s="4">
         <f t="shared" si="23"/>
         <v>23190</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B189" s="4" t="s">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B190" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C189" s="5">
+      <c r="C190" s="5">
         <v>-20000</v>
       </c>
-      <c r="D189" s="4">
+      <c r="D190" s="4">
         <f t="shared" si="23"/>
         <v>3190</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A190" s="16" t="s">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A191" s="16" t="s">
         <v>216</v>
       </c>
-      <c r="B190" s="4" t="s">
+      <c r="B191" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C190" s="5">
+      <c r="C191" s="5">
         <v>500</v>
       </c>
-      <c r="D190" s="4">
-        <f>D189+C190</f>
+      <c r="D191" s="4">
+        <f t="shared" ref="D191:D196" si="24">D190+C191</f>
         <v>3690</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B191" s="4" t="s">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B192" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C191" s="5">
+      <c r="C192" s="5">
         <v>3000</v>
       </c>
-      <c r="D191" s="4">
-        <f>D190+C191</f>
+      <c r="D192" s="4">
+        <f t="shared" si="24"/>
         <v>6690</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A192" s="16" t="s">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A193" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="B192" s="4" t="s">
+      <c r="B193" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="C192" s="5">
+      <c r="C193" s="5">
         <v>12000</v>
       </c>
-      <c r="D192" s="4">
-        <f>D191+C192</f>
+      <c r="D193" s="4">
+        <f t="shared" si="24"/>
         <v>18690</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B193" s="4" t="s">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B194" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C193" s="5">
+      <c r="C194" s="5">
         <v>-10000</v>
       </c>
-      <c r="D193" s="4">
-        <f>D192+C193</f>
+      <c r="D194" s="4">
+        <f t="shared" si="24"/>
         <v>8690</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194" s="16" t="s">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A195" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="B194" s="4" t="s">
+      <c r="B195" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="C194" s="5">
+      <c r="C195" s="5">
         <v>5000</v>
       </c>
-      <c r="D194" s="4">
-        <f>D193+C194</f>
+      <c r="D195" s="4">
+        <f t="shared" si="24"/>
         <v>13690</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B195" s="4" t="s">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B196" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C195" s="5">
+      <c r="C196" s="5">
         <v>-10000</v>
       </c>
-      <c r="D195" s="4">
-        <f>D194+C195</f>
+      <c r="D196" s="4">
+        <f t="shared" si="24"/>
         <v>3690</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A197" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="B197" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="C197" s="5">
+        <v>12000</v>
+      </c>
+      <c r="D197" s="4">
+        <f>D196+C197</f>
+        <v>15690</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B198" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C198" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D198" s="4">
+        <f>D197+C198</f>
+        <v>5690</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chi diem tra 500k
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="CÔ DIỄM" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="HÀ" sheetId="4" r:id="rId3"/>
     <sheet name="GIANG" sheetId="5" r:id="rId4"/>
     <sheet name="Tổng Kết" sheetId="6" r:id="rId5"/>
+    <sheet name="chị Diễm" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="226">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -687,6 +688,15 @@
   </si>
   <si>
     <t>Duy lấy tiền lãi 12tr</t>
+  </si>
+  <si>
+    <t>Chị Diễm chuyển 500k</t>
+  </si>
+  <si>
+    <t>Còn</t>
+  </si>
+  <si>
+    <t>Tổng nợ</t>
   </si>
 </sst>
 </file>
@@ -696,7 +706,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -712,8 +722,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -729,6 +754,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -793,7 +824,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -852,6 +883,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1158,8 +1199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K198"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
@@ -4465,4 +4506,74 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" style="20" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" style="21" customWidth="1"/>
+    <col min="3" max="3" width="31.85546875" style="22" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" style="21" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="21"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="23"/>
+      <c r="B2" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="C2" s="25">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="23" t="s">
+        <v>221</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>223</v>
+      </c>
+      <c r="C3" s="27">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="23"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="27"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="23"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="27"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="23"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="27"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="23" t="s">
+        <v>221</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>224</v>
+      </c>
+      <c r="C7" s="29">
+        <f>C2-SUM(C3:C6)</f>
+        <v>2500</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
duy lay tien loi co diem 1tr
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="CÔ DIỄM" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="229">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -700,6 +700,12 @@
   </si>
   <si>
     <t>03/10/2024</t>
+  </si>
+  <si>
+    <t>06/10/2024</t>
+  </si>
+  <si>
+    <t>Duy lấy 1tr tiền lời</t>
   </si>
 </sst>
 </file>
@@ -1200,11 +1206,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K199"/>
+  <dimension ref="A1:K200"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A176" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D200" sqref="D200"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A179" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D201" sqref="D201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3905,6 +3911,21 @@
       <c r="D199" s="4">
         <f>D198+C199</f>
         <v>7690</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A200" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="B200" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="C200" s="5">
+        <v>1000</v>
+      </c>
+      <c r="D200" s="4">
+        <f>D199+C200</f>
+        <v>8690</v>
       </c>
     </row>
   </sheetData>
@@ -4530,7 +4551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
duy lay tien loi co diem ngay 13
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="230">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -706,6 +706,9 @@
   </si>
   <si>
     <t>Duy lấy 1tr tiền lời</t>
+  </si>
+  <si>
+    <t>13/10/2024</t>
   </si>
 </sst>
 </file>
@@ -1206,11 +1209,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K200"/>
+  <dimension ref="A1:K203"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A179" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D201" sqref="D201"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1286,8 +1289,8 @@
         <v>20</v>
       </c>
       <c r="J3" s="4">
-        <f>SUM(I3:I67)</f>
-        <v>560</v>
+        <f>SUM(I3:I68)</f>
+        <v>570</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1307,18 +1310,8 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="5">
-        <v>14560</v>
-      </c>
-      <c r="D6" s="4">
-        <f>C6+D3</f>
-        <v>18490</v>
-      </c>
       <c r="H6" s="16" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="I6" s="5">
         <v>10</v>
@@ -1326,17 +1319,17 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C7" s="5">
-        <v>-10000</v>
+        <v>14560</v>
       </c>
       <c r="D7" s="4">
-        <f t="shared" ref="D7:D23" si="0">D6+C7</f>
-        <v>8490</v>
+        <f>C7+D3</f>
+        <v>18490</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I7" s="5">
         <v>10</v>
@@ -1344,25 +1337,35 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D8" s="4">
+        <f t="shared" ref="D8:D24" si="0">D7+C8</f>
+        <v>8490</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C9" s="5">
         <v>2000</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D9" s="4">
         <f t="shared" si="0"/>
         <v>10490</v>
       </c>
-      <c r="H8" s="16" t="s">
+      <c r="H9" s="16" t="s">
         <v>9</v>
-      </c>
-      <c r="I8" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H9" s="16" t="s">
-        <v>41</v>
       </c>
       <c r="I9" s="5">
         <v>10</v>
@@ -1370,16 +1373,15 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H10" s="16" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="I10" s="5">
         <v>10</v>
       </c>
-      <c r="K10" s="14"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H11" s="16" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="I11" s="5">
         <v>10</v>
@@ -1388,7 +1390,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H12" s="16" t="s">
-        <v>127</v>
+        <v>96</v>
       </c>
       <c r="I12" s="5">
         <v>10</v>
@@ -1397,7 +1399,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H13" s="16" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="I13" s="5">
         <v>10</v>
@@ -1406,7 +1408,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H14" s="16" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="I14" s="5">
         <v>10</v>
@@ -1415,7 +1417,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H15" s="16" t="s">
-        <v>177</v>
+        <v>142</v>
       </c>
       <c r="I15" s="5">
         <v>10</v>
@@ -1424,7 +1426,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H16" s="16" t="s">
-        <v>200</v>
+        <v>177</v>
       </c>
       <c r="I16" s="5">
         <v>10</v>
@@ -1433,25 +1435,25 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H17" s="16" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="I17" s="5">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K17" s="14"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H18" s="16" t="s">
-        <v>70</v>
+        <v>215</v>
       </c>
       <c r="I18" s="5">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="K18" s="14"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H19" s="16" t="s">
-        <v>107</v>
+        <v>70</v>
       </c>
       <c r="I19" s="5">
         <v>10</v>
@@ -1460,79 +1462,79 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H20" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="I20" s="5">
+        <v>10</v>
+      </c>
+      <c r="K20" s="14"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H21" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="I20" s="5">
-        <v>10</v>
-      </c>
-      <c r="K20" s="14"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="4" t="s">
+      <c r="I21" s="5">
+        <v>10</v>
+      </c>
+      <c r="K21" s="14"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C22" s="5">
         <v>-10000</v>
       </c>
-      <c r="D21" s="4">
-        <f>D8+C21</f>
+      <c r="D22" s="4">
+        <f>D9+C22</f>
         <v>490</v>
       </c>
-      <c r="H21" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="I21" s="5">
-        <v>10</v>
-      </c>
-      <c r="K21" s="14"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="16" t="s">
+      <c r="H22" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" s="5">
+        <v>10</v>
+      </c>
+      <c r="K22" s="14"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B23" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C23" s="5">
         <v>2000</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D23" s="4">
         <f t="shared" si="0"/>
         <v>2490</v>
       </c>
-      <c r="H22" s="16" t="s">
+      <c r="H23" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="I22" s="5">
-        <v>10</v>
-      </c>
-      <c r="K22" s="14"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="16" t="s">
+      <c r="I23" s="5">
+        <v>10</v>
+      </c>
+      <c r="K23" s="14"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B24" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C24" s="5">
         <v>3000</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D24" s="4">
         <f t="shared" si="0"/>
         <v>5490</v>
       </c>
-      <c r="H23" s="16" t="s">
+      <c r="H24" s="16" t="s">
         <v>24</v>
-      </c>
-      <c r="I23" s="5">
-        <v>10</v>
-      </c>
-      <c r="K23" s="14"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H24" s="16" t="s">
-        <v>59</v>
       </c>
       <c r="I24" s="5">
         <v>10</v>
@@ -1541,7 +1543,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H25" s="16" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="I25" s="5">
         <v>10</v>
@@ -1550,7 +1552,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H26" s="16" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="I26" s="5">
         <v>10</v>
@@ -1559,7 +1561,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H27" s="16" t="s">
-        <v>119</v>
+        <v>91</v>
       </c>
       <c r="I27" s="5">
         <v>10</v>
@@ -1568,7 +1570,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H28" s="16" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="I28" s="5">
         <v>10</v>
@@ -1577,7 +1579,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H29" s="16" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="I29" s="5">
         <v>10</v>
@@ -1586,7 +1588,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H30" s="16" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="I30" s="5">
         <v>10</v>
@@ -1595,7 +1597,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H31" s="16" t="s">
-        <v>181</v>
+        <v>144</v>
       </c>
       <c r="I31" s="5">
         <v>10</v>
@@ -1604,7 +1606,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H32" s="16" t="s">
-        <v>205</v>
+        <v>181</v>
       </c>
       <c r="I32" s="5">
         <v>10</v>
@@ -1613,38 +1615,38 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H33" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="I33" s="5">
+        <v>10</v>
+      </c>
+      <c r="K33" s="14"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H34" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="I33" s="5">
-        <v>10</v>
-      </c>
-      <c r="K33" s="14"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="16" t="s">
+      <c r="I34" s="5">
+        <v>10</v>
+      </c>
+      <c r="K34" s="14"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B35" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C35" s="5">
         <v>3000</v>
       </c>
-      <c r="D34" s="4">
-        <f>D23+C34</f>
+      <c r="D35" s="4">
+        <f>D24+C35</f>
         <v>8490</v>
       </c>
-      <c r="H34" s="16" t="s">
+      <c r="H35" s="16" t="s">
         <v>12</v>
-      </c>
-      <c r="I34" s="5">
-        <v>10</v>
-      </c>
-      <c r="K34" s="14"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H35" s="16" t="s">
-        <v>43</v>
       </c>
       <c r="I35" s="5">
         <v>10</v>
@@ -1653,7 +1655,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H36" s="16" t="s">
-        <v>139</v>
+        <v>43</v>
       </c>
       <c r="I36" s="5">
         <v>10</v>
@@ -1662,7 +1664,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H37" s="16" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="I37" s="5">
         <v>10</v>
@@ -1671,7 +1673,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H38" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I38" s="5">
         <v>10</v>
@@ -1680,64 +1682,54 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H39" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="I39" s="5">
+        <v>10</v>
+      </c>
+      <c r="K39" s="14"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H40" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="I39" s="5">
-        <v>10</v>
-      </c>
-      <c r="K39" s="14"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B40" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C40" s="5">
-        <v>4400</v>
-      </c>
-      <c r="D40" s="4">
-        <f>D34+C40</f>
-        <v>12890</v>
-      </c>
-      <c r="H40" s="16" t="s">
-        <v>157</v>
-      </c>
       <c r="I40" s="5">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K40" s="14"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C41" s="5">
-        <v>-10000</v>
+        <v>4400</v>
       </c>
       <c r="D41" s="4">
-        <f>D40+C41</f>
-        <v>2890</v>
+        <f>D35+C41</f>
+        <v>12890</v>
       </c>
       <c r="H41" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I41" s="5">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="K41" s="14"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C42" s="5">
-        <v>1600</v>
+        <v>-10000</v>
       </c>
       <c r="D42" s="4">
-        <f t="shared" ref="D42:D49" si="1">D41+C42</f>
-        <v>4490</v>
+        <f>D41+C42</f>
+        <v>2890</v>
       </c>
       <c r="H42" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I42" s="5">
         <v>10</v>
@@ -1746,171 +1738,181 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C43" s="5">
+        <v>1600</v>
+      </c>
+      <c r="D43" s="4">
+        <f t="shared" ref="D43:D50" si="1">D42+C43</f>
+        <v>4490</v>
+      </c>
+      <c r="H43" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="I43" s="5">
+        <v>10</v>
+      </c>
+      <c r="K43" s="14"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B44" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C43" s="5">
+      <c r="C44" s="5">
         <v>3000</v>
       </c>
-      <c r="D43" s="4">
+      <c r="D44" s="4">
         <f t="shared" si="1"/>
         <v>7490</v>
       </c>
-      <c r="H43" s="16" t="s">
+      <c r="H44" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="I43" s="5">
-        <v>10</v>
-      </c>
-      <c r="K43" s="14"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="16" t="s">
+      <c r="I44" s="5">
+        <v>10</v>
+      </c>
+      <c r="K44" s="14"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B45" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C45" s="5">
         <v>2000</v>
       </c>
-      <c r="D44" s="4">
+      <c r="D45" s="4">
         <f t="shared" si="1"/>
         <v>9490</v>
       </c>
-      <c r="H44" s="16" t="s">
+      <c r="H45" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="I44" s="5">
-        <v>10</v>
-      </c>
-      <c r="K44" s="14"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="16" t="s">
+      <c r="I45" s="5">
+        <v>10</v>
+      </c>
+      <c r="K45" s="14"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B46" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C45" s="5">
+      <c r="C46" s="5">
         <v>3000</v>
       </c>
-      <c r="D45" s="4">
+      <c r="D46" s="4">
         <f t="shared" si="1"/>
         <v>12490</v>
       </c>
-      <c r="H45" s="16" t="s">
+      <c r="H46" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="I45" s="5">
-        <v>10</v>
-      </c>
-      <c r="K45" s="14"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B46" s="4" t="s">
+      <c r="I46" s="5">
+        <v>10</v>
+      </c>
+      <c r="K46" s="14"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B47" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C46" s="5">
+      <c r="C47" s="5">
         <v>-10000</v>
       </c>
-      <c r="D46" s="4">
+      <c r="D47" s="4">
         <f t="shared" si="1"/>
         <v>2490</v>
       </c>
-      <c r="H46" s="16" t="s">
+      <c r="H47" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="I46" s="5">
-        <v>10</v>
-      </c>
-      <c r="K46" s="14"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="16" t="s">
+      <c r="I47" s="5">
+        <v>10</v>
+      </c>
+      <c r="K47" s="14"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B48" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C48" s="5">
         <v>4960</v>
       </c>
-      <c r="D47" s="4">
+      <c r="D48" s="4">
         <f t="shared" si="1"/>
         <v>7450</v>
       </c>
-      <c r="H47" s="16" t="s">
+      <c r="H48" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="I47" s="5">
-        <v>10</v>
-      </c>
-      <c r="K47" s="14"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="16" t="s">
+      <c r="I48" s="5">
+        <v>10</v>
+      </c>
+      <c r="K48" s="14"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B49" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C48" s="5">
+      <c r="C49" s="5">
         <v>4000</v>
       </c>
-      <c r="D48" s="4">
+      <c r="D49" s="4">
         <f t="shared" si="1"/>
         <v>11450</v>
       </c>
-      <c r="H48" s="16" t="s">
+      <c r="H49" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="I48" s="5">
-        <v>10</v>
-      </c>
-      <c r="K48" s="14"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B49" s="4" t="s">
+      <c r="I49" s="5">
+        <v>10</v>
+      </c>
+      <c r="K49" s="14"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B50" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C49" s="5">
+      <c r="C50" s="5">
         <v>-10000</v>
       </c>
-      <c r="D49" s="4">
+      <c r="D50" s="4">
         <f t="shared" si="1"/>
         <v>1450</v>
       </c>
-      <c r="H49" s="16" t="s">
+      <c r="H50" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="I49" s="5">
-        <v>10</v>
-      </c>
-      <c r="K49" s="14"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B50" s="4" t="s">
+      <c r="I50" s="5">
+        <v>10</v>
+      </c>
+      <c r="K50" s="14"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B51" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C50" s="5">
+      <c r="C51" s="5">
         <v>7640</v>
       </c>
-      <c r="D50" s="4">
-        <f t="shared" ref="D50:D57" si="2">D49+C50</f>
+      <c r="D51" s="4">
+        <f t="shared" ref="D51:D58" si="2">D50+C51</f>
         <v>9090</v>
       </c>
-      <c r="H50" s="16" t="s">
+      <c r="H51" s="16" t="s">
         <v>185</v>
-      </c>
-      <c r="I50" s="5">
-        <v>10</v>
-      </c>
-      <c r="K50" s="14"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H51" s="16" t="s">
-        <v>221</v>
       </c>
       <c r="I51" s="5">
         <v>10</v>
@@ -1919,366 +1921,360 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H52" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="I52" s="5">
+        <v>10</v>
+      </c>
+      <c r="K52" s="14"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H53" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="I52" s="5">
+      <c r="I53" s="5">
         <v>20</v>
       </c>
-      <c r="K52" s="14"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B53" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C53" s="5">
-        <v>3000</v>
-      </c>
-      <c r="D53" s="4">
-        <f>D50+C53</f>
-        <v>12090</v>
-      </c>
-      <c r="H53" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="I53" s="5">
-        <v>10</v>
-      </c>
+      <c r="K53" s="14"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B54" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C54" s="5">
+        <v>3000</v>
+      </c>
+      <c r="D54" s="4">
+        <f>D51+C54</f>
+        <v>12090</v>
+      </c>
+      <c r="H54" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="I54" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B55" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C54" s="5">
+      <c r="C55" s="5">
         <v>-10000</v>
       </c>
-      <c r="D54" s="4">
+      <c r="D55" s="4">
         <f t="shared" si="2"/>
         <v>2090</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B55" s="4" t="s">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B56" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C55" s="5">
+      <c r="C56" s="5">
         <v>800</v>
       </c>
-      <c r="D55" s="4">
+      <c r="D56" s="4">
         <f t="shared" si="2"/>
         <v>2890</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="16" t="s">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B57" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C56" s="5">
+      <c r="C57" s="5">
         <v>2000</v>
       </c>
-      <c r="D56" s="4">
+      <c r="D57" s="4">
         <f t="shared" si="2"/>
         <v>4890</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="16" t="s">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B58" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C57" s="5">
+      <c r="C58" s="5">
         <v>4000</v>
       </c>
-      <c r="D57" s="4">
+      <c r="D58" s="4">
         <f t="shared" si="2"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="16" t="s">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B59" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C58" s="5">
+      <c r="C59" s="5">
         <v>4000</v>
       </c>
-      <c r="D58" s="4">
-        <f t="shared" ref="D58:D63" si="3">D57+C58</f>
+      <c r="D59" s="4">
+        <f t="shared" ref="D59:D64" si="3">D58+C59</f>
         <v>12890</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B59" s="4" t="s">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B60" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C59" s="5">
+      <c r="C60" s="5">
         <v>5000</v>
       </c>
-      <c r="D59" s="4">
+      <c r="D60" s="4">
         <f t="shared" si="3"/>
         <v>17890</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B60" s="4" t="s">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B61" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C60" s="5">
+      <c r="C61" s="5">
         <v>-10000</v>
       </c>
-      <c r="D60" s="4">
+      <c r="D61" s="4">
         <f t="shared" si="3"/>
         <v>7890</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61" s="16">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" s="16">
         <v>44969</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B62" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C61" s="5">
+      <c r="C62" s="5">
         <v>900</v>
       </c>
-      <c r="D61" s="4">
+      <c r="D62" s="4">
         <f t="shared" si="3"/>
         <v>8790</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B62" s="4" t="s">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B63" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C62" s="5">
+      <c r="C63" s="5">
         <v>4000</v>
       </c>
-      <c r="D62" s="4">
+      <c r="D63" s="4">
         <f t="shared" si="3"/>
         <v>12790</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B63" s="4" t="s">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B64" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C63" s="5">
+      <c r="C64" s="5">
         <v>-10000</v>
       </c>
-      <c r="D63" s="4">
+      <c r="D64" s="4">
         <f t="shared" si="3"/>
         <v>2790</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C64" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D64" s="4">
-        <f t="shared" ref="D64:D71" si="4">D63+C64</f>
-        <v>4790</v>
-      </c>
-    </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C65" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D65" s="4">
+        <f t="shared" ref="D65:D72" si="4">D64+C65</f>
+        <v>4790</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B66" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C65" s="5">
+      <c r="C66" s="5">
         <v>700</v>
       </c>
-      <c r="D65" s="4">
+      <c r="D66" s="4">
         <f t="shared" si="4"/>
         <v>5490</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B66" s="4" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B67" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C66" s="5">
+      <c r="C67" s="5">
         <v>4000</v>
       </c>
-      <c r="D66" s="4">
+      <c r="D67" s="4">
         <f t="shared" si="4"/>
         <v>9490</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="16" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B68" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C67" s="5">
+      <c r="C68" s="5">
         <v>600</v>
       </c>
-      <c r="D67" s="4">
+      <c r="D68" s="4">
         <f t="shared" si="4"/>
         <v>10090</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B68" s="4" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B69" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C68" s="5">
+      <c r="C69" s="5">
         <v>-10000</v>
       </c>
-      <c r="D68" s="4">
+      <c r="D69" s="4">
         <f t="shared" si="4"/>
         <v>90</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="16" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B70" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C69" s="5">
+      <c r="C70" s="5">
         <f>700+5000+300+600+400+1000+800</f>
         <v>8800</v>
       </c>
-      <c r="D69" s="4">
+      <c r="D70" s="4">
         <f t="shared" si="4"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B70" s="4" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B71" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C70" s="5">
+      <c r="C71" s="5">
         <v>6000</v>
       </c>
-      <c r="D70" s="4">
+      <c r="D71" s="4">
         <f t="shared" si="4"/>
         <v>14890</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B71" s="4" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B72" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C71" s="5">
+      <c r="C72" s="5">
         <v>-10000</v>
       </c>
-      <c r="D71" s="4">
+      <c r="D72" s="4">
         <f t="shared" si="4"/>
         <v>4890</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="16" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B73" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C72" s="5">
+      <c r="C73" s="5">
         <v>500</v>
       </c>
-      <c r="D72" s="4">
-        <f t="shared" ref="D72:D77" si="5">D71+C72</f>
+      <c r="D73" s="4">
+        <f t="shared" ref="D73:D78" si="5">D72+C73</f>
         <v>5390</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B73" s="4" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C73" s="5">
+      <c r="C74" s="5">
         <v>700</v>
       </c>
-      <c r="D73" s="4">
+      <c r="D74" s="4">
         <f t="shared" si="5"/>
         <v>6090</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B74" s="4" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B75" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C74" s="5">
+      <c r="C75" s="5">
         <v>1500</v>
       </c>
-      <c r="D74" s="4">
+      <c r="D75" s="4">
         <f t="shared" si="5"/>
         <v>7590</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B75" s="4" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B76" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C75" s="5">
+      <c r="C76" s="5">
         <v>5000</v>
       </c>
-      <c r="D75" s="4">
+      <c r="D76" s="4">
         <f t="shared" si="5"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B76" s="4" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B77" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C76" s="5">
+      <c r="C77" s="5">
         <v>-10000</v>
       </c>
-      <c r="D76" s="4">
+      <c r="D77" s="4">
         <f t="shared" si="5"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="16" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="B78" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C77" s="5">
+      <c r="C78" s="5">
         <v>2000</v>
       </c>
-      <c r="D77" s="4">
+      <c r="D78" s="4">
         <f t="shared" si="5"/>
         <v>4590</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B78" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C78" s="5">
-        <v>700</v>
-      </c>
-      <c r="D78" s="4">
-        <f t="shared" ref="D78:D83" si="6">D77+C78</f>
-        <v>5290</v>
-      </c>
-    </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="16" t="s">
-        <v>82</v>
-      </c>
       <c r="B79" s="4" t="s">
         <v>77</v>
       </c>
@@ -2286,401 +2282,404 @@
         <v>700</v>
       </c>
       <c r="D79" s="4">
+        <f t="shared" ref="D79:D84" si="6">D78+C79</f>
+        <v>5290</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C80" s="5">
+        <v>700</v>
+      </c>
+      <c r="D80" s="4">
         <f t="shared" si="6"/>
         <v>5990</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="16" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B81" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C80" s="5">
+      <c r="C81" s="5">
         <v>700</v>
       </c>
-      <c r="D80" s="4">
+      <c r="D81" s="4">
         <f t="shared" si="6"/>
         <v>6690</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="16" t="s">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="B81" s="4" t="s">
+      <c r="B82" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C81" s="5">
+      <c r="C82" s="5">
         <v>4000</v>
       </c>
-      <c r="D81" s="4">
+      <c r="D82" s="4">
         <f t="shared" si="6"/>
         <v>10690</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B82" s="4" t="s">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B83" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C82" s="5">
+      <c r="C83" s="5">
         <v>-10000</v>
       </c>
-      <c r="D82" s="4">
+      <c r="D83" s="4">
         <f t="shared" si="6"/>
         <v>690</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="16" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="B84" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C83" s="5">
+      <c r="C84" s="5">
         <v>1000</v>
       </c>
-      <c r="D83" s="4">
+      <c r="D84" s="4">
         <f t="shared" si="6"/>
         <v>1690</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="16" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="B84" s="4" t="s">
+      <c r="B85" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C84" s="5">
+      <c r="C85" s="5">
         <v>7000</v>
       </c>
-      <c r="D84" s="4">
-        <f t="shared" ref="D84:D89" si="7">D83+C84</f>
+      <c r="D85" s="4">
+        <f t="shared" ref="D85:D90" si="7">D84+C85</f>
         <v>8690</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B85" s="4" t="s">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B86" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C85" s="5">
+      <c r="C86" s="5">
         <v>10000</v>
       </c>
-      <c r="D85" s="4">
+      <c r="D86" s="4">
         <f t="shared" si="7"/>
         <v>18690</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B86" s="4" t="s">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B87" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C86" s="5">
+      <c r="C87" s="5">
         <v>-10000</v>
       </c>
-      <c r="D86" s="4">
+      <c r="D87" s="4">
         <f t="shared" si="7"/>
         <v>8690</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B87" s="4" t="s">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B88" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C87" s="5">
+      <c r="C88" s="5">
         <v>1700</v>
       </c>
-      <c r="D87" s="4">
+      <c r="D88" s="4">
         <f t="shared" si="7"/>
         <v>10390</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B88" s="4" t="s">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B89" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C88" s="5">
+      <c r="C89" s="5">
         <v>-10000</v>
       </c>
-      <c r="D88" s="4">
+      <c r="D89" s="4">
         <f t="shared" si="7"/>
         <v>390</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B89" s="4" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B90" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C89" s="5">
+      <c r="C90" s="5">
         <v>6000</v>
       </c>
-      <c r="D89" s="4">
+      <c r="D90" s="4">
         <f t="shared" si="7"/>
         <v>6390</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="B90" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C90" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D90" s="4">
-        <f t="shared" ref="D90:D95" si="8">D89+C90</f>
-        <v>8390</v>
-      </c>
-    </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C91" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D91" s="4">
+        <f t="shared" ref="D91:D96" si="8">D90+C91</f>
+        <v>8390</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="B91" s="4" t="s">
+      <c r="B92" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C91" s="5">
+      <c r="C92" s="5">
         <v>5000</v>
       </c>
-      <c r="D91" s="4">
+      <c r="D92" s="4">
         <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B92" s="4" t="s">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B93" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C92" s="5">
+      <c r="C93" s="5">
         <v>-10000</v>
       </c>
-      <c r="D92" s="4">
+      <c r="D93" s="4">
         <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="16" t="s">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="B93" s="4" t="s">
+      <c r="B94" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C93" s="5">
+      <c r="C94" s="5">
         <v>1000</v>
       </c>
-      <c r="D93" s="4">
+      <c r="D94" s="4">
         <f t="shared" si="8"/>
         <v>4390</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B94" s="4" t="s">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B95" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C94" s="5">
+      <c r="C95" s="5">
         <v>9000</v>
       </c>
-      <c r="D94" s="4">
+      <c r="D95" s="4">
         <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B95" s="4" t="s">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B96" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C95" s="5">
+      <c r="C96" s="5">
         <v>-10000</v>
       </c>
-      <c r="D95" s="4">
+      <c r="D96" s="4">
         <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B96" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C96" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D96" s="4">
-        <f t="shared" ref="D96:D101" si="9">D95+C96</f>
-        <v>5390</v>
-      </c>
-    </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B97" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C97" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D97" s="4">
+        <f t="shared" ref="D97:D102" si="9">D96+C97</f>
+        <v>5390</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B98" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C97" s="5">
+      <c r="C98" s="5">
         <v>6000</v>
       </c>
-      <c r="D97" s="4">
+      <c r="D98" s="4">
         <f t="shared" si="9"/>
         <v>11390</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B98" s="4" t="s">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B99" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C98" s="5">
+      <c r="C99" s="5">
         <v>-10000</v>
       </c>
-      <c r="D98" s="4">
+      <c r="D99" s="4">
         <f t="shared" si="9"/>
         <v>1390</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B99" s="4" t="s">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B100" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C99" s="5">
+      <c r="C100" s="5">
         <v>400</v>
       </c>
-      <c r="D99" s="4">
+      <c r="D100" s="4">
         <f t="shared" si="9"/>
         <v>1790</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="16" t="s">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="B100" s="4" t="s">
+      <c r="B101" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C100" s="5">
+      <c r="C101" s="5">
         <v>2000</v>
       </c>
-      <c r="D100" s="4">
+      <c r="D101" s="4">
         <f t="shared" si="9"/>
         <v>3790</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="16" t="s">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="B101" s="4" t="s">
+      <c r="B102" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C101" s="5">
+      <c r="C102" s="5">
         <v>6000</v>
       </c>
-      <c r="D101" s="4">
+      <c r="D102" s="4">
         <f t="shared" si="9"/>
         <v>9790</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="16" t="s">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="B102" s="4" t="s">
+      <c r="B103" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C102" s="5">
+      <c r="C103" s="5">
         <v>1000</v>
       </c>
-      <c r="D102" s="4">
-        <f t="shared" ref="D102:D107" si="10">D101+C102</f>
+      <c r="D103" s="4">
+        <f t="shared" ref="D103:D108" si="10">D102+C103</f>
         <v>10790</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B103" s="4" t="s">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B104" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C103" s="5">
+      <c r="C104" s="5">
         <v>-10000</v>
       </c>
-      <c r="D103" s="4">
+      <c r="D104" s="4">
         <f t="shared" si="10"/>
         <v>790</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="16" t="s">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="B104" s="4" t="s">
+      <c r="B105" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C104" s="5">
+      <c r="C105" s="5">
         <v>800</v>
       </c>
-      <c r="D104" s="4">
+      <c r="D105" s="4">
         <f t="shared" si="10"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="16" t="s">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="B105" s="4" t="s">
+      <c r="B106" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C105" s="5">
+      <c r="C106" s="5">
         <v>5000</v>
       </c>
-      <c r="D105" s="4">
+      <c r="D106" s="4">
         <f t="shared" si="10"/>
         <v>6590</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="16" t="s">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="B106" s="4" t="s">
+      <c r="B107" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C106" s="5">
+      <c r="C107" s="5">
         <v>6000</v>
       </c>
-      <c r="D106" s="4">
+      <c r="D107" s="4">
         <f t="shared" si="10"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B107" s="4" t="s">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B108" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C107" s="5">
+      <c r="C108" s="5">
         <v>-10000</v>
       </c>
-      <c r="D107" s="4">
+      <c r="D108" s="4">
         <f t="shared" si="10"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="16" t="s">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="B108" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C108" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D108" s="4">
-        <f t="shared" ref="D108:D114" si="11">D107+C108</f>
-        <v>4590</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B109" s="4" t="s">
         <v>65</v>
       </c>
@@ -2688,926 +2687,926 @@
         <v>2000</v>
       </c>
       <c r="D109" s="4">
+        <f t="shared" ref="D109:D115" si="11">D108+C109</f>
+        <v>4590</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B110" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C110" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D110" s="4">
         <f t="shared" si="11"/>
         <v>6590</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B110" s="4" t="s">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B111" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C110" s="5">
+      <c r="C111" s="5">
         <v>7000</v>
       </c>
-      <c r="D110" s="4">
+      <c r="D111" s="4">
         <f t="shared" si="11"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B111" s="4" t="s">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B112" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C111" s="5">
+      <c r="C112" s="5">
         <v>-10000</v>
       </c>
-      <c r="D111" s="4">
+      <c r="D112" s="4">
         <f t="shared" si="11"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="16" t="s">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="B112" s="4" t="s">
+      <c r="B113" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C112" s="5">
+      <c r="C113" s="5">
         <v>2000</v>
       </c>
-      <c r="D112" s="4">
+      <c r="D113" s="4">
         <f t="shared" si="11"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="16" t="s">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="B113" s="4" t="s">
+      <c r="B114" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C113" s="5">
+      <c r="C114" s="5">
         <v>6000</v>
       </c>
-      <c r="D113" s="4">
+      <c r="D114" s="4">
         <f t="shared" si="11"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B114" s="4" t="s">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B115" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C114" s="5">
+      <c r="C115" s="5">
         <v>-10000</v>
       </c>
-      <c r="D114" s="4">
+      <c r="D115" s="4">
         <f t="shared" si="11"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="B115" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C115" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D115" s="4">
-        <f t="shared" ref="D115:D120" si="12">D114+C115</f>
-        <v>3590</v>
-      </c>
-    </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B116" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C116" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D116" s="4">
+        <f t="shared" ref="D116:D121" si="12">D115+C116</f>
+        <v>3590</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="B116" s="4" t="s">
+      <c r="B117" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C116" s="5">
+      <c r="C117" s="5">
         <v>7000</v>
       </c>
-      <c r="D116" s="4">
+      <c r="D117" s="4">
         <f t="shared" si="12"/>
         <v>10590</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B117" s="4" t="s">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B118" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C117" s="5">
+      <c r="C118" s="5">
         <v>-10000</v>
       </c>
-      <c r="D117" s="4">
+      <c r="D118" s="4">
         <f t="shared" si="12"/>
         <v>590</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B118" s="4" t="s">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B119" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C118" s="5">
+      <c r="C119" s="5">
         <v>12000</v>
       </c>
-      <c r="D118" s="4">
+      <c r="D119" s="4">
         <f t="shared" si="12"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B119" s="4" t="s">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B120" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C119" s="5">
+      <c r="C120" s="5">
         <v>-10000</v>
       </c>
-      <c r="D119" s="4">
+      <c r="D120" s="4">
         <f t="shared" si="12"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B120" s="4" t="s">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B121" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C120" s="5">
+      <c r="C121" s="5">
         <v>2000</v>
       </c>
-      <c r="D120" s="4">
+      <c r="D121" s="4">
         <f t="shared" si="12"/>
         <v>4590</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="B121" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C121" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D121" s="4">
-        <f t="shared" ref="D121:D126" si="13">D120+C121</f>
-        <v>6590</v>
-      </c>
-    </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="B122" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C122" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D122" s="4">
+        <f t="shared" ref="D122:D127" si="13">D121+C122</f>
+        <v>6590</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="B122" s="4" t="s">
+      <c r="B123" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C122" s="5">
+      <c r="C123" s="5">
         <v>7000</v>
       </c>
-      <c r="D122" s="4">
+      <c r="D123" s="4">
         <f t="shared" si="13"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B123" s="4" t="s">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B124" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C123" s="5">
+      <c r="C124" s="5">
         <v>-10000</v>
       </c>
-      <c r="D123" s="4">
+      <c r="D124" s="4">
         <f t="shared" si="13"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="16" t="s">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="B124" s="4" t="s">
+      <c r="B125" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C124" s="5">
+      <c r="C125" s="5">
         <v>2000</v>
       </c>
-      <c r="D124" s="4">
+      <c r="D125" s="4">
         <f t="shared" si="13"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="16" t="s">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="B125" s="4" t="s">
+      <c r="B126" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C125" s="5">
+      <c r="C126" s="5">
         <v>8000</v>
       </c>
-      <c r="D125" s="4">
+      <c r="D126" s="4">
         <f t="shared" si="13"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B126" s="4" t="s">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B127" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C126" s="5">
+      <c r="C127" s="5">
         <v>-10000</v>
       </c>
-      <c r="D126" s="4">
+      <c r="D127" s="4">
         <f t="shared" si="13"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="16" t="s">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="B127" s="4" t="s">
+      <c r="B128" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C127" s="5">
+      <c r="C128" s="5">
         <v>2000</v>
       </c>
-      <c r="D127" s="4">
-        <f t="shared" ref="D127:D132" si="14">D126+C127</f>
+      <c r="D128" s="4">
+        <f t="shared" ref="D128:D133" si="14">D127+C128</f>
         <v>5590</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B128" s="4" t="s">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B129" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C128" s="5">
+      <c r="C129" s="5">
         <v>5000</v>
       </c>
-      <c r="D128" s="4">
+      <c r="D129" s="4">
         <f t="shared" si="14"/>
         <v>10590</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B129" s="4" t="s">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B130" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C129" s="5">
+      <c r="C130" s="5">
         <v>-10000</v>
       </c>
-      <c r="D129" s="4">
+      <c r="D130" s="4">
         <f t="shared" si="14"/>
         <v>590</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B130" s="4" t="s">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B131" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C130" s="5">
+      <c r="C131" s="5">
         <v>2000</v>
       </c>
-      <c r="D130" s="4">
+      <c r="D131" s="4">
         <f t="shared" si="14"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B131" s="4" t="s">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B132" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C131" s="5">
+      <c r="C132" s="5">
         <v>9000</v>
       </c>
-      <c r="D131" s="4">
+      <c r="D132" s="4">
         <f t="shared" si="14"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B132" s="4" t="s">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B133" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C132" s="5">
+      <c r="C133" s="5">
         <v>-10000</v>
       </c>
-      <c r="D132" s="4">
+      <c r="D133" s="4">
         <f t="shared" si="14"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B133" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C133" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D133" s="4">
-        <f t="shared" ref="D133:D138" si="15">D132+C133</f>
-        <v>3590</v>
-      </c>
-    </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B134" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C134" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D134" s="4">
+        <f t="shared" ref="D134:D139" si="15">D133+C134</f>
+        <v>3590</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="B134" s="4" t="s">
+      <c r="B135" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C134" s="5">
+      <c r="C135" s="5">
         <v>8000</v>
       </c>
-      <c r="D134" s="4">
+      <c r="D135" s="4">
         <f t="shared" si="15"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B135" s="4" t="s">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B136" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C135" s="5">
+      <c r="C136" s="5">
         <v>-10000</v>
       </c>
-      <c r="D135" s="4">
+      <c r="D136" s="4">
         <f t="shared" si="15"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="16" t="s">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="B136" s="4" t="s">
+      <c r="B137" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C136" s="5">
+      <c r="C137" s="5">
         <v>2000</v>
       </c>
-      <c r="D136" s="4">
+      <c r="D137" s="4">
         <f t="shared" si="15"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="16" t="s">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="B137" s="4" t="s">
+      <c r="B138" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C137" s="5">
+      <c r="C138" s="5">
         <v>12000</v>
       </c>
-      <c r="D137" s="4">
+      <c r="D138" s="4">
         <f t="shared" si="15"/>
         <v>15590</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B138" s="4" t="s">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B139" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C138" s="5">
+      <c r="C139" s="5">
         <v>-10000</v>
       </c>
-      <c r="D138" s="4">
+      <c r="D139" s="4">
         <f t="shared" si="15"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="B139" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="C139" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D139" s="4">
-        <f t="shared" ref="D139:D144" si="16">D138+C139</f>
-        <v>7590</v>
-      </c>
-    </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="B140" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C140" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D140" s="4">
+        <f t="shared" ref="D140:D145" si="16">D139+C140</f>
+        <v>7590</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="B140" s="4" t="s">
+      <c r="B141" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="C140" s="5">
+      <c r="C141" s="5">
         <v>10000</v>
       </c>
-      <c r="D140" s="4">
+      <c r="D141" s="4">
         <f t="shared" si="16"/>
         <v>17590</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B141" s="4" t="s">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B142" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C141" s="5">
+      <c r="C142" s="5">
         <v>-10000</v>
       </c>
-      <c r="D141" s="4">
+      <c r="D142" s="4">
         <f t="shared" si="16"/>
         <v>7590</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B142" s="4" t="s">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B143" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="C142" s="5">
+      <c r="C143" s="5">
         <v>2000</v>
       </c>
-      <c r="D142" s="4">
+      <c r="D143" s="4">
         <f t="shared" si="16"/>
         <v>9590</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="16" t="s">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="B143" s="4" t="s">
+      <c r="B144" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="C143" s="5">
+      <c r="C144" s="5">
         <v>-1200</v>
       </c>
-      <c r="D143" s="4">
+      <c r="D144" s="4">
         <f t="shared" si="16"/>
         <v>8390</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B144" s="4" t="s">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B145" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="C144" s="5">
+      <c r="C145" s="5">
         <v>500</v>
       </c>
-      <c r="D144" s="4">
+      <c r="D145" s="4">
         <f t="shared" si="16"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="16" t="s">
-        <v>165</v>
-      </c>
-      <c r="B145" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="C145" s="5">
-        <v>750</v>
-      </c>
-      <c r="D145" s="4">
-        <f t="shared" ref="D145:D150" si="17">D144+C145</f>
-        <v>9640</v>
-      </c>
-    </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="B146" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C146" s="5">
+        <v>750</v>
+      </c>
+      <c r="D146" s="4">
+        <f t="shared" ref="D146:D151" si="17">D145+C146</f>
+        <v>9640</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="B146" s="4" t="s">
+      <c r="B147" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C146" s="5">
+      <c r="C147" s="5">
         <v>2000</v>
       </c>
-      <c r="D146" s="4">
+      <c r="D147" s="4">
         <f t="shared" si="17"/>
         <v>11640</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B147" s="4" t="s">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B148" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C147" s="5">
+      <c r="C148" s="5">
         <v>2000</v>
       </c>
-      <c r="D147" s="4">
+      <c r="D148" s="4">
         <f t="shared" si="17"/>
         <v>13640</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B148" s="4" t="s">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B149" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C148" s="5">
+      <c r="C149" s="5">
         <v>-10000</v>
       </c>
-      <c r="D148" s="4">
+      <c r="D149" s="4">
         <f t="shared" si="17"/>
         <v>3640</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B149" s="4" t="s">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B150" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="C149" s="5">
+      <c r="C150" s="5">
         <v>350</v>
       </c>
-      <c r="D149" s="4">
+      <c r="D150" s="4">
         <f t="shared" si="17"/>
         <v>3990</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="16" t="s">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="B150" s="4" t="s">
+      <c r="B151" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="C150" s="5">
+      <c r="C151" s="5">
         <v>300</v>
       </c>
-      <c r="D150" s="4">
+      <c r="D151" s="4">
         <f t="shared" si="17"/>
         <v>4290</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="16" t="s">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="B151" s="4" t="s">
+      <c r="B152" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="C151" s="5">
+      <c r="C152" s="5">
         <v>3800</v>
       </c>
-      <c r="D151" s="4">
-        <f t="shared" ref="D151:D157" si="18">D150+C151</f>
+      <c r="D152" s="4">
+        <f t="shared" ref="D152:D158" si="18">D151+C152</f>
         <v>8090</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B152" s="4" t="s">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B153" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C152" s="5">
+      <c r="C153" s="5">
         <v>500</v>
       </c>
-      <c r="D152" s="4">
+      <c r="D153" s="4">
         <f t="shared" si="18"/>
         <v>8590</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" s="16" t="s">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="B153" s="4" t="s">
+      <c r="B154" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="C153" s="5">
+      <c r="C154" s="5">
         <v>1300</v>
       </c>
-      <c r="D153" s="4">
+      <c r="D154" s="4">
         <f t="shared" si="18"/>
         <v>9890</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="16" t="s">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="B154" s="4" t="s">
+      <c r="B155" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C154" s="5">
+      <c r="C155" s="5">
         <v>9000</v>
       </c>
-      <c r="D154" s="4">
+      <c r="D155" s="4">
         <f t="shared" si="18"/>
         <v>18890</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B155" s="4" t="s">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B156" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C155" s="5">
+      <c r="C156" s="5">
         <v>-10000</v>
       </c>
-      <c r="D155" s="4">
+      <c r="D156" s="4">
         <f t="shared" si="18"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="16" t="s">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="B156" s="4" t="s">
+      <c r="B157" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C156" s="5">
+      <c r="C157" s="5">
         <v>2000</v>
       </c>
-      <c r="D156" s="4">
+      <c r="D157" s="4">
         <f t="shared" si="18"/>
         <v>10890</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B157" s="4" t="s">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B158" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C157" s="5">
+      <c r="C158" s="5">
         <v>-10000</v>
       </c>
-      <c r="D157" s="4">
+      <c r="D158" s="4">
         <f t="shared" si="18"/>
         <v>890</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="B158" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="C158" s="5">
-        <v>500</v>
-      </c>
-      <c r="D158" s="4">
-        <f t="shared" ref="D158:D163" si="19">D157+C158</f>
-        <v>1390</v>
-      </c>
-    </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="B159" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C159" s="5">
+        <v>500</v>
+      </c>
+      <c r="D159" s="4">
+        <f t="shared" ref="D159:D164" si="19">D158+C159</f>
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="B159" s="4" t="s">
+      <c r="B160" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="C159" s="5">
+      <c r="C160" s="5">
         <v>10000</v>
       </c>
-      <c r="D159" s="4">
+      <c r="D160" s="4">
         <f t="shared" si="19"/>
         <v>11390</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B160" s="4" t="s">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B161" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C160" s="5">
+      <c r="C161" s="5">
         <v>-10000</v>
       </c>
-      <c r="D160" s="4">
+      <c r="D161" s="4">
         <f t="shared" si="19"/>
         <v>1390</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" s="16" t="s">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="B161" s="4" t="s">
+      <c r="B162" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C161" s="5">
+      <c r="C162" s="5">
         <v>3000</v>
       </c>
-      <c r="D161" s="4">
+      <c r="D162" s="4">
         <f t="shared" si="19"/>
         <v>4390</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" s="16" t="s">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="B162" s="4" t="s">
+      <c r="B163" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C162" s="5">
+      <c r="C163" s="5">
         <v>2000</v>
       </c>
-      <c r="D162" s="4">
+      <c r="D163" s="4">
         <f t="shared" si="19"/>
         <v>6390</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B163" s="4" t="s">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B164" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C163" s="5">
+      <c r="C164" s="5">
         <v>2000</v>
       </c>
-      <c r="D163" s="4">
+      <c r="D164" s="4">
         <f t="shared" si="19"/>
         <v>8390</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164" s="16" t="s">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="B164" s="4" t="s">
+      <c r="B165" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C164" s="5">
+      <c r="C165" s="5">
         <v>11000</v>
       </c>
-      <c r="D164" s="4">
-        <f t="shared" ref="D164:D169" si="20">D163+C164</f>
+      <c r="D165" s="4">
+        <f t="shared" ref="D165:D170" si="20">D164+C165</f>
         <v>19390</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B165" s="4" t="s">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B166" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C165" s="5">
+      <c r="C166" s="5">
         <v>-10000</v>
       </c>
-      <c r="D165" s="4">
+      <c r="D166" s="4">
         <f t="shared" si="20"/>
         <v>9390</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A166" s="16" t="s">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" s="16" t="s">
         <v>187</v>
       </c>
-      <c r="B166" s="4" t="s">
+      <c r="B167" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C166" s="5">
+      <c r="C167" s="5">
         <v>3000</v>
       </c>
-      <c r="D166" s="4">
+      <c r="D167" s="4">
         <f t="shared" si="20"/>
         <v>12390</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B167" s="4" t="s">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B168" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C167" s="5">
+      <c r="C168" s="5">
         <v>-10000</v>
       </c>
-      <c r="D167" s="4">
+      <c r="D168" s="4">
         <f t="shared" si="20"/>
         <v>2390</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B168" s="4" t="s">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B169" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C168" s="5">
+      <c r="C169" s="5">
         <v>500</v>
       </c>
-      <c r="D168" s="4">
+      <c r="D169" s="4">
         <f t="shared" si="20"/>
         <v>2890</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A169" s="16" t="s">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" s="16" t="s">
         <v>189</v>
       </c>
-      <c r="B169" s="4" t="s">
+      <c r="B170" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C169" s="5">
+      <c r="C170" s="5">
         <v>5600</v>
       </c>
-      <c r="D169" s="4">
+      <c r="D170" s="4">
         <f t="shared" si="20"/>
         <v>8490</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B170" s="4" t="s">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B171" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="C170" s="5">
+      <c r="C171" s="5">
         <v>4700</v>
       </c>
-      <c r="D170" s="4">
-        <f t="shared" ref="D170:D176" si="21">D169+C170</f>
+      <c r="D171" s="4">
+        <f t="shared" ref="D171:D177" si="21">D170+C171</f>
         <v>13190</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" s="16" t="s">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" s="16" t="s">
         <v>192</v>
       </c>
-      <c r="B171" s="4" t="s">
+      <c r="B172" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C171" s="5">
+      <c r="C172" s="5">
         <v>1500</v>
       </c>
-      <c r="D171" s="4">
+      <c r="D172" s="4">
         <f t="shared" si="21"/>
         <v>14690</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B172" s="4" t="s">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B173" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C172" s="5">
+      <c r="C173" s="5">
         <v>500</v>
       </c>
-      <c r="D172" s="4">
+      <c r="D173" s="4">
         <f t="shared" si="21"/>
         <v>15190</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173" s="16" t="s">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="B173" s="4" t="s">
+      <c r="B174" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="C173" s="5">
+      <c r="C174" s="5">
         <v>1000</v>
       </c>
-      <c r="D173" s="4">
+      <c r="D174" s="4">
         <f t="shared" si="21"/>
         <v>16190</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174" s="16" t="s">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="B174" s="4" t="s">
+      <c r="B175" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="C174" s="5">
+      <c r="C175" s="5">
         <v>1000</v>
       </c>
-      <c r="D174" s="4">
+      <c r="D175" s="4">
         <f t="shared" si="21"/>
         <v>17190</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A175" s="16" t="s">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="B175" s="4" t="s">
+      <c r="B176" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C175" s="5">
+      <c r="C176" s="5">
         <v>3000</v>
       </c>
-      <c r="D175" s="4">
+      <c r="D176" s="4">
         <f t="shared" si="21"/>
         <v>20190</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B176" s="4" t="s">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B177" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C176" s="5">
+      <c r="C177" s="5">
         <v>-20000</v>
       </c>
-      <c r="D176" s="4">
+      <c r="D177" s="4">
         <f t="shared" si="21"/>
         <v>190</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B177" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C177" s="5">
-        <v>500</v>
-      </c>
-      <c r="D177" s="4">
-        <f t="shared" ref="D177:D183" si="22">D176+C177</f>
-        <v>690</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
@@ -3618,314 +3617,353 @@
         <v>500</v>
       </c>
       <c r="D178" s="4">
+        <f t="shared" ref="D178:D184" si="22">D177+C178</f>
+        <v>690</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B179" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C179" s="5">
+        <v>500</v>
+      </c>
+      <c r="D179" s="4">
         <f t="shared" si="22"/>
         <v>1190</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A179" s="16" t="s">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="B179" s="4" t="s">
+      <c r="B180" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="C179" s="5">
+      <c r="C180" s="5">
         <v>10000</v>
       </c>
-      <c r="D179" s="4">
+      <c r="D180" s="4">
         <f t="shared" si="22"/>
         <v>11190</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B180" s="4" t="s">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B181" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C180" s="5">
+      <c r="C181" s="5">
         <v>-10000</v>
       </c>
-      <c r="D180" s="4">
+      <c r="D181" s="4">
         <f t="shared" si="22"/>
         <v>1190</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="16" t="s">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="B181" s="4" t="s">
+      <c r="B182" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C181" s="5">
+      <c r="C182" s="5">
         <v>3000</v>
       </c>
-      <c r="D181" s="4">
+      <c r="D182" s="4">
         <f t="shared" si="22"/>
         <v>4190</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" s="16" t="s">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A183" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="B182" s="4" t="s">
+      <c r="B183" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C182" s="5">
+      <c r="C183" s="5">
         <v>11000</v>
       </c>
-      <c r="D182" s="4">
+      <c r="D183" s="4">
         <f t="shared" si="22"/>
         <v>15190</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B183" s="4" t="s">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B184" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C183" s="5">
+      <c r="C184" s="5">
         <v>-10000</v>
       </c>
-      <c r="D183" s="4">
+      <c r="D184" s="4">
         <f t="shared" si="22"/>
         <v>5190</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="B184" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C184" s="5">
-        <v>3000</v>
-      </c>
-      <c r="D184" s="4">
-        <f t="shared" ref="D184:D190" si="23">D183+C184</f>
-        <v>8190</v>
-      </c>
-    </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="B185" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C185" s="5">
+        <v>3000</v>
+      </c>
+      <c r="D185" s="4">
+        <f t="shared" ref="D185:D191" si="23">D184+C185</f>
+        <v>8190</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="B185" s="4" t="s">
+      <c r="B186" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="C185" s="5">
+      <c r="C186" s="5">
         <v>14000</v>
       </c>
-      <c r="D185" s="4">
+      <c r="D186" s="4">
         <f t="shared" si="23"/>
         <v>22190</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B186" s="4" t="s">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B187" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="C186" s="5">
+      <c r="C187" s="5">
         <v>-20000</v>
       </c>
-      <c r="D186" s="4">
+      <c r="D187" s="4">
         <f t="shared" si="23"/>
         <v>2190</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A187" s="16" t="s">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A188" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="B187" s="4" t="s">
+      <c r="B188" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="C187" s="5">
+      <c r="C188" s="5">
         <v>5000</v>
       </c>
-      <c r="D187" s="4">
+      <c r="D188" s="4">
         <f t="shared" si="23"/>
         <v>7190</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A188" s="16" t="s">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189" s="16" t="s">
         <v>213</v>
       </c>
-      <c r="B188" s="4" t="s">
+      <c r="B189" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="C188" s="5">
+      <c r="C189" s="5">
         <v>5000</v>
       </c>
-      <c r="D188" s="4">
+      <c r="D189" s="4">
         <f t="shared" si="23"/>
         <v>12190</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" s="16" t="s">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A190" s="16" t="s">
         <v>215</v>
       </c>
-      <c r="B189" s="4" t="s">
+      <c r="B190" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C189" s="5">
+      <c r="C190" s="5">
         <v>11000</v>
       </c>
-      <c r="D189" s="4">
+      <c r="D190" s="4">
         <f t="shared" si="23"/>
         <v>23190</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B190" s="4" t="s">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B191" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C190" s="5">
+      <c r="C191" s="5">
         <v>-20000</v>
       </c>
-      <c r="D190" s="4">
+      <c r="D191" s="4">
         <f t="shared" si="23"/>
         <v>3190</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A191" s="16" t="s">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A192" s="16" t="s">
         <v>216</v>
       </c>
-      <c r="B191" s="4" t="s">
+      <c r="B192" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C191" s="5">
+      <c r="C192" s="5">
         <v>500</v>
       </c>
-      <c r="D191" s="4">
-        <f t="shared" ref="D191:D196" si="24">D190+C191</f>
+      <c r="D192" s="4">
+        <f t="shared" ref="D192:D197" si="24">D191+C192</f>
         <v>3690</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B192" s="4" t="s">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B193" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C192" s="5">
+      <c r="C193" s="5">
         <v>3000</v>
       </c>
-      <c r="D192" s="4">
+      <c r="D193" s="4">
         <f t="shared" si="24"/>
         <v>6690</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A193" s="16" t="s">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A194" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="B193" s="4" t="s">
+      <c r="B194" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="C193" s="5">
+      <c r="C194" s="5">
         <v>12000</v>
       </c>
-      <c r="D193" s="4">
+      <c r="D194" s="4">
         <f t="shared" si="24"/>
         <v>18690</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B194" s="4" t="s">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B195" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C194" s="5">
+      <c r="C195" s="5">
         <v>-10000</v>
       </c>
-      <c r="D194" s="4">
+      <c r="D195" s="4">
         <f t="shared" si="24"/>
         <v>8690</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A195" s="16" t="s">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A196" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="B195" s="4" t="s">
+      <c r="B196" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="C195" s="5">
+      <c r="C196" s="5">
         <v>5000</v>
       </c>
-      <c r="D195" s="4">
+      <c r="D196" s="4">
         <f t="shared" si="24"/>
         <v>13690</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B196" s="4" t="s">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B197" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C196" s="5">
+      <c r="C197" s="5">
         <v>-10000</v>
       </c>
-      <c r="D196" s="4">
+      <c r="D197" s="4">
         <f t="shared" si="24"/>
         <v>3690</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A197" s="16" t="s">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A198" s="16" t="s">
         <v>221</v>
       </c>
-      <c r="B197" s="4" t="s">
+      <c r="B198" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="C197" s="5">
+      <c r="C198" s="5">
         <v>12000</v>
-      </c>
-      <c r="D197" s="4">
-        <f>D196+C197</f>
-        <v>15690</v>
-      </c>
-    </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B198" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C198" s="5">
-        <v>-10000</v>
       </c>
       <c r="D198" s="4">
         <f>D197+C198</f>
-        <v>5690</v>
+        <v>15690</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A199" s="16" t="s">
-        <v>226</v>
-      </c>
       <c r="B199" s="4" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C199" s="5">
-        <v>2000</v>
+        <v>-10000</v>
       </c>
       <c r="D199" s="4">
         <f>D198+C199</f>
-        <v>7690</v>
+        <v>5690</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" s="16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B200" s="4" t="s">
-        <v>228</v>
+        <v>40</v>
       </c>
       <c r="C200" s="5">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="D200" s="4">
         <f>D199+C200</f>
+        <v>7690</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A201" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="B201" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="C201" s="5">
+        <v>1000</v>
+      </c>
+      <c r="D201" s="4">
+        <f>D200+C201</f>
         <v>8690</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A202" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="B202" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="C202" s="5">
+        <v>5000</v>
+      </c>
+      <c r="D202" s="4">
+        <f>D201+C202</f>
+        <v>13690</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B203" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="C203" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D203" s="4">
+        <f>D202+C203</f>
+        <v>3690</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lay tien loi co diem ngay 23
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="CÔ DIỄM" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="234">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -718,6 +718,9 @@
   </si>
   <si>
     <t>Duy lấy tiền lời 13tr</t>
+  </si>
+  <si>
+    <t>23/10/2024</t>
   </si>
 </sst>
 </file>
@@ -1218,11 +1221,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K206"/>
+  <dimension ref="A1:K207"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L31" sqref="L31"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A169" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D208" sqref="D208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4009,6 +4012,21 @@
       <c r="D206" s="4">
         <f>D205+C206</f>
         <v>6690</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A207" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="B207" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C207" s="5">
+        <v>3000</v>
+      </c>
+      <c r="D207" s="4">
+        <f>D206+C207</f>
+        <v>9690</v>
       </c>
     </row>
   </sheetData>
@@ -4540,7 +4558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
duy tinh tien loi co diem
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="CÔ DIỄM" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="235">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -721,6 +721,9 @@
   </si>
   <si>
     <t>23/10/2024</t>
+  </si>
+  <si>
+    <t>30/10/2024</t>
   </si>
 </sst>
 </file>
@@ -1221,11 +1224,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K207"/>
+  <dimension ref="A1:K210"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A169" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D208" sqref="D208"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1301,8 +1304,8 @@
         <v>20</v>
       </c>
       <c r="J3" s="4">
-        <f>SUM(I3:I69)</f>
-        <v>580</v>
+        <f>SUM(I3:I70)</f>
+        <v>600</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1653,30 +1656,30 @@
       <c r="K35" s="14"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="16" t="s">
+      <c r="H36" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="I36" s="5">
+        <v>20</v>
+      </c>
+      <c r="K36" s="14"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B37" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="5">
+      <c r="C37" s="5">
         <v>3000</v>
       </c>
-      <c r="D36" s="4">
-        <f>D25+C36</f>
+      <c r="D37" s="4">
+        <f>D25+C37</f>
         <v>8490</v>
       </c>
-      <c r="H36" s="16" t="s">
+      <c r="H37" s="16" t="s">
         <v>12</v>
-      </c>
-      <c r="I36" s="5">
-        <v>10</v>
-      </c>
-      <c r="K36" s="14"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H37" s="16" t="s">
-        <v>43</v>
       </c>
       <c r="I37" s="5">
         <v>10</v>
@@ -1685,7 +1688,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H38" s="16" t="s">
-        <v>139</v>
+        <v>43</v>
       </c>
       <c r="I38" s="5">
         <v>10</v>
@@ -1694,7 +1697,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H39" s="16" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="I39" s="5">
         <v>10</v>
@@ -1703,7 +1706,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H40" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I40" s="5">
         <v>10</v>
@@ -1712,64 +1715,54 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H41" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="I41" s="5">
+        <v>10</v>
+      </c>
+      <c r="K41" s="14"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H42" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="I41" s="5">
-        <v>10</v>
-      </c>
-      <c r="K41" s="14"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B42" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C42" s="5">
-        <v>4400</v>
-      </c>
-      <c r="D42" s="4">
-        <f>D36+C42</f>
-        <v>12890</v>
-      </c>
-      <c r="H42" s="16" t="s">
-        <v>157</v>
-      </c>
       <c r="I42" s="5">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K42" s="14"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C43" s="5">
-        <v>-10000</v>
+        <v>4400</v>
       </c>
       <c r="D43" s="4">
-        <f>D42+C43</f>
-        <v>2890</v>
+        <f>D37+C43</f>
+        <v>12890</v>
       </c>
       <c r="H43" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I43" s="5">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="K43" s="14"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C44" s="5">
-        <v>1600</v>
+        <v>-10000</v>
       </c>
       <c r="D44" s="4">
-        <f t="shared" ref="D44:D51" si="1">D43+C44</f>
-        <v>4490</v>
+        <f>D43+C44</f>
+        <v>2890</v>
       </c>
       <c r="H44" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I44" s="5">
         <v>10</v>
@@ -1778,171 +1771,181 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C45" s="5">
+        <v>1600</v>
+      </c>
+      <c r="D45" s="4">
+        <f t="shared" ref="D45:D52" si="1">D44+C45</f>
+        <v>4490</v>
+      </c>
+      <c r="H45" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="I45" s="5">
+        <v>10</v>
+      </c>
+      <c r="K45" s="14"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B46" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C45" s="5">
+      <c r="C46" s="5">
         <v>3000</v>
       </c>
-      <c r="D45" s="4">
+      <c r="D46" s="4">
         <f t="shared" si="1"/>
         <v>7490</v>
       </c>
-      <c r="H45" s="16" t="s">
+      <c r="H46" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="I45" s="5">
-        <v>10</v>
-      </c>
-      <c r="K45" s="14"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="16" t="s">
+      <c r="I46" s="5">
+        <v>10</v>
+      </c>
+      <c r="K46" s="14"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B47" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C46" s="5">
+      <c r="C47" s="5">
         <v>2000</v>
       </c>
-      <c r="D46" s="4">
+      <c r="D47" s="4">
         <f t="shared" si="1"/>
         <v>9490</v>
       </c>
-      <c r="H46" s="16" t="s">
+      <c r="H47" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="I46" s="5">
-        <v>10</v>
-      </c>
-      <c r="K46" s="14"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="16" t="s">
+      <c r="I47" s="5">
+        <v>10</v>
+      </c>
+      <c r="K47" s="14"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B48" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C48" s="5">
         <v>3000</v>
       </c>
-      <c r="D47" s="4">
+      <c r="D48" s="4">
         <f t="shared" si="1"/>
         <v>12490</v>
       </c>
-      <c r="H47" s="16" t="s">
+      <c r="H48" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="I47" s="5">
-        <v>10</v>
-      </c>
-      <c r="K47" s="14"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B48" s="4" t="s">
+      <c r="I48" s="5">
+        <v>10</v>
+      </c>
+      <c r="K48" s="14"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B49" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C48" s="5">
+      <c r="C49" s="5">
         <v>-10000</v>
       </c>
-      <c r="D48" s="4">
+      <c r="D49" s="4">
         <f t="shared" si="1"/>
         <v>2490</v>
       </c>
-      <c r="H48" s="16" t="s">
+      <c r="H49" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="I48" s="5">
-        <v>10</v>
-      </c>
-      <c r="K48" s="14"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="16" t="s">
+      <c r="I49" s="5">
+        <v>10</v>
+      </c>
+      <c r="K49" s="14"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B50" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C49" s="5">
+      <c r="C50" s="5">
         <v>4960</v>
       </c>
-      <c r="D49" s="4">
+      <c r="D50" s="4">
         <f t="shared" si="1"/>
         <v>7450</v>
       </c>
-      <c r="H49" s="16" t="s">
+      <c r="H50" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="I49" s="5">
-        <v>10</v>
-      </c>
-      <c r="K49" s="14"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="16" t="s">
+      <c r="I50" s="5">
+        <v>10</v>
+      </c>
+      <c r="K50" s="14"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B51" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C50" s="5">
+      <c r="C51" s="5">
         <v>4000</v>
       </c>
-      <c r="D50" s="4">
+      <c r="D51" s="4">
         <f t="shared" si="1"/>
         <v>11450</v>
       </c>
-      <c r="H50" s="16" t="s">
+      <c r="H51" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="I50" s="5">
-        <v>10</v>
-      </c>
-      <c r="K50" s="14"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B51" s="4" t="s">
+      <c r="I51" s="5">
+        <v>10</v>
+      </c>
+      <c r="K51" s="14"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B52" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C51" s="5">
+      <c r="C52" s="5">
         <v>-10000</v>
       </c>
-      <c r="D51" s="4">
+      <c r="D52" s="4">
         <f t="shared" si="1"/>
         <v>1450</v>
       </c>
-      <c r="H51" s="16" t="s">
+      <c r="H52" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="I51" s="5">
-        <v>10</v>
-      </c>
-      <c r="K51" s="14"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B52" s="4" t="s">
+      <c r="I52" s="5">
+        <v>10</v>
+      </c>
+      <c r="K52" s="14"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B53" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C52" s="5">
+      <c r="C53" s="5">
         <v>7640</v>
       </c>
-      <c r="D52" s="4">
-        <f t="shared" ref="D52:D59" si="2">D51+C52</f>
+      <c r="D53" s="4">
+        <f t="shared" ref="D53:D60" si="2">D52+C53</f>
         <v>9090</v>
       </c>
-      <c r="H52" s="16" t="s">
+      <c r="H53" s="16" t="s">
         <v>185</v>
-      </c>
-      <c r="I52" s="5">
-        <v>10</v>
-      </c>
-      <c r="K52" s="14"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H53" s="16" t="s">
-        <v>221</v>
       </c>
       <c r="I53" s="5">
         <v>10</v>
@@ -1951,366 +1954,360 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H54" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="I54" s="5">
+        <v>10</v>
+      </c>
+      <c r="K54" s="14"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H55" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="I54" s="5">
+      <c r="I55" s="5">
         <v>20</v>
       </c>
-      <c r="K54" s="14"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B55" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C55" s="5">
-        <v>3000</v>
-      </c>
-      <c r="D55" s="4">
-        <f>D52+C55</f>
-        <v>12090</v>
-      </c>
-      <c r="H55" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="I55" s="5">
-        <v>10</v>
-      </c>
+      <c r="K55" s="14"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B56" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C56" s="5">
+        <v>3000</v>
+      </c>
+      <c r="D56" s="4">
+        <f>D53+C56</f>
+        <v>12090</v>
+      </c>
+      <c r="H56" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="I56" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B57" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C56" s="5">
+      <c r="C57" s="5">
         <v>-10000</v>
       </c>
-      <c r="D56" s="4">
+      <c r="D57" s="4">
         <f t="shared" si="2"/>
         <v>2090</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B57" s="4" t="s">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B58" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C57" s="5">
+      <c r="C58" s="5">
         <v>800</v>
       </c>
-      <c r="D57" s="4">
+      <c r="D58" s="4">
         <f t="shared" si="2"/>
         <v>2890</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="16" t="s">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B59" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C58" s="5">
+      <c r="C59" s="5">
         <v>2000</v>
       </c>
-      <c r="D58" s="4">
+      <c r="D59" s="4">
         <f t="shared" si="2"/>
         <v>4890</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="16" t="s">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B60" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C59" s="5">
+      <c r="C60" s="5">
         <v>4000</v>
       </c>
-      <c r="D59" s="4">
+      <c r="D60" s="4">
         <f t="shared" si="2"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" s="16" t="s">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B61" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C60" s="5">
+      <c r="C61" s="5">
         <v>4000</v>
       </c>
-      <c r="D60" s="4">
-        <f t="shared" ref="D60:D65" si="3">D59+C60</f>
+      <c r="D61" s="4">
+        <f t="shared" ref="D61:D66" si="3">D60+C61</f>
         <v>12890</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B61" s="4" t="s">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B62" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C61" s="5">
+      <c r="C62" s="5">
         <v>5000</v>
       </c>
-      <c r="D61" s="4">
+      <c r="D62" s="4">
         <f t="shared" si="3"/>
         <v>17890</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B62" s="4" t="s">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B63" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C62" s="5">
+      <c r="C63" s="5">
         <v>-10000</v>
       </c>
-      <c r="D62" s="4">
+      <c r="D63" s="4">
         <f t="shared" si="3"/>
         <v>7890</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" s="16">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" s="16">
         <v>44969</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B64" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C63" s="5">
+      <c r="C64" s="5">
         <v>900</v>
       </c>
-      <c r="D63" s="4">
+      <c r="D64" s="4">
         <f t="shared" si="3"/>
         <v>8790</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B64" s="4" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B65" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C64" s="5">
+      <c r="C65" s="5">
         <v>4000</v>
       </c>
-      <c r="D64" s="4">
+      <c r="D65" s="4">
         <f t="shared" si="3"/>
         <v>12790</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B65" s="4" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C65" s="5">
+      <c r="C66" s="5">
         <v>-10000</v>
       </c>
-      <c r="D65" s="4">
+      <c r="D66" s="4">
         <f t="shared" si="3"/>
         <v>2790</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C66" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D66" s="4">
-        <f t="shared" ref="D66:D73" si="4">D65+C66</f>
-        <v>4790</v>
-      </c>
-    </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C67" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D67" s="4">
+        <f t="shared" ref="D67:D74" si="4">D66+C67</f>
+        <v>4790</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B68" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C67" s="5">
+      <c r="C68" s="5">
         <v>700</v>
       </c>
-      <c r="D67" s="4">
+      <c r="D68" s="4">
         <f t="shared" si="4"/>
         <v>5490</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B68" s="4" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B69" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C68" s="5">
+      <c r="C69" s="5">
         <v>4000</v>
       </c>
-      <c r="D68" s="4">
+      <c r="D69" s="4">
         <f t="shared" si="4"/>
         <v>9490</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="16" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B70" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C69" s="5">
+      <c r="C70" s="5">
         <v>600</v>
       </c>
-      <c r="D69" s="4">
+      <c r="D70" s="4">
         <f t="shared" si="4"/>
         <v>10090</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B70" s="4" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B71" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C70" s="5">
+      <c r="C71" s="5">
         <v>-10000</v>
       </c>
-      <c r="D70" s="4">
+      <c r="D71" s="4">
         <f t="shared" si="4"/>
         <v>90</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="16" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B72" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C71" s="5">
+      <c r="C72" s="5">
         <f>700+5000+300+600+400+1000+800</f>
         <v>8800</v>
       </c>
-      <c r="D71" s="4">
+      <c r="D72" s="4">
         <f t="shared" si="4"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B72" s="4" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B73" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C72" s="5">
+      <c r="C73" s="5">
         <v>6000</v>
       </c>
-      <c r="D72" s="4">
+      <c r="D73" s="4">
         <f t="shared" si="4"/>
         <v>14890</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B73" s="4" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C73" s="5">
+      <c r="C74" s="5">
         <v>-10000</v>
       </c>
-      <c r="D73" s="4">
+      <c r="D74" s="4">
         <f t="shared" si="4"/>
         <v>4890</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="16" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B75" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C74" s="5">
+      <c r="C75" s="5">
         <v>500</v>
       </c>
-      <c r="D74" s="4">
-        <f t="shared" ref="D74:D79" si="5">D73+C74</f>
+      <c r="D75" s="4">
+        <f t="shared" ref="D75:D80" si="5">D74+C75</f>
         <v>5390</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B75" s="4" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B76" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C75" s="5">
+      <c r="C76" s="5">
         <v>700</v>
       </c>
-      <c r="D75" s="4">
+      <c r="D76" s="4">
         <f t="shared" si="5"/>
         <v>6090</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B76" s="4" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B77" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C76" s="5">
+      <c r="C77" s="5">
         <v>1500</v>
       </c>
-      <c r="D76" s="4">
+      <c r="D77" s="4">
         <f t="shared" si="5"/>
         <v>7590</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B77" s="4" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B78" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C77" s="5">
+      <c r="C78" s="5">
         <v>5000</v>
       </c>
-      <c r="D77" s="4">
+      <c r="D78" s="4">
         <f t="shared" si="5"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B78" s="4" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B79" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C78" s="5">
+      <c r="C79" s="5">
         <v>-10000</v>
       </c>
-      <c r="D78" s="4">
+      <c r="D79" s="4">
         <f t="shared" si="5"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="16" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="B79" s="4" t="s">
+      <c r="B80" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C79" s="5">
+      <c r="C80" s="5">
         <v>2000</v>
       </c>
-      <c r="D79" s="4">
+      <c r="D80" s="4">
         <f t="shared" si="5"/>
         <v>4590</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B80" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C80" s="5">
-        <v>700</v>
-      </c>
-      <c r="D80" s="4">
-        <f t="shared" ref="D80:D85" si="6">D79+C80</f>
-        <v>5290</v>
-      </c>
-    </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="16" t="s">
-        <v>82</v>
-      </c>
       <c r="B81" s="4" t="s">
         <v>77</v>
       </c>
@@ -2318,401 +2315,404 @@
         <v>700</v>
       </c>
       <c r="D81" s="4">
+        <f t="shared" ref="D81:D86" si="6">D80+C81</f>
+        <v>5290</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C82" s="5">
+        <v>700</v>
+      </c>
+      <c r="D82" s="4">
         <f t="shared" si="6"/>
         <v>5990</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="16" t="s">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="B82" s="4" t="s">
+      <c r="B83" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C82" s="5">
+      <c r="C83" s="5">
         <v>700</v>
       </c>
-      <c r="D82" s="4">
+      <c r="D83" s="4">
         <f t="shared" si="6"/>
         <v>6690</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="16" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="B84" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C83" s="5">
+      <c r="C84" s="5">
         <v>4000</v>
       </c>
-      <c r="D83" s="4">
+      <c r="D84" s="4">
         <f t="shared" si="6"/>
         <v>10690</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B84" s="4" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B85" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C84" s="5">
+      <c r="C85" s="5">
         <v>-10000</v>
       </c>
-      <c r="D84" s="4">
+      <c r="D85" s="4">
         <f t="shared" si="6"/>
         <v>690</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="16" t="s">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="B85" s="4" t="s">
+      <c r="B86" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C85" s="5">
+      <c r="C86" s="5">
         <v>1000</v>
       </c>
-      <c r="D85" s="4">
+      <c r="D86" s="4">
         <f t="shared" si="6"/>
         <v>1690</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="16" t="s">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="B87" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C86" s="5">
+      <c r="C87" s="5">
         <v>7000</v>
       </c>
-      <c r="D86" s="4">
-        <f t="shared" ref="D86:D91" si="7">D85+C86</f>
+      <c r="D87" s="4">
+        <f t="shared" ref="D87:D92" si="7">D86+C87</f>
         <v>8690</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B87" s="4" t="s">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B88" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C87" s="5">
+      <c r="C88" s="5">
         <v>10000</v>
       </c>
-      <c r="D87" s="4">
+      <c r="D88" s="4">
         <f t="shared" si="7"/>
         <v>18690</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B88" s="4" t="s">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B89" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C88" s="5">
+      <c r="C89" s="5">
         <v>-10000</v>
       </c>
-      <c r="D88" s="4">
+      <c r="D89" s="4">
         <f t="shared" si="7"/>
         <v>8690</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B89" s="4" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B90" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C89" s="5">
+      <c r="C90" s="5">
         <v>1700</v>
       </c>
-      <c r="D89" s="4">
+      <c r="D90" s="4">
         <f t="shared" si="7"/>
         <v>10390</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B90" s="4" t="s">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B91" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C90" s="5">
+      <c r="C91" s="5">
         <v>-10000</v>
       </c>
-      <c r="D90" s="4">
+      <c r="D91" s="4">
         <f t="shared" si="7"/>
         <v>390</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B91" s="4" t="s">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B92" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C91" s="5">
+      <c r="C92" s="5">
         <v>6000</v>
       </c>
-      <c r="D91" s="4">
+      <c r="D92" s="4">
         <f t="shared" si="7"/>
         <v>6390</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="B92" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C92" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D92" s="4">
-        <f t="shared" ref="D92:D97" si="8">D91+C92</f>
-        <v>8390</v>
-      </c>
-    </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C93" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D93" s="4">
+        <f t="shared" ref="D93:D98" si="8">D92+C93</f>
+        <v>8390</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="B93" s="4" t="s">
+      <c r="B94" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C93" s="5">
+      <c r="C94" s="5">
         <v>5000</v>
       </c>
-      <c r="D93" s="4">
+      <c r="D94" s="4">
         <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B94" s="4" t="s">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B95" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C94" s="5">
+      <c r="C95" s="5">
         <v>-10000</v>
       </c>
-      <c r="D94" s="4">
+      <c r="D95" s="4">
         <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="16" t="s">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="B95" s="4" t="s">
+      <c r="B96" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C95" s="5">
+      <c r="C96" s="5">
         <v>1000</v>
       </c>
-      <c r="D95" s="4">
+      <c r="D96" s="4">
         <f t="shared" si="8"/>
         <v>4390</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B96" s="4" t="s">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B97" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C96" s="5">
+      <c r="C97" s="5">
         <v>9000</v>
       </c>
-      <c r="D96" s="4">
+      <c r="D97" s="4">
         <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B97" s="4" t="s">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B98" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C97" s="5">
+      <c r="C98" s="5">
         <v>-10000</v>
       </c>
-      <c r="D97" s="4">
+      <c r="D98" s="4">
         <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B98" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C98" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D98" s="4">
-        <f t="shared" ref="D98:D103" si="9">D97+C98</f>
-        <v>5390</v>
-      </c>
-    </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B99" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C99" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D99" s="4">
+        <f t="shared" ref="D99:D104" si="9">D98+C99</f>
+        <v>5390</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B100" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C99" s="5">
+      <c r="C100" s="5">
         <v>6000</v>
       </c>
-      <c r="D99" s="4">
+      <c r="D100" s="4">
         <f t="shared" si="9"/>
         <v>11390</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B100" s="4" t="s">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B101" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C100" s="5">
+      <c r="C101" s="5">
         <v>-10000</v>
       </c>
-      <c r="D100" s="4">
+      <c r="D101" s="4">
         <f t="shared" si="9"/>
         <v>1390</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B101" s="4" t="s">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B102" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C101" s="5">
+      <c r="C102" s="5">
         <v>400</v>
       </c>
-      <c r="D101" s="4">
+      <c r="D102" s="4">
         <f t="shared" si="9"/>
         <v>1790</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="16" t="s">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="B102" s="4" t="s">
+      <c r="B103" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C102" s="5">
+      <c r="C103" s="5">
         <v>2000</v>
       </c>
-      <c r="D102" s="4">
+      <c r="D103" s="4">
         <f t="shared" si="9"/>
         <v>3790</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="16" t="s">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="B103" s="4" t="s">
+      <c r="B104" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C103" s="5">
+      <c r="C104" s="5">
         <v>6000</v>
       </c>
-      <c r="D103" s="4">
+      <c r="D104" s="4">
         <f t="shared" si="9"/>
         <v>9790</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="16" t="s">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="B104" s="4" t="s">
+      <c r="B105" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C104" s="5">
+      <c r="C105" s="5">
         <v>1000</v>
       </c>
-      <c r="D104" s="4">
-        <f t="shared" ref="D104:D109" si="10">D103+C104</f>
+      <c r="D105" s="4">
+        <f t="shared" ref="D105:D110" si="10">D104+C105</f>
         <v>10790</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B105" s="4" t="s">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B106" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C105" s="5">
+      <c r="C106" s="5">
         <v>-10000</v>
       </c>
-      <c r="D105" s="4">
+      <c r="D106" s="4">
         <f t="shared" si="10"/>
         <v>790</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="16" t="s">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="B106" s="4" t="s">
+      <c r="B107" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C106" s="5">
+      <c r="C107" s="5">
         <v>800</v>
       </c>
-      <c r="D106" s="4">
+      <c r="D107" s="4">
         <f t="shared" si="10"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="16" t="s">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="B107" s="4" t="s">
+      <c r="B108" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C107" s="5">
+      <c r="C108" s="5">
         <v>5000</v>
       </c>
-      <c r="D107" s="4">
+      <c r="D108" s="4">
         <f t="shared" si="10"/>
         <v>6590</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="16" t="s">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="B108" s="4" t="s">
+      <c r="B109" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C108" s="5">
+      <c r="C109" s="5">
         <v>6000</v>
       </c>
-      <c r="D108" s="4">
+      <c r="D109" s="4">
         <f t="shared" si="10"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B109" s="4" t="s">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B110" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C109" s="5">
+      <c r="C110" s="5">
         <v>-10000</v>
       </c>
-      <c r="D109" s="4">
+      <c r="D110" s="4">
         <f t="shared" si="10"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="16" t="s">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="B110" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C110" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D110" s="4">
-        <f t="shared" ref="D110:D116" si="11">D109+C110</f>
-        <v>4590</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B111" s="4" t="s">
         <v>65</v>
       </c>
@@ -2720,926 +2720,926 @@
         <v>2000</v>
       </c>
       <c r="D111" s="4">
+        <f t="shared" ref="D111:D117" si="11">D110+C111</f>
+        <v>4590</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B112" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C112" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D112" s="4">
         <f t="shared" si="11"/>
         <v>6590</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B112" s="4" t="s">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B113" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C112" s="5">
+      <c r="C113" s="5">
         <v>7000</v>
       </c>
-      <c r="D112" s="4">
+      <c r="D113" s="4">
         <f t="shared" si="11"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B113" s="4" t="s">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B114" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C113" s="5">
+      <c r="C114" s="5">
         <v>-10000</v>
       </c>
-      <c r="D113" s="4">
+      <c r="D114" s="4">
         <f t="shared" si="11"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="16" t="s">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="B114" s="4" t="s">
+      <c r="B115" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C114" s="5">
+      <c r="C115" s="5">
         <v>2000</v>
       </c>
-      <c r="D114" s="4">
+      <c r="D115" s="4">
         <f t="shared" si="11"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="16" t="s">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="B115" s="4" t="s">
+      <c r="B116" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C115" s="5">
+      <c r="C116" s="5">
         <v>6000</v>
       </c>
-      <c r="D115" s="4">
+      <c r="D116" s="4">
         <f t="shared" si="11"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B116" s="4" t="s">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B117" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C116" s="5">
+      <c r="C117" s="5">
         <v>-10000</v>
       </c>
-      <c r="D116" s="4">
+      <c r="D117" s="4">
         <f t="shared" si="11"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="B117" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C117" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D117" s="4">
-        <f t="shared" ref="D117:D122" si="12">D116+C117</f>
-        <v>3590</v>
-      </c>
-    </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B118" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C118" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D118" s="4">
+        <f t="shared" ref="D118:D123" si="12">D117+C118</f>
+        <v>3590</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="B118" s="4" t="s">
+      <c r="B119" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C118" s="5">
+      <c r="C119" s="5">
         <v>7000</v>
       </c>
-      <c r="D118" s="4">
+      <c r="D119" s="4">
         <f t="shared" si="12"/>
         <v>10590</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B119" s="4" t="s">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B120" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C119" s="5">
+      <c r="C120" s="5">
         <v>-10000</v>
       </c>
-      <c r="D119" s="4">
+      <c r="D120" s="4">
         <f t="shared" si="12"/>
         <v>590</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B120" s="4" t="s">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B121" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C120" s="5">
+      <c r="C121" s="5">
         <v>12000</v>
       </c>
-      <c r="D120" s="4">
+      <c r="D121" s="4">
         <f t="shared" si="12"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B121" s="4" t="s">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B122" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C121" s="5">
+      <c r="C122" s="5">
         <v>-10000</v>
       </c>
-      <c r="D121" s="4">
+      <c r="D122" s="4">
         <f t="shared" si="12"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B122" s="4" t="s">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B123" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C122" s="5">
+      <c r="C123" s="5">
         <v>2000</v>
       </c>
-      <c r="D122" s="4">
+      <c r="D123" s="4">
         <f t="shared" si="12"/>
         <v>4590</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="B123" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C123" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D123" s="4">
-        <f t="shared" ref="D123:D128" si="13">D122+C123</f>
-        <v>6590</v>
-      </c>
-    </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="B124" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C124" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D124" s="4">
+        <f t="shared" ref="D124:D129" si="13">D123+C124</f>
+        <v>6590</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="B124" s="4" t="s">
+      <c r="B125" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C124" s="5">
+      <c r="C125" s="5">
         <v>7000</v>
       </c>
-      <c r="D124" s="4">
+      <c r="D125" s="4">
         <f t="shared" si="13"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B125" s="4" t="s">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B126" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C125" s="5">
+      <c r="C126" s="5">
         <v>-10000</v>
       </c>
-      <c r="D125" s="4">
+      <c r="D126" s="4">
         <f t="shared" si="13"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="16" t="s">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="B126" s="4" t="s">
+      <c r="B127" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C126" s="5">
+      <c r="C127" s="5">
         <v>2000</v>
       </c>
-      <c r="D126" s="4">
+      <c r="D127" s="4">
         <f t="shared" si="13"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="16" t="s">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="B127" s="4" t="s">
+      <c r="B128" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C127" s="5">
+      <c r="C128" s="5">
         <v>8000</v>
       </c>
-      <c r="D127" s="4">
+      <c r="D128" s="4">
         <f t="shared" si="13"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B128" s="4" t="s">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B129" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C128" s="5">
+      <c r="C129" s="5">
         <v>-10000</v>
       </c>
-      <c r="D128" s="4">
+      <c r="D129" s="4">
         <f t="shared" si="13"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="16" t="s">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="B129" s="4" t="s">
+      <c r="B130" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C129" s="5">
+      <c r="C130" s="5">
         <v>2000</v>
       </c>
-      <c r="D129" s="4">
-        <f t="shared" ref="D129:D134" si="14">D128+C129</f>
+      <c r="D130" s="4">
+        <f t="shared" ref="D130:D135" si="14">D129+C130</f>
         <v>5590</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B130" s="4" t="s">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B131" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C130" s="5">
+      <c r="C131" s="5">
         <v>5000</v>
       </c>
-      <c r="D130" s="4">
+      <c r="D131" s="4">
         <f t="shared" si="14"/>
         <v>10590</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B131" s="4" t="s">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B132" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C131" s="5">
+      <c r="C132" s="5">
         <v>-10000</v>
       </c>
-      <c r="D131" s="4">
+      <c r="D132" s="4">
         <f t="shared" si="14"/>
         <v>590</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B132" s="4" t="s">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B133" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C132" s="5">
+      <c r="C133" s="5">
         <v>2000</v>
       </c>
-      <c r="D132" s="4">
+      <c r="D133" s="4">
         <f t="shared" si="14"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B133" s="4" t="s">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B134" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C133" s="5">
+      <c r="C134" s="5">
         <v>9000</v>
       </c>
-      <c r="D133" s="4">
+      <c r="D134" s="4">
         <f t="shared" si="14"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B134" s="4" t="s">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B135" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C134" s="5">
+      <c r="C135" s="5">
         <v>-10000</v>
       </c>
-      <c r="D134" s="4">
+      <c r="D135" s="4">
         <f t="shared" si="14"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B135" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C135" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D135" s="4">
-        <f t="shared" ref="D135:D140" si="15">D134+C135</f>
-        <v>3590</v>
-      </c>
-    </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B136" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C136" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D136" s="4">
+        <f t="shared" ref="D136:D141" si="15">D135+C136</f>
+        <v>3590</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="B136" s="4" t="s">
+      <c r="B137" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C136" s="5">
+      <c r="C137" s="5">
         <v>8000</v>
       </c>
-      <c r="D136" s="4">
+      <c r="D137" s="4">
         <f t="shared" si="15"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B137" s="4" t="s">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B138" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C137" s="5">
+      <c r="C138" s="5">
         <v>-10000</v>
       </c>
-      <c r="D137" s="4">
+      <c r="D138" s="4">
         <f t="shared" si="15"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="16" t="s">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="B138" s="4" t="s">
+      <c r="B139" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C138" s="5">
+      <c r="C139" s="5">
         <v>2000</v>
       </c>
-      <c r="D138" s="4">
+      <c r="D139" s="4">
         <f t="shared" si="15"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="16" t="s">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="B139" s="4" t="s">
+      <c r="B140" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C139" s="5">
+      <c r="C140" s="5">
         <v>12000</v>
       </c>
-      <c r="D139" s="4">
+      <c r="D140" s="4">
         <f t="shared" si="15"/>
         <v>15590</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B140" s="4" t="s">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B141" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C140" s="5">
+      <c r="C141" s="5">
         <v>-10000</v>
       </c>
-      <c r="D140" s="4">
+      <c r="D141" s="4">
         <f t="shared" si="15"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="B141" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="C141" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D141" s="4">
-        <f t="shared" ref="D141:D146" si="16">D140+C141</f>
-        <v>7590</v>
-      </c>
-    </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="B142" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C142" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D142" s="4">
+        <f t="shared" ref="D142:D147" si="16">D141+C142</f>
+        <v>7590</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="B142" s="4" t="s">
+      <c r="B143" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="C142" s="5">
+      <c r="C143" s="5">
         <v>10000</v>
       </c>
-      <c r="D142" s="4">
+      <c r="D143" s="4">
         <f t="shared" si="16"/>
         <v>17590</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B143" s="4" t="s">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B144" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C143" s="5">
+      <c r="C144" s="5">
         <v>-10000</v>
       </c>
-      <c r="D143" s="4">
+      <c r="D144" s="4">
         <f t="shared" si="16"/>
         <v>7590</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B144" s="4" t="s">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B145" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="C144" s="5">
+      <c r="C145" s="5">
         <v>2000</v>
       </c>
-      <c r="D144" s="4">
+      <c r="D145" s="4">
         <f t="shared" si="16"/>
         <v>9590</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="16" t="s">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="B145" s="4" t="s">
+      <c r="B146" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="C145" s="5">
+      <c r="C146" s="5">
         <v>-1200</v>
       </c>
-      <c r="D145" s="4">
+      <c r="D146" s="4">
         <f t="shared" si="16"/>
         <v>8390</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B146" s="4" t="s">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B147" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="C146" s="5">
+      <c r="C147" s="5">
         <v>500</v>
       </c>
-      <c r="D146" s="4">
+      <c r="D147" s="4">
         <f t="shared" si="16"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="16" t="s">
-        <v>165</v>
-      </c>
-      <c r="B147" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="C147" s="5">
-        <v>750</v>
-      </c>
-      <c r="D147" s="4">
-        <f t="shared" ref="D147:D152" si="17">D146+C147</f>
-        <v>9640</v>
-      </c>
-    </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="B148" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C148" s="5">
+        <v>750</v>
+      </c>
+      <c r="D148" s="4">
+        <f t="shared" ref="D148:D153" si="17">D147+C148</f>
+        <v>9640</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="B148" s="4" t="s">
+      <c r="B149" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C148" s="5">
+      <c r="C149" s="5">
         <v>2000</v>
       </c>
-      <c r="D148" s="4">
+      <c r="D149" s="4">
         <f t="shared" si="17"/>
         <v>11640</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B149" s="4" t="s">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B150" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C149" s="5">
+      <c r="C150" s="5">
         <v>2000</v>
       </c>
-      <c r="D149" s="4">
+      <c r="D150" s="4">
         <f t="shared" si="17"/>
         <v>13640</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B150" s="4" t="s">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B151" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C150" s="5">
+      <c r="C151" s="5">
         <v>-10000</v>
       </c>
-      <c r="D150" s="4">
+      <c r="D151" s="4">
         <f t="shared" si="17"/>
         <v>3640</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B151" s="4" t="s">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B152" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="C151" s="5">
+      <c r="C152" s="5">
         <v>350</v>
       </c>
-      <c r="D151" s="4">
+      <c r="D152" s="4">
         <f t="shared" si="17"/>
         <v>3990</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="16" t="s">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="B152" s="4" t="s">
+      <c r="B153" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="C152" s="5">
+      <c r="C153" s="5">
         <v>300</v>
       </c>
-      <c r="D152" s="4">
+      <c r="D153" s="4">
         <f t="shared" si="17"/>
         <v>4290</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" s="16" t="s">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="B153" s="4" t="s">
+      <c r="B154" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="C153" s="5">
+      <c r="C154" s="5">
         <v>3800</v>
       </c>
-      <c r="D153" s="4">
-        <f t="shared" ref="D153:D159" si="18">D152+C153</f>
+      <c r="D154" s="4">
+        <f t="shared" ref="D154:D160" si="18">D153+C154</f>
         <v>8090</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B154" s="4" t="s">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B155" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C154" s="5">
+      <c r="C155" s="5">
         <v>500</v>
       </c>
-      <c r="D154" s="4">
+      <c r="D155" s="4">
         <f t="shared" si="18"/>
         <v>8590</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="16" t="s">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="B155" s="4" t="s">
+      <c r="B156" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="C155" s="5">
+      <c r="C156" s="5">
         <v>1300</v>
       </c>
-      <c r="D155" s="4">
+      <c r="D156" s="4">
         <f t="shared" si="18"/>
         <v>9890</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="16" t="s">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="B156" s="4" t="s">
+      <c r="B157" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C156" s="5">
+      <c r="C157" s="5">
         <v>9000</v>
       </c>
-      <c r="D156" s="4">
+      <c r="D157" s="4">
         <f t="shared" si="18"/>
         <v>18890</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B157" s="4" t="s">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B158" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C157" s="5">
+      <c r="C158" s="5">
         <v>-10000</v>
       </c>
-      <c r="D157" s="4">
+      <c r="D158" s="4">
         <f t="shared" si="18"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="16" t="s">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="B158" s="4" t="s">
+      <c r="B159" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C158" s="5">
+      <c r="C159" s="5">
         <v>2000</v>
       </c>
-      <c r="D158" s="4">
+      <c r="D159" s="4">
         <f t="shared" si="18"/>
         <v>10890</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B159" s="4" t="s">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B160" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C159" s="5">
+      <c r="C160" s="5">
         <v>-10000</v>
       </c>
-      <c r="D159" s="4">
+      <c r="D160" s="4">
         <f t="shared" si="18"/>
         <v>890</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="B160" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="C160" s="5">
-        <v>500</v>
-      </c>
-      <c r="D160" s="4">
-        <f t="shared" ref="D160:D165" si="19">D159+C160</f>
-        <v>1390</v>
-      </c>
-    </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="B161" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C161" s="5">
+        <v>500</v>
+      </c>
+      <c r="D161" s="4">
+        <f t="shared" ref="D161:D166" si="19">D160+C161</f>
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="B161" s="4" t="s">
+      <c r="B162" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="C161" s="5">
+      <c r="C162" s="5">
         <v>10000</v>
       </c>
-      <c r="D161" s="4">
+      <c r="D162" s="4">
         <f t="shared" si="19"/>
         <v>11390</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B162" s="4" t="s">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B163" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C162" s="5">
+      <c r="C163" s="5">
         <v>-10000</v>
       </c>
-      <c r="D162" s="4">
+      <c r="D163" s="4">
         <f t="shared" si="19"/>
         <v>1390</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163" s="16" t="s">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="B163" s="4" t="s">
+      <c r="B164" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C163" s="5">
+      <c r="C164" s="5">
         <v>3000</v>
       </c>
-      <c r="D163" s="4">
+      <c r="D164" s="4">
         <f t="shared" si="19"/>
         <v>4390</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164" s="16" t="s">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="B164" s="4" t="s">
+      <c r="B165" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C164" s="5">
+      <c r="C165" s="5">
         <v>2000</v>
       </c>
-      <c r="D164" s="4">
+      <c r="D165" s="4">
         <f t="shared" si="19"/>
         <v>6390</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B165" s="4" t="s">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B166" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C165" s="5">
+      <c r="C166" s="5">
         <v>2000</v>
       </c>
-      <c r="D165" s="4">
+      <c r="D166" s="4">
         <f t="shared" si="19"/>
         <v>8390</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A166" s="16" t="s">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="B166" s="4" t="s">
+      <c r="B167" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C166" s="5">
+      <c r="C167" s="5">
         <v>11000</v>
       </c>
-      <c r="D166" s="4">
-        <f t="shared" ref="D166:D171" si="20">D165+C166</f>
+      <c r="D167" s="4">
+        <f t="shared" ref="D167:D172" si="20">D166+C167</f>
         <v>19390</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B167" s="4" t="s">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B168" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C167" s="5">
+      <c r="C168" s="5">
         <v>-10000</v>
       </c>
-      <c r="D167" s="4">
+      <c r="D168" s="4">
         <f t="shared" si="20"/>
         <v>9390</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A168" s="16" t="s">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" s="16" t="s">
         <v>187</v>
       </c>
-      <c r="B168" s="4" t="s">
+      <c r="B169" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C168" s="5">
+      <c r="C169" s="5">
         <v>3000</v>
       </c>
-      <c r="D168" s="4">
+      <c r="D169" s="4">
         <f t="shared" si="20"/>
         <v>12390</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B169" s="4" t="s">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B170" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C169" s="5">
+      <c r="C170" s="5">
         <v>-10000</v>
       </c>
-      <c r="D169" s="4">
+      <c r="D170" s="4">
         <f t="shared" si="20"/>
         <v>2390</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B170" s="4" t="s">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B171" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C170" s="5">
+      <c r="C171" s="5">
         <v>500</v>
       </c>
-      <c r="D170" s="4">
+      <c r="D171" s="4">
         <f t="shared" si="20"/>
         <v>2890</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" s="16" t="s">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" s="16" t="s">
         <v>189</v>
       </c>
-      <c r="B171" s="4" t="s">
+      <c r="B172" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C171" s="5">
+      <c r="C172" s="5">
         <v>5600</v>
       </c>
-      <c r="D171" s="4">
+      <c r="D172" s="4">
         <f t="shared" si="20"/>
         <v>8490</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B172" s="4" t="s">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B173" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="C172" s="5">
+      <c r="C173" s="5">
         <v>4700</v>
       </c>
-      <c r="D172" s="4">
-        <f t="shared" ref="D172:D178" si="21">D171+C172</f>
+      <c r="D173" s="4">
+        <f t="shared" ref="D173:D179" si="21">D172+C173</f>
         <v>13190</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173" s="16" t="s">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174" s="16" t="s">
         <v>192</v>
       </c>
-      <c r="B173" s="4" t="s">
+      <c r="B174" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C173" s="5">
+      <c r="C174" s="5">
         <v>1500</v>
       </c>
-      <c r="D173" s="4">
+      <c r="D174" s="4">
         <f t="shared" si="21"/>
         <v>14690</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B174" s="4" t="s">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B175" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C174" s="5">
+      <c r="C175" s="5">
         <v>500</v>
       </c>
-      <c r="D174" s="4">
+      <c r="D175" s="4">
         <f t="shared" si="21"/>
         <v>15190</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A175" s="16" t="s">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="B175" s="4" t="s">
+      <c r="B176" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="C175" s="5">
+      <c r="C176" s="5">
         <v>1000</v>
       </c>
-      <c r="D175" s="4">
+      <c r="D176" s="4">
         <f t="shared" si="21"/>
         <v>16190</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176" s="16" t="s">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="B176" s="4" t="s">
+      <c r="B177" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="C176" s="5">
+      <c r="C177" s="5">
         <v>1000</v>
       </c>
-      <c r="D176" s="4">
+      <c r="D177" s="4">
         <f t="shared" si="21"/>
         <v>17190</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A177" s="16" t="s">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A178" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="B177" s="4" t="s">
+      <c r="B178" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C177" s="5">
+      <c r="C178" s="5">
         <v>3000</v>
       </c>
-      <c r="D177" s="4">
+      <c r="D178" s="4">
         <f t="shared" si="21"/>
         <v>20190</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B178" s="4" t="s">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B179" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C178" s="5">
+      <c r="C179" s="5">
         <v>-20000</v>
       </c>
-      <c r="D178" s="4">
+      <c r="D179" s="4">
         <f t="shared" si="21"/>
         <v>190</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B179" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C179" s="5">
-        <v>500</v>
-      </c>
-      <c r="D179" s="4">
-        <f t="shared" ref="D179:D185" si="22">D178+C179</f>
-        <v>690</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -3650,383 +3650,422 @@
         <v>500</v>
       </c>
       <c r="D180" s="4">
+        <f t="shared" ref="D180:D186" si="22">D179+C180</f>
+        <v>690</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B181" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C181" s="5">
+        <v>500</v>
+      </c>
+      <c r="D181" s="4">
         <f t="shared" si="22"/>
         <v>1190</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="16" t="s">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="B181" s="4" t="s">
+      <c r="B182" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="C181" s="5">
+      <c r="C182" s="5">
         <v>10000</v>
       </c>
-      <c r="D181" s="4">
+      <c r="D182" s="4">
         <f t="shared" si="22"/>
         <v>11190</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B182" s="4" t="s">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B183" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C182" s="5">
+      <c r="C183" s="5">
         <v>-10000</v>
       </c>
-      <c r="D182" s="4">
+      <c r="D183" s="4">
         <f t="shared" si="22"/>
         <v>1190</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183" s="16" t="s">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A184" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="B183" s="4" t="s">
+      <c r="B184" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C183" s="5">
+      <c r="C184" s="5">
         <v>3000</v>
       </c>
-      <c r="D183" s="4">
+      <c r="D184" s="4">
         <f t="shared" si="22"/>
         <v>4190</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" s="16" t="s">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A185" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="B184" s="4" t="s">
+      <c r="B185" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C184" s="5">
+      <c r="C185" s="5">
         <v>11000</v>
       </c>
-      <c r="D184" s="4">
+      <c r="D185" s="4">
         <f t="shared" si="22"/>
         <v>15190</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B185" s="4" t="s">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B186" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C185" s="5">
+      <c r="C186" s="5">
         <v>-10000</v>
       </c>
-      <c r="D185" s="4">
+      <c r="D186" s="4">
         <f t="shared" si="22"/>
         <v>5190</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A186" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="B186" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C186" s="5">
-        <v>3000</v>
-      </c>
-      <c r="D186" s="4">
-        <f t="shared" ref="D186:D192" si="23">D185+C186</f>
-        <v>8190</v>
-      </c>
-    </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="B187" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C187" s="5">
+        <v>3000</v>
+      </c>
+      <c r="D187" s="4">
+        <f t="shared" ref="D187:D193" si="23">D186+C187</f>
+        <v>8190</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A188" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="B187" s="4" t="s">
+      <c r="B188" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="C187" s="5">
+      <c r="C188" s="5">
         <v>14000</v>
       </c>
-      <c r="D187" s="4">
+      <c r="D188" s="4">
         <f t="shared" si="23"/>
         <v>22190</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B188" s="4" t="s">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B189" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="C188" s="5">
+      <c r="C189" s="5">
         <v>-20000</v>
       </c>
-      <c r="D188" s="4">
+      <c r="D189" s="4">
         <f t="shared" si="23"/>
         <v>2190</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" s="16" t="s">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A190" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="B189" s="4" t="s">
+      <c r="B190" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="C189" s="5">
+      <c r="C190" s="5">
         <v>5000</v>
       </c>
-      <c r="D189" s="4">
+      <c r="D190" s="4">
         <f t="shared" si="23"/>
         <v>7190</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A190" s="16" t="s">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A191" s="16" t="s">
         <v>213</v>
       </c>
-      <c r="B190" s="4" t="s">
+      <c r="B191" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="C190" s="5">
+      <c r="C191" s="5">
         <v>5000</v>
       </c>
-      <c r="D190" s="4">
+      <c r="D191" s="4">
         <f t="shared" si="23"/>
         <v>12190</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A191" s="16" t="s">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A192" s="16" t="s">
         <v>215</v>
       </c>
-      <c r="B191" s="4" t="s">
+      <c r="B192" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C191" s="5">
+      <c r="C192" s="5">
         <v>11000</v>
       </c>
-      <c r="D191" s="4">
+      <c r="D192" s="4">
         <f t="shared" si="23"/>
         <v>23190</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B192" s="4" t="s">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B193" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C192" s="5">
+      <c r="C193" s="5">
         <v>-20000</v>
       </c>
-      <c r="D192" s="4">
+      <c r="D193" s="4">
         <f t="shared" si="23"/>
         <v>3190</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A193" s="16" t="s">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A194" s="16" t="s">
         <v>216</v>
       </c>
-      <c r="B193" s="4" t="s">
+      <c r="B194" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C193" s="5">
+      <c r="C194" s="5">
         <v>500</v>
       </c>
-      <c r="D193" s="4">
-        <f t="shared" ref="D193:D198" si="24">D192+C193</f>
+      <c r="D194" s="4">
+        <f t="shared" ref="D194:D199" si="24">D193+C194</f>
         <v>3690</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B194" s="4" t="s">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B195" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C194" s="5">
+      <c r="C195" s="5">
         <v>3000</v>
       </c>
-      <c r="D194" s="4">
+      <c r="D195" s="4">
         <f t="shared" si="24"/>
         <v>6690</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A195" s="16" t="s">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A196" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="B195" s="4" t="s">
+      <c r="B196" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="C195" s="5">
+      <c r="C196" s="5">
         <v>12000</v>
       </c>
-      <c r="D195" s="4">
+      <c r="D196" s="4">
         <f t="shared" si="24"/>
         <v>18690</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B196" s="4" t="s">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B197" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C196" s="5">
+      <c r="C197" s="5">
         <v>-10000</v>
       </c>
-      <c r="D196" s="4">
+      <c r="D197" s="4">
         <f t="shared" si="24"/>
         <v>8690</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A197" s="16" t="s">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A198" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="B197" s="4" t="s">
+      <c r="B198" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="C197" s="5">
+      <c r="C198" s="5">
         <v>5000</v>
       </c>
-      <c r="D197" s="4">
+      <c r="D198" s="4">
         <f t="shared" si="24"/>
         <v>13690</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B198" s="4" t="s">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B199" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C198" s="5">
+      <c r="C199" s="5">
         <v>-10000</v>
       </c>
-      <c r="D198" s="4">
+      <c r="D199" s="4">
         <f t="shared" si="24"/>
         <v>3690</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A199" s="16" t="s">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A200" s="16" t="s">
         <v>221</v>
       </c>
-      <c r="B199" s="4" t="s">
+      <c r="B200" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="C199" s="5">
+      <c r="C200" s="5">
         <v>12000</v>
       </c>
-      <c r="D199" s="4">
-        <f t="shared" ref="D199:D204" si="25">D198+C199</f>
+      <c r="D200" s="4">
+        <f t="shared" ref="D200:D205" si="25">D199+C200</f>
         <v>15690</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B200" s="4" t="s">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B201" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C200" s="5">
+      <c r="C201" s="5">
         <v>-10000</v>
       </c>
-      <c r="D200" s="4">
+      <c r="D201" s="4">
         <f t="shared" si="25"/>
         <v>5690</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A201" s="16" t="s">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A202" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="B201" s="4" t="s">
+      <c r="B202" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C201" s="5">
+      <c r="C202" s="5">
         <v>2000</v>
       </c>
-      <c r="D201" s="4">
+      <c r="D202" s="4">
         <f t="shared" si="25"/>
         <v>7690</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A202" s="16" t="s">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A203" s="16" t="s">
         <v>227</v>
       </c>
-      <c r="B202" s="4" t="s">
+      <c r="B203" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="C202" s="5">
+      <c r="C203" s="5">
         <v>1000</v>
       </c>
-      <c r="D202" s="4">
+      <c r="D203" s="4">
         <f t="shared" si="25"/>
         <v>8690</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A203" s="16" t="s">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A204" s="16" t="s">
         <v>229</v>
       </c>
-      <c r="B203" s="4" t="s">
+      <c r="B204" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="C203" s="5">
+      <c r="C204" s="5">
         <v>5000</v>
       </c>
-      <c r="D203" s="4">
+      <c r="D204" s="4">
         <f t="shared" si="25"/>
         <v>13690</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B204" s="4" t="s">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B205" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C204" s="5">
+      <c r="C205" s="5">
         <v>-10000</v>
       </c>
-      <c r="D204" s="4">
+      <c r="D205" s="4">
         <f t="shared" si="25"/>
         <v>3690</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A205" s="16" t="s">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A206" s="16" t="s">
         <v>231</v>
       </c>
-      <c r="B205" s="4" t="s">
+      <c r="B206" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="C205" s="5">
+      <c r="C206" s="5">
         <v>13000</v>
-      </c>
-      <c r="D205" s="4">
-        <f>D204+C205</f>
-        <v>16690</v>
-      </c>
-    </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B206" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C206" s="5">
-        <v>-10000</v>
       </c>
       <c r="D206" s="4">
         <f>D205+C206</f>
-        <v>6690</v>
+        <v>16690</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A207" s="16" t="s">
-        <v>233</v>
-      </c>
       <c r="B207" s="4" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C207" s="5">
-        <v>3000</v>
+        <v>-10000</v>
       </c>
       <c r="D207" s="4">
         <f>D206+C207</f>
+        <v>6690</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A208" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="B208" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C208" s="5">
+        <v>3000</v>
+      </c>
+      <c r="D208" s="4">
+        <f>D207+C208</f>
         <v>9690</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A209" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="B209" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C209" s="5">
+        <v>13000</v>
+      </c>
+      <c r="D209" s="4">
+        <f>D208+C209</f>
+        <v>22690</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B210" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="C210" s="5">
+        <v>-20000</v>
+      </c>
+      <c r="D210" s="4">
+        <f>D209+C210</f>
+        <v>2690</v>
       </c>
     </row>
   </sheetData>
@@ -4558,7 +4597,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
duy lay tien loi 3tr co diem
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="236">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -724,6 +724,9 @@
   </si>
   <si>
     <t>30/10/2024</t>
+  </si>
+  <si>
+    <t>31/10/2024</t>
   </si>
 </sst>
 </file>
@@ -1224,11 +1227,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K210"/>
+  <dimension ref="A1:K211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I37" sqref="I37"/>
+      <pane ySplit="1" topLeftCell="A180" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D212" sqref="D212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4066,6 +4069,21 @@
       <c r="D210" s="4">
         <f>D209+C210</f>
         <v>2690</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A211" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="B211" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C211" s="5">
+        <v>3000</v>
+      </c>
+      <c r="D211" s="4">
+        <f>D210+C211</f>
+        <v>5690</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
duy lay tien loi co diem ngay 01,02
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="238">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -727,6 +727,12 @@
   </si>
   <si>
     <t>31/10/2024</t>
+  </si>
+  <si>
+    <t>Duy lấy 16tr tiền lời</t>
+  </si>
+  <si>
+    <t>02/11/2024</t>
   </si>
 </sst>
 </file>
@@ -1227,11 +1233,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K211"/>
+  <dimension ref="A1:K214"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A180" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D212" sqref="D212"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I56" sqref="I56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1307,8 +1313,8 @@
         <v>20</v>
       </c>
       <c r="J3" s="4">
-        <f>SUM(I3:I70)</f>
-        <v>600</v>
+        <f>SUM(I3:I71)</f>
+        <v>620</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1944,7 +1950,7 @@
         <v>7640</v>
       </c>
       <c r="D53" s="4">
-        <f t="shared" ref="D53:D60" si="2">D52+C53</f>
+        <f t="shared" ref="D53:D61" si="2">D52+C53</f>
         <v>9090</v>
       </c>
       <c r="H53" s="16" t="s">
@@ -1966,7 +1972,7 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H55" s="16" t="s">
-        <v>207</v>
+        <v>237</v>
       </c>
       <c r="I55" s="5">
         <v>20</v>
@@ -1974,358 +1980,352 @@
       <c r="K55" s="14"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B56" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C56" s="5">
-        <v>3000</v>
-      </c>
-      <c r="D56" s="4">
-        <f>D53+C56</f>
-        <v>12090</v>
-      </c>
       <c r="H56" s="16" t="s">
-        <v>187</v>
+        <v>207</v>
       </c>
       <c r="I56" s="5">
-        <v>10</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="K56" s="14"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B57" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C57" s="5">
+        <v>3000</v>
+      </c>
+      <c r="D57" s="4">
+        <f>D53+C57</f>
+        <v>12090</v>
+      </c>
+      <c r="H57" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="I57" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B58" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C57" s="5">
+      <c r="C58" s="5">
         <v>-10000</v>
       </c>
-      <c r="D57" s="4">
+      <c r="D58" s="4">
         <f t="shared" si="2"/>
         <v>2090</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B58" s="4" t="s">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B59" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C58" s="5">
+      <c r="C59" s="5">
         <v>800</v>
       </c>
-      <c r="D58" s="4">
+      <c r="D59" s="4">
         <f t="shared" si="2"/>
         <v>2890</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="16" t="s">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B60" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C59" s="5">
+      <c r="C60" s="5">
         <v>2000</v>
       </c>
-      <c r="D59" s="4">
+      <c r="D60" s="4">
         <f t="shared" si="2"/>
         <v>4890</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" s="16" t="s">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B61" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C60" s="5">
+      <c r="C61" s="5">
         <v>4000</v>
       </c>
-      <c r="D60" s="4">
+      <c r="D61" s="4">
         <f t="shared" si="2"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61" s="16" t="s">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B62" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C61" s="5">
+      <c r="C62" s="5">
         <v>4000</v>
       </c>
-      <c r="D61" s="4">
-        <f t="shared" ref="D61:D66" si="3">D60+C61</f>
+      <c r="D62" s="4">
+        <f t="shared" ref="D62:D67" si="3">D61+C62</f>
         <v>12890</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B62" s="4" t="s">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B63" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C62" s="5">
+      <c r="C63" s="5">
         <v>5000</v>
       </c>
-      <c r="D62" s="4">
+      <c r="D63" s="4">
         <f t="shared" si="3"/>
         <v>17890</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B63" s="4" t="s">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B64" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C63" s="5">
+      <c r="C64" s="5">
         <v>-10000</v>
       </c>
-      <c r="D63" s="4">
+      <c r="D64" s="4">
         <f t="shared" si="3"/>
         <v>7890</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64" s="16">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="16">
         <v>44969</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B65" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C64" s="5">
+      <c r="C65" s="5">
         <v>900</v>
       </c>
-      <c r="D64" s="4">
+      <c r="D65" s="4">
         <f t="shared" si="3"/>
         <v>8790</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B65" s="4" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C65" s="5">
+      <c r="C66" s="5">
         <v>4000</v>
       </c>
-      <c r="D65" s="4">
+      <c r="D66" s="4">
         <f t="shared" si="3"/>
         <v>12790</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B66" s="4" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B67" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C66" s="5">
+      <c r="C67" s="5">
         <v>-10000</v>
       </c>
-      <c r="D66" s="4">
+      <c r="D67" s="4">
         <f t="shared" si="3"/>
         <v>2790</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C67" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D67" s="4">
-        <f t="shared" ref="D67:D74" si="4">D66+C67</f>
-        <v>4790</v>
-      </c>
-    </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C68" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D68" s="4">
+        <f t="shared" ref="D68:D75" si="4">D67+C68</f>
+        <v>4790</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B69" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C68" s="5">
+      <c r="C69" s="5">
         <v>700</v>
       </c>
-      <c r="D68" s="4">
+      <c r="D69" s="4">
         <f t="shared" si="4"/>
         <v>5490</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B69" s="4" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B70" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C69" s="5">
+      <c r="C70" s="5">
         <v>4000</v>
       </c>
-      <c r="D69" s="4">
+      <c r="D70" s="4">
         <f t="shared" si="4"/>
         <v>9490</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="16" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B71" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C70" s="5">
+      <c r="C71" s="5">
         <v>600</v>
       </c>
-      <c r="D70" s="4">
+      <c r="D71" s="4">
         <f t="shared" si="4"/>
         <v>10090</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B71" s="4" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B72" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C71" s="5">
+      <c r="C72" s="5">
         <v>-10000</v>
       </c>
-      <c r="D71" s="4">
+      <c r="D72" s="4">
         <f t="shared" si="4"/>
         <v>90</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="16" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B73" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C72" s="5">
+      <c r="C73" s="5">
         <f>700+5000+300+600+400+1000+800</f>
         <v>8800</v>
       </c>
-      <c r="D72" s="4">
+      <c r="D73" s="4">
         <f t="shared" si="4"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B73" s="4" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C73" s="5">
+      <c r="C74" s="5">
         <v>6000</v>
       </c>
-      <c r="D73" s="4">
+      <c r="D74" s="4">
         <f t="shared" si="4"/>
         <v>14890</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B74" s="4" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B75" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C74" s="5">
+      <c r="C75" s="5">
         <v>-10000</v>
       </c>
-      <c r="D74" s="4">
+      <c r="D75" s="4">
         <f t="shared" si="4"/>
         <v>4890</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="16" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="B76" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C75" s="5">
+      <c r="C76" s="5">
         <v>500</v>
       </c>
-      <c r="D75" s="4">
-        <f t="shared" ref="D75:D80" si="5">D74+C75</f>
+      <c r="D76" s="4">
+        <f t="shared" ref="D76:D81" si="5">D75+C76</f>
         <v>5390</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B76" s="4" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B77" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C76" s="5">
+      <c r="C77" s="5">
         <v>700</v>
       </c>
-      <c r="D76" s="4">
+      <c r="D77" s="4">
         <f t="shared" si="5"/>
         <v>6090</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B77" s="4" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B78" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C77" s="5">
+      <c r="C78" s="5">
         <v>1500</v>
       </c>
-      <c r="D77" s="4">
+      <c r="D78" s="4">
         <f t="shared" si="5"/>
         <v>7590</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B78" s="4" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B79" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C78" s="5">
+      <c r="C79" s="5">
         <v>5000</v>
       </c>
-      <c r="D78" s="4">
+      <c r="D79" s="4">
         <f t="shared" si="5"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B79" s="4" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B80" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C79" s="5">
+      <c r="C80" s="5">
         <v>-10000</v>
       </c>
-      <c r="D79" s="4">
+      <c r="D80" s="4">
         <f t="shared" si="5"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="16" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B81" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C80" s="5">
+      <c r="C81" s="5">
         <v>2000</v>
       </c>
-      <c r="D80" s="4">
+      <c r="D81" s="4">
         <f t="shared" si="5"/>
         <v>4590</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B81" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C81" s="5">
-        <v>700</v>
-      </c>
-      <c r="D81" s="4">
-        <f t="shared" ref="D81:D86" si="6">D80+C81</f>
-        <v>5290</v>
-      </c>
-    </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="16" t="s">
-        <v>82</v>
-      </c>
       <c r="B82" s="4" t="s">
         <v>77</v>
       </c>
@@ -2333,401 +2333,404 @@
         <v>700</v>
       </c>
       <c r="D82" s="4">
+        <f t="shared" ref="D82:D87" si="6">D81+C82</f>
+        <v>5290</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C83" s="5">
+        <v>700</v>
+      </c>
+      <c r="D83" s="4">
         <f t="shared" si="6"/>
         <v>5990</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="16" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="B84" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C83" s="5">
+      <c r="C84" s="5">
         <v>700</v>
       </c>
-      <c r="D83" s="4">
+      <c r="D84" s="4">
         <f t="shared" si="6"/>
         <v>6690</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="16" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="B84" s="4" t="s">
+      <c r="B85" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C84" s="5">
+      <c r="C85" s="5">
         <v>4000</v>
       </c>
-      <c r="D84" s="4">
+      <c r="D85" s="4">
         <f t="shared" si="6"/>
         <v>10690</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B85" s="4" t="s">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B86" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C85" s="5">
+      <c r="C86" s="5">
         <v>-10000</v>
       </c>
-      <c r="D85" s="4">
+      <c r="D86" s="4">
         <f t="shared" si="6"/>
         <v>690</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="16" t="s">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="B87" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C86" s="5">
+      <c r="C87" s="5">
         <v>1000</v>
       </c>
-      <c r="D86" s="4">
+      <c r="D87" s="4">
         <f t="shared" si="6"/>
         <v>1690</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="16" t="s">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="B87" s="4" t="s">
+      <c r="B88" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C87" s="5">
+      <c r="C88" s="5">
         <v>7000</v>
       </c>
-      <c r="D87" s="4">
-        <f t="shared" ref="D87:D92" si="7">D86+C87</f>
+      <c r="D88" s="4">
+        <f t="shared" ref="D88:D93" si="7">D87+C88</f>
         <v>8690</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B88" s="4" t="s">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B89" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C88" s="5">
+      <c r="C89" s="5">
         <v>10000</v>
       </c>
-      <c r="D88" s="4">
+      <c r="D89" s="4">
         <f t="shared" si="7"/>
         <v>18690</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B89" s="4" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B90" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C89" s="5">
+      <c r="C90" s="5">
         <v>-10000</v>
       </c>
-      <c r="D89" s="4">
+      <c r="D90" s="4">
         <f t="shared" si="7"/>
         <v>8690</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B90" s="4" t="s">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B91" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C90" s="5">
+      <c r="C91" s="5">
         <v>1700</v>
       </c>
-      <c r="D90" s="4">
+      <c r="D91" s="4">
         <f t="shared" si="7"/>
         <v>10390</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B91" s="4" t="s">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B92" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C91" s="5">
+      <c r="C92" s="5">
         <v>-10000</v>
       </c>
-      <c r="D91" s="4">
+      <c r="D92" s="4">
         <f t="shared" si="7"/>
         <v>390</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B92" s="4" t="s">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B93" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C92" s="5">
+      <c r="C93" s="5">
         <v>6000</v>
       </c>
-      <c r="D92" s="4">
+      <c r="D93" s="4">
         <f t="shared" si="7"/>
         <v>6390</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="B93" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C93" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D93" s="4">
-        <f t="shared" ref="D93:D98" si="8">D92+C93</f>
-        <v>8390</v>
-      </c>
-    </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C94" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D94" s="4">
+        <f t="shared" ref="D94:D99" si="8">D93+C94</f>
+        <v>8390</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="B94" s="4" t="s">
+      <c r="B95" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C94" s="5">
+      <c r="C95" s="5">
         <v>5000</v>
       </c>
-      <c r="D94" s="4">
+      <c r="D95" s="4">
         <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B95" s="4" t="s">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B96" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C95" s="5">
+      <c r="C96" s="5">
         <v>-10000</v>
       </c>
-      <c r="D95" s="4">
+      <c r="D96" s="4">
         <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="16" t="s">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="B96" s="4" t="s">
+      <c r="B97" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C96" s="5">
+      <c r="C97" s="5">
         <v>1000</v>
       </c>
-      <c r="D96" s="4">
+      <c r="D97" s="4">
         <f t="shared" si="8"/>
         <v>4390</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B97" s="4" t="s">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B98" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C97" s="5">
+      <c r="C98" s="5">
         <v>9000</v>
       </c>
-      <c r="D97" s="4">
+      <c r="D98" s="4">
         <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B98" s="4" t="s">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B99" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C98" s="5">
+      <c r="C99" s="5">
         <v>-10000</v>
       </c>
-      <c r="D98" s="4">
+      <c r="D99" s="4">
         <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B99" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C99" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D99" s="4">
-        <f t="shared" ref="D99:D104" si="9">D98+C99</f>
-        <v>5390</v>
-      </c>
-    </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B100" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C100" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D100" s="4">
+        <f t="shared" ref="D100:D105" si="9">D99+C100</f>
+        <v>5390</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B101" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C100" s="5">
+      <c r="C101" s="5">
         <v>6000</v>
       </c>
-      <c r="D100" s="4">
+      <c r="D101" s="4">
         <f t="shared" si="9"/>
         <v>11390</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B101" s="4" t="s">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B102" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C101" s="5">
+      <c r="C102" s="5">
         <v>-10000</v>
       </c>
-      <c r="D101" s="4">
+      <c r="D102" s="4">
         <f t="shared" si="9"/>
         <v>1390</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B102" s="4" t="s">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B103" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C102" s="5">
+      <c r="C103" s="5">
         <v>400</v>
       </c>
-      <c r="D102" s="4">
+      <c r="D103" s="4">
         <f t="shared" si="9"/>
         <v>1790</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="16" t="s">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="B103" s="4" t="s">
+      <c r="B104" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C103" s="5">
+      <c r="C104" s="5">
         <v>2000</v>
       </c>
-      <c r="D103" s="4">
+      <c r="D104" s="4">
         <f t="shared" si="9"/>
         <v>3790</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="16" t="s">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="B104" s="4" t="s">
+      <c r="B105" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C104" s="5">
+      <c r="C105" s="5">
         <v>6000</v>
       </c>
-      <c r="D104" s="4">
+      <c r="D105" s="4">
         <f t="shared" si="9"/>
         <v>9790</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="16" t="s">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="B105" s="4" t="s">
+      <c r="B106" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C105" s="5">
+      <c r="C106" s="5">
         <v>1000</v>
       </c>
-      <c r="D105" s="4">
-        <f t="shared" ref="D105:D110" si="10">D104+C105</f>
+      <c r="D106" s="4">
+        <f t="shared" ref="D106:D111" si="10">D105+C106</f>
         <v>10790</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B106" s="4" t="s">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B107" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C106" s="5">
+      <c r="C107" s="5">
         <v>-10000</v>
       </c>
-      <c r="D106" s="4">
+      <c r="D107" s="4">
         <f t="shared" si="10"/>
         <v>790</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="16" t="s">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="B107" s="4" t="s">
+      <c r="B108" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C107" s="5">
+      <c r="C108" s="5">
         <v>800</v>
       </c>
-      <c r="D107" s="4">
+      <c r="D108" s="4">
         <f t="shared" si="10"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="16" t="s">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="B108" s="4" t="s">
+      <c r="B109" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C108" s="5">
+      <c r="C109" s="5">
         <v>5000</v>
       </c>
-      <c r="D108" s="4">
+      <c r="D109" s="4">
         <f t="shared" si="10"/>
         <v>6590</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="16" t="s">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="B109" s="4" t="s">
+      <c r="B110" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C109" s="5">
+      <c r="C110" s="5">
         <v>6000</v>
       </c>
-      <c r="D109" s="4">
+      <c r="D110" s="4">
         <f t="shared" si="10"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B110" s="4" t="s">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B111" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C110" s="5">
+      <c r="C111" s="5">
         <v>-10000</v>
       </c>
-      <c r="D110" s="4">
+      <c r="D111" s="4">
         <f t="shared" si="10"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="16" t="s">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="B111" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C111" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D111" s="4">
-        <f t="shared" ref="D111:D117" si="11">D110+C111</f>
-        <v>4590</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B112" s="4" t="s">
         <v>65</v>
       </c>
@@ -2735,926 +2738,926 @@
         <v>2000</v>
       </c>
       <c r="D112" s="4">
+        <f t="shared" ref="D112:D118" si="11">D111+C112</f>
+        <v>4590</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B113" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C113" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D113" s="4">
         <f t="shared" si="11"/>
         <v>6590</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B113" s="4" t="s">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B114" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C113" s="5">
+      <c r="C114" s="5">
         <v>7000</v>
       </c>
-      <c r="D113" s="4">
+      <c r="D114" s="4">
         <f t="shared" si="11"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B114" s="4" t="s">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B115" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C114" s="5">
+      <c r="C115" s="5">
         <v>-10000</v>
       </c>
-      <c r="D114" s="4">
+      <c r="D115" s="4">
         <f t="shared" si="11"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="16" t="s">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="B115" s="4" t="s">
+      <c r="B116" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C115" s="5">
+      <c r="C116" s="5">
         <v>2000</v>
       </c>
-      <c r="D115" s="4">
+      <c r="D116" s="4">
         <f t="shared" si="11"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="16" t="s">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="B116" s="4" t="s">
+      <c r="B117" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C116" s="5">
+      <c r="C117" s="5">
         <v>6000</v>
       </c>
-      <c r="D116" s="4">
+      <c r="D117" s="4">
         <f t="shared" si="11"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B117" s="4" t="s">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B118" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C117" s="5">
+      <c r="C118" s="5">
         <v>-10000</v>
       </c>
-      <c r="D117" s="4">
+      <c r="D118" s="4">
         <f t="shared" si="11"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="B118" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C118" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D118" s="4">
-        <f t="shared" ref="D118:D123" si="12">D117+C118</f>
-        <v>3590</v>
-      </c>
-    </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B119" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C119" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D119" s="4">
+        <f t="shared" ref="D119:D124" si="12">D118+C119</f>
+        <v>3590</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="B119" s="4" t="s">
+      <c r="B120" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C119" s="5">
+      <c r="C120" s="5">
         <v>7000</v>
       </c>
-      <c r="D119" s="4">
+      <c r="D120" s="4">
         <f t="shared" si="12"/>
         <v>10590</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B120" s="4" t="s">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B121" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C120" s="5">
+      <c r="C121" s="5">
         <v>-10000</v>
       </c>
-      <c r="D120" s="4">
+      <c r="D121" s="4">
         <f t="shared" si="12"/>
         <v>590</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B121" s="4" t="s">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B122" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C121" s="5">
+      <c r="C122" s="5">
         <v>12000</v>
       </c>
-      <c r="D121" s="4">
+      <c r="D122" s="4">
         <f t="shared" si="12"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B122" s="4" t="s">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B123" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C122" s="5">
+      <c r="C123" s="5">
         <v>-10000</v>
       </c>
-      <c r="D122" s="4">
+      <c r="D123" s="4">
         <f t="shared" si="12"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B123" s="4" t="s">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B124" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C123" s="5">
+      <c r="C124" s="5">
         <v>2000</v>
       </c>
-      <c r="D123" s="4">
+      <c r="D124" s="4">
         <f t="shared" si="12"/>
         <v>4590</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="B124" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C124" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D124" s="4">
-        <f t="shared" ref="D124:D129" si="13">D123+C124</f>
-        <v>6590</v>
-      </c>
-    </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="B125" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C125" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D125" s="4">
+        <f t="shared" ref="D125:D130" si="13">D124+C125</f>
+        <v>6590</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="B125" s="4" t="s">
+      <c r="B126" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C125" s="5">
+      <c r="C126" s="5">
         <v>7000</v>
       </c>
-      <c r="D125" s="4">
+      <c r="D126" s="4">
         <f t="shared" si="13"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B126" s="4" t="s">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B127" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C126" s="5">
+      <c r="C127" s="5">
         <v>-10000</v>
       </c>
-      <c r="D126" s="4">
+      <c r="D127" s="4">
         <f t="shared" si="13"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="16" t="s">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="B127" s="4" t="s">
+      <c r="B128" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C127" s="5">
+      <c r="C128" s="5">
         <v>2000</v>
       </c>
-      <c r="D127" s="4">
+      <c r="D128" s="4">
         <f t="shared" si="13"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="16" t="s">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="B128" s="4" t="s">
+      <c r="B129" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C128" s="5">
+      <c r="C129" s="5">
         <v>8000</v>
       </c>
-      <c r="D128" s="4">
+      <c r="D129" s="4">
         <f t="shared" si="13"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B129" s="4" t="s">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B130" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C129" s="5">
+      <c r="C130" s="5">
         <v>-10000</v>
       </c>
-      <c r="D129" s="4">
+      <c r="D130" s="4">
         <f t="shared" si="13"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="16" t="s">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="B130" s="4" t="s">
+      <c r="B131" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C130" s="5">
+      <c r="C131" s="5">
         <v>2000</v>
       </c>
-      <c r="D130" s="4">
-        <f t="shared" ref="D130:D135" si="14">D129+C130</f>
+      <c r="D131" s="4">
+        <f t="shared" ref="D131:D136" si="14">D130+C131</f>
         <v>5590</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B131" s="4" t="s">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B132" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C131" s="5">
+      <c r="C132" s="5">
         <v>5000</v>
       </c>
-      <c r="D131" s="4">
+      <c r="D132" s="4">
         <f t="shared" si="14"/>
         <v>10590</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B132" s="4" t="s">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B133" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C132" s="5">
+      <c r="C133" s="5">
         <v>-10000</v>
       </c>
-      <c r="D132" s="4">
+      <c r="D133" s="4">
         <f t="shared" si="14"/>
         <v>590</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B133" s="4" t="s">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B134" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C133" s="5">
+      <c r="C134" s="5">
         <v>2000</v>
       </c>
-      <c r="D133" s="4">
+      <c r="D134" s="4">
         <f t="shared" si="14"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B134" s="4" t="s">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B135" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C134" s="5">
+      <c r="C135" s="5">
         <v>9000</v>
       </c>
-      <c r="D134" s="4">
+      <c r="D135" s="4">
         <f t="shared" si="14"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B135" s="4" t="s">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B136" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C135" s="5">
+      <c r="C136" s="5">
         <v>-10000</v>
       </c>
-      <c r="D135" s="4">
+      <c r="D136" s="4">
         <f t="shared" si="14"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B136" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C136" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D136" s="4">
-        <f t="shared" ref="D136:D141" si="15">D135+C136</f>
-        <v>3590</v>
-      </c>
-    </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B137" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C137" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D137" s="4">
+        <f t="shared" ref="D137:D142" si="15">D136+C137</f>
+        <v>3590</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="B137" s="4" t="s">
+      <c r="B138" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C137" s="5">
+      <c r="C138" s="5">
         <v>8000</v>
       </c>
-      <c r="D137" s="4">
+      <c r="D138" s="4">
         <f t="shared" si="15"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B138" s="4" t="s">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B139" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C138" s="5">
+      <c r="C139" s="5">
         <v>-10000</v>
       </c>
-      <c r="D138" s="4">
+      <c r="D139" s="4">
         <f t="shared" si="15"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="16" t="s">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="B139" s="4" t="s">
+      <c r="B140" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C139" s="5">
+      <c r="C140" s="5">
         <v>2000</v>
       </c>
-      <c r="D139" s="4">
+      <c r="D140" s="4">
         <f t="shared" si="15"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="16" t="s">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="B140" s="4" t="s">
+      <c r="B141" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C140" s="5">
+      <c r="C141" s="5">
         <v>12000</v>
       </c>
-      <c r="D140" s="4">
+      <c r="D141" s="4">
         <f t="shared" si="15"/>
         <v>15590</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B141" s="4" t="s">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B142" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C141" s="5">
+      <c r="C142" s="5">
         <v>-10000</v>
       </c>
-      <c r="D141" s="4">
+      <c r="D142" s="4">
         <f t="shared" si="15"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="B142" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="C142" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D142" s="4">
-        <f t="shared" ref="D142:D147" si="16">D141+C142</f>
-        <v>7590</v>
-      </c>
-    </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="B143" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C143" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D143" s="4">
+        <f t="shared" ref="D143:D148" si="16">D142+C143</f>
+        <v>7590</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="B143" s="4" t="s">
+      <c r="B144" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="C143" s="5">
+      <c r="C144" s="5">
         <v>10000</v>
       </c>
-      <c r="D143" s="4">
+      <c r="D144" s="4">
         <f t="shared" si="16"/>
         <v>17590</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B144" s="4" t="s">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B145" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C144" s="5">
+      <c r="C145" s="5">
         <v>-10000</v>
       </c>
-      <c r="D144" s="4">
+      <c r="D145" s="4">
         <f t="shared" si="16"/>
         <v>7590</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B145" s="4" t="s">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B146" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="C145" s="5">
+      <c r="C146" s="5">
         <v>2000</v>
       </c>
-      <c r="D145" s="4">
+      <c r="D146" s="4">
         <f t="shared" si="16"/>
         <v>9590</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="16" t="s">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="B146" s="4" t="s">
+      <c r="B147" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="C146" s="5">
+      <c r="C147" s="5">
         <v>-1200</v>
       </c>
-      <c r="D146" s="4">
+      <c r="D147" s="4">
         <f t="shared" si="16"/>
         <v>8390</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B147" s="4" t="s">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B148" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="C147" s="5">
+      <c r="C148" s="5">
         <v>500</v>
       </c>
-      <c r="D147" s="4">
+      <c r="D148" s="4">
         <f t="shared" si="16"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="16" t="s">
-        <v>165</v>
-      </c>
-      <c r="B148" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="C148" s="5">
-        <v>750</v>
-      </c>
-      <c r="D148" s="4">
-        <f t="shared" ref="D148:D153" si="17">D147+C148</f>
-        <v>9640</v>
-      </c>
-    </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="B149" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C149" s="5">
+        <v>750</v>
+      </c>
+      <c r="D149" s="4">
+        <f t="shared" ref="D149:D154" si="17">D148+C149</f>
+        <v>9640</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="B149" s="4" t="s">
+      <c r="B150" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C149" s="5">
+      <c r="C150" s="5">
         <v>2000</v>
       </c>
-      <c r="D149" s="4">
+      <c r="D150" s="4">
         <f t="shared" si="17"/>
         <v>11640</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B150" s="4" t="s">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B151" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C150" s="5">
+      <c r="C151" s="5">
         <v>2000</v>
       </c>
-      <c r="D150" s="4">
+      <c r="D151" s="4">
         <f t="shared" si="17"/>
         <v>13640</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B151" s="4" t="s">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B152" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C151" s="5">
+      <c r="C152" s="5">
         <v>-10000</v>
       </c>
-      <c r="D151" s="4">
+      <c r="D152" s="4">
         <f t="shared" si="17"/>
         <v>3640</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B152" s="4" t="s">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B153" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="C152" s="5">
+      <c r="C153" s="5">
         <v>350</v>
       </c>
-      <c r="D152" s="4">
+      <c r="D153" s="4">
         <f t="shared" si="17"/>
         <v>3990</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" s="16" t="s">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="B153" s="4" t="s">
+      <c r="B154" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="C153" s="5">
+      <c r="C154" s="5">
         <v>300</v>
       </c>
-      <c r="D153" s="4">
+      <c r="D154" s="4">
         <f t="shared" si="17"/>
         <v>4290</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="16" t="s">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="B154" s="4" t="s">
+      <c r="B155" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="C154" s="5">
+      <c r="C155" s="5">
         <v>3800</v>
       </c>
-      <c r="D154" s="4">
-        <f t="shared" ref="D154:D160" si="18">D153+C154</f>
+      <c r="D155" s="4">
+        <f t="shared" ref="D155:D161" si="18">D154+C155</f>
         <v>8090</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B155" s="4" t="s">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B156" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C155" s="5">
+      <c r="C156" s="5">
         <v>500</v>
       </c>
-      <c r="D155" s="4">
+      <c r="D156" s="4">
         <f t="shared" si="18"/>
         <v>8590</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="16" t="s">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="B156" s="4" t="s">
+      <c r="B157" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="C156" s="5">
+      <c r="C157" s="5">
         <v>1300</v>
       </c>
-      <c r="D156" s="4">
+      <c r="D157" s="4">
         <f t="shared" si="18"/>
         <v>9890</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="16" t="s">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="B157" s="4" t="s">
+      <c r="B158" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C157" s="5">
+      <c r="C158" s="5">
         <v>9000</v>
       </c>
-      <c r="D157" s="4">
+      <c r="D158" s="4">
         <f t="shared" si="18"/>
         <v>18890</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B158" s="4" t="s">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B159" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C158" s="5">
+      <c r="C159" s="5">
         <v>-10000</v>
       </c>
-      <c r="D158" s="4">
+      <c r="D159" s="4">
         <f t="shared" si="18"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="16" t="s">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="B159" s="4" t="s">
+      <c r="B160" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C159" s="5">
+      <c r="C160" s="5">
         <v>2000</v>
       </c>
-      <c r="D159" s="4">
+      <c r="D160" s="4">
         <f t="shared" si="18"/>
         <v>10890</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B160" s="4" t="s">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B161" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C160" s="5">
+      <c r="C161" s="5">
         <v>-10000</v>
       </c>
-      <c r="D160" s="4">
+      <c r="D161" s="4">
         <f t="shared" si="18"/>
         <v>890</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="B161" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="C161" s="5">
-        <v>500</v>
-      </c>
-      <c r="D161" s="4">
-        <f t="shared" ref="D161:D166" si="19">D160+C161</f>
-        <v>1390</v>
-      </c>
-    </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="B162" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C162" s="5">
+        <v>500</v>
+      </c>
+      <c r="D162" s="4">
+        <f t="shared" ref="D162:D167" si="19">D161+C162</f>
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="B162" s="4" t="s">
+      <c r="B163" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="C162" s="5">
+      <c r="C163" s="5">
         <v>10000</v>
       </c>
-      <c r="D162" s="4">
+      <c r="D163" s="4">
         <f t="shared" si="19"/>
         <v>11390</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B163" s="4" t="s">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B164" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C163" s="5">
+      <c r="C164" s="5">
         <v>-10000</v>
       </c>
-      <c r="D163" s="4">
+      <c r="D164" s="4">
         <f t="shared" si="19"/>
         <v>1390</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164" s="16" t="s">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="B164" s="4" t="s">
+      <c r="B165" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C164" s="5">
+      <c r="C165" s="5">
         <v>3000</v>
       </c>
-      <c r="D164" s="4">
+      <c r="D165" s="4">
         <f t="shared" si="19"/>
         <v>4390</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" s="16" t="s">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="B165" s="4" t="s">
+      <c r="B166" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C165" s="5">
+      <c r="C166" s="5">
         <v>2000</v>
       </c>
-      <c r="D165" s="4">
+      <c r="D166" s="4">
         <f t="shared" si="19"/>
         <v>6390</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B166" s="4" t="s">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B167" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C166" s="5">
+      <c r="C167" s="5">
         <v>2000</v>
       </c>
-      <c r="D166" s="4">
+      <c r="D167" s="4">
         <f t="shared" si="19"/>
         <v>8390</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A167" s="16" t="s">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="B167" s="4" t="s">
+      <c r="B168" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C167" s="5">
+      <c r="C168" s="5">
         <v>11000</v>
       </c>
-      <c r="D167" s="4">
-        <f t="shared" ref="D167:D172" si="20">D166+C167</f>
+      <c r="D168" s="4">
+        <f t="shared" ref="D168:D173" si="20">D167+C168</f>
         <v>19390</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B168" s="4" t="s">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B169" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C168" s="5">
+      <c r="C169" s="5">
         <v>-10000</v>
       </c>
-      <c r="D168" s="4">
+      <c r="D169" s="4">
         <f t="shared" si="20"/>
         <v>9390</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A169" s="16" t="s">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" s="16" t="s">
         <v>187</v>
       </c>
-      <c r="B169" s="4" t="s">
+      <c r="B170" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C169" s="5">
+      <c r="C170" s="5">
         <v>3000</v>
       </c>
-      <c r="D169" s="4">
+      <c r="D170" s="4">
         <f t="shared" si="20"/>
         <v>12390</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B170" s="4" t="s">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B171" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C170" s="5">
+      <c r="C171" s="5">
         <v>-10000</v>
       </c>
-      <c r="D170" s="4">
+      <c r="D171" s="4">
         <f t="shared" si="20"/>
         <v>2390</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B171" s="4" t="s">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B172" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C171" s="5">
+      <c r="C172" s="5">
         <v>500</v>
       </c>
-      <c r="D171" s="4">
+      <c r="D172" s="4">
         <f t="shared" si="20"/>
         <v>2890</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A172" s="16" t="s">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" s="16" t="s">
         <v>189</v>
       </c>
-      <c r="B172" s="4" t="s">
+      <c r="B173" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C172" s="5">
+      <c r="C173" s="5">
         <v>5600</v>
       </c>
-      <c r="D172" s="4">
+      <c r="D173" s="4">
         <f t="shared" si="20"/>
         <v>8490</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B173" s="4" t="s">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B174" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="C173" s="5">
+      <c r="C174" s="5">
         <v>4700</v>
       </c>
-      <c r="D173" s="4">
-        <f t="shared" ref="D173:D179" si="21">D172+C173</f>
+      <c r="D174" s="4">
+        <f t="shared" ref="D174:D180" si="21">D173+C174</f>
         <v>13190</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174" s="16" t="s">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175" s="16" t="s">
         <v>192</v>
       </c>
-      <c r="B174" s="4" t="s">
+      <c r="B175" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C174" s="5">
+      <c r="C175" s="5">
         <v>1500</v>
       </c>
-      <c r="D174" s="4">
+      <c r="D175" s="4">
         <f t="shared" si="21"/>
         <v>14690</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B175" s="4" t="s">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B176" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C175" s="5">
+      <c r="C176" s="5">
         <v>500</v>
       </c>
-      <c r="D175" s="4">
+      <c r="D176" s="4">
         <f t="shared" si="21"/>
         <v>15190</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176" s="16" t="s">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="B176" s="4" t="s">
+      <c r="B177" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="C176" s="5">
+      <c r="C177" s="5">
         <v>1000</v>
       </c>
-      <c r="D176" s="4">
+      <c r="D177" s="4">
         <f t="shared" si="21"/>
         <v>16190</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A177" s="16" t="s">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A178" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="B177" s="4" t="s">
+      <c r="B178" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="C177" s="5">
+      <c r="C178" s="5">
         <v>1000</v>
       </c>
-      <c r="D177" s="4">
+      <c r="D178" s="4">
         <f t="shared" si="21"/>
         <v>17190</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A178" s="16" t="s">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A179" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="B178" s="4" t="s">
+      <c r="B179" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C178" s="5">
+      <c r="C179" s="5">
         <v>3000</v>
       </c>
-      <c r="D178" s="4">
+      <c r="D179" s="4">
         <f t="shared" si="21"/>
         <v>20190</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B179" s="4" t="s">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B180" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C179" s="5">
+      <c r="C180" s="5">
         <v>-20000</v>
       </c>
-      <c r="D179" s="4">
+      <c r="D180" s="4">
         <f t="shared" si="21"/>
         <v>190</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B180" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C180" s="5">
-        <v>500</v>
-      </c>
-      <c r="D180" s="4">
-        <f t="shared" ref="D180:D186" si="22">D179+C180</f>
-        <v>690</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -3665,425 +3668,464 @@
         <v>500</v>
       </c>
       <c r="D181" s="4">
+        <f t="shared" ref="D181:D187" si="22">D180+C181</f>
+        <v>690</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B182" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C182" s="5">
+        <v>500</v>
+      </c>
+      <c r="D182" s="4">
         <f t="shared" si="22"/>
         <v>1190</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" s="16" t="s">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A183" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="B182" s="4" t="s">
+      <c r="B183" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="C182" s="5">
+      <c r="C183" s="5">
         <v>10000</v>
       </c>
-      <c r="D182" s="4">
+      <c r="D183" s="4">
         <f t="shared" si="22"/>
         <v>11190</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B183" s="4" t="s">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B184" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C183" s="5">
+      <c r="C184" s="5">
         <v>-10000</v>
       </c>
-      <c r="D183" s="4">
+      <c r="D184" s="4">
         <f t="shared" si="22"/>
         <v>1190</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" s="16" t="s">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A185" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="B184" s="4" t="s">
+      <c r="B185" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C184" s="5">
+      <c r="C185" s="5">
         <v>3000</v>
       </c>
-      <c r="D184" s="4">
+      <c r="D185" s="4">
         <f t="shared" si="22"/>
         <v>4190</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A185" s="16" t="s">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="B185" s="4" t="s">
+      <c r="B186" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C185" s="5">
+      <c r="C186" s="5">
         <v>11000</v>
       </c>
-      <c r="D185" s="4">
+      <c r="D186" s="4">
         <f t="shared" si="22"/>
         <v>15190</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B186" s="4" t="s">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B187" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C186" s="5">
+      <c r="C187" s="5">
         <v>-10000</v>
       </c>
-      <c r="D186" s="4">
+      <c r="D187" s="4">
         <f t="shared" si="22"/>
         <v>5190</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A187" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="B187" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C187" s="5">
-        <v>3000</v>
-      </c>
-      <c r="D187" s="4">
-        <f t="shared" ref="D187:D193" si="23">D186+C187</f>
-        <v>8190</v>
-      </c>
-    </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="B188" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C188" s="5">
+        <v>3000</v>
+      </c>
+      <c r="D188" s="4">
+        <f t="shared" ref="D188:D194" si="23">D187+C188</f>
+        <v>8190</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="B188" s="4" t="s">
+      <c r="B189" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="C188" s="5">
+      <c r="C189" s="5">
         <v>14000</v>
       </c>
-      <c r="D188" s="4">
+      <c r="D189" s="4">
         <f t="shared" si="23"/>
         <v>22190</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B189" s="4" t="s">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B190" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="C189" s="5">
+      <c r="C190" s="5">
         <v>-20000</v>
       </c>
-      <c r="D189" s="4">
+      <c r="D190" s="4">
         <f t="shared" si="23"/>
         <v>2190</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A190" s="16" t="s">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A191" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="B190" s="4" t="s">
+      <c r="B191" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="C190" s="5">
+      <c r="C191" s="5">
         <v>5000</v>
       </c>
-      <c r="D190" s="4">
+      <c r="D191" s="4">
         <f t="shared" si="23"/>
         <v>7190</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A191" s="16" t="s">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A192" s="16" t="s">
         <v>213</v>
       </c>
-      <c r="B191" s="4" t="s">
+      <c r="B192" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="C191" s="5">
+      <c r="C192" s="5">
         <v>5000</v>
       </c>
-      <c r="D191" s="4">
+      <c r="D192" s="4">
         <f t="shared" si="23"/>
         <v>12190</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A192" s="16" t="s">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A193" s="16" t="s">
         <v>215</v>
       </c>
-      <c r="B192" s="4" t="s">
+      <c r="B193" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C192" s="5">
+      <c r="C193" s="5">
         <v>11000</v>
       </c>
-      <c r="D192" s="4">
+      <c r="D193" s="4">
         <f t="shared" si="23"/>
         <v>23190</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B193" s="4" t="s">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B194" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C193" s="5">
+      <c r="C194" s="5">
         <v>-20000</v>
       </c>
-      <c r="D193" s="4">
+      <c r="D194" s="4">
         <f t="shared" si="23"/>
         <v>3190</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194" s="16" t="s">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A195" s="16" t="s">
         <v>216</v>
       </c>
-      <c r="B194" s="4" t="s">
+      <c r="B195" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C194" s="5">
+      <c r="C195" s="5">
         <v>500</v>
       </c>
-      <c r="D194" s="4">
-        <f t="shared" ref="D194:D199" si="24">D193+C194</f>
+      <c r="D195" s="4">
+        <f t="shared" ref="D195:D200" si="24">D194+C195</f>
         <v>3690</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B195" s="4" t="s">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B196" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C195" s="5">
+      <c r="C196" s="5">
         <v>3000</v>
       </c>
-      <c r="D195" s="4">
+      <c r="D196" s="4">
         <f t="shared" si="24"/>
         <v>6690</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A196" s="16" t="s">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A197" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="B196" s="4" t="s">
+      <c r="B197" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="C196" s="5">
+      <c r="C197" s="5">
         <v>12000</v>
       </c>
-      <c r="D196" s="4">
+      <c r="D197" s="4">
         <f t="shared" si="24"/>
         <v>18690</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B197" s="4" t="s">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B198" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C197" s="5">
+      <c r="C198" s="5">
         <v>-10000</v>
       </c>
-      <c r="D197" s="4">
+      <c r="D198" s="4">
         <f t="shared" si="24"/>
         <v>8690</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A198" s="16" t="s">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A199" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="B198" s="4" t="s">
+      <c r="B199" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="C198" s="5">
+      <c r="C199" s="5">
         <v>5000</v>
       </c>
-      <c r="D198" s="4">
+      <c r="D199" s="4">
         <f t="shared" si="24"/>
         <v>13690</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B199" s="4" t="s">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B200" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C199" s="5">
+      <c r="C200" s="5">
         <v>-10000</v>
       </c>
-      <c r="D199" s="4">
+      <c r="D200" s="4">
         <f t="shared" si="24"/>
         <v>3690</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A200" s="16" t="s">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A201" s="16" t="s">
         <v>221</v>
       </c>
-      <c r="B200" s="4" t="s">
+      <c r="B201" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="C200" s="5">
+      <c r="C201" s="5">
         <v>12000</v>
       </c>
-      <c r="D200" s="4">
-        <f t="shared" ref="D200:D205" si="25">D199+C200</f>
+      <c r="D201" s="4">
+        <f t="shared" ref="D201:D206" si="25">D200+C201</f>
         <v>15690</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B201" s="4" t="s">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B202" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C201" s="5">
+      <c r="C202" s="5">
         <v>-10000</v>
       </c>
-      <c r="D201" s="4">
+      <c r="D202" s="4">
         <f t="shared" si="25"/>
         <v>5690</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A202" s="16" t="s">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A203" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="B202" s="4" t="s">
+      <c r="B203" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C202" s="5">
+      <c r="C203" s="5">
         <v>2000</v>
       </c>
-      <c r="D202" s="4">
+      <c r="D203" s="4">
         <f t="shared" si="25"/>
         <v>7690</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A203" s="16" t="s">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A204" s="16" t="s">
         <v>227</v>
       </c>
-      <c r="B203" s="4" t="s">
+      <c r="B204" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="C203" s="5">
+      <c r="C204" s="5">
         <v>1000</v>
       </c>
-      <c r="D203" s="4">
+      <c r="D204" s="4">
         <f t="shared" si="25"/>
         <v>8690</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A204" s="16" t="s">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A205" s="16" t="s">
         <v>229</v>
       </c>
-      <c r="B204" s="4" t="s">
+      <c r="B205" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="C204" s="5">
+      <c r="C205" s="5">
         <v>5000</v>
       </c>
-      <c r="D204" s="4">
+      <c r="D205" s="4">
         <f t="shared" si="25"/>
         <v>13690</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B205" s="4" t="s">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B206" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C205" s="5">
+      <c r="C206" s="5">
         <v>-10000</v>
       </c>
-      <c r="D205" s="4">
+      <c r="D206" s="4">
         <f t="shared" si="25"/>
         <v>3690</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A206" s="16" t="s">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A207" s="16" t="s">
         <v>231</v>
       </c>
-      <c r="B206" s="4" t="s">
+      <c r="B207" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="C206" s="5">
+      <c r="C207" s="5">
         <v>13000</v>
       </c>
-      <c r="D206" s="4">
-        <f>D205+C206</f>
+      <c r="D207" s="4">
+        <f t="shared" ref="D207:D212" si="26">D206+C207</f>
         <v>16690</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B207" s="4" t="s">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B208" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C207" s="5">
+      <c r="C208" s="5">
         <v>-10000</v>
       </c>
-      <c r="D207" s="4">
-        <f>D206+C207</f>
+      <c r="D208" s="4">
+        <f t="shared" si="26"/>
         <v>6690</v>
-      </c>
-    </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A208" s="16" t="s">
-        <v>233</v>
-      </c>
-      <c r="B208" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C208" s="5">
-        <v>3000</v>
-      </c>
-      <c r="D208" s="4">
-        <f>D207+C208</f>
-        <v>9690</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="B209" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C209" s="5">
+        <v>3000</v>
+      </c>
+      <c r="D209" s="4">
+        <f t="shared" si="26"/>
+        <v>9690</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A210" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="B209" s="4" t="s">
+      <c r="B210" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="C209" s="5">
+      <c r="C210" s="5">
         <v>13000</v>
       </c>
-      <c r="D209" s="4">
-        <f>D208+C209</f>
+      <c r="D210" s="4">
+        <f t="shared" si="26"/>
         <v>22690</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B210" s="4" t="s">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B211" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C210" s="5">
+      <c r="C211" s="5">
         <v>-20000</v>
       </c>
-      <c r="D210" s="4">
-        <f>D209+C210</f>
+      <c r="D211" s="4">
+        <f t="shared" si="26"/>
         <v>2690</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A211" s="16" t="s">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A212" s="16" t="s">
         <v>235</v>
       </c>
-      <c r="B211" s="4" t="s">
+      <c r="B212" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C211" s="5">
+      <c r="C212" s="5">
         <v>3000</v>
       </c>
-      <c r="D211" s="4">
-        <f>D210+C211</f>
+      <c r="D212" s="4">
+        <f t="shared" si="26"/>
         <v>5690</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A213" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="B213" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="C213" s="5">
+        <v>16000</v>
+      </c>
+      <c r="D213" s="4">
+        <f>D212+C213</f>
+        <v>21690</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B214" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="C214" s="5">
+        <v>-20000</v>
+      </c>
+      <c r="D214" s="4">
+        <f>D213+C214</f>
+        <v>1690</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chi diem tra 300k
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="CÔ DIỄM" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="241">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -736,6 +736,12 @@
   </si>
   <si>
     <t xml:space="preserve">Châu </t>
+  </si>
+  <si>
+    <t>07/11/2024</t>
+  </si>
+  <si>
+    <t>Chị Diễm chuyển 300k</t>
   </si>
 </sst>
 </file>
@@ -4675,7 +4681,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -4798,10 +4804,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C7"/>
+  <dimension ref="A2:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -4834,9 +4840,15 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="22"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="26"/>
+      <c r="A4" s="22" t="s">
+        <v>239</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="C4" s="26">
+        <v>300</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="22"/>
@@ -4849,15 +4861,25 @@
       <c r="C6" s="26"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="22" t="s">
-        <v>221</v>
-      </c>
-      <c r="B7" s="27" t="s">
+      <c r="A7" s="22"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="26"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="22"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="26"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="22" t="s">
+        <v>239</v>
+      </c>
+      <c r="B9" s="27" t="s">
         <v>224</v>
       </c>
-      <c r="C7" s="28">
-        <f>C2-SUM(C3:C6)</f>
-        <v>2500</v>
+      <c r="C9" s="28">
+        <f>C2-SUM(C3:C8)</f>
+        <v>2200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ha gui tra 500k
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CÔ DIỄM" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="241">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -1245,7 +1245,7 @@
   <dimension ref="A1:K215"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A197" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A188" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B239" sqref="B239"/>
     </sheetView>
   </sheetViews>
@@ -4302,11 +4302,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4530,6 +4530,21 @@
       <c r="D13" s="4">
         <f>D12+C13</f>
         <v>4000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>45603</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="5">
+        <v>-500</v>
+      </c>
+      <c r="D14" s="4">
+        <f>D13+C14</f>
+        <v>3500</v>
       </c>
     </row>
   </sheetData>
@@ -4806,7 +4821,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
kiem tra tong ket
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="CÔ DIỄM" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="244">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -733,9 +733,6 @@
   </si>
   <si>
     <t>02/11/2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Châu </t>
   </si>
   <si>
     <t>07/11/2024</t>
@@ -1256,7 +1253,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K219"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
     </sheetView>
@@ -1364,7 +1361,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H7" s="16" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I7" s="5">
         <v>10</v>
@@ -4141,7 +4138,7 @@
         <v>16000</v>
       </c>
       <c r="D214" s="4">
-        <f>D213+C214</f>
+        <f t="shared" ref="D214:D219" si="27">D213+C214</f>
         <v>21690</v>
       </c>
     </row>
@@ -4153,13 +4150,13 @@
         <v>-20000</v>
       </c>
       <c r="D215" s="4">
-        <f>D214+C215</f>
+        <f t="shared" si="27"/>
         <v>1690</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" s="16" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B216" s="4" t="s">
         <v>40</v>
@@ -4168,13 +4165,13 @@
         <v>2000</v>
       </c>
       <c r="D216" s="4">
-        <f>D215+C216</f>
+        <f t="shared" si="27"/>
         <v>3690</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" s="16" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B217" s="4" t="s">
         <v>228</v>
@@ -4183,22 +4180,22 @@
         <v>1000</v>
       </c>
       <c r="D217" s="4">
-        <f>D216+C217</f>
+        <f t="shared" si="27"/>
         <v>4690</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" s="16" t="s">
+        <v>242</v>
+      </c>
+      <c r="B218" s="4" t="s">
         <v>243</v>
-      </c>
-      <c r="B218" s="4" t="s">
-        <v>244</v>
       </c>
       <c r="C218" s="5">
         <v>6000</v>
       </c>
       <c r="D218" s="4">
-        <f>D217+C218</f>
+        <f t="shared" si="27"/>
         <v>10690</v>
       </c>
     </row>
@@ -4210,7 +4207,7 @@
         <v>-10000</v>
       </c>
       <c r="D219" s="4">
-        <f>D218+C219</f>
+        <f t="shared" si="27"/>
         <v>690</v>
       </c>
     </row>
@@ -4758,8 +4755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4775,7 +4772,7 @@
         <v>108</v>
       </c>
       <c r="B1">
-        <v>570000</v>
+        <v>470000</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -4807,7 +4804,7 @@
         <v>112</v>
       </c>
       <c r="B5">
-        <v>4000</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4856,21 +4853,13 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>238</v>
-      </c>
-      <c r="B11">
-        <v>10000</v>
-      </c>
-    </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>5</v>
       </c>
       <c r="B22">
         <f>SUM(B1:B19)</f>
-        <v>676380</v>
+        <v>565880</v>
       </c>
     </row>
   </sheetData>
@@ -4918,10 +4907,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
+        <v>238</v>
+      </c>
+      <c r="B4" s="25" t="s">
         <v>239</v>
-      </c>
-      <c r="B4" s="25" t="s">
-        <v>240</v>
       </c>
       <c r="C4" s="26">
         <v>300</v>
@@ -4949,7 +4938,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B9" s="27" t="s">
         <v>224</v>

</xml_diff>

<commit_message>
duy lay tien loi co diem ngay 21
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="CÔ DIỄM" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="245">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -751,6 +751,9 @@
   </si>
   <si>
     <t>Duy lấy 6tr tiền lời</t>
+  </si>
+  <si>
+    <t>21/11/2024</t>
   </si>
 </sst>
 </file>
@@ -1251,11 +1254,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K219"/>
+  <dimension ref="A1:K185"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A157" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1331,11 +1334,21 @@
         <v>20</v>
       </c>
       <c r="J3" s="4">
-        <f>SUM(I3:I72)</f>
-        <v>630</v>
+        <f>SUM(I3:I73)</f>
+        <v>640</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="5">
+        <v>14560</v>
+      </c>
+      <c r="D4" s="4">
+        <f>C4+D3</f>
+        <v>18490</v>
+      </c>
       <c r="H4" s="16" t="s">
         <v>168</v>
       </c>
@@ -1344,6 +1357,16 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D5" s="4">
+        <f t="shared" ref="D5:D9" si="0">D4+C5</f>
+        <v>8490</v>
+      </c>
       <c r="H5" s="16" t="s">
         <v>197</v>
       </c>
@@ -1352,6 +1375,16 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D6" s="4">
+        <f t="shared" si="0"/>
+        <v>10490</v>
+      </c>
       <c r="H6" s="16" t="s">
         <v>229</v>
       </c>
@@ -1360,6 +1393,16 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D7" s="4">
+        <f>D6+C7</f>
+        <v>490</v>
+      </c>
       <c r="H7" s="16" t="s">
         <v>242</v>
       </c>
@@ -1368,15 +1411,18 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>21</v>
+      </c>
       <c r="B8" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C8" s="5">
-        <v>14560</v>
+        <v>2000</v>
       </c>
       <c r="D8" s="4">
-        <f>C8+D3</f>
-        <v>18490</v>
+        <f t="shared" si="0"/>
+        <v>2490</v>
       </c>
       <c r="H8" s="16" t="s">
         <v>7</v>
@@ -1386,15 +1432,18 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>22</v>
+      </c>
       <c r="B9" s="4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C9" s="5">
-        <v>-10000</v>
+        <v>3000</v>
       </c>
       <c r="D9" s="4">
-        <f t="shared" ref="D9:D26" si="0">D8+C9</f>
-        <v>8490</v>
+        <f t="shared" si="0"/>
+        <v>5490</v>
       </c>
       <c r="H9" s="16" t="s">
         <v>8</v>
@@ -1404,15 +1453,18 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>24</v>
+      </c>
       <c r="B10" s="4" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C10" s="5">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="D10" s="4">
-        <f t="shared" si="0"/>
-        <v>10490</v>
+        <f>D9+C10</f>
+        <v>8490</v>
       </c>
       <c r="H10" s="16" t="s">
         <v>9</v>
@@ -1422,6 +1474,16 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="5">
+        <v>4400</v>
+      </c>
+      <c r="D11" s="4">
+        <f>D10+C11</f>
+        <v>12890</v>
+      </c>
       <c r="H11" s="16" t="s">
         <v>41</v>
       </c>
@@ -1430,6 +1492,16 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D12" s="4">
+        <f>D11+C12</f>
+        <v>2890</v>
+      </c>
       <c r="H12" s="16" t="s">
         <v>84</v>
       </c>
@@ -1439,6 +1511,16 @@
       <c r="K12" s="14"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="5">
+        <v>1600</v>
+      </c>
+      <c r="D13" s="4">
+        <f t="shared" ref="D13:D20" si="1">D12+C13</f>
+        <v>4490</v>
+      </c>
       <c r="H13" s="16" t="s">
         <v>96</v>
       </c>
@@ -1448,6 +1530,16 @@
       <c r="K13" s="14"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="5">
+        <v>3000</v>
+      </c>
+      <c r="D14" s="4">
+        <f t="shared" si="1"/>
+        <v>7490</v>
+      </c>
       <c r="H14" s="16" t="s">
         <v>127</v>
       </c>
@@ -1457,6 +1549,19 @@
       <c r="K14" s="14"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D15" s="4">
+        <f t="shared" si="1"/>
+        <v>9490</v>
+      </c>
       <c r="H15" s="16" t="s">
         <v>133</v>
       </c>
@@ -1466,6 +1571,19 @@
       <c r="K15" s="14"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="5">
+        <v>3000</v>
+      </c>
+      <c r="D16" s="4">
+        <f t="shared" si="1"/>
+        <v>12490</v>
+      </c>
       <c r="H16" s="16" t="s">
         <v>142</v>
       </c>
@@ -1475,6 +1593,16 @@
       <c r="K16" s="14"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D17" s="4">
+        <f t="shared" si="1"/>
+        <v>2490</v>
+      </c>
       <c r="H17" s="16" t="s">
         <v>177</v>
       </c>
@@ -1484,6 +1612,19 @@
       <c r="K17" s="14"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="5">
+        <v>4960</v>
+      </c>
+      <c r="D18" s="4">
+        <f t="shared" si="1"/>
+        <v>7450</v>
+      </c>
       <c r="H18" s="16" t="s">
         <v>200</v>
       </c>
@@ -1493,6 +1634,19 @@
       <c r="K18" s="14"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="5">
+        <v>4000</v>
+      </c>
+      <c r="D19" s="4">
+        <f t="shared" si="1"/>
+        <v>11450</v>
+      </c>
       <c r="H19" s="16" t="s">
         <v>215</v>
       </c>
@@ -1502,6 +1656,16 @@
       <c r="K19" s="14"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D20" s="4">
+        <f t="shared" si="1"/>
+        <v>1450</v>
+      </c>
       <c r="H20" s="16" t="s">
         <v>231</v>
       </c>
@@ -1511,26 +1675,56 @@
       <c r="K20" s="14"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="5">
+        <v>7640</v>
+      </c>
+      <c r="D21" s="4">
+        <f t="shared" ref="D21:D26" si="2">D20+C21</f>
+        <v>9090</v>
+      </c>
       <c r="H21" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="I21" s="5">
+        <v>10</v>
+      </c>
+      <c r="K21" s="14"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="5">
+        <v>3000</v>
+      </c>
+      <c r="D22" s="4">
+        <f>D21+C22</f>
+        <v>12090</v>
+      </c>
+      <c r="H22" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="I21" s="5">
-        <v>10</v>
-      </c>
-      <c r="K21" s="14"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H22" s="16" t="s">
+      <c r="I22" s="5">
+        <v>10</v>
+      </c>
+      <c r="K22" s="14"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D23" s="4">
+        <f t="shared" si="2"/>
+        <v>2090</v>
+      </c>
+      <c r="H23" s="16" t="s">
         <v>107</v>
-      </c>
-      <c r="I22" s="5">
-        <v>10</v>
-      </c>
-      <c r="K22" s="14"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H23" s="16" t="s">
-        <v>178</v>
       </c>
       <c r="I23" s="5">
         <v>10</v>
@@ -1539,17 +1733,17 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="C24" s="5">
-        <v>-10000</v>
+        <v>800</v>
       </c>
       <c r="D24" s="4">
-        <f>D10+C24</f>
-        <v>490</v>
+        <f t="shared" si="2"/>
+        <v>2890</v>
       </c>
       <c r="H24" s="16" t="s">
-        <v>10</v>
+        <v>178</v>
       </c>
       <c r="I24" s="5">
         <v>10</v>
@@ -1558,20 +1752,20 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="C25" s="5">
         <v>2000</v>
       </c>
       <c r="D25" s="4">
-        <f t="shared" si="0"/>
-        <v>2490</v>
+        <f t="shared" si="2"/>
+        <v>4890</v>
       </c>
       <c r="H25" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I25" s="5">
         <v>10</v>
@@ -1580,186 +1774,365 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="C26" s="5">
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="D26" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
+        <v>8890</v>
+      </c>
+      <c r="H26" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="I26" s="5">
+        <v>10</v>
+      </c>
+      <c r="K26" s="14"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" s="5">
+        <v>4000</v>
+      </c>
+      <c r="D27" s="4">
+        <f t="shared" ref="D27:D32" si="3">D26+C27</f>
+        <v>12890</v>
+      </c>
+      <c r="H27" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="I27" s="5">
+        <v>10</v>
+      </c>
+      <c r="K27" s="14"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="5">
+        <v>5000</v>
+      </c>
+      <c r="D28" s="4">
+        <f t="shared" si="3"/>
+        <v>17890</v>
+      </c>
+      <c r="H28" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="I28" s="5">
+        <v>10</v>
+      </c>
+      <c r="K28" s="14"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D29" s="4">
+        <f t="shared" si="3"/>
+        <v>7890</v>
+      </c>
+      <c r="H29" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="I29" s="5">
+        <v>10</v>
+      </c>
+      <c r="K29" s="14"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="16">
+        <v>44969</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="5">
+        <v>900</v>
+      </c>
+      <c r="D30" s="4">
+        <f t="shared" si="3"/>
+        <v>8790</v>
+      </c>
+      <c r="H30" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="I30" s="5">
+        <v>10</v>
+      </c>
+      <c r="K30" s="14"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" s="5">
+        <v>4000</v>
+      </c>
+      <c r="D31" s="4">
+        <f t="shared" si="3"/>
+        <v>12790</v>
+      </c>
+      <c r="H31" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="I31" s="5">
+        <v>10</v>
+      </c>
+      <c r="K31" s="14"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D32" s="4">
+        <f t="shared" si="3"/>
+        <v>2790</v>
+      </c>
+      <c r="H32" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="I32" s="5">
+        <v>10</v>
+      </c>
+      <c r="K32" s="14"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D33" s="4">
+        <f t="shared" ref="D33:D40" si="4">D32+C33</f>
+        <v>4790</v>
+      </c>
+      <c r="H33" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="I33" s="5">
+        <v>10</v>
+      </c>
+      <c r="K33" s="14"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" s="5">
+        <v>700</v>
+      </c>
+      <c r="D34" s="4">
+        <f t="shared" si="4"/>
         <v>5490</v>
       </c>
-      <c r="H26" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="I26" s="5">
-        <v>10</v>
-      </c>
-      <c r="K26" s="14"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H27" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="I27" s="5">
-        <v>10</v>
-      </c>
-      <c r="K27" s="14"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H28" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="I28" s="5">
-        <v>10</v>
-      </c>
-      <c r="K28" s="14"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H29" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="I29" s="5">
-        <v>10</v>
-      </c>
-      <c r="K29" s="14"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H30" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="I30" s="5">
-        <v>10</v>
-      </c>
-      <c r="K30" s="14"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H31" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="I31" s="5">
-        <v>10</v>
-      </c>
-      <c r="K31" s="14"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H32" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="I32" s="5">
-        <v>10</v>
-      </c>
-      <c r="K32" s="14"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H33" s="16" t="s">
+      <c r="H34" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="I33" s="5">
-        <v>10</v>
-      </c>
-      <c r="K33" s="14"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H34" s="16" t="s">
+      <c r="I34" s="5">
+        <v>10</v>
+      </c>
+      <c r="K34" s="14"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B35" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" s="5">
+        <v>4000</v>
+      </c>
+      <c r="D35" s="4">
+        <f t="shared" si="4"/>
+        <v>9490</v>
+      </c>
+      <c r="H35" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="I34" s="5">
-        <v>10</v>
-      </c>
-      <c r="K34" s="14"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H35" s="16" t="s">
+      <c r="I35" s="5">
+        <v>10</v>
+      </c>
+      <c r="K35" s="14"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C36" s="5">
+        <v>600</v>
+      </c>
+      <c r="D36" s="4">
+        <f t="shared" si="4"/>
+        <v>10090</v>
+      </c>
+      <c r="H36" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="I35" s="5">
-        <v>10</v>
-      </c>
-      <c r="K35" s="14"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H36" s="16" t="s">
+      <c r="I36" s="5">
+        <v>10</v>
+      </c>
+      <c r="K36" s="14"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B37" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D37" s="4">
+        <f t="shared" si="4"/>
+        <v>90</v>
+      </c>
+      <c r="H37" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="I36" s="5">
-        <v>10</v>
-      </c>
-      <c r="K36" s="14"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H37" s="16" t="s">
-        <v>234</v>
-      </c>
       <c r="I37" s="5">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K37" s="14"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="C38" s="5">
-        <v>3000</v>
+        <f>700+5000+300+600+400+1000+800</f>
+        <v>8800</v>
       </c>
       <c r="D38" s="4">
-        <f>D26+C38</f>
-        <v>8490</v>
+        <f t="shared" si="4"/>
+        <v>8890</v>
       </c>
       <c r="H38" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="I38" s="5">
+        <v>20</v>
+      </c>
+      <c r="K38" s="14"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B39" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C39" s="5">
+        <v>6000</v>
+      </c>
+      <c r="D39" s="4">
+        <f t="shared" si="4"/>
+        <v>14890</v>
+      </c>
+      <c r="H39" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I38" s="5">
-        <v>10</v>
-      </c>
-      <c r="K38" s="14"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H39" s="16" t="s">
+      <c r="I39" s="5">
+        <v>10</v>
+      </c>
+      <c r="K39" s="14"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D40" s="4">
+        <f t="shared" si="4"/>
+        <v>4890</v>
+      </c>
+      <c r="H40" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="I39" s="5">
-        <v>10</v>
-      </c>
-      <c r="K39" s="14"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H40" s="16" t="s">
+      <c r="I40" s="5">
+        <v>10</v>
+      </c>
+      <c r="K40" s="14"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C41" s="5">
+        <v>500</v>
+      </c>
+      <c r="D41" s="4">
+        <f t="shared" ref="D41:D46" si="5">D40+C41</f>
+        <v>5390</v>
+      </c>
+      <c r="H41" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="I40" s="5">
-        <v>10</v>
-      </c>
-      <c r="K40" s="14"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H41" s="16" t="s">
+      <c r="I41" s="5">
+        <v>10</v>
+      </c>
+      <c r="K41" s="14"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B42" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C42" s="5">
+        <v>700</v>
+      </c>
+      <c r="D42" s="4">
+        <f t="shared" si="5"/>
+        <v>6090</v>
+      </c>
+      <c r="H42" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="I41" s="5">
-        <v>10</v>
-      </c>
-      <c r="K41" s="14"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H42" s="16" t="s">
+      <c r="I42" s="5">
+        <v>10</v>
+      </c>
+      <c r="K42" s="14"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B43" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" s="5">
+        <v>1500</v>
+      </c>
+      <c r="D43" s="4">
+        <f t="shared" si="5"/>
+        <v>7590</v>
+      </c>
+      <c r="H43" s="16" t="s">
         <v>156</v>
-      </c>
-      <c r="I42" s="5">
-        <v>10</v>
-      </c>
-      <c r="K42" s="14"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H43" s="16" t="s">
-        <v>219</v>
       </c>
       <c r="I43" s="5">
         <v>10</v>
@@ -1768,55 +2141,58 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="C44" s="5">
-        <v>4400</v>
+        <v>5000</v>
       </c>
       <c r="D44" s="4">
-        <f>D38+C44</f>
-        <v>12890</v>
+        <f t="shared" si="5"/>
+        <v>12590</v>
       </c>
       <c r="H44" s="16" t="s">
-        <v>157</v>
+        <v>219</v>
       </c>
       <c r="I44" s="5">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K44" s="14"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C45" s="5">
         <v>-10000</v>
       </c>
       <c r="D45" s="4">
-        <f>D44+C45</f>
-        <v>2890</v>
+        <f t="shared" si="5"/>
+        <v>2590</v>
       </c>
       <c r="H45" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="I45" s="5">
+        <v>20</v>
+      </c>
+      <c r="K45" s="14"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C46" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D46" s="4">
+        <f t="shared" si="5"/>
+        <v>4590</v>
+      </c>
+      <c r="H46" s="16" t="s">
         <v>158</v>
-      </c>
-      <c r="I45" s="5">
-        <v>10</v>
-      </c>
-      <c r="K45" s="14"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B46" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C46" s="5">
-        <v>1600</v>
-      </c>
-      <c r="D46" s="4">
-        <f t="shared" ref="D46:D53" si="1">D45+C46</f>
-        <v>4490</v>
-      </c>
-      <c r="H46" s="16" t="s">
-        <v>159</v>
       </c>
       <c r="I46" s="5">
         <v>10</v>
@@ -1825,17 +2201,17 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B47" s="4" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="C47" s="5">
-        <v>3000</v>
+        <v>700</v>
       </c>
       <c r="D47" s="4">
-        <f t="shared" si="1"/>
-        <v>7490</v>
+        <f t="shared" ref="D47:D52" si="6">D46+C47</f>
+        <v>5290</v>
       </c>
       <c r="H47" s="16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I47" s="5">
         <v>10</v>
@@ -1844,20 +2220,20 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="16" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="C48" s="5">
-        <v>2000</v>
+        <v>700</v>
       </c>
       <c r="D48" s="4">
-        <f t="shared" si="1"/>
-        <v>9490</v>
+        <f t="shared" si="6"/>
+        <v>5990</v>
       </c>
       <c r="H48" s="16" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="I48" s="5">
         <v>10</v>
@@ -1866,61 +2242,61 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="16" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="C49" s="5">
-        <v>3000</v>
+        <v>700</v>
       </c>
       <c r="D49" s="4">
-        <f t="shared" si="1"/>
-        <v>12490</v>
+        <f t="shared" si="6"/>
+        <v>6690</v>
       </c>
       <c r="H49" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="I49" s="5">
+        <v>10</v>
+      </c>
+      <c r="K49" s="14"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C50" s="5">
+        <v>4000</v>
+      </c>
+      <c r="D50" s="4">
+        <f t="shared" si="6"/>
+        <v>10690</v>
+      </c>
+      <c r="H50" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="I49" s="5">
-        <v>10</v>
-      </c>
-      <c r="K49" s="14"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B50" s="4" t="s">
+      <c r="I50" s="5">
+        <v>10</v>
+      </c>
+      <c r="K50" s="14"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B51" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C50" s="5">
+      <c r="C51" s="5">
         <v>-10000</v>
       </c>
-      <c r="D50" s="4">
-        <f t="shared" si="1"/>
-        <v>2490</v>
-      </c>
-      <c r="H50" s="16" t="s">
+      <c r="D51" s="4">
+        <f t="shared" si="6"/>
+        <v>690</v>
+      </c>
+      <c r="H51" s="16" t="s">
         <v>152</v>
-      </c>
-      <c r="I50" s="5">
-        <v>10</v>
-      </c>
-      <c r="K50" s="14"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C51" s="5">
-        <v>4960</v>
-      </c>
-      <c r="D51" s="4">
-        <f t="shared" si="1"/>
-        <v>7450</v>
-      </c>
-      <c r="H51" s="16" t="s">
-        <v>151</v>
       </c>
       <c r="I51" s="5">
         <v>10</v>
@@ -1929,39 +2305,42 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="16" t="s">
-        <v>43</v>
+        <v>86</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>44</v>
+        <v>87</v>
       </c>
       <c r="C52" s="5">
-        <v>4000</v>
+        <v>1000</v>
       </c>
       <c r="D52" s="4">
-        <f t="shared" si="1"/>
-        <v>11450</v>
+        <f t="shared" si="6"/>
+        <v>1690</v>
       </c>
       <c r="H52" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="I52" s="5">
+        <v>10</v>
+      </c>
+      <c r="K52" s="14"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C53" s="5">
+        <v>7000</v>
+      </c>
+      <c r="D53" s="4">
+        <f t="shared" ref="D53:D58" si="7">D52+C53</f>
+        <v>8690</v>
+      </c>
+      <c r="H53" s="16" t="s">
         <v>150</v>
-      </c>
-      <c r="I52" s="5">
-        <v>10</v>
-      </c>
-      <c r="K52" s="14"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B53" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C53" s="5">
-        <v>-10000</v>
-      </c>
-      <c r="D53" s="4">
-        <f t="shared" si="1"/>
-        <v>1450</v>
-      </c>
-      <c r="H53" s="16" t="s">
-        <v>149</v>
       </c>
       <c r="I53" s="5">
         <v>10</v>
@@ -1970,44 +2349,74 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B54" s="4" t="s">
-        <v>51</v>
+        <v>90</v>
       </c>
       <c r="C54" s="5">
-        <v>7640</v>
+        <v>10000</v>
       </c>
       <c r="D54" s="4">
-        <f t="shared" ref="D54:D62" si="2">D53+C54</f>
-        <v>9090</v>
+        <f t="shared" si="7"/>
+        <v>18690</v>
       </c>
       <c r="H54" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="I54" s="5">
+        <v>10</v>
+      </c>
+      <c r="K54" s="14"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B55" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C55" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D55" s="4">
+        <f t="shared" si="7"/>
+        <v>8690</v>
+      </c>
+      <c r="H55" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="I54" s="5">
-        <v>10</v>
-      </c>
-      <c r="K54" s="14"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H55" s="16" t="s">
+      <c r="I55" s="5">
+        <v>10</v>
+      </c>
+      <c r="K55" s="14"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B56" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C56" s="5">
+        <v>1700</v>
+      </c>
+      <c r="D56" s="4">
+        <f t="shared" si="7"/>
+        <v>10390</v>
+      </c>
+      <c r="H56" s="16" t="s">
         <v>221</v>
       </c>
-      <c r="I55" s="5">
-        <v>10</v>
-      </c>
-      <c r="K55" s="14"/>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H56" s="16" t="s">
+      <c r="I56" s="5">
+        <v>10</v>
+      </c>
+      <c r="K56" s="14"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B57" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C57" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D57" s="4">
+        <f t="shared" si="7"/>
+        <v>390</v>
+      </c>
+      <c r="H57" s="16" t="s">
         <v>237</v>
-      </c>
-      <c r="I56" s="5">
-        <v>20</v>
-      </c>
-      <c r="K56" s="14"/>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H57" s="16" t="s">
-        <v>207</v>
       </c>
       <c r="I57" s="5">
         <v>20</v>
@@ -2016,157 +2425,161 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B58" s="4" t="s">
-        <v>28</v>
+        <v>93</v>
       </c>
       <c r="C58" s="5">
-        <v>3000</v>
+        <v>6000</v>
       </c>
       <c r="D58" s="4">
-        <f>D54+C58</f>
-        <v>12090</v>
+        <f t="shared" si="7"/>
+        <v>6390</v>
       </c>
       <c r="H58" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="I58" s="5">
+        <v>20</v>
+      </c>
+      <c r="K58" s="14"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C59" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D59" s="4">
+        <f t="shared" ref="D59:D64" si="8">D58+C59</f>
+        <v>8390</v>
+      </c>
+      <c r="H59" s="16" t="s">
         <v>187</v>
       </c>
-      <c r="I58" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B59" s="4" t="s">
+      <c r="I59" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C60" s="5">
+        <v>5000</v>
+      </c>
+      <c r="D60" s="4">
+        <f t="shared" si="8"/>
+        <v>13390</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B61" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C59" s="5">
+      <c r="C61" s="5">
         <v>-10000</v>
       </c>
-      <c r="D59" s="4">
-        <f t="shared" si="2"/>
-        <v>2090</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B60" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C60" s="5">
-        <v>800</v>
-      </c>
-      <c r="D60" s="4">
-        <f t="shared" si="2"/>
-        <v>2890</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C61" s="5">
-        <v>2000</v>
-      </c>
       <c r="D61" s="4">
-        <f t="shared" si="2"/>
-        <v>4890</v>
+        <f t="shared" si="8"/>
+        <v>3390</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="16" t="s">
-        <v>57</v>
+        <v>98</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>58</v>
+        <v>99</v>
       </c>
       <c r="C62" s="5">
-        <v>4000</v>
+        <v>1000</v>
       </c>
       <c r="D62" s="4">
-        <f t="shared" si="2"/>
-        <v>8890</v>
+        <f t="shared" si="8"/>
+        <v>4390</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" s="16" t="s">
-        <v>59</v>
-      </c>
       <c r="B63" s="4" t="s">
-        <v>61</v>
+        <v>100</v>
       </c>
       <c r="C63" s="5">
-        <v>4000</v>
+        <v>9000</v>
       </c>
       <c r="D63" s="4">
-        <f t="shared" ref="D63:D68" si="3">D62+C63</f>
-        <v>12890</v>
+        <f t="shared" si="8"/>
+        <v>13390</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B64" s="4" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="C64" s="5">
-        <v>5000</v>
+        <v>-10000</v>
       </c>
       <c r="D64" s="4">
-        <f t="shared" si="3"/>
-        <v>17890</v>
+        <f t="shared" si="8"/>
+        <v>3390</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B65" s="4" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
       <c r="C65" s="5">
-        <v>-10000</v>
+        <v>2000</v>
       </c>
       <c r="D65" s="4">
-        <f t="shared" si="3"/>
-        <v>7890</v>
+        <f t="shared" ref="D65:D70" si="9">D64+C65</f>
+        <v>5390</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="16">
-        <v>44969</v>
-      </c>
       <c r="B66" s="4" t="s">
-        <v>62</v>
+        <v>102</v>
       </c>
       <c r="C66" s="5">
-        <v>900</v>
+        <v>6000</v>
       </c>
       <c r="D66" s="4">
-        <f t="shared" si="3"/>
-        <v>8790</v>
+        <f t="shared" si="9"/>
+        <v>11390</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B67" s="4" t="s">
-        <v>63</v>
+        <v>20</v>
       </c>
       <c r="C67" s="5">
-        <v>4000</v>
+        <v>-10000</v>
       </c>
       <c r="D67" s="4">
-        <f t="shared" si="3"/>
-        <v>12790</v>
+        <f t="shared" si="9"/>
+        <v>1390</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B68" s="4" t="s">
-        <v>20</v>
+        <v>103</v>
       </c>
       <c r="C68" s="5">
-        <v>-10000</v>
+        <v>400</v>
       </c>
       <c r="D68" s="4">
-        <f t="shared" si="3"/>
-        <v>2790</v>
+        <f t="shared" si="9"/>
+        <v>1790</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="16" t="s">
-        <v>64</v>
+        <v>104</v>
       </c>
       <c r="B69" s="4" t="s">
         <v>65</v>
@@ -2175,90 +2588,95 @@
         <v>2000</v>
       </c>
       <c r="D69" s="4">
-        <f t="shared" ref="D69:D76" si="4">D68+C69</f>
-        <v>4790</v>
+        <f t="shared" si="9"/>
+        <v>3790</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="16" t="s">
-        <v>66</v>
+        <v>105</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="C70" s="5">
-        <v>700</v>
+        <v>6000</v>
       </c>
       <c r="D70" s="4">
-        <f t="shared" si="4"/>
-        <v>5490</v>
+        <f t="shared" si="9"/>
+        <v>9790</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="16" t="s">
+        <v>106</v>
+      </c>
       <c r="B71" s="4" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="C71" s="5">
-        <v>4000</v>
+        <v>1000</v>
       </c>
       <c r="D71" s="4">
-        <f t="shared" si="4"/>
-        <v>9490</v>
+        <f t="shared" ref="D71:D76" si="10">D70+C71</f>
+        <v>10790</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="16" t="s">
-        <v>68</v>
-      </c>
       <c r="B72" s="4" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="C72" s="5">
-        <v>600</v>
+        <v>-10000</v>
       </c>
       <c r="D72" s="4">
-        <f t="shared" si="4"/>
-        <v>10090</v>
+        <f t="shared" si="10"/>
+        <v>790</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="16" t="s">
+        <v>115</v>
+      </c>
       <c r="B73" s="4" t="s">
-        <v>20</v>
+        <v>116</v>
       </c>
       <c r="C73" s="5">
-        <v>-10000</v>
+        <v>800</v>
       </c>
       <c r="D73" s="4">
-        <f t="shared" si="4"/>
-        <v>90</v>
+        <f t="shared" si="10"/>
+        <v>1590</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="16" t="s">
-        <v>71</v>
+        <v>117</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>74</v>
+        <v>118</v>
       </c>
       <c r="C74" s="5">
-        <f>700+5000+300+600+400+1000+800</f>
-        <v>8800</v>
+        <v>5000</v>
       </c>
       <c r="D74" s="4">
-        <f t="shared" si="4"/>
-        <v>8890</v>
+        <f t="shared" si="10"/>
+        <v>6590</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="16" t="s">
+        <v>119</v>
+      </c>
       <c r="B75" s="4" t="s">
-        <v>72</v>
+        <v>102</v>
       </c>
       <c r="C75" s="5">
         <v>6000</v>
       </c>
       <c r="D75" s="4">
-        <f t="shared" si="4"/>
-        <v>14890</v>
+        <f t="shared" si="10"/>
+        <v>12590</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -2269,379 +2687,385 @@
         <v>-10000</v>
       </c>
       <c r="D76" s="4">
-        <f t="shared" si="4"/>
-        <v>4890</v>
+        <f t="shared" si="10"/>
+        <v>2590</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="16" t="s">
-        <v>75</v>
+        <v>122</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="C77" s="5">
-        <v>500</v>
+        <v>2000</v>
       </c>
       <c r="D77" s="4">
-        <f t="shared" ref="D77:D82" si="5">D76+C77</f>
-        <v>5390</v>
+        <f t="shared" ref="D77:D83" si="11">D76+C77</f>
+        <v>4590</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B78" s="4" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C78" s="5">
-        <v>700</v>
+        <v>2000</v>
       </c>
       <c r="D78" s="4">
-        <f t="shared" si="5"/>
-        <v>6090</v>
+        <f t="shared" si="11"/>
+        <v>6590</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B79" s="4" t="s">
-        <v>78</v>
+        <v>124</v>
       </c>
       <c r="C79" s="5">
-        <v>1500</v>
+        <v>7000</v>
       </c>
       <c r="D79" s="4">
-        <f t="shared" si="5"/>
-        <v>7590</v>
+        <f t="shared" si="11"/>
+        <v>13590</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B80" s="4" t="s">
-        <v>79</v>
+        <v>20</v>
       </c>
       <c r="C80" s="5">
-        <v>5000</v>
+        <v>-10000</v>
       </c>
       <c r="D80" s="4">
-        <f t="shared" si="5"/>
-        <v>12590</v>
+        <f t="shared" si="11"/>
+        <v>3590</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="16" t="s">
+        <v>126</v>
+      </c>
       <c r="B81" s="4" t="s">
-        <v>20</v>
+        <v>65</v>
       </c>
       <c r="C81" s="5">
-        <v>-10000</v>
+        <v>2000</v>
       </c>
       <c r="D81" s="4">
-        <f t="shared" si="5"/>
-        <v>2590</v>
+        <f t="shared" si="11"/>
+        <v>5590</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="16" t="s">
-        <v>81</v>
+        <v>127</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>65</v>
+        <v>102</v>
       </c>
       <c r="C82" s="5">
-        <v>2000</v>
+        <v>6000</v>
       </c>
       <c r="D82" s="4">
-        <f t="shared" si="5"/>
-        <v>4590</v>
+        <f t="shared" si="11"/>
+        <v>11590</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B83" s="4" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="C83" s="5">
-        <v>700</v>
+        <v>-10000</v>
       </c>
       <c r="D83" s="4">
-        <f t="shared" ref="D83:D88" si="6">D82+C83</f>
-        <v>5290</v>
+        <f t="shared" si="11"/>
+        <v>1590</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="16" t="s">
-        <v>82</v>
+        <v>128</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C84" s="5">
-        <v>700</v>
+        <v>2000</v>
       </c>
       <c r="D84" s="4">
-        <f t="shared" si="6"/>
-        <v>5990</v>
+        <f t="shared" ref="D84:D89" si="12">D83+C84</f>
+        <v>3590</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="16" t="s">
-        <v>83</v>
+        <v>129</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>77</v>
+        <v>124</v>
       </c>
       <c r="C85" s="5">
-        <v>700</v>
+        <v>7000</v>
       </c>
       <c r="D85" s="4">
-        <f t="shared" si="6"/>
-        <v>6690</v>
+        <f t="shared" si="12"/>
+        <v>10590</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="16" t="s">
-        <v>84</v>
-      </c>
       <c r="B86" s="4" t="s">
-        <v>85</v>
+        <v>20</v>
       </c>
       <c r="C86" s="5">
-        <v>4000</v>
+        <v>-10000</v>
       </c>
       <c r="D86" s="4">
-        <f t="shared" si="6"/>
-        <v>10690</v>
+        <f t="shared" si="12"/>
+        <v>590</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B87" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C87" s="5">
+        <v>12000</v>
+      </c>
+      <c r="D87" s="4">
+        <f t="shared" si="12"/>
+        <v>12590</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B88" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C87" s="5">
+      <c r="C88" s="5">
         <v>-10000</v>
       </c>
-      <c r="D87" s="4">
-        <f t="shared" si="6"/>
-        <v>690</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="B88" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C88" s="5">
-        <v>1000</v>
-      </c>
       <c r="D88" s="4">
-        <f t="shared" si="6"/>
-        <v>1690</v>
+        <f t="shared" si="12"/>
+        <v>2590</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="16" t="s">
-        <v>88</v>
-      </c>
       <c r="B89" s="4" t="s">
-        <v>89</v>
+        <v>131</v>
       </c>
       <c r="C89" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D89" s="4">
+        <f t="shared" si="12"/>
+        <v>4590</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C90" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D90" s="4">
+        <f t="shared" ref="D90:D95" si="13">D89+C90</f>
+        <v>6590</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C91" s="5">
         <v>7000</v>
       </c>
-      <c r="D89" s="4">
-        <f t="shared" ref="D89:D94" si="7">D88+C89</f>
-        <v>8690</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B90" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C90" s="5">
-        <v>10000</v>
-      </c>
-      <c r="D90" s="4">
-        <f t="shared" si="7"/>
-        <v>18690</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B91" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C91" s="5">
-        <v>-10000</v>
-      </c>
       <c r="D91" s="4">
-        <f t="shared" si="7"/>
-        <v>8690</v>
+        <f t="shared" si="13"/>
+        <v>13590</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B92" s="4" t="s">
-        <v>92</v>
+        <v>20</v>
       </c>
       <c r="C92" s="5">
-        <v>1700</v>
+        <v>-10000</v>
       </c>
       <c r="D92" s="4">
-        <f t="shared" si="7"/>
-        <v>10390</v>
+        <f t="shared" si="13"/>
+        <v>3590</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="16" t="s">
+        <v>134</v>
+      </c>
       <c r="B93" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C93" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D93" s="4">
+        <f t="shared" si="13"/>
+        <v>5590</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C94" s="5">
+        <v>8000</v>
+      </c>
+      <c r="D94" s="4">
+        <f t="shared" si="13"/>
+        <v>13590</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B95" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C93" s="5">
+      <c r="C95" s="5">
         <v>-10000</v>
       </c>
-      <c r="D93" s="4">
-        <f t="shared" si="7"/>
-        <v>390</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B94" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C94" s="5">
-        <v>6000</v>
-      </c>
-      <c r="D94" s="4">
-        <f t="shared" si="7"/>
-        <v>6390</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="B95" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C95" s="5">
-        <v>2000</v>
-      </c>
       <c r="D95" s="4">
-        <f t="shared" ref="D95:D100" si="8">D94+C95</f>
-        <v>8390</v>
+        <f t="shared" si="13"/>
+        <v>3590</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="16" t="s">
-        <v>96</v>
+        <v>137</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="C96" s="5">
-        <v>5000</v>
+        <v>2000</v>
       </c>
       <c r="D96" s="4">
-        <f t="shared" si="8"/>
-        <v>13390</v>
+        <f t="shared" ref="D96:D101" si="14">D95+C96</f>
+        <v>5590</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B97" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C97" s="5">
+        <v>5000</v>
+      </c>
+      <c r="D97" s="4">
+        <f t="shared" si="14"/>
+        <v>10590</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B98" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C97" s="5">
+      <c r="C98" s="5">
         <v>-10000</v>
       </c>
-      <c r="D97" s="4">
-        <f t="shared" si="8"/>
-        <v>3390</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="B98" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C98" s="5">
-        <v>1000</v>
-      </c>
       <c r="D98" s="4">
-        <f t="shared" si="8"/>
-        <v>4390</v>
+        <f t="shared" si="14"/>
+        <v>590</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B99" s="4" t="s">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="C99" s="5">
-        <v>9000</v>
+        <v>2000</v>
       </c>
       <c r="D99" s="4">
-        <f t="shared" si="8"/>
-        <v>13390</v>
+        <f t="shared" si="14"/>
+        <v>2590</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B100" s="4" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="C100" s="5">
-        <v>-10000</v>
+        <v>9000</v>
       </c>
       <c r="D100" s="4">
-        <f t="shared" si="8"/>
-        <v>3390</v>
+        <f t="shared" si="14"/>
+        <v>11590</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B101" s="4" t="s">
-        <v>101</v>
+        <v>20</v>
       </c>
       <c r="C101" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D101" s="4">
+        <f t="shared" si="14"/>
+        <v>1590</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C102" s="5">
         <v>2000</v>
       </c>
-      <c r="D101" s="4">
-        <f t="shared" ref="D101:D106" si="9">D100+C101</f>
-        <v>5390</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B102" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C102" s="5">
-        <v>6000</v>
-      </c>
       <c r="D102" s="4">
-        <f t="shared" si="9"/>
-        <v>11390</v>
+        <f t="shared" ref="D102:D107" si="15">D101+C102</f>
+        <v>3590</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="16" t="s">
+        <v>142</v>
+      </c>
       <c r="B103" s="4" t="s">
-        <v>20</v>
+        <v>136</v>
       </c>
       <c r="C103" s="5">
-        <v>-10000</v>
+        <v>8000</v>
       </c>
       <c r="D103" s="4">
-        <f t="shared" si="9"/>
-        <v>1390</v>
+        <f t="shared" si="15"/>
+        <v>11590</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B104" s="4" t="s">
-        <v>103</v>
+        <v>20</v>
       </c>
       <c r="C104" s="5">
-        <v>400</v>
+        <v>-10000</v>
       </c>
       <c r="D104" s="4">
-        <f t="shared" si="9"/>
-        <v>1790</v>
+        <f t="shared" si="15"/>
+        <v>1590</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="16" t="s">
-        <v>104</v>
+        <v>143</v>
       </c>
       <c r="B105" s="4" t="s">
         <v>65</v>
@@ -2650,254 +3074,254 @@
         <v>2000</v>
       </c>
       <c r="D105" s="4">
-        <f t="shared" si="9"/>
-        <v>3790</v>
+        <f t="shared" si="15"/>
+        <v>3590</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="16" t="s">
-        <v>105</v>
+        <v>144</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>102</v>
+        <v>145</v>
       </c>
       <c r="C106" s="5">
-        <v>6000</v>
+        <v>12000</v>
       </c>
       <c r="D106" s="4">
-        <f t="shared" si="9"/>
-        <v>9790</v>
+        <f t="shared" si="15"/>
+        <v>15590</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="16" t="s">
-        <v>106</v>
-      </c>
       <c r="B107" s="4" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="C107" s="5">
-        <v>1000</v>
+        <v>-10000</v>
       </c>
       <c r="D107" s="4">
-        <f t="shared" ref="D107:D112" si="10">D106+C107</f>
-        <v>10790</v>
+        <f t="shared" si="15"/>
+        <v>5590</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="16" t="s">
+        <v>161</v>
+      </c>
       <c r="B108" s="4" t="s">
-        <v>20</v>
+        <v>146</v>
       </c>
       <c r="C108" s="5">
-        <v>-10000</v>
+        <v>2000</v>
       </c>
       <c r="D108" s="4">
-        <f t="shared" si="10"/>
-        <v>790</v>
+        <f t="shared" ref="D108:D113" si="16">D107+C108</f>
+        <v>7590</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="16" t="s">
-        <v>115</v>
+        <v>149</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>116</v>
+        <v>147</v>
       </c>
       <c r="C109" s="5">
-        <v>800</v>
+        <v>10000</v>
       </c>
       <c r="D109" s="4">
-        <f t="shared" si="10"/>
-        <v>1590</v>
+        <f t="shared" si="16"/>
+        <v>17590</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="16" t="s">
-        <v>117</v>
-      </c>
       <c r="B110" s="4" t="s">
-        <v>118</v>
+        <v>20</v>
       </c>
       <c r="C110" s="5">
-        <v>5000</v>
+        <v>-10000</v>
       </c>
       <c r="D110" s="4">
-        <f t="shared" si="10"/>
-        <v>6590</v>
+        <f t="shared" si="16"/>
+        <v>7590</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="16" t="s">
-        <v>119</v>
-      </c>
       <c r="B111" s="4" t="s">
-        <v>102</v>
+        <v>148</v>
       </c>
       <c r="C111" s="5">
-        <v>6000</v>
+        <v>2000</v>
       </c>
       <c r="D111" s="4">
-        <f t="shared" si="10"/>
-        <v>12590</v>
+        <f t="shared" si="16"/>
+        <v>9590</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="16" t="s">
+        <v>162</v>
+      </c>
       <c r="B112" s="4" t="s">
-        <v>20</v>
+        <v>163</v>
       </c>
       <c r="C112" s="5">
-        <v>-10000</v>
+        <v>-1200</v>
       </c>
       <c r="D112" s="4">
-        <f t="shared" si="10"/>
-        <v>2590</v>
+        <f t="shared" si="16"/>
+        <v>8390</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="16" t="s">
-        <v>122</v>
-      </c>
       <c r="B113" s="4" t="s">
-        <v>65</v>
+        <v>164</v>
       </c>
       <c r="C113" s="5">
+        <v>500</v>
+      </c>
+      <c r="D113" s="4">
+        <f t="shared" si="16"/>
+        <v>8890</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="B114" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C114" s="5">
+        <v>750</v>
+      </c>
+      <c r="D114" s="4">
+        <f t="shared" ref="D114:D119" si="17">D113+C114</f>
+        <v>9640</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="B115" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C115" s="5">
         <v>2000</v>
       </c>
-      <c r="D113" s="4">
-        <f t="shared" ref="D113:D119" si="11">D112+C113</f>
-        <v>4590</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B114" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C114" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D114" s="4">
-        <f t="shared" si="11"/>
-        <v>6590</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B115" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="C115" s="5">
-        <v>7000</v>
-      </c>
       <c r="D115" s="4">
-        <f t="shared" si="11"/>
-        <v>13590</v>
+        <f t="shared" si="17"/>
+        <v>11640</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B116" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C116" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D116" s="4">
+        <f t="shared" si="17"/>
+        <v>13640</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B117" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C116" s="5">
+      <c r="C117" s="5">
         <v>-10000</v>
       </c>
-      <c r="D116" s="4">
-        <f t="shared" si="11"/>
-        <v>3590</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="B117" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C117" s="5">
-        <v>2000</v>
-      </c>
       <c r="D117" s="4">
-        <f t="shared" si="11"/>
-        <v>5590</v>
+        <f t="shared" si="17"/>
+        <v>3640</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="16" t="s">
-        <v>127</v>
-      </c>
       <c r="B118" s="4" t="s">
-        <v>102</v>
+        <v>170</v>
       </c>
       <c r="C118" s="5">
-        <v>6000</v>
+        <v>350</v>
       </c>
       <c r="D118" s="4">
-        <f t="shared" si="11"/>
-        <v>11590</v>
+        <f t="shared" si="17"/>
+        <v>3990</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="16" t="s">
+        <v>171</v>
+      </c>
       <c r="B119" s="4" t="s">
-        <v>20</v>
+        <v>172</v>
       </c>
       <c r="C119" s="5">
-        <v>-10000</v>
+        <v>300</v>
       </c>
       <c r="D119" s="4">
-        <f t="shared" si="11"/>
-        <v>1590</v>
+        <f t="shared" si="17"/>
+        <v>4290</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="16" t="s">
-        <v>128</v>
+        <v>173</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>65</v>
+        <v>174</v>
       </c>
       <c r="C120" s="5">
-        <v>2000</v>
+        <v>3800</v>
       </c>
       <c r="D120" s="4">
-        <f t="shared" ref="D120:D125" si="12">D119+C120</f>
-        <v>3590</v>
+        <f t="shared" ref="D120:D126" si="18">D119+C120</f>
+        <v>8090</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="16" t="s">
-        <v>129</v>
-      </c>
       <c r="B121" s="4" t="s">
-        <v>124</v>
+        <v>76</v>
       </c>
       <c r="C121" s="5">
-        <v>7000</v>
+        <v>500</v>
       </c>
       <c r="D121" s="4">
-        <f t="shared" si="12"/>
-        <v>10590</v>
+        <f t="shared" si="18"/>
+        <v>8590</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="16" t="s">
+        <v>175</v>
+      </c>
       <c r="B122" s="4" t="s">
-        <v>20</v>
+        <v>176</v>
       </c>
       <c r="C122" s="5">
-        <v>-10000</v>
+        <v>1300</v>
       </c>
       <c r="D122" s="4">
-        <f t="shared" si="12"/>
-        <v>590</v>
+        <f t="shared" si="18"/>
+        <v>9890</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="16" t="s">
+        <v>177</v>
+      </c>
       <c r="B123" s="4" t="s">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="C123" s="5">
-        <v>12000</v>
+        <v>9000</v>
       </c>
       <c r="D123" s="4">
-        <f t="shared" si="12"/>
-        <v>12590</v>
+        <f t="shared" si="18"/>
+        <v>18890</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -2908,131 +3332,134 @@
         <v>-10000</v>
       </c>
       <c r="D124" s="4">
-        <f t="shared" si="12"/>
-        <v>2590</v>
+        <f t="shared" si="18"/>
+        <v>8890</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="16" t="s">
+        <v>178</v>
+      </c>
       <c r="B125" s="4" t="s">
-        <v>131</v>
+        <v>65</v>
       </c>
       <c r="C125" s="5">
         <v>2000</v>
       </c>
       <c r="D125" s="4">
-        <f t="shared" si="12"/>
-        <v>4590</v>
+        <f t="shared" si="18"/>
+        <v>10890</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="16" t="s">
-        <v>132</v>
-      </c>
       <c r="B126" s="4" t="s">
-        <v>65</v>
+        <v>20</v>
       </c>
       <c r="C126" s="5">
-        <v>2000</v>
+        <v>-10000</v>
       </c>
       <c r="D126" s="4">
-        <f t="shared" ref="D126:D131" si="13">D125+C126</f>
-        <v>6590</v>
+        <f t="shared" si="18"/>
+        <v>890</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="16" t="s">
-        <v>133</v>
+        <v>179</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>124</v>
+        <v>180</v>
       </c>
       <c r="C127" s="5">
-        <v>7000</v>
+        <v>500</v>
       </c>
       <c r="D127" s="4">
-        <f t="shared" si="13"/>
-        <v>13590</v>
+        <f t="shared" ref="D127:D132" si="19">D126+C127</f>
+        <v>1390</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="16" t="s">
+        <v>181</v>
+      </c>
       <c r="B128" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C128" s="5">
+        <v>10000</v>
+      </c>
+      <c r="D128" s="4">
+        <f t="shared" si="19"/>
+        <v>11390</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B129" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C128" s="5">
+      <c r="C129" s="5">
         <v>-10000</v>
       </c>
-      <c r="D128" s="4">
-        <f t="shared" si="13"/>
-        <v>3590</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="B129" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C129" s="5">
-        <v>2000</v>
-      </c>
       <c r="D129" s="4">
-        <f t="shared" si="13"/>
-        <v>5590</v>
+        <f t="shared" si="19"/>
+        <v>1390</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="16" t="s">
-        <v>135</v>
+        <v>183</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>136</v>
+        <v>25</v>
       </c>
       <c r="C130" s="5">
-        <v>8000</v>
+        <v>3000</v>
       </c>
       <c r="D130" s="4">
-        <f t="shared" si="13"/>
-        <v>13590</v>
+        <f t="shared" si="19"/>
+        <v>4390</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="16" t="s">
+        <v>184</v>
+      </c>
       <c r="B131" s="4" t="s">
-        <v>20</v>
+        <v>65</v>
       </c>
       <c r="C131" s="5">
-        <v>-10000</v>
+        <v>2000</v>
       </c>
       <c r="D131" s="4">
-        <f t="shared" si="13"/>
-        <v>3590</v>
+        <f t="shared" si="19"/>
+        <v>6390</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="16" t="s">
-        <v>137</v>
-      </c>
       <c r="B132" s="4" t="s">
-        <v>65</v>
+        <v>131</v>
       </c>
       <c r="C132" s="5">
         <v>2000</v>
       </c>
       <c r="D132" s="4">
-        <f t="shared" ref="D132:D137" si="14">D131+C132</f>
-        <v>5590</v>
+        <f t="shared" si="19"/>
+        <v>8390</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="16" t="s">
+        <v>185</v>
+      </c>
       <c r="B133" s="4" t="s">
-        <v>138</v>
+        <v>186</v>
       </c>
       <c r="C133" s="5">
-        <v>5000</v>
+        <v>11000</v>
       </c>
       <c r="D133" s="4">
-        <f t="shared" si="14"/>
-        <v>10590</v>
+        <f t="shared" ref="D133:D138" si="20">D132+C133</f>
+        <v>19390</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -3043,1172 +3470,710 @@
         <v>-10000</v>
       </c>
       <c r="D134" s="4">
-        <f t="shared" si="14"/>
-        <v>590</v>
+        <f t="shared" si="20"/>
+        <v>9390</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" s="16" t="s">
+        <v>187</v>
+      </c>
       <c r="B135" s="4" t="s">
-        <v>65</v>
+        <v>188</v>
       </c>
       <c r="C135" s="5">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="D135" s="4">
-        <f t="shared" si="14"/>
-        <v>2590</v>
+        <f t="shared" si="20"/>
+        <v>12390</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B136" s="4" t="s">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="C136" s="5">
-        <v>9000</v>
+        <v>-10000</v>
       </c>
       <c r="D136" s="4">
-        <f t="shared" si="14"/>
-        <v>11590</v>
+        <f t="shared" si="20"/>
+        <v>2390</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B137" s="4" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="C137" s="5">
-        <v>-10000</v>
+        <v>500</v>
       </c>
       <c r="D137" s="4">
-        <f t="shared" si="14"/>
-        <v>1590</v>
+        <f t="shared" si="20"/>
+        <v>2890</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="16" t="s">
-        <v>141</v>
+        <v>189</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>65</v>
+        <v>190</v>
       </c>
       <c r="C138" s="5">
-        <v>2000</v>
+        <v>5600</v>
       </c>
       <c r="D138" s="4">
-        <f t="shared" ref="D138:D143" si="15">D137+C138</f>
-        <v>3590</v>
+        <f t="shared" si="20"/>
+        <v>8490</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="16" t="s">
-        <v>142</v>
-      </c>
       <c r="B139" s="4" t="s">
-        <v>136</v>
+        <v>191</v>
       </c>
       <c r="C139" s="5">
-        <v>8000</v>
+        <v>4700</v>
       </c>
       <c r="D139" s="4">
-        <f t="shared" si="15"/>
-        <v>11590</v>
+        <f t="shared" ref="D139:D145" si="21">D138+C139</f>
+        <v>13190</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" s="16" t="s">
+        <v>192</v>
+      </c>
       <c r="B140" s="4" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="C140" s="5">
-        <v>-10000</v>
+        <v>1500</v>
       </c>
       <c r="D140" s="4">
-        <f t="shared" si="15"/>
-        <v>1590</v>
+        <f t="shared" si="21"/>
+        <v>14690</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="16" t="s">
-        <v>143</v>
-      </c>
       <c r="B141" s="4" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="C141" s="5">
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="D141" s="4">
-        <f t="shared" si="15"/>
-        <v>3590</v>
+        <f t="shared" si="21"/>
+        <v>15190</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="16" t="s">
-        <v>144</v>
+        <v>193</v>
       </c>
       <c r="B142" s="4" t="s">
-        <v>145</v>
+        <v>194</v>
       </c>
       <c r="C142" s="5">
-        <v>12000</v>
+        <v>1000</v>
       </c>
       <c r="D142" s="4">
-        <f t="shared" si="15"/>
-        <v>15590</v>
+        <f t="shared" si="21"/>
+        <v>16190</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" s="16" t="s">
+        <v>195</v>
+      </c>
       <c r="B143" s="4" t="s">
-        <v>20</v>
+        <v>196</v>
       </c>
       <c r="C143" s="5">
-        <v>-10000</v>
+        <v>1000</v>
       </c>
       <c r="D143" s="4">
-        <f t="shared" si="15"/>
-        <v>5590</v>
+        <f t="shared" si="21"/>
+        <v>17190</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="16" t="s">
-        <v>161</v>
+        <v>197</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>146</v>
+        <v>28</v>
       </c>
       <c r="C144" s="5">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="D144" s="4">
-        <f t="shared" ref="D144:D149" si="16">D143+C144</f>
-        <v>7590</v>
+        <f t="shared" si="21"/>
+        <v>20190</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="16" t="s">
-        <v>149</v>
-      </c>
       <c r="B145" s="4" t="s">
-        <v>147</v>
+        <v>198</v>
       </c>
       <c r="C145" s="5">
-        <v>10000</v>
+        <v>-20000</v>
       </c>
       <c r="D145" s="4">
-        <f t="shared" si="16"/>
-        <v>17590</v>
+        <f t="shared" si="21"/>
+        <v>190</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B146" s="4" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="C146" s="5">
-        <v>-10000</v>
+        <v>500</v>
       </c>
       <c r="D146" s="4">
-        <f t="shared" si="16"/>
-        <v>7590</v>
+        <f t="shared" ref="D146:D152" si="22">D145+C146</f>
+        <v>690</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B147" s="4" t="s">
-        <v>148</v>
+        <v>76</v>
       </c>
       <c r="C147" s="5">
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="D147" s="4">
-        <f t="shared" si="16"/>
-        <v>9590</v>
+        <f t="shared" si="22"/>
+        <v>1190</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="16" t="s">
-        <v>162</v>
+        <v>200</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>163</v>
+        <v>201</v>
       </c>
       <c r="C148" s="5">
-        <v>-1200</v>
+        <v>10000</v>
       </c>
       <c r="D148" s="4">
-        <f t="shared" si="16"/>
-        <v>8390</v>
+        <f t="shared" si="22"/>
+        <v>11190</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B149" s="4" t="s">
-        <v>164</v>
+        <v>202</v>
       </c>
       <c r="C149" s="5">
-        <v>500</v>
+        <v>-10000</v>
       </c>
       <c r="D149" s="4">
-        <f t="shared" si="16"/>
-        <v>8890</v>
+        <f t="shared" si="22"/>
+        <v>1190</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="16" t="s">
-        <v>165</v>
+        <v>204</v>
       </c>
       <c r="B150" s="4" t="s">
-        <v>166</v>
+        <v>28</v>
       </c>
       <c r="C150" s="5">
-        <v>750</v>
+        <v>3000</v>
       </c>
       <c r="D150" s="4">
-        <f t="shared" ref="D150:D155" si="17">D149+C150</f>
-        <v>9640</v>
+        <f t="shared" si="22"/>
+        <v>4190</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="16" t="s">
-        <v>167</v>
+        <v>205</v>
       </c>
       <c r="B151" s="4" t="s">
-        <v>131</v>
+        <v>186</v>
       </c>
       <c r="C151" s="5">
-        <v>2000</v>
+        <v>11000</v>
       </c>
       <c r="D151" s="4">
-        <f t="shared" si="17"/>
-        <v>11640</v>
+        <f t="shared" si="22"/>
+        <v>15190</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B152" s="4" t="s">
-        <v>65</v>
+        <v>20</v>
       </c>
       <c r="C152" s="5">
-        <v>2000</v>
+        <v>-10000</v>
       </c>
       <c r="D152" s="4">
-        <f t="shared" si="17"/>
-        <v>13640</v>
+        <f t="shared" si="22"/>
+        <v>5190</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" s="16" t="s">
+        <v>206</v>
+      </c>
       <c r="B153" s="4" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C153" s="5">
-        <v>-10000</v>
+        <v>3000</v>
       </c>
       <c r="D153" s="4">
-        <f t="shared" si="17"/>
-        <v>3640</v>
+        <f t="shared" ref="D153:D159" si="23">D152+C153</f>
+        <v>8190</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" s="16" t="s">
+        <v>210</v>
+      </c>
       <c r="B154" s="4" t="s">
-        <v>170</v>
+        <v>208</v>
       </c>
       <c r="C154" s="5">
-        <v>350</v>
+        <v>14000</v>
       </c>
       <c r="D154" s="4">
-        <f t="shared" si="17"/>
-        <v>3990</v>
+        <f t="shared" si="23"/>
+        <v>22190</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="16" t="s">
-        <v>171</v>
-      </c>
       <c r="B155" s="4" t="s">
-        <v>172</v>
+        <v>209</v>
       </c>
       <c r="C155" s="5">
-        <v>300</v>
+        <v>-20000</v>
       </c>
       <c r="D155" s="4">
-        <f t="shared" si="17"/>
-        <v>4290</v>
+        <f t="shared" si="23"/>
+        <v>2190</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="16" t="s">
-        <v>173</v>
+        <v>211</v>
       </c>
       <c r="B156" s="4" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="C156" s="5">
-        <v>3800</v>
+        <v>5000</v>
       </c>
       <c r="D156" s="4">
-        <f t="shared" ref="D156:D162" si="18">D155+C156</f>
-        <v>8090</v>
+        <f t="shared" si="23"/>
+        <v>7190</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" s="16" t="s">
+        <v>213</v>
+      </c>
       <c r="B157" s="4" t="s">
-        <v>76</v>
+        <v>214</v>
       </c>
       <c r="C157" s="5">
-        <v>500</v>
+        <v>5000</v>
       </c>
       <c r="D157" s="4">
-        <f t="shared" si="18"/>
-        <v>8590</v>
+        <f t="shared" si="23"/>
+        <v>12190</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="16" t="s">
-        <v>175</v>
+        <v>215</v>
       </c>
       <c r="B158" s="4" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="C158" s="5">
-        <v>1300</v>
+        <v>11000</v>
       </c>
       <c r="D158" s="4">
-        <f t="shared" si="18"/>
-        <v>9890</v>
+        <f t="shared" si="23"/>
+        <v>23190</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="16" t="s">
-        <v>177</v>
-      </c>
       <c r="B159" s="4" t="s">
-        <v>100</v>
+        <v>198</v>
       </c>
       <c r="C159" s="5">
-        <v>9000</v>
+        <v>-20000</v>
       </c>
       <c r="D159" s="4">
-        <f t="shared" si="18"/>
-        <v>18890</v>
+        <f t="shared" si="23"/>
+        <v>3190</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" s="16" t="s">
+        <v>216</v>
+      </c>
       <c r="B160" s="4" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="C160" s="5">
+        <v>500</v>
+      </c>
+      <c r="D160" s="4">
+        <f t="shared" ref="D160:D165" si="24">D159+C160</f>
+        <v>3690</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B161" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C161" s="5">
+        <v>3000</v>
+      </c>
+      <c r="D161" s="4">
+        <f t="shared" si="24"/>
+        <v>6690</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="B162" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="C162" s="5">
+        <v>12000</v>
+      </c>
+      <c r="D162" s="4">
+        <f t="shared" si="24"/>
+        <v>18690</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B163" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="C163" s="5">
         <v>-10000</v>
       </c>
-      <c r="D160" s="4">
-        <f t="shared" si="18"/>
-        <v>8890</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" s="16" t="s">
-        <v>178</v>
-      </c>
-      <c r="B161" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C161" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D161" s="4">
-        <f t="shared" si="18"/>
-        <v>10890</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B162" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C162" s="5">
-        <v>-10000</v>
-      </c>
-      <c r="D162" s="4">
-        <f t="shared" si="18"/>
-        <v>890</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="B163" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="C163" s="5">
-        <v>500</v>
-      </c>
       <c r="D163" s="4">
-        <f t="shared" ref="D163:D168" si="19">D162+C163</f>
-        <v>1390</v>
+        <f t="shared" si="24"/>
+        <v>8690</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="16" t="s">
-        <v>181</v>
+        <v>219</v>
       </c>
       <c r="B164" s="4" t="s">
-        <v>182</v>
+        <v>220</v>
       </c>
       <c r="C164" s="5">
-        <v>10000</v>
+        <v>5000</v>
       </c>
       <c r="D164" s="4">
-        <f t="shared" si="19"/>
-        <v>11390</v>
+        <f t="shared" si="24"/>
+        <v>13690</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B165" s="4" t="s">
-        <v>20</v>
+        <v>202</v>
       </c>
       <c r="C165" s="5">
         <v>-10000</v>
       </c>
       <c r="D165" s="4">
-        <f t="shared" si="19"/>
-        <v>1390</v>
+        <f t="shared" si="24"/>
+        <v>3690</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="16" t="s">
-        <v>183</v>
+        <v>221</v>
       </c>
       <c r="B166" s="4" t="s">
-        <v>25</v>
+        <v>222</v>
       </c>
       <c r="C166" s="5">
-        <v>3000</v>
+        <v>12000</v>
       </c>
       <c r="D166" s="4">
-        <f t="shared" si="19"/>
-        <v>4390</v>
+        <f t="shared" ref="D166:D171" si="25">D165+C166</f>
+        <v>15690</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A167" s="16" t="s">
-        <v>184</v>
-      </c>
       <c r="B167" s="4" t="s">
-        <v>65</v>
+        <v>20</v>
       </c>
       <c r="C167" s="5">
-        <v>2000</v>
+        <v>-10000</v>
       </c>
       <c r="D167" s="4">
-        <f t="shared" si="19"/>
-        <v>6390</v>
+        <f t="shared" si="25"/>
+        <v>5690</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" s="16" t="s">
+        <v>226</v>
+      </c>
       <c r="B168" s="4" t="s">
-        <v>131</v>
+        <v>40</v>
       </c>
       <c r="C168" s="5">
         <v>2000</v>
       </c>
       <c r="D168" s="4">
-        <f t="shared" si="19"/>
-        <v>8390</v>
+        <f t="shared" si="25"/>
+        <v>7690</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="16" t="s">
-        <v>185</v>
+        <v>227</v>
       </c>
       <c r="B169" s="4" t="s">
-        <v>186</v>
+        <v>228</v>
       </c>
       <c r="C169" s="5">
-        <v>11000</v>
+        <v>1000</v>
       </c>
       <c r="D169" s="4">
-        <f t="shared" ref="D169:D174" si="20">D168+C169</f>
-        <v>19390</v>
+        <f t="shared" si="25"/>
+        <v>8690</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" s="16" t="s">
+        <v>229</v>
+      </c>
       <c r="B170" s="4" t="s">
-        <v>20</v>
+        <v>212</v>
       </c>
       <c r="C170" s="5">
+        <v>5000</v>
+      </c>
+      <c r="D170" s="4">
+        <f t="shared" si="25"/>
+        <v>13690</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B171" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="C171" s="5">
         <v>-10000</v>
       </c>
-      <c r="D170" s="4">
-        <f t="shared" si="20"/>
-        <v>9390</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="B171" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="C171" s="5">
-        <v>3000</v>
-      </c>
       <c r="D171" s="4">
-        <f t="shared" si="20"/>
-        <v>12390</v>
+        <f t="shared" si="25"/>
+        <v>3690</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" s="16" t="s">
+        <v>231</v>
+      </c>
       <c r="B172" s="4" t="s">
-        <v>20</v>
+        <v>232</v>
       </c>
       <c r="C172" s="5">
-        <v>-10000</v>
+        <v>13000</v>
       </c>
       <c r="D172" s="4">
-        <f t="shared" si="20"/>
-        <v>2390</v>
+        <f t="shared" ref="D172:D177" si="26">D171+C172</f>
+        <v>16690</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B173" s="4" t="s">
-        <v>76</v>
+        <v>20</v>
       </c>
       <c r="C173" s="5">
-        <v>500</v>
+        <v>-10000</v>
       </c>
       <c r="D173" s="4">
-        <f t="shared" si="20"/>
-        <v>2890</v>
+        <f t="shared" si="26"/>
+        <v>6690</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="16" t="s">
-        <v>189</v>
+        <v>233</v>
       </c>
       <c r="B174" s="4" t="s">
-        <v>190</v>
+        <v>28</v>
       </c>
       <c r="C174" s="5">
-        <v>5600</v>
+        <v>3000</v>
       </c>
       <c r="D174" s="4">
-        <f t="shared" si="20"/>
-        <v>8490</v>
+        <f t="shared" si="26"/>
+        <v>9690</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175" s="16" t="s">
+        <v>234</v>
+      </c>
       <c r="B175" s="4" t="s">
-        <v>191</v>
+        <v>232</v>
       </c>
       <c r="C175" s="5">
-        <v>4700</v>
+        <v>13000</v>
       </c>
       <c r="D175" s="4">
-        <f t="shared" ref="D175:D181" si="21">D174+C175</f>
-        <v>13190</v>
+        <f t="shared" si="26"/>
+        <v>22690</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176" s="16" t="s">
-        <v>192</v>
-      </c>
       <c r="B176" s="4" t="s">
-        <v>78</v>
+        <v>198</v>
       </c>
       <c r="C176" s="5">
-        <v>1500</v>
+        <v>-20000</v>
       </c>
       <c r="D176" s="4">
-        <f t="shared" si="21"/>
-        <v>14690</v>
+        <f t="shared" si="26"/>
+        <v>2690</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177" s="16" t="s">
+        <v>235</v>
+      </c>
       <c r="B177" s="4" t="s">
-        <v>76</v>
+        <v>28</v>
       </c>
       <c r="C177" s="5">
-        <v>500</v>
+        <v>3000</v>
       </c>
       <c r="D177" s="4">
-        <f t="shared" si="21"/>
-        <v>15190</v>
+        <f t="shared" si="26"/>
+        <v>5690</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="16" t="s">
-        <v>193</v>
+        <v>237</v>
       </c>
       <c r="B178" s="4" t="s">
-        <v>194</v>
+        <v>236</v>
       </c>
       <c r="C178" s="5">
-        <v>1000</v>
+        <v>16000</v>
       </c>
       <c r="D178" s="4">
-        <f t="shared" si="21"/>
-        <v>16190</v>
+        <f t="shared" ref="D178:D183" si="27">D177+C178</f>
+        <v>21690</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A179" s="16" t="s">
-        <v>195</v>
-      </c>
       <c r="B179" s="4" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C179" s="5">
-        <v>1000</v>
+        <v>-20000</v>
       </c>
       <c r="D179" s="4">
-        <f t="shared" si="21"/>
-        <v>17190</v>
+        <f t="shared" si="27"/>
+        <v>1690</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="16" t="s">
-        <v>197</v>
+        <v>240</v>
       </c>
       <c r="B180" s="4" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="C180" s="5">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="D180" s="4">
-        <f t="shared" si="21"/>
-        <v>20190</v>
+        <f t="shared" si="27"/>
+        <v>3690</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A181" s="16" t="s">
+        <v>241</v>
+      </c>
       <c r="B181" s="4" t="s">
-        <v>198</v>
+        <v>228</v>
       </c>
       <c r="C181" s="5">
-        <v>-20000</v>
+        <v>1000</v>
       </c>
       <c r="D181" s="4">
-        <f t="shared" si="21"/>
-        <v>190</v>
+        <f t="shared" si="27"/>
+        <v>4690</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182" s="16" t="s">
+        <v>242</v>
+      </c>
       <c r="B182" s="4" t="s">
-        <v>76</v>
+        <v>243</v>
       </c>
       <c r="C182" s="5">
-        <v>500</v>
+        <v>6000</v>
       </c>
       <c r="D182" s="4">
-        <f t="shared" ref="D182:D188" si="22">D181+C182</f>
-        <v>690</v>
+        <f t="shared" si="27"/>
+        <v>10690</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B183" s="4" t="s">
-        <v>76</v>
+        <v>20</v>
       </c>
       <c r="C183" s="5">
-        <v>500</v>
+        <v>-10000</v>
       </c>
       <c r="D183" s="4">
-        <f t="shared" si="22"/>
-        <v>1190</v>
+        <f t="shared" si="27"/>
+        <v>690</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="16" t="s">
-        <v>200</v>
+        <v>244</v>
       </c>
       <c r="B184" s="4" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="C184" s="5">
-        <v>10000</v>
+        <v>14000</v>
       </c>
       <c r="D184" s="4">
-        <f t="shared" si="22"/>
-        <v>11190</v>
+        <f>D183+C184</f>
+        <v>14690</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B185" s="4" t="s">
-        <v>202</v>
+        <v>20</v>
       </c>
       <c r="C185" s="5">
         <v>-10000</v>
       </c>
       <c r="D185" s="4">
-        <f t="shared" si="22"/>
-        <v>1190</v>
-      </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A186" s="16" t="s">
-        <v>204</v>
-      </c>
-      <c r="B186" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C186" s="5">
-        <v>3000</v>
-      </c>
-      <c r="D186" s="4">
-        <f t="shared" si="22"/>
-        <v>4190</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A187" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="B187" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="C187" s="5">
-        <v>11000</v>
-      </c>
-      <c r="D187" s="4">
-        <f t="shared" si="22"/>
-        <v>15190</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B188" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C188" s="5">
-        <v>-10000</v>
-      </c>
-      <c r="D188" s="4">
-        <f t="shared" si="22"/>
-        <v>5190</v>
-      </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="B189" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C189" s="5">
-        <v>3000</v>
-      </c>
-      <c r="D189" s="4">
-        <f t="shared" ref="D189:D195" si="23">D188+C189</f>
-        <v>8190</v>
-      </c>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A190" s="16" t="s">
-        <v>210</v>
-      </c>
-      <c r="B190" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="C190" s="5">
-        <v>14000</v>
-      </c>
-      <c r="D190" s="4">
-        <f t="shared" si="23"/>
-        <v>22190</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B191" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="C191" s="5">
-        <v>-20000</v>
-      </c>
-      <c r="D191" s="4">
-        <f t="shared" si="23"/>
-        <v>2190</v>
-      </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A192" s="16" t="s">
-        <v>211</v>
-      </c>
-      <c r="B192" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="C192" s="5">
-        <v>5000</v>
-      </c>
-      <c r="D192" s="4">
-        <f t="shared" si="23"/>
-        <v>7190</v>
-      </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A193" s="16" t="s">
-        <v>213</v>
-      </c>
-      <c r="B193" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="C193" s="5">
-        <v>5000</v>
-      </c>
-      <c r="D193" s="4">
-        <f t="shared" si="23"/>
-        <v>12190</v>
-      </c>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="B194" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="C194" s="5">
-        <v>11000</v>
-      </c>
-      <c r="D194" s="4">
-        <f t="shared" si="23"/>
-        <v>23190</v>
-      </c>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B195" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="C195" s="5">
-        <v>-20000</v>
-      </c>
-      <c r="D195" s="4">
-        <f t="shared" si="23"/>
-        <v>3190</v>
-      </c>
-    </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A196" s="16" t="s">
-        <v>216</v>
-      </c>
-      <c r="B196" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C196" s="5">
-        <v>500</v>
-      </c>
-      <c r="D196" s="4">
-        <f t="shared" ref="D196:D201" si="24">D195+C196</f>
-        <v>3690</v>
-      </c>
-    </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B197" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C197" s="5">
-        <v>3000</v>
-      </c>
-      <c r="D197" s="4">
-        <f t="shared" si="24"/>
-        <v>6690</v>
-      </c>
-    </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A198" s="16" t="s">
-        <v>217</v>
-      </c>
-      <c r="B198" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="C198" s="5">
-        <v>12000</v>
-      </c>
-      <c r="D198" s="4">
-        <f t="shared" si="24"/>
-        <v>18690</v>
-      </c>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B199" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="C199" s="5">
-        <v>-10000</v>
-      </c>
-      <c r="D199" s="4">
-        <f t="shared" si="24"/>
-        <v>8690</v>
-      </c>
-    </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A200" s="16" t="s">
-        <v>219</v>
-      </c>
-      <c r="B200" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="C200" s="5">
-        <v>5000</v>
-      </c>
-      <c r="D200" s="4">
-        <f t="shared" si="24"/>
-        <v>13690</v>
-      </c>
-    </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B201" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="C201" s="5">
-        <v>-10000</v>
-      </c>
-      <c r="D201" s="4">
-        <f t="shared" si="24"/>
-        <v>3690</v>
-      </c>
-    </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A202" s="16" t="s">
-        <v>221</v>
-      </c>
-      <c r="B202" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="C202" s="5">
-        <v>12000</v>
-      </c>
-      <c r="D202" s="4">
-        <f t="shared" ref="D202:D207" si="25">D201+C202</f>
-        <v>15690</v>
-      </c>
-    </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B203" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C203" s="5">
-        <v>-10000</v>
-      </c>
-      <c r="D203" s="4">
-        <f t="shared" si="25"/>
-        <v>5690</v>
-      </c>
-    </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A204" s="16" t="s">
-        <v>226</v>
-      </c>
-      <c r="B204" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C204" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D204" s="4">
-        <f t="shared" si="25"/>
-        <v>7690</v>
-      </c>
-    </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A205" s="16" t="s">
-        <v>227</v>
-      </c>
-      <c r="B205" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="C205" s="5">
-        <v>1000</v>
-      </c>
-      <c r="D205" s="4">
-        <f t="shared" si="25"/>
-        <v>8690</v>
-      </c>
-    </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A206" s="16" t="s">
-        <v>229</v>
-      </c>
-      <c r="B206" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="C206" s="5">
-        <v>5000</v>
-      </c>
-      <c r="D206" s="4">
-        <f t="shared" si="25"/>
-        <v>13690</v>
-      </c>
-    </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B207" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="C207" s="5">
-        <v>-10000</v>
-      </c>
-      <c r="D207" s="4">
-        <f t="shared" si="25"/>
-        <v>3690</v>
-      </c>
-    </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A208" s="16" t="s">
-        <v>231</v>
-      </c>
-      <c r="B208" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="C208" s="5">
-        <v>13000</v>
-      </c>
-      <c r="D208" s="4">
-        <f t="shared" ref="D208:D213" si="26">D207+C208</f>
-        <v>16690</v>
-      </c>
-    </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B209" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C209" s="5">
-        <v>-10000</v>
-      </c>
-      <c r="D209" s="4">
-        <f t="shared" si="26"/>
-        <v>6690</v>
-      </c>
-    </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A210" s="16" t="s">
-        <v>233</v>
-      </c>
-      <c r="B210" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C210" s="5">
-        <v>3000</v>
-      </c>
-      <c r="D210" s="4">
-        <f t="shared" si="26"/>
-        <v>9690</v>
-      </c>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A211" s="16" t="s">
-        <v>234</v>
-      </c>
-      <c r="B211" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="C211" s="5">
-        <v>13000</v>
-      </c>
-      <c r="D211" s="4">
-        <f t="shared" si="26"/>
-        <v>22690</v>
-      </c>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B212" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="C212" s="5">
-        <v>-20000</v>
-      </c>
-      <c r="D212" s="4">
-        <f t="shared" si="26"/>
-        <v>2690</v>
-      </c>
-    </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A213" s="16" t="s">
-        <v>235</v>
-      </c>
-      <c r="B213" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C213" s="5">
-        <v>3000</v>
-      </c>
-      <c r="D213" s="4">
-        <f t="shared" si="26"/>
-        <v>5690</v>
-      </c>
-    </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A214" s="16" t="s">
-        <v>237</v>
-      </c>
-      <c r="B214" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="C214" s="5">
-        <v>16000</v>
-      </c>
-      <c r="D214" s="4">
-        <f t="shared" ref="D214:D219" si="27">D213+C214</f>
-        <v>21690</v>
-      </c>
-    </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B215" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="C215" s="5">
-        <v>-20000</v>
-      </c>
-      <c r="D215" s="4">
-        <f t="shared" si="27"/>
-        <v>1690</v>
-      </c>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A216" s="16" t="s">
-        <v>240</v>
-      </c>
-      <c r="B216" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C216" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D216" s="4">
-        <f t="shared" si="27"/>
-        <v>3690</v>
-      </c>
-    </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A217" s="16" t="s">
-        <v>241</v>
-      </c>
-      <c r="B217" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="C217" s="5">
-        <v>1000</v>
-      </c>
-      <c r="D217" s="4">
-        <f t="shared" si="27"/>
+        <f>D184+C185</f>
         <v>4690</v>
-      </c>
-    </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A218" s="16" t="s">
-        <v>242</v>
-      </c>
-      <c r="B218" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="C218" s="5">
-        <v>6000</v>
-      </c>
-      <c r="D218" s="4">
-        <f t="shared" si="27"/>
-        <v>10690</v>
-      </c>
-    </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B219" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C219" s="5">
-        <v>-10000</v>
-      </c>
-      <c r="D219" s="4">
-        <f t="shared" si="27"/>
-        <v>690</v>
       </c>
     </row>
   </sheetData>
@@ -4755,7 +4720,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
duy lay tien loi co diem ngay 23
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="246">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -754,6 +754,9 @@
   </si>
   <si>
     <t>21/11/2024</t>
+  </si>
+  <si>
+    <t>23/11/2024</t>
   </si>
 </sst>
 </file>
@@ -1254,11 +1257,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K185"/>
+  <dimension ref="A1:K186"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A157" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
+      <pane ySplit="1" topLeftCell="A168" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F191" sqref="F191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4174,6 +4177,21 @@
       <c r="D185" s="4">
         <f>D184+C185</f>
         <v>4690</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" s="16" t="s">
+        <v>245</v>
+      </c>
+      <c r="B186" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C186" s="5">
+        <v>3000</v>
+      </c>
+      <c r="D186" s="4">
+        <f>D185+C186</f>
+        <v>7690</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
duy tinh tien loi co diem ngay 02
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="252">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -769,6 +769,12 @@
   </si>
   <si>
     <t>Duy tính tiền lời ngày 31,01</t>
+  </si>
+  <si>
+    <t>02/12/2024</t>
+  </si>
+  <si>
+    <t>Duy tính tiền lời 15tr</t>
   </si>
 </sst>
 </file>
@@ -1269,11 +1275,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K190"/>
+  <dimension ref="A1:K193"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A173" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F198" sqref="F198"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1349,8 +1355,8 @@
         <v>20</v>
       </c>
       <c r="J3" s="4">
-        <f>SUM(I3:I74)</f>
-        <v>660</v>
+        <f>SUM(I3:I75)</f>
+        <v>680</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -2360,7 +2366,7 @@
         <v>7000</v>
       </c>
       <c r="D54" s="4">
-        <f t="shared" ref="D54:D59" si="7">D53+C54</f>
+        <f t="shared" ref="D54:D58" si="7">D53+C54</f>
         <v>8690</v>
       </c>
       <c r="H54" s="16" t="s">
@@ -2448,18 +2454,8 @@
       <c r="K58" s="14"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B59" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C59" s="5">
-        <v>6000</v>
-      </c>
-      <c r="D59" s="4">
-        <f t="shared" si="7"/>
-        <v>6390</v>
-      </c>
       <c r="H59" s="16" t="s">
-        <v>207</v>
+        <v>250</v>
       </c>
       <c r="I59" s="5">
         <v>20</v>
@@ -2467,270 +2463,277 @@
       <c r="K59" s="14"/>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" s="16" t="s">
-        <v>94</v>
-      </c>
       <c r="B60" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C60" s="5">
-        <v>2000</v>
+        <v>6000</v>
       </c>
       <c r="D60" s="4">
-        <f t="shared" ref="D60:D65" si="8">D59+C60</f>
-        <v>8390</v>
+        <f>D58+C60</f>
+        <v>6390</v>
       </c>
       <c r="H60" s="16" t="s">
-        <v>187</v>
+        <v>207</v>
       </c>
       <c r="I60" s="5">
-        <v>10</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="K60" s="14"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C61" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D61" s="4">
+        <f t="shared" ref="D61:D66" si="8">D60+C61</f>
+        <v>8390</v>
+      </c>
+      <c r="H61" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="I61" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B62" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C61" s="5">
+      <c r="C62" s="5">
         <v>5000</v>
       </c>
-      <c r="D61" s="4">
+      <c r="D62" s="4">
         <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B62" s="4" t="s">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B63" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C62" s="5">
+      <c r="C63" s="5">
         <v>-10000</v>
       </c>
-      <c r="D62" s="4">
+      <c r="D63" s="4">
         <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" s="16" t="s">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B64" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C63" s="5">
+      <c r="C64" s="5">
         <v>1000</v>
       </c>
-      <c r="D63" s="4">
+      <c r="D64" s="4">
         <f t="shared" si="8"/>
         <v>4390</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B64" s="4" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B65" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C64" s="5">
+      <c r="C65" s="5">
         <v>9000</v>
       </c>
-      <c r="D64" s="4">
+      <c r="D65" s="4">
         <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B65" s="4" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C65" s="5">
+      <c r="C66" s="5">
         <v>-10000</v>
       </c>
-      <c r="D65" s="4">
+      <c r="D66" s="4">
         <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B66" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C66" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D66" s="4">
-        <f t="shared" ref="D66:D71" si="9">D65+C66</f>
-        <v>5390</v>
-      </c>
-    </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B67" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C67" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D67" s="4">
+        <f t="shared" ref="D67:D72" si="9">D66+C67</f>
+        <v>5390</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B68" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C67" s="5">
+      <c r="C68" s="5">
         <v>6000</v>
       </c>
-      <c r="D67" s="4">
+      <c r="D68" s="4">
         <f t="shared" si="9"/>
         <v>11390</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B68" s="4" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B69" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C68" s="5">
+      <c r="C69" s="5">
         <v>-10000</v>
       </c>
-      <c r="D68" s="4">
+      <c r="D69" s="4">
         <f t="shared" si="9"/>
         <v>1390</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B69" s="4" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B70" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C69" s="5">
+      <c r="C70" s="5">
         <v>400</v>
       </c>
-      <c r="D69" s="4">
+      <c r="D70" s="4">
         <f t="shared" si="9"/>
         <v>1790</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="16" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B71" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C70" s="5">
+      <c r="C71" s="5">
         <v>2000</v>
       </c>
-      <c r="D70" s="4">
+      <c r="D71" s="4">
         <f t="shared" si="9"/>
         <v>3790</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="16" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B72" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C71" s="5">
+      <c r="C72" s="5">
         <v>6000</v>
       </c>
-      <c r="D71" s="4">
+      <c r="D72" s="4">
         <f t="shared" si="9"/>
         <v>9790</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="16" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B73" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C72" s="5">
+      <c r="C73" s="5">
         <v>1000</v>
       </c>
-      <c r="D72" s="4">
-        <f t="shared" ref="D72:D77" si="10">D71+C72</f>
+      <c r="D73" s="4">
+        <f t="shared" ref="D73:D78" si="10">D72+C73</f>
         <v>10790</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B73" s="4" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C73" s="5">
+      <c r="C74" s="5">
         <v>-10000</v>
       </c>
-      <c r="D73" s="4">
+      <c r="D74" s="4">
         <f t="shared" si="10"/>
         <v>790</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="16" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B75" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C74" s="5">
+      <c r="C75" s="5">
         <v>800</v>
       </c>
-      <c r="D74" s="4">
+      <c r="D75" s="4">
         <f t="shared" si="10"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="16" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="B76" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C75" s="5">
+      <c r="C76" s="5">
         <v>5000</v>
       </c>
-      <c r="D75" s="4">
+      <c r="D76" s="4">
         <f t="shared" si="10"/>
         <v>6590</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="16" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B77" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C76" s="5">
+      <c r="C77" s="5">
         <v>6000</v>
       </c>
-      <c r="D76" s="4">
+      <c r="D77" s="4">
         <f t="shared" si="10"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B77" s="4" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B78" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C77" s="5">
+      <c r="C78" s="5">
         <v>-10000</v>
       </c>
-      <c r="D77" s="4">
+      <c r="D78" s="4">
         <f t="shared" si="10"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="16" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="B78" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C78" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D78" s="4">
-        <f t="shared" ref="D78:D84" si="11">D77+C78</f>
-        <v>4590</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B79" s="4" t="s">
         <v>65</v>
       </c>
@@ -2738,926 +2741,926 @@
         <v>2000</v>
       </c>
       <c r="D79" s="4">
+        <f t="shared" ref="D79:D85" si="11">D78+C79</f>
+        <v>4590</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B80" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C80" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D80" s="4">
         <f t="shared" si="11"/>
         <v>6590</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B80" s="4" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B81" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C80" s="5">
+      <c r="C81" s="5">
         <v>7000</v>
       </c>
-      <c r="D80" s="4">
+      <c r="D81" s="4">
         <f t="shared" si="11"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B81" s="4" t="s">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B82" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C81" s="5">
+      <c r="C82" s="5">
         <v>-10000</v>
       </c>
-      <c r="D81" s="4">
+      <c r="D82" s="4">
         <f t="shared" si="11"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="16" t="s">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="B82" s="4" t="s">
+      <c r="B83" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C82" s="5">
+      <c r="C83" s="5">
         <v>2000</v>
       </c>
-      <c r="D82" s="4">
+      <c r="D83" s="4">
         <f t="shared" si="11"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="16" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="B84" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C83" s="5">
+      <c r="C84" s="5">
         <v>6000</v>
       </c>
-      <c r="D83" s="4">
+      <c r="D84" s="4">
         <f t="shared" si="11"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B84" s="4" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B85" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C84" s="5">
+      <c r="C85" s="5">
         <v>-10000</v>
       </c>
-      <c r="D84" s="4">
+      <c r="D85" s="4">
         <f t="shared" si="11"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="B85" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C85" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D85" s="4">
-        <f t="shared" ref="D85:D90" si="12">D84+C85</f>
-        <v>3590</v>
-      </c>
-    </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C86" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D86" s="4">
+        <f t="shared" ref="D86:D91" si="12">D85+C86</f>
+        <v>3590</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="B87" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C86" s="5">
+      <c r="C87" s="5">
         <v>7000</v>
       </c>
-      <c r="D86" s="4">
+      <c r="D87" s="4">
         <f t="shared" si="12"/>
         <v>10590</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B87" s="4" t="s">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B88" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C87" s="5">
+      <c r="C88" s="5">
         <v>-10000</v>
       </c>
-      <c r="D87" s="4">
+      <c r="D88" s="4">
         <f t="shared" si="12"/>
         <v>590</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B88" s="4" t="s">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B89" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C88" s="5">
+      <c r="C89" s="5">
         <v>12000</v>
       </c>
-      <c r="D88" s="4">
+      <c r="D89" s="4">
         <f t="shared" si="12"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B89" s="4" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B90" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C89" s="5">
+      <c r="C90" s="5">
         <v>-10000</v>
       </c>
-      <c r="D89" s="4">
+      <c r="D90" s="4">
         <f t="shared" si="12"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B90" s="4" t="s">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B91" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C90" s="5">
+      <c r="C91" s="5">
         <v>2000</v>
       </c>
-      <c r="D90" s="4">
+      <c r="D91" s="4">
         <f t="shared" si="12"/>
         <v>4590</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="B91" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C91" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D91" s="4">
-        <f t="shared" ref="D91:D96" si="13">D90+C91</f>
-        <v>6590</v>
-      </c>
-    </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C92" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D92" s="4">
+        <f t="shared" ref="D92:D97" si="13">D91+C92</f>
+        <v>6590</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="B92" s="4" t="s">
+      <c r="B93" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C92" s="5">
+      <c r="C93" s="5">
         <v>7000</v>
       </c>
-      <c r="D92" s="4">
+      <c r="D93" s="4">
         <f t="shared" si="13"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B93" s="4" t="s">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B94" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C93" s="5">
+      <c r="C94" s="5">
         <v>-10000</v>
       </c>
-      <c r="D93" s="4">
+      <c r="D94" s="4">
         <f t="shared" si="13"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="16" t="s">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="B94" s="4" t="s">
+      <c r="B95" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C94" s="5">
+      <c r="C95" s="5">
         <v>2000</v>
       </c>
-      <c r="D94" s="4">
+      <c r="D95" s="4">
         <f t="shared" si="13"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="16" t="s">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="B95" s="4" t="s">
+      <c r="B96" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C95" s="5">
+      <c r="C96" s="5">
         <v>8000</v>
       </c>
-      <c r="D95" s="4">
+      <c r="D96" s="4">
         <f t="shared" si="13"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B96" s="4" t="s">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B97" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C96" s="5">
+      <c r="C97" s="5">
         <v>-10000</v>
       </c>
-      <c r="D96" s="4">
+      <c r="D97" s="4">
         <f t="shared" si="13"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="16" t="s">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="B97" s="4" t="s">
+      <c r="B98" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C97" s="5">
+      <c r="C98" s="5">
         <v>2000</v>
       </c>
-      <c r="D97" s="4">
-        <f t="shared" ref="D97:D102" si="14">D96+C97</f>
+      <c r="D98" s="4">
+        <f t="shared" ref="D98:D103" si="14">D97+C98</f>
         <v>5590</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B98" s="4" t="s">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B99" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C98" s="5">
+      <c r="C99" s="5">
         <v>5000</v>
       </c>
-      <c r="D98" s="4">
+      <c r="D99" s="4">
         <f t="shared" si="14"/>
         <v>10590</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B99" s="4" t="s">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B100" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C99" s="5">
+      <c r="C100" s="5">
         <v>-10000</v>
       </c>
-      <c r="D99" s="4">
+      <c r="D100" s="4">
         <f t="shared" si="14"/>
         <v>590</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B100" s="4" t="s">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B101" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C100" s="5">
+      <c r="C101" s="5">
         <v>2000</v>
       </c>
-      <c r="D100" s="4">
+      <c r="D101" s="4">
         <f t="shared" si="14"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B101" s="4" t="s">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B102" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C101" s="5">
+      <c r="C102" s="5">
         <v>9000</v>
       </c>
-      <c r="D101" s="4">
+      <c r="D102" s="4">
         <f t="shared" si="14"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B102" s="4" t="s">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B103" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C102" s="5">
+      <c r="C103" s="5">
         <v>-10000</v>
       </c>
-      <c r="D102" s="4">
+      <c r="D103" s="4">
         <f t="shared" si="14"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B103" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C103" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D103" s="4">
-        <f t="shared" ref="D103:D108" si="15">D102+C103</f>
-        <v>3590</v>
-      </c>
-    </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C104" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D104" s="4">
+        <f t="shared" ref="D104:D109" si="15">D103+C104</f>
+        <v>3590</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="B104" s="4" t="s">
+      <c r="B105" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C104" s="5">
+      <c r="C105" s="5">
         <v>8000</v>
       </c>
-      <c r="D104" s="4">
+      <c r="D105" s="4">
         <f t="shared" si="15"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B105" s="4" t="s">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B106" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C105" s="5">
+      <c r="C106" s="5">
         <v>-10000</v>
       </c>
-      <c r="D105" s="4">
+      <c r="D106" s="4">
         <f t="shared" si="15"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="16" t="s">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="B106" s="4" t="s">
+      <c r="B107" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C106" s="5">
+      <c r="C107" s="5">
         <v>2000</v>
       </c>
-      <c r="D106" s="4">
+      <c r="D107" s="4">
         <f t="shared" si="15"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="16" t="s">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="B107" s="4" t="s">
+      <c r="B108" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C107" s="5">
+      <c r="C108" s="5">
         <v>12000</v>
       </c>
-      <c r="D107" s="4">
+      <c r="D108" s="4">
         <f t="shared" si="15"/>
         <v>15590</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B108" s="4" t="s">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B109" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C108" s="5">
+      <c r="C109" s="5">
         <v>-10000</v>
       </c>
-      <c r="D108" s="4">
+      <c r="D109" s="4">
         <f t="shared" si="15"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="B109" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="C109" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D109" s="4">
-        <f t="shared" ref="D109:D114" si="16">D108+C109</f>
-        <v>7590</v>
-      </c>
-    </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="B110" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C110" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D110" s="4">
+        <f t="shared" ref="D110:D115" si="16">D109+C110</f>
+        <v>7590</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="B110" s="4" t="s">
+      <c r="B111" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="C110" s="5">
+      <c r="C111" s="5">
         <v>10000</v>
       </c>
-      <c r="D110" s="4">
+      <c r="D111" s="4">
         <f t="shared" si="16"/>
         <v>17590</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B111" s="4" t="s">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B112" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C111" s="5">
+      <c r="C112" s="5">
         <v>-10000</v>
       </c>
-      <c r="D111" s="4">
+      <c r="D112" s="4">
         <f t="shared" si="16"/>
         <v>7590</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B112" s="4" t="s">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B113" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="C112" s="5">
+      <c r="C113" s="5">
         <v>2000</v>
       </c>
-      <c r="D112" s="4">
+      <c r="D113" s="4">
         <f t="shared" si="16"/>
         <v>9590</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="16" t="s">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="B113" s="4" t="s">
+      <c r="B114" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="C113" s="5">
+      <c r="C114" s="5">
         <v>-1200</v>
       </c>
-      <c r="D113" s="4">
+      <c r="D114" s="4">
         <f t="shared" si="16"/>
         <v>8390</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B114" s="4" t="s">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B115" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="C114" s="5">
+      <c r="C115" s="5">
         <v>500</v>
       </c>
-      <c r="D114" s="4">
+      <c r="D115" s="4">
         <f t="shared" si="16"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="16" t="s">
-        <v>165</v>
-      </c>
-      <c r="B115" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="C115" s="5">
-        <v>750</v>
-      </c>
-      <c r="D115" s="4">
-        <f t="shared" ref="D115:D120" si="17">D114+C115</f>
-        <v>9640</v>
-      </c>
-    </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="B116" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C116" s="5">
+        <v>750</v>
+      </c>
+      <c r="D116" s="4">
+        <f t="shared" ref="D116:D121" si="17">D115+C116</f>
+        <v>9640</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="B116" s="4" t="s">
+      <c r="B117" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C116" s="5">
+      <c r="C117" s="5">
         <v>2000</v>
       </c>
-      <c r="D116" s="4">
+      <c r="D117" s="4">
         <f t="shared" si="17"/>
         <v>11640</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B117" s="4" t="s">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B118" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C117" s="5">
+      <c r="C118" s="5">
         <v>2000</v>
       </c>
-      <c r="D117" s="4">
+      <c r="D118" s="4">
         <f t="shared" si="17"/>
         <v>13640</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B118" s="4" t="s">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B119" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C118" s="5">
+      <c r="C119" s="5">
         <v>-10000</v>
       </c>
-      <c r="D118" s="4">
+      <c r="D119" s="4">
         <f t="shared" si="17"/>
         <v>3640</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B119" s="4" t="s">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B120" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="C119" s="5">
+      <c r="C120" s="5">
         <v>350</v>
       </c>
-      <c r="D119" s="4">
+      <c r="D120" s="4">
         <f t="shared" si="17"/>
         <v>3990</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="16" t="s">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="B120" s="4" t="s">
+      <c r="B121" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="C120" s="5">
+      <c r="C121" s="5">
         <v>300</v>
       </c>
-      <c r="D120" s="4">
+      <c r="D121" s="4">
         <f t="shared" si="17"/>
         <v>4290</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="16" t="s">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="B121" s="4" t="s">
+      <c r="B122" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="C121" s="5">
+      <c r="C122" s="5">
         <v>3800</v>
       </c>
-      <c r="D121" s="4">
-        <f t="shared" ref="D121:D127" si="18">D120+C121</f>
+      <c r="D122" s="4">
+        <f t="shared" ref="D122:D128" si="18">D121+C122</f>
         <v>8090</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B122" s="4" t="s">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B123" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C122" s="5">
+      <c r="C123" s="5">
         <v>500</v>
       </c>
-      <c r="D122" s="4">
+      <c r="D123" s="4">
         <f t="shared" si="18"/>
         <v>8590</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="16" t="s">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="B123" s="4" t="s">
+      <c r="B124" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="C123" s="5">
+      <c r="C124" s="5">
         <v>1300</v>
       </c>
-      <c r="D123" s="4">
+      <c r="D124" s="4">
         <f t="shared" si="18"/>
         <v>9890</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="16" t="s">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="B124" s="4" t="s">
+      <c r="B125" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C124" s="5">
+      <c r="C125" s="5">
         <v>9000</v>
       </c>
-      <c r="D124" s="4">
+      <c r="D125" s="4">
         <f t="shared" si="18"/>
         <v>18890</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B125" s="4" t="s">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B126" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C125" s="5">
+      <c r="C126" s="5">
         <v>-10000</v>
       </c>
-      <c r="D125" s="4">
+      <c r="D126" s="4">
         <f t="shared" si="18"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="16" t="s">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="B126" s="4" t="s">
+      <c r="B127" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C126" s="5">
+      <c r="C127" s="5">
         <v>2000</v>
       </c>
-      <c r="D126" s="4">
+      <c r="D127" s="4">
         <f t="shared" si="18"/>
         <v>10890</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B127" s="4" t="s">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B128" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C127" s="5">
+      <c r="C128" s="5">
         <v>-10000</v>
       </c>
-      <c r="D127" s="4">
+      <c r="D128" s="4">
         <f t="shared" si="18"/>
         <v>890</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="B128" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="C128" s="5">
-        <v>500</v>
-      </c>
-      <c r="D128" s="4">
-        <f t="shared" ref="D128:D133" si="19">D127+C128</f>
-        <v>1390</v>
-      </c>
-    </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="B129" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C129" s="5">
+        <v>500</v>
+      </c>
+      <c r="D129" s="4">
+        <f t="shared" ref="D129:D134" si="19">D128+C129</f>
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="B129" s="4" t="s">
+      <c r="B130" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="C129" s="5">
+      <c r="C130" s="5">
         <v>10000</v>
       </c>
-      <c r="D129" s="4">
+      <c r="D130" s="4">
         <f t="shared" si="19"/>
         <v>11390</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B130" s="4" t="s">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B131" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C130" s="5">
+      <c r="C131" s="5">
         <v>-10000</v>
       </c>
-      <c r="D130" s="4">
+      <c r="D131" s="4">
         <f t="shared" si="19"/>
         <v>1390</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="16" t="s">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="B131" s="4" t="s">
+      <c r="B132" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C131" s="5">
+      <c r="C132" s="5">
         <v>3000</v>
       </c>
-      <c r="D131" s="4">
+      <c r="D132" s="4">
         <f t="shared" si="19"/>
         <v>4390</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="16" t="s">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="B132" s="4" t="s">
+      <c r="B133" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C132" s="5">
+      <c r="C133" s="5">
         <v>2000</v>
       </c>
-      <c r="D132" s="4">
+      <c r="D133" s="4">
         <f t="shared" si="19"/>
         <v>6390</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B133" s="4" t="s">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B134" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C133" s="5">
+      <c r="C134" s="5">
         <v>2000</v>
       </c>
-      <c r="D133" s="4">
+      <c r="D134" s="4">
         <f t="shared" si="19"/>
         <v>8390</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="16" t="s">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="B134" s="4" t="s">
+      <c r="B135" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C134" s="5">
+      <c r="C135" s="5">
         <v>11000</v>
       </c>
-      <c r="D134" s="4">
-        <f t="shared" ref="D134:D139" si="20">D133+C134</f>
+      <c r="D135" s="4">
+        <f t="shared" ref="D135:D140" si="20">D134+C135</f>
         <v>19390</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B135" s="4" t="s">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B136" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C135" s="5">
+      <c r="C136" s="5">
         <v>-10000</v>
       </c>
-      <c r="D135" s="4">
+      <c r="D136" s="4">
         <f t="shared" si="20"/>
         <v>9390</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="16" t="s">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" s="16" t="s">
         <v>187</v>
       </c>
-      <c r="B136" s="4" t="s">
+      <c r="B137" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C136" s="5">
+      <c r="C137" s="5">
         <v>3000</v>
       </c>
-      <c r="D136" s="4">
+      <c r="D137" s="4">
         <f t="shared" si="20"/>
         <v>12390</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B137" s="4" t="s">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B138" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C137" s="5">
+      <c r="C138" s="5">
         <v>-10000</v>
       </c>
-      <c r="D137" s="4">
+      <c r="D138" s="4">
         <f t="shared" si="20"/>
         <v>2390</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B138" s="4" t="s">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B139" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C138" s="5">
+      <c r="C139" s="5">
         <v>500</v>
       </c>
-      <c r="D138" s="4">
+      <c r="D139" s="4">
         <f t="shared" si="20"/>
         <v>2890</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="16" t="s">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" s="16" t="s">
         <v>189</v>
       </c>
-      <c r="B139" s="4" t="s">
+      <c r="B140" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C139" s="5">
+      <c r="C140" s="5">
         <v>5600</v>
       </c>
-      <c r="D139" s="4">
+      <c r="D140" s="4">
         <f t="shared" si="20"/>
         <v>8490</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B140" s="4" t="s">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B141" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="C140" s="5">
+      <c r="C141" s="5">
         <v>4700</v>
       </c>
-      <c r="D140" s="4">
-        <f t="shared" ref="D140:D146" si="21">D139+C140</f>
+      <c r="D141" s="4">
+        <f t="shared" ref="D141:D147" si="21">D140+C141</f>
         <v>13190</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="16" t="s">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" s="16" t="s">
         <v>192</v>
       </c>
-      <c r="B141" s="4" t="s">
+      <c r="B142" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C141" s="5">
+      <c r="C142" s="5">
         <v>1500</v>
       </c>
-      <c r="D141" s="4">
+      <c r="D142" s="4">
         <f t="shared" si="21"/>
         <v>14690</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B142" s="4" t="s">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B143" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C142" s="5">
+      <c r="C143" s="5">
         <v>500</v>
       </c>
-      <c r="D142" s="4">
+      <c r="D143" s="4">
         <f t="shared" si="21"/>
         <v>15190</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="16" t="s">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="B143" s="4" t="s">
+      <c r="B144" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="C143" s="5">
+      <c r="C144" s="5">
         <v>1000</v>
       </c>
-      <c r="D143" s="4">
+      <c r="D144" s="4">
         <f t="shared" si="21"/>
         <v>16190</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="16" t="s">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="B144" s="4" t="s">
+      <c r="B145" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="C144" s="5">
+      <c r="C145" s="5">
         <v>1000</v>
       </c>
-      <c r="D144" s="4">
+      <c r="D145" s="4">
         <f t="shared" si="21"/>
         <v>17190</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="16" t="s">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="B145" s="4" t="s">
+      <c r="B146" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C145" s="5">
+      <c r="C146" s="5">
         <v>3000</v>
       </c>
-      <c r="D145" s="4">
+      <c r="D146" s="4">
         <f t="shared" si="21"/>
         <v>20190</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B146" s="4" t="s">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B147" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C146" s="5">
+      <c r="C147" s="5">
         <v>-20000</v>
       </c>
-      <c r="D146" s="4">
+      <c r="D147" s="4">
         <f t="shared" si="21"/>
         <v>190</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B147" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C147" s="5">
-        <v>500</v>
-      </c>
-      <c r="D147" s="4">
-        <f t="shared" ref="D147:D153" si="22">D146+C147</f>
-        <v>690</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -3668,593 +3671,632 @@
         <v>500</v>
       </c>
       <c r="D148" s="4">
+        <f t="shared" ref="D148:D154" si="22">D147+C148</f>
+        <v>690</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B149" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C149" s="5">
+        <v>500</v>
+      </c>
+      <c r="D149" s="4">
         <f t="shared" si="22"/>
         <v>1190</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="16" t="s">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="B149" s="4" t="s">
+      <c r="B150" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="C149" s="5">
+      <c r="C150" s="5">
         <v>10000</v>
       </c>
-      <c r="D149" s="4">
+      <c r="D150" s="4">
         <f t="shared" si="22"/>
         <v>11190</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B150" s="4" t="s">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B151" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C150" s="5">
+      <c r="C151" s="5">
         <v>-10000</v>
       </c>
-      <c r="D150" s="4">
+      <c r="D151" s="4">
         <f t="shared" si="22"/>
         <v>1190</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="16" t="s">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="B151" s="4" t="s">
+      <c r="B152" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C151" s="5">
+      <c r="C152" s="5">
         <v>3000</v>
       </c>
-      <c r="D151" s="4">
+      <c r="D152" s="4">
         <f t="shared" si="22"/>
         <v>4190</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="16" t="s">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="B152" s="4" t="s">
+      <c r="B153" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C152" s="5">
+      <c r="C153" s="5">
         <v>11000</v>
       </c>
-      <c r="D152" s="4">
+      <c r="D153" s="4">
         <f t="shared" si="22"/>
         <v>15190</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B153" s="4" t="s">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B154" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C153" s="5">
+      <c r="C154" s="5">
         <v>-10000</v>
       </c>
-      <c r="D153" s="4">
+      <c r="D154" s="4">
         <f t="shared" si="22"/>
         <v>5190</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="B154" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C154" s="5">
-        <v>3000</v>
-      </c>
-      <c r="D154" s="4">
-        <f t="shared" ref="D154:D160" si="23">D153+C154</f>
-        <v>8190</v>
-      </c>
-    </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="B155" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C155" s="5">
+        <v>3000</v>
+      </c>
+      <c r="D155" s="4">
+        <f t="shared" ref="D155:D161" si="23">D154+C155</f>
+        <v>8190</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="B155" s="4" t="s">
+      <c r="B156" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="C155" s="5">
+      <c r="C156" s="5">
         <v>14000</v>
       </c>
-      <c r="D155" s="4">
+      <c r="D156" s="4">
         <f t="shared" si="23"/>
         <v>22190</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B156" s="4" t="s">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B157" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="C156" s="5">
+      <c r="C157" s="5">
         <v>-20000</v>
       </c>
-      <c r="D156" s="4">
+      <c r="D157" s="4">
         <f t="shared" si="23"/>
         <v>2190</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="16" t="s">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="B157" s="4" t="s">
+      <c r="B158" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="C157" s="5">
+      <c r="C158" s="5">
         <v>5000</v>
       </c>
-      <c r="D157" s="4">
+      <c r="D158" s="4">
         <f t="shared" si="23"/>
         <v>7190</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="16" t="s">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" s="16" t="s">
         <v>213</v>
       </c>
-      <c r="B158" s="4" t="s">
+      <c r="B159" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="C158" s="5">
+      <c r="C159" s="5">
         <v>5000</v>
       </c>
-      <c r="D158" s="4">
+      <c r="D159" s="4">
         <f t="shared" si="23"/>
         <v>12190</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="16" t="s">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" s="16" t="s">
         <v>215</v>
       </c>
-      <c r="B159" s="4" t="s">
+      <c r="B160" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C159" s="5">
+      <c r="C160" s="5">
         <v>11000</v>
       </c>
-      <c r="D159" s="4">
+      <c r="D160" s="4">
         <f t="shared" si="23"/>
         <v>23190</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B160" s="4" t="s">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B161" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C160" s="5">
+      <c r="C161" s="5">
         <v>-20000</v>
       </c>
-      <c r="D160" s="4">
+      <c r="D161" s="4">
         <f t="shared" si="23"/>
         <v>3190</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" s="16" t="s">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" s="16" t="s">
         <v>216</v>
       </c>
-      <c r="B161" s="4" t="s">
+      <c r="B162" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C161" s="5">
+      <c r="C162" s="5">
         <v>500</v>
       </c>
-      <c r="D161" s="4">
-        <f t="shared" ref="D161:D166" si="24">D160+C161</f>
+      <c r="D162" s="4">
+        <f t="shared" ref="D162:D167" si="24">D161+C162</f>
         <v>3690</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B162" s="4" t="s">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B163" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C162" s="5">
+      <c r="C163" s="5">
         <v>3000</v>
       </c>
-      <c r="D162" s="4">
+      <c r="D163" s="4">
         <f t="shared" si="24"/>
         <v>6690</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163" s="16" t="s">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="B163" s="4" t="s">
+      <c r="B164" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="C163" s="5">
+      <c r="C164" s="5">
         <v>12000</v>
       </c>
-      <c r="D163" s="4">
+      <c r="D164" s="4">
         <f t="shared" si="24"/>
         <v>18690</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B164" s="4" t="s">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B165" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C164" s="5">
+      <c r="C165" s="5">
         <v>-10000</v>
       </c>
-      <c r="D164" s="4">
+      <c r="D165" s="4">
         <f t="shared" si="24"/>
         <v>8690</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" s="16" t="s">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="B165" s="4" t="s">
+      <c r="B166" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="C165" s="5">
+      <c r="C166" s="5">
         <v>5000</v>
       </c>
-      <c r="D165" s="4">
+      <c r="D166" s="4">
         <f t="shared" si="24"/>
         <v>13690</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B166" s="4" t="s">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B167" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C166" s="5">
+      <c r="C167" s="5">
         <v>-10000</v>
       </c>
-      <c r="D166" s="4">
+      <c r="D167" s="4">
         <f t="shared" si="24"/>
         <v>3690</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A167" s="16" t="s">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" s="16" t="s">
         <v>221</v>
       </c>
-      <c r="B167" s="4" t="s">
+      <c r="B168" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="C167" s="5">
+      <c r="C168" s="5">
         <v>12000</v>
       </c>
-      <c r="D167" s="4">
-        <f t="shared" ref="D167:D172" si="25">D166+C167</f>
+      <c r="D168" s="4">
+        <f t="shared" ref="D168:D173" si="25">D167+C168</f>
         <v>15690</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B168" s="4" t="s">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B169" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C168" s="5">
+      <c r="C169" s="5">
         <v>-10000</v>
       </c>
-      <c r="D168" s="4">
+      <c r="D169" s="4">
         <f t="shared" si="25"/>
         <v>5690</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A169" s="16" t="s">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="B169" s="4" t="s">
+      <c r="B170" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C169" s="5">
+      <c r="C170" s="5">
         <v>2000</v>
       </c>
-      <c r="D169" s="4">
+      <c r="D170" s="4">
         <f t="shared" si="25"/>
         <v>7690</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" s="16" t="s">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" s="16" t="s">
         <v>227</v>
       </c>
-      <c r="B170" s="4" t="s">
+      <c r="B171" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="C170" s="5">
+      <c r="C171" s="5">
         <v>1000</v>
       </c>
-      <c r="D170" s="4">
+      <c r="D171" s="4">
         <f t="shared" si="25"/>
         <v>8690</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" s="16" t="s">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" s="16" t="s">
         <v>229</v>
       </c>
-      <c r="B171" s="4" t="s">
+      <c r="B172" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="C171" s="5">
+      <c r="C172" s="5">
         <v>5000</v>
       </c>
-      <c r="D171" s="4">
+      <c r="D172" s="4">
         <f t="shared" si="25"/>
         <v>13690</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B172" s="4" t="s">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B173" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C172" s="5">
+      <c r="C173" s="5">
         <v>-10000</v>
       </c>
-      <c r="D172" s="4">
+      <c r="D173" s="4">
         <f t="shared" si="25"/>
         <v>3690</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173" s="16" t="s">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174" s="16" t="s">
         <v>231</v>
       </c>
-      <c r="B173" s="4" t="s">
+      <c r="B174" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="C173" s="5">
+      <c r="C174" s="5">
         <v>13000</v>
       </c>
-      <c r="D173" s="4">
-        <f t="shared" ref="D173:D178" si="26">D172+C173</f>
+      <c r="D174" s="4">
+        <f t="shared" ref="D174:D179" si="26">D173+C174</f>
         <v>16690</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B174" s="4" t="s">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B175" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C174" s="5">
+      <c r="C175" s="5">
         <v>-10000</v>
       </c>
-      <c r="D174" s="4">
+      <c r="D175" s="4">
         <f t="shared" si="26"/>
         <v>6690</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A175" s="16" t="s">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176" s="16" t="s">
         <v>233</v>
       </c>
-      <c r="B175" s="4" t="s">
+      <c r="B176" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C175" s="5">
+      <c r="C176" s="5">
         <v>3000</v>
       </c>
-      <c r="D175" s="4">
+      <c r="D176" s="4">
         <f t="shared" si="26"/>
         <v>9690</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176" s="16" t="s">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="B176" s="4" t="s">
+      <c r="B177" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="C176" s="5">
+      <c r="C177" s="5">
         <v>13000</v>
       </c>
-      <c r="D176" s="4">
+      <c r="D177" s="4">
         <f t="shared" si="26"/>
         <v>22690</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B177" s="4" t="s">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B178" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C177" s="5">
+      <c r="C178" s="5">
         <v>-20000</v>
       </c>
-      <c r="D177" s="4">
+      <c r="D178" s="4">
         <f t="shared" si="26"/>
         <v>2690</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A178" s="16" t="s">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A179" s="16" t="s">
         <v>235</v>
       </c>
-      <c r="B178" s="4" t="s">
+      <c r="B179" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C178" s="5">
+      <c r="C179" s="5">
         <v>3000</v>
       </c>
-      <c r="D178" s="4">
+      <c r="D179" s="4">
         <f t="shared" si="26"/>
         <v>5690</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A179" s="16" t="s">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180" s="16" t="s">
         <v>237</v>
       </c>
-      <c r="B179" s="4" t="s">
+      <c r="B180" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="C179" s="5">
+      <c r="C180" s="5">
         <v>16000</v>
       </c>
-      <c r="D179" s="4">
-        <f t="shared" ref="D179:D184" si="27">D178+C179</f>
+      <c r="D180" s="4">
+        <f t="shared" ref="D180:D185" si="27">D179+C180</f>
         <v>21690</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B180" s="4" t="s">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B181" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C180" s="5">
+      <c r="C181" s="5">
         <v>-20000</v>
       </c>
-      <c r="D180" s="4">
+      <c r="D181" s="4">
         <f t="shared" si="27"/>
         <v>1690</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="16" t="s">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182" s="16" t="s">
         <v>240</v>
       </c>
-      <c r="B181" s="4" t="s">
+      <c r="B182" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C181" s="5">
+      <c r="C182" s="5">
         <v>2000</v>
       </c>
-      <c r="D181" s="4">
+      <c r="D182" s="4">
         <f t="shared" si="27"/>
         <v>3690</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" s="16" t="s">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A183" s="16" t="s">
         <v>241</v>
       </c>
-      <c r="B182" s="4" t="s">
+      <c r="B183" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="C182" s="5">
+      <c r="C183" s="5">
         <v>1000</v>
       </c>
-      <c r="D182" s="4">
+      <c r="D183" s="4">
         <f t="shared" si="27"/>
         <v>4690</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183" s="16" t="s">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A184" s="16" t="s">
         <v>242</v>
       </c>
-      <c r="B183" s="4" t="s">
+      <c r="B184" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="C183" s="5">
+      <c r="C184" s="5">
         <v>6000</v>
       </c>
-      <c r="D183" s="4">
+      <c r="D184" s="4">
         <f t="shared" si="27"/>
         <v>10690</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B184" s="4" t="s">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B185" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C184" s="5">
+      <c r="C185" s="5">
         <v>-10000</v>
       </c>
-      <c r="D184" s="4">
+      <c r="D185" s="4">
         <f t="shared" si="27"/>
         <v>690</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A185" s="16" t="s">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" s="16" t="s">
         <v>244</v>
       </c>
-      <c r="B185" s="4" t="s">
+      <c r="B186" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="C185" s="5">
+      <c r="C186" s="5">
         <v>14000</v>
       </c>
-      <c r="D185" s="4">
-        <f>D184+C185</f>
+      <c r="D186" s="4">
+        <f t="shared" ref="D186:D191" si="28">D185+C186</f>
         <v>14690</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B186" s="4" t="s">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B187" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C186" s="5">
+      <c r="C187" s="5">
         <v>-10000</v>
       </c>
-      <c r="D186" s="4">
-        <f>D185+C186</f>
+      <c r="D187" s="4">
+        <f t="shared" si="28"/>
         <v>4690</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A187" s="16" t="s">
-        <v>245</v>
-      </c>
-      <c r="B187" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C187" s="5">
-        <v>3000</v>
-      </c>
-      <c r="D187" s="4">
-        <f>D186+C187</f>
-        <v>7690</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="16" t="s">
+        <v>245</v>
+      </c>
+      <c r="B188" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C188" s="5">
+        <v>3000</v>
+      </c>
+      <c r="D188" s="4">
+        <f t="shared" si="28"/>
+        <v>7690</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189" s="16" t="s">
         <v>247</v>
       </c>
-      <c r="B188" s="4" t="s">
+      <c r="B189" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="C188" s="5">
+      <c r="C189" s="5">
         <v>15000</v>
       </c>
-      <c r="D188" s="4">
-        <f>D187+C188</f>
+      <c r="D189" s="4">
+        <f t="shared" si="28"/>
         <v>22690</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B189" s="4" t="s">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B190" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C189" s="5">
+      <c r="C190" s="5">
         <v>-20000</v>
       </c>
-      <c r="D189" s="4">
-        <f>D188+C189</f>
+      <c r="D190" s="4">
+        <f t="shared" si="28"/>
         <v>2690</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A190" s="16" t="s">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A191" s="16" t="s">
         <v>248</v>
       </c>
-      <c r="B190" s="4" t="s">
+      <c r="B191" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="C190" s="5">
+      <c r="C191" s="5">
         <v>6000</v>
       </c>
-      <c r="D190" s="4">
-        <f>D189+C190</f>
+      <c r="D191" s="4">
+        <f t="shared" si="28"/>
         <v>8690</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A192" s="16" t="s">
+        <v>250</v>
+      </c>
+      <c r="B192" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="C192" s="5">
+        <v>15000</v>
+      </c>
+      <c r="D192" s="4">
+        <f>D191+C192</f>
+        <v>23690</v>
+      </c>
+    </row>
+    <row r="193" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B193" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="C193" s="5">
+        <v>-20000</v>
+      </c>
+      <c r="D193" s="4">
+        <f>D192+C193</f>
+        <v>3690</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
duy tinh tien loi co diem 2tr
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="256">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -775,6 +775,18 @@
   </si>
   <si>
     <t>Duy tính tiền lời 15tr</t>
+  </si>
+  <si>
+    <t>07/11/24</t>
+  </si>
+  <si>
+    <t>03/12/24</t>
+  </si>
+  <si>
+    <t>03/12/2024</t>
+  </si>
+  <si>
+    <t>Duy tính tiền lời 2tr</t>
   </si>
 </sst>
 </file>
@@ -1275,11 +1287,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K193"/>
+  <dimension ref="A1:K194"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q11" sqref="Q11"/>
+      <pane ySplit="1" topLeftCell="A165" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H199" sqref="H199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4287,7 +4299,7 @@
         <v>23690</v>
       </c>
     </row>
-    <row r="193" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B193" s="4" t="s">
         <v>198</v>
       </c>
@@ -4297,6 +4309,21 @@
       <c r="D193" s="4">
         <f>D192+C193</f>
         <v>3690</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A194" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="B194" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="C194" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D194" s="4">
+        <f>D193+C194</f>
+        <v>5690</v>
       </c>
     </row>
   </sheetData>
@@ -4449,11 +4476,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4680,8 +4707,8 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
-        <v>45603</v>
+      <c r="A14" s="16" t="s">
+        <v>252</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>36</v>
@@ -4693,6 +4720,147 @@
         <f t="shared" si="1"/>
         <v>3500</v>
       </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>253</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="5">
+        <v>-500</v>
+      </c>
+      <c r="D15" s="4">
+        <f>D14+C15</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="16"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="16"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="16"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="16"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="16"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="16"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="16"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="16"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="16"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="16"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="16"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="16"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="16"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="16"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="16"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="16"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="16"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="16"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="16"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="16"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="16"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="16"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="16"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="16"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="16"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="16"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="16"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="16"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="16"/>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="16"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="16"/>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="16"/>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="16"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="16"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="16"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="16"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="16"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="16"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="16"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="16"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="16"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
duy tinh tien loi co diem ngay 13
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="CÔ DIỄM" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="259">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -790,6 +790,12 @@
   </si>
   <si>
     <t>06/12/2024</t>
+  </si>
+  <si>
+    <t>13/12/2024</t>
+  </si>
+  <si>
+    <t>Duy tính tiền lời 7tr</t>
   </si>
 </sst>
 </file>
@@ -983,11 +989,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1293,11 +1299,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K194"/>
+  <dimension ref="A1:K197"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
+      <selection pane="bottomLeft" activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1327,10 +1333,10 @@
       <c r="D1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="H1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="29"/>
+      <c r="I1" s="30"/>
       <c r="J1" s="15"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1373,8 +1379,8 @@
         <v>20</v>
       </c>
       <c r="J3" s="4">
-        <f>SUM(I3:I75)</f>
-        <v>680</v>
+        <f>SUM(I3:I76)</f>
+        <v>690</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1403,7 +1409,7 @@
         <v>-10000</v>
       </c>
       <c r="D5" s="4">
-        <f t="shared" ref="D5:D9" si="0">D4+C5</f>
+        <f t="shared" ref="D5:D10" si="0">D4+C5</f>
         <v>8490</v>
       </c>
       <c r="H5" s="16" t="s">
@@ -1450,21 +1456,8 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D8" s="4">
-        <f t="shared" si="0"/>
-        <v>2490</v>
-      </c>
       <c r="H8" s="16" t="s">
-        <v>7</v>
+        <v>257</v>
       </c>
       <c r="I8" s="5">
         <v>10</v>
@@ -1472,59 +1465,62 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D9" s="4">
+        <f>D7+C9</f>
+        <v>2490</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C10" s="5">
         <v>3000</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D10" s="4">
         <f t="shared" si="0"/>
         <v>5490</v>
       </c>
-      <c r="H9" s="16" t="s">
+      <c r="H10" s="16" t="s">
         <v>8</v>
-      </c>
-      <c r="I9" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="5">
-        <v>3000</v>
-      </c>
-      <c r="D10" s="4">
-        <f>D9+C10</f>
-        <v>8490</v>
-      </c>
-      <c r="H10" s="16" t="s">
-        <v>9</v>
       </c>
       <c r="I10" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>24</v>
+      </c>
       <c r="B11" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="5">
-        <v>4400</v>
+        <v>3000</v>
       </c>
       <c r="D11" s="4">
         <f>D10+C11</f>
-        <v>12890</v>
+        <v>8490</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="I11" s="5">
         <v>10</v>
@@ -1532,36 +1528,35 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="5">
-        <v>-10000</v>
+        <v>4400</v>
       </c>
       <c r="D12" s="4">
         <f>D11+C12</f>
-        <v>2890</v>
+        <v>12890</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="I12" s="5">
         <v>10</v>
       </c>
-      <c r="K12" s="14"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C13" s="5">
-        <v>1600</v>
+        <v>-10000</v>
       </c>
       <c r="D13" s="4">
-        <f t="shared" ref="D13:D20" si="1">D12+C13</f>
-        <v>4490</v>
+        <f>D12+C13</f>
+        <v>2890</v>
       </c>
       <c r="H13" s="16" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="I13" s="5">
         <v>10</v>
@@ -1570,162 +1565,162 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="5">
+        <v>1600</v>
+      </c>
+      <c r="D14" s="4">
+        <f t="shared" ref="D14:D21" si="1">D13+C14</f>
+        <v>4490</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="I14" s="5">
+        <v>10</v>
+      </c>
+      <c r="K14" s="14"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C15" s="5">
         <v>3000</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D15" s="4">
         <f t="shared" si="1"/>
         <v>7490</v>
       </c>
-      <c r="H14" s="16" t="s">
+      <c r="H15" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="I14" s="5">
+      <c r="I15" s="5">
         <v>10</v>
       </c>
-      <c r="K14" s="14"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
+      <c r="K15" s="14"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B16" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C16" s="5">
         <v>2000</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D16" s="4">
         <f t="shared" si="1"/>
         <v>9490</v>
       </c>
-      <c r="H15" s="16" t="s">
+      <c r="H16" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="I15" s="5">
+      <c r="I16" s="5">
         <v>10</v>
       </c>
-      <c r="K15" s="14"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+      <c r="K16" s="14"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B17" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C17" s="5">
         <v>3000</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D17" s="4">
         <f t="shared" si="1"/>
         <v>12490</v>
       </c>
-      <c r="H16" s="16" t="s">
+      <c r="H17" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="I16" s="5">
+      <c r="I17" s="5">
         <v>10</v>
       </c>
-      <c r="K16" s="14"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
+      <c r="K17" s="14"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C18" s="5">
         <v>-10000</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D18" s="4">
         <f t="shared" si="1"/>
         <v>2490</v>
       </c>
-      <c r="H17" s="16" t="s">
+      <c r="H18" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="I17" s="5">
+      <c r="I18" s="5">
         <v>10</v>
       </c>
-      <c r="K17" s="14"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
+      <c r="K18" s="14"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B19" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C19" s="5">
         <v>4960</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D19" s="4">
         <f t="shared" si="1"/>
         <v>7450</v>
       </c>
-      <c r="H18" s="16" t="s">
+      <c r="H19" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="I18" s="5">
+      <c r="I19" s="5">
         <v>10</v>
       </c>
-      <c r="K18" s="14"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
+      <c r="K19" s="14"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B20" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C20" s="5">
         <v>4000</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D20" s="4">
         <f t="shared" si="1"/>
         <v>11450</v>
       </c>
-      <c r="H19" s="16" t="s">
+      <c r="H20" s="16" t="s">
         <v>215</v>
       </c>
-      <c r="I19" s="5">
+      <c r="I20" s="5">
         <v>20</v>
       </c>
-      <c r="K19" s="14"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="4" t="s">
+      <c r="K20" s="14"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C21" s="5">
         <v>-10000</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D21" s="4">
         <f t="shared" si="1"/>
         <v>1450</v>
       </c>
-      <c r="H20" s="16" t="s">
+      <c r="H21" s="16" t="s">
         <v>231</v>
-      </c>
-      <c r="I20" s="5">
-        <v>10</v>
-      </c>
-      <c r="K20" s="14"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="5">
-        <v>7640</v>
-      </c>
-      <c r="D21" s="4">
-        <f t="shared" ref="D21:D26" si="2">D20+C21</f>
-        <v>9090</v>
-      </c>
-      <c r="H21" s="16" t="s">
-        <v>244</v>
       </c>
       <c r="I21" s="5">
         <v>10</v>
@@ -1734,17 +1729,17 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="C22" s="5">
-        <v>3000</v>
+        <v>7640</v>
       </c>
       <c r="D22" s="4">
-        <f>D21+C22</f>
-        <v>12090</v>
+        <f t="shared" ref="D22:D27" si="2">D21+C22</f>
+        <v>9090</v>
       </c>
       <c r="H22" s="16" t="s">
-        <v>70</v>
+        <v>244</v>
       </c>
       <c r="I22" s="5">
         <v>10</v>
@@ -1753,102 +1748,99 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="5">
+        <v>3000</v>
+      </c>
+      <c r="D23" s="4">
+        <f>D22+C23</f>
+        <v>12090</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="I23" s="5">
+        <v>10</v>
+      </c>
+      <c r="K23" s="14"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C24" s="5">
         <v>-10000</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D24" s="4">
         <f t="shared" si="2"/>
         <v>2090</v>
       </c>
-      <c r="H23" s="16" t="s">
+      <c r="H24" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="I23" s="5">
+      <c r="I24" s="5">
         <v>10</v>
       </c>
-      <c r="K23" s="14"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="4" t="s">
+      <c r="K24" s="14"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C25" s="5">
         <v>800</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D25" s="4">
         <f t="shared" si="2"/>
         <v>2890</v>
       </c>
-      <c r="H24" s="16" t="s">
+      <c r="H25" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="I24" s="5">
+      <c r="I25" s="5">
         <v>10</v>
       </c>
-      <c r="K24" s="14"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="16" t="s">
+      <c r="K25" s="14"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B26" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C26" s="5">
         <v>2000</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D26" s="4">
         <f t="shared" si="2"/>
         <v>4890</v>
       </c>
-      <c r="H25" s="16" t="s">
+      <c r="H26" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="I25" s="5">
+      <c r="I26" s="5">
         <v>10</v>
       </c>
-      <c r="K25" s="14"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="16" t="s">
+      <c r="K26" s="14"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B27" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C27" s="5">
         <v>4000</v>
       </c>
-      <c r="D26" s="4">
+      <c r="D27" s="4">
         <f t="shared" si="2"/>
         <v>8890</v>
       </c>
-      <c r="H26" s="16" t="s">
+      <c r="H27" s="16" t="s">
         <v>11</v>
-      </c>
-      <c r="I26" s="5">
-        <v>10</v>
-      </c>
-      <c r="K26" s="14"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C27" s="5">
-        <v>4000</v>
-      </c>
-      <c r="D27" s="4">
-        <f t="shared" ref="D27:D32" si="3">D26+C27</f>
-        <v>12890</v>
-      </c>
-      <c r="H27" s="16" t="s">
-        <v>24</v>
       </c>
       <c r="I27" s="5">
         <v>10</v>
@@ -1856,119 +1848,119 @@
       <c r="K27" s="14"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="16" t="s">
+        <v>59</v>
+      </c>
       <c r="B28" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="5">
+        <v>4000</v>
+      </c>
+      <c r="D28" s="4">
+        <f t="shared" ref="D28:D33" si="3">D27+C28</f>
+        <v>12890</v>
+      </c>
+      <c r="H28" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="I28" s="5">
+        <v>10</v>
+      </c>
+      <c r="K28" s="14"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C29" s="5">
         <v>5000</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D29" s="4">
         <f t="shared" si="3"/>
         <v>17890</v>
       </c>
-      <c r="H28" s="16" t="s">
+      <c r="H29" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="I28" s="5">
+      <c r="I29" s="5">
         <v>10</v>
       </c>
-      <c r="K28" s="14"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="4" t="s">
+      <c r="K29" s="14"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C30" s="5">
         <v>-10000</v>
       </c>
-      <c r="D29" s="4">
+      <c r="D30" s="4">
         <f t="shared" si="3"/>
         <v>7890</v>
       </c>
-      <c r="H29" s="16" t="s">
+      <c r="H30" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="I29" s="5">
+      <c r="I30" s="5">
         <v>10</v>
       </c>
-      <c r="K29" s="14"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="16">
+      <c r="K30" s="14"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="16">
         <v>44969</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B31" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C31" s="5">
         <v>900</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D31" s="4">
         <f t="shared" si="3"/>
         <v>8790</v>
       </c>
-      <c r="H30" s="16" t="s">
+      <c r="H31" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="I30" s="5">
+      <c r="I31" s="5">
         <v>10</v>
       </c>
-      <c r="K30" s="14"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B31" s="4" t="s">
+      <c r="K31" s="14"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C32" s="5">
         <v>4000</v>
       </c>
-      <c r="D31" s="4">
+      <c r="D32" s="4">
         <f t="shared" si="3"/>
         <v>12790</v>
       </c>
-      <c r="H31" s="16" t="s">
+      <c r="H32" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="I31" s="5">
+      <c r="I32" s="5">
         <v>10</v>
       </c>
-      <c r="K31" s="14"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B32" s="4" t="s">
+      <c r="K32" s="14"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C33" s="5">
         <v>-10000</v>
       </c>
-      <c r="D32" s="4">
+      <c r="D33" s="4">
         <f t="shared" si="3"/>
         <v>2790</v>
       </c>
-      <c r="H32" s="16" t="s">
+      <c r="H33" s="16" t="s">
         <v>129</v>
-      </c>
-      <c r="I32" s="5">
-        <v>10</v>
-      </c>
-      <c r="K32" s="14"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C33" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D33" s="4">
-        <f t="shared" ref="D33:D41" si="4">D32+C33</f>
-        <v>4790</v>
-      </c>
-      <c r="H33" s="16" t="s">
-        <v>135</v>
       </c>
       <c r="I33" s="5">
         <v>10</v>
@@ -1977,112 +1969,125 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D34" s="4">
+        <f t="shared" ref="D34:D42" si="4">D33+C34</f>
+        <v>4790</v>
+      </c>
+      <c r="H34" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="I34" s="5">
+        <v>10</v>
+      </c>
+      <c r="K34" s="14"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B35" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C35" s="5">
         <v>700</v>
       </c>
-      <c r="D34" s="4">
+      <c r="D35" s="4">
         <f t="shared" si="4"/>
         <v>5490</v>
       </c>
-      <c r="H34" s="16" t="s">
+      <c r="H35" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="I34" s="5">
+      <c r="I35" s="5">
         <v>10</v>
       </c>
-      <c r="K34" s="14"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B35" s="4" t="s">
+      <c r="K35" s="14"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C35" s="5">
+      <c r="C36" s="5">
         <v>4000</v>
       </c>
-      <c r="D35" s="4">
+      <c r="D36" s="4">
         <f t="shared" si="4"/>
         <v>9490</v>
       </c>
-      <c r="H35" s="16" t="s">
+      <c r="H36" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="I35" s="5">
+      <c r="I36" s="5">
         <v>10</v>
       </c>
-      <c r="K35" s="14"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="16" t="s">
+      <c r="K36" s="14"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B37" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C36" s="5">
+      <c r="C37" s="5">
         <v>600</v>
       </c>
-      <c r="D36" s="4">
+      <c r="D37" s="4">
         <f t="shared" si="4"/>
         <v>10090</v>
       </c>
-      <c r="H36" s="16" t="s">
+      <c r="H37" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="I36" s="5">
+      <c r="I37" s="5">
         <v>10</v>
       </c>
-      <c r="K36" s="14"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B37" s="4" t="s">
+      <c r="K37" s="14"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B38" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="5">
+      <c r="C38" s="5">
         <v>-10000</v>
       </c>
-      <c r="D37" s="4">
+      <c r="D38" s="4">
         <f t="shared" si="4"/>
         <v>90</v>
       </c>
-      <c r="H37" s="16" t="s">
+      <c r="H38" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="I37" s="5">
+      <c r="I38" s="5">
         <v>10</v>
       </c>
-      <c r="K37" s="14"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="16" t="s">
+      <c r="K38" s="14"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B39" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C38" s="5">
+      <c r="C39" s="5">
         <f>700+5000+300+600+400+1000+800</f>
         <v>8800</v>
       </c>
-      <c r="D38" s="4">
+      <c r="D39" s="4">
         <f t="shared" si="4"/>
         <v>8890</v>
       </c>
-      <c r="H38" s="16" t="s">
+      <c r="H39" s="16" t="s">
         <v>234</v>
-      </c>
-      <c r="I38" s="5">
-        <v>20</v>
-      </c>
-      <c r="K38" s="14"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H39" s="16" t="s">
-        <v>247</v>
       </c>
       <c r="I39" s="5">
         <v>20</v>
@@ -2090,59 +2095,46 @@
       <c r="K39" s="14"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B40" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C40" s="5">
-        <v>6000</v>
-      </c>
-      <c r="D40" s="4">
-        <f>D38+C40</f>
-        <v>14890</v>
-      </c>
       <c r="H40" s="16" t="s">
-        <v>12</v>
+        <v>247</v>
       </c>
       <c r="I40" s="5">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="K40" s="14"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C41" s="5">
+        <v>6000</v>
+      </c>
+      <c r="D41" s="4">
+        <f>D39+C41</f>
+        <v>14890</v>
+      </c>
+      <c r="H41" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="I41" s="5">
+        <v>10</v>
+      </c>
+      <c r="K41" s="14"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B42" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C41" s="5">
+      <c r="C42" s="5">
         <v>-10000</v>
       </c>
-      <c r="D41" s="4">
+      <c r="D42" s="4">
         <f t="shared" si="4"/>
         <v>4890</v>
       </c>
-      <c r="H41" s="16" t="s">
+      <c r="H42" s="16" t="s">
         <v>43</v>
-      </c>
-      <c r="I41" s="5">
-        <v>10</v>
-      </c>
-      <c r="K41" s="14"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C42" s="5">
-        <v>500</v>
-      </c>
-      <c r="D42" s="4">
-        <f t="shared" ref="D42:D47" si="5">D41+C42</f>
-        <v>5390</v>
-      </c>
-      <c r="H42" s="16" t="s">
-        <v>139</v>
       </c>
       <c r="I42" s="5">
         <v>10</v>
@@ -2150,116 +2142,119 @@
       <c r="K42" s="14"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="16" t="s">
+        <v>75</v>
+      </c>
       <c r="B43" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C43" s="5">
+        <v>500</v>
+      </c>
+      <c r="D43" s="4">
+        <f t="shared" ref="D43:D48" si="5">D42+C43</f>
+        <v>5390</v>
+      </c>
+      <c r="H43" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="I43" s="5">
+        <v>10</v>
+      </c>
+      <c r="K43" s="14"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B44" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C43" s="5">
+      <c r="C44" s="5">
         <v>700</v>
       </c>
-      <c r="D43" s="4">
+      <c r="D44" s="4">
         <f t="shared" si="5"/>
         <v>6090</v>
       </c>
-      <c r="H43" s="16" t="s">
+      <c r="H44" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="I43" s="5">
+      <c r="I44" s="5">
         <v>10</v>
       </c>
-      <c r="K43" s="14"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B44" s="4" t="s">
+      <c r="K44" s="14"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B45" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C45" s="5">
         <v>1500</v>
       </c>
-      <c r="D44" s="4">
+      <c r="D45" s="4">
         <f t="shared" si="5"/>
         <v>7590</v>
       </c>
-      <c r="H44" s="16" t="s">
+      <c r="H45" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="I44" s="5">
+      <c r="I45" s="5">
         <v>10</v>
       </c>
-      <c r="K44" s="14"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B45" s="4" t="s">
+      <c r="K45" s="14"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B46" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C45" s="5">
+      <c r="C46" s="5">
         <v>5000</v>
       </c>
-      <c r="D45" s="4">
+      <c r="D46" s="4">
         <f t="shared" si="5"/>
         <v>12590</v>
       </c>
-      <c r="H45" s="16" t="s">
+      <c r="H46" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="I45" s="5">
+      <c r="I46" s="5">
         <v>10</v>
       </c>
-      <c r="K45" s="14"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B46" s="4" t="s">
+      <c r="K46" s="14"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B47" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C46" s="5">
+      <c r="C47" s="5">
         <v>-10000</v>
       </c>
-      <c r="D46" s="4">
+      <c r="D47" s="4">
         <f t="shared" si="5"/>
         <v>2590</v>
       </c>
-      <c r="H46" s="16" t="s">
+      <c r="H47" s="16" t="s">
         <v>157</v>
       </c>
-      <c r="I46" s="5">
+      <c r="I47" s="5">
         <v>20</v>
       </c>
-      <c r="K46" s="14"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="16" t="s">
+      <c r="K47" s="14"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B48" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C48" s="5">
         <v>2000</v>
       </c>
-      <c r="D47" s="4">
+      <c r="D48" s="4">
         <f t="shared" si="5"/>
         <v>4590</v>
       </c>
-      <c r="H47" s="16" t="s">
+      <c r="H48" s="16" t="s">
         <v>158</v>
-      </c>
-      <c r="I47" s="5">
-        <v>10</v>
-      </c>
-      <c r="K47" s="14"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B48" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C48" s="5">
-        <v>700</v>
-      </c>
-      <c r="D48" s="4">
-        <f t="shared" ref="D48:D53" si="6">D47+C48</f>
-        <v>5290</v>
-      </c>
-      <c r="H48" s="16" t="s">
-        <v>159</v>
       </c>
       <c r="I48" s="5">
         <v>10</v>
@@ -2267,9 +2262,6 @@
       <c r="K48" s="14"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="16" t="s">
-        <v>82</v>
-      </c>
       <c r="B49" s="4" t="s">
         <v>77</v>
       </c>
@@ -2277,118 +2269,118 @@
         <v>700</v>
       </c>
       <c r="D49" s="4">
+        <f t="shared" ref="D49:D54" si="6">D48+C49</f>
+        <v>5290</v>
+      </c>
+      <c r="H49" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="I49" s="5">
+        <v>10</v>
+      </c>
+      <c r="K49" s="14"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C50" s="5">
+        <v>700</v>
+      </c>
+      <c r="D50" s="4">
         <f t="shared" si="6"/>
         <v>5990</v>
       </c>
-      <c r="H49" s="16" t="s">
+      <c r="H50" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="I49" s="5">
+      <c r="I50" s="5">
         <v>10</v>
       </c>
-      <c r="K49" s="14"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="16" t="s">
+      <c r="K50" s="14"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B51" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C50" s="5">
+      <c r="C51" s="5">
         <v>700</v>
       </c>
-      <c r="D50" s="4">
+      <c r="D51" s="4">
         <f t="shared" si="6"/>
         <v>6690</v>
       </c>
-      <c r="H50" s="16" t="s">
+      <c r="H51" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="I50" s="5">
+      <c r="I51" s="5">
         <v>10</v>
       </c>
-      <c r="K50" s="14"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="16" t="s">
+      <c r="K51" s="14"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B52" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C51" s="5">
+      <c r="C52" s="5">
         <v>4000</v>
       </c>
-      <c r="D51" s="4">
+      <c r="D52" s="4">
         <f t="shared" si="6"/>
         <v>10690</v>
       </c>
-      <c r="H51" s="16" t="s">
+      <c r="H52" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="I51" s="5">
+      <c r="I52" s="5">
         <v>10</v>
       </c>
-      <c r="K51" s="14"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B52" s="4" t="s">
+      <c r="K52" s="14"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B53" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C52" s="5">
+      <c r="C53" s="5">
         <v>-10000</v>
       </c>
-      <c r="D52" s="4">
+      <c r="D53" s="4">
         <f t="shared" si="6"/>
         <v>690</v>
       </c>
-      <c r="H52" s="16" t="s">
+      <c r="H53" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="I52" s="5">
+      <c r="I53" s="5">
         <v>10</v>
       </c>
-      <c r="K52" s="14"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="16" t="s">
+      <c r="K53" s="14"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B54" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C53" s="5">
+      <c r="C54" s="5">
         <v>1000</v>
       </c>
-      <c r="D53" s="4">
+      <c r="D54" s="4">
         <f t="shared" si="6"/>
         <v>1690</v>
       </c>
-      <c r="H53" s="16" t="s">
+      <c r="H54" s="16" t="s">
         <v>151</v>
-      </c>
-      <c r="I53" s="5">
-        <v>10</v>
-      </c>
-      <c r="K53" s="14"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C54" s="5">
-        <v>7000</v>
-      </c>
-      <c r="D54" s="4">
-        <f t="shared" ref="D54:D58" si="7">D53+C54</f>
-        <v>8690</v>
-      </c>
-      <c r="H54" s="16" t="s">
-        <v>150</v>
       </c>
       <c r="I54" s="5">
         <v>10</v>
@@ -2396,84 +2388,97 @@
       <c r="K54" s="14"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="16" t="s">
+        <v>88</v>
+      </c>
       <c r="B55" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C55" s="5">
+        <v>7000</v>
+      </c>
+      <c r="D55" s="4">
+        <f t="shared" ref="D55:D59" si="7">D54+C55</f>
+        <v>8690</v>
+      </c>
+      <c r="H55" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="I55" s="5">
+        <v>10</v>
+      </c>
+      <c r="K55" s="14"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B56" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C55" s="5">
+      <c r="C56" s="5">
         <v>10000</v>
       </c>
-      <c r="D55" s="4">
+      <c r="D56" s="4">
         <f t="shared" si="7"/>
         <v>18690</v>
       </c>
-      <c r="H55" s="16" t="s">
+      <c r="H56" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="I55" s="5">
+      <c r="I56" s="5">
         <v>10</v>
       </c>
-      <c r="K55" s="14"/>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B56" s="4" t="s">
+      <c r="K56" s="14"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B57" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C56" s="5">
+      <c r="C57" s="5">
         <v>-10000</v>
       </c>
-      <c r="D56" s="4">
+      <c r="D57" s="4">
         <f t="shared" si="7"/>
         <v>8690</v>
       </c>
-      <c r="H56" s="16" t="s">
+      <c r="H57" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="I56" s="5">
+      <c r="I57" s="5">
         <v>10</v>
       </c>
-      <c r="K56" s="14"/>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B57" s="4" t="s">
+      <c r="K57" s="14"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B58" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C57" s="5">
+      <c r="C58" s="5">
         <v>1700</v>
       </c>
-      <c r="D57" s="4">
+      <c r="D58" s="4">
         <f t="shared" si="7"/>
         <v>10390</v>
       </c>
-      <c r="H57" s="16" t="s">
+      <c r="H58" s="16" t="s">
         <v>221</v>
       </c>
-      <c r="I57" s="5">
+      <c r="I58" s="5">
         <v>10</v>
       </c>
-      <c r="K57" s="14"/>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B58" s="4" t="s">
+      <c r="K58" s="14"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B59" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C58" s="5">
+      <c r="C59" s="5">
         <v>-10000</v>
       </c>
-      <c r="D58" s="4">
+      <c r="D59" s="4">
         <f t="shared" si="7"/>
         <v>390</v>
       </c>
-      <c r="H58" s="16" t="s">
+      <c r="H59" s="16" t="s">
         <v>237</v>
-      </c>
-      <c r="I58" s="5">
-        <v>20</v>
-      </c>
-      <c r="K58" s="14"/>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H59" s="16" t="s">
-        <v>250</v>
       </c>
       <c r="I59" s="5">
         <v>20</v>
@@ -2481,18 +2486,8 @@
       <c r="K59" s="14"/>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B60" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C60" s="5">
-        <v>6000</v>
-      </c>
-      <c r="D60" s="4">
-        <f>D58+C60</f>
-        <v>6390</v>
-      </c>
       <c r="H60" s="16" t="s">
-        <v>207</v>
+        <v>250</v>
       </c>
       <c r="I60" s="5">
         <v>20</v>
@@ -2500,270 +2495,277 @@
       <c r="K60" s="14"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61" s="16" t="s">
-        <v>94</v>
-      </c>
       <c r="B61" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C61" s="5">
-        <v>2000</v>
+        <v>6000</v>
       </c>
       <c r="D61" s="4">
-        <f t="shared" ref="D61:D66" si="8">D60+C61</f>
-        <v>8390</v>
+        <f>D59+C61</f>
+        <v>6390</v>
       </c>
       <c r="H61" s="16" t="s">
-        <v>187</v>
+        <v>207</v>
       </c>
       <c r="I61" s="5">
-        <v>10</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="K61" s="14"/>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C62" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D62" s="4">
+        <f t="shared" ref="D62:D67" si="8">D61+C62</f>
+        <v>8390</v>
+      </c>
+      <c r="H62" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="I62" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B63" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C62" s="5">
+      <c r="C63" s="5">
         <v>5000</v>
       </c>
-      <c r="D62" s="4">
+      <c r="D63" s="4">
         <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B63" s="4" t="s">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B64" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C63" s="5">
+      <c r="C64" s="5">
         <v>-10000</v>
       </c>
-      <c r="D63" s="4">
+      <c r="D64" s="4">
         <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64" s="16" t="s">
+    <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B65" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C64" s="5">
+      <c r="C65" s="5">
         <v>1000</v>
       </c>
-      <c r="D64" s="4">
+      <c r="D65" s="4">
         <f t="shared" si="8"/>
         <v>4390</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B65" s="4" t="s">
+    <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C65" s="5">
+      <c r="C66" s="5">
         <v>9000</v>
       </c>
-      <c r="D65" s="4">
+      <c r="D66" s="4">
         <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B66" s="4" t="s">
+    <row r="67" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C66" s="5">
+      <c r="C67" s="5">
         <v>-10000</v>
       </c>
-      <c r="D66" s="4">
+      <c r="D67" s="4">
         <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B67" s="4" t="s">
+    <row r="68" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C67" s="5">
+      <c r="C68" s="5">
         <v>2000</v>
       </c>
-      <c r="D67" s="4">
-        <f t="shared" ref="D67:D72" si="9">D66+C67</f>
+      <c r="D68" s="4">
+        <f t="shared" ref="D68:D73" si="9">D67+C68</f>
         <v>5390</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B68" s="4" t="s">
+    <row r="69" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C68" s="5">
+      <c r="C69" s="5">
         <v>6000</v>
       </c>
-      <c r="D68" s="4">
+      <c r="D69" s="4">
         <f t="shared" si="9"/>
         <v>11390</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B69" s="4" t="s">
+    <row r="70" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C69" s="5">
+      <c r="C70" s="5">
         <v>-10000</v>
       </c>
-      <c r="D69" s="4">
+      <c r="D70" s="4">
         <f t="shared" si="9"/>
         <v>1390</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B70" s="4" t="s">
+    <row r="71" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C70" s="5">
+      <c r="C71" s="5">
         <v>400</v>
       </c>
-      <c r="D70" s="4">
+      <c r="D71" s="4">
         <f t="shared" si="9"/>
         <v>1790</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="16" t="s">
+    <row r="72" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B72" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C71" s="5">
+      <c r="C72" s="5">
         <v>2000</v>
       </c>
-      <c r="D71" s="4">
+      <c r="D72" s="4">
         <f t="shared" si="9"/>
         <v>3790</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="16" t="s">
+    <row r="73" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B73" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C72" s="5">
+      <c r="C73" s="5">
         <v>6000</v>
       </c>
-      <c r="D72" s="4">
+      <c r="D73" s="4">
         <f t="shared" si="9"/>
         <v>9790</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="16" t="s">
+    <row r="74" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B74" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C73" s="5">
+      <c r="C74" s="5">
         <v>1000</v>
       </c>
-      <c r="D73" s="4">
-        <f t="shared" ref="D73:D78" si="10">D72+C73</f>
+      <c r="D74" s="4">
+        <f t="shared" ref="D74:D79" si="10">D73+C74</f>
         <v>10790</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B74" s="4" t="s">
+    <row r="75" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B75" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C74" s="5">
+      <c r="C75" s="5">
         <v>-10000</v>
       </c>
-      <c r="D74" s="4">
+      <c r="D75" s="4">
         <f t="shared" si="10"/>
         <v>790</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="16" t="s">
+    <row r="76" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="B76" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C75" s="5">
+      <c r="C76" s="5">
         <v>800</v>
       </c>
-      <c r="D75" s="4">
+      <c r="D76" s="4">
         <f t="shared" si="10"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="16" t="s">
+    <row r="77" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B77" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C76" s="5">
+      <c r="C77" s="5">
         <v>5000</v>
       </c>
-      <c r="D76" s="4">
+      <c r="D77" s="4">
         <f t="shared" si="10"/>
         <v>6590</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="16" t="s">
+    <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="B78" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C77" s="5">
+      <c r="C78" s="5">
         <v>6000</v>
       </c>
-      <c r="D77" s="4">
+      <c r="D78" s="4">
         <f t="shared" si="10"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B78" s="4" t="s">
+    <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B79" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C78" s="5">
+      <c r="C79" s="5">
         <v>-10000</v>
       </c>
-      <c r="D78" s="4">
+      <c r="D79" s="4">
         <f t="shared" si="10"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="16" t="s">
+    <row r="80" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="B79" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C79" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D79" s="4">
-        <f t="shared" ref="D79:D85" si="11">D78+C79</f>
-        <v>4590</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B80" s="4" t="s">
         <v>65</v>
       </c>
@@ -2771,929 +2773,929 @@
         <v>2000</v>
       </c>
       <c r="D80" s="4">
+        <f t="shared" ref="D80:D86" si="11">D79+C80</f>
+        <v>4590</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B81" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C81" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D81" s="4">
         <f t="shared" si="11"/>
         <v>6590</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B81" s="4" t="s">
+    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B82" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C81" s="5">
+      <c r="C82" s="5">
         <v>7000</v>
       </c>
-      <c r="D81" s="4">
+      <c r="D82" s="4">
         <f t="shared" si="11"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B82" s="4" t="s">
+    <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B83" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C82" s="5">
+      <c r="C83" s="5">
         <v>-10000</v>
       </c>
-      <c r="D82" s="4">
+      <c r="D83" s="4">
         <f t="shared" si="11"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="16" t="s">
+    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="B84" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C83" s="5">
+      <c r="C84" s="5">
         <v>2000</v>
       </c>
-      <c r="D83" s="4">
+      <c r="D84" s="4">
         <f t="shared" si="11"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="16" t="s">
+    <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="B84" s="4" t="s">
+      <c r="B85" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C84" s="5">
+      <c r="C85" s="5">
         <v>6000</v>
       </c>
-      <c r="D84" s="4">
+      <c r="D85" s="4">
         <f t="shared" si="11"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B85" s="4" t="s">
+    <row r="86" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B86" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C85" s="5">
+      <c r="C86" s="5">
         <v>-10000</v>
       </c>
-      <c r="D85" s="4">
+      <c r="D86" s="4">
         <f t="shared" si="11"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="16" t="s">
+    <row r="87" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="B87" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C86" s="5">
+      <c r="C87" s="5">
         <v>2000</v>
       </c>
-      <c r="D86" s="4">
-        <f t="shared" ref="D86:D91" si="12">D85+C86</f>
+      <c r="D87" s="4">
+        <f t="shared" ref="D87:D92" si="12">D86+C87</f>
         <v>3590</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="16" t="s">
+    <row r="88" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="B87" s="4" t="s">
+      <c r="B88" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C87" s="5">
+      <c r="C88" s="5">
         <v>7000</v>
       </c>
-      <c r="D87" s="4">
+      <c r="D88" s="4">
         <f t="shared" si="12"/>
         <v>10590</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B88" s="4" t="s">
+    <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B89" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C88" s="5">
+      <c r="C89" s="5">
         <v>-10000</v>
       </c>
-      <c r="D88" s="4">
+      <c r="D89" s="4">
         <f t="shared" si="12"/>
         <v>590</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B89" s="4" t="s">
+    <row r="90" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B90" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C89" s="5">
+      <c r="C90" s="5">
         <v>12000</v>
       </c>
-      <c r="D89" s="4">
+      <c r="D90" s="4">
         <f t="shared" si="12"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B90" s="4" t="s">
+    <row r="91" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B91" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C90" s="5">
+      <c r="C91" s="5">
         <v>-10000</v>
       </c>
-      <c r="D90" s="4">
+      <c r="D91" s="4">
         <f t="shared" si="12"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B91" s="4" t="s">
+    <row r="92" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B92" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C91" s="5">
+      <c r="C92" s="5">
         <v>2000</v>
       </c>
-      <c r="D91" s="4">
+      <c r="D92" s="4">
         <f t="shared" si="12"/>
         <v>4590</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="16" t="s">
+    <row r="93" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="B92" s="4" t="s">
+      <c r="B93" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C92" s="5">
+      <c r="C93" s="5">
         <v>2000</v>
       </c>
-      <c r="D92" s="4">
-        <f t="shared" ref="D92:D97" si="13">D91+C92</f>
+      <c r="D93" s="4">
+        <f t="shared" ref="D93:D98" si="13">D92+C93</f>
         <v>6590</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="16" t="s">
+    <row r="94" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="B93" s="4" t="s">
+      <c r="B94" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C93" s="5">
+      <c r="C94" s="5">
         <v>7000</v>
       </c>
-      <c r="D93" s="4">
+      <c r="D94" s="4">
         <f t="shared" si="13"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B94" s="4" t="s">
+    <row r="95" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B95" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C94" s="5">
+      <c r="C95" s="5">
         <v>-10000</v>
       </c>
-      <c r="D94" s="4">
+      <c r="D95" s="4">
         <f t="shared" si="13"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="16" t="s">
+    <row r="96" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="B95" s="4" t="s">
+      <c r="B96" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C95" s="5">
+      <c r="C96" s="5">
         <v>2000</v>
       </c>
-      <c r="D95" s="4">
+      <c r="D96" s="4">
         <f t="shared" si="13"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="16" t="s">
+    <row r="97" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="B96" s="4" t="s">
+      <c r="B97" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C96" s="5">
+      <c r="C97" s="5">
         <v>8000</v>
       </c>
-      <c r="D96" s="4">
+      <c r="D97" s="4">
         <f t="shared" si="13"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B97" s="4" t="s">
+    <row r="98" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B98" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C97" s="5">
+      <c r="C98" s="5">
         <v>-10000</v>
       </c>
-      <c r="D97" s="4">
+      <c r="D98" s="4">
         <f t="shared" si="13"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="16" t="s">
+    <row r="99" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="B98" s="4" t="s">
+      <c r="B99" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C98" s="5">
+      <c r="C99" s="5">
         <v>2000</v>
       </c>
-      <c r="D98" s="4">
-        <f t="shared" ref="D98:D103" si="14">D97+C98</f>
+      <c r="D99" s="4">
+        <f t="shared" ref="D99:D104" si="14">D98+C99</f>
         <v>5590</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B99" s="4" t="s">
+    <row r="100" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B100" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C99" s="5">
+      <c r="C100" s="5">
         <v>5000</v>
       </c>
-      <c r="D99" s="4">
+      <c r="D100" s="4">
         <f t="shared" si="14"/>
         <v>10590</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B100" s="4" t="s">
+    <row r="101" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B101" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C100" s="5">
+      <c r="C101" s="5">
         <v>-10000</v>
       </c>
-      <c r="D100" s="4">
+      <c r="D101" s="4">
         <f t="shared" si="14"/>
         <v>590</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B101" s="4" t="s">
+    <row r="102" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B102" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C101" s="5">
+      <c r="C102" s="5">
         <v>2000</v>
       </c>
-      <c r="D101" s="4">
+      <c r="D102" s="4">
         <f t="shared" si="14"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B102" s="4" t="s">
+    <row r="103" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B103" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C102" s="5">
+      <c r="C103" s="5">
         <v>9000</v>
       </c>
-      <c r="D102" s="4">
+      <c r="D103" s="4">
         <f t="shared" si="14"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B103" s="4" t="s">
+    <row r="104" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B104" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C103" s="5">
+      <c r="C104" s="5">
         <v>-10000</v>
       </c>
-      <c r="D103" s="4">
+      <c r="D104" s="4">
         <f t="shared" si="14"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="16" t="s">
+    <row r="105" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="B104" s="4" t="s">
+      <c r="B105" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C104" s="5">
+      <c r="C105" s="5">
         <v>2000</v>
       </c>
-      <c r="D104" s="4">
-        <f t="shared" ref="D104:D109" si="15">D103+C104</f>
+      <c r="D105" s="4">
+        <f t="shared" ref="D105:D110" si="15">D104+C105</f>
         <v>3590</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="16" t="s">
+    <row r="106" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="B105" s="4" t="s">
+      <c r="B106" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C105" s="5">
+      <c r="C106" s="5">
         <v>8000</v>
       </c>
-      <c r="D105" s="4">
+      <c r="D106" s="4">
         <f t="shared" si="15"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B106" s="4" t="s">
+    <row r="107" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B107" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C106" s="5">
+      <c r="C107" s="5">
         <v>-10000</v>
       </c>
-      <c r="D106" s="4">
+      <c r="D107" s="4">
         <f t="shared" si="15"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="16" t="s">
+    <row r="108" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="B107" s="4" t="s">
+      <c r="B108" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C107" s="5">
+      <c r="C108" s="5">
         <v>2000</v>
       </c>
-      <c r="D107" s="4">
+      <c r="D108" s="4">
         <f t="shared" si="15"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="16" t="s">
+    <row r="109" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="B108" s="4" t="s">
+      <c r="B109" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C108" s="5">
+      <c r="C109" s="5">
         <v>12000</v>
       </c>
-      <c r="D108" s="4">
+      <c r="D109" s="4">
         <f t="shared" si="15"/>
         <v>15590</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B109" s="4" t="s">
+    <row r="110" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B110" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C109" s="5">
+      <c r="C110" s="5">
         <v>-10000</v>
       </c>
-      <c r="D109" s="4">
+      <c r="D110" s="4">
         <f t="shared" si="15"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="16" t="s">
+    <row r="111" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="B110" s="4" t="s">
+      <c r="B111" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="C110" s="5">
+      <c r="C111" s="5">
         <v>2000</v>
       </c>
-      <c r="D110" s="4">
-        <f t="shared" ref="D110:D115" si="16">D109+C110</f>
+      <c r="D111" s="4">
+        <f t="shared" ref="D111:D116" si="16">D110+C111</f>
         <v>7590</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="16" t="s">
+    <row r="112" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="B111" s="4" t="s">
+      <c r="B112" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="C111" s="5">
+      <c r="C112" s="5">
         <v>10000</v>
       </c>
-      <c r="D111" s="4">
+      <c r="D112" s="4">
         <f t="shared" si="16"/>
         <v>17590</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B112" s="4" t="s">
+    <row r="113" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B113" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C112" s="5">
+      <c r="C113" s="5">
         <v>-10000</v>
       </c>
-      <c r="D112" s="4">
+      <c r="D113" s="4">
         <f t="shared" si="16"/>
         <v>7590</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B113" s="4" t="s">
+    <row r="114" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B114" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="C113" s="5">
+      <c r="C114" s="5">
         <v>2000</v>
       </c>
-      <c r="D113" s="4">
+      <c r="D114" s="4">
         <f t="shared" si="16"/>
         <v>9590</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="16" t="s">
+    <row r="115" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="B114" s="4" t="s">
+      <c r="B115" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="C114" s="5">
+      <c r="C115" s="5">
         <v>-1200</v>
       </c>
-      <c r="D114" s="4">
+      <c r="D115" s="4">
         <f t="shared" si="16"/>
         <v>8390</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B115" s="4" t="s">
+    <row r="116" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B116" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="C115" s="5">
+      <c r="C116" s="5">
         <v>500</v>
       </c>
-      <c r="D115" s="4">
+      <c r="D116" s="4">
         <f t="shared" si="16"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="16" t="s">
+    <row r="117" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="B116" s="4" t="s">
+      <c r="B117" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="C116" s="5">
+      <c r="C117" s="5">
         <v>750</v>
       </c>
-      <c r="D116" s="4">
-        <f t="shared" ref="D116:D121" si="17">D115+C116</f>
+      <c r="D117" s="4">
+        <f t="shared" ref="D117:D122" si="17">D116+C117</f>
         <v>9640</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="16" t="s">
+    <row r="118" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="B117" s="4" t="s">
+      <c r="B118" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C117" s="5">
+      <c r="C118" s="5">
         <v>2000</v>
       </c>
-      <c r="D117" s="4">
+      <c r="D118" s="4">
         <f t="shared" si="17"/>
         <v>11640</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B118" s="4" t="s">
+    <row r="119" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B119" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C118" s="5">
+      <c r="C119" s="5">
         <v>2000</v>
       </c>
-      <c r="D118" s="4">
+      <c r="D119" s="4">
         <f t="shared" si="17"/>
         <v>13640</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B119" s="4" t="s">
+    <row r="120" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B120" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C119" s="5">
+      <c r="C120" s="5">
         <v>-10000</v>
       </c>
-      <c r="D119" s="4">
+      <c r="D120" s="4">
         <f t="shared" si="17"/>
         <v>3640</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B120" s="4" t="s">
+    <row r="121" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B121" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="C120" s="5">
+      <c r="C121" s="5">
         <v>350</v>
       </c>
-      <c r="D120" s="4">
+      <c r="D121" s="4">
         <f t="shared" si="17"/>
         <v>3990</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="16" t="s">
+    <row r="122" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="B121" s="4" t="s">
+      <c r="B122" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="C121" s="5">
+      <c r="C122" s="5">
         <v>300</v>
       </c>
-      <c r="D121" s="4">
+      <c r="D122" s="4">
         <f t="shared" si="17"/>
         <v>4290</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="16" t="s">
+    <row r="123" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="B122" s="4" t="s">
+      <c r="B123" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="C122" s="5">
+      <c r="C123" s="5">
         <v>3800</v>
       </c>
-      <c r="D122" s="4">
-        <f t="shared" ref="D122:D128" si="18">D121+C122</f>
+      <c r="D123" s="4">
+        <f t="shared" ref="D123:D129" si="18">D122+C123</f>
         <v>8090</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B123" s="4" t="s">
+    <row r="124" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B124" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C123" s="5">
+      <c r="C124" s="5">
         <v>500</v>
       </c>
-      <c r="D123" s="4">
+      <c r="D124" s="4">
         <f t="shared" si="18"/>
         <v>8590</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="16" t="s">
+    <row r="125" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="B124" s="4" t="s">
+      <c r="B125" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="C124" s="5">
+      <c r="C125" s="5">
         <v>1300</v>
       </c>
-      <c r="D124" s="4">
+      <c r="D125" s="4">
         <f t="shared" si="18"/>
         <v>9890</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="16" t="s">
+    <row r="126" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="B125" s="4" t="s">
+      <c r="B126" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C125" s="5">
+      <c r="C126" s="5">
         <v>9000</v>
       </c>
-      <c r="D125" s="4">
+      <c r="D126" s="4">
         <f t="shared" si="18"/>
         <v>18890</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B126" s="4" t="s">
+    <row r="127" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B127" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C126" s="5">
+      <c r="C127" s="5">
         <v>-10000</v>
       </c>
-      <c r="D126" s="4">
+      <c r="D127" s="4">
         <f t="shared" si="18"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="16" t="s">
+    <row r="128" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="B127" s="4" t="s">
+      <c r="B128" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C127" s="5">
+      <c r="C128" s="5">
         <v>2000</v>
       </c>
-      <c r="D127" s="4">
+      <c r="D128" s="4">
         <f t="shared" si="18"/>
         <v>10890</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B128" s="4" t="s">
+    <row r="129" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B129" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C128" s="5">
+      <c r="C129" s="5">
         <v>-10000</v>
       </c>
-      <c r="D128" s="4">
+      <c r="D129" s="4">
         <f t="shared" si="18"/>
         <v>890</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="16" t="s">
+    <row r="130" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="B129" s="4" t="s">
+      <c r="B130" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="C129" s="5">
+      <c r="C130" s="5">
         <v>500</v>
       </c>
-      <c r="D129" s="4">
-        <f t="shared" ref="D129:D134" si="19">D128+C129</f>
+      <c r="D130" s="4">
+        <f t="shared" ref="D130:D135" si="19">D129+C130</f>
         <v>1390</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="16" t="s">
+    <row r="131" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="B130" s="4" t="s">
+      <c r="B131" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="C130" s="5">
+      <c r="C131" s="5">
         <v>10000</v>
       </c>
-      <c r="D130" s="4">
+      <c r="D131" s="4">
         <f t="shared" si="19"/>
         <v>11390</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B131" s="4" t="s">
+    <row r="132" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B132" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C131" s="5">
+      <c r="C132" s="5">
         <v>-10000</v>
       </c>
-      <c r="D131" s="4">
+      <c r="D132" s="4">
         <f t="shared" si="19"/>
         <v>1390</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="16" t="s">
+    <row r="133" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="B132" s="4" t="s">
+      <c r="B133" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C132" s="5">
+      <c r="C133" s="5">
         <v>3000</v>
       </c>
-      <c r="D132" s="4">
+      <c r="D133" s="4">
         <f t="shared" si="19"/>
         <v>4390</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="16" t="s">
+    <row r="134" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="B133" s="4" t="s">
+      <c r="B134" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C133" s="5">
+      <c r="C134" s="5">
         <v>2000</v>
       </c>
-      <c r="D133" s="4">
+      <c r="D134" s="4">
         <f t="shared" si="19"/>
         <v>6390</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B134" s="4" t="s">
+    <row r="135" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B135" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C134" s="5">
+      <c r="C135" s="5">
         <v>2000</v>
       </c>
-      <c r="D134" s="4">
+      <c r="D135" s="4">
         <f t="shared" si="19"/>
         <v>8390</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="16" t="s">
+    <row r="136" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="B135" s="4" t="s">
+      <c r="B136" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C135" s="5">
+      <c r="C136" s="5">
         <v>11000</v>
       </c>
-      <c r="D135" s="4">
-        <f t="shared" ref="D135:D140" si="20">D134+C135</f>
+      <c r="D136" s="4">
+        <f t="shared" ref="D136:D141" si="20">D135+C136</f>
         <v>19390</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B136" s="4" t="s">
+    <row r="137" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B137" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C136" s="5">
+      <c r="C137" s="5">
         <v>-10000</v>
       </c>
-      <c r="D136" s="4">
+      <c r="D137" s="4">
         <f t="shared" si="20"/>
         <v>9390</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="16" t="s">
+    <row r="138" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="16" t="s">
         <v>187</v>
       </c>
-      <c r="B137" s="4" t="s">
+      <c r="B138" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C137" s="5">
+      <c r="C138" s="5">
         <v>3000</v>
       </c>
-      <c r="D137" s="4">
+      <c r="D138" s="4">
         <f t="shared" si="20"/>
         <v>12390</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B138" s="4" t="s">
+    <row r="139" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B139" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C138" s="5">
+      <c r="C139" s="5">
         <v>-10000</v>
       </c>
-      <c r="D138" s="4">
+      <c r="D139" s="4">
         <f t="shared" si="20"/>
         <v>2390</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B139" s="4" t="s">
+    <row r="140" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B140" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C139" s="5">
+      <c r="C140" s="5">
         <v>500</v>
       </c>
-      <c r="D139" s="4">
+      <c r="D140" s="4">
         <f t="shared" si="20"/>
         <v>2890</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="16" t="s">
+    <row r="141" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="16" t="s">
         <v>189</v>
       </c>
-      <c r="B140" s="4" t="s">
+      <c r="B141" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C140" s="5">
+      <c r="C141" s="5">
         <v>5600</v>
       </c>
-      <c r="D140" s="4">
+      <c r="D141" s="4">
         <f t="shared" si="20"/>
         <v>8490</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B141" s="4" t="s">
+    <row r="142" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B142" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="C141" s="5">
+      <c r="C142" s="5">
         <v>4700</v>
       </c>
-      <c r="D141" s="4">
-        <f t="shared" ref="D141:D147" si="21">D140+C141</f>
+      <c r="D142" s="4">
+        <f t="shared" ref="D142:D148" si="21">D141+C142</f>
         <v>13190</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="16" t="s">
+    <row r="143" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="16" t="s">
         <v>192</v>
       </c>
-      <c r="B142" s="4" t="s">
+      <c r="B143" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C142" s="5">
+      <c r="C143" s="5">
         <v>1500</v>
       </c>
-      <c r="D142" s="4">
+      <c r="D143" s="4">
         <f t="shared" si="21"/>
         <v>14690</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B143" s="4" t="s">
+    <row r="144" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B144" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C143" s="5">
+      <c r="C144" s="5">
         <v>500</v>
       </c>
-      <c r="D143" s="4">
+      <c r="D144" s="4">
         <f t="shared" si="21"/>
         <v>15190</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="16" t="s">
+    <row r="145" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="B144" s="4" t="s">
+      <c r="B145" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="C144" s="5">
+      <c r="C145" s="5">
         <v>1000</v>
       </c>
-      <c r="D144" s="4">
+      <c r="D145" s="4">
         <f t="shared" si="21"/>
         <v>16190</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="16" t="s">
+    <row r="146" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="B145" s="4" t="s">
+      <c r="B146" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="C145" s="5">
+      <c r="C146" s="5">
         <v>1000</v>
       </c>
-      <c r="D145" s="4">
+      <c r="D146" s="4">
         <f t="shared" si="21"/>
         <v>17190</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="16" t="s">
+    <row r="147" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="B146" s="4" t="s">
+      <c r="B147" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C146" s="5">
+      <c r="C147" s="5">
         <v>3000</v>
       </c>
-      <c r="D146" s="4">
+      <c r="D147" s="4">
         <f t="shared" si="21"/>
         <v>20190</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B147" s="4" t="s">
+    <row r="148" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B148" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C147" s="5">
+      <c r="C148" s="5">
         <v>-20000</v>
       </c>
-      <c r="D147" s="4">
+      <c r="D148" s="4">
         <f t="shared" si="21"/>
         <v>190</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B148" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C148" s="5">
-        <v>500</v>
-      </c>
-      <c r="D148" s="4">
-        <f t="shared" ref="D148:D154" si="22">D147+C148</f>
-        <v>690</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B149" s="4" t="s">
         <v>76</v>
       </c>
@@ -3701,635 +3703,674 @@
         <v>500</v>
       </c>
       <c r="D149" s="4">
+        <f t="shared" ref="D149:D155" si="22">D148+C149</f>
+        <v>690</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B150" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C150" s="5">
+        <v>500</v>
+      </c>
+      <c r="D150" s="4">
         <f t="shared" si="22"/>
         <v>1190</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="16" t="s">
+    <row r="151" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="B150" s="4" t="s">
+      <c r="B151" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="C150" s="5">
+      <c r="C151" s="5">
         <v>10000</v>
       </c>
-      <c r="D150" s="4">
+      <c r="D151" s="4">
         <f t="shared" si="22"/>
         <v>11190</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B151" s="4" t="s">
+    <row r="152" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B152" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C151" s="5">
+      <c r="C152" s="5">
         <v>-10000</v>
       </c>
-      <c r="D151" s="4">
+      <c r="D152" s="4">
         <f t="shared" si="22"/>
         <v>1190</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="16" t="s">
+    <row r="153" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="B152" s="4" t="s">
+      <c r="B153" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C152" s="5">
+      <c r="C153" s="5">
         <v>3000</v>
       </c>
-      <c r="D152" s="4">
+      <c r="D153" s="4">
         <f t="shared" si="22"/>
         <v>4190</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" s="16" t="s">
+    <row r="154" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="B153" s="4" t="s">
+      <c r="B154" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C153" s="5">
+      <c r="C154" s="5">
         <v>11000</v>
       </c>
-      <c r="D153" s="4">
+      <c r="D154" s="4">
         <f t="shared" si="22"/>
         <v>15190</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B154" s="4" t="s">
+    <row r="155" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B155" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C154" s="5">
+      <c r="C155" s="5">
         <v>-10000</v>
       </c>
-      <c r="D154" s="4">
+      <c r="D155" s="4">
         <f t="shared" si="22"/>
         <v>5190</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="16" t="s">
+    <row r="156" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="16" t="s">
         <v>206</v>
       </c>
-      <c r="B155" s="4" t="s">
+      <c r="B156" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C155" s="5">
+      <c r="C156" s="5">
         <v>3000</v>
       </c>
-      <c r="D155" s="4">
-        <f t="shared" ref="D155:D161" si="23">D154+C155</f>
+      <c r="D156" s="4">
+        <f t="shared" ref="D156:D162" si="23">D155+C156</f>
         <v>8190</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="16" t="s">
+    <row r="157" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="B156" s="4" t="s">
+      <c r="B157" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="C156" s="5">
+      <c r="C157" s="5">
         <v>14000</v>
       </c>
-      <c r="D156" s="4">
+      <c r="D157" s="4">
         <f t="shared" si="23"/>
         <v>22190</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B157" s="4" t="s">
+    <row r="158" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B158" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="C157" s="5">
+      <c r="C158" s="5">
         <v>-20000</v>
       </c>
-      <c r="D157" s="4">
+      <c r="D158" s="4">
         <f t="shared" si="23"/>
         <v>2190</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="16" t="s">
+    <row r="159" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="B158" s="4" t="s">
+      <c r="B159" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="C158" s="5">
+      <c r="C159" s="5">
         <v>5000</v>
       </c>
-      <c r="D158" s="4">
+      <c r="D159" s="4">
         <f t="shared" si="23"/>
         <v>7190</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="16" t="s">
+    <row r="160" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="16" t="s">
         <v>213</v>
       </c>
-      <c r="B159" s="4" t="s">
+      <c r="B160" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="C159" s="5">
+      <c r="C160" s="5">
         <v>5000</v>
       </c>
-      <c r="D159" s="4">
+      <c r="D160" s="4">
         <f t="shared" si="23"/>
         <v>12190</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="16" t="s">
+    <row r="161" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A161" s="16" t="s">
         <v>215</v>
       </c>
-      <c r="B160" s="4" t="s">
+      <c r="B161" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C160" s="5">
+      <c r="C161" s="5">
         <v>11000</v>
       </c>
-      <c r="D160" s="4">
+      <c r="D161" s="4">
         <f t="shared" si="23"/>
         <v>23190</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B161" s="4" t="s">
+    <row r="162" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B162" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C161" s="5">
+      <c r="C162" s="5">
         <v>-20000</v>
       </c>
-      <c r="D161" s="4">
+      <c r="D162" s="4">
         <f t="shared" si="23"/>
         <v>3190</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" s="16" t="s">
+    <row r="163" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="16" t="s">
         <v>216</v>
       </c>
-      <c r="B162" s="4" t="s">
+      <c r="B163" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C162" s="5">
+      <c r="C163" s="5">
         <v>500</v>
       </c>
-      <c r="D162" s="4">
-        <f t="shared" ref="D162:D167" si="24">D161+C162</f>
+      <c r="D163" s="4">
+        <f t="shared" ref="D163:D168" si="24">D162+C163</f>
         <v>3690</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B163" s="4" t="s">
+    <row r="164" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B164" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C163" s="5">
+      <c r="C164" s="5">
         <v>3000</v>
       </c>
-      <c r="D163" s="4">
+      <c r="D164" s="4">
         <f t="shared" si="24"/>
         <v>6690</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164" s="16" t="s">
+    <row r="165" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A165" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="B164" s="4" t="s">
+      <c r="B165" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="C164" s="5">
+      <c r="C165" s="5">
         <v>12000</v>
       </c>
-      <c r="D164" s="4">
+      <c r="D165" s="4">
         <f t="shared" si="24"/>
         <v>18690</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B165" s="4" t="s">
+    <row r="166" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B166" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C165" s="5">
+      <c r="C166" s="5">
         <v>-10000</v>
       </c>
-      <c r="D165" s="4">
+      <c r="D166" s="4">
         <f t="shared" si="24"/>
         <v>8690</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A166" s="16" t="s">
+    <row r="167" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A167" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="B166" s="4" t="s">
+      <c r="B167" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="C166" s="5">
+      <c r="C167" s="5">
         <v>5000</v>
       </c>
-      <c r="D166" s="4">
+      <c r="D167" s="4">
         <f t="shared" si="24"/>
         <v>13690</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B167" s="4" t="s">
+    <row r="168" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B168" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C167" s="5">
+      <c r="C168" s="5">
         <v>-10000</v>
       </c>
-      <c r="D167" s="4">
+      <c r="D168" s="4">
         <f t="shared" si="24"/>
         <v>3690</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A168" s="16" t="s">
+    <row r="169" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A169" s="16" t="s">
         <v>221</v>
       </c>
-      <c r="B168" s="4" t="s">
+      <c r="B169" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="C168" s="5">
+      <c r="C169" s="5">
         <v>12000</v>
       </c>
-      <c r="D168" s="4">
-        <f t="shared" ref="D168:D173" si="25">D167+C168</f>
+      <c r="D169" s="4">
+        <f t="shared" ref="D169:D174" si="25">D168+C169</f>
         <v>15690</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B169" s="4" t="s">
+    <row r="170" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B170" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C169" s="5">
+      <c r="C170" s="5">
         <v>-10000</v>
       </c>
-      <c r="D169" s="4">
+      <c r="D170" s="4">
         <f t="shared" si="25"/>
         <v>5690</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" s="16" t="s">
+    <row r="171" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A171" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="B170" s="4" t="s">
+      <c r="B171" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C170" s="5">
+      <c r="C171" s="5">
         <v>2000</v>
       </c>
-      <c r="D170" s="4">
+      <c r="D171" s="4">
         <f t="shared" si="25"/>
         <v>7690</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" s="16" t="s">
+    <row r="172" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A172" s="16" t="s">
         <v>227</v>
       </c>
-      <c r="B171" s="4" t="s">
+      <c r="B172" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="C171" s="5">
+      <c r="C172" s="5">
         <v>1000</v>
       </c>
-      <c r="D171" s="4">
+      <c r="D172" s="4">
         <f t="shared" si="25"/>
         <v>8690</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A172" s="16" t="s">
+    <row r="173" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A173" s="16" t="s">
         <v>229</v>
       </c>
-      <c r="B172" s="4" t="s">
+      <c r="B173" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="C172" s="5">
+      <c r="C173" s="5">
         <v>5000</v>
       </c>
-      <c r="D172" s="4">
+      <c r="D173" s="4">
         <f t="shared" si="25"/>
         <v>13690</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B173" s="4" t="s">
+    <row r="174" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B174" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C173" s="5">
+      <c r="C174" s="5">
         <v>-10000</v>
       </c>
-      <c r="D173" s="4">
+      <c r="D174" s="4">
         <f t="shared" si="25"/>
         <v>3690</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174" s="16" t="s">
+    <row r="175" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A175" s="16" t="s">
         <v>231</v>
       </c>
-      <c r="B174" s="4" t="s">
+      <c r="B175" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="C174" s="5">
+      <c r="C175" s="5">
         <v>13000</v>
       </c>
-      <c r="D174" s="4">
-        <f t="shared" ref="D174:D179" si="26">D173+C174</f>
+      <c r="D175" s="4">
+        <f t="shared" ref="D175:D180" si="26">D174+C175</f>
         <v>16690</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B175" s="4" t="s">
+    <row r="176" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B176" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C175" s="5">
+      <c r="C176" s="5">
         <v>-10000</v>
       </c>
-      <c r="D175" s="4">
+      <c r="D176" s="4">
         <f t="shared" si="26"/>
         <v>6690</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176" s="16" t="s">
+    <row r="177" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A177" s="16" t="s">
         <v>233</v>
       </c>
-      <c r="B176" s="4" t="s">
+      <c r="B177" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C176" s="5">
+      <c r="C177" s="5">
         <v>3000</v>
       </c>
-      <c r="D176" s="4">
+      <c r="D177" s="4">
         <f t="shared" si="26"/>
         <v>9690</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A177" s="16" t="s">
+    <row r="178" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A178" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="B177" s="4" t="s">
+      <c r="B178" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="C177" s="5">
+      <c r="C178" s="5">
         <v>13000</v>
       </c>
-      <c r="D177" s="4">
+      <c r="D178" s="4">
         <f t="shared" si="26"/>
         <v>22690</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B178" s="4" t="s">
+    <row r="179" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B179" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C178" s="5">
+      <c r="C179" s="5">
         <v>-20000</v>
       </c>
-      <c r="D178" s="4">
+      <c r="D179" s="4">
         <f t="shared" si="26"/>
         <v>2690</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A179" s="16" t="s">
+    <row r="180" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A180" s="16" t="s">
         <v>235</v>
       </c>
-      <c r="B179" s="4" t="s">
+      <c r="B180" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C179" s="5">
+      <c r="C180" s="5">
         <v>3000</v>
       </c>
-      <c r="D179" s="4">
+      <c r="D180" s="4">
         <f t="shared" si="26"/>
         <v>5690</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" s="16" t="s">
+    <row r="181" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A181" s="16" t="s">
         <v>237</v>
       </c>
-      <c r="B180" s="4" t="s">
+      <c r="B181" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="C180" s="5">
+      <c r="C181" s="5">
         <v>16000</v>
       </c>
-      <c r="D180" s="4">
-        <f t="shared" ref="D180:D185" si="27">D179+C180</f>
+      <c r="D181" s="4">
+        <f t="shared" ref="D181:D186" si="27">D180+C181</f>
         <v>21690</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B181" s="4" t="s">
+    <row r="182" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B182" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C181" s="5">
+      <c r="C182" s="5">
         <v>-20000</v>
       </c>
-      <c r="D181" s="4">
+      <c r="D182" s="4">
         <f t="shared" si="27"/>
         <v>1690</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" s="16" t="s">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A183" s="16" t="s">
         <v>240</v>
       </c>
-      <c r="B182" s="4" t="s">
+      <c r="B183" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C182" s="5">
+      <c r="C183" s="5">
         <v>2000</v>
       </c>
-      <c r="D182" s="4">
+      <c r="D183" s="4">
         <f t="shared" si="27"/>
         <v>3690</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183" s="16" t="s">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A184" s="16" t="s">
         <v>241</v>
       </c>
-      <c r="B183" s="4" t="s">
+      <c r="B184" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="C183" s="5">
+      <c r="C184" s="5">
         <v>1000</v>
       </c>
-      <c r="D183" s="4">
+      <c r="D184" s="4">
         <f t="shared" si="27"/>
         <v>4690</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" s="16" t="s">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A185" s="16" t="s">
         <v>242</v>
       </c>
-      <c r="B184" s="4" t="s">
+      <c r="B185" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="C184" s="5">
+      <c r="C185" s="5">
         <v>6000</v>
       </c>
-      <c r="D184" s="4">
+      <c r="D185" s="4">
         <f t="shared" si="27"/>
         <v>10690</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B185" s="4" t="s">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B186" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C185" s="5">
+      <c r="C186" s="5">
         <v>-10000</v>
       </c>
-      <c r="D185" s="4">
+      <c r="D186" s="4">
         <f t="shared" si="27"/>
         <v>690</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A186" s="16" t="s">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A187" s="16" t="s">
         <v>244</v>
       </c>
-      <c r="B186" s="4" t="s">
+      <c r="B187" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="C186" s="5">
+      <c r="C187" s="5">
         <v>14000</v>
       </c>
-      <c r="D186" s="4">
-        <f t="shared" ref="D186:D191" si="28">D185+C186</f>
+      <c r="D187" s="4">
+        <f t="shared" ref="D187:D192" si="28">D186+C187</f>
         <v>14690</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B187" s="4" t="s">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B188" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C187" s="5">
+      <c r="C188" s="5">
         <v>-10000</v>
       </c>
-      <c r="D187" s="4">
+      <c r="D188" s="4">
         <f t="shared" si="28"/>
         <v>4690</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A188" s="16" t="s">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189" s="16" t="s">
         <v>245</v>
       </c>
-      <c r="B188" s="4" t="s">
+      <c r="B189" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C188" s="5">
+      <c r="C189" s="5">
         <v>3000</v>
       </c>
-      <c r="D188" s="4">
+      <c r="D189" s="4">
         <f t="shared" si="28"/>
         <v>7690</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" s="16" t="s">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A190" s="16" t="s">
         <v>247</v>
       </c>
-      <c r="B189" s="4" t="s">
+      <c r="B190" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="C189" s="5">
+      <c r="C190" s="5">
         <v>15000</v>
       </c>
-      <c r="D189" s="4">
+      <c r="D190" s="4">
         <f t="shared" si="28"/>
         <v>22690</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B190" s="4" t="s">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B191" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C190" s="5">
+      <c r="C191" s="5">
         <v>-20000</v>
       </c>
-      <c r="D190" s="4">
+      <c r="D191" s="4">
         <f t="shared" si="28"/>
         <v>2690</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A191" s="16" t="s">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A192" s="16" t="s">
         <v>248</v>
       </c>
-      <c r="B191" s="4" t="s">
+      <c r="B192" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="C191" s="5">
+      <c r="C192" s="5">
         <v>6000</v>
       </c>
-      <c r="D191" s="4">
+      <c r="D192" s="4">
         <f t="shared" si="28"/>
         <v>8690</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A192" s="16" t="s">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A193" s="16" t="s">
         <v>250</v>
       </c>
-      <c r="B192" s="4" t="s">
+      <c r="B193" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="C192" s="5">
+      <c r="C193" s="5">
         <v>15000</v>
-      </c>
-      <c r="D192" s="4">
-        <f>D191+C192</f>
-        <v>23690</v>
-      </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B193" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="C193" s="5">
-        <v>-20000</v>
       </c>
       <c r="D193" s="4">
         <f>D192+C193</f>
-        <v>3690</v>
+        <v>23690</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194" s="16" t="s">
-        <v>254</v>
-      </c>
       <c r="B194" s="4" t="s">
-        <v>255</v>
+        <v>198</v>
       </c>
       <c r="C194" s="5">
-        <v>2000</v>
+        <v>-20000</v>
       </c>
       <c r="D194" s="4">
         <f>D193+C194</f>
+        <v>3690</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A195" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="B195" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="C195" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D195" s="4">
+        <f>D194+C195</f>
         <v>5690</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A196" s="16" t="s">
+        <v>257</v>
+      </c>
+      <c r="B196" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="C196" s="5">
+        <v>7000</v>
+      </c>
+      <c r="D196" s="4">
+        <f>D195+C196</f>
+        <v>12690</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B197" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C197" s="5">
+        <v>-10000</v>
+      </c>
+      <c r="D197" s="4">
+        <f>D196+C197</f>
+        <v>2690</v>
       </c>
     </row>
   </sheetData>
@@ -4380,10 +4421,10 @@
       <c r="E1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="H1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="29"/>
+      <c r="I1" s="30"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
@@ -4519,10 +4560,10 @@
       <c r="E1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="H1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="29"/>
+      <c r="I1" s="30"/>
     </row>
     <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -4916,10 +4957,10 @@
       <c r="E1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="H1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="29"/>
+      <c r="I1" s="30"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -5017,7 +5058,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -5114,7 +5155,7 @@
       <c r="B10">
         <v>15000</v>
       </c>
-      <c r="C10" s="30">
+      <c r="C10" s="29">
         <v>45559</v>
       </c>
     </row>

</xml_diff>

<commit_message>
duy tinh tien loi co diem ngay 21
</commit_message>
<xml_diff>
--- a/DEBIT_BOOK.xlsx
+++ b/DEBIT_BOOK.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="CÔ DIỄM" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="262">
   <si>
     <t>NGÀY THÁNG</t>
   </si>
@@ -799,6 +799,12 @@
   </si>
   <si>
     <t>đã xong</t>
+  </si>
+  <si>
+    <t>21/12/2024</t>
+  </si>
+  <si>
+    <t>Duy lấy tiền lời 15tr</t>
   </si>
 </sst>
 </file>
@@ -1302,11 +1308,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K197"/>
+  <dimension ref="A1:K200"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1382,8 +1388,8 @@
         <v>20</v>
       </c>
       <c r="J3" s="4">
-        <f>SUM(I3:I76)</f>
-        <v>690</v>
+        <f>SUM(I3:I77)</f>
+        <v>700</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1738,7 +1744,7 @@
         <v>7640</v>
       </c>
       <c r="D22" s="4">
-        <f t="shared" ref="D22:D27" si="2">D21+C22</f>
+        <f t="shared" ref="D22:D28" si="2">D21+C22</f>
         <v>9090</v>
       </c>
       <c r="H22" s="16" t="s">
@@ -1750,18 +1756,8 @@
       <c r="K22" s="14"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="5">
-        <v>3000</v>
-      </c>
-      <c r="D23" s="4">
-        <f>D22+C23</f>
-        <v>12090</v>
-      </c>
       <c r="H23" s="16" t="s">
-        <v>70</v>
+        <v>260</v>
       </c>
       <c r="I23" s="5">
         <v>10</v>
@@ -1770,102 +1766,99 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="5">
+        <v>3000</v>
+      </c>
+      <c r="D24" s="4">
+        <f>D22+C24</f>
+        <v>12090</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="I24" s="5">
+        <v>10</v>
+      </c>
+      <c r="K24" s="14"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C25" s="5">
         <v>-10000</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D25" s="4">
         <f t="shared" si="2"/>
         <v>2090</v>
       </c>
-      <c r="H24" s="16" t="s">
+      <c r="H25" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="I24" s="5">
+      <c r="I25" s="5">
         <v>10</v>
       </c>
-      <c r="K24" s="14"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="4" t="s">
+      <c r="K25" s="14"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C26" s="5">
         <v>800</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D26" s="4">
         <f t="shared" si="2"/>
         <v>2890</v>
       </c>
-      <c r="H25" s="16" t="s">
+      <c r="H26" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="I25" s="5">
+      <c r="I26" s="5">
         <v>10</v>
       </c>
-      <c r="K25" s="14"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="16" t="s">
+      <c r="K26" s="14"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B27" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C27" s="5">
         <v>2000</v>
       </c>
-      <c r="D26" s="4">
+      <c r="D27" s="4">
         <f t="shared" si="2"/>
         <v>4890</v>
       </c>
-      <c r="H26" s="16" t="s">
+      <c r="H27" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="I26" s="5">
+      <c r="I27" s="5">
         <v>10</v>
       </c>
-      <c r="K26" s="14"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="16" t="s">
+      <c r="K27" s="14"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B28" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C28" s="5">
         <v>4000</v>
       </c>
-      <c r="D27" s="4">
+      <c r="D28" s="4">
         <f t="shared" si="2"/>
         <v>8890</v>
       </c>
-      <c r="H27" s="16" t="s">
+      <c r="H28" s="16" t="s">
         <v>11</v>
-      </c>
-      <c r="I27" s="5">
-        <v>10</v>
-      </c>
-      <c r="K27" s="14"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C28" s="5">
-        <v>4000</v>
-      </c>
-      <c r="D28" s="4">
-        <f t="shared" ref="D28:D33" si="3">D27+C28</f>
-        <v>12890</v>
-      </c>
-      <c r="H28" s="16" t="s">
-        <v>24</v>
       </c>
       <c r="I28" s="5">
         <v>10</v>
@@ -1873,119 +1866,119 @@
       <c r="K28" s="14"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="16" t="s">
+        <v>59</v>
+      </c>
       <c r="B29" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="5">
+        <v>4000</v>
+      </c>
+      <c r="D29" s="4">
+        <f t="shared" ref="D29:D34" si="3">D28+C29</f>
+        <v>12890</v>
+      </c>
+      <c r="H29" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="I29" s="5">
+        <v>10</v>
+      </c>
+      <c r="K29" s="14"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C30" s="5">
         <v>5000</v>
       </c>
-      <c r="D29" s="4">
+      <c r="D30" s="4">
         <f t="shared" si="3"/>
         <v>17890</v>
       </c>
-      <c r="H29" s="16" t="s">
+      <c r="H30" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="I29" s="5">
+      <c r="I30" s="5">
         <v>10</v>
       </c>
-      <c r="K29" s="14"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B30" s="4" t="s">
+      <c r="K30" s="14"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C31" s="5">
         <v>-10000</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D31" s="4">
         <f t="shared" si="3"/>
         <v>7890</v>
       </c>
-      <c r="H30" s="16" t="s">
+      <c r="H31" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="I30" s="5">
+      <c r="I31" s="5">
         <v>10</v>
       </c>
-      <c r="K30" s="14"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="16">
+      <c r="K31" s="14"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="16">
         <v>44969</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B32" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C32" s="5">
         <v>900</v>
       </c>
-      <c r="D31" s="4">
+      <c r="D32" s="4">
         <f t="shared" si="3"/>
         <v>8790</v>
       </c>
-      <c r="H31" s="16" t="s">
+      <c r="H32" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="I31" s="5">
+      <c r="I32" s="5">
         <v>10</v>
       </c>
-      <c r="K31" s="14"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B32" s="4" t="s">
+      <c r="K32" s="14"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C33" s="5">
         <v>4000</v>
       </c>
-      <c r="D32" s="4">
+      <c r="D33" s="4">
         <f t="shared" si="3"/>
         <v>12790</v>
       </c>
-      <c r="H32" s="16" t="s">
+      <c r="H33" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="I32" s="5">
+      <c r="I33" s="5">
         <v>10</v>
       </c>
-      <c r="K32" s="14"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B33" s="4" t="s">
+      <c r="K33" s="14"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B34" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C34" s="5">
         <v>-10000</v>
       </c>
-      <c r="D33" s="4">
+      <c r="D34" s="4">
         <f t="shared" si="3"/>
         <v>2790</v>
       </c>
-      <c r="H33" s="16" t="s">
+      <c r="H34" s="16" t="s">
         <v>129</v>
-      </c>
-      <c r="I33" s="5">
-        <v>10</v>
-      </c>
-      <c r="K33" s="14"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C34" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D34" s="4">
-        <f t="shared" ref="D34:D42" si="4">D33+C34</f>
-        <v>4790</v>
-      </c>
-      <c r="H34" s="16" t="s">
-        <v>135</v>
       </c>
       <c r="I34" s="5">
         <v>10</v>
@@ -1994,112 +1987,125 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C35" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D35" s="4">
+        <f t="shared" ref="D35:D43" si="4">D34+C35</f>
+        <v>4790</v>
+      </c>
+      <c r="H35" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="I35" s="5">
+        <v>10</v>
+      </c>
+      <c r="K35" s="14"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B36" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C35" s="5">
+      <c r="C36" s="5">
         <v>700</v>
       </c>
-      <c r="D35" s="4">
+      <c r="D36" s="4">
         <f t="shared" si="4"/>
         <v>5490</v>
       </c>
-      <c r="H35" s="16" t="s">
+      <c r="H36" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="I35" s="5">
+      <c r="I36" s="5">
         <v>10</v>
       </c>
-      <c r="K35" s="14"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B36" s="4" t="s">
+      <c r="K36" s="14"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B37" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C36" s="5">
+      <c r="C37" s="5">
         <v>4000</v>
       </c>
-      <c r="D36" s="4">
+      <c r="D37" s="4">
         <f t="shared" si="4"/>
         <v>9490</v>
       </c>
-      <c r="H36" s="16" t="s">
+      <c r="H37" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="I36" s="5">
+      <c r="I37" s="5">
         <v>10</v>
       </c>
-      <c r="K36" s="14"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="16" t="s">
+      <c r="K37" s="14"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B38" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C37" s="5">
+      <c r="C38" s="5">
         <v>600</v>
       </c>
-      <c r="D37" s="4">
+      <c r="D38" s="4">
         <f t="shared" si="4"/>
         <v>10090</v>
       </c>
-      <c r="H37" s="16" t="s">
+      <c r="H38" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="I37" s="5">
+      <c r="I38" s="5">
         <v>10</v>
       </c>
-      <c r="K37" s="14"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B38" s="4" t="s">
+      <c r="K38" s="14"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B39" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C38" s="5">
+      <c r="C39" s="5">
         <v>-10000</v>
       </c>
-      <c r="D38" s="4">
+      <c r="D39" s="4">
         <f t="shared" si="4"/>
         <v>90</v>
       </c>
-      <c r="H38" s="16" t="s">
+      <c r="H39" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="I38" s="5">
+      <c r="I39" s="5">
         <v>10</v>
       </c>
-      <c r="K38" s="14"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="16" t="s">
+      <c r="K39" s="14"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B40" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C39" s="5">
+      <c r="C40" s="5">
         <f>700+5000+300+600+400+1000+800</f>
         <v>8800</v>
       </c>
-      <c r="D39" s="4">
+      <c r="D40" s="4">
         <f t="shared" si="4"/>
         <v>8890</v>
       </c>
-      <c r="H39" s="16" t="s">
+      <c r="H40" s="16" t="s">
         <v>234</v>
-      </c>
-      <c r="I39" s="5">
-        <v>20</v>
-      </c>
-      <c r="K39" s="14"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H40" s="16" t="s">
-        <v>247</v>
       </c>
       <c r="I40" s="5">
         <v>20</v>
@@ -2107,59 +2113,46 @@
       <c r="K40" s="14"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B41" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C41" s="5">
-        <v>6000</v>
-      </c>
-      <c r="D41" s="4">
-        <f>D39+C41</f>
-        <v>14890</v>
-      </c>
       <c r="H41" s="16" t="s">
-        <v>12</v>
+        <v>247</v>
       </c>
       <c r="I41" s="5">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="K41" s="14"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C42" s="5">
+        <v>6000</v>
+      </c>
+      <c r="D42" s="4">
+        <f>D40+C42</f>
+        <v>14890</v>
+      </c>
+      <c r="H42" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="I42" s="5">
+        <v>10</v>
+      </c>
+      <c r="K42" s="14"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B43" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C43" s="5">
         <v>-10000</v>
       </c>
-      <c r="D42" s="4">
+      <c r="D43" s="4">
         <f t="shared" si="4"/>
         <v>4890</v>
       </c>
-      <c r="H42" s="16" t="s">
+      <c r="H43" s="16" t="s">
         <v>43</v>
-      </c>
-      <c r="I42" s="5">
-        <v>10</v>
-      </c>
-      <c r="K42" s="14"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C43" s="5">
-        <v>500</v>
-      </c>
-      <c r="D43" s="4">
-        <f t="shared" ref="D43:D48" si="5">D42+C43</f>
-        <v>5390</v>
-      </c>
-      <c r="H43" s="16" t="s">
-        <v>139</v>
       </c>
       <c r="I43" s="5">
         <v>10</v>
@@ -2167,116 +2160,119 @@
       <c r="K43" s="14"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="16" t="s">
+        <v>75</v>
+      </c>
       <c r="B44" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C44" s="5">
+        <v>500</v>
+      </c>
+      <c r="D44" s="4">
+        <f t="shared" ref="D44:D49" si="5">D43+C44</f>
+        <v>5390</v>
+      </c>
+      <c r="H44" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="I44" s="5">
+        <v>10</v>
+      </c>
+      <c r="K44" s="14"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B45" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C45" s="5">
         <v>700</v>
       </c>
-      <c r="D44" s="4">
+      <c r="D45" s="4">
         <f t="shared" si="5"/>
         <v>6090</v>
       </c>
-      <c r="H44" s="16" t="s">
+      <c r="H45" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="I44" s="5">
+      <c r="I45" s="5">
         <v>10</v>
       </c>
-      <c r="K44" s="14"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B45" s="4" t="s">
+      <c r="K45" s="14"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B46" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C45" s="5">
+      <c r="C46" s="5">
         <v>1500</v>
       </c>
-      <c r="D45" s="4">
+      <c r="D46" s="4">
         <f t="shared" si="5"/>
         <v>7590</v>
       </c>
-      <c r="H45" s="16" t="s">
+      <c r="H46" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="I45" s="5">
+      <c r="I46" s="5">
         <v>10</v>
       </c>
-      <c r="K45" s="14"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B46" s="4" t="s">
+      <c r="K46" s="14"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B47" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C46" s="5">
+      <c r="C47" s="5">
         <v>5000</v>
       </c>
-      <c r="D46" s="4">
+      <c r="D47" s="4">
         <f t="shared" si="5"/>
         <v>12590</v>
       </c>
-      <c r="H46" s="16" t="s">
+      <c r="H47" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="I46" s="5">
+      <c r="I47" s="5">
         <v>10</v>
       </c>
-      <c r="K46" s="14"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B47" s="4" t="s">
+      <c r="K47" s="14"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B48" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C48" s="5">
         <v>-10000</v>
       </c>
-      <c r="D47" s="4">
+      <c r="D48" s="4">
         <f t="shared" si="5"/>
         <v>2590</v>
       </c>
-      <c r="H47" s="16" t="s">
+      <c r="H48" s="16" t="s">
         <v>157</v>
       </c>
-      <c r="I47" s="5">
+      <c r="I48" s="5">
         <v>20</v>
       </c>
-      <c r="K47" s="14"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="16" t="s">
+      <c r="K48" s="14"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B49" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C48" s="5">
+      <c r="C49" s="5">
         <v>2000</v>
       </c>
-      <c r="D48" s="4">
+      <c r="D49" s="4">
         <f t="shared" si="5"/>
         <v>4590</v>
       </c>
-      <c r="H48" s="16" t="s">
+      <c r="H49" s="16" t="s">
         <v>158</v>
-      </c>
-      <c r="I48" s="5">
-        <v>10</v>
-      </c>
-      <c r="K48" s="14"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B49" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C49" s="5">
-        <v>700</v>
-      </c>
-      <c r="D49" s="4">
-        <f t="shared" ref="D49:D54" si="6">D48+C49</f>
-        <v>5290</v>
-      </c>
-      <c r="H49" s="16" t="s">
-        <v>159</v>
       </c>
       <c r="I49" s="5">
         <v>10</v>
@@ -2284,9 +2280,6 @@
       <c r="K49" s="14"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="16" t="s">
-        <v>82</v>
-      </c>
       <c r="B50" s="4" t="s">
         <v>77</v>
       </c>
@@ -2294,118 +2287,118 @@
         <v>700</v>
       </c>
       <c r="D50" s="4">
+        <f t="shared" ref="D50:D55" si="6">D49+C50</f>
+        <v>5290</v>
+      </c>
+      <c r="H50" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="I50" s="5">
+        <v>10</v>
+      </c>
+      <c r="K50" s="14"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C51" s="5">
+        <v>700</v>
+      </c>
+      <c r="D51" s="4">
         <f t="shared" si="6"/>
         <v>5990</v>
       </c>
-      <c r="H50" s="16" t="s">
+      <c r="H51" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="I50" s="5">
+      <c r="I51" s="5">
         <v>10</v>
       </c>
-      <c r="K50" s="14"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="16" t="s">
+      <c r="K51" s="14"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B52" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C51" s="5">
+      <c r="C52" s="5">
         <v>700</v>
       </c>
-      <c r="D51" s="4">
+      <c r="D52" s="4">
         <f t="shared" si="6"/>
         <v>6690</v>
       </c>
-      <c r="H51" s="16" t="s">
+      <c r="H52" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="I51" s="5">
+      <c r="I52" s="5">
         <v>10</v>
       </c>
-      <c r="K51" s="14"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="16" t="s">
+      <c r="K52" s="14"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B53" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C52" s="5">
+      <c r="C53" s="5">
         <v>4000</v>
       </c>
-      <c r="D52" s="4">
+      <c r="D53" s="4">
         <f t="shared" si="6"/>
         <v>10690</v>
       </c>
-      <c r="H52" s="16" t="s">
+      <c r="H53" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="I52" s="5">
+      <c r="I53" s="5">
         <v>10</v>
       </c>
-      <c r="K52" s="14"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B53" s="4" t="s">
+      <c r="K53" s="14"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B54" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="5">
+      <c r="C54" s="5">
         <v>-10000</v>
       </c>
-      <c r="D53" s="4">
+      <c r="D54" s="4">
         <f t="shared" si="6"/>
         <v>690</v>
       </c>
-      <c r="H53" s="16" t="s">
+      <c r="H54" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="I53" s="5">
+      <c r="I54" s="5">
         <v>10</v>
       </c>
-      <c r="K53" s="14"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="16" t="s">
+      <c r="K54" s="14"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B55" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C54" s="5">
+      <c r="C55" s="5">
         <v>1000</v>
       </c>
-      <c r="D54" s="4">
+      <c r="D55" s="4">
         <f t="shared" si="6"/>
         <v>1690</v>
       </c>
-      <c r="H54" s="16" t="s">
+      <c r="H55" s="16" t="s">
         <v>151</v>
-      </c>
-      <c r="I54" s="5">
-        <v>10</v>
-      </c>
-      <c r="K54" s="14"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C55" s="5">
-        <v>7000</v>
-      </c>
-      <c r="D55" s="4">
-        <f t="shared" ref="D55:D59" si="7">D54+C55</f>
-        <v>8690</v>
-      </c>
-      <c r="H55" s="16" t="s">
-        <v>150</v>
       </c>
       <c r="I55" s="5">
         <v>10</v>
@@ -2413,84 +2406,97 @@
       <c r="K55" s="14"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="16" t="s">
+        <v>88</v>
+      </c>
       <c r="B56" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C56" s="5">
+        <v>7000</v>
+      </c>
+      <c r="D56" s="4">
+        <f t="shared" ref="D56:D60" si="7">D55+C56</f>
+        <v>8690</v>
+      </c>
+      <c r="H56" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="I56" s="5">
+        <v>10</v>
+      </c>
+      <c r="K56" s="14"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B57" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C56" s="5">
+      <c r="C57" s="5">
         <v>10000</v>
       </c>
-      <c r="D56" s="4">
+      <c r="D57" s="4">
         <f t="shared" si="7"/>
         <v>18690</v>
       </c>
-      <c r="H56" s="16" t="s">
+      <c r="H57" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="I56" s="5">
+      <c r="I57" s="5">
         <v>10</v>
       </c>
-      <c r="K56" s="14"/>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B57" s="4" t="s">
+      <c r="K57" s="14"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B58" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C57" s="5">
+      <c r="C58" s="5">
         <v>-10000</v>
       </c>
-      <c r="D57" s="4">
+      <c r="D58" s="4">
         <f t="shared" si="7"/>
         <v>8690</v>
       </c>
-      <c r="H57" s="16" t="s">
+      <c r="H58" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="I57" s="5">
+      <c r="I58" s="5">
         <v>10</v>
       </c>
-      <c r="K57" s="14"/>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B58" s="4" t="s">
+      <c r="K58" s="14"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B59" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C58" s="5">
+      <c r="C59" s="5">
         <v>1700</v>
       </c>
-      <c r="D58" s="4">
+      <c r="D59" s="4">
         <f t="shared" si="7"/>
         <v>10390</v>
       </c>
-      <c r="H58" s="16" t="s">
+      <c r="H59" s="16" t="s">
         <v>221</v>
       </c>
-      <c r="I58" s="5">
+      <c r="I59" s="5">
         <v>10</v>
       </c>
-      <c r="K58" s="14"/>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B59" s="4" t="s">
+      <c r="K59" s="14"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B60" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C59" s="5">
+      <c r="C60" s="5">
         <v>-10000</v>
       </c>
-      <c r="D59" s="4">
+      <c r="D60" s="4">
         <f t="shared" si="7"/>
         <v>390</v>
       </c>
-      <c r="H59" s="16" t="s">
+      <c r="H60" s="16" t="s">
         <v>237</v>
-      </c>
-      <c r="I59" s="5">
-        <v>20</v>
-      </c>
-      <c r="K59" s="14"/>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H60" s="16" t="s">
-        <v>250</v>
       </c>
       <c r="I60" s="5">
         <v>20</v>
@@ -2498,18 +2504,8 @@
       <c r="K60" s="14"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B61" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C61" s="5">
-        <v>6000</v>
-      </c>
-      <c r="D61" s="4">
-        <f>D59+C61</f>
-        <v>6390</v>
-      </c>
       <c r="H61" s="16" t="s">
-        <v>207</v>
+        <v>250</v>
       </c>
       <c r="I61" s="5">
         <v>20</v>
@@ -2517,270 +2513,277 @@
       <c r="K61" s="14"/>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" s="16" t="s">
-        <v>94</v>
-      </c>
       <c r="B62" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C62" s="5">
-        <v>2000</v>
+        <v>6000</v>
       </c>
       <c r="D62" s="4">
-        <f t="shared" ref="D62:D67" si="8">D61+C62</f>
-        <v>8390</v>
+        <f>D60+C62</f>
+        <v>6390</v>
       </c>
       <c r="H62" s="16" t="s">
-        <v>187</v>
+        <v>207</v>
       </c>
       <c r="I62" s="5">
-        <v>10</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="K62" s="14"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C63" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D63" s="4">
+        <f t="shared" ref="D63:D68" si="8">D62+C63</f>
+        <v>8390</v>
+      </c>
+      <c r="H63" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="I63" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B64" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C63" s="5">
+      <c r="C64" s="5">
         <v>5000</v>
       </c>
-      <c r="D63" s="4">
+      <c r="D64" s="4">
         <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B64" s="4" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B65" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C64" s="5">
+      <c r="C65" s="5">
         <v>-10000</v>
       </c>
-      <c r="D64" s="4">
+      <c r="D65" s="4">
         <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
-    <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="16" t="s">
+    <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B66" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C65" s="5">
+      <c r="C66" s="5">
         <v>1000</v>
       </c>
-      <c r="D65" s="4">
+      <c r="D66" s="4">
         <f t="shared" si="8"/>
         <v>4390</v>
       </c>
     </row>
-    <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="4" t="s">
+    <row r="67" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C66" s="5">
+      <c r="C67" s="5">
         <v>9000</v>
       </c>
-      <c r="D66" s="4">
+      <c r="D67" s="4">
         <f t="shared" si="8"/>
         <v>13390</v>
       </c>
     </row>
-    <row r="67" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="4" t="s">
+    <row r="68" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C67" s="5">
+      <c r="C68" s="5">
         <v>-10000</v>
       </c>
-      <c r="D67" s="4">
+      <c r="D68" s="4">
         <f t="shared" si="8"/>
         <v>3390</v>
       </c>
     </row>
-    <row r="68" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C68" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D68" s="4">
-        <f t="shared" ref="D68:D73" si="9">D67+C68</f>
-        <v>5390</v>
-      </c>
-    </row>
     <row r="69" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B69" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C69" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D69" s="4">
+        <f t="shared" ref="D69:D74" si="9">D68+C69</f>
+        <v>5390</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C69" s="5">
+      <c r="C70" s="5">
         <v>6000</v>
       </c>
-      <c r="D69" s="4">
+      <c r="D70" s="4">
         <f t="shared" si="9"/>
         <v>11390</v>
       </c>
     </row>
-    <row r="70" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="4" t="s">
+    <row r="71" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C70" s="5">
+      <c r="C71" s="5">
         <v>-10000</v>
       </c>
-      <c r="D70" s="4">
+      <c r="D71" s="4">
         <f t="shared" si="9"/>
         <v>1390</v>
       </c>
     </row>
-    <row r="71" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="4" t="s">
+    <row r="72" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C71" s="5">
+      <c r="C72" s="5">
         <v>400</v>
       </c>
-      <c r="D71" s="4">
+      <c r="D72" s="4">
         <f t="shared" si="9"/>
         <v>1790</v>
       </c>
     </row>
-    <row r="72" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="16" t="s">
+    <row r="73" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B73" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C72" s="5">
+      <c r="C73" s="5">
         <v>2000</v>
       </c>
-      <c r="D72" s="4">
+      <c r="D73" s="4">
         <f t="shared" si="9"/>
         <v>3790</v>
       </c>
     </row>
-    <row r="73" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="16" t="s">
+    <row r="74" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B74" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C73" s="5">
+      <c r="C74" s="5">
         <v>6000</v>
       </c>
-      <c r="D73" s="4">
+      <c r="D74" s="4">
         <f t="shared" si="9"/>
         <v>9790</v>
       </c>
     </row>
-    <row r="74" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="16" t="s">
+    <row r="75" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B75" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C74" s="5">
+      <c r="C75" s="5">
         <v>1000</v>
       </c>
-      <c r="D74" s="4">
-        <f t="shared" ref="D74:D79" si="10">D73+C74</f>
+      <c r="D75" s="4">
+        <f t="shared" ref="D75:D80" si="10">D74+C75</f>
         <v>10790</v>
       </c>
     </row>
-    <row r="75" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="4" t="s">
+    <row r="76" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B76" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C75" s="5">
+      <c r="C76" s="5">
         <v>-10000</v>
       </c>
-      <c r="D75" s="4">
+      <c r="D76" s="4">
         <f t="shared" si="10"/>
         <v>790</v>
       </c>
     </row>
-    <row r="76" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="16" t="s">
+    <row r="77" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B77" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C76" s="5">
+      <c r="C77" s="5">
         <v>800</v>
       </c>
-      <c r="D76" s="4">
+      <c r="D77" s="4">
         <f t="shared" si="10"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="77" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="16" t="s">
+    <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="B78" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C77" s="5">
+      <c r="C78" s="5">
         <v>5000</v>
       </c>
-      <c r="D77" s="4">
+      <c r="D78" s="4">
         <f t="shared" si="10"/>
         <v>6590</v>
       </c>
     </row>
-    <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="16" t="s">
+    <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B79" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C78" s="5">
+      <c r="C79" s="5">
         <v>6000</v>
       </c>
-      <c r="D78" s="4">
+      <c r="D79" s="4">
         <f t="shared" si="10"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="4" t="s">
+    <row r="80" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B80" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C79" s="5">
+      <c r="C80" s="5">
         <v>-10000</v>
       </c>
-      <c r="D79" s="4">
+      <c r="D80" s="4">
         <f t="shared" si="10"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="80" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="16" t="s">
+    <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="B80" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C80" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D80" s="4">
-        <f t="shared" ref="D80:D86" si="11">D79+C80</f>
-        <v>4590</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B81" s="4" t="s">
         <v>65</v>
       </c>
@@ -2788,926 +2791,926 @@
         <v>2000</v>
       </c>
       <c r="D81" s="4">
+        <f t="shared" ref="D81:D87" si="11">D80+C81</f>
+        <v>4590</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B82" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C82" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D82" s="4">
         <f t="shared" si="11"/>
         <v>6590</v>
       </c>
     </row>
-    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="4" t="s">
+    <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B83" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C82" s="5">
+      <c r="C83" s="5">
         <v>7000</v>
       </c>
-      <c r="D82" s="4">
+      <c r="D83" s="4">
         <f t="shared" si="11"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="4" t="s">
+    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B84" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C83" s="5">
+      <c r="C84" s="5">
         <v>-10000</v>
       </c>
-      <c r="D83" s="4">
+      <c r="D84" s="4">
         <f t="shared" si="11"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="16" t="s">
+    <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="B84" s="4" t="s">
+      <c r="B85" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C84" s="5">
+      <c r="C85" s="5">
         <v>2000</v>
       </c>
-      <c r="D84" s="4">
+      <c r="D85" s="4">
         <f t="shared" si="11"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="16" t="s">
+    <row r="86" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="B85" s="4" t="s">
+      <c r="B86" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C85" s="5">
+      <c r="C86" s="5">
         <v>6000</v>
       </c>
-      <c r="D85" s="4">
+      <c r="D86" s="4">
         <f t="shared" si="11"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="86" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="4" t="s">
+    <row r="87" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B87" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C86" s="5">
+      <c r="C87" s="5">
         <v>-10000</v>
       </c>
-      <c r="D86" s="4">
+      <c r="D87" s="4">
         <f t="shared" si="11"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="87" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="B87" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C87" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D87" s="4">
-        <f t="shared" ref="D87:D92" si="12">D86+C87</f>
-        <v>3590</v>
-      </c>
-    </row>
     <row r="88" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C88" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D88" s="4">
+        <f t="shared" ref="D88:D93" si="12">D87+C88</f>
+        <v>3590</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="B88" s="4" t="s">
+      <c r="B89" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C88" s="5">
+      <c r="C89" s="5">
         <v>7000</v>
       </c>
-      <c r="D88" s="4">
+      <c r="D89" s="4">
         <f t="shared" si="12"/>
         <v>10590</v>
       </c>
     </row>
-    <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="4" t="s">
+    <row r="90" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B90" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C89" s="5">
+      <c r="C90" s="5">
         <v>-10000</v>
       </c>
-      <c r="D89" s="4">
+      <c r="D90" s="4">
         <f t="shared" si="12"/>
         <v>590</v>
       </c>
     </row>
-    <row r="90" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="4" t="s">
+    <row r="91" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B91" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C90" s="5">
+      <c r="C91" s="5">
         <v>12000</v>
       </c>
-      <c r="D90" s="4">
+      <c r="D91" s="4">
         <f t="shared" si="12"/>
         <v>12590</v>
       </c>
     </row>
-    <row r="91" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="4" t="s">
+    <row r="92" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B92" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C91" s="5">
+      <c r="C92" s="5">
         <v>-10000</v>
       </c>
-      <c r="D91" s="4">
+      <c r="D92" s="4">
         <f t="shared" si="12"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="92" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B92" s="4" t="s">
+    <row r="93" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B93" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C92" s="5">
+      <c r="C93" s="5">
         <v>2000</v>
       </c>
-      <c r="D92" s="4">
+      <c r="D93" s="4">
         <f t="shared" si="12"/>
         <v>4590</v>
       </c>
     </row>
-    <row r="93" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="B93" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C93" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D93" s="4">
-        <f t="shared" ref="D93:D98" si="13">D92+C93</f>
-        <v>6590</v>
-      </c>
-    </row>
     <row r="94" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C94" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D94" s="4">
+        <f t="shared" ref="D94:D99" si="13">D93+C94</f>
+        <v>6590</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="B94" s="4" t="s">
+      <c r="B95" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C94" s="5">
+      <c r="C95" s="5">
         <v>7000</v>
       </c>
-      <c r="D94" s="4">
+      <c r="D95" s="4">
         <f t="shared" si="13"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="95" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B95" s="4" t="s">
+    <row r="96" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B96" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C95" s="5">
+      <c r="C96" s="5">
         <v>-10000</v>
       </c>
-      <c r="D95" s="4">
+      <c r="D96" s="4">
         <f t="shared" si="13"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="96" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="16" t="s">
+    <row r="97" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="B96" s="4" t="s">
+      <c r="B97" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C96" s="5">
+      <c r="C97" s="5">
         <v>2000</v>
       </c>
-      <c r="D96" s="4">
+      <c r="D97" s="4">
         <f t="shared" si="13"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="97" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="16" t="s">
+    <row r="98" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="B97" s="4" t="s">
+      <c r="B98" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C97" s="5">
+      <c r="C98" s="5">
         <v>8000</v>
       </c>
-      <c r="D97" s="4">
+      <c r="D98" s="4">
         <f t="shared" si="13"/>
         <v>13590</v>
       </c>
     </row>
-    <row r="98" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B98" s="4" t="s">
+    <row r="99" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B99" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C98" s="5">
+      <c r="C99" s="5">
         <v>-10000</v>
       </c>
-      <c r="D98" s="4">
+      <c r="D99" s="4">
         <f t="shared" si="13"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="99" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="16" t="s">
+    <row r="100" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="B99" s="4" t="s">
+      <c r="B100" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C99" s="5">
+      <c r="C100" s="5">
         <v>2000</v>
       </c>
-      <c r="D99" s="4">
-        <f t="shared" ref="D99:D104" si="14">D98+C99</f>
+      <c r="D100" s="4">
+        <f t="shared" ref="D100:D105" si="14">D99+C100</f>
         <v>5590</v>
       </c>
     </row>
-    <row r="100" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B100" s="4" t="s">
+    <row r="101" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B101" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C100" s="5">
+      <c r="C101" s="5">
         <v>5000</v>
       </c>
-      <c r="D100" s="4">
+      <c r="D101" s="4">
         <f t="shared" si="14"/>
         <v>10590</v>
       </c>
     </row>
-    <row r="101" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B101" s="4" t="s">
+    <row r="102" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B102" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C101" s="5">
+      <c r="C102" s="5">
         <v>-10000</v>
       </c>
-      <c r="D101" s="4">
+      <c r="D102" s="4">
         <f t="shared" si="14"/>
         <v>590</v>
       </c>
     </row>
-    <row r="102" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B102" s="4" t="s">
+    <row r="103" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B103" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C102" s="5">
+      <c r="C103" s="5">
         <v>2000</v>
       </c>
-      <c r="D102" s="4">
+      <c r="D103" s="4">
         <f t="shared" si="14"/>
         <v>2590</v>
       </c>
     </row>
-    <row r="103" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B103" s="4" t="s">
+    <row r="104" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B104" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C103" s="5">
+      <c r="C104" s="5">
         <v>9000</v>
       </c>
-      <c r="D103" s="4">
+      <c r="D104" s="4">
         <f t="shared" si="14"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="104" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B104" s="4" t="s">
+    <row r="105" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B105" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C104" s="5">
+      <c r="C105" s="5">
         <v>-10000</v>
       </c>
-      <c r="D104" s="4">
+      <c r="D105" s="4">
         <f t="shared" si="14"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="105" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B105" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C105" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D105" s="4">
-        <f t="shared" ref="D105:D110" si="15">D104+C105</f>
-        <v>3590</v>
-      </c>
-    </row>
     <row r="106" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C106" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D106" s="4">
+        <f t="shared" ref="D106:D111" si="15">D105+C106</f>
+        <v>3590</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="B106" s="4" t="s">
+      <c r="B107" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C106" s="5">
+      <c r="C107" s="5">
         <v>8000</v>
       </c>
-      <c r="D106" s="4">
+      <c r="D107" s="4">
         <f t="shared" si="15"/>
         <v>11590</v>
       </c>
     </row>
-    <row r="107" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B107" s="4" t="s">
+    <row r="108" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B108" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C107" s="5">
+      <c r="C108" s="5">
         <v>-10000</v>
       </c>
-      <c r="D107" s="4">
+      <c r="D108" s="4">
         <f t="shared" si="15"/>
         <v>1590</v>
       </c>
     </row>
-    <row r="108" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="16" t="s">
+    <row r="109" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="B108" s="4" t="s">
+      <c r="B109" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C108" s="5">
+      <c r="C109" s="5">
         <v>2000</v>
       </c>
-      <c r="D108" s="4">
+      <c r="D109" s="4">
         <f t="shared" si="15"/>
         <v>3590</v>
       </c>
     </row>
-    <row r="109" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="16" t="s">
+    <row r="110" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="B109" s="4" t="s">
+      <c r="B110" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C109" s="5">
+      <c r="C110" s="5">
         <v>12000</v>
       </c>
-      <c r="D109" s="4">
+      <c r="D110" s="4">
         <f t="shared" si="15"/>
         <v>15590</v>
       </c>
     </row>
-    <row r="110" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B110" s="4" t="s">
+    <row r="111" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B111" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C110" s="5">
+      <c r="C111" s="5">
         <v>-10000</v>
       </c>
-      <c r="D110" s="4">
+      <c r="D111" s="4">
         <f t="shared" si="15"/>
         <v>5590</v>
       </c>
     </row>
-    <row r="111" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="B111" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="C111" s="5">
-        <v>2000</v>
-      </c>
-      <c r="D111" s="4">
-        <f t="shared" ref="D111:D116" si="16">D110+C111</f>
-        <v>7590</v>
-      </c>
-    </row>
     <row r="112" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="B112" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C112" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D112" s="4">
+        <f t="shared" ref="D112:D117" si="16">D111+C112</f>
+        <v>7590</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="B112" s="4" t="s">
+      <c r="B113" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="C112" s="5">
+      <c r="C113" s="5">
         <v>10000</v>
       </c>
-      <c r="D112" s="4">
+      <c r="D113" s="4">
         <f t="shared" si="16"/>
         <v>17590</v>
       </c>
     </row>
-    <row r="113" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B113" s="4" t="s">
+    <row r="114" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B114" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C113" s="5">
+      <c r="C114" s="5">
         <v>-10000</v>
       </c>
-      <c r="D113" s="4">
+      <c r="D114" s="4">
         <f t="shared" si="16"/>
         <v>7590</v>
       </c>
     </row>
-    <row r="114" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B114" s="4" t="s">
+    <row r="115" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B115" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="C114" s="5">
+      <c r="C115" s="5">
         <v>2000</v>
       </c>
-      <c r="D114" s="4">
+      <c r="D115" s="4">
         <f t="shared" si="16"/>
         <v>9590</v>
       </c>
     </row>
-    <row r="115" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="16" t="s">
+    <row r="116" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="B115" s="4" t="s">
+      <c r="B116" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="C115" s="5">
+      <c r="C116" s="5">
         <v>-1200</v>
       </c>
-      <c r="D115" s="4">
+      <c r="D116" s="4">
         <f t="shared" si="16"/>
         <v>8390</v>
       </c>
     </row>
-    <row r="116" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B116" s="4" t="s">
+    <row r="117" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B117" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="C116" s="5">
+      <c r="C117" s="5">
         <v>500</v>
       </c>
-      <c r="D116" s="4">
+      <c r="D117" s="4">
         <f t="shared" si="16"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="117" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="16" t="s">
-        <v>165</v>
-      </c>
-      <c r="B117" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="C117" s="5">
-        <v>750</v>
-      </c>
-      <c r="D117" s="4">
-        <f t="shared" ref="D117:D122" si="17">D116+C117</f>
-        <v>9640</v>
-      </c>
-    </row>
     <row r="118" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="B118" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C118" s="5">
+        <v>750</v>
+      </c>
+      <c r="D118" s="4">
+        <f t="shared" ref="D118:D123" si="17">D117+C118</f>
+        <v>9640</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="B118" s="4" t="s">
+      <c r="B119" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C118" s="5">
+      <c r="C119" s="5">
         <v>2000</v>
       </c>
-      <c r="D118" s="4">
+      <c r="D119" s="4">
         <f t="shared" si="17"/>
         <v>11640</v>
       </c>
     </row>
-    <row r="119" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B119" s="4" t="s">
+    <row r="120" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B120" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C119" s="5">
+      <c r="C120" s="5">
         <v>2000</v>
       </c>
-      <c r="D119" s="4">
+      <c r="D120" s="4">
         <f t="shared" si="17"/>
         <v>13640</v>
       </c>
     </row>
-    <row r="120" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B120" s="4" t="s">
+    <row r="121" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B121" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C120" s="5">
+      <c r="C121" s="5">
         <v>-10000</v>
       </c>
-      <c r="D120" s="4">
+      <c r="D121" s="4">
         <f t="shared" si="17"/>
         <v>3640</v>
       </c>
     </row>
-    <row r="121" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B121" s="4" t="s">
+    <row r="122" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B122" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="C121" s="5">
+      <c r="C122" s="5">
         <v>350</v>
       </c>
-      <c r="D121" s="4">
+      <c r="D122" s="4">
         <f t="shared" si="17"/>
         <v>3990</v>
       </c>
     </row>
-    <row r="122" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="16" t="s">
+    <row r="123" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="B122" s="4" t="s">
+      <c r="B123" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="C122" s="5">
+      <c r="C123" s="5">
         <v>300</v>
       </c>
-      <c r="D122" s="4">
+      <c r="D123" s="4">
         <f t="shared" si="17"/>
         <v>4290</v>
       </c>
     </row>
-    <row r="123" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="16" t="s">
+    <row r="124" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="B123" s="4" t="s">
+      <c r="B124" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="C123" s="5">
+      <c r="C124" s="5">
         <v>3800</v>
       </c>
-      <c r="D123" s="4">
-        <f t="shared" ref="D123:D129" si="18">D122+C123</f>
+      <c r="D124" s="4">
+        <f t="shared" ref="D124:D130" si="18">D123+C124</f>
         <v>8090</v>
       </c>
     </row>
-    <row r="124" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B124" s="4" t="s">
+    <row r="125" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B125" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C124" s="5">
+      <c r="C125" s="5">
         <v>500</v>
       </c>
-      <c r="D124" s="4">
+      <c r="D125" s="4">
         <f t="shared" si="18"/>
         <v>8590</v>
       </c>
     </row>
-    <row r="125" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="16" t="s">
+    <row r="126" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="B125" s="4" t="s">
+      <c r="B126" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="C125" s="5">
+      <c r="C126" s="5">
         <v>1300</v>
       </c>
-      <c r="D125" s="4">
+      <c r="D126" s="4">
         <f t="shared" si="18"/>
         <v>9890</v>
       </c>
     </row>
-    <row r="126" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="16" t="s">
+    <row r="127" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="B126" s="4" t="s">
+      <c r="B127" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C126" s="5">
+      <c r="C127" s="5">
         <v>9000</v>
       </c>
-      <c r="D126" s="4">
+      <c r="D127" s="4">
         <f t="shared" si="18"/>
         <v>18890</v>
       </c>
     </row>
-    <row r="127" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B127" s="4" t="s">
+    <row r="128" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B128" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C127" s="5">
+      <c r="C128" s="5">
         <v>-10000</v>
       </c>
-      <c r="D127" s="4">
+      <c r="D128" s="4">
         <f t="shared" si="18"/>
         <v>8890</v>
       </c>
     </row>
-    <row r="128" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="16" t="s">
+    <row r="129" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="B128" s="4" t="s">
+      <c r="B129" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C128" s="5">
+      <c r="C129" s="5">
         <v>2000</v>
       </c>
-      <c r="D128" s="4">
+      <c r="D129" s="4">
         <f t="shared" si="18"/>
         <v>10890</v>
       </c>
     </row>
-    <row r="129" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B129" s="4" t="s">
+    <row r="130" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B130" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C129" s="5">
+      <c r="C130" s="5">
         <v>-10000</v>
       </c>
-      <c r="D129" s="4">
+      <c r="D130" s="4">
         <f t="shared" si="18"/>
         <v>890</v>
       </c>
     </row>
-    <row r="130" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="B130" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="C130" s="5">
-        <v>500</v>
-      </c>
-      <c r="D130" s="4">
-        <f t="shared" ref="D130:D135" si="19">D129+C130</f>
-        <v>1390</v>
-      </c>
-    </row>
     <row r="131" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="B131" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C131" s="5">
+        <v>500</v>
+      </c>
+      <c r="D131" s="4">
+        <f t="shared" ref="D131:D136" si="19">D130+C131</f>
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="B131" s="4" t="s">
+      <c r="B132" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="C131" s="5">
+      <c r="C132" s="5">
         <v>10000</v>
       </c>
-      <c r="D131" s="4">
+      <c r="D132" s="4">
         <f t="shared" si="19"/>
         <v>11390</v>
       </c>
     </row>
-    <row r="132" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B132" s="4" t="s">
+    <row r="133" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B133" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C132" s="5">
+      <c r="C133" s="5">
         <v>-10000</v>
       </c>
-      <c r="D132" s="4">
+      <c r="D133" s="4">
         <f t="shared" si="19"/>
         <v>1390</v>
       </c>
     </row>
-    <row r="133" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="16" t="s">
+    <row r="134" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="B133" s="4" t="s">
+      <c r="B134" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C133" s="5">
+      <c r="C134" s="5">
         <v>3000</v>
       </c>
-      <c r="D133" s="4">
+      <c r="D134" s="4">
         <f t="shared" si="19"/>
         <v>4390</v>
       </c>
     </row>
-    <row r="134" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="16" t="s">
+    <row r="135" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="B134" s="4" t="s">
+      <c r="B135" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C134" s="5">
+      <c r="C135" s="5">
         <v>2000</v>
       </c>
-      <c r="D134" s="4">
+      <c r="D135" s="4">
         <f t="shared" si="19"/>
         <v>6390</v>
       </c>
     </row>
-    <row r="135" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B135" s="4" t="s">
+    <row r="136" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B136" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C135" s="5">
+      <c r="C136" s="5">
         <v>2000</v>
       </c>
-      <c r="D135" s="4">
+      <c r="D136" s="4">
         <f t="shared" si="19"/>
         <v>8390</v>
       </c>
     </row>
-    <row r="136" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="16" t="s">
+    <row r="137" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="B136" s="4" t="s">
+      <c r="B137" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C136" s="5">
+      <c r="C137" s="5">
         <v>11000</v>
       </c>
-      <c r="D136" s="4">
-        <f t="shared" ref="D136:D141" si="20">D135+C136</f>
+      <c r="D137" s="4">
+        <f t="shared" ref="D137:D142" si="20">D136+C137</f>
         <v>19390</v>
       </c>
     </row>
-    <row r="137" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B137" s="4" t="s">
+    <row r="138" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B138" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C137" s="5">
+      <c r="C138" s="5">
         <v>-10000</v>
       </c>
-      <c r="D137" s="4">
+      <c r="D138" s="4">
         <f t="shared" si="20"/>
         <v>9390</v>
       </c>
     </row>
-    <row r="138" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="16" t="s">
+    <row r="139" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="16" t="s">
         <v>187</v>
       </c>
-      <c r="B138" s="4" t="s">
+      <c r="B139" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C138" s="5">
+      <c r="C139" s="5">
         <v>3000</v>
       </c>
-      <c r="D138" s="4">
+      <c r="D139" s="4">
         <f t="shared" si="20"/>
         <v>12390</v>
       </c>
     </row>
-    <row r="139" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B139" s="4" t="s">
+    <row r="140" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B140" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C139" s="5">
+      <c r="C140" s="5">
         <v>-10000</v>
       </c>
-      <c r="D139" s="4">
+      <c r="D140" s="4">
         <f t="shared" si="20"/>
         <v>2390</v>
       </c>
     </row>
-    <row r="140" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B140" s="4" t="s">
+    <row r="141" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B141" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C140" s="5">
+      <c r="C141" s="5">
         <v>500</v>
       </c>
-      <c r="D140" s="4">
+      <c r="D141" s="4">
         <f t="shared" si="20"/>
         <v>2890</v>
       </c>
     </row>
-    <row r="141" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="16" t="s">
+    <row r="142" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="16" t="s">
         <v>189</v>
       </c>
-      <c r="B141" s="4" t="s">
+      <c r="B142" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C141" s="5">
+      <c r="C142" s="5">
         <v>5600</v>
       </c>
-      <c r="D141" s="4">
+      <c r="D142" s="4">
         <f t="shared" si="20"/>
         <v>8490</v>
       </c>
     </row>
-    <row r="142" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B142" s="4" t="s">
+    <row r="143" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B143" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="C142" s="5">
+      <c r="C143" s="5">
         <v>4700</v>
       </c>
-      <c r="D142" s="4">
-        <f t="shared" ref="D142:D148" si="21">D141+C142</f>
+      <c r="D143" s="4">
+        <f t="shared" ref="D143:D149" si="21">D142+C143</f>
         <v>13190</v>
       </c>
     </row>
-    <row r="143" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="16" t="s">
+    <row r="144" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="16" t="s">
         <v>192</v>
       </c>
-      <c r="B143" s="4" t="s">
+      <c r="B144" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C143" s="5">
+      <c r="C144" s="5">
         <v>1500</v>
       </c>
-      <c r="D143" s="4">
+      <c r="D144" s="4">
         <f t="shared" si="21"/>
         <v>14690</v>
       </c>
     </row>
-    <row r="144" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B144" s="4" t="s">
+    <row r="145" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B145" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C144" s="5">
+      <c r="C145" s="5">
         <v>500</v>
       </c>
-      <c r="D144" s="4">
+      <c r="D145" s="4">
         <f t="shared" si="21"/>
         <v>15190</v>
       </c>
     </row>
-    <row r="145" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="16" t="s">
+    <row r="146" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="B145" s="4" t="s">
+      <c r="B146" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="C145" s="5">
+      <c r="C146" s="5">
         <v>1000</v>
       </c>
-      <c r="D145" s="4">
+      <c r="D146" s="4">
         <f t="shared" si="21"/>
         <v>16190</v>
       </c>
     </row>
-    <row r="146" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="16" t="s">
+    <row r="147" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="B146" s="4" t="s">
+      <c r="B147" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="C146" s="5">
+      <c r="C147" s="5">
         <v>1000</v>
       </c>
-      <c r="D146" s="4">
+      <c r="D147" s="4">
         <f t="shared" si="21"/>
         <v>17190</v>
       </c>
     </row>
-    <row r="147" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="16" t="s">
+    <row r="148" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="B147" s="4" t="s">
+      <c r="B148" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C147" s="5">
+      <c r="C148" s="5">
         <v>3000</v>
       </c>
-      <c r="D147" s="4">
+      <c r="D148" s="4">
         <f t="shared" si="21"/>
         <v>20190</v>
       </c>
     </row>
-    <row r="148" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B148" s="4" t="s">
+    <row r="149" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B149" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C148" s="5">
+      <c r="C149" s="5">
         <v>-20000</v>
       </c>
-      <c r="D148" s="4">
+      <c r="D149" s="4">
         <f t="shared" si="21"/>
         <v>190</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B149" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C149" s="5">
-        <v>500</v>
-      </c>
-      <c r="D149" s="4">
-        <f t="shared" ref="D149:D155" si="22">D148+C149</f>
-        <v>690</v>
       </c>
     </row>
     <row r="150" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -3718,662 +3721,701 @@
         <v>500</v>
       </c>
       <c r="D150" s="4">
+        <f t="shared" ref="D150:D156" si="22">D149+C150</f>
+        <v>690</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B151" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C151" s="5">
+        <v>500</v>
+      </c>
+      <c r="D151" s="4">
         <f t="shared" si="22"/>
         <v>1190</v>
       </c>
     </row>
-    <row r="151" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="16" t="s">
+    <row r="152" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A152" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="B151" s="4" t="s">
+      <c r="B152" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="C151" s="5">
+      <c r="C152" s="5">
         <v>10000</v>
       </c>
-      <c r="D151" s="4">
+      <c r="D152" s="4">
         <f t="shared" si="22"/>
         <v>11190</v>
       </c>
     </row>
-    <row r="152" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B152" s="4" t="s">
+    <row r="153" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B153" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="C152" s="5">
+      <c r="C153" s="5">
         <v>-10000</v>
       </c>
-      <c r="D152" s="4">
+      <c r="D153" s="4">
         <f t="shared" si="22"/>
         <v>1190</v>
       </c>
     </row>
-    <row r="153" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="16" t="s">
+    <row r="154" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="B153" s="4" t="s">
+      <c r="B154" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C153" s="5">
+      <c r="C154" s="5">
         <v>3000</v>
       </c>
-      <c r="D153" s="4">
+      <c r="D154" s="4">
         <f t="shared" si="22"/>
         <v>4190</v>
       </c>
     </row>
-    <row r="154" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="16" t="s">
+    <row r="155" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="B154" s="4" t="s">
+      <c r="B155" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C154" s="5">
+      <c r="C155" s="5">
         <v>11000</v>
       </c>
-      <c r="D154" s="4">
+      <c r="D155" s="4">
         <f t="shared" si="22"/>
         <v>15190</v>
       </c>
     </row>
-    <row r="155" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B155" s="4" t="s">
+    <row r="156" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B156" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C155" s="5">
+      <c r="C156" s="5">
         <v>-10000</v>
       </c>
-      <c r="D155" s="4">
+      <c r="D156" s="4">
         <f t="shared" si="22"/>
         <v>5190</v>
       </c>
     </row>
-    <row r="156" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="B156" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C156" s="5">
-        <v>3000</v>
-      </c>
-      <c r="D156" s="4">
-        <f t="shared" ref="D156:D162" si="23">D155+C156</f>
-        <v>8190</v>
-      </c>
-    </row>
     <row r="157" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="B157" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C157" s="5">
+        <v>3000</v>
+      </c>
+      <c r="D157" s="4">
+        <f t="shared" ref="D157:D163" si="23">D156+C157</f>
+        <v>8190</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="B157" s="4" t="s">
+      <c r="B158" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="C157" s="5">
+      <c r="C158" s="5">
         <v>14000</v>
       </c>
-      <c r="D157" s="4">
+      <c r="D158" s="4">
         <f t="shared" si="23"/>
         <v>22190</v>
       </c>
     </row>
-    <row r="158" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B158" s="4" t="s">
+    <row r="159" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B159" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="C158" s="5">
+      <c r="C159" s="5">
         <v>-20000</v>
       </c>
-      <c r="D158" s="4">
+      <c r="D159" s="4">
         <f t="shared" si="23"/>
         <v>2190</v>
       </c>
     </row>
-    <row r="159" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="16" t="s">
+    <row r="160" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="B159" s="4" t="s">
+      <c r="B160" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="C159" s="5">
+      <c r="C160" s="5">
         <v>5000</v>
       </c>
-      <c r="D159" s="4">
+      <c r="D160" s="4">
         <f t="shared" si="23"/>
         <v>7190</v>
       </c>
     </row>
-    <row r="160" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="16" t="s">
+    <row r="161" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A161" s="16" t="s">
         <v>213</v>
       </c>
-      <c r="B160" s="4" t="s">
+      <c r="B161" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="C160" s="5">
+      <c r="C161" s="5">
         <v>5000</v>
       </c>
-      <c r="D160" s="4">
+      <c r="D161" s="4">
         <f t="shared" si="23"/>
         <v>12190</v>
       </c>
     </row>
-    <row r="161" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="16" t="s">
+    <row r="162" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="16" t="s">
         <v>215</v>
       </c>
-      <c r="B161" s="4" t="s">
+      <c r="B162" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C161" s="5">
+      <c r="C162" s="5">
         <v>11000</v>
       </c>
-      <c r="D161" s="4">
+      <c r="D162" s="4">
         <f t="shared" si="23"/>
         <v>23190</v>
       </c>
     </row>
-    <row r="162" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B162" s="4" t="s">
+    <row r="163" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B163" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C162" s="5">
+      <c r="C163" s="5">
         <v>-20000</v>
       </c>
-      <c r="D162" s="4">
+      <c r="D163" s="4">
         <f t="shared" si="23"/>
         <v>3190</v>
       </c>
     </row>
-    <row r="163" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="16" t="s">
+    <row r="164" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="16" t="s">
         <v>216</v>
       </c>
-      <c r="B163" s="4" t="s">
+      <c r="B164" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C163" s="5">
+      <c r="C164" s="5">
         <v>500</v>
       </c>
-      <c r="D163" s="4">
-        <f t="shared" ref="D163:D168" si="24">D162+C163</f>
+      <c r="D164" s="4">
+        <f t="shared" ref="D164:D169" si="24">D163+C164</f>
         <v>3690</v>
       </c>
     </row>
-    <row r="164" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B164" s="4" t="s">
+    <row r="165" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B165" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C164" s="5">
+     